<commit_message>
GH ACTION Headlines Mon Sep 18 23:08:47 UTC 2023
</commit_message>
<xml_diff>
--- a/Data/obligacje_screener.xlsx
+++ b/Data/obligacje_screener.xlsx
@@ -512,7 +512,7 @@
         <v>45340</v>
       </c>
       <c r="I2">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="J2" t="inlineStr">
         <is>
@@ -600,13 +600,13 @@
         <v>45121</v>
       </c>
       <c r="G3">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="H3" s="2">
         <v>45305</v>
       </c>
       <c r="I3">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="J3" t="inlineStr">
         <is>
@@ -703,13 +703,13 @@
         <v>45039</v>
       </c>
       <c r="G4">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="H4" s="2">
         <v>45222</v>
       </c>
       <c r="I4">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="J4" t="inlineStr">
         <is>
@@ -806,13 +806,13 @@
         <v>45039</v>
       </c>
       <c r="G5">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="H5" s="2">
         <v>45222</v>
       </c>
       <c r="I5">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="J5" t="inlineStr">
         <is>
@@ -909,13 +909,13 @@
         <v>45129</v>
       </c>
       <c r="G6">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="H6" s="2">
         <v>45221</v>
       </c>
       <c r="I6">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="J6" t="inlineStr">
         <is>
@@ -1012,13 +1012,13 @@
         <v>45162</v>
       </c>
       <c r="G7">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="H7" s="2">
         <v>45254</v>
       </c>
       <c r="I7">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="J7" t="inlineStr">
         <is>
@@ -1110,13 +1110,13 @@
         <v>45156</v>
       </c>
       <c r="G8">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="H8" s="2">
         <v>45248</v>
       </c>
       <c r="I8">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="J8" t="inlineStr">
         <is>
@@ -1213,13 +1213,13 @@
         <v>45141</v>
       </c>
       <c r="G9">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="H9" s="2">
         <v>45233</v>
       </c>
       <c r="I9">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="J9" t="inlineStr">
         <is>
@@ -1316,13 +1316,13 @@
         <v>45062</v>
       </c>
       <c r="G10">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="H10" s="2">
         <v>45246</v>
       </c>
       <c r="I10">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="J10" t="inlineStr">
         <is>
@@ -1419,7 +1419,7 @@
         <v>45286</v>
       </c>
       <c r="I11">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="J11" t="inlineStr">
         <is>
@@ -1516,13 +1516,13 @@
         <v>45011</v>
       </c>
       <c r="G12">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="H12" s="2">
         <v>45195</v>
       </c>
       <c r="I12">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="J12" t="inlineStr">
         <is>
@@ -1614,13 +1614,13 @@
         <v>45036</v>
       </c>
       <c r="G13">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="H13" s="2">
         <v>45219</v>
       </c>
       <c r="I13">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="J13" t="inlineStr">
         <is>
@@ -1717,13 +1717,13 @@
         <v>45036</v>
       </c>
       <c r="G14">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="H14" s="2">
         <v>45219</v>
       </c>
       <c r="I14">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="J14" t="inlineStr">
         <is>
@@ -1820,13 +1820,13 @@
         <v>45106</v>
       </c>
       <c r="G15">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="H15" s="2">
         <v>45289</v>
       </c>
       <c r="I15">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="J15" t="inlineStr">
         <is>
@@ -1923,13 +1923,13 @@
         <v>45094</v>
       </c>
       <c r="G16">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="H16" s="2">
         <v>45186</v>
       </c>
       <c r="I16">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="J16" t="inlineStr">
         <is>
@@ -2026,13 +2026,13 @@
         <v>45094</v>
       </c>
       <c r="G17">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="H17" s="2">
         <v>45186</v>
       </c>
       <c r="I17">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="J17" t="inlineStr">
         <is>
@@ -2129,13 +2129,13 @@
         <v>45132</v>
       </c>
       <c r="G18">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="H18" s="2">
         <v>45224</v>
       </c>
       <c r="I18">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="J18" t="inlineStr">
         <is>
@@ -2232,13 +2232,13 @@
         <v>45137</v>
       </c>
       <c r="G19">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="H19" s="2">
         <v>45229</v>
       </c>
       <c r="I19">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="J19" t="inlineStr">
         <is>
@@ -2330,13 +2330,13 @@
         <v>45183</v>
       </c>
       <c r="G20">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="H20" s="2">
         <v>45274</v>
       </c>
       <c r="I20">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="J20" t="inlineStr">
         <is>
@@ -2433,13 +2433,13 @@
         <v>45093</v>
       </c>
       <c r="G21">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="H21" s="2">
         <v>45187</v>
       </c>
       <c r="I21">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J21" t="inlineStr">
         <is>
@@ -2536,13 +2536,13 @@
         <v>45096</v>
       </c>
       <c r="G22">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="H22" s="2">
         <v>45187</v>
       </c>
       <c r="I22">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J22" t="inlineStr">
         <is>
@@ -2639,7 +2639,7 @@
         <v>45245</v>
       </c>
       <c r="I23">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="J23" t="inlineStr">
         <is>
@@ -2736,7 +2736,7 @@
         <v>45245</v>
       </c>
       <c r="I24">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="J24" t="inlineStr">
         <is>
@@ -2833,13 +2833,13 @@
         <v>45021</v>
       </c>
       <c r="G25">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="H25" s="2">
         <v>45204</v>
       </c>
       <c r="I25">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="J25" t="inlineStr">
         <is>
@@ -2936,13 +2936,13 @@
         <v>45160</v>
       </c>
       <c r="G26">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="H26" s="2">
         <v>45344</v>
       </c>
       <c r="I26">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="J26" t="inlineStr">
         <is>
@@ -3039,13 +3039,13 @@
         <v>45118</v>
       </c>
       <c r="G27">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="H27" s="2">
         <v>45302</v>
       </c>
       <c r="I27">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="J27" t="inlineStr">
         <is>
@@ -3142,13 +3142,13 @@
         <v>45085</v>
       </c>
       <c r="G28">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="H28" s="2">
         <v>45268</v>
       </c>
       <c r="I28">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="J28" t="inlineStr">
         <is>
@@ -3245,13 +3245,13 @@
         <v>45183</v>
       </c>
       <c r="G29">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="H29" s="2">
         <v>45274</v>
       </c>
       <c r="I29">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="J29" t="inlineStr">
         <is>
@@ -3348,7 +3348,7 @@
         <v>45224</v>
       </c>
       <c r="I30">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="J30" t="inlineStr">
         <is>
@@ -3445,13 +3445,13 @@
         <v>45153</v>
       </c>
       <c r="G31">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="H31" s="2">
         <v>45245</v>
       </c>
       <c r="I31">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="J31" t="inlineStr">
         <is>
@@ -3548,13 +3548,13 @@
         <v>45155</v>
       </c>
       <c r="G32">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="H32" s="2">
         <v>45247</v>
       </c>
       <c r="I32">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="J32" t="inlineStr">
         <is>
@@ -3651,7 +3651,7 @@
         <v>45255</v>
       </c>
       <c r="I33">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="J33" t="inlineStr">
         <is>
@@ -3739,13 +3739,13 @@
         <v>45176</v>
       </c>
       <c r="G34">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="H34" s="2">
         <v>45267</v>
       </c>
       <c r="I34">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="J34" t="inlineStr">
         <is>
@@ -3842,13 +3842,13 @@
         <v>45130</v>
       </c>
       <c r="G35">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="H35" s="2">
         <v>45222</v>
       </c>
       <c r="I35">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="J35" t="inlineStr">
         <is>
@@ -3940,13 +3940,13 @@
         <v>45115</v>
       </c>
       <c r="G36">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="H36" s="2">
         <v>45207</v>
       </c>
       <c r="I36">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="J36" t="inlineStr">
         <is>
@@ -4043,13 +4043,13 @@
         <v>45097</v>
       </c>
       <c r="G37">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="H37" s="2">
         <v>45189</v>
       </c>
       <c r="I37">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="J37" t="inlineStr">
         <is>
@@ -4141,13 +4141,13 @@
         <v>45107</v>
       </c>
       <c r="G38">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="H38" s="2">
         <v>45290</v>
       </c>
       <c r="I38">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="J38" t="inlineStr">
         <is>
@@ -4244,13 +4244,13 @@
         <v>45063</v>
       </c>
       <c r="G39">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="H39" s="2">
         <v>45247</v>
       </c>
       <c r="I39">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="J39" t="inlineStr">
         <is>
@@ -4347,13 +4347,13 @@
         <v>45177</v>
       </c>
       <c r="G40">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="H40" s="2">
         <v>45359</v>
       </c>
       <c r="I40">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="J40" t="inlineStr">
         <is>
@@ -4450,13 +4450,13 @@
         <v>45107</v>
       </c>
       <c r="G41">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="H41" s="2">
         <v>45290</v>
       </c>
       <c r="I41">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="J41" t="inlineStr">
         <is>
@@ -4553,7 +4553,7 @@
         <v>45265</v>
       </c>
       <c r="I42">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="J42" t="inlineStr">
         <is>
@@ -4650,13 +4650,13 @@
         <v>45098</v>
       </c>
       <c r="G43">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="H43" s="2">
         <v>45281</v>
       </c>
       <c r="I43">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="J43" t="inlineStr">
         <is>
@@ -4753,13 +4753,13 @@
         <v>45099</v>
       </c>
       <c r="G44">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="H44" s="2">
         <v>45282</v>
       </c>
       <c r="I44">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="J44" t="inlineStr">
         <is>
@@ -4856,13 +4856,13 @@
         <v>45106</v>
       </c>
       <c r="G45">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="H45" s="2">
         <v>45289</v>
       </c>
       <c r="I45">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="J45" t="inlineStr">
         <is>
@@ -4959,13 +4959,13 @@
         <v>45106</v>
       </c>
       <c r="G46">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="H46" s="2">
         <v>45289</v>
       </c>
       <c r="I46">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="J46" t="inlineStr">
         <is>
@@ -5062,13 +5062,13 @@
         <v>45120</v>
       </c>
       <c r="G47">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="H47" s="2">
         <v>45304</v>
       </c>
       <c r="I47">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="J47" t="inlineStr">
         <is>
@@ -5165,13 +5165,13 @@
         <v>45118</v>
       </c>
       <c r="G48">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="H48" s="2">
         <v>45302</v>
       </c>
       <c r="I48">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="J48" t="inlineStr">
         <is>
@@ -5268,13 +5268,13 @@
         <v>45152</v>
       </c>
       <c r="G49">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="H49" s="2">
         <v>45336</v>
       </c>
       <c r="I49">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="J49" t="inlineStr">
         <is>
@@ -5371,13 +5371,13 @@
         <v>45042</v>
       </c>
       <c r="G50">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="H50" s="2">
         <v>45225</v>
       </c>
       <c r="I50">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="J50" t="inlineStr">
         <is>
@@ -5474,13 +5474,13 @@
         <v>45122</v>
       </c>
       <c r="G51">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="H51" s="2">
         <v>45306</v>
       </c>
       <c r="I51">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="J51" t="inlineStr">
         <is>
@@ -5577,13 +5577,13 @@
         <v>45139</v>
       </c>
       <c r="G52">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="H52" s="2">
         <v>45323</v>
       </c>
       <c r="I52">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="J52" t="inlineStr">
         <is>
@@ -5671,13 +5671,13 @@
         <v>45099</v>
       </c>
       <c r="G53">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="H53" s="2">
         <v>45282</v>
       </c>
       <c r="I53">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="J53" t="inlineStr">
         <is>
@@ -5774,7 +5774,7 @@
         <v>45196</v>
       </c>
       <c r="I54">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="J54" t="inlineStr">
         <is>
@@ -5871,13 +5871,13 @@
         <v>45044</v>
       </c>
       <c r="G55">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="H55" s="2">
         <v>45227</v>
       </c>
       <c r="I55">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="J55" t="inlineStr">
         <is>
@@ -5974,13 +5974,13 @@
         <v>45151</v>
       </c>
       <c r="G56">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="H56" s="2">
         <v>45243</v>
       </c>
       <c r="I56">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="J56" t="inlineStr">
         <is>
@@ -6072,7 +6072,7 @@
         <v>45196</v>
       </c>
       <c r="I57">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="J57" t="inlineStr">
         <is>
@@ -6169,13 +6169,13 @@
         <v>45069</v>
       </c>
       <c r="G58">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="H58" s="2">
         <v>45253</v>
       </c>
       <c r="I58">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="J58" t="inlineStr">
         <is>
@@ -6272,13 +6272,13 @@
         <v>45099</v>
       </c>
       <c r="G59">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="H59" s="2">
         <v>45191</v>
       </c>
       <c r="I59">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="J59" t="inlineStr">
         <is>
@@ -6370,13 +6370,13 @@
         <v>45113</v>
       </c>
       <c r="G60">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="H60" s="2">
         <v>45205</v>
       </c>
       <c r="I60">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="J60" t="inlineStr">
         <is>
@@ -6473,13 +6473,13 @@
         <v>45127</v>
       </c>
       <c r="G61">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="H61" s="2">
         <v>45219</v>
       </c>
       <c r="I61">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="J61" t="inlineStr">
         <is>
@@ -6576,13 +6576,13 @@
         <v>45058</v>
       </c>
       <c r="G62">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="H62" s="2">
         <v>45242</v>
       </c>
       <c r="I62">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="J62" t="inlineStr">
         <is>
@@ -6679,13 +6679,13 @@
         <v>45010</v>
       </c>
       <c r="G63">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="H63" s="2">
         <v>45194</v>
       </c>
       <c r="I63">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="J63" t="inlineStr">
         <is>
@@ -6777,13 +6777,13 @@
         <v>45025</v>
       </c>
       <c r="G64">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="H64" s="2">
         <v>45208</v>
       </c>
       <c r="I64">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="J64" t="inlineStr">
         <is>
@@ -6880,13 +6880,13 @@
         <v>45025</v>
       </c>
       <c r="G65">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="H65" s="2">
         <v>45208</v>
       </c>
       <c r="I65">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="J65" t="inlineStr">
         <is>
@@ -6983,13 +6983,13 @@
         <v>45089</v>
       </c>
       <c r="G66">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="H66" s="2">
         <v>45272</v>
       </c>
       <c r="I66">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="J66" t="inlineStr">
         <is>
@@ -7086,13 +7086,13 @@
         <v>45178</v>
       </c>
       <c r="G67">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="H67" s="2">
         <v>45269</v>
       </c>
       <c r="I67">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="J67" t="inlineStr">
         <is>
@@ -7184,13 +7184,13 @@
         <v>45104</v>
       </c>
       <c r="G68">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="H68" s="2">
         <v>45196</v>
       </c>
       <c r="I68">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="J68" t="inlineStr">
         <is>
@@ -7287,13 +7287,13 @@
         <v>45149</v>
       </c>
       <c r="G69">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="H69" s="2">
         <v>45241</v>
       </c>
       <c r="I69">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="J69" t="inlineStr">
         <is>
@@ -7390,7 +7390,7 @@
         <v>45205</v>
       </c>
       <c r="I70">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="J70" t="inlineStr">
         <is>
@@ -7487,13 +7487,13 @@
         <v>45114</v>
       </c>
       <c r="G71">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="H71" s="2">
         <v>45205</v>
       </c>
       <c r="I71">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="J71" t="inlineStr">
         <is>
@@ -7590,13 +7590,13 @@
         <v>45115</v>
       </c>
       <c r="G72">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="H72" s="2">
         <v>45207</v>
       </c>
       <c r="I72">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="J72" t="inlineStr">
         <is>
@@ -7693,13 +7693,13 @@
         <v>45097</v>
       </c>
       <c r="G73">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="H73" s="2">
         <v>45189</v>
       </c>
       <c r="I73">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="J73" t="inlineStr">
         <is>
@@ -7791,13 +7791,13 @@
         <v>45038</v>
       </c>
       <c r="G74">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="H74" s="2">
         <v>45221</v>
       </c>
       <c r="I74">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="J74" t="inlineStr">
         <is>
@@ -7889,13 +7889,13 @@
         <v>45117</v>
       </c>
       <c r="G75">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="H75" s="2">
         <v>45301</v>
       </c>
       <c r="I75">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="J75" t="inlineStr">
         <is>
@@ -7992,13 +7992,13 @@
         <v>45160</v>
       </c>
       <c r="G76">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="H76" s="2">
         <v>45344</v>
       </c>
       <c r="I76">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="J76" t="inlineStr">
         <is>
@@ -8095,13 +8095,13 @@
         <v>45002</v>
       </c>
       <c r="G77">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="H77" s="2">
         <v>45186</v>
       </c>
       <c r="I77">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="J77" t="inlineStr">
         <is>
@@ -8198,13 +8198,13 @@
         <v>45043</v>
       </c>
       <c r="G78">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="H78" s="2">
         <v>45226</v>
       </c>
       <c r="I78">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="J78" t="inlineStr">
         <is>
@@ -8301,13 +8301,13 @@
         <v>45079</v>
       </c>
       <c r="G79">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="H79" s="2">
         <v>45262</v>
       </c>
       <c r="I79">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="J79" t="inlineStr">
         <is>
@@ -8404,7 +8404,7 @@
         <v>45254</v>
       </c>
       <c r="I80">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="J80" t="inlineStr">
         <is>
@@ -8501,13 +8501,13 @@
         <v>45104</v>
       </c>
       <c r="G81">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="H81" s="2">
         <v>45287</v>
       </c>
       <c r="I81">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="J81" t="inlineStr">
         <is>
@@ -8604,7 +8604,7 @@
         <v>45288</v>
       </c>
       <c r="I82">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="J82" t="inlineStr">
         <is>
@@ -8696,13 +8696,13 @@
         <v>45175</v>
       </c>
       <c r="G83">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="H83" s="2">
         <v>45357</v>
       </c>
       <c r="I83">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="J83" t="inlineStr">
         <is>
@@ -8799,13 +8799,13 @@
         <v>45054</v>
       </c>
       <c r="G84">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="H84" s="2">
         <v>45238</v>
       </c>
       <c r="I84">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="J84" t="inlineStr">
         <is>
@@ -8902,13 +8902,13 @@
         <v>45056</v>
       </c>
       <c r="G85">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="H85" s="2">
         <v>45240</v>
       </c>
       <c r="I85">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="J85" t="inlineStr">
         <is>
@@ -9005,13 +9005,13 @@
         <v>45085</v>
       </c>
       <c r="G86">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="H86" s="2">
         <v>45268</v>
       </c>
       <c r="I86">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="J86" t="inlineStr">
         <is>
@@ -9108,7 +9108,7 @@
         <v>45194</v>
       </c>
       <c r="I87">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="J87" t="inlineStr">
         <is>
@@ -9195,13 +9195,13 @@
         <v>45103</v>
       </c>
       <c r="G88">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="H88" s="2">
         <v>45286</v>
       </c>
       <c r="I88">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="J88" t="inlineStr">
         <is>
@@ -9298,13 +9298,13 @@
         <v>45103</v>
       </c>
       <c r="G89">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="H89" s="2">
         <v>45286</v>
       </c>
       <c r="I89">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="J89" t="inlineStr">
         <is>
@@ -9401,13 +9401,13 @@
         <v>45008</v>
       </c>
       <c r="G90">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="H90" s="2">
         <v>45192</v>
       </c>
       <c r="I90">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="J90" t="inlineStr">
         <is>
@@ -9499,13 +9499,13 @@
         <v>45100</v>
       </c>
       <c r="G91">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="H91" s="2">
         <v>45287</v>
       </c>
       <c r="I91">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="J91" t="inlineStr">
         <is>
@@ -9602,13 +9602,13 @@
         <v>45003</v>
       </c>
       <c r="G92">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="H92" s="2">
         <v>45187</v>
       </c>
       <c r="I92">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J92" t="inlineStr">
         <is>
@@ -9705,13 +9705,13 @@
         <v>45104</v>
       </c>
       <c r="G93">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="H93" s="2">
         <v>45287</v>
       </c>
       <c r="I93">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="J93" t="inlineStr">
         <is>
@@ -9808,13 +9808,13 @@
         <v>45104</v>
       </c>
       <c r="G94">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="H94" s="2">
         <v>45287</v>
       </c>
       <c r="I94">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="J94" t="inlineStr">
         <is>
@@ -9911,13 +9911,13 @@
         <v>45049</v>
       </c>
       <c r="G95">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="H95" s="2">
         <v>45233</v>
       </c>
       <c r="I95">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="J95" t="inlineStr">
         <is>
@@ -10014,13 +10014,13 @@
         <v>45122</v>
       </c>
       <c r="G96">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="H96" s="2">
         <v>45306</v>
       </c>
       <c r="I96">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="J96" t="inlineStr">
         <is>
@@ -10112,13 +10112,13 @@
         <v>45141</v>
       </c>
       <c r="G97">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="H97" s="2">
         <v>45325</v>
       </c>
       <c r="I97">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="J97" t="inlineStr">
         <is>
@@ -10215,13 +10215,13 @@
         <v>45010</v>
       </c>
       <c r="G98">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="H98" s="2">
         <v>45194</v>
       </c>
       <c r="I98">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="J98" t="inlineStr">
         <is>
@@ -10313,13 +10313,13 @@
         <v>45093</v>
       </c>
       <c r="G99">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="H99" s="2">
         <v>45276</v>
       </c>
       <c r="I99">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="J99" t="inlineStr">
         <is>
@@ -10416,13 +10416,13 @@
         <v>45123</v>
       </c>
       <c r="G100">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="H100" s="2">
         <v>45307</v>
       </c>
       <c r="I100">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="J100" t="inlineStr">
         <is>
@@ -10519,13 +10519,13 @@
         <v>45014</v>
       </c>
       <c r="G101">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="H101" s="2">
         <v>45198</v>
       </c>
       <c r="I101">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="J101" t="inlineStr">
         <is>
@@ -10622,13 +10622,13 @@
         <v>45093</v>
       </c>
       <c r="G102">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="H102" s="2">
         <v>45276</v>
       </c>
       <c r="I102">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="J102" t="inlineStr">
         <is>
@@ -10725,13 +10725,13 @@
         <v>45122</v>
       </c>
       <c r="G103">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="H103" s="2">
         <v>45306</v>
       </c>
       <c r="I103">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="J103" t="inlineStr">
         <is>
@@ -10828,13 +10828,13 @@
         <v>45122</v>
       </c>
       <c r="G104">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="H104" s="2">
         <v>45306</v>
       </c>
       <c r="I104">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="J104" t="inlineStr">
         <is>
@@ -10926,13 +10926,13 @@
         <v>45050</v>
       </c>
       <c r="G105">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="H105" s="2">
         <v>45234</v>
       </c>
       <c r="I105">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="J105" t="inlineStr">
         <is>
@@ -11029,13 +11029,13 @@
         <v>45085</v>
       </c>
       <c r="G106">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="H106" s="2">
         <v>45268</v>
       </c>
       <c r="I106">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="J106" t="inlineStr">
         <is>
@@ -11132,13 +11132,13 @@
         <v>45093</v>
       </c>
       <c r="G107">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="H107" s="2">
         <v>45185</v>
       </c>
       <c r="I107">
-        <v>-1</v>
+        <v>-2</v>
       </c>
       <c r="J107" t="inlineStr">
         <is>
@@ -11230,13 +11230,13 @@
         <v>45093</v>
       </c>
       <c r="G108">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="H108" s="2">
         <v>45185</v>
       </c>
       <c r="I108">
-        <v>-1</v>
+        <v>-2</v>
       </c>
       <c r="J108" t="inlineStr">
         <is>
@@ -11328,13 +11328,13 @@
         <v>45093</v>
       </c>
       <c r="G109">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="H109" s="2">
         <v>45185</v>
       </c>
       <c r="I109">
-        <v>-1</v>
+        <v>-2</v>
       </c>
       <c r="J109" t="inlineStr">
         <is>
@@ -11431,13 +11431,13 @@
         <v>45148</v>
       </c>
       <c r="G110">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="H110" s="2">
         <v>45240</v>
       </c>
       <c r="I110">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="J110" t="inlineStr">
         <is>
@@ -11534,13 +11534,13 @@
         <v>45119</v>
       </c>
       <c r="G111">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="H111" s="2">
         <v>45211</v>
       </c>
       <c r="I111">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="J111" t="inlineStr">
         <is>
@@ -11637,13 +11637,13 @@
         <v>45172</v>
       </c>
       <c r="G112">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="H112" s="2">
         <v>45263</v>
       </c>
       <c r="I112">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="J112" t="inlineStr">
         <is>
@@ -11740,13 +11740,13 @@
         <v>45023</v>
       </c>
       <c r="G113">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="H113" s="2">
         <v>45206</v>
       </c>
       <c r="I113">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="J113" t="inlineStr">
         <is>
@@ -11843,13 +11843,13 @@
         <v>45111</v>
       </c>
       <c r="G114">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="H114" s="2">
         <v>45203</v>
       </c>
       <c r="I114">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="J114" t="inlineStr">
         <is>
@@ -11946,7 +11946,7 @@
         <v>45218</v>
       </c>
       <c r="I115">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="J115" t="inlineStr">
         <is>
@@ -12043,13 +12043,13 @@
         <v>45161</v>
       </c>
       <c r="G116">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="H116" s="2">
         <v>45253</v>
       </c>
       <c r="I116">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="J116" t="inlineStr">
         <is>
@@ -12146,13 +12146,13 @@
         <v>45115</v>
       </c>
       <c r="G117">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="H117" s="2">
         <v>45299</v>
       </c>
       <c r="I117">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="J117" t="inlineStr">
         <is>
@@ -12244,13 +12244,13 @@
         <v>45094</v>
       </c>
       <c r="G118">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="H118" s="2">
         <v>45277</v>
       </c>
       <c r="I118">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="J118" t="inlineStr">
         <is>
@@ -12347,13 +12347,13 @@
         <v>45104</v>
       </c>
       <c r="G119">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="H119" s="2">
         <v>45287</v>
       </c>
       <c r="I119">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="J119" t="inlineStr">
         <is>
@@ -12450,13 +12450,13 @@
         <v>45104</v>
       </c>
       <c r="G120">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="H120" s="2">
         <v>45287</v>
       </c>
       <c r="I120">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="J120" t="inlineStr">
         <is>
@@ -12553,13 +12553,13 @@
         <v>45104</v>
       </c>
       <c r="G121">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="H121" s="2">
         <v>45287</v>
       </c>
       <c r="I121">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="J121" t="inlineStr">
         <is>
@@ -12656,13 +12656,13 @@
         <v>45104</v>
       </c>
       <c r="G122">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="H122" s="2">
         <v>45287</v>
       </c>
       <c r="I122">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="J122" t="inlineStr">
         <is>
@@ -12759,13 +12759,13 @@
         <v>45107</v>
       </c>
       <c r="G123">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="H123" s="2">
         <v>45199</v>
       </c>
       <c r="I123">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="J123" t="inlineStr">
         <is>
@@ -12862,13 +12862,13 @@
         <v>45013</v>
       </c>
       <c r="G124">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="H124" s="2">
         <v>45197</v>
       </c>
       <c r="I124">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="J124" t="inlineStr">
         <is>
@@ -12965,13 +12965,13 @@
         <v>45121</v>
       </c>
       <c r="G125">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="H125" s="2">
         <v>45213</v>
       </c>
       <c r="I125">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="J125" t="inlineStr">
         <is>
@@ -13068,13 +13068,13 @@
         <v>45134</v>
       </c>
       <c r="G126">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="H126" s="2">
         <v>45226</v>
       </c>
       <c r="I126">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="J126" t="inlineStr">
         <is>
@@ -13171,7 +13171,7 @@
         <v>45212</v>
       </c>
       <c r="I127">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="J127" t="inlineStr">
         <is>
@@ -13268,13 +13268,13 @@
         <v>45126</v>
       </c>
       <c r="G128">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="H128" s="2">
         <v>45218</v>
       </c>
       <c r="I128">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="J128" t="inlineStr">
         <is>
@@ -13366,13 +13366,13 @@
         <v>45158</v>
       </c>
       <c r="G129">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="H129" s="2">
         <v>45250</v>
       </c>
       <c r="I129">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="J129" t="inlineStr">
         <is>
@@ -13469,13 +13469,13 @@
         <v>45171</v>
       </c>
       <c r="G130">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H130" s="2">
         <v>45262</v>
       </c>
       <c r="I130">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="J130" t="inlineStr">
         <is>
@@ -13572,13 +13572,13 @@
         <v>45111</v>
       </c>
       <c r="G131">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="H131" s="2">
         <v>45203</v>
       </c>
       <c r="I131">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="J131" t="inlineStr">
         <is>
@@ -13675,13 +13675,13 @@
         <v>45144</v>
       </c>
       <c r="G132">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="H132" s="2">
         <v>45236</v>
       </c>
       <c r="I132">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="J132" t="inlineStr">
         <is>
@@ -13778,13 +13778,13 @@
         <v>45156</v>
       </c>
       <c r="G133">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="H133" s="2">
         <v>45248</v>
       </c>
       <c r="I133">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="J133" t="inlineStr">
         <is>
@@ -13876,13 +13876,13 @@
         <v>45146</v>
       </c>
       <c r="G134">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="H134" s="2">
         <v>45238</v>
       </c>
       <c r="I134">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="J134" t="inlineStr">
         <is>
@@ -13979,13 +13979,13 @@
         <v>45140</v>
       </c>
       <c r="G135">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="H135" s="2">
         <v>45232</v>
       </c>
       <c r="I135">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="J135" t="inlineStr">
         <is>
@@ -14082,13 +14082,13 @@
         <v>45104</v>
       </c>
       <c r="G136">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="H136" s="2">
         <v>45196</v>
       </c>
       <c r="I136">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="J136" t="inlineStr">
         <is>
@@ -14185,13 +14185,13 @@
         <v>45105</v>
       </c>
       <c r="G137">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="H137" s="2">
         <v>45197</v>
       </c>
       <c r="I137">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="J137" t="inlineStr">
         <is>
@@ -14288,13 +14288,13 @@
         <v>45179</v>
       </c>
       <c r="G138">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="H138" s="2">
         <v>45270</v>
       </c>
       <c r="I138">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="J138" t="inlineStr">
         <is>
@@ -14386,13 +14386,13 @@
         <v>45105</v>
       </c>
       <c r="G139">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="H139" s="2">
         <v>45197</v>
       </c>
       <c r="I139">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="J139" t="inlineStr">
         <is>
@@ -14489,13 +14489,13 @@
         <v>45182</v>
       </c>
       <c r="G140">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="H140" s="2">
         <v>45273</v>
       </c>
       <c r="I140">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="J140" t="inlineStr">
         <is>
@@ -14592,13 +14592,13 @@
         <v>45116</v>
       </c>
       <c r="G141">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="H141" s="2">
         <v>45208</v>
       </c>
       <c r="I141">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="J141" t="inlineStr">
         <is>
@@ -14690,13 +14690,13 @@
         <v>45150</v>
       </c>
       <c r="G142">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="H142" s="2">
         <v>45242</v>
       </c>
       <c r="I142">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="J142" t="inlineStr">
         <is>
@@ -14793,7 +14793,7 @@
         <v>45238</v>
       </c>
       <c r="I143">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="J143" t="inlineStr">
         <is>
@@ -14890,13 +14890,13 @@
         <v>45171</v>
       </c>
       <c r="G144">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H144" s="2">
         <v>45262</v>
       </c>
       <c r="I144">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="J144" t="inlineStr">
         <is>
@@ -14993,13 +14993,13 @@
         <v>45102</v>
       </c>
       <c r="G145">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="H145" s="2">
         <v>45194</v>
       </c>
       <c r="I145">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="J145" t="inlineStr">
         <is>
@@ -15086,13 +15086,13 @@
         <v>45119</v>
       </c>
       <c r="G146">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="H146" s="2">
         <v>45211</v>
       </c>
       <c r="I146">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="J146" t="inlineStr">
         <is>
@@ -15189,13 +15189,13 @@
         <v>45165</v>
       </c>
       <c r="G147">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="H147" s="2">
         <v>45257</v>
       </c>
       <c r="I147">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="J147" t="inlineStr">
         <is>
@@ -15292,13 +15292,13 @@
         <v>45166</v>
       </c>
       <c r="G148">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="H148" s="2">
         <v>45258</v>
       </c>
       <c r="I148">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="J148" t="inlineStr">
         <is>
@@ -15395,13 +15395,13 @@
         <v>45093</v>
       </c>
       <c r="G149">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="H149" s="2">
         <v>45185</v>
       </c>
       <c r="I149">
-        <v>-1</v>
+        <v>-2</v>
       </c>
       <c r="J149" t="inlineStr">
         <is>
@@ -15498,13 +15498,13 @@
         <v>45035</v>
       </c>
       <c r="G150">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="H150" s="2">
         <v>45218</v>
       </c>
       <c r="I150">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="J150" t="inlineStr">
         <is>
@@ -15601,13 +15601,13 @@
         <v>45174</v>
       </c>
       <c r="G151">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="H151" s="2">
         <v>45356</v>
       </c>
       <c r="I151">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="J151" t="inlineStr">
         <is>
@@ -15704,13 +15704,13 @@
         <v>45089</v>
       </c>
       <c r="G152">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="H152" s="2">
         <v>45272</v>
       </c>
       <c r="I152">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="J152" t="inlineStr">
         <is>
@@ -15807,13 +15807,13 @@
         <v>45124</v>
       </c>
       <c r="G153">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="H153" s="2">
         <v>45308</v>
       </c>
       <c r="I153">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="J153" t="inlineStr">
         <is>
@@ -15910,13 +15910,13 @@
         <v>45124</v>
       </c>
       <c r="G154">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="H154" s="2">
         <v>45308</v>
       </c>
       <c r="I154">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="J154" t="inlineStr">
         <is>
@@ -16013,13 +16013,13 @@
         <v>45026</v>
       </c>
       <c r="G155">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="H155" s="2">
         <v>45209</v>
       </c>
       <c r="I155">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="J155" t="inlineStr">
         <is>
@@ -16116,13 +16116,13 @@
         <v>45026</v>
       </c>
       <c r="G156">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="H156" s="2">
         <v>45209</v>
       </c>
       <c r="I156">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="J156" t="inlineStr">
         <is>
@@ -16219,13 +16219,13 @@
         <v>45026</v>
       </c>
       <c r="G157">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="H157" s="2">
         <v>45209</v>
       </c>
       <c r="I157">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="J157" t="inlineStr">
         <is>
@@ -16322,13 +16322,13 @@
         <v>45026</v>
       </c>
       <c r="G158">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="H158" s="2">
         <v>45209</v>
       </c>
       <c r="I158">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="J158" t="inlineStr">
         <is>
@@ -16425,13 +16425,13 @@
         <v>45156</v>
       </c>
       <c r="G159">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="H159" s="2">
         <v>45247</v>
       </c>
       <c r="I159">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="J159" t="inlineStr">
         <is>
@@ -16528,13 +16528,13 @@
         <v>45153</v>
       </c>
       <c r="G160">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="H160" s="2">
         <v>45245</v>
       </c>
       <c r="I160">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="J160" t="inlineStr">
         <is>
@@ -16631,13 +16631,13 @@
         <v>45135</v>
       </c>
       <c r="G161">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="H161" s="2">
         <v>45319</v>
       </c>
       <c r="I161">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="J161" t="inlineStr">
         <is>
@@ -16734,13 +16734,13 @@
         <v>45091</v>
       </c>
       <c r="G162">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="H162" s="2">
         <v>45274</v>
       </c>
       <c r="I162">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="J162" t="inlineStr">
         <is>
@@ -16832,13 +16832,13 @@
         <v>45091</v>
       </c>
       <c r="G163">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="H163" s="2">
         <v>45274</v>
       </c>
       <c r="I163">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="J163" t="inlineStr">
         <is>
@@ -16930,13 +16930,13 @@
         <v>45138</v>
       </c>
       <c r="G164">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="H164" s="2">
         <v>45322</v>
       </c>
       <c r="I164">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="J164" t="inlineStr">
         <is>
@@ -17033,13 +17033,13 @@
         <v>45138</v>
       </c>
       <c r="G165">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="H165" s="2">
         <v>45322</v>
       </c>
       <c r="I165">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="J165" t="inlineStr">
         <is>
@@ -17136,13 +17136,13 @@
         <v>45085</v>
       </c>
       <c r="G166">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="H166" s="2">
         <v>45268</v>
       </c>
       <c r="I166">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="J166" t="inlineStr">
         <is>
@@ -17239,13 +17239,13 @@
         <v>45085</v>
       </c>
       <c r="G167">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="H167" s="2">
         <v>45268</v>
       </c>
       <c r="I167">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="J167" t="inlineStr">
         <is>
@@ -17342,7 +17342,7 @@
         <v>45326</v>
       </c>
       <c r="I168">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="J168" t="inlineStr">
         <is>
@@ -17439,13 +17439,13 @@
         <v>45173</v>
       </c>
       <c r="G169">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="H169" s="2">
         <v>45355</v>
       </c>
       <c r="I169">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="J169" t="inlineStr">
         <is>
@@ -17542,13 +17542,13 @@
         <v>45056</v>
       </c>
       <c r="G170">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="H170" s="2">
         <v>45240</v>
       </c>
       <c r="I170">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="J170" t="inlineStr">
         <is>
@@ -17645,7 +17645,7 @@
         <v>45238</v>
       </c>
       <c r="I171">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="J171" t="inlineStr">
         <is>
@@ -17742,13 +17742,13 @@
         <v>45141</v>
       </c>
       <c r="G172">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="H172" s="2">
         <v>45325</v>
       </c>
       <c r="I172">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="J172" t="inlineStr">
         <is>
@@ -17845,13 +17845,13 @@
         <v>45037</v>
       </c>
       <c r="G173">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="H173" s="2">
         <v>45220</v>
       </c>
       <c r="I173">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="J173" t="inlineStr">
         <is>
@@ -17948,13 +17948,13 @@
         <v>45171</v>
       </c>
       <c r="G174">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H174" s="2">
         <v>45262</v>
       </c>
       <c r="I174">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="J174" t="inlineStr">
         <is>
@@ -18051,13 +18051,13 @@
         <v>45105</v>
       </c>
       <c r="G175">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="H175" s="2">
         <v>45197</v>
       </c>
       <c r="I175">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="J175" t="inlineStr">
         <is>
@@ -18154,13 +18154,13 @@
         <v>45162</v>
       </c>
       <c r="G176">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="H176" s="2">
         <v>45254</v>
       </c>
       <c r="I176">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="J176" t="inlineStr">
         <is>
@@ -18257,13 +18257,13 @@
         <v>45061</v>
       </c>
       <c r="G177">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="H177" s="2">
         <v>45245</v>
       </c>
       <c r="I177">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="J177" t="inlineStr">
         <is>
@@ -18360,13 +18360,13 @@
         <v>45120</v>
       </c>
       <c r="G178">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="H178" s="2">
         <v>45212</v>
       </c>
       <c r="I178">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="J178" t="inlineStr">
         <is>
@@ -18463,7 +18463,7 @@
         <v>45191</v>
       </c>
       <c r="I179">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="J179" t="inlineStr">
         <is>
@@ -18560,13 +18560,13 @@
         <v>45088</v>
       </c>
       <c r="G180">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="H180" s="2">
         <v>45271</v>
       </c>
       <c r="I180">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="J180" t="inlineStr">
         <is>
@@ -18663,13 +18663,13 @@
         <v>45100</v>
       </c>
       <c r="G181">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="H181" s="2">
         <v>45192</v>
       </c>
       <c r="I181">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="J181" t="inlineStr">
         <is>
@@ -18756,13 +18756,13 @@
         <v>45131</v>
       </c>
       <c r="G182">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="H182" s="2">
         <v>45223</v>
       </c>
       <c r="I182">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="J182" t="inlineStr">
         <is>
@@ -18854,13 +18854,13 @@
         <v>45136</v>
       </c>
       <c r="G183">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="H183" s="2">
         <v>45228</v>
       </c>
       <c r="I183">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="J183" t="inlineStr">
         <is>
@@ -18952,13 +18952,13 @@
         <v>45150</v>
       </c>
       <c r="G184">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="H184" s="2">
         <v>45242</v>
       </c>
       <c r="I184">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="J184" t="inlineStr">
         <is>
@@ -19050,13 +19050,13 @@
         <v>45118</v>
       </c>
       <c r="G185">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="H185" s="2">
         <v>45210</v>
       </c>
       <c r="I185">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="J185" t="inlineStr">
         <is>
@@ -19148,13 +19148,13 @@
         <v>45129</v>
       </c>
       <c r="G186">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="H186" s="2">
         <v>45221</v>
       </c>
       <c r="I186">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="J186" t="inlineStr">
         <is>
@@ -19246,13 +19246,13 @@
         <v>45097</v>
       </c>
       <c r="G187">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="H187" s="2">
         <v>45189</v>
       </c>
       <c r="I187">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="J187" t="inlineStr">
         <is>
@@ -19339,13 +19339,13 @@
         <v>45101</v>
       </c>
       <c r="G188">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="H188" s="2">
         <v>45193</v>
       </c>
       <c r="I188">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="J188" t="inlineStr">
         <is>
@@ -19432,13 +19432,13 @@
         <v>45165</v>
       </c>
       <c r="G189">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="H189" s="2">
         <v>45257</v>
       </c>
       <c r="I189">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="J189" t="inlineStr">
         <is>
@@ -19530,7 +19530,7 @@
         <v>45202</v>
       </c>
       <c r="I190">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="J190" t="inlineStr">
         <is>
@@ -19627,13 +19627,13 @@
         <v>45081</v>
       </c>
       <c r="G191">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="H191" s="2">
         <v>45264</v>
       </c>
       <c r="I191">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="J191" t="inlineStr">
         <is>
@@ -19730,13 +19730,13 @@
         <v>45081</v>
       </c>
       <c r="G192">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="H192" s="2">
         <v>45264</v>
       </c>
       <c r="I192">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="J192" t="inlineStr">
         <is>
@@ -19833,7 +19833,7 @@
         <v>45319</v>
       </c>
       <c r="I193">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="J193" t="inlineStr">
         <is>
@@ -19930,7 +19930,7 @@
         <v>45319</v>
       </c>
       <c r="I194">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="J194" t="inlineStr">
         <is>
@@ -20022,13 +20022,13 @@
         <v>45046</v>
       </c>
       <c r="G195">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="H195" s="2">
         <v>45230</v>
       </c>
       <c r="I195">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="J195" t="inlineStr">
         <is>
@@ -20125,13 +20125,13 @@
         <v>45046</v>
       </c>
       <c r="G196">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="H196" s="2">
         <v>45230</v>
       </c>
       <c r="I196">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="J196" t="inlineStr">
         <is>
@@ -20228,13 +20228,13 @@
         <v>45031</v>
       </c>
       <c r="G197">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="H197" s="2">
         <v>45214</v>
       </c>
       <c r="I197">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="J197" t="inlineStr">
         <is>
@@ -20331,13 +20331,13 @@
         <v>45031</v>
       </c>
       <c r="G198">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="H198" s="2">
         <v>45214</v>
       </c>
       <c r="I198">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="J198" t="inlineStr">
         <is>
@@ -20434,13 +20434,13 @@
         <v>45031</v>
       </c>
       <c r="G199">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="H199" s="2">
         <v>45214</v>
       </c>
       <c r="I199">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="J199" t="inlineStr">
         <is>
@@ -20537,13 +20537,13 @@
         <v>45031</v>
       </c>
       <c r="G200">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="H200" s="2">
         <v>45214</v>
       </c>
       <c r="I200">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="J200" t="inlineStr">
         <is>
@@ -20640,13 +20640,13 @@
         <v>45067</v>
       </c>
       <c r="G201">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="H201" s="2">
         <v>45251</v>
       </c>
       <c r="I201">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="J201" t="inlineStr">
         <is>
@@ -20743,13 +20743,13 @@
         <v>45067</v>
       </c>
       <c r="G202">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="H202" s="2">
         <v>45251</v>
       </c>
       <c r="I202">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="J202" t="inlineStr">
         <is>
@@ -20846,13 +20846,13 @@
         <v>45067</v>
       </c>
       <c r="G203">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="H203" s="2">
         <v>45251</v>
       </c>
       <c r="I203">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="J203" t="inlineStr">
         <is>
@@ -20949,13 +20949,13 @@
         <v>45067</v>
       </c>
       <c r="G204">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="H204" s="2">
         <v>45251</v>
       </c>
       <c r="I204">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="J204" t="inlineStr">
         <is>
@@ -21052,13 +21052,13 @@
         <v>45178</v>
       </c>
       <c r="G205">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="H205" s="2">
         <v>45269</v>
       </c>
       <c r="I205">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="J205" t="inlineStr">
         <is>
@@ -21155,7 +21155,7 @@
         <v>45252</v>
       </c>
       <c r="I206">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="J206" t="inlineStr">
         <is>
@@ -21252,13 +21252,13 @@
         <v>45087</v>
       </c>
       <c r="G207">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="H207" s="2">
         <v>45270</v>
       </c>
       <c r="I207">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="J207" t="inlineStr">
         <is>
@@ -21355,13 +21355,13 @@
         <v>45099</v>
       </c>
       <c r="G208">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="H208" s="2">
         <v>45282</v>
       </c>
       <c r="I208">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="J208" t="inlineStr">
         <is>
@@ -21458,13 +21458,13 @@
         <v>45175</v>
       </c>
       <c r="G209">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="H209" s="2">
         <v>45356</v>
       </c>
       <c r="I209">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="J209" t="inlineStr">
         <is>
@@ -21561,13 +21561,13 @@
         <v>45175</v>
       </c>
       <c r="G210">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="H210" s="2">
         <v>45356</v>
       </c>
       <c r="I210">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="J210" t="inlineStr">
         <is>
@@ -21664,13 +21664,13 @@
         <v>45166</v>
       </c>
       <c r="G211">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="H211" s="2">
         <v>45350</v>
       </c>
       <c r="I211">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="J211" t="inlineStr">
         <is>
@@ -21767,13 +21767,13 @@
         <v>45166</v>
       </c>
       <c r="G212">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="H212" s="2">
         <v>45350</v>
       </c>
       <c r="I212">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="J212" t="inlineStr">
         <is>
@@ -21870,13 +21870,13 @@
         <v>45090</v>
       </c>
       <c r="G213">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="H213" s="2">
         <v>45273</v>
       </c>
       <c r="I213">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="J213" t="inlineStr">
         <is>
@@ -21973,13 +21973,13 @@
         <v>45106</v>
       </c>
       <c r="G214">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="H214" s="2">
         <v>45289</v>
       </c>
       <c r="I214">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="J214" t="inlineStr">
         <is>
@@ -22076,13 +22076,13 @@
         <v>45134</v>
       </c>
       <c r="G215">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="H215" s="2">
         <v>45226</v>
       </c>
       <c r="I215">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="J215" t="inlineStr">
         <is>
@@ -22179,13 +22179,13 @@
         <v>45132</v>
       </c>
       <c r="G216">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="H216" s="2">
         <v>45224</v>
       </c>
       <c r="I216">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="J216" t="inlineStr">
         <is>
@@ -22282,13 +22282,13 @@
         <v>45150</v>
       </c>
       <c r="G217">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="H217" s="2">
         <v>45242</v>
       </c>
       <c r="I217">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="J217" t="inlineStr">
         <is>
@@ -22385,13 +22385,13 @@
         <v>45095</v>
       </c>
       <c r="G218">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="H218" s="2">
         <v>45187</v>
       </c>
       <c r="I218">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J218" t="inlineStr">
         <is>
@@ -22483,13 +22483,13 @@
         <v>45182</v>
       </c>
       <c r="G219">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="H219" s="2">
         <v>45273</v>
       </c>
       <c r="I219">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="J219" t="inlineStr">
         <is>
@@ -22586,7 +22586,7 @@
         <v>45196</v>
       </c>
       <c r="I220">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="J220" t="inlineStr">
         <is>
@@ -22683,13 +22683,13 @@
         <v>45108</v>
       </c>
       <c r="G221">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="H221" s="2">
         <v>45200</v>
       </c>
       <c r="I221">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="J221" t="inlineStr">
         <is>
@@ -22786,13 +22786,13 @@
         <v>45135</v>
       </c>
       <c r="G222">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="H222" s="2">
         <v>45227</v>
       </c>
       <c r="I222">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="J222" t="inlineStr">
         <is>
@@ -22889,13 +22889,13 @@
         <v>45148</v>
       </c>
       <c r="G223">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="H223" s="2">
         <v>45240</v>
       </c>
       <c r="I223">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="J223" t="inlineStr">
         <is>
@@ -22987,13 +22987,13 @@
         <v>45100</v>
       </c>
       <c r="G224">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="H224" s="2">
         <v>45192</v>
       </c>
       <c r="I224">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="J224" t="inlineStr">
         <is>
@@ -23085,13 +23085,13 @@
         <v>45136</v>
       </c>
       <c r="G225">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="H225" s="2">
         <v>45320</v>
       </c>
       <c r="I225">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="J225" t="inlineStr">
         <is>
@@ -23188,13 +23188,13 @@
         <v>45136</v>
       </c>
       <c r="G226">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="H226" s="2">
         <v>45320</v>
       </c>
       <c r="I226">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="J226" t="inlineStr">
         <is>
@@ -23291,13 +23291,13 @@
         <v>45094</v>
       </c>
       <c r="G227">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="H227" s="2">
         <v>45277</v>
       </c>
       <c r="I227">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="J227" t="inlineStr">
         <is>
@@ -23394,13 +23394,13 @@
         <v>45081</v>
       </c>
       <c r="G228">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="H228" s="2">
         <v>45264</v>
       </c>
       <c r="I228">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="J228" t="inlineStr">
         <is>
@@ -23497,13 +23497,13 @@
         <v>45099</v>
       </c>
       <c r="G229">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="H229" s="2">
         <v>45282</v>
       </c>
       <c r="I229">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="J229" t="inlineStr">
         <is>
@@ -23600,13 +23600,13 @@
         <v>45018</v>
       </c>
       <c r="G230">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="H230" s="2">
         <v>45201</v>
       </c>
       <c r="I230">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="J230" t="inlineStr">
         <is>
@@ -23703,13 +23703,13 @@
         <v>45031</v>
       </c>
       <c r="G231">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="H231" s="2">
         <v>45214</v>
       </c>
       <c r="I231">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="J231" t="inlineStr">
         <is>
@@ -23806,7 +23806,7 @@
         <v>45294</v>
       </c>
       <c r="I232">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="J232" t="inlineStr">
         <is>
@@ -23903,13 +23903,13 @@
         <v>45079</v>
       </c>
       <c r="G233">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="H233" s="2">
         <v>45262</v>
       </c>
       <c r="I233">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="J233" t="inlineStr">
         <is>
@@ -24006,7 +24006,7 @@
         <v>45199</v>
       </c>
       <c r="I234">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="J234" t="inlineStr">
         <is>
@@ -24103,13 +24103,13 @@
         <v>45021</v>
       </c>
       <c r="G235">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="H235" s="2">
         <v>45204</v>
       </c>
       <c r="I235">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="J235" t="inlineStr">
         <is>
@@ -24206,13 +24206,13 @@
         <v>45021</v>
       </c>
       <c r="G236">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="H236" s="2">
         <v>45204</v>
       </c>
       <c r="I236">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="J236" t="inlineStr">
         <is>
@@ -24309,13 +24309,13 @@
         <v>45080</v>
       </c>
       <c r="G237">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="H237" s="2">
         <v>45263</v>
       </c>
       <c r="I237">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="J237" t="inlineStr">
         <is>
@@ -24412,13 +24412,13 @@
         <v>45046</v>
       </c>
       <c r="G238">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="H238" s="2">
         <v>45229</v>
       </c>
       <c r="I238">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="J238" t="inlineStr">
         <is>
@@ -24515,13 +24515,13 @@
         <v>45112</v>
       </c>
       <c r="G239">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="H239" s="2">
         <v>45204</v>
       </c>
       <c r="I239">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="J239" t="inlineStr">
         <is>
@@ -24609,13 +24609,13 @@
         <v>45112</v>
       </c>
       <c r="G240">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="H240" s="2">
         <v>45204</v>
       </c>
       <c r="I240">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="J240" t="inlineStr">
         <is>
@@ -24703,13 +24703,13 @@
         <v>45016</v>
       </c>
       <c r="G241">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="H241" s="2">
         <v>45199</v>
       </c>
       <c r="I241">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="J241" t="inlineStr">
         <is>
@@ -24806,13 +24806,13 @@
         <v>45070</v>
       </c>
       <c r="G242">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="H242" s="2">
         <v>45254</v>
       </c>
       <c r="I242">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="J242" t="inlineStr">
         <is>
@@ -24909,13 +24909,13 @@
         <v>45168</v>
       </c>
       <c r="G243">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="H243" s="2">
         <v>45260</v>
       </c>
       <c r="I243">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="J243" t="inlineStr">
         <is>
@@ -25012,13 +25012,13 @@
         <v>45027</v>
       </c>
       <c r="G244">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="H244" s="2">
         <v>45210</v>
       </c>
       <c r="I244">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="J244" t="inlineStr">
         <is>
@@ -25115,13 +25115,13 @@
         <v>45077</v>
       </c>
       <c r="G245">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="H245" s="2">
         <v>45260</v>
       </c>
       <c r="I245">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="J245" t="inlineStr">
         <is>
@@ -25218,13 +25218,13 @@
         <v>45100</v>
       </c>
       <c r="G246">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="H246" s="2">
         <v>45283</v>
       </c>
       <c r="I246">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="J246" t="inlineStr">
         <is>
@@ -25321,7 +25321,7 @@
         <v>45281</v>
       </c>
       <c r="I247">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="J247" t="inlineStr">
         <is>
@@ -25418,13 +25418,13 @@
         <v>45044</v>
       </c>
       <c r="G248">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="H248" s="2">
         <v>45227</v>
       </c>
       <c r="I248">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="J248" t="inlineStr">
         <is>
@@ -25521,13 +25521,13 @@
         <v>45101</v>
       </c>
       <c r="G249">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="H249" s="2">
         <v>45283</v>
       </c>
       <c r="I249">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="J249" t="inlineStr">
         <is>
@@ -25624,13 +25624,13 @@
         <v>45134</v>
       </c>
       <c r="G250">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="H250" s="2">
         <v>45226</v>
       </c>
       <c r="I250">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="J250" t="inlineStr">
         <is>
@@ -25727,13 +25727,13 @@
         <v>45158</v>
       </c>
       <c r="G251">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="H251" s="2">
         <v>45250</v>
       </c>
       <c r="I251">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="J251" t="inlineStr">
         <is>
@@ -25830,13 +25830,13 @@
         <v>45108</v>
       </c>
       <c r="G252">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="H252" s="2">
         <v>45200</v>
       </c>
       <c r="I252">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="J252" t="inlineStr">
         <is>
@@ -25933,7 +25933,7 @@
         <v>45317</v>
       </c>
       <c r="I253">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="J253" t="inlineStr">
         <is>
@@ -26030,13 +26030,13 @@
         <v>45039</v>
       </c>
       <c r="G254">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="H254" s="2">
         <v>45222</v>
       </c>
       <c r="I254">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="J254" t="inlineStr">
         <is>
@@ -26128,13 +26128,13 @@
         <v>45129</v>
       </c>
       <c r="G255">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="H255" s="2">
         <v>45221</v>
       </c>
       <c r="I255">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="J255" t="inlineStr">
         <is>
@@ -26231,13 +26231,13 @@
         <v>45157</v>
       </c>
       <c r="G256">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="H256" s="2">
         <v>45341</v>
       </c>
       <c r="I256">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="J256" t="inlineStr">
         <is>
@@ -26334,13 +26334,13 @@
         <v>45063</v>
       </c>
       <c r="G257">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="H257" s="2">
         <v>45247</v>
       </c>
       <c r="I257">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="J257" t="inlineStr">
         <is>
@@ -26437,7 +26437,7 @@
         <v>45254</v>
       </c>
       <c r="I258">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="J258" t="inlineStr">
         <is>
@@ -26534,7 +26534,7 @@
         <v>45486</v>
       </c>
       <c r="I259">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="J259" t="inlineStr">
         <is>
@@ -26626,13 +26626,13 @@
         <v>45073</v>
       </c>
       <c r="G260">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="H260" s="2">
         <v>45439</v>
       </c>
       <c r="I260">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="J260" t="inlineStr">
         <is>
@@ -26724,7 +26724,7 @@
         <v>45323</v>
       </c>
       <c r="I261">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="J261" t="inlineStr">
         <is>
@@ -26816,7 +26816,7 @@
         <v>45303</v>
       </c>
       <c r="I262">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="J262" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
GH ACTION Headlines Tue Sep 19 23:08:23 UTC 2023
</commit_message>
<xml_diff>
--- a/Data/obligacje_screener.xlsx
+++ b/Data/obligacje_screener.xlsx
@@ -512,7 +512,7 @@
         <v>45340</v>
       </c>
       <c r="I2">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="J2" t="inlineStr">
         <is>
@@ -600,13 +600,13 @@
         <v>45121</v>
       </c>
       <c r="G3">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="H3" s="2">
         <v>45305</v>
       </c>
       <c r="I3">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="J3" t="inlineStr">
         <is>
@@ -703,13 +703,13 @@
         <v>45039</v>
       </c>
       <c r="G4">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="H4" s="2">
         <v>45222</v>
       </c>
       <c r="I4">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="J4" t="inlineStr">
         <is>
@@ -806,13 +806,13 @@
         <v>45039</v>
       </c>
       <c r="G5">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="H5" s="2">
         <v>45222</v>
       </c>
       <c r="I5">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="J5" t="inlineStr">
         <is>
@@ -909,13 +909,13 @@
         <v>45129</v>
       </c>
       <c r="G6">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="H6" s="2">
         <v>45221</v>
       </c>
       <c r="I6">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="J6" t="inlineStr">
         <is>
@@ -1012,13 +1012,13 @@
         <v>45162</v>
       </c>
       <c r="G7">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="H7" s="2">
         <v>45254</v>
       </c>
       <c r="I7">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="J7" t="inlineStr">
         <is>
@@ -1110,13 +1110,13 @@
         <v>45156</v>
       </c>
       <c r="G8">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="H8" s="2">
         <v>45248</v>
       </c>
       <c r="I8">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="J8" t="inlineStr">
         <is>
@@ -1213,13 +1213,13 @@
         <v>45141</v>
       </c>
       <c r="G9">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="H9" s="2">
         <v>45233</v>
       </c>
       <c r="I9">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="J9" t="inlineStr">
         <is>
@@ -1316,13 +1316,13 @@
         <v>45062</v>
       </c>
       <c r="G10">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="H10" s="2">
         <v>45246</v>
       </c>
       <c r="I10">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="J10" t="inlineStr">
         <is>
@@ -1419,7 +1419,7 @@
         <v>45286</v>
       </c>
       <c r="I11">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="J11" t="inlineStr">
         <is>
@@ -1516,13 +1516,13 @@
         <v>45011</v>
       </c>
       <c r="G12">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="H12" s="2">
         <v>45195</v>
       </c>
       <c r="I12">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="J12" t="inlineStr">
         <is>
@@ -1614,13 +1614,13 @@
         <v>45036</v>
       </c>
       <c r="G13">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="H13" s="2">
         <v>45219</v>
       </c>
       <c r="I13">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="J13" t="inlineStr">
         <is>
@@ -1717,13 +1717,13 @@
         <v>45036</v>
       </c>
       <c r="G14">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="H14" s="2">
         <v>45219</v>
       </c>
       <c r="I14">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="J14" t="inlineStr">
         <is>
@@ -1820,13 +1820,13 @@
         <v>45106</v>
       </c>
       <c r="G15">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="H15" s="2">
         <v>45289</v>
       </c>
       <c r="I15">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="J15" t="inlineStr">
         <is>
@@ -1923,13 +1923,13 @@
         <v>45094</v>
       </c>
       <c r="G16">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="H16" s="2">
         <v>45186</v>
       </c>
       <c r="I16">
-        <v>-1</v>
+        <v>-2</v>
       </c>
       <c r="J16" t="inlineStr">
         <is>
@@ -2026,13 +2026,13 @@
         <v>45094</v>
       </c>
       <c r="G17">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="H17" s="2">
         <v>45186</v>
       </c>
       <c r="I17">
-        <v>-1</v>
+        <v>-2</v>
       </c>
       <c r="J17" t="inlineStr">
         <is>
@@ -2129,13 +2129,13 @@
         <v>45132</v>
       </c>
       <c r="G18">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="H18" s="2">
         <v>45224</v>
       </c>
       <c r="I18">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="J18" t="inlineStr">
         <is>
@@ -2232,13 +2232,13 @@
         <v>45137</v>
       </c>
       <c r="G19">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="H19" s="2">
         <v>45229</v>
       </c>
       <c r="I19">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="J19" t="inlineStr">
         <is>
@@ -2330,13 +2330,13 @@
         <v>45183</v>
       </c>
       <c r="G20">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="H20" s="2">
         <v>45274</v>
       </c>
       <c r="I20">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="J20" t="inlineStr">
         <is>
@@ -2433,13 +2433,13 @@
         <v>45093</v>
       </c>
       <c r="G21">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="H21" s="2">
         <v>45187</v>
       </c>
       <c r="I21">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="J21" t="inlineStr">
         <is>
@@ -2536,13 +2536,13 @@
         <v>45096</v>
       </c>
       <c r="G22">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="H22" s="2">
         <v>45187</v>
       </c>
       <c r="I22">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="J22" t="inlineStr">
         <is>
@@ -2639,7 +2639,7 @@
         <v>45245</v>
       </c>
       <c r="I23">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="J23" t="inlineStr">
         <is>
@@ -2736,7 +2736,7 @@
         <v>45245</v>
       </c>
       <c r="I24">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="J24" t="inlineStr">
         <is>
@@ -2833,13 +2833,13 @@
         <v>45021</v>
       </c>
       <c r="G25">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="H25" s="2">
         <v>45204</v>
       </c>
       <c r="I25">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="J25" t="inlineStr">
         <is>
@@ -2936,13 +2936,13 @@
         <v>45160</v>
       </c>
       <c r="G26">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="H26" s="2">
         <v>45344</v>
       </c>
       <c r="I26">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="J26" t="inlineStr">
         <is>
@@ -3039,13 +3039,13 @@
         <v>45118</v>
       </c>
       <c r="G27">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="H27" s="2">
         <v>45302</v>
       </c>
       <c r="I27">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="J27" t="inlineStr">
         <is>
@@ -3142,13 +3142,13 @@
         <v>45085</v>
       </c>
       <c r="G28">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="H28" s="2">
         <v>45268</v>
       </c>
       <c r="I28">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="J28" t="inlineStr">
         <is>
@@ -3245,13 +3245,13 @@
         <v>45183</v>
       </c>
       <c r="G29">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="H29" s="2">
         <v>45274</v>
       </c>
       <c r="I29">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="J29" t="inlineStr">
         <is>
@@ -3348,7 +3348,7 @@
         <v>45224</v>
       </c>
       <c r="I30">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="J30" t="inlineStr">
         <is>
@@ -3445,13 +3445,13 @@
         <v>45153</v>
       </c>
       <c r="G31">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="H31" s="2">
         <v>45245</v>
       </c>
       <c r="I31">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="J31" t="inlineStr">
         <is>
@@ -3548,13 +3548,13 @@
         <v>45155</v>
       </c>
       <c r="G32">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="H32" s="2">
         <v>45247</v>
       </c>
       <c r="I32">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="J32" t="inlineStr">
         <is>
@@ -3651,7 +3651,7 @@
         <v>45255</v>
       </c>
       <c r="I33">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="J33" t="inlineStr">
         <is>
@@ -3739,13 +3739,13 @@
         <v>45176</v>
       </c>
       <c r="G34">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="H34" s="2">
         <v>45267</v>
       </c>
       <c r="I34">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="J34" t="inlineStr">
         <is>
@@ -3842,13 +3842,13 @@
         <v>45130</v>
       </c>
       <c r="G35">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="H35" s="2">
         <v>45222</v>
       </c>
       <c r="I35">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="J35" t="inlineStr">
         <is>
@@ -3940,13 +3940,13 @@
         <v>45115</v>
       </c>
       <c r="G36">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="H36" s="2">
         <v>45207</v>
       </c>
       <c r="I36">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="J36" t="inlineStr">
         <is>
@@ -4043,13 +4043,13 @@
         <v>45097</v>
       </c>
       <c r="G37">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="H37" s="2">
         <v>45189</v>
       </c>
       <c r="I37">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J37" t="inlineStr">
         <is>
@@ -4141,13 +4141,13 @@
         <v>45107</v>
       </c>
       <c r="G38">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="H38" s="2">
         <v>45290</v>
       </c>
       <c r="I38">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="J38" t="inlineStr">
         <is>
@@ -4244,13 +4244,13 @@
         <v>45063</v>
       </c>
       <c r="G39">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="H39" s="2">
         <v>45247</v>
       </c>
       <c r="I39">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="J39" t="inlineStr">
         <is>
@@ -4347,13 +4347,13 @@
         <v>45177</v>
       </c>
       <c r="G40">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="H40" s="2">
         <v>45359</v>
       </c>
       <c r="I40">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="J40" t="inlineStr">
         <is>
@@ -4450,13 +4450,13 @@
         <v>45107</v>
       </c>
       <c r="G41">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="H41" s="2">
         <v>45290</v>
       </c>
       <c r="I41">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="J41" t="inlineStr">
         <is>
@@ -4553,7 +4553,7 @@
         <v>45265</v>
       </c>
       <c r="I42">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="J42" t="inlineStr">
         <is>
@@ -4650,13 +4650,13 @@
         <v>45098</v>
       </c>
       <c r="G43">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="H43" s="2">
         <v>45281</v>
       </c>
       <c r="I43">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="J43" t="inlineStr">
         <is>
@@ -4753,13 +4753,13 @@
         <v>45099</v>
       </c>
       <c r="G44">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="H44" s="2">
         <v>45282</v>
       </c>
       <c r="I44">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="J44" t="inlineStr">
         <is>
@@ -4856,13 +4856,13 @@
         <v>45106</v>
       </c>
       <c r="G45">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="H45" s="2">
         <v>45289</v>
       </c>
       <c r="I45">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="J45" t="inlineStr">
         <is>
@@ -4959,13 +4959,13 @@
         <v>45106</v>
       </c>
       <c r="G46">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="H46" s="2">
         <v>45289</v>
       </c>
       <c r="I46">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="J46" t="inlineStr">
         <is>
@@ -5062,13 +5062,13 @@
         <v>45120</v>
       </c>
       <c r="G47">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="H47" s="2">
         <v>45304</v>
       </c>
       <c r="I47">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="J47" t="inlineStr">
         <is>
@@ -5165,13 +5165,13 @@
         <v>45118</v>
       </c>
       <c r="G48">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="H48" s="2">
         <v>45302</v>
       </c>
       <c r="I48">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="J48" t="inlineStr">
         <is>
@@ -5268,13 +5268,13 @@
         <v>45152</v>
       </c>
       <c r="G49">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="H49" s="2">
         <v>45336</v>
       </c>
       <c r="I49">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="J49" t="inlineStr">
         <is>
@@ -5371,13 +5371,13 @@
         <v>45042</v>
       </c>
       <c r="G50">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="H50" s="2">
         <v>45225</v>
       </c>
       <c r="I50">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="J50" t="inlineStr">
         <is>
@@ -5474,13 +5474,13 @@
         <v>45122</v>
       </c>
       <c r="G51">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="H51" s="2">
         <v>45306</v>
       </c>
       <c r="I51">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="J51" t="inlineStr">
         <is>
@@ -5577,13 +5577,13 @@
         <v>45139</v>
       </c>
       <c r="G52">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="H52" s="2">
         <v>45323</v>
       </c>
       <c r="I52">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="J52" t="inlineStr">
         <is>
@@ -5671,13 +5671,13 @@
         <v>45099</v>
       </c>
       <c r="G53">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="H53" s="2">
         <v>45282</v>
       </c>
       <c r="I53">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="J53" t="inlineStr">
         <is>
@@ -5774,7 +5774,7 @@
         <v>45196</v>
       </c>
       <c r="I54">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="J54" t="inlineStr">
         <is>
@@ -5871,13 +5871,13 @@
         <v>45044</v>
       </c>
       <c r="G55">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="H55" s="2">
         <v>45227</v>
       </c>
       <c r="I55">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="J55" t="inlineStr">
         <is>
@@ -5974,13 +5974,13 @@
         <v>45151</v>
       </c>
       <c r="G56">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="H56" s="2">
         <v>45243</v>
       </c>
       <c r="I56">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="J56" t="inlineStr">
         <is>
@@ -6072,7 +6072,7 @@
         <v>45196</v>
       </c>
       <c r="I57">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="J57" t="inlineStr">
         <is>
@@ -6169,13 +6169,13 @@
         <v>45069</v>
       </c>
       <c r="G58">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="H58" s="2">
         <v>45253</v>
       </c>
       <c r="I58">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="J58" t="inlineStr">
         <is>
@@ -6272,13 +6272,13 @@
         <v>45099</v>
       </c>
       <c r="G59">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="H59" s="2">
         <v>45191</v>
       </c>
       <c r="I59">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="J59" t="inlineStr">
         <is>
@@ -6370,13 +6370,13 @@
         <v>45113</v>
       </c>
       <c r="G60">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="H60" s="2">
         <v>45205</v>
       </c>
       <c r="I60">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="J60" t="inlineStr">
         <is>
@@ -6473,13 +6473,13 @@
         <v>45127</v>
       </c>
       <c r="G61">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="H61" s="2">
         <v>45219</v>
       </c>
       <c r="I61">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="J61" t="inlineStr">
         <is>
@@ -6576,13 +6576,13 @@
         <v>45058</v>
       </c>
       <c r="G62">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="H62" s="2">
         <v>45242</v>
       </c>
       <c r="I62">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="J62" t="inlineStr">
         <is>
@@ -6679,13 +6679,13 @@
         <v>45010</v>
       </c>
       <c r="G63">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="H63" s="2">
         <v>45194</v>
       </c>
       <c r="I63">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="J63" t="inlineStr">
         <is>
@@ -6777,13 +6777,13 @@
         <v>45025</v>
       </c>
       <c r="G64">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="H64" s="2">
         <v>45208</v>
       </c>
       <c r="I64">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="J64" t="inlineStr">
         <is>
@@ -6880,13 +6880,13 @@
         <v>45025</v>
       </c>
       <c r="G65">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="H65" s="2">
         <v>45208</v>
       </c>
       <c r="I65">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="J65" t="inlineStr">
         <is>
@@ -6983,13 +6983,13 @@
         <v>45089</v>
       </c>
       <c r="G66">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="H66" s="2">
         <v>45272</v>
       </c>
       <c r="I66">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="J66" t="inlineStr">
         <is>
@@ -7086,13 +7086,13 @@
         <v>45178</v>
       </c>
       <c r="G67">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="H67" s="2">
         <v>45269</v>
       </c>
       <c r="I67">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="J67" t="inlineStr">
         <is>
@@ -7184,13 +7184,13 @@
         <v>45104</v>
       </c>
       <c r="G68">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="H68" s="2">
         <v>45196</v>
       </c>
       <c r="I68">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="J68" t="inlineStr">
         <is>
@@ -7287,13 +7287,13 @@
         <v>45149</v>
       </c>
       <c r="G69">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="H69" s="2">
         <v>45241</v>
       </c>
       <c r="I69">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="J69" t="inlineStr">
         <is>
@@ -7390,7 +7390,7 @@
         <v>45205</v>
       </c>
       <c r="I70">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="J70" t="inlineStr">
         <is>
@@ -7487,13 +7487,13 @@
         <v>45114</v>
       </c>
       <c r="G71">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="H71" s="2">
         <v>45205</v>
       </c>
       <c r="I71">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="J71" t="inlineStr">
         <is>
@@ -7590,13 +7590,13 @@
         <v>45115</v>
       </c>
       <c r="G72">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="H72" s="2">
         <v>45207</v>
       </c>
       <c r="I72">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="J72" t="inlineStr">
         <is>
@@ -7693,13 +7693,13 @@
         <v>45097</v>
       </c>
       <c r="G73">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="H73" s="2">
         <v>45189</v>
       </c>
       <c r="I73">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J73" t="inlineStr">
         <is>
@@ -7791,13 +7791,13 @@
         <v>45038</v>
       </c>
       <c r="G74">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="H74" s="2">
         <v>45221</v>
       </c>
       <c r="I74">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="J74" t="inlineStr">
         <is>
@@ -7889,13 +7889,13 @@
         <v>45117</v>
       </c>
       <c r="G75">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="H75" s="2">
         <v>45301</v>
       </c>
       <c r="I75">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="J75" t="inlineStr">
         <is>
@@ -7992,13 +7992,13 @@
         <v>45160</v>
       </c>
       <c r="G76">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="H76" s="2">
         <v>45344</v>
       </c>
       <c r="I76">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="J76" t="inlineStr">
         <is>
@@ -8095,13 +8095,13 @@
         <v>45002</v>
       </c>
       <c r="G77">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="H77" s="2">
         <v>45186</v>
       </c>
       <c r="I77">
-        <v>-1</v>
+        <v>-2</v>
       </c>
       <c r="J77" t="inlineStr">
         <is>
@@ -8198,13 +8198,13 @@
         <v>45043</v>
       </c>
       <c r="G78">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="H78" s="2">
         <v>45226</v>
       </c>
       <c r="I78">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="J78" t="inlineStr">
         <is>
@@ -8301,13 +8301,13 @@
         <v>45079</v>
       </c>
       <c r="G79">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="H79" s="2">
         <v>45262</v>
       </c>
       <c r="I79">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="J79" t="inlineStr">
         <is>
@@ -8404,7 +8404,7 @@
         <v>45254</v>
       </c>
       <c r="I80">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="J80" t="inlineStr">
         <is>
@@ -8501,13 +8501,13 @@
         <v>45104</v>
       </c>
       <c r="G81">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="H81" s="2">
         <v>45287</v>
       </c>
       <c r="I81">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="J81" t="inlineStr">
         <is>
@@ -8604,7 +8604,7 @@
         <v>45288</v>
       </c>
       <c r="I82">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="J82" t="inlineStr">
         <is>
@@ -8696,13 +8696,13 @@
         <v>45175</v>
       </c>
       <c r="G83">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="H83" s="2">
         <v>45357</v>
       </c>
       <c r="I83">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="J83" t="inlineStr">
         <is>
@@ -8799,13 +8799,13 @@
         <v>45054</v>
       </c>
       <c r="G84">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="H84" s="2">
         <v>45238</v>
       </c>
       <c r="I84">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="J84" t="inlineStr">
         <is>
@@ -8902,13 +8902,13 @@
         <v>45056</v>
       </c>
       <c r="G85">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="H85" s="2">
         <v>45240</v>
       </c>
       <c r="I85">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="J85" t="inlineStr">
         <is>
@@ -9005,13 +9005,13 @@
         <v>45085</v>
       </c>
       <c r="G86">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="H86" s="2">
         <v>45268</v>
       </c>
       <c r="I86">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="J86" t="inlineStr">
         <is>
@@ -9108,7 +9108,7 @@
         <v>45194</v>
       </c>
       <c r="I87">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="J87" t="inlineStr">
         <is>
@@ -9195,13 +9195,13 @@
         <v>45103</v>
       </c>
       <c r="G88">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="H88" s="2">
         <v>45286</v>
       </c>
       <c r="I88">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="J88" t="inlineStr">
         <is>
@@ -9298,13 +9298,13 @@
         <v>45103</v>
       </c>
       <c r="G89">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="H89" s="2">
         <v>45286</v>
       </c>
       <c r="I89">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="J89" t="inlineStr">
         <is>
@@ -9401,13 +9401,13 @@
         <v>45008</v>
       </c>
       <c r="G90">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="H90" s="2">
         <v>45192</v>
       </c>
       <c r="I90">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="J90" t="inlineStr">
         <is>
@@ -9499,13 +9499,13 @@
         <v>45100</v>
       </c>
       <c r="G91">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="H91" s="2">
         <v>45287</v>
       </c>
       <c r="I91">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="J91" t="inlineStr">
         <is>
@@ -9602,13 +9602,13 @@
         <v>45003</v>
       </c>
       <c r="G92">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="H92" s="2">
         <v>45187</v>
       </c>
       <c r="I92">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="J92" t="inlineStr">
         <is>
@@ -9705,13 +9705,13 @@
         <v>45104</v>
       </c>
       <c r="G93">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="H93" s="2">
         <v>45287</v>
       </c>
       <c r="I93">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="J93" t="inlineStr">
         <is>
@@ -9808,13 +9808,13 @@
         <v>45104</v>
       </c>
       <c r="G94">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="H94" s="2">
         <v>45287</v>
       </c>
       <c r="I94">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="J94" t="inlineStr">
         <is>
@@ -9911,13 +9911,13 @@
         <v>45049</v>
       </c>
       <c r="G95">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="H95" s="2">
         <v>45233</v>
       </c>
       <c r="I95">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="J95" t="inlineStr">
         <is>
@@ -10014,13 +10014,13 @@
         <v>45122</v>
       </c>
       <c r="G96">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="H96" s="2">
         <v>45306</v>
       </c>
       <c r="I96">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="J96" t="inlineStr">
         <is>
@@ -10112,13 +10112,13 @@
         <v>45141</v>
       </c>
       <c r="G97">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="H97" s="2">
         <v>45325</v>
       </c>
       <c r="I97">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="J97" t="inlineStr">
         <is>
@@ -10215,13 +10215,13 @@
         <v>45010</v>
       </c>
       <c r="G98">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="H98" s="2">
         <v>45194</v>
       </c>
       <c r="I98">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="J98" t="inlineStr">
         <is>
@@ -10313,13 +10313,13 @@
         <v>45093</v>
       </c>
       <c r="G99">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="H99" s="2">
         <v>45276</v>
       </c>
       <c r="I99">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="J99" t="inlineStr">
         <is>
@@ -10416,13 +10416,13 @@
         <v>45123</v>
       </c>
       <c r="G100">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="H100" s="2">
         <v>45307</v>
       </c>
       <c r="I100">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="J100" t="inlineStr">
         <is>
@@ -10519,13 +10519,13 @@
         <v>45014</v>
       </c>
       <c r="G101">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="H101" s="2">
         <v>45198</v>
       </c>
       <c r="I101">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="J101" t="inlineStr">
         <is>
@@ -10622,13 +10622,13 @@
         <v>45093</v>
       </c>
       <c r="G102">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="H102" s="2">
         <v>45276</v>
       </c>
       <c r="I102">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="J102" t="inlineStr">
         <is>
@@ -10725,13 +10725,13 @@
         <v>45122</v>
       </c>
       <c r="G103">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="H103" s="2">
         <v>45306</v>
       </c>
       <c r="I103">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="J103" t="inlineStr">
         <is>
@@ -10828,13 +10828,13 @@
         <v>45122</v>
       </c>
       <c r="G104">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="H104" s="2">
         <v>45306</v>
       </c>
       <c r="I104">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="J104" t="inlineStr">
         <is>
@@ -10926,13 +10926,13 @@
         <v>45050</v>
       </c>
       <c r="G105">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="H105" s="2">
         <v>45234</v>
       </c>
       <c r="I105">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="J105" t="inlineStr">
         <is>
@@ -11029,13 +11029,13 @@
         <v>45085</v>
       </c>
       <c r="G106">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="H106" s="2">
         <v>45268</v>
       </c>
       <c r="I106">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="J106" t="inlineStr">
         <is>
@@ -11132,13 +11132,13 @@
         <v>45093</v>
       </c>
       <c r="G107">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="H107" s="2">
         <v>45185</v>
       </c>
       <c r="I107">
-        <v>-2</v>
+        <v>-3</v>
       </c>
       <c r="J107" t="inlineStr">
         <is>
@@ -11230,13 +11230,13 @@
         <v>45093</v>
       </c>
       <c r="G108">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="H108" s="2">
         <v>45185</v>
       </c>
       <c r="I108">
-        <v>-2</v>
+        <v>-3</v>
       </c>
       <c r="J108" t="inlineStr">
         <is>
@@ -11328,13 +11328,13 @@
         <v>45093</v>
       </c>
       <c r="G109">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="H109" s="2">
         <v>45185</v>
       </c>
       <c r="I109">
-        <v>-2</v>
+        <v>-3</v>
       </c>
       <c r="J109" t="inlineStr">
         <is>
@@ -11431,13 +11431,13 @@
         <v>45148</v>
       </c>
       <c r="G110">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="H110" s="2">
         <v>45240</v>
       </c>
       <c r="I110">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="J110" t="inlineStr">
         <is>
@@ -11534,13 +11534,13 @@
         <v>45119</v>
       </c>
       <c r="G111">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="H111" s="2">
         <v>45211</v>
       </c>
       <c r="I111">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="J111" t="inlineStr">
         <is>
@@ -11637,13 +11637,13 @@
         <v>45172</v>
       </c>
       <c r="G112">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H112" s="2">
         <v>45263</v>
       </c>
       <c r="I112">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="J112" t="inlineStr">
         <is>
@@ -11740,13 +11740,13 @@
         <v>45023</v>
       </c>
       <c r="G113">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="H113" s="2">
         <v>45206</v>
       </c>
       <c r="I113">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="J113" t="inlineStr">
         <is>
@@ -11843,13 +11843,13 @@
         <v>45111</v>
       </c>
       <c r="G114">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="H114" s="2">
         <v>45203</v>
       </c>
       <c r="I114">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="J114" t="inlineStr">
         <is>
@@ -11946,7 +11946,7 @@
         <v>45218</v>
       </c>
       <c r="I115">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="J115" t="inlineStr">
         <is>
@@ -12043,13 +12043,13 @@
         <v>45161</v>
       </c>
       <c r="G116">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="H116" s="2">
         <v>45253</v>
       </c>
       <c r="I116">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="J116" t="inlineStr">
         <is>
@@ -12146,13 +12146,13 @@
         <v>45115</v>
       </c>
       <c r="G117">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="H117" s="2">
         <v>45299</v>
       </c>
       <c r="I117">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="J117" t="inlineStr">
         <is>
@@ -12244,13 +12244,13 @@
         <v>45094</v>
       </c>
       <c r="G118">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="H118" s="2">
         <v>45277</v>
       </c>
       <c r="I118">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="J118" t="inlineStr">
         <is>
@@ -12347,13 +12347,13 @@
         <v>45104</v>
       </c>
       <c r="G119">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="H119" s="2">
         <v>45287</v>
       </c>
       <c r="I119">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="J119" t="inlineStr">
         <is>
@@ -12450,13 +12450,13 @@
         <v>45104</v>
       </c>
       <c r="G120">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="H120" s="2">
         <v>45287</v>
       </c>
       <c r="I120">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="J120" t="inlineStr">
         <is>
@@ -12553,13 +12553,13 @@
         <v>45104</v>
       </c>
       <c r="G121">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="H121" s="2">
         <v>45287</v>
       </c>
       <c r="I121">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="J121" t="inlineStr">
         <is>
@@ -12656,13 +12656,13 @@
         <v>45104</v>
       </c>
       <c r="G122">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="H122" s="2">
         <v>45287</v>
       </c>
       <c r="I122">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="J122" t="inlineStr">
         <is>
@@ -12759,13 +12759,13 @@
         <v>45107</v>
       </c>
       <c r="G123">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="H123" s="2">
         <v>45199</v>
       </c>
       <c r="I123">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="J123" t="inlineStr">
         <is>
@@ -12862,13 +12862,13 @@
         <v>45013</v>
       </c>
       <c r="G124">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="H124" s="2">
         <v>45197</v>
       </c>
       <c r="I124">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="J124" t="inlineStr">
         <is>
@@ -12965,13 +12965,13 @@
         <v>45121</v>
       </c>
       <c r="G125">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="H125" s="2">
         <v>45213</v>
       </c>
       <c r="I125">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="J125" t="inlineStr">
         <is>
@@ -13068,13 +13068,13 @@
         <v>45134</v>
       </c>
       <c r="G126">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="H126" s="2">
         <v>45226</v>
       </c>
       <c r="I126">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="J126" t="inlineStr">
         <is>
@@ -13171,7 +13171,7 @@
         <v>45212</v>
       </c>
       <c r="I127">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="J127" t="inlineStr">
         <is>
@@ -13268,13 +13268,13 @@
         <v>45126</v>
       </c>
       <c r="G128">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="H128" s="2">
         <v>45218</v>
       </c>
       <c r="I128">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="J128" t="inlineStr">
         <is>
@@ -13366,13 +13366,13 @@
         <v>45158</v>
       </c>
       <c r="G129">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="H129" s="2">
         <v>45250</v>
       </c>
       <c r="I129">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="J129" t="inlineStr">
         <is>
@@ -13469,13 +13469,13 @@
         <v>45171</v>
       </c>
       <c r="G130">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="H130" s="2">
         <v>45262</v>
       </c>
       <c r="I130">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="J130" t="inlineStr">
         <is>
@@ -13572,13 +13572,13 @@
         <v>45111</v>
       </c>
       <c r="G131">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="H131" s="2">
         <v>45203</v>
       </c>
       <c r="I131">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="J131" t="inlineStr">
         <is>
@@ -13675,13 +13675,13 @@
         <v>45144</v>
       </c>
       <c r="G132">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="H132" s="2">
         <v>45236</v>
       </c>
       <c r="I132">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="J132" t="inlineStr">
         <is>
@@ -13778,13 +13778,13 @@
         <v>45156</v>
       </c>
       <c r="G133">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="H133" s="2">
         <v>45248</v>
       </c>
       <c r="I133">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="J133" t="inlineStr">
         <is>
@@ -13876,13 +13876,13 @@
         <v>45146</v>
       </c>
       <c r="G134">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="H134" s="2">
         <v>45238</v>
       </c>
       <c r="I134">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="J134" t="inlineStr">
         <is>
@@ -13979,13 +13979,13 @@
         <v>45140</v>
       </c>
       <c r="G135">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="H135" s="2">
         <v>45232</v>
       </c>
       <c r="I135">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="J135" t="inlineStr">
         <is>
@@ -14082,13 +14082,13 @@
         <v>45104</v>
       </c>
       <c r="G136">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="H136" s="2">
         <v>45196</v>
       </c>
       <c r="I136">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="J136" t="inlineStr">
         <is>
@@ -14185,13 +14185,13 @@
         <v>45105</v>
       </c>
       <c r="G137">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="H137" s="2">
         <v>45197</v>
       </c>
       <c r="I137">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="J137" t="inlineStr">
         <is>
@@ -14288,13 +14288,13 @@
         <v>45179</v>
       </c>
       <c r="G138">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="H138" s="2">
         <v>45270</v>
       </c>
       <c r="I138">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="J138" t="inlineStr">
         <is>
@@ -14386,13 +14386,13 @@
         <v>45105</v>
       </c>
       <c r="G139">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="H139" s="2">
         <v>45197</v>
       </c>
       <c r="I139">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="J139" t="inlineStr">
         <is>
@@ -14489,13 +14489,13 @@
         <v>45182</v>
       </c>
       <c r="G140">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="H140" s="2">
         <v>45273</v>
       </c>
       <c r="I140">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="J140" t="inlineStr">
         <is>
@@ -14592,13 +14592,13 @@
         <v>45116</v>
       </c>
       <c r="G141">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="H141" s="2">
         <v>45208</v>
       </c>
       <c r="I141">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="J141" t="inlineStr">
         <is>
@@ -14690,13 +14690,13 @@
         <v>45150</v>
       </c>
       <c r="G142">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="H142" s="2">
         <v>45242</v>
       </c>
       <c r="I142">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="J142" t="inlineStr">
         <is>
@@ -14793,7 +14793,7 @@
         <v>45238</v>
       </c>
       <c r="I143">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="J143" t="inlineStr">
         <is>
@@ -14890,13 +14890,13 @@
         <v>45171</v>
       </c>
       <c r="G144">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="H144" s="2">
         <v>45262</v>
       </c>
       <c r="I144">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="J144" t="inlineStr">
         <is>
@@ -14993,13 +14993,13 @@
         <v>45102</v>
       </c>
       <c r="G145">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="H145" s="2">
         <v>45194</v>
       </c>
       <c r="I145">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="J145" t="inlineStr">
         <is>
@@ -15086,13 +15086,13 @@
         <v>45119</v>
       </c>
       <c r="G146">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="H146" s="2">
         <v>45211</v>
       </c>
       <c r="I146">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="J146" t="inlineStr">
         <is>
@@ -15189,13 +15189,13 @@
         <v>45165</v>
       </c>
       <c r="G147">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="H147" s="2">
         <v>45257</v>
       </c>
       <c r="I147">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="J147" t="inlineStr">
         <is>
@@ -15292,13 +15292,13 @@
         <v>45166</v>
       </c>
       <c r="G148">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="H148" s="2">
         <v>45258</v>
       </c>
       <c r="I148">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="J148" t="inlineStr">
         <is>
@@ -15395,13 +15395,13 @@
         <v>45093</v>
       </c>
       <c r="G149">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="H149" s="2">
         <v>45185</v>
       </c>
       <c r="I149">
-        <v>-2</v>
+        <v>-3</v>
       </c>
       <c r="J149" t="inlineStr">
         <is>
@@ -15498,13 +15498,13 @@
         <v>45035</v>
       </c>
       <c r="G150">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="H150" s="2">
         <v>45218</v>
       </c>
       <c r="I150">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="J150" t="inlineStr">
         <is>
@@ -15601,13 +15601,13 @@
         <v>45174</v>
       </c>
       <c r="G151">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="H151" s="2">
         <v>45356</v>
       </c>
       <c r="I151">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="J151" t="inlineStr">
         <is>
@@ -15704,13 +15704,13 @@
         <v>45089</v>
       </c>
       <c r="G152">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="H152" s="2">
         <v>45272</v>
       </c>
       <c r="I152">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="J152" t="inlineStr">
         <is>
@@ -15807,13 +15807,13 @@
         <v>45124</v>
       </c>
       <c r="G153">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="H153" s="2">
         <v>45308</v>
       </c>
       <c r="I153">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="J153" t="inlineStr">
         <is>
@@ -15910,13 +15910,13 @@
         <v>45124</v>
       </c>
       <c r="G154">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="H154" s="2">
         <v>45308</v>
       </c>
       <c r="I154">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="J154" t="inlineStr">
         <is>
@@ -16013,13 +16013,13 @@
         <v>45026</v>
       </c>
       <c r="G155">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="H155" s="2">
         <v>45209</v>
       </c>
       <c r="I155">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="J155" t="inlineStr">
         <is>
@@ -16116,13 +16116,13 @@
         <v>45026</v>
       </c>
       <c r="G156">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="H156" s="2">
         <v>45209</v>
       </c>
       <c r="I156">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="J156" t="inlineStr">
         <is>
@@ -16219,13 +16219,13 @@
         <v>45026</v>
       </c>
       <c r="G157">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="H157" s="2">
         <v>45209</v>
       </c>
       <c r="I157">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="J157" t="inlineStr">
         <is>
@@ -16322,13 +16322,13 @@
         <v>45026</v>
       </c>
       <c r="G158">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="H158" s="2">
         <v>45209</v>
       </c>
       <c r="I158">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="J158" t="inlineStr">
         <is>
@@ -16425,13 +16425,13 @@
         <v>45156</v>
       </c>
       <c r="G159">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="H159" s="2">
         <v>45247</v>
       </c>
       <c r="I159">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="J159" t="inlineStr">
         <is>
@@ -16528,13 +16528,13 @@
         <v>45153</v>
       </c>
       <c r="G160">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="H160" s="2">
         <v>45245</v>
       </c>
       <c r="I160">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="J160" t="inlineStr">
         <is>
@@ -16631,13 +16631,13 @@
         <v>45135</v>
       </c>
       <c r="G161">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="H161" s="2">
         <v>45319</v>
       </c>
       <c r="I161">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="J161" t="inlineStr">
         <is>
@@ -16734,13 +16734,13 @@
         <v>45091</v>
       </c>
       <c r="G162">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="H162" s="2">
         <v>45274</v>
       </c>
       <c r="I162">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="J162" t="inlineStr">
         <is>
@@ -16832,13 +16832,13 @@
         <v>45091</v>
       </c>
       <c r="G163">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="H163" s="2">
         <v>45274</v>
       </c>
       <c r="I163">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="J163" t="inlineStr">
         <is>
@@ -16930,13 +16930,13 @@
         <v>45138</v>
       </c>
       <c r="G164">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="H164" s="2">
         <v>45322</v>
       </c>
       <c r="I164">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="J164" t="inlineStr">
         <is>
@@ -17033,13 +17033,13 @@
         <v>45138</v>
       </c>
       <c r="G165">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="H165" s="2">
         <v>45322</v>
       </c>
       <c r="I165">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="J165" t="inlineStr">
         <is>
@@ -17136,13 +17136,13 @@
         <v>45085</v>
       </c>
       <c r="G166">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="H166" s="2">
         <v>45268</v>
       </c>
       <c r="I166">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="J166" t="inlineStr">
         <is>
@@ -17239,13 +17239,13 @@
         <v>45085</v>
       </c>
       <c r="G167">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="H167" s="2">
         <v>45268</v>
       </c>
       <c r="I167">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="J167" t="inlineStr">
         <is>
@@ -17342,7 +17342,7 @@
         <v>45326</v>
       </c>
       <c r="I168">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="J168" t="inlineStr">
         <is>
@@ -17439,13 +17439,13 @@
         <v>45173</v>
       </c>
       <c r="G169">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="H169" s="2">
         <v>45355</v>
       </c>
       <c r="I169">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="J169" t="inlineStr">
         <is>
@@ -17542,13 +17542,13 @@
         <v>45056</v>
       </c>
       <c r="G170">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="H170" s="2">
         <v>45240</v>
       </c>
       <c r="I170">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="J170" t="inlineStr">
         <is>
@@ -17645,7 +17645,7 @@
         <v>45238</v>
       </c>
       <c r="I171">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="J171" t="inlineStr">
         <is>
@@ -17742,13 +17742,13 @@
         <v>45141</v>
       </c>
       <c r="G172">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="H172" s="2">
         <v>45325</v>
       </c>
       <c r="I172">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="J172" t="inlineStr">
         <is>
@@ -17845,13 +17845,13 @@
         <v>45037</v>
       </c>
       <c r="G173">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="H173" s="2">
         <v>45220</v>
       </c>
       <c r="I173">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="J173" t="inlineStr">
         <is>
@@ -17948,13 +17948,13 @@
         <v>45171</v>
       </c>
       <c r="G174">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="H174" s="2">
         <v>45262</v>
       </c>
       <c r="I174">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="J174" t="inlineStr">
         <is>
@@ -18051,13 +18051,13 @@
         <v>45105</v>
       </c>
       <c r="G175">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="H175" s="2">
         <v>45197</v>
       </c>
       <c r="I175">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="J175" t="inlineStr">
         <is>
@@ -18154,13 +18154,13 @@
         <v>45162</v>
       </c>
       <c r="G176">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="H176" s="2">
         <v>45254</v>
       </c>
       <c r="I176">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="J176" t="inlineStr">
         <is>
@@ -18257,13 +18257,13 @@
         <v>45061</v>
       </c>
       <c r="G177">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="H177" s="2">
         <v>45245</v>
       </c>
       <c r="I177">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="J177" t="inlineStr">
         <is>
@@ -18360,13 +18360,13 @@
         <v>45120</v>
       </c>
       <c r="G178">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="H178" s="2">
         <v>45212</v>
       </c>
       <c r="I178">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="J178" t="inlineStr">
         <is>
@@ -18463,7 +18463,7 @@
         <v>45191</v>
       </c>
       <c r="I179">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="J179" t="inlineStr">
         <is>
@@ -18560,13 +18560,13 @@
         <v>45088</v>
       </c>
       <c r="G180">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="H180" s="2">
         <v>45271</v>
       </c>
       <c r="I180">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="J180" t="inlineStr">
         <is>
@@ -18663,13 +18663,13 @@
         <v>45100</v>
       </c>
       <c r="G181">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="H181" s="2">
         <v>45192</v>
       </c>
       <c r="I181">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="J181" t="inlineStr">
         <is>
@@ -18756,13 +18756,13 @@
         <v>45131</v>
       </c>
       <c r="G182">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="H182" s="2">
         <v>45223</v>
       </c>
       <c r="I182">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="J182" t="inlineStr">
         <is>
@@ -18854,13 +18854,13 @@
         <v>45136</v>
       </c>
       <c r="G183">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="H183" s="2">
         <v>45228</v>
       </c>
       <c r="I183">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="J183" t="inlineStr">
         <is>
@@ -18952,13 +18952,13 @@
         <v>45150</v>
       </c>
       <c r="G184">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="H184" s="2">
         <v>45242</v>
       </c>
       <c r="I184">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="J184" t="inlineStr">
         <is>
@@ -19050,13 +19050,13 @@
         <v>45118</v>
       </c>
       <c r="G185">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="H185" s="2">
         <v>45210</v>
       </c>
       <c r="I185">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="J185" t="inlineStr">
         <is>
@@ -19148,13 +19148,13 @@
         <v>45129</v>
       </c>
       <c r="G186">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="H186" s="2">
         <v>45221</v>
       </c>
       <c r="I186">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="J186" t="inlineStr">
         <is>
@@ -19246,13 +19246,13 @@
         <v>45097</v>
       </c>
       <c r="G187">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="H187" s="2">
         <v>45189</v>
       </c>
       <c r="I187">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J187" t="inlineStr">
         <is>
@@ -19339,13 +19339,13 @@
         <v>45101</v>
       </c>
       <c r="G188">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="H188" s="2">
         <v>45193</v>
       </c>
       <c r="I188">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="J188" t="inlineStr">
         <is>
@@ -19432,13 +19432,13 @@
         <v>45165</v>
       </c>
       <c r="G189">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="H189" s="2">
         <v>45257</v>
       </c>
       <c r="I189">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="J189" t="inlineStr">
         <is>
@@ -19530,7 +19530,7 @@
         <v>45202</v>
       </c>
       <c r="I190">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="J190" t="inlineStr">
         <is>
@@ -19627,13 +19627,13 @@
         <v>45081</v>
       </c>
       <c r="G191">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="H191" s="2">
         <v>45264</v>
       </c>
       <c r="I191">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="J191" t="inlineStr">
         <is>
@@ -19730,13 +19730,13 @@
         <v>45081</v>
       </c>
       <c r="G192">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="H192" s="2">
         <v>45264</v>
       </c>
       <c r="I192">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="J192" t="inlineStr">
         <is>
@@ -19833,7 +19833,7 @@
         <v>45319</v>
       </c>
       <c r="I193">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="J193" t="inlineStr">
         <is>
@@ -19930,7 +19930,7 @@
         <v>45319</v>
       </c>
       <c r="I194">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="J194" t="inlineStr">
         <is>
@@ -20022,13 +20022,13 @@
         <v>45046</v>
       </c>
       <c r="G195">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="H195" s="2">
         <v>45230</v>
       </c>
       <c r="I195">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="J195" t="inlineStr">
         <is>
@@ -20125,13 +20125,13 @@
         <v>45046</v>
       </c>
       <c r="G196">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="H196" s="2">
         <v>45230</v>
       </c>
       <c r="I196">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="J196" t="inlineStr">
         <is>
@@ -20228,13 +20228,13 @@
         <v>45031</v>
       </c>
       <c r="G197">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="H197" s="2">
         <v>45214</v>
       </c>
       <c r="I197">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="J197" t="inlineStr">
         <is>
@@ -20331,13 +20331,13 @@
         <v>45031</v>
       </c>
       <c r="G198">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="H198" s="2">
         <v>45214</v>
       </c>
       <c r="I198">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="J198" t="inlineStr">
         <is>
@@ -20434,13 +20434,13 @@
         <v>45031</v>
       </c>
       <c r="G199">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="H199" s="2">
         <v>45214</v>
       </c>
       <c r="I199">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="J199" t="inlineStr">
         <is>
@@ -20537,13 +20537,13 @@
         <v>45031</v>
       </c>
       <c r="G200">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="H200" s="2">
         <v>45214</v>
       </c>
       <c r="I200">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="J200" t="inlineStr">
         <is>
@@ -20640,13 +20640,13 @@
         <v>45067</v>
       </c>
       <c r="G201">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="H201" s="2">
         <v>45251</v>
       </c>
       <c r="I201">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="J201" t="inlineStr">
         <is>
@@ -20743,13 +20743,13 @@
         <v>45067</v>
       </c>
       <c r="G202">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="H202" s="2">
         <v>45251</v>
       </c>
       <c r="I202">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="J202" t="inlineStr">
         <is>
@@ -20846,13 +20846,13 @@
         <v>45067</v>
       </c>
       <c r="G203">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="H203" s="2">
         <v>45251</v>
       </c>
       <c r="I203">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="J203" t="inlineStr">
         <is>
@@ -20949,13 +20949,13 @@
         <v>45067</v>
       </c>
       <c r="G204">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="H204" s="2">
         <v>45251</v>
       </c>
       <c r="I204">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="J204" t="inlineStr">
         <is>
@@ -21052,13 +21052,13 @@
         <v>45178</v>
       </c>
       <c r="G205">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="H205" s="2">
         <v>45269</v>
       </c>
       <c r="I205">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="J205" t="inlineStr">
         <is>
@@ -21155,7 +21155,7 @@
         <v>45252</v>
       </c>
       <c r="I206">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="J206" t="inlineStr">
         <is>
@@ -21252,13 +21252,13 @@
         <v>45087</v>
       </c>
       <c r="G207">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="H207" s="2">
         <v>45270</v>
       </c>
       <c r="I207">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="J207" t="inlineStr">
         <is>
@@ -21355,13 +21355,13 @@
         <v>45099</v>
       </c>
       <c r="G208">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="H208" s="2">
         <v>45282</v>
       </c>
       <c r="I208">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="J208" t="inlineStr">
         <is>
@@ -21458,13 +21458,13 @@
         <v>45175</v>
       </c>
       <c r="G209">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="H209" s="2">
         <v>45356</v>
       </c>
       <c r="I209">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="J209" t="inlineStr">
         <is>
@@ -21561,13 +21561,13 @@
         <v>45175</v>
       </c>
       <c r="G210">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="H210" s="2">
         <v>45356</v>
       </c>
       <c r="I210">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="J210" t="inlineStr">
         <is>
@@ -21664,13 +21664,13 @@
         <v>45166</v>
       </c>
       <c r="G211">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="H211" s="2">
         <v>45350</v>
       </c>
       <c r="I211">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="J211" t="inlineStr">
         <is>
@@ -21767,13 +21767,13 @@
         <v>45166</v>
       </c>
       <c r="G212">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="H212" s="2">
         <v>45350</v>
       </c>
       <c r="I212">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="J212" t="inlineStr">
         <is>
@@ -21870,13 +21870,13 @@
         <v>45090</v>
       </c>
       <c r="G213">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="H213" s="2">
         <v>45273</v>
       </c>
       <c r="I213">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="J213" t="inlineStr">
         <is>
@@ -21973,13 +21973,13 @@
         <v>45106</v>
       </c>
       <c r="G214">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="H214" s="2">
         <v>45289</v>
       </c>
       <c r="I214">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="J214" t="inlineStr">
         <is>
@@ -22076,13 +22076,13 @@
         <v>45134</v>
       </c>
       <c r="G215">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="H215" s="2">
         <v>45226</v>
       </c>
       <c r="I215">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="J215" t="inlineStr">
         <is>
@@ -22179,13 +22179,13 @@
         <v>45132</v>
       </c>
       <c r="G216">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="H216" s="2">
         <v>45224</v>
       </c>
       <c r="I216">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="J216" t="inlineStr">
         <is>
@@ -22282,13 +22282,13 @@
         <v>45150</v>
       </c>
       <c r="G217">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="H217" s="2">
         <v>45242</v>
       </c>
       <c r="I217">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="J217" t="inlineStr">
         <is>
@@ -22385,13 +22385,13 @@
         <v>45095</v>
       </c>
       <c r="G218">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="H218" s="2">
         <v>45187</v>
       </c>
       <c r="I218">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="J218" t="inlineStr">
         <is>
@@ -22483,13 +22483,13 @@
         <v>45182</v>
       </c>
       <c r="G219">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="H219" s="2">
         <v>45273</v>
       </c>
       <c r="I219">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="J219" t="inlineStr">
         <is>
@@ -22586,7 +22586,7 @@
         <v>45196</v>
       </c>
       <c r="I220">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="J220" t="inlineStr">
         <is>
@@ -22683,13 +22683,13 @@
         <v>45108</v>
       </c>
       <c r="G221">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="H221" s="2">
         <v>45200</v>
       </c>
       <c r="I221">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="J221" t="inlineStr">
         <is>
@@ -22786,13 +22786,13 @@
         <v>45135</v>
       </c>
       <c r="G222">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="H222" s="2">
         <v>45227</v>
       </c>
       <c r="I222">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="J222" t="inlineStr">
         <is>
@@ -22889,13 +22889,13 @@
         <v>45148</v>
       </c>
       <c r="G223">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="H223" s="2">
         <v>45240</v>
       </c>
       <c r="I223">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="J223" t="inlineStr">
         <is>
@@ -22987,13 +22987,13 @@
         <v>45100</v>
       </c>
       <c r="G224">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="H224" s="2">
         <v>45192</v>
       </c>
       <c r="I224">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="J224" t="inlineStr">
         <is>
@@ -23085,13 +23085,13 @@
         <v>45136</v>
       </c>
       <c r="G225">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="H225" s="2">
         <v>45320</v>
       </c>
       <c r="I225">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="J225" t="inlineStr">
         <is>
@@ -23188,13 +23188,13 @@
         <v>45136</v>
       </c>
       <c r="G226">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="H226" s="2">
         <v>45320</v>
       </c>
       <c r="I226">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="J226" t="inlineStr">
         <is>
@@ -23291,13 +23291,13 @@
         <v>45094</v>
       </c>
       <c r="G227">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="H227" s="2">
         <v>45277</v>
       </c>
       <c r="I227">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="J227" t="inlineStr">
         <is>
@@ -23394,13 +23394,13 @@
         <v>45081</v>
       </c>
       <c r="G228">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="H228" s="2">
         <v>45264</v>
       </c>
       <c r="I228">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="J228" t="inlineStr">
         <is>
@@ -23497,13 +23497,13 @@
         <v>45099</v>
       </c>
       <c r="G229">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="H229" s="2">
         <v>45282</v>
       </c>
       <c r="I229">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="J229" t="inlineStr">
         <is>
@@ -23600,13 +23600,13 @@
         <v>45018</v>
       </c>
       <c r="G230">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="H230" s="2">
         <v>45201</v>
       </c>
       <c r="I230">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="J230" t="inlineStr">
         <is>
@@ -23703,13 +23703,13 @@
         <v>45031</v>
       </c>
       <c r="G231">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="H231" s="2">
         <v>45214</v>
       </c>
       <c r="I231">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="J231" t="inlineStr">
         <is>
@@ -23806,7 +23806,7 @@
         <v>45294</v>
       </c>
       <c r="I232">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="J232" t="inlineStr">
         <is>
@@ -23903,13 +23903,13 @@
         <v>45079</v>
       </c>
       <c r="G233">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="H233" s="2">
         <v>45262</v>
       </c>
       <c r="I233">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="J233" t="inlineStr">
         <is>
@@ -24006,7 +24006,7 @@
         <v>45199</v>
       </c>
       <c r="I234">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="J234" t="inlineStr">
         <is>
@@ -24103,13 +24103,13 @@
         <v>45021</v>
       </c>
       <c r="G235">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="H235" s="2">
         <v>45204</v>
       </c>
       <c r="I235">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="J235" t="inlineStr">
         <is>
@@ -24206,13 +24206,13 @@
         <v>45021</v>
       </c>
       <c r="G236">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="H236" s="2">
         <v>45204</v>
       </c>
       <c r="I236">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="J236" t="inlineStr">
         <is>
@@ -24309,13 +24309,13 @@
         <v>45080</v>
       </c>
       <c r="G237">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="H237" s="2">
         <v>45263</v>
       </c>
       <c r="I237">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="J237" t="inlineStr">
         <is>
@@ -24412,13 +24412,13 @@
         <v>45046</v>
       </c>
       <c r="G238">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="H238" s="2">
         <v>45229</v>
       </c>
       <c r="I238">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="J238" t="inlineStr">
         <is>
@@ -24515,13 +24515,13 @@
         <v>45112</v>
       </c>
       <c r="G239">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="H239" s="2">
         <v>45204</v>
       </c>
       <c r="I239">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="J239" t="inlineStr">
         <is>
@@ -24609,13 +24609,13 @@
         <v>45112</v>
       </c>
       <c r="G240">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="H240" s="2">
         <v>45204</v>
       </c>
       <c r="I240">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="J240" t="inlineStr">
         <is>
@@ -24703,13 +24703,13 @@
         <v>45016</v>
       </c>
       <c r="G241">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="H241" s="2">
         <v>45199</v>
       </c>
       <c r="I241">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="J241" t="inlineStr">
         <is>
@@ -24806,13 +24806,13 @@
         <v>45070</v>
       </c>
       <c r="G242">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="H242" s="2">
         <v>45254</v>
       </c>
       <c r="I242">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="J242" t="inlineStr">
         <is>
@@ -24909,13 +24909,13 @@
         <v>45168</v>
       </c>
       <c r="G243">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="H243" s="2">
         <v>45260</v>
       </c>
       <c r="I243">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="J243" t="inlineStr">
         <is>
@@ -25012,13 +25012,13 @@
         <v>45027</v>
       </c>
       <c r="G244">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="H244" s="2">
         <v>45210</v>
       </c>
       <c r="I244">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="J244" t="inlineStr">
         <is>
@@ -25115,13 +25115,13 @@
         <v>45077</v>
       </c>
       <c r="G245">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="H245" s="2">
         <v>45260</v>
       </c>
       <c r="I245">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="J245" t="inlineStr">
         <is>
@@ -25218,13 +25218,13 @@
         <v>45100</v>
       </c>
       <c r="G246">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="H246" s="2">
         <v>45283</v>
       </c>
       <c r="I246">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="J246" t="inlineStr">
         <is>
@@ -25321,7 +25321,7 @@
         <v>45281</v>
       </c>
       <c r="I247">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="J247" t="inlineStr">
         <is>
@@ -25418,13 +25418,13 @@
         <v>45044</v>
       </c>
       <c r="G248">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="H248" s="2">
         <v>45227</v>
       </c>
       <c r="I248">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="J248" t="inlineStr">
         <is>
@@ -25521,13 +25521,13 @@
         <v>45101</v>
       </c>
       <c r="G249">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="H249" s="2">
         <v>45283</v>
       </c>
       <c r="I249">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="J249" t="inlineStr">
         <is>
@@ -25624,13 +25624,13 @@
         <v>45134</v>
       </c>
       <c r="G250">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="H250" s="2">
         <v>45226</v>
       </c>
       <c r="I250">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="J250" t="inlineStr">
         <is>
@@ -25727,13 +25727,13 @@
         <v>45158</v>
       </c>
       <c r="G251">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="H251" s="2">
         <v>45250</v>
       </c>
       <c r="I251">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="J251" t="inlineStr">
         <is>
@@ -25830,13 +25830,13 @@
         <v>45108</v>
       </c>
       <c r="G252">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="H252" s="2">
         <v>45200</v>
       </c>
       <c r="I252">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="J252" t="inlineStr">
         <is>
@@ -25933,7 +25933,7 @@
         <v>45317</v>
       </c>
       <c r="I253">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="J253" t="inlineStr">
         <is>
@@ -26030,13 +26030,13 @@
         <v>45039</v>
       </c>
       <c r="G254">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="H254" s="2">
         <v>45222</v>
       </c>
       <c r="I254">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="J254" t="inlineStr">
         <is>
@@ -26128,13 +26128,13 @@
         <v>45129</v>
       </c>
       <c r="G255">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="H255" s="2">
         <v>45221</v>
       </c>
       <c r="I255">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="J255" t="inlineStr">
         <is>
@@ -26231,13 +26231,13 @@
         <v>45157</v>
       </c>
       <c r="G256">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="H256" s="2">
         <v>45341</v>
       </c>
       <c r="I256">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="J256" t="inlineStr">
         <is>
@@ -26334,13 +26334,13 @@
         <v>45063</v>
       </c>
       <c r="G257">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="H257" s="2">
         <v>45247</v>
       </c>
       <c r="I257">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="J257" t="inlineStr">
         <is>
@@ -26437,7 +26437,7 @@
         <v>45254</v>
       </c>
       <c r="I258">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="J258" t="inlineStr">
         <is>
@@ -26534,7 +26534,7 @@
         <v>45486</v>
       </c>
       <c r="I259">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="J259" t="inlineStr">
         <is>
@@ -26626,13 +26626,13 @@
         <v>45073</v>
       </c>
       <c r="G260">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="H260" s="2">
         <v>45439</v>
       </c>
       <c r="I260">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="J260" t="inlineStr">
         <is>
@@ -26724,7 +26724,7 @@
         <v>45323</v>
       </c>
       <c r="I261">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="J261" t="inlineStr">
         <is>
@@ -26816,7 +26816,7 @@
         <v>45303</v>
       </c>
       <c r="I262">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="J262" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
GH ACTION Headlines Wed Sep 20 18:39:15 UTC 2023
</commit_message>
<xml_diff>
--- a/Data/obligacje_screener.xlsx
+++ b/Data/obligacje_screener.xlsx
@@ -512,7 +512,7 @@
         <v>45340</v>
       </c>
       <c r="I2">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="J2" t="inlineStr">
         <is>
@@ -600,13 +600,13 @@
         <v>45121</v>
       </c>
       <c r="G3">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="H3" s="2">
         <v>45305</v>
       </c>
       <c r="I3">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="J3" t="inlineStr">
         <is>
@@ -703,13 +703,13 @@
         <v>45039</v>
       </c>
       <c r="G4">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="H4" s="2">
         <v>45222</v>
       </c>
       <c r="I4">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="J4" t="inlineStr">
         <is>
@@ -806,13 +806,13 @@
         <v>45039</v>
       </c>
       <c r="G5">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="H5" s="2">
         <v>45222</v>
       </c>
       <c r="I5">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="J5" t="inlineStr">
         <is>
@@ -909,13 +909,13 @@
         <v>45129</v>
       </c>
       <c r="G6">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="H6" s="2">
         <v>45221</v>
       </c>
       <c r="I6">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="J6" t="inlineStr">
         <is>
@@ -1012,13 +1012,13 @@
         <v>45162</v>
       </c>
       <c r="G7">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="H7" s="2">
         <v>45254</v>
       </c>
       <c r="I7">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="J7" t="inlineStr">
         <is>
@@ -1110,13 +1110,13 @@
         <v>45156</v>
       </c>
       <c r="G8">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="H8" s="2">
         <v>45248</v>
       </c>
       <c r="I8">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="J8" t="inlineStr">
         <is>
@@ -1213,13 +1213,13 @@
         <v>45141</v>
       </c>
       <c r="G9">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="H9" s="2">
         <v>45233</v>
       </c>
       <c r="I9">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="J9" t="inlineStr">
         <is>
@@ -1316,13 +1316,13 @@
         <v>45062</v>
       </c>
       <c r="G10">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="H10" s="2">
         <v>45246</v>
       </c>
       <c r="I10">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="J10" t="inlineStr">
         <is>
@@ -1419,7 +1419,7 @@
         <v>45286</v>
       </c>
       <c r="I11">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="J11" t="inlineStr">
         <is>
@@ -1516,13 +1516,13 @@
         <v>45011</v>
       </c>
       <c r="G12">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="H12" s="2">
         <v>45195</v>
       </c>
       <c r="I12">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="J12" t="inlineStr">
         <is>
@@ -1614,13 +1614,13 @@
         <v>45036</v>
       </c>
       <c r="G13">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="H13" s="2">
         <v>45219</v>
       </c>
       <c r="I13">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="J13" t="inlineStr">
         <is>
@@ -1717,13 +1717,13 @@
         <v>45036</v>
       </c>
       <c r="G14">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="H14" s="2">
         <v>45219</v>
       </c>
       <c r="I14">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="J14" t="inlineStr">
         <is>
@@ -1820,13 +1820,13 @@
         <v>45106</v>
       </c>
       <c r="G15">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="H15" s="2">
         <v>45289</v>
       </c>
       <c r="I15">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="J15" t="inlineStr">
         <is>
@@ -1923,13 +1923,13 @@
         <v>45094</v>
       </c>
       <c r="G16">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="H16" s="2">
         <v>45186</v>
       </c>
       <c r="I16">
-        <v>-2</v>
+        <v>-3</v>
       </c>
       <c r="J16" t="inlineStr">
         <is>
@@ -2026,13 +2026,13 @@
         <v>45094</v>
       </c>
       <c r="G17">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="H17" s="2">
         <v>45186</v>
       </c>
       <c r="I17">
-        <v>-2</v>
+        <v>-3</v>
       </c>
       <c r="J17" t="inlineStr">
         <is>
@@ -2129,13 +2129,13 @@
         <v>45132</v>
       </c>
       <c r="G18">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="H18" s="2">
         <v>45224</v>
       </c>
       <c r="I18">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="J18" t="inlineStr">
         <is>
@@ -2232,13 +2232,13 @@
         <v>45137</v>
       </c>
       <c r="G19">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="H19" s="2">
         <v>45229</v>
       </c>
       <c r="I19">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="J19" t="inlineStr">
         <is>
@@ -2330,13 +2330,13 @@
         <v>45183</v>
       </c>
       <c r="G20">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="H20" s="2">
         <v>45274</v>
       </c>
       <c r="I20">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="J20" t="inlineStr">
         <is>
@@ -2433,13 +2433,13 @@
         <v>45093</v>
       </c>
       <c r="G21">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="H21" s="2">
         <v>45187</v>
       </c>
       <c r="I21">
-        <v>-1</v>
+        <v>-2</v>
       </c>
       <c r="J21" t="inlineStr">
         <is>
@@ -2536,13 +2536,13 @@
         <v>45096</v>
       </c>
       <c r="G22">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="H22" s="2">
         <v>45187</v>
       </c>
       <c r="I22">
-        <v>-1</v>
+        <v>-2</v>
       </c>
       <c r="J22" t="inlineStr">
         <is>
@@ -2639,7 +2639,7 @@
         <v>45245</v>
       </c>
       <c r="I23">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="J23" t="inlineStr">
         <is>
@@ -2736,7 +2736,7 @@
         <v>45245</v>
       </c>
       <c r="I24">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="J24" t="inlineStr">
         <is>
@@ -2833,13 +2833,13 @@
         <v>45021</v>
       </c>
       <c r="G25">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="H25" s="2">
         <v>45204</v>
       </c>
       <c r="I25">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="J25" t="inlineStr">
         <is>
@@ -2936,13 +2936,13 @@
         <v>45160</v>
       </c>
       <c r="G26">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="H26" s="2">
         <v>45344</v>
       </c>
       <c r="I26">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="J26" t="inlineStr">
         <is>
@@ -3039,13 +3039,13 @@
         <v>45118</v>
       </c>
       <c r="G27">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="H27" s="2">
         <v>45302</v>
       </c>
       <c r="I27">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="J27" t="inlineStr">
         <is>
@@ -3142,13 +3142,13 @@
         <v>45085</v>
       </c>
       <c r="G28">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="H28" s="2">
         <v>45268</v>
       </c>
       <c r="I28">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="J28" t="inlineStr">
         <is>
@@ -3245,13 +3245,13 @@
         <v>45183</v>
       </c>
       <c r="G29">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="H29" s="2">
         <v>45274</v>
       </c>
       <c r="I29">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="J29" t="inlineStr">
         <is>
@@ -3348,7 +3348,7 @@
         <v>45224</v>
       </c>
       <c r="I30">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="J30" t="inlineStr">
         <is>
@@ -3445,13 +3445,13 @@
         <v>45153</v>
       </c>
       <c r="G31">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="H31" s="2">
         <v>45245</v>
       </c>
       <c r="I31">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="J31" t="inlineStr">
         <is>
@@ -3548,13 +3548,13 @@
         <v>45155</v>
       </c>
       <c r="G32">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="H32" s="2">
         <v>45247</v>
       </c>
       <c r="I32">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="J32" t="inlineStr">
         <is>
@@ -3651,7 +3651,7 @@
         <v>45255</v>
       </c>
       <c r="I33">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="J33" t="inlineStr">
         <is>
@@ -3739,13 +3739,13 @@
         <v>45176</v>
       </c>
       <c r="G34">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="H34" s="2">
         <v>45267</v>
       </c>
       <c r="I34">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="J34" t="inlineStr">
         <is>
@@ -3842,13 +3842,13 @@
         <v>45130</v>
       </c>
       <c r="G35">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="H35" s="2">
         <v>45222</v>
       </c>
       <c r="I35">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="J35" t="inlineStr">
         <is>
@@ -3940,13 +3940,13 @@
         <v>45115</v>
       </c>
       <c r="G36">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="H36" s="2">
         <v>45207</v>
       </c>
       <c r="I36">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="J36" t="inlineStr">
         <is>
@@ -4043,13 +4043,13 @@
         <v>45097</v>
       </c>
       <c r="G37">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="H37" s="2">
         <v>45189</v>
       </c>
       <c r="I37">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J37" t="inlineStr">
         <is>
@@ -4141,13 +4141,13 @@
         <v>45107</v>
       </c>
       <c r="G38">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="H38" s="2">
         <v>45290</v>
       </c>
       <c r="I38">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="J38" t="inlineStr">
         <is>
@@ -4244,13 +4244,13 @@
         <v>45063</v>
       </c>
       <c r="G39">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="H39" s="2">
         <v>45247</v>
       </c>
       <c r="I39">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="J39" t="inlineStr">
         <is>
@@ -4347,13 +4347,13 @@
         <v>45177</v>
       </c>
       <c r="G40">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="H40" s="2">
         <v>45359</v>
       </c>
       <c r="I40">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="J40" t="inlineStr">
         <is>
@@ -4450,13 +4450,13 @@
         <v>45107</v>
       </c>
       <c r="G41">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="H41" s="2">
         <v>45290</v>
       </c>
       <c r="I41">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="J41" t="inlineStr">
         <is>
@@ -4553,7 +4553,7 @@
         <v>45265</v>
       </c>
       <c r="I42">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="J42" t="inlineStr">
         <is>
@@ -4650,13 +4650,13 @@
         <v>45098</v>
       </c>
       <c r="G43">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="H43" s="2">
         <v>45281</v>
       </c>
       <c r="I43">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="J43" t="inlineStr">
         <is>
@@ -4753,13 +4753,13 @@
         <v>45099</v>
       </c>
       <c r="G44">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="H44" s="2">
         <v>45282</v>
       </c>
       <c r="I44">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="J44" t="inlineStr">
         <is>
@@ -4856,13 +4856,13 @@
         <v>45106</v>
       </c>
       <c r="G45">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="H45" s="2">
         <v>45289</v>
       </c>
       <c r="I45">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="J45" t="inlineStr">
         <is>
@@ -4959,13 +4959,13 @@
         <v>45106</v>
       </c>
       <c r="G46">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="H46" s="2">
         <v>45289</v>
       </c>
       <c r="I46">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="J46" t="inlineStr">
         <is>
@@ -5062,13 +5062,13 @@
         <v>45120</v>
       </c>
       <c r="G47">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="H47" s="2">
         <v>45304</v>
       </c>
       <c r="I47">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="J47" t="inlineStr">
         <is>
@@ -5165,13 +5165,13 @@
         <v>45118</v>
       </c>
       <c r="G48">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="H48" s="2">
         <v>45302</v>
       </c>
       <c r="I48">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="J48" t="inlineStr">
         <is>
@@ -5268,13 +5268,13 @@
         <v>45152</v>
       </c>
       <c r="G49">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="H49" s="2">
         <v>45336</v>
       </c>
       <c r="I49">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="J49" t="inlineStr">
         <is>
@@ -5371,13 +5371,13 @@
         <v>45042</v>
       </c>
       <c r="G50">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="H50" s="2">
         <v>45225</v>
       </c>
       <c r="I50">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="J50" t="inlineStr">
         <is>
@@ -5474,13 +5474,13 @@
         <v>45122</v>
       </c>
       <c r="G51">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="H51" s="2">
         <v>45306</v>
       </c>
       <c r="I51">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="J51" t="inlineStr">
         <is>
@@ -5577,13 +5577,13 @@
         <v>45139</v>
       </c>
       <c r="G52">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="H52" s="2">
         <v>45323</v>
       </c>
       <c r="I52">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="J52" t="inlineStr">
         <is>
@@ -5671,13 +5671,13 @@
         <v>45099</v>
       </c>
       <c r="G53">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="H53" s="2">
         <v>45282</v>
       </c>
       <c r="I53">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="J53" t="inlineStr">
         <is>
@@ -5774,7 +5774,7 @@
         <v>45196</v>
       </c>
       <c r="I54">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="J54" t="inlineStr">
         <is>
@@ -5871,13 +5871,13 @@
         <v>45044</v>
       </c>
       <c r="G55">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="H55" s="2">
         <v>45227</v>
       </c>
       <c r="I55">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="J55" t="inlineStr">
         <is>
@@ -5974,13 +5974,13 @@
         <v>45151</v>
       </c>
       <c r="G56">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="H56" s="2">
         <v>45243</v>
       </c>
       <c r="I56">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="J56" t="inlineStr">
         <is>
@@ -6072,7 +6072,7 @@
         <v>45196</v>
       </c>
       <c r="I57">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="J57" t="inlineStr">
         <is>
@@ -6169,13 +6169,13 @@
         <v>45069</v>
       </c>
       <c r="G58">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="H58" s="2">
         <v>45253</v>
       </c>
       <c r="I58">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="J58" t="inlineStr">
         <is>
@@ -6272,13 +6272,13 @@
         <v>45099</v>
       </c>
       <c r="G59">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="H59" s="2">
         <v>45191</v>
       </c>
       <c r="I59">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="J59" t="inlineStr">
         <is>
@@ -6370,13 +6370,13 @@
         <v>45113</v>
       </c>
       <c r="G60">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="H60" s="2">
         <v>45205</v>
       </c>
       <c r="I60">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="J60" t="inlineStr">
         <is>
@@ -6473,13 +6473,13 @@
         <v>45127</v>
       </c>
       <c r="G61">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="H61" s="2">
         <v>45219</v>
       </c>
       <c r="I61">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="J61" t="inlineStr">
         <is>
@@ -6576,13 +6576,13 @@
         <v>45058</v>
       </c>
       <c r="G62">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="H62" s="2">
         <v>45242</v>
       </c>
       <c r="I62">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="J62" t="inlineStr">
         <is>
@@ -6679,13 +6679,13 @@
         <v>45010</v>
       </c>
       <c r="G63">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="H63" s="2">
         <v>45194</v>
       </c>
       <c r="I63">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="J63" t="inlineStr">
         <is>
@@ -6777,13 +6777,13 @@
         <v>45025</v>
       </c>
       <c r="G64">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="H64" s="2">
         <v>45208</v>
       </c>
       <c r="I64">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="J64" t="inlineStr">
         <is>
@@ -6880,13 +6880,13 @@
         <v>45025</v>
       </c>
       <c r="G65">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="H65" s="2">
         <v>45208</v>
       </c>
       <c r="I65">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="J65" t="inlineStr">
         <is>
@@ -6983,13 +6983,13 @@
         <v>45089</v>
       </c>
       <c r="G66">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="H66" s="2">
         <v>45272</v>
       </c>
       <c r="I66">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="J66" t="inlineStr">
         <is>
@@ -7086,13 +7086,13 @@
         <v>45178</v>
       </c>
       <c r="G67">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="H67" s="2">
         <v>45269</v>
       </c>
       <c r="I67">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="J67" t="inlineStr">
         <is>
@@ -7184,13 +7184,13 @@
         <v>45104</v>
       </c>
       <c r="G68">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="H68" s="2">
         <v>45196</v>
       </c>
       <c r="I68">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="J68" t="inlineStr">
         <is>
@@ -7287,13 +7287,13 @@
         <v>45149</v>
       </c>
       <c r="G69">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="H69" s="2">
         <v>45241</v>
       </c>
       <c r="I69">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="J69" t="inlineStr">
         <is>
@@ -7390,7 +7390,7 @@
         <v>45205</v>
       </c>
       <c r="I70">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="J70" t="inlineStr">
         <is>
@@ -7487,13 +7487,13 @@
         <v>45114</v>
       </c>
       <c r="G71">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="H71" s="2">
         <v>45205</v>
       </c>
       <c r="I71">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="J71" t="inlineStr">
         <is>
@@ -7590,13 +7590,13 @@
         <v>45115</v>
       </c>
       <c r="G72">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="H72" s="2">
         <v>45207</v>
       </c>
       <c r="I72">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="J72" t="inlineStr">
         <is>
@@ -7693,13 +7693,13 @@
         <v>45097</v>
       </c>
       <c r="G73">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="H73" s="2">
         <v>45189</v>
       </c>
       <c r="I73">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J73" t="inlineStr">
         <is>
@@ -7791,13 +7791,13 @@
         <v>45038</v>
       </c>
       <c r="G74">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="H74" s="2">
         <v>45221</v>
       </c>
       <c r="I74">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="J74" t="inlineStr">
         <is>
@@ -7889,13 +7889,13 @@
         <v>45117</v>
       </c>
       <c r="G75">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="H75" s="2">
         <v>45301</v>
       </c>
       <c r="I75">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="J75" t="inlineStr">
         <is>
@@ -7992,13 +7992,13 @@
         <v>45160</v>
       </c>
       <c r="G76">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="H76" s="2">
         <v>45344</v>
       </c>
       <c r="I76">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="J76" t="inlineStr">
         <is>
@@ -8095,13 +8095,13 @@
         <v>45002</v>
       </c>
       <c r="G77">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="H77" s="2">
         <v>45186</v>
       </c>
       <c r="I77">
-        <v>-2</v>
+        <v>-3</v>
       </c>
       <c r="J77" t="inlineStr">
         <is>
@@ -8198,13 +8198,13 @@
         <v>45043</v>
       </c>
       <c r="G78">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="H78" s="2">
         <v>45226</v>
       </c>
       <c r="I78">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="J78" t="inlineStr">
         <is>
@@ -8301,13 +8301,13 @@
         <v>45079</v>
       </c>
       <c r="G79">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="H79" s="2">
         <v>45262</v>
       </c>
       <c r="I79">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="J79" t="inlineStr">
         <is>
@@ -8404,7 +8404,7 @@
         <v>45254</v>
       </c>
       <c r="I80">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="J80" t="inlineStr">
         <is>
@@ -8501,13 +8501,13 @@
         <v>45104</v>
       </c>
       <c r="G81">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="H81" s="2">
         <v>45287</v>
       </c>
       <c r="I81">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="J81" t="inlineStr">
         <is>
@@ -8604,7 +8604,7 @@
         <v>45288</v>
       </c>
       <c r="I82">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="J82" t="inlineStr">
         <is>
@@ -8696,13 +8696,13 @@
         <v>45175</v>
       </c>
       <c r="G83">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="H83" s="2">
         <v>45357</v>
       </c>
       <c r="I83">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="J83" t="inlineStr">
         <is>
@@ -8799,13 +8799,13 @@
         <v>45054</v>
       </c>
       <c r="G84">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="H84" s="2">
         <v>45238</v>
       </c>
       <c r="I84">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="J84" t="inlineStr">
         <is>
@@ -8902,13 +8902,13 @@
         <v>45056</v>
       </c>
       <c r="G85">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="H85" s="2">
         <v>45240</v>
       </c>
       <c r="I85">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="J85" t="inlineStr">
         <is>
@@ -9005,13 +9005,13 @@
         <v>45085</v>
       </c>
       <c r="G86">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="H86" s="2">
         <v>45268</v>
       </c>
       <c r="I86">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="J86" t="inlineStr">
         <is>
@@ -9108,7 +9108,7 @@
         <v>45194</v>
       </c>
       <c r="I87">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="J87" t="inlineStr">
         <is>
@@ -9195,13 +9195,13 @@
         <v>45103</v>
       </c>
       <c r="G88">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="H88" s="2">
         <v>45286</v>
       </c>
       <c r="I88">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="J88" t="inlineStr">
         <is>
@@ -9298,13 +9298,13 @@
         <v>45103</v>
       </c>
       <c r="G89">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="H89" s="2">
         <v>45286</v>
       </c>
       <c r="I89">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="J89" t="inlineStr">
         <is>
@@ -9401,13 +9401,13 @@
         <v>45008</v>
       </c>
       <c r="G90">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="H90" s="2">
         <v>45192</v>
       </c>
       <c r="I90">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="J90" t="inlineStr">
         <is>
@@ -9499,13 +9499,13 @@
         <v>45100</v>
       </c>
       <c r="G91">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="H91" s="2">
         <v>45287</v>
       </c>
       <c r="I91">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="J91" t="inlineStr">
         <is>
@@ -9602,13 +9602,13 @@
         <v>45003</v>
       </c>
       <c r="G92">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="H92" s="2">
         <v>45187</v>
       </c>
       <c r="I92">
-        <v>-1</v>
+        <v>-2</v>
       </c>
       <c r="J92" t="inlineStr">
         <is>
@@ -9705,13 +9705,13 @@
         <v>45104</v>
       </c>
       <c r="G93">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="H93" s="2">
         <v>45287</v>
       </c>
       <c r="I93">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="J93" t="inlineStr">
         <is>
@@ -9808,13 +9808,13 @@
         <v>45104</v>
       </c>
       <c r="G94">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="H94" s="2">
         <v>45287</v>
       </c>
       <c r="I94">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="J94" t="inlineStr">
         <is>
@@ -9911,13 +9911,13 @@
         <v>45049</v>
       </c>
       <c r="G95">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="H95" s="2">
         <v>45233</v>
       </c>
       <c r="I95">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="J95" t="inlineStr">
         <is>
@@ -10014,13 +10014,13 @@
         <v>45122</v>
       </c>
       <c r="G96">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="H96" s="2">
         <v>45306</v>
       </c>
       <c r="I96">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="J96" t="inlineStr">
         <is>
@@ -10112,13 +10112,13 @@
         <v>45141</v>
       </c>
       <c r="G97">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="H97" s="2">
         <v>45325</v>
       </c>
       <c r="I97">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="J97" t="inlineStr">
         <is>
@@ -10215,13 +10215,13 @@
         <v>45010</v>
       </c>
       <c r="G98">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="H98" s="2">
         <v>45194</v>
       </c>
       <c r="I98">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="J98" t="inlineStr">
         <is>
@@ -10313,13 +10313,13 @@
         <v>45093</v>
       </c>
       <c r="G99">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="H99" s="2">
         <v>45276</v>
       </c>
       <c r="I99">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="J99" t="inlineStr">
         <is>
@@ -10416,13 +10416,13 @@
         <v>45123</v>
       </c>
       <c r="G100">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="H100" s="2">
         <v>45307</v>
       </c>
       <c r="I100">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="J100" t="inlineStr">
         <is>
@@ -10519,13 +10519,13 @@
         <v>45014</v>
       </c>
       <c r="G101">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="H101" s="2">
         <v>45198</v>
       </c>
       <c r="I101">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="J101" t="inlineStr">
         <is>
@@ -10622,13 +10622,13 @@
         <v>45093</v>
       </c>
       <c r="G102">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="H102" s="2">
         <v>45276</v>
       </c>
       <c r="I102">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="J102" t="inlineStr">
         <is>
@@ -10725,13 +10725,13 @@
         <v>45122</v>
       </c>
       <c r="G103">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="H103" s="2">
         <v>45306</v>
       </c>
       <c r="I103">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="J103" t="inlineStr">
         <is>
@@ -10828,13 +10828,13 @@
         <v>45122</v>
       </c>
       <c r="G104">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="H104" s="2">
         <v>45306</v>
       </c>
       <c r="I104">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="J104" t="inlineStr">
         <is>
@@ -10926,13 +10926,13 @@
         <v>45050</v>
       </c>
       <c r="G105">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="H105" s="2">
         <v>45234</v>
       </c>
       <c r="I105">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="J105" t="inlineStr">
         <is>
@@ -11029,13 +11029,13 @@
         <v>45085</v>
       </c>
       <c r="G106">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="H106" s="2">
         <v>45268</v>
       </c>
       <c r="I106">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="J106" t="inlineStr">
         <is>
@@ -11132,13 +11132,13 @@
         <v>45093</v>
       </c>
       <c r="G107">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="H107" s="2">
         <v>45185</v>
       </c>
       <c r="I107">
-        <v>-3</v>
+        <v>-4</v>
       </c>
       <c r="J107" t="inlineStr">
         <is>
@@ -11230,13 +11230,13 @@
         <v>45093</v>
       </c>
       <c r="G108">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="H108" s="2">
         <v>45185</v>
       </c>
       <c r="I108">
-        <v>-3</v>
+        <v>-4</v>
       </c>
       <c r="J108" t="inlineStr">
         <is>
@@ -11328,13 +11328,13 @@
         <v>45093</v>
       </c>
       <c r="G109">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="H109" s="2">
         <v>45185</v>
       </c>
       <c r="I109">
-        <v>-3</v>
+        <v>-4</v>
       </c>
       <c r="J109" t="inlineStr">
         <is>
@@ -11431,13 +11431,13 @@
         <v>45148</v>
       </c>
       <c r="G110">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="H110" s="2">
         <v>45240</v>
       </c>
       <c r="I110">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="J110" t="inlineStr">
         <is>
@@ -11534,13 +11534,13 @@
         <v>45119</v>
       </c>
       <c r="G111">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="H111" s="2">
         <v>45211</v>
       </c>
       <c r="I111">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="J111" t="inlineStr">
         <is>
@@ -11637,13 +11637,13 @@
         <v>45172</v>
       </c>
       <c r="G112">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="H112" s="2">
         <v>45263</v>
       </c>
       <c r="I112">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="J112" t="inlineStr">
         <is>
@@ -11740,13 +11740,13 @@
         <v>45023</v>
       </c>
       <c r="G113">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="H113" s="2">
         <v>45206</v>
       </c>
       <c r="I113">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="J113" t="inlineStr">
         <is>
@@ -11843,13 +11843,13 @@
         <v>45111</v>
       </c>
       <c r="G114">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="H114" s="2">
         <v>45203</v>
       </c>
       <c r="I114">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="J114" t="inlineStr">
         <is>
@@ -11946,7 +11946,7 @@
         <v>45218</v>
       </c>
       <c r="I115">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="J115" t="inlineStr">
         <is>
@@ -12043,13 +12043,13 @@
         <v>45161</v>
       </c>
       <c r="G116">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="H116" s="2">
         <v>45253</v>
       </c>
       <c r="I116">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="J116" t="inlineStr">
         <is>
@@ -12146,13 +12146,13 @@
         <v>45115</v>
       </c>
       <c r="G117">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="H117" s="2">
         <v>45299</v>
       </c>
       <c r="I117">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="J117" t="inlineStr">
         <is>
@@ -12244,13 +12244,13 @@
         <v>45094</v>
       </c>
       <c r="G118">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="H118" s="2">
         <v>45277</v>
       </c>
       <c r="I118">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="J118" t="inlineStr">
         <is>
@@ -12347,13 +12347,13 @@
         <v>45104</v>
       </c>
       <c r="G119">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="H119" s="2">
         <v>45287</v>
       </c>
       <c r="I119">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="J119" t="inlineStr">
         <is>
@@ -12450,13 +12450,13 @@
         <v>45104</v>
       </c>
       <c r="G120">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="H120" s="2">
         <v>45287</v>
       </c>
       <c r="I120">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="J120" t="inlineStr">
         <is>
@@ -12553,13 +12553,13 @@
         <v>45104</v>
       </c>
       <c r="G121">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="H121" s="2">
         <v>45287</v>
       </c>
       <c r="I121">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="J121" t="inlineStr">
         <is>
@@ -12656,13 +12656,13 @@
         <v>45104</v>
       </c>
       <c r="G122">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="H122" s="2">
         <v>45287</v>
       </c>
       <c r="I122">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="J122" t="inlineStr">
         <is>
@@ -12759,13 +12759,13 @@
         <v>45107</v>
       </c>
       <c r="G123">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="H123" s="2">
         <v>45199</v>
       </c>
       <c r="I123">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="J123" t="inlineStr">
         <is>
@@ -12862,13 +12862,13 @@
         <v>45013</v>
       </c>
       <c r="G124">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="H124" s="2">
         <v>45197</v>
       </c>
       <c r="I124">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="J124" t="inlineStr">
         <is>
@@ -12965,13 +12965,13 @@
         <v>45121</v>
       </c>
       <c r="G125">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="H125" s="2">
         <v>45213</v>
       </c>
       <c r="I125">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="J125" t="inlineStr">
         <is>
@@ -13068,13 +13068,13 @@
         <v>45134</v>
       </c>
       <c r="G126">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="H126" s="2">
         <v>45226</v>
       </c>
       <c r="I126">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="J126" t="inlineStr">
         <is>
@@ -13171,7 +13171,7 @@
         <v>45212</v>
       </c>
       <c r="I127">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="J127" t="inlineStr">
         <is>
@@ -13268,13 +13268,13 @@
         <v>45126</v>
       </c>
       <c r="G128">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="H128" s="2">
         <v>45218</v>
       </c>
       <c r="I128">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="J128" t="inlineStr">
         <is>
@@ -13366,13 +13366,13 @@
         <v>45158</v>
       </c>
       <c r="G129">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="H129" s="2">
         <v>45250</v>
       </c>
       <c r="I129">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="J129" t="inlineStr">
         <is>
@@ -13469,13 +13469,13 @@
         <v>45171</v>
       </c>
       <c r="G130">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="H130" s="2">
         <v>45262</v>
       </c>
       <c r="I130">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="J130" t="inlineStr">
         <is>
@@ -13572,13 +13572,13 @@
         <v>45111</v>
       </c>
       <c r="G131">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="H131" s="2">
         <v>45203</v>
       </c>
       <c r="I131">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="J131" t="inlineStr">
         <is>
@@ -13675,13 +13675,13 @@
         <v>45144</v>
       </c>
       <c r="G132">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="H132" s="2">
         <v>45236</v>
       </c>
       <c r="I132">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="J132" t="inlineStr">
         <is>
@@ -13778,13 +13778,13 @@
         <v>45156</v>
       </c>
       <c r="G133">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="H133" s="2">
         <v>45248</v>
       </c>
       <c r="I133">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="J133" t="inlineStr">
         <is>
@@ -13876,13 +13876,13 @@
         <v>45146</v>
       </c>
       <c r="G134">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="H134" s="2">
         <v>45238</v>
       </c>
       <c r="I134">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="J134" t="inlineStr">
         <is>
@@ -13979,13 +13979,13 @@
         <v>45140</v>
       </c>
       <c r="G135">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="H135" s="2">
         <v>45232</v>
       </c>
       <c r="I135">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="J135" t="inlineStr">
         <is>
@@ -14082,13 +14082,13 @@
         <v>45104</v>
       </c>
       <c r="G136">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="H136" s="2">
         <v>45196</v>
       </c>
       <c r="I136">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="J136" t="inlineStr">
         <is>
@@ -14185,13 +14185,13 @@
         <v>45105</v>
       </c>
       <c r="G137">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="H137" s="2">
         <v>45197</v>
       </c>
       <c r="I137">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="J137" t="inlineStr">
         <is>
@@ -14288,13 +14288,13 @@
         <v>45179</v>
       </c>
       <c r="G138">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="H138" s="2">
         <v>45270</v>
       </c>
       <c r="I138">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="J138" t="inlineStr">
         <is>
@@ -14386,13 +14386,13 @@
         <v>45105</v>
       </c>
       <c r="G139">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="H139" s="2">
         <v>45197</v>
       </c>
       <c r="I139">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="J139" t="inlineStr">
         <is>
@@ -14489,13 +14489,13 @@
         <v>45182</v>
       </c>
       <c r="G140">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="H140" s="2">
         <v>45273</v>
       </c>
       <c r="I140">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="J140" t="inlineStr">
         <is>
@@ -14592,13 +14592,13 @@
         <v>45116</v>
       </c>
       <c r="G141">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="H141" s="2">
         <v>45208</v>
       </c>
       <c r="I141">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="J141" t="inlineStr">
         <is>
@@ -14690,13 +14690,13 @@
         <v>45150</v>
       </c>
       <c r="G142">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="H142" s="2">
         <v>45242</v>
       </c>
       <c r="I142">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="J142" t="inlineStr">
         <is>
@@ -14793,7 +14793,7 @@
         <v>45238</v>
       </c>
       <c r="I143">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="J143" t="inlineStr">
         <is>
@@ -14890,13 +14890,13 @@
         <v>45171</v>
       </c>
       <c r="G144">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="H144" s="2">
         <v>45262</v>
       </c>
       <c r="I144">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="J144" t="inlineStr">
         <is>
@@ -14993,13 +14993,13 @@
         <v>45102</v>
       </c>
       <c r="G145">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="H145" s="2">
         <v>45194</v>
       </c>
       <c r="I145">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="J145" t="inlineStr">
         <is>
@@ -15086,13 +15086,13 @@
         <v>45119</v>
       </c>
       <c r="G146">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="H146" s="2">
         <v>45211</v>
       </c>
       <c r="I146">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="J146" t="inlineStr">
         <is>
@@ -15189,13 +15189,13 @@
         <v>45165</v>
       </c>
       <c r="G147">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="H147" s="2">
         <v>45257</v>
       </c>
       <c r="I147">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="J147" t="inlineStr">
         <is>
@@ -15292,13 +15292,13 @@
         <v>45166</v>
       </c>
       <c r="G148">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="H148" s="2">
         <v>45258</v>
       </c>
       <c r="I148">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="J148" t="inlineStr">
         <is>
@@ -15395,13 +15395,13 @@
         <v>45093</v>
       </c>
       <c r="G149">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="H149" s="2">
         <v>45185</v>
       </c>
       <c r="I149">
-        <v>-3</v>
+        <v>-4</v>
       </c>
       <c r="J149" t="inlineStr">
         <is>
@@ -15498,13 +15498,13 @@
         <v>45035</v>
       </c>
       <c r="G150">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="H150" s="2">
         <v>45218</v>
       </c>
       <c r="I150">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="J150" t="inlineStr">
         <is>
@@ -15601,13 +15601,13 @@
         <v>45174</v>
       </c>
       <c r="G151">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="H151" s="2">
         <v>45356</v>
       </c>
       <c r="I151">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="J151" t="inlineStr">
         <is>
@@ -15704,13 +15704,13 @@
         <v>45089</v>
       </c>
       <c r="G152">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="H152" s="2">
         <v>45272</v>
       </c>
       <c r="I152">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="J152" t="inlineStr">
         <is>
@@ -15807,13 +15807,13 @@
         <v>45124</v>
       </c>
       <c r="G153">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="H153" s="2">
         <v>45308</v>
       </c>
       <c r="I153">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="J153" t="inlineStr">
         <is>
@@ -15910,13 +15910,13 @@
         <v>45124</v>
       </c>
       <c r="G154">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="H154" s="2">
         <v>45308</v>
       </c>
       <c r="I154">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="J154" t="inlineStr">
         <is>
@@ -16013,13 +16013,13 @@
         <v>45026</v>
       </c>
       <c r="G155">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="H155" s="2">
         <v>45209</v>
       </c>
       <c r="I155">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="J155" t="inlineStr">
         <is>
@@ -16116,13 +16116,13 @@
         <v>45026</v>
       </c>
       <c r="G156">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="H156" s="2">
         <v>45209</v>
       </c>
       <c r="I156">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="J156" t="inlineStr">
         <is>
@@ -16219,13 +16219,13 @@
         <v>45026</v>
       </c>
       <c r="G157">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="H157" s="2">
         <v>45209</v>
       </c>
       <c r="I157">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="J157" t="inlineStr">
         <is>
@@ -16322,13 +16322,13 @@
         <v>45026</v>
       </c>
       <c r="G158">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="H158" s="2">
         <v>45209</v>
       </c>
       <c r="I158">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="J158" t="inlineStr">
         <is>
@@ -16425,13 +16425,13 @@
         <v>45156</v>
       </c>
       <c r="G159">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="H159" s="2">
         <v>45247</v>
       </c>
       <c r="I159">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="J159" t="inlineStr">
         <is>
@@ -16528,13 +16528,13 @@
         <v>45153</v>
       </c>
       <c r="G160">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="H160" s="2">
         <v>45245</v>
       </c>
       <c r="I160">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="J160" t="inlineStr">
         <is>
@@ -16631,13 +16631,13 @@
         <v>45135</v>
       </c>
       <c r="G161">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="H161" s="2">
         <v>45319</v>
       </c>
       <c r="I161">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="J161" t="inlineStr">
         <is>
@@ -16734,13 +16734,13 @@
         <v>45091</v>
       </c>
       <c r="G162">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="H162" s="2">
         <v>45274</v>
       </c>
       <c r="I162">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="J162" t="inlineStr">
         <is>
@@ -16832,13 +16832,13 @@
         <v>45091</v>
       </c>
       <c r="G163">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="H163" s="2">
         <v>45274</v>
       </c>
       <c r="I163">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="J163" t="inlineStr">
         <is>
@@ -16930,13 +16930,13 @@
         <v>45138</v>
       </c>
       <c r="G164">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="H164" s="2">
         <v>45322</v>
       </c>
       <c r="I164">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="J164" t="inlineStr">
         <is>
@@ -17033,13 +17033,13 @@
         <v>45138</v>
       </c>
       <c r="G165">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="H165" s="2">
         <v>45322</v>
       </c>
       <c r="I165">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="J165" t="inlineStr">
         <is>
@@ -17136,13 +17136,13 @@
         <v>45085</v>
       </c>
       <c r="G166">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="H166" s="2">
         <v>45268</v>
       </c>
       <c r="I166">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="J166" t="inlineStr">
         <is>
@@ -17239,13 +17239,13 @@
         <v>45085</v>
       </c>
       <c r="G167">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="H167" s="2">
         <v>45268</v>
       </c>
       <c r="I167">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="J167" t="inlineStr">
         <is>
@@ -17342,7 +17342,7 @@
         <v>45326</v>
       </c>
       <c r="I168">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="J168" t="inlineStr">
         <is>
@@ -17439,13 +17439,13 @@
         <v>45173</v>
       </c>
       <c r="G169">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H169" s="2">
         <v>45355</v>
       </c>
       <c r="I169">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="J169" t="inlineStr">
         <is>
@@ -17542,13 +17542,13 @@
         <v>45056</v>
       </c>
       <c r="G170">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="H170" s="2">
         <v>45240</v>
       </c>
       <c r="I170">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="J170" t="inlineStr">
         <is>
@@ -17645,7 +17645,7 @@
         <v>45238</v>
       </c>
       <c r="I171">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="J171" t="inlineStr">
         <is>
@@ -17742,13 +17742,13 @@
         <v>45141</v>
       </c>
       <c r="G172">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="H172" s="2">
         <v>45325</v>
       </c>
       <c r="I172">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="J172" t="inlineStr">
         <is>
@@ -17845,13 +17845,13 @@
         <v>45037</v>
       </c>
       <c r="G173">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="H173" s="2">
         <v>45220</v>
       </c>
       <c r="I173">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="J173" t="inlineStr">
         <is>
@@ -17948,13 +17948,13 @@
         <v>45171</v>
       </c>
       <c r="G174">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="H174" s="2">
         <v>45262</v>
       </c>
       <c r="I174">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="J174" t="inlineStr">
         <is>
@@ -18051,13 +18051,13 @@
         <v>45105</v>
       </c>
       <c r="G175">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="H175" s="2">
         <v>45197</v>
       </c>
       <c r="I175">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="J175" t="inlineStr">
         <is>
@@ -18154,13 +18154,13 @@
         <v>45162</v>
       </c>
       <c r="G176">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="H176" s="2">
         <v>45254</v>
       </c>
       <c r="I176">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="J176" t="inlineStr">
         <is>
@@ -18257,13 +18257,13 @@
         <v>45061</v>
       </c>
       <c r="G177">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="H177" s="2">
         <v>45245</v>
       </c>
       <c r="I177">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="J177" t="inlineStr">
         <is>
@@ -18360,13 +18360,13 @@
         <v>45120</v>
       </c>
       <c r="G178">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="H178" s="2">
         <v>45212</v>
       </c>
       <c r="I178">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="J178" t="inlineStr">
         <is>
@@ -18463,7 +18463,7 @@
         <v>45191</v>
       </c>
       <c r="I179">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="J179" t="inlineStr">
         <is>
@@ -18560,13 +18560,13 @@
         <v>45088</v>
       </c>
       <c r="G180">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="H180" s="2">
         <v>45271</v>
       </c>
       <c r="I180">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="J180" t="inlineStr">
         <is>
@@ -18663,13 +18663,13 @@
         <v>45100</v>
       </c>
       <c r="G181">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="H181" s="2">
         <v>45192</v>
       </c>
       <c r="I181">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="J181" t="inlineStr">
         <is>
@@ -18756,13 +18756,13 @@
         <v>45131</v>
       </c>
       <c r="G182">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="H182" s="2">
         <v>45223</v>
       </c>
       <c r="I182">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="J182" t="inlineStr">
         <is>
@@ -18854,13 +18854,13 @@
         <v>45136</v>
       </c>
       <c r="G183">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="H183" s="2">
         <v>45228</v>
       </c>
       <c r="I183">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="J183" t="inlineStr">
         <is>
@@ -18952,13 +18952,13 @@
         <v>45150</v>
       </c>
       <c r="G184">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="H184" s="2">
         <v>45242</v>
       </c>
       <c r="I184">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="J184" t="inlineStr">
         <is>
@@ -19050,13 +19050,13 @@
         <v>45118</v>
       </c>
       <c r="G185">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="H185" s="2">
         <v>45210</v>
       </c>
       <c r="I185">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="J185" t="inlineStr">
         <is>
@@ -19148,13 +19148,13 @@
         <v>45129</v>
       </c>
       <c r="G186">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="H186" s="2">
         <v>45221</v>
       </c>
       <c r="I186">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="J186" t="inlineStr">
         <is>
@@ -19246,13 +19246,13 @@
         <v>45097</v>
       </c>
       <c r="G187">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="H187" s="2">
         <v>45189</v>
       </c>
       <c r="I187">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J187" t="inlineStr">
         <is>
@@ -19339,13 +19339,13 @@
         <v>45101</v>
       </c>
       <c r="G188">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="H188" s="2">
         <v>45193</v>
       </c>
       <c r="I188">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="J188" t="inlineStr">
         <is>
@@ -19432,13 +19432,13 @@
         <v>45165</v>
       </c>
       <c r="G189">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="H189" s="2">
         <v>45257</v>
       </c>
       <c r="I189">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="J189" t="inlineStr">
         <is>
@@ -19530,7 +19530,7 @@
         <v>45202</v>
       </c>
       <c r="I190">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="J190" t="inlineStr">
         <is>
@@ -19627,13 +19627,13 @@
         <v>45081</v>
       </c>
       <c r="G191">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="H191" s="2">
         <v>45264</v>
       </c>
       <c r="I191">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="J191" t="inlineStr">
         <is>
@@ -19730,13 +19730,13 @@
         <v>45081</v>
       </c>
       <c r="G192">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="H192" s="2">
         <v>45264</v>
       </c>
       <c r="I192">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="J192" t="inlineStr">
         <is>
@@ -19833,7 +19833,7 @@
         <v>45319</v>
       </c>
       <c r="I193">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="J193" t="inlineStr">
         <is>
@@ -19930,7 +19930,7 @@
         <v>45319</v>
       </c>
       <c r="I194">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="J194" t="inlineStr">
         <is>
@@ -20022,13 +20022,13 @@
         <v>45046</v>
       </c>
       <c r="G195">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="H195" s="2">
         <v>45230</v>
       </c>
       <c r="I195">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="J195" t="inlineStr">
         <is>
@@ -20125,13 +20125,13 @@
         <v>45046</v>
       </c>
       <c r="G196">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="H196" s="2">
         <v>45230</v>
       </c>
       <c r="I196">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="J196" t="inlineStr">
         <is>
@@ -20228,13 +20228,13 @@
         <v>45031</v>
       </c>
       <c r="G197">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="H197" s="2">
         <v>45214</v>
       </c>
       <c r="I197">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="J197" t="inlineStr">
         <is>
@@ -20331,13 +20331,13 @@
         <v>45031</v>
       </c>
       <c r="G198">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="H198" s="2">
         <v>45214</v>
       </c>
       <c r="I198">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="J198" t="inlineStr">
         <is>
@@ -20434,13 +20434,13 @@
         <v>45031</v>
       </c>
       <c r="G199">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="H199" s="2">
         <v>45214</v>
       </c>
       <c r="I199">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="J199" t="inlineStr">
         <is>
@@ -20537,13 +20537,13 @@
         <v>45031</v>
       </c>
       <c r="G200">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="H200" s="2">
         <v>45214</v>
       </c>
       <c r="I200">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="J200" t="inlineStr">
         <is>
@@ -20640,13 +20640,13 @@
         <v>45067</v>
       </c>
       <c r="G201">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="H201" s="2">
         <v>45251</v>
       </c>
       <c r="I201">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="J201" t="inlineStr">
         <is>
@@ -20743,13 +20743,13 @@
         <v>45067</v>
       </c>
       <c r="G202">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="H202" s="2">
         <v>45251</v>
       </c>
       <c r="I202">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="J202" t="inlineStr">
         <is>
@@ -20846,13 +20846,13 @@
         <v>45067</v>
       </c>
       <c r="G203">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="H203" s="2">
         <v>45251</v>
       </c>
       <c r="I203">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="J203" t="inlineStr">
         <is>
@@ -20949,13 +20949,13 @@
         <v>45067</v>
       </c>
       <c r="G204">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="H204" s="2">
         <v>45251</v>
       </c>
       <c r="I204">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="J204" t="inlineStr">
         <is>
@@ -21052,13 +21052,13 @@
         <v>45178</v>
       </c>
       <c r="G205">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="H205" s="2">
         <v>45269</v>
       </c>
       <c r="I205">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="J205" t="inlineStr">
         <is>
@@ -21155,7 +21155,7 @@
         <v>45252</v>
       </c>
       <c r="I206">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="J206" t="inlineStr">
         <is>
@@ -21252,13 +21252,13 @@
         <v>45087</v>
       </c>
       <c r="G207">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="H207" s="2">
         <v>45270</v>
       </c>
       <c r="I207">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="J207" t="inlineStr">
         <is>
@@ -21355,13 +21355,13 @@
         <v>45099</v>
       </c>
       <c r="G208">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="H208" s="2">
         <v>45282</v>
       </c>
       <c r="I208">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="J208" t="inlineStr">
         <is>
@@ -21458,13 +21458,13 @@
         <v>45175</v>
       </c>
       <c r="G209">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="H209" s="2">
         <v>45356</v>
       </c>
       <c r="I209">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="J209" t="inlineStr">
         <is>
@@ -21561,13 +21561,13 @@
         <v>45175</v>
       </c>
       <c r="G210">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="H210" s="2">
         <v>45356</v>
       </c>
       <c r="I210">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="J210" t="inlineStr">
         <is>
@@ -21664,13 +21664,13 @@
         <v>45166</v>
       </c>
       <c r="G211">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="H211" s="2">
         <v>45350</v>
       </c>
       <c r="I211">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="J211" t="inlineStr">
         <is>
@@ -21767,13 +21767,13 @@
         <v>45166</v>
       </c>
       <c r="G212">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="H212" s="2">
         <v>45350</v>
       </c>
       <c r="I212">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="J212" t="inlineStr">
         <is>
@@ -21870,13 +21870,13 @@
         <v>45090</v>
       </c>
       <c r="G213">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="H213" s="2">
         <v>45273</v>
       </c>
       <c r="I213">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="J213" t="inlineStr">
         <is>
@@ -21973,13 +21973,13 @@
         <v>45106</v>
       </c>
       <c r="G214">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="H214" s="2">
         <v>45289</v>
       </c>
       <c r="I214">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="J214" t="inlineStr">
         <is>
@@ -22076,13 +22076,13 @@
         <v>45134</v>
       </c>
       <c r="G215">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="H215" s="2">
         <v>45226</v>
       </c>
       <c r="I215">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="J215" t="inlineStr">
         <is>
@@ -22179,13 +22179,13 @@
         <v>45132</v>
       </c>
       <c r="G216">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="H216" s="2">
         <v>45224</v>
       </c>
       <c r="I216">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="J216" t="inlineStr">
         <is>
@@ -22282,13 +22282,13 @@
         <v>45150</v>
       </c>
       <c r="G217">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="H217" s="2">
         <v>45242</v>
       </c>
       <c r="I217">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="J217" t="inlineStr">
         <is>
@@ -22385,13 +22385,13 @@
         <v>45095</v>
       </c>
       <c r="G218">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="H218" s="2">
         <v>45187</v>
       </c>
       <c r="I218">
-        <v>-1</v>
+        <v>-2</v>
       </c>
       <c r="J218" t="inlineStr">
         <is>
@@ -22483,13 +22483,13 @@
         <v>45182</v>
       </c>
       <c r="G219">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="H219" s="2">
         <v>45273</v>
       </c>
       <c r="I219">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="J219" t="inlineStr">
         <is>
@@ -22586,7 +22586,7 @@
         <v>45196</v>
       </c>
       <c r="I220">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="J220" t="inlineStr">
         <is>
@@ -22683,13 +22683,13 @@
         <v>45108</v>
       </c>
       <c r="G221">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="H221" s="2">
         <v>45200</v>
       </c>
       <c r="I221">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="J221" t="inlineStr">
         <is>
@@ -22786,13 +22786,13 @@
         <v>45135</v>
       </c>
       <c r="G222">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="H222" s="2">
         <v>45227</v>
       </c>
       <c r="I222">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="J222" t="inlineStr">
         <is>
@@ -22889,13 +22889,13 @@
         <v>45148</v>
       </c>
       <c r="G223">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="H223" s="2">
         <v>45240</v>
       </c>
       <c r="I223">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="J223" t="inlineStr">
         <is>
@@ -22987,13 +22987,13 @@
         <v>45100</v>
       </c>
       <c r="G224">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="H224" s="2">
         <v>45192</v>
       </c>
       <c r="I224">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="J224" t="inlineStr">
         <is>
@@ -23085,13 +23085,13 @@
         <v>45136</v>
       </c>
       <c r="G225">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="H225" s="2">
         <v>45320</v>
       </c>
       <c r="I225">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="J225" t="inlineStr">
         <is>
@@ -23188,13 +23188,13 @@
         <v>45136</v>
       </c>
       <c r="G226">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="H226" s="2">
         <v>45320</v>
       </c>
       <c r="I226">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="J226" t="inlineStr">
         <is>
@@ -23291,13 +23291,13 @@
         <v>45094</v>
       </c>
       <c r="G227">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="H227" s="2">
         <v>45277</v>
       </c>
       <c r="I227">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="J227" t="inlineStr">
         <is>
@@ -23394,13 +23394,13 @@
         <v>45081</v>
       </c>
       <c r="G228">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="H228" s="2">
         <v>45264</v>
       </c>
       <c r="I228">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="J228" t="inlineStr">
         <is>
@@ -23497,13 +23497,13 @@
         <v>45099</v>
       </c>
       <c r="G229">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="H229" s="2">
         <v>45282</v>
       </c>
       <c r="I229">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="J229" t="inlineStr">
         <is>
@@ -23600,13 +23600,13 @@
         <v>45018</v>
       </c>
       <c r="G230">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="H230" s="2">
         <v>45201</v>
       </c>
       <c r="I230">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="J230" t="inlineStr">
         <is>
@@ -23703,13 +23703,13 @@
         <v>45031</v>
       </c>
       <c r="G231">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="H231" s="2">
         <v>45214</v>
       </c>
       <c r="I231">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="J231" t="inlineStr">
         <is>
@@ -23806,7 +23806,7 @@
         <v>45294</v>
       </c>
       <c r="I232">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="J232" t="inlineStr">
         <is>
@@ -23903,13 +23903,13 @@
         <v>45079</v>
       </c>
       <c r="G233">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="H233" s="2">
         <v>45262</v>
       </c>
       <c r="I233">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="J233" t="inlineStr">
         <is>
@@ -24006,7 +24006,7 @@
         <v>45199</v>
       </c>
       <c r="I234">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="J234" t="inlineStr">
         <is>
@@ -24103,13 +24103,13 @@
         <v>45021</v>
       </c>
       <c r="G235">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="H235" s="2">
         <v>45204</v>
       </c>
       <c r="I235">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="J235" t="inlineStr">
         <is>
@@ -24206,13 +24206,13 @@
         <v>45021</v>
       </c>
       <c r="G236">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="H236" s="2">
         <v>45204</v>
       </c>
       <c r="I236">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="J236" t="inlineStr">
         <is>
@@ -24309,13 +24309,13 @@
         <v>45080</v>
       </c>
       <c r="G237">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="H237" s="2">
         <v>45263</v>
       </c>
       <c r="I237">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="J237" t="inlineStr">
         <is>
@@ -24412,13 +24412,13 @@
         <v>45046</v>
       </c>
       <c r="G238">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="H238" s="2">
         <v>45229</v>
       </c>
       <c r="I238">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="J238" t="inlineStr">
         <is>
@@ -24515,13 +24515,13 @@
         <v>45112</v>
       </c>
       <c r="G239">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="H239" s="2">
         <v>45204</v>
       </c>
       <c r="I239">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="J239" t="inlineStr">
         <is>
@@ -24609,13 +24609,13 @@
         <v>45112</v>
       </c>
       <c r="G240">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="H240" s="2">
         <v>45204</v>
       </c>
       <c r="I240">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="J240" t="inlineStr">
         <is>
@@ -24703,13 +24703,13 @@
         <v>45016</v>
       </c>
       <c r="G241">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="H241" s="2">
         <v>45199</v>
       </c>
       <c r="I241">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="J241" t="inlineStr">
         <is>
@@ -24806,13 +24806,13 @@
         <v>45070</v>
       </c>
       <c r="G242">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="H242" s="2">
         <v>45254</v>
       </c>
       <c r="I242">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="J242" t="inlineStr">
         <is>
@@ -24909,13 +24909,13 @@
         <v>45168</v>
       </c>
       <c r="G243">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="H243" s="2">
         <v>45260</v>
       </c>
       <c r="I243">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="J243" t="inlineStr">
         <is>
@@ -25012,13 +25012,13 @@
         <v>45027</v>
       </c>
       <c r="G244">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="H244" s="2">
         <v>45210</v>
       </c>
       <c r="I244">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="J244" t="inlineStr">
         <is>
@@ -25115,13 +25115,13 @@
         <v>45077</v>
       </c>
       <c r="G245">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="H245" s="2">
         <v>45260</v>
       </c>
       <c r="I245">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="J245" t="inlineStr">
         <is>
@@ -25218,13 +25218,13 @@
         <v>45100</v>
       </c>
       <c r="G246">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="H246" s="2">
         <v>45283</v>
       </c>
       <c r="I246">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="J246" t="inlineStr">
         <is>
@@ -25321,7 +25321,7 @@
         <v>45281</v>
       </c>
       <c r="I247">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="J247" t="inlineStr">
         <is>
@@ -25418,13 +25418,13 @@
         <v>45044</v>
       </c>
       <c r="G248">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="H248" s="2">
         <v>45227</v>
       </c>
       <c r="I248">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="J248" t="inlineStr">
         <is>
@@ -25521,13 +25521,13 @@
         <v>45101</v>
       </c>
       <c r="G249">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="H249" s="2">
         <v>45283</v>
       </c>
       <c r="I249">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="J249" t="inlineStr">
         <is>
@@ -25624,13 +25624,13 @@
         <v>45134</v>
       </c>
       <c r="G250">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="H250" s="2">
         <v>45226</v>
       </c>
       <c r="I250">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="J250" t="inlineStr">
         <is>
@@ -25727,13 +25727,13 @@
         <v>45158</v>
       </c>
       <c r="G251">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="H251" s="2">
         <v>45250</v>
       </c>
       <c r="I251">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="J251" t="inlineStr">
         <is>
@@ -25830,13 +25830,13 @@
         <v>45108</v>
       </c>
       <c r="G252">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="H252" s="2">
         <v>45200</v>
       </c>
       <c r="I252">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="J252" t="inlineStr">
         <is>
@@ -25933,7 +25933,7 @@
         <v>45317</v>
       </c>
       <c r="I253">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="J253" t="inlineStr">
         <is>
@@ -26030,13 +26030,13 @@
         <v>45039</v>
       </c>
       <c r="G254">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="H254" s="2">
         <v>45222</v>
       </c>
       <c r="I254">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="J254" t="inlineStr">
         <is>
@@ -26128,13 +26128,13 @@
         <v>45129</v>
       </c>
       <c r="G255">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="H255" s="2">
         <v>45221</v>
       </c>
       <c r="I255">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="J255" t="inlineStr">
         <is>
@@ -26231,13 +26231,13 @@
         <v>45157</v>
       </c>
       <c r="G256">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="H256" s="2">
         <v>45341</v>
       </c>
       <c r="I256">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="J256" t="inlineStr">
         <is>
@@ -26334,13 +26334,13 @@
         <v>45063</v>
       </c>
       <c r="G257">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="H257" s="2">
         <v>45247</v>
       </c>
       <c r="I257">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="J257" t="inlineStr">
         <is>
@@ -26437,7 +26437,7 @@
         <v>45254</v>
       </c>
       <c r="I258">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="J258" t="inlineStr">
         <is>
@@ -26534,7 +26534,7 @@
         <v>45486</v>
       </c>
       <c r="I259">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="J259" t="inlineStr">
         <is>
@@ -26626,13 +26626,13 @@
         <v>45073</v>
       </c>
       <c r="G260">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="H260" s="2">
         <v>45439</v>
       </c>
       <c r="I260">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="J260" t="inlineStr">
         <is>
@@ -26724,7 +26724,7 @@
         <v>45323</v>
       </c>
       <c r="I261">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="J261" t="inlineStr">
         <is>
@@ -26816,7 +26816,7 @@
         <v>45303</v>
       </c>
       <c r="I262">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="J262" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
Bond dates update Thu Sep 21 23:11:20 UTC 2023
</commit_message>
<xml_diff>
--- a/Data/obligacje_screener.xlsx
+++ b/Data/obligacje_screener.xlsx
@@ -512,7 +512,7 @@
         <v>45340</v>
       </c>
       <c r="I2">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="J2" t="inlineStr">
         <is>
@@ -600,13 +600,13 @@
         <v>45121</v>
       </c>
       <c r="G3">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="H3" s="2">
         <v>45305</v>
       </c>
       <c r="I3">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="J3" t="inlineStr">
         <is>
@@ -703,13 +703,13 @@
         <v>45039</v>
       </c>
       <c r="G4">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="H4" s="2">
         <v>45222</v>
       </c>
       <c r="I4">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="J4" t="inlineStr">
         <is>
@@ -806,13 +806,13 @@
         <v>45039</v>
       </c>
       <c r="G5">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="H5" s="2">
         <v>45222</v>
       </c>
       <c r="I5">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="J5" t="inlineStr">
         <is>
@@ -909,13 +909,13 @@
         <v>45129</v>
       </c>
       <c r="G6">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="H6" s="2">
         <v>45221</v>
       </c>
       <c r="I6">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="J6" t="inlineStr">
         <is>
@@ -1012,13 +1012,13 @@
         <v>45162</v>
       </c>
       <c r="G7">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="H7" s="2">
         <v>45254</v>
       </c>
       <c r="I7">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="J7" t="inlineStr">
         <is>
@@ -1110,13 +1110,13 @@
         <v>45156</v>
       </c>
       <c r="G8">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="H8" s="2">
         <v>45248</v>
       </c>
       <c r="I8">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="J8" t="inlineStr">
         <is>
@@ -1213,13 +1213,13 @@
         <v>45141</v>
       </c>
       <c r="G9">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="H9" s="2">
         <v>45233</v>
       </c>
       <c r="I9">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="J9" t="inlineStr">
         <is>
@@ -1316,13 +1316,13 @@
         <v>45062</v>
       </c>
       <c r="G10">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="H10" s="2">
         <v>45246</v>
       </c>
       <c r="I10">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="J10" t="inlineStr">
         <is>
@@ -1419,7 +1419,7 @@
         <v>45286</v>
       </c>
       <c r="I11">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="J11" t="inlineStr">
         <is>
@@ -1516,13 +1516,13 @@
         <v>45011</v>
       </c>
       <c r="G12">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="H12" s="2">
         <v>45195</v>
       </c>
       <c r="I12">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="J12" t="inlineStr">
         <is>
@@ -1614,13 +1614,13 @@
         <v>45036</v>
       </c>
       <c r="G13">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="H13" s="2">
         <v>45219</v>
       </c>
       <c r="I13">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="J13" t="inlineStr">
         <is>
@@ -1717,13 +1717,13 @@
         <v>45036</v>
       </c>
       <c r="G14">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="H14" s="2">
         <v>45219</v>
       </c>
       <c r="I14">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="J14" t="inlineStr">
         <is>
@@ -1820,13 +1820,13 @@
         <v>45106</v>
       </c>
       <c r="G15">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="H15" s="2">
         <v>45289</v>
       </c>
       <c r="I15">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="J15" t="inlineStr">
         <is>
@@ -1923,13 +1923,13 @@
         <v>45094</v>
       </c>
       <c r="G16">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="H16" s="2">
         <v>45186</v>
       </c>
       <c r="I16">
-        <v>-3</v>
+        <v>-4</v>
       </c>
       <c r="J16" t="inlineStr">
         <is>
@@ -2026,13 +2026,13 @@
         <v>45094</v>
       </c>
       <c r="G17">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="H17" s="2">
         <v>45186</v>
       </c>
       <c r="I17">
-        <v>-3</v>
+        <v>-4</v>
       </c>
       <c r="J17" t="inlineStr">
         <is>
@@ -2129,13 +2129,13 @@
         <v>45132</v>
       </c>
       <c r="G18">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="H18" s="2">
         <v>45224</v>
       </c>
       <c r="I18">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="J18" t="inlineStr">
         <is>
@@ -2232,13 +2232,13 @@
         <v>45137</v>
       </c>
       <c r="G19">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="H19" s="2">
         <v>45229</v>
       </c>
       <c r="I19">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="J19" t="inlineStr">
         <is>
@@ -2330,13 +2330,13 @@
         <v>45183</v>
       </c>
       <c r="G20">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="H20" s="2">
         <v>45274</v>
       </c>
       <c r="I20">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="J20" t="inlineStr">
         <is>
@@ -2433,13 +2433,13 @@
         <v>45093</v>
       </c>
       <c r="G21">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="H21" s="2">
         <v>45187</v>
       </c>
       <c r="I21">
-        <v>-2</v>
+        <v>-3</v>
       </c>
       <c r="J21" t="inlineStr">
         <is>
@@ -2536,13 +2536,13 @@
         <v>45096</v>
       </c>
       <c r="G22">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="H22" s="2">
         <v>45187</v>
       </c>
       <c r="I22">
-        <v>-2</v>
+        <v>-3</v>
       </c>
       <c r="J22" t="inlineStr">
         <is>
@@ -2639,7 +2639,7 @@
         <v>45245</v>
       </c>
       <c r="I23">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="J23" t="inlineStr">
         <is>
@@ -2736,7 +2736,7 @@
         <v>45245</v>
       </c>
       <c r="I24">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="J24" t="inlineStr">
         <is>
@@ -2833,13 +2833,13 @@
         <v>45021</v>
       </c>
       <c r="G25">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="H25" s="2">
         <v>45204</v>
       </c>
       <c r="I25">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="J25" t="inlineStr">
         <is>
@@ -2936,13 +2936,13 @@
         <v>45160</v>
       </c>
       <c r="G26">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="H26" s="2">
         <v>45344</v>
       </c>
       <c r="I26">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="J26" t="inlineStr">
         <is>
@@ -3039,13 +3039,13 @@
         <v>45118</v>
       </c>
       <c r="G27">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="H27" s="2">
         <v>45302</v>
       </c>
       <c r="I27">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="J27" t="inlineStr">
         <is>
@@ -3142,13 +3142,13 @@
         <v>45085</v>
       </c>
       <c r="G28">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="H28" s="2">
         <v>45268</v>
       </c>
       <c r="I28">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="J28" t="inlineStr">
         <is>
@@ -3245,13 +3245,13 @@
         <v>45183</v>
       </c>
       <c r="G29">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="H29" s="2">
         <v>45274</v>
       </c>
       <c r="I29">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="J29" t="inlineStr">
         <is>
@@ -3348,7 +3348,7 @@
         <v>45224</v>
       </c>
       <c r="I30">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="J30" t="inlineStr">
         <is>
@@ -3445,13 +3445,13 @@
         <v>45153</v>
       </c>
       <c r="G31">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="H31" s="2">
         <v>45245</v>
       </c>
       <c r="I31">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="J31" t="inlineStr">
         <is>
@@ -3548,13 +3548,13 @@
         <v>45155</v>
       </c>
       <c r="G32">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="H32" s="2">
         <v>45247</v>
       </c>
       <c r="I32">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="J32" t="inlineStr">
         <is>
@@ -3651,7 +3651,7 @@
         <v>45255</v>
       </c>
       <c r="I33">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="J33" t="inlineStr">
         <is>
@@ -3739,13 +3739,13 @@
         <v>45176</v>
       </c>
       <c r="G34">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="H34" s="2">
         <v>45267</v>
       </c>
       <c r="I34">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="J34" t="inlineStr">
         <is>
@@ -3842,13 +3842,13 @@
         <v>45130</v>
       </c>
       <c r="G35">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="H35" s="2">
         <v>45222</v>
       </c>
       <c r="I35">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="J35" t="inlineStr">
         <is>
@@ -3940,13 +3940,13 @@
         <v>45115</v>
       </c>
       <c r="G36">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="H36" s="2">
         <v>45207</v>
       </c>
       <c r="I36">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="J36" t="inlineStr">
         <is>
@@ -4043,13 +4043,13 @@
         <v>45097</v>
       </c>
       <c r="G37">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="H37" s="2">
         <v>45189</v>
       </c>
       <c r="I37">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="J37" t="inlineStr">
         <is>
@@ -4141,13 +4141,13 @@
         <v>45107</v>
       </c>
       <c r="G38">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="H38" s="2">
         <v>45290</v>
       </c>
       <c r="I38">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="J38" t="inlineStr">
         <is>
@@ -4244,13 +4244,13 @@
         <v>45063</v>
       </c>
       <c r="G39">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="H39" s="2">
         <v>45247</v>
       </c>
       <c r="I39">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="J39" t="inlineStr">
         <is>
@@ -4347,13 +4347,13 @@
         <v>45177</v>
       </c>
       <c r="G40">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="H40" s="2">
         <v>45359</v>
       </c>
       <c r="I40">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="J40" t="inlineStr">
         <is>
@@ -4450,13 +4450,13 @@
         <v>45107</v>
       </c>
       <c r="G41">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="H41" s="2">
         <v>45290</v>
       </c>
       <c r="I41">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="J41" t="inlineStr">
         <is>
@@ -4553,7 +4553,7 @@
         <v>45265</v>
       </c>
       <c r="I42">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="J42" t="inlineStr">
         <is>
@@ -4650,13 +4650,13 @@
         <v>45098</v>
       </c>
       <c r="G43">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="H43" s="2">
         <v>45281</v>
       </c>
       <c r="I43">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="J43" t="inlineStr">
         <is>
@@ -4753,13 +4753,13 @@
         <v>45099</v>
       </c>
       <c r="G44">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="H44" s="2">
         <v>45282</v>
       </c>
       <c r="I44">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="J44" t="inlineStr">
         <is>
@@ -4856,13 +4856,13 @@
         <v>45106</v>
       </c>
       <c r="G45">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="H45" s="2">
         <v>45289</v>
       </c>
       <c r="I45">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="J45" t="inlineStr">
         <is>
@@ -4959,13 +4959,13 @@
         <v>45106</v>
       </c>
       <c r="G46">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="H46" s="2">
         <v>45289</v>
       </c>
       <c r="I46">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="J46" t="inlineStr">
         <is>
@@ -5062,13 +5062,13 @@
         <v>45120</v>
       </c>
       <c r="G47">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="H47" s="2">
         <v>45304</v>
       </c>
       <c r="I47">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="J47" t="inlineStr">
         <is>
@@ -5165,13 +5165,13 @@
         <v>45118</v>
       </c>
       <c r="G48">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="H48" s="2">
         <v>45302</v>
       </c>
       <c r="I48">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="J48" t="inlineStr">
         <is>
@@ -5268,13 +5268,13 @@
         <v>45152</v>
       </c>
       <c r="G49">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="H49" s="2">
         <v>45336</v>
       </c>
       <c r="I49">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="J49" t="inlineStr">
         <is>
@@ -5371,13 +5371,13 @@
         <v>45042</v>
       </c>
       <c r="G50">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="H50" s="2">
         <v>45225</v>
       </c>
       <c r="I50">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="J50" t="inlineStr">
         <is>
@@ -5474,13 +5474,13 @@
         <v>45122</v>
       </c>
       <c r="G51">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="H51" s="2">
         <v>45306</v>
       </c>
       <c r="I51">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="J51" t="inlineStr">
         <is>
@@ -5577,13 +5577,13 @@
         <v>45139</v>
       </c>
       <c r="G52">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="H52" s="2">
         <v>45323</v>
       </c>
       <c r="I52">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="J52" t="inlineStr">
         <is>
@@ -5671,13 +5671,13 @@
         <v>45099</v>
       </c>
       <c r="G53">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="H53" s="2">
         <v>45282</v>
       </c>
       <c r="I53">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="J53" t="inlineStr">
         <is>
@@ -5774,7 +5774,7 @@
         <v>45196</v>
       </c>
       <c r="I54">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="J54" t="inlineStr">
         <is>
@@ -5871,13 +5871,13 @@
         <v>45044</v>
       </c>
       <c r="G55">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="H55" s="2">
         <v>45227</v>
       </c>
       <c r="I55">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="J55" t="inlineStr">
         <is>
@@ -5974,13 +5974,13 @@
         <v>45151</v>
       </c>
       <c r="G56">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="H56" s="2">
         <v>45243</v>
       </c>
       <c r="I56">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="J56" t="inlineStr">
         <is>
@@ -6072,7 +6072,7 @@
         <v>45196</v>
       </c>
       <c r="I57">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="J57" t="inlineStr">
         <is>
@@ -6169,13 +6169,13 @@
         <v>45069</v>
       </c>
       <c r="G58">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="H58" s="2">
         <v>45253</v>
       </c>
       <c r="I58">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="J58" t="inlineStr">
         <is>
@@ -6272,13 +6272,13 @@
         <v>45099</v>
       </c>
       <c r="G59">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="H59" s="2">
         <v>45191</v>
       </c>
       <c r="I59">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J59" t="inlineStr">
         <is>
@@ -6370,13 +6370,13 @@
         <v>45113</v>
       </c>
       <c r="G60">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="H60" s="2">
         <v>45205</v>
       </c>
       <c r="I60">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="J60" t="inlineStr">
         <is>
@@ -6473,13 +6473,13 @@
         <v>45127</v>
       </c>
       <c r="G61">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="H61" s="2">
         <v>45219</v>
       </c>
       <c r="I61">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="J61" t="inlineStr">
         <is>
@@ -6576,13 +6576,13 @@
         <v>45058</v>
       </c>
       <c r="G62">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="H62" s="2">
         <v>45242</v>
       </c>
       <c r="I62">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="J62" t="inlineStr">
         <is>
@@ -6679,13 +6679,13 @@
         <v>45010</v>
       </c>
       <c r="G63">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="H63" s="2">
         <v>45194</v>
       </c>
       <c r="I63">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="J63" t="inlineStr">
         <is>
@@ -6777,13 +6777,13 @@
         <v>45025</v>
       </c>
       <c r="G64">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="H64" s="2">
         <v>45208</v>
       </c>
       <c r="I64">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="J64" t="inlineStr">
         <is>
@@ -6880,13 +6880,13 @@
         <v>45025</v>
       </c>
       <c r="G65">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="H65" s="2">
         <v>45208</v>
       </c>
       <c r="I65">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="J65" t="inlineStr">
         <is>
@@ -6983,13 +6983,13 @@
         <v>45089</v>
       </c>
       <c r="G66">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="H66" s="2">
         <v>45272</v>
       </c>
       <c r="I66">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="J66" t="inlineStr">
         <is>
@@ -7086,13 +7086,13 @@
         <v>45178</v>
       </c>
       <c r="G67">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="H67" s="2">
         <v>45269</v>
       </c>
       <c r="I67">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="J67" t="inlineStr">
         <is>
@@ -7184,13 +7184,13 @@
         <v>45104</v>
       </c>
       <c r="G68">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="H68" s="2">
         <v>45196</v>
       </c>
       <c r="I68">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="J68" t="inlineStr">
         <is>
@@ -7287,13 +7287,13 @@
         <v>45149</v>
       </c>
       <c r="G69">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="H69" s="2">
         <v>45241</v>
       </c>
       <c r="I69">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="J69" t="inlineStr">
         <is>
@@ -7390,7 +7390,7 @@
         <v>45205</v>
       </c>
       <c r="I70">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="J70" t="inlineStr">
         <is>
@@ -7487,13 +7487,13 @@
         <v>45114</v>
       </c>
       <c r="G71">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="H71" s="2">
         <v>45205</v>
       </c>
       <c r="I71">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="J71" t="inlineStr">
         <is>
@@ -7590,13 +7590,13 @@
         <v>45115</v>
       </c>
       <c r="G72">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="H72" s="2">
         <v>45207</v>
       </c>
       <c r="I72">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="J72" t="inlineStr">
         <is>
@@ -7693,13 +7693,13 @@
         <v>45097</v>
       </c>
       <c r="G73">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="H73" s="2">
         <v>45189</v>
       </c>
       <c r="I73">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="J73" t="inlineStr">
         <is>
@@ -7791,13 +7791,13 @@
         <v>45038</v>
       </c>
       <c r="G74">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="H74" s="2">
         <v>45221</v>
       </c>
       <c r="I74">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="J74" t="inlineStr">
         <is>
@@ -7889,13 +7889,13 @@
         <v>45117</v>
       </c>
       <c r="G75">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="H75" s="2">
         <v>45301</v>
       </c>
       <c r="I75">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="J75" t="inlineStr">
         <is>
@@ -7992,13 +7992,13 @@
         <v>45160</v>
       </c>
       <c r="G76">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="H76" s="2">
         <v>45344</v>
       </c>
       <c r="I76">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="J76" t="inlineStr">
         <is>
@@ -8095,13 +8095,13 @@
         <v>45002</v>
       </c>
       <c r="G77">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="H77" s="2">
         <v>45186</v>
       </c>
       <c r="I77">
-        <v>-3</v>
+        <v>-4</v>
       </c>
       <c r="J77" t="inlineStr">
         <is>
@@ -8198,13 +8198,13 @@
         <v>45043</v>
       </c>
       <c r="G78">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="H78" s="2">
         <v>45226</v>
       </c>
       <c r="I78">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="J78" t="inlineStr">
         <is>
@@ -8301,13 +8301,13 @@
         <v>45079</v>
       </c>
       <c r="G79">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="H79" s="2">
         <v>45262</v>
       </c>
       <c r="I79">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="J79" t="inlineStr">
         <is>
@@ -8404,7 +8404,7 @@
         <v>45254</v>
       </c>
       <c r="I80">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="J80" t="inlineStr">
         <is>
@@ -8501,13 +8501,13 @@
         <v>45104</v>
       </c>
       <c r="G81">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="H81" s="2">
         <v>45287</v>
       </c>
       <c r="I81">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="J81" t="inlineStr">
         <is>
@@ -8604,7 +8604,7 @@
         <v>45288</v>
       </c>
       <c r="I82">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="J82" t="inlineStr">
         <is>
@@ -8696,13 +8696,13 @@
         <v>45175</v>
       </c>
       <c r="G83">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="H83" s="2">
         <v>45357</v>
       </c>
       <c r="I83">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="J83" t="inlineStr">
         <is>
@@ -8799,13 +8799,13 @@
         <v>45054</v>
       </c>
       <c r="G84">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="H84" s="2">
         <v>45238</v>
       </c>
       <c r="I84">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="J84" t="inlineStr">
         <is>
@@ -8902,13 +8902,13 @@
         <v>45056</v>
       </c>
       <c r="G85">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="H85" s="2">
         <v>45240</v>
       </c>
       <c r="I85">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="J85" t="inlineStr">
         <is>
@@ -9005,13 +9005,13 @@
         <v>45085</v>
       </c>
       <c r="G86">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="H86" s="2">
         <v>45268</v>
       </c>
       <c r="I86">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="J86" t="inlineStr">
         <is>
@@ -9108,7 +9108,7 @@
         <v>45194</v>
       </c>
       <c r="I87">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="J87" t="inlineStr">
         <is>
@@ -9195,13 +9195,13 @@
         <v>45103</v>
       </c>
       <c r="G88">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="H88" s="2">
         <v>45286</v>
       </c>
       <c r="I88">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="J88" t="inlineStr">
         <is>
@@ -9298,13 +9298,13 @@
         <v>45103</v>
       </c>
       <c r="G89">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="H89" s="2">
         <v>45286</v>
       </c>
       <c r="I89">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="J89" t="inlineStr">
         <is>
@@ -9401,13 +9401,13 @@
         <v>45008</v>
       </c>
       <c r="G90">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="H90" s="2">
         <v>45192</v>
       </c>
       <c r="I90">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="J90" t="inlineStr">
         <is>
@@ -9499,13 +9499,13 @@
         <v>45100</v>
       </c>
       <c r="G91">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="H91" s="2">
         <v>45287</v>
       </c>
       <c r="I91">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="J91" t="inlineStr">
         <is>
@@ -9602,13 +9602,13 @@
         <v>45003</v>
       </c>
       <c r="G92">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="H92" s="2">
         <v>45187</v>
       </c>
       <c r="I92">
-        <v>-2</v>
+        <v>-3</v>
       </c>
       <c r="J92" t="inlineStr">
         <is>
@@ -9705,13 +9705,13 @@
         <v>45104</v>
       </c>
       <c r="G93">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="H93" s="2">
         <v>45287</v>
       </c>
       <c r="I93">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="J93" t="inlineStr">
         <is>
@@ -9808,13 +9808,13 @@
         <v>45104</v>
       </c>
       <c r="G94">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="H94" s="2">
         <v>45287</v>
       </c>
       <c r="I94">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="J94" t="inlineStr">
         <is>
@@ -9911,13 +9911,13 @@
         <v>45049</v>
       </c>
       <c r="G95">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="H95" s="2">
         <v>45233</v>
       </c>
       <c r="I95">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="J95" t="inlineStr">
         <is>
@@ -10014,13 +10014,13 @@
         <v>45122</v>
       </c>
       <c r="G96">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="H96" s="2">
         <v>45306</v>
       </c>
       <c r="I96">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="J96" t="inlineStr">
         <is>
@@ -10112,13 +10112,13 @@
         <v>45141</v>
       </c>
       <c r="G97">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="H97" s="2">
         <v>45325</v>
       </c>
       <c r="I97">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="J97" t="inlineStr">
         <is>
@@ -10215,13 +10215,13 @@
         <v>45010</v>
       </c>
       <c r="G98">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="H98" s="2">
         <v>45194</v>
       </c>
       <c r="I98">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="J98" t="inlineStr">
         <is>
@@ -10313,13 +10313,13 @@
         <v>45093</v>
       </c>
       <c r="G99">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="H99" s="2">
         <v>45276</v>
       </c>
       <c r="I99">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="J99" t="inlineStr">
         <is>
@@ -10416,13 +10416,13 @@
         <v>45123</v>
       </c>
       <c r="G100">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="H100" s="2">
         <v>45307</v>
       </c>
       <c r="I100">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="J100" t="inlineStr">
         <is>
@@ -10519,13 +10519,13 @@
         <v>45014</v>
       </c>
       <c r="G101">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="H101" s="2">
         <v>45198</v>
       </c>
       <c r="I101">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="J101" t="inlineStr">
         <is>
@@ -10622,13 +10622,13 @@
         <v>45093</v>
       </c>
       <c r="G102">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="H102" s="2">
         <v>45276</v>
       </c>
       <c r="I102">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="J102" t="inlineStr">
         <is>
@@ -10725,13 +10725,13 @@
         <v>45122</v>
       </c>
       <c r="G103">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="H103" s="2">
         <v>45306</v>
       </c>
       <c r="I103">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="J103" t="inlineStr">
         <is>
@@ -10828,13 +10828,13 @@
         <v>45122</v>
       </c>
       <c r="G104">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="H104" s="2">
         <v>45306</v>
       </c>
       <c r="I104">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="J104" t="inlineStr">
         <is>
@@ -10926,13 +10926,13 @@
         <v>45050</v>
       </c>
       <c r="G105">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="H105" s="2">
         <v>45234</v>
       </c>
       <c r="I105">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="J105" t="inlineStr">
         <is>
@@ -11029,13 +11029,13 @@
         <v>45085</v>
       </c>
       <c r="G106">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="H106" s="2">
         <v>45268</v>
       </c>
       <c r="I106">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="J106" t="inlineStr">
         <is>
@@ -11132,13 +11132,13 @@
         <v>45093</v>
       </c>
       <c r="G107">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="H107" s="2">
         <v>45185</v>
       </c>
       <c r="I107">
-        <v>-4</v>
+        <v>-5</v>
       </c>
       <c r="J107" t="inlineStr">
         <is>
@@ -11230,13 +11230,13 @@
         <v>45093</v>
       </c>
       <c r="G108">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="H108" s="2">
         <v>45185</v>
       </c>
       <c r="I108">
-        <v>-4</v>
+        <v>-5</v>
       </c>
       <c r="J108" t="inlineStr">
         <is>
@@ -11328,13 +11328,13 @@
         <v>45093</v>
       </c>
       <c r="G109">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="H109" s="2">
         <v>45185</v>
       </c>
       <c r="I109">
-        <v>-4</v>
+        <v>-5</v>
       </c>
       <c r="J109" t="inlineStr">
         <is>
@@ -11431,13 +11431,13 @@
         <v>45148</v>
       </c>
       <c r="G110">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="H110" s="2">
         <v>45240</v>
       </c>
       <c r="I110">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="J110" t="inlineStr">
         <is>
@@ -11534,13 +11534,13 @@
         <v>45119</v>
       </c>
       <c r="G111">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="H111" s="2">
         <v>45211</v>
       </c>
       <c r="I111">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="J111" t="inlineStr">
         <is>
@@ -11637,13 +11637,13 @@
         <v>45172</v>
       </c>
       <c r="G112">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="H112" s="2">
         <v>45263</v>
       </c>
       <c r="I112">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="J112" t="inlineStr">
         <is>
@@ -11740,13 +11740,13 @@
         <v>45023</v>
       </c>
       <c r="G113">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="H113" s="2">
         <v>45206</v>
       </c>
       <c r="I113">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="J113" t="inlineStr">
         <is>
@@ -11843,13 +11843,13 @@
         <v>45111</v>
       </c>
       <c r="G114">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="H114" s="2">
         <v>45203</v>
       </c>
       <c r="I114">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="J114" t="inlineStr">
         <is>
@@ -11946,7 +11946,7 @@
         <v>45218</v>
       </c>
       <c r="I115">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="J115" t="inlineStr">
         <is>
@@ -12043,13 +12043,13 @@
         <v>45161</v>
       </c>
       <c r="G116">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="H116" s="2">
         <v>45253</v>
       </c>
       <c r="I116">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="J116" t="inlineStr">
         <is>
@@ -12146,13 +12146,13 @@
         <v>45115</v>
       </c>
       <c r="G117">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="H117" s="2">
         <v>45299</v>
       </c>
       <c r="I117">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="J117" t="inlineStr">
         <is>
@@ -12244,13 +12244,13 @@
         <v>45094</v>
       </c>
       <c r="G118">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="H118" s="2">
         <v>45277</v>
       </c>
       <c r="I118">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="J118" t="inlineStr">
         <is>
@@ -12347,13 +12347,13 @@
         <v>45104</v>
       </c>
       <c r="G119">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="H119" s="2">
         <v>45287</v>
       </c>
       <c r="I119">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="J119" t="inlineStr">
         <is>
@@ -12450,13 +12450,13 @@
         <v>45104</v>
       </c>
       <c r="G120">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="H120" s="2">
         <v>45287</v>
       </c>
       <c r="I120">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="J120" t="inlineStr">
         <is>
@@ -12553,13 +12553,13 @@
         <v>45104</v>
       </c>
       <c r="G121">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="H121" s="2">
         <v>45287</v>
       </c>
       <c r="I121">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="J121" t="inlineStr">
         <is>
@@ -12656,13 +12656,13 @@
         <v>45104</v>
       </c>
       <c r="G122">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="H122" s="2">
         <v>45287</v>
       </c>
       <c r="I122">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="J122" t="inlineStr">
         <is>
@@ -12759,13 +12759,13 @@
         <v>45107</v>
       </c>
       <c r="G123">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="H123" s="2">
         <v>45199</v>
       </c>
       <c r="I123">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="J123" t="inlineStr">
         <is>
@@ -12862,13 +12862,13 @@
         <v>45013</v>
       </c>
       <c r="G124">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="H124" s="2">
         <v>45197</v>
       </c>
       <c r="I124">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="J124" t="inlineStr">
         <is>
@@ -12965,13 +12965,13 @@
         <v>45121</v>
       </c>
       <c r="G125">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="H125" s="2">
         <v>45213</v>
       </c>
       <c r="I125">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="J125" t="inlineStr">
         <is>
@@ -13068,13 +13068,13 @@
         <v>45134</v>
       </c>
       <c r="G126">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="H126" s="2">
         <v>45226</v>
       </c>
       <c r="I126">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="J126" t="inlineStr">
         <is>
@@ -13171,7 +13171,7 @@
         <v>45212</v>
       </c>
       <c r="I127">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="J127" t="inlineStr">
         <is>
@@ -13268,13 +13268,13 @@
         <v>45126</v>
       </c>
       <c r="G128">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="H128" s="2">
         <v>45218</v>
       </c>
       <c r="I128">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="J128" t="inlineStr">
         <is>
@@ -13366,13 +13366,13 @@
         <v>45158</v>
       </c>
       <c r="G129">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="H129" s="2">
         <v>45250</v>
       </c>
       <c r="I129">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="J129" t="inlineStr">
         <is>
@@ -13469,13 +13469,13 @@
         <v>45171</v>
       </c>
       <c r="G130">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="H130" s="2">
         <v>45262</v>
       </c>
       <c r="I130">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="J130" t="inlineStr">
         <is>
@@ -13572,13 +13572,13 @@
         <v>45111</v>
       </c>
       <c r="G131">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="H131" s="2">
         <v>45203</v>
       </c>
       <c r="I131">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="J131" t="inlineStr">
         <is>
@@ -13675,13 +13675,13 @@
         <v>45144</v>
       </c>
       <c r="G132">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="H132" s="2">
         <v>45236</v>
       </c>
       <c r="I132">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="J132" t="inlineStr">
         <is>
@@ -13778,13 +13778,13 @@
         <v>45156</v>
       </c>
       <c r="G133">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="H133" s="2">
         <v>45248</v>
       </c>
       <c r="I133">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="J133" t="inlineStr">
         <is>
@@ -13876,13 +13876,13 @@
         <v>45146</v>
       </c>
       <c r="G134">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="H134" s="2">
         <v>45238</v>
       </c>
       <c r="I134">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="J134" t="inlineStr">
         <is>
@@ -13979,13 +13979,13 @@
         <v>45140</v>
       </c>
       <c r="G135">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="H135" s="2">
         <v>45232</v>
       </c>
       <c r="I135">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="J135" t="inlineStr">
         <is>
@@ -14082,13 +14082,13 @@
         <v>45104</v>
       </c>
       <c r="G136">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="H136" s="2">
         <v>45196</v>
       </c>
       <c r="I136">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="J136" t="inlineStr">
         <is>
@@ -14185,13 +14185,13 @@
         <v>45105</v>
       </c>
       <c r="G137">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="H137" s="2">
         <v>45197</v>
       </c>
       <c r="I137">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="J137" t="inlineStr">
         <is>
@@ -14288,13 +14288,13 @@
         <v>45179</v>
       </c>
       <c r="G138">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="H138" s="2">
         <v>45270</v>
       </c>
       <c r="I138">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="J138" t="inlineStr">
         <is>
@@ -14386,13 +14386,13 @@
         <v>45105</v>
       </c>
       <c r="G139">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="H139" s="2">
         <v>45197</v>
       </c>
       <c r="I139">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="J139" t="inlineStr">
         <is>
@@ -14489,13 +14489,13 @@
         <v>45182</v>
       </c>
       <c r="G140">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="H140" s="2">
         <v>45273</v>
       </c>
       <c r="I140">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="J140" t="inlineStr">
         <is>
@@ -14592,13 +14592,13 @@
         <v>45116</v>
       </c>
       <c r="G141">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="H141" s="2">
         <v>45208</v>
       </c>
       <c r="I141">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="J141" t="inlineStr">
         <is>
@@ -14690,13 +14690,13 @@
         <v>45150</v>
       </c>
       <c r="G142">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="H142" s="2">
         <v>45242</v>
       </c>
       <c r="I142">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="J142" t="inlineStr">
         <is>
@@ -14793,7 +14793,7 @@
         <v>45238</v>
       </c>
       <c r="I143">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="J143" t="inlineStr">
         <is>
@@ -14890,13 +14890,13 @@
         <v>45171</v>
       </c>
       <c r="G144">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="H144" s="2">
         <v>45262</v>
       </c>
       <c r="I144">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="J144" t="inlineStr">
         <is>
@@ -14993,13 +14993,13 @@
         <v>45102</v>
       </c>
       <c r="G145">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="H145" s="2">
         <v>45194</v>
       </c>
       <c r="I145">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="J145" t="inlineStr">
         <is>
@@ -15086,13 +15086,13 @@
         <v>45119</v>
       </c>
       <c r="G146">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="H146" s="2">
         <v>45211</v>
       </c>
       <c r="I146">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="J146" t="inlineStr">
         <is>
@@ -15189,13 +15189,13 @@
         <v>45165</v>
       </c>
       <c r="G147">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="H147" s="2">
         <v>45257</v>
       </c>
       <c r="I147">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="J147" t="inlineStr">
         <is>
@@ -15292,13 +15292,13 @@
         <v>45166</v>
       </c>
       <c r="G148">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="H148" s="2">
         <v>45258</v>
       </c>
       <c r="I148">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="J148" t="inlineStr">
         <is>
@@ -15395,13 +15395,13 @@
         <v>45093</v>
       </c>
       <c r="G149">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="H149" s="2">
         <v>45185</v>
       </c>
       <c r="I149">
-        <v>-4</v>
+        <v>-5</v>
       </c>
       <c r="J149" t="inlineStr">
         <is>
@@ -15498,13 +15498,13 @@
         <v>45035</v>
       </c>
       <c r="G150">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="H150" s="2">
         <v>45218</v>
       </c>
       <c r="I150">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="J150" t="inlineStr">
         <is>
@@ -15601,13 +15601,13 @@
         <v>45174</v>
       </c>
       <c r="G151">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H151" s="2">
         <v>45356</v>
       </c>
       <c r="I151">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="J151" t="inlineStr">
         <is>
@@ -15704,13 +15704,13 @@
         <v>45089</v>
       </c>
       <c r="G152">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="H152" s="2">
         <v>45272</v>
       </c>
       <c r="I152">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="J152" t="inlineStr">
         <is>
@@ -15807,13 +15807,13 @@
         <v>45124</v>
       </c>
       <c r="G153">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="H153" s="2">
         <v>45308</v>
       </c>
       <c r="I153">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="J153" t="inlineStr">
         <is>
@@ -15910,13 +15910,13 @@
         <v>45124</v>
       </c>
       <c r="G154">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="H154" s="2">
         <v>45308</v>
       </c>
       <c r="I154">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="J154" t="inlineStr">
         <is>
@@ -16013,13 +16013,13 @@
         <v>45026</v>
       </c>
       <c r="G155">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="H155" s="2">
         <v>45209</v>
       </c>
       <c r="I155">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="J155" t="inlineStr">
         <is>
@@ -16116,13 +16116,13 @@
         <v>45026</v>
       </c>
       <c r="G156">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="H156" s="2">
         <v>45209</v>
       </c>
       <c r="I156">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="J156" t="inlineStr">
         <is>
@@ -16219,13 +16219,13 @@
         <v>45026</v>
       </c>
       <c r="G157">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="H157" s="2">
         <v>45209</v>
       </c>
       <c r="I157">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="J157" t="inlineStr">
         <is>
@@ -16322,13 +16322,13 @@
         <v>45026</v>
       </c>
       <c r="G158">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="H158" s="2">
         <v>45209</v>
       </c>
       <c r="I158">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="J158" t="inlineStr">
         <is>
@@ -16425,13 +16425,13 @@
         <v>45156</v>
       </c>
       <c r="G159">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="H159" s="2">
         <v>45247</v>
       </c>
       <c r="I159">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="J159" t="inlineStr">
         <is>
@@ -16528,13 +16528,13 @@
         <v>45153</v>
       </c>
       <c r="G160">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="H160" s="2">
         <v>45245</v>
       </c>
       <c r="I160">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="J160" t="inlineStr">
         <is>
@@ -16631,13 +16631,13 @@
         <v>45135</v>
       </c>
       <c r="G161">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="H161" s="2">
         <v>45319</v>
       </c>
       <c r="I161">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="J161" t="inlineStr">
         <is>
@@ -16734,13 +16734,13 @@
         <v>45091</v>
       </c>
       <c r="G162">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="H162" s="2">
         <v>45274</v>
       </c>
       <c r="I162">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="J162" t="inlineStr">
         <is>
@@ -16832,13 +16832,13 @@
         <v>45091</v>
       </c>
       <c r="G163">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="H163" s="2">
         <v>45274</v>
       </c>
       <c r="I163">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="J163" t="inlineStr">
         <is>
@@ -16930,13 +16930,13 @@
         <v>45138</v>
       </c>
       <c r="G164">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="H164" s="2">
         <v>45322</v>
       </c>
       <c r="I164">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="J164" t="inlineStr">
         <is>
@@ -17033,13 +17033,13 @@
         <v>45138</v>
       </c>
       <c r="G165">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="H165" s="2">
         <v>45322</v>
       </c>
       <c r="I165">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="J165" t="inlineStr">
         <is>
@@ -17136,13 +17136,13 @@
         <v>45085</v>
       </c>
       <c r="G166">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="H166" s="2">
         <v>45268</v>
       </c>
       <c r="I166">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="J166" t="inlineStr">
         <is>
@@ -17239,13 +17239,13 @@
         <v>45085</v>
       </c>
       <c r="G167">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="H167" s="2">
         <v>45268</v>
       </c>
       <c r="I167">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="J167" t="inlineStr">
         <is>
@@ -17342,7 +17342,7 @@
         <v>45326</v>
       </c>
       <c r="I168">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="J168" t="inlineStr">
         <is>
@@ -17439,13 +17439,13 @@
         <v>45173</v>
       </c>
       <c r="G169">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="H169" s="2">
         <v>45355</v>
       </c>
       <c r="I169">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="J169" t="inlineStr">
         <is>
@@ -17542,13 +17542,13 @@
         <v>45056</v>
       </c>
       <c r="G170">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="H170" s="2">
         <v>45240</v>
       </c>
       <c r="I170">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="J170" t="inlineStr">
         <is>
@@ -17645,7 +17645,7 @@
         <v>45238</v>
       </c>
       <c r="I171">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="J171" t="inlineStr">
         <is>
@@ -17742,13 +17742,13 @@
         <v>45141</v>
       </c>
       <c r="G172">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="H172" s="2">
         <v>45325</v>
       </c>
       <c r="I172">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="J172" t="inlineStr">
         <is>
@@ -17845,13 +17845,13 @@
         <v>45037</v>
       </c>
       <c r="G173">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="H173" s="2">
         <v>45220</v>
       </c>
       <c r="I173">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="J173" t="inlineStr">
         <is>
@@ -17948,13 +17948,13 @@
         <v>45171</v>
       </c>
       <c r="G174">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="H174" s="2">
         <v>45262</v>
       </c>
       <c r="I174">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="J174" t="inlineStr">
         <is>
@@ -18051,13 +18051,13 @@
         <v>45105</v>
       </c>
       <c r="G175">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="H175" s="2">
         <v>45197</v>
       </c>
       <c r="I175">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="J175" t="inlineStr">
         <is>
@@ -18154,13 +18154,13 @@
         <v>45162</v>
       </c>
       <c r="G176">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="H176" s="2">
         <v>45254</v>
       </c>
       <c r="I176">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="J176" t="inlineStr">
         <is>
@@ -18257,13 +18257,13 @@
         <v>45061</v>
       </c>
       <c r="G177">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="H177" s="2">
         <v>45245</v>
       </c>
       <c r="I177">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="J177" t="inlineStr">
         <is>
@@ -18360,13 +18360,13 @@
         <v>45120</v>
       </c>
       <c r="G178">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="H178" s="2">
         <v>45212</v>
       </c>
       <c r="I178">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="J178" t="inlineStr">
         <is>
@@ -18463,7 +18463,7 @@
         <v>45191</v>
       </c>
       <c r="I179">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J179" t="inlineStr">
         <is>
@@ -18560,13 +18560,13 @@
         <v>45088</v>
       </c>
       <c r="G180">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="H180" s="2">
         <v>45271</v>
       </c>
       <c r="I180">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="J180" t="inlineStr">
         <is>
@@ -18663,13 +18663,13 @@
         <v>45100</v>
       </c>
       <c r="G181">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="H181" s="2">
         <v>45192</v>
       </c>
       <c r="I181">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="J181" t="inlineStr">
         <is>
@@ -18756,13 +18756,13 @@
         <v>45131</v>
       </c>
       <c r="G182">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="H182" s="2">
         <v>45223</v>
       </c>
       <c r="I182">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="J182" t="inlineStr">
         <is>
@@ -18854,13 +18854,13 @@
         <v>45136</v>
       </c>
       <c r="G183">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="H183" s="2">
         <v>45228</v>
       </c>
       <c r="I183">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="J183" t="inlineStr">
         <is>
@@ -18952,13 +18952,13 @@
         <v>45150</v>
       </c>
       <c r="G184">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="H184" s="2">
         <v>45242</v>
       </c>
       <c r="I184">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="J184" t="inlineStr">
         <is>
@@ -19050,13 +19050,13 @@
         <v>45118</v>
       </c>
       <c r="G185">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="H185" s="2">
         <v>45210</v>
       </c>
       <c r="I185">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="J185" t="inlineStr">
         <is>
@@ -19148,13 +19148,13 @@
         <v>45129</v>
       </c>
       <c r="G186">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="H186" s="2">
         <v>45221</v>
       </c>
       <c r="I186">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="J186" t="inlineStr">
         <is>
@@ -19246,13 +19246,13 @@
         <v>45097</v>
       </c>
       <c r="G187">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="H187" s="2">
         <v>45189</v>
       </c>
       <c r="I187">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="J187" t="inlineStr">
         <is>
@@ -19339,13 +19339,13 @@
         <v>45101</v>
       </c>
       <c r="G188">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="H188" s="2">
         <v>45193</v>
       </c>
       <c r="I188">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="J188" t="inlineStr">
         <is>
@@ -19432,13 +19432,13 @@
         <v>45165</v>
       </c>
       <c r="G189">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="H189" s="2">
         <v>45257</v>
       </c>
       <c r="I189">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="J189" t="inlineStr">
         <is>
@@ -19530,7 +19530,7 @@
         <v>45202</v>
       </c>
       <c r="I190">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="J190" t="inlineStr">
         <is>
@@ -19627,13 +19627,13 @@
         <v>45081</v>
       </c>
       <c r="G191">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="H191" s="2">
         <v>45264</v>
       </c>
       <c r="I191">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="J191" t="inlineStr">
         <is>
@@ -19730,13 +19730,13 @@
         <v>45081</v>
       </c>
       <c r="G192">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="H192" s="2">
         <v>45264</v>
       </c>
       <c r="I192">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="J192" t="inlineStr">
         <is>
@@ -19833,7 +19833,7 @@
         <v>45319</v>
       </c>
       <c r="I193">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="J193" t="inlineStr">
         <is>
@@ -19930,7 +19930,7 @@
         <v>45319</v>
       </c>
       <c r="I194">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="J194" t="inlineStr">
         <is>
@@ -20022,13 +20022,13 @@
         <v>45046</v>
       </c>
       <c r="G195">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="H195" s="2">
         <v>45230</v>
       </c>
       <c r="I195">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="J195" t="inlineStr">
         <is>
@@ -20125,13 +20125,13 @@
         <v>45046</v>
       </c>
       <c r="G196">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="H196" s="2">
         <v>45230</v>
       </c>
       <c r="I196">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="J196" t="inlineStr">
         <is>
@@ -20228,13 +20228,13 @@
         <v>45031</v>
       </c>
       <c r="G197">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="H197" s="2">
         <v>45214</v>
       </c>
       <c r="I197">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="J197" t="inlineStr">
         <is>
@@ -20331,13 +20331,13 @@
         <v>45031</v>
       </c>
       <c r="G198">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="H198" s="2">
         <v>45214</v>
       </c>
       <c r="I198">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="J198" t="inlineStr">
         <is>
@@ -20434,13 +20434,13 @@
         <v>45031</v>
       </c>
       <c r="G199">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="H199" s="2">
         <v>45214</v>
       </c>
       <c r="I199">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="J199" t="inlineStr">
         <is>
@@ -20537,13 +20537,13 @@
         <v>45031</v>
       </c>
       <c r="G200">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="H200" s="2">
         <v>45214</v>
       </c>
       <c r="I200">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="J200" t="inlineStr">
         <is>
@@ -20640,13 +20640,13 @@
         <v>45067</v>
       </c>
       <c r="G201">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="H201" s="2">
         <v>45251</v>
       </c>
       <c r="I201">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="J201" t="inlineStr">
         <is>
@@ -20743,13 +20743,13 @@
         <v>45067</v>
       </c>
       <c r="G202">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="H202" s="2">
         <v>45251</v>
       </c>
       <c r="I202">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="J202" t="inlineStr">
         <is>
@@ -20846,13 +20846,13 @@
         <v>45067</v>
       </c>
       <c r="G203">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="H203" s="2">
         <v>45251</v>
       </c>
       <c r="I203">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="J203" t="inlineStr">
         <is>
@@ -20949,13 +20949,13 @@
         <v>45067</v>
       </c>
       <c r="G204">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="H204" s="2">
         <v>45251</v>
       </c>
       <c r="I204">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="J204" t="inlineStr">
         <is>
@@ -21052,13 +21052,13 @@
         <v>45178</v>
       </c>
       <c r="G205">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="H205" s="2">
         <v>45269</v>
       </c>
       <c r="I205">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="J205" t="inlineStr">
         <is>
@@ -21155,7 +21155,7 @@
         <v>45252</v>
       </c>
       <c r="I206">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="J206" t="inlineStr">
         <is>
@@ -21252,13 +21252,13 @@
         <v>45087</v>
       </c>
       <c r="G207">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="H207" s="2">
         <v>45270</v>
       </c>
       <c r="I207">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="J207" t="inlineStr">
         <is>
@@ -21355,13 +21355,13 @@
         <v>45099</v>
       </c>
       <c r="G208">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="H208" s="2">
         <v>45282</v>
       </c>
       <c r="I208">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="J208" t="inlineStr">
         <is>
@@ -21458,13 +21458,13 @@
         <v>45175</v>
       </c>
       <c r="G209">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="H209" s="2">
         <v>45356</v>
       </c>
       <c r="I209">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="J209" t="inlineStr">
         <is>
@@ -21561,13 +21561,13 @@
         <v>45175</v>
       </c>
       <c r="G210">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="H210" s="2">
         <v>45356</v>
       </c>
       <c r="I210">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="J210" t="inlineStr">
         <is>
@@ -21664,13 +21664,13 @@
         <v>45166</v>
       </c>
       <c r="G211">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="H211" s="2">
         <v>45350</v>
       </c>
       <c r="I211">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="J211" t="inlineStr">
         <is>
@@ -21767,13 +21767,13 @@
         <v>45166</v>
       </c>
       <c r="G212">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="H212" s="2">
         <v>45350</v>
       </c>
       <c r="I212">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="J212" t="inlineStr">
         <is>
@@ -21870,13 +21870,13 @@
         <v>45090</v>
       </c>
       <c r="G213">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="H213" s="2">
         <v>45273</v>
       </c>
       <c r="I213">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="J213" t="inlineStr">
         <is>
@@ -21973,13 +21973,13 @@
         <v>45106</v>
       </c>
       <c r="G214">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="H214" s="2">
         <v>45289</v>
       </c>
       <c r="I214">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="J214" t="inlineStr">
         <is>
@@ -22076,13 +22076,13 @@
         <v>45134</v>
       </c>
       <c r="G215">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="H215" s="2">
         <v>45226</v>
       </c>
       <c r="I215">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="J215" t="inlineStr">
         <is>
@@ -22179,13 +22179,13 @@
         <v>45132</v>
       </c>
       <c r="G216">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="H216" s="2">
         <v>45224</v>
       </c>
       <c r="I216">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="J216" t="inlineStr">
         <is>
@@ -22282,13 +22282,13 @@
         <v>45150</v>
       </c>
       <c r="G217">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="H217" s="2">
         <v>45242</v>
       </c>
       <c r="I217">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="J217" t="inlineStr">
         <is>
@@ -22385,13 +22385,13 @@
         <v>45095</v>
       </c>
       <c r="G218">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="H218" s="2">
         <v>45187</v>
       </c>
       <c r="I218">
-        <v>-2</v>
+        <v>-3</v>
       </c>
       <c r="J218" t="inlineStr">
         <is>
@@ -22483,13 +22483,13 @@
         <v>45182</v>
       </c>
       <c r="G219">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="H219" s="2">
         <v>45273</v>
       </c>
       <c r="I219">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="J219" t="inlineStr">
         <is>
@@ -22586,7 +22586,7 @@
         <v>45196</v>
       </c>
       <c r="I220">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="J220" t="inlineStr">
         <is>
@@ -22683,13 +22683,13 @@
         <v>45108</v>
       </c>
       <c r="G221">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="H221" s="2">
         <v>45200</v>
       </c>
       <c r="I221">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="J221" t="inlineStr">
         <is>
@@ -22786,13 +22786,13 @@
         <v>45135</v>
       </c>
       <c r="G222">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="H222" s="2">
         <v>45227</v>
       </c>
       <c r="I222">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="J222" t="inlineStr">
         <is>
@@ -22889,13 +22889,13 @@
         <v>45148</v>
       </c>
       <c r="G223">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="H223" s="2">
         <v>45240</v>
       </c>
       <c r="I223">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="J223" t="inlineStr">
         <is>
@@ -22987,13 +22987,13 @@
         <v>45100</v>
       </c>
       <c r="G224">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="H224" s="2">
         <v>45192</v>
       </c>
       <c r="I224">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="J224" t="inlineStr">
         <is>
@@ -23085,13 +23085,13 @@
         <v>45136</v>
       </c>
       <c r="G225">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="H225" s="2">
         <v>45320</v>
       </c>
       <c r="I225">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="J225" t="inlineStr">
         <is>
@@ -23188,13 +23188,13 @@
         <v>45136</v>
       </c>
       <c r="G226">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="H226" s="2">
         <v>45320</v>
       </c>
       <c r="I226">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="J226" t="inlineStr">
         <is>
@@ -23291,13 +23291,13 @@
         <v>45094</v>
       </c>
       <c r="G227">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="H227" s="2">
         <v>45277</v>
       </c>
       <c r="I227">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="J227" t="inlineStr">
         <is>
@@ -23394,13 +23394,13 @@
         <v>45081</v>
       </c>
       <c r="G228">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="H228" s="2">
         <v>45264</v>
       </c>
       <c r="I228">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="J228" t="inlineStr">
         <is>
@@ -23497,13 +23497,13 @@
         <v>45099</v>
       </c>
       <c r="G229">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="H229" s="2">
         <v>45282</v>
       </c>
       <c r="I229">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="J229" t="inlineStr">
         <is>
@@ -23600,13 +23600,13 @@
         <v>45018</v>
       </c>
       <c r="G230">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="H230" s="2">
         <v>45201</v>
       </c>
       <c r="I230">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="J230" t="inlineStr">
         <is>
@@ -23703,13 +23703,13 @@
         <v>45031</v>
       </c>
       <c r="G231">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="H231" s="2">
         <v>45214</v>
       </c>
       <c r="I231">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="J231" t="inlineStr">
         <is>
@@ -23806,7 +23806,7 @@
         <v>45294</v>
       </c>
       <c r="I232">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="J232" t="inlineStr">
         <is>
@@ -23903,13 +23903,13 @@
         <v>45079</v>
       </c>
       <c r="G233">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="H233" s="2">
         <v>45262</v>
       </c>
       <c r="I233">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="J233" t="inlineStr">
         <is>
@@ -24006,7 +24006,7 @@
         <v>45199</v>
       </c>
       <c r="I234">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="J234" t="inlineStr">
         <is>
@@ -24103,13 +24103,13 @@
         <v>45021</v>
       </c>
       <c r="G235">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="H235" s="2">
         <v>45204</v>
       </c>
       <c r="I235">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="J235" t="inlineStr">
         <is>
@@ -24206,13 +24206,13 @@
         <v>45021</v>
       </c>
       <c r="G236">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="H236" s="2">
         <v>45204</v>
       </c>
       <c r="I236">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="J236" t="inlineStr">
         <is>
@@ -24309,13 +24309,13 @@
         <v>45080</v>
       </c>
       <c r="G237">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="H237" s="2">
         <v>45263</v>
       </c>
       <c r="I237">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="J237" t="inlineStr">
         <is>
@@ -24412,13 +24412,13 @@
         <v>45046</v>
       </c>
       <c r="G238">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="H238" s="2">
         <v>45229</v>
       </c>
       <c r="I238">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="J238" t="inlineStr">
         <is>
@@ -24515,13 +24515,13 @@
         <v>45112</v>
       </c>
       <c r="G239">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="H239" s="2">
         <v>45204</v>
       </c>
       <c r="I239">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="J239" t="inlineStr">
         <is>
@@ -24609,13 +24609,13 @@
         <v>45112</v>
       </c>
       <c r="G240">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="H240" s="2">
         <v>45204</v>
       </c>
       <c r="I240">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="J240" t="inlineStr">
         <is>
@@ -24703,13 +24703,13 @@
         <v>45016</v>
       </c>
       <c r="G241">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="H241" s="2">
         <v>45199</v>
       </c>
       <c r="I241">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="J241" t="inlineStr">
         <is>
@@ -24806,13 +24806,13 @@
         <v>45070</v>
       </c>
       <c r="G242">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="H242" s="2">
         <v>45254</v>
       </c>
       <c r="I242">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="J242" t="inlineStr">
         <is>
@@ -24909,13 +24909,13 @@
         <v>45168</v>
       </c>
       <c r="G243">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="H243" s="2">
         <v>45260</v>
       </c>
       <c r="I243">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="J243" t="inlineStr">
         <is>
@@ -25012,13 +25012,13 @@
         <v>45027</v>
       </c>
       <c r="G244">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="H244" s="2">
         <v>45210</v>
       </c>
       <c r="I244">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="J244" t="inlineStr">
         <is>
@@ -25115,13 +25115,13 @@
         <v>45077</v>
       </c>
       <c r="G245">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="H245" s="2">
         <v>45260</v>
       </c>
       <c r="I245">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="J245" t="inlineStr">
         <is>
@@ -25218,13 +25218,13 @@
         <v>45100</v>
       </c>
       <c r="G246">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="H246" s="2">
         <v>45283</v>
       </c>
       <c r="I246">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="J246" t="inlineStr">
         <is>
@@ -25321,7 +25321,7 @@
         <v>45281</v>
       </c>
       <c r="I247">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="J247" t="inlineStr">
         <is>
@@ -25418,13 +25418,13 @@
         <v>45044</v>
       </c>
       <c r="G248">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="H248" s="2">
         <v>45227</v>
       </c>
       <c r="I248">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="J248" t="inlineStr">
         <is>
@@ -25521,13 +25521,13 @@
         <v>45101</v>
       </c>
       <c r="G249">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="H249" s="2">
         <v>45283</v>
       </c>
       <c r="I249">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="J249" t="inlineStr">
         <is>
@@ -25624,13 +25624,13 @@
         <v>45134</v>
       </c>
       <c r="G250">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="H250" s="2">
         <v>45226</v>
       </c>
       <c r="I250">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="J250" t="inlineStr">
         <is>
@@ -25727,13 +25727,13 @@
         <v>45158</v>
       </c>
       <c r="G251">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="H251" s="2">
         <v>45250</v>
       </c>
       <c r="I251">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="J251" t="inlineStr">
         <is>
@@ -25830,13 +25830,13 @@
         <v>45108</v>
       </c>
       <c r="G252">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="H252" s="2">
         <v>45200</v>
       </c>
       <c r="I252">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="J252" t="inlineStr">
         <is>
@@ -25933,7 +25933,7 @@
         <v>45317</v>
       </c>
       <c r="I253">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="J253" t="inlineStr">
         <is>
@@ -26030,13 +26030,13 @@
         <v>45039</v>
       </c>
       <c r="G254">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="H254" s="2">
         <v>45222</v>
       </c>
       <c r="I254">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="J254" t="inlineStr">
         <is>
@@ -26128,13 +26128,13 @@
         <v>45129</v>
       </c>
       <c r="G255">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="H255" s="2">
         <v>45221</v>
       </c>
       <c r="I255">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="J255" t="inlineStr">
         <is>
@@ -26231,13 +26231,13 @@
         <v>45157</v>
       </c>
       <c r="G256">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="H256" s="2">
         <v>45341</v>
       </c>
       <c r="I256">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="J256" t="inlineStr">
         <is>
@@ -26334,13 +26334,13 @@
         <v>45063</v>
       </c>
       <c r="G257">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="H257" s="2">
         <v>45247</v>
       </c>
       <c r="I257">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="J257" t="inlineStr">
         <is>
@@ -26437,7 +26437,7 @@
         <v>45254</v>
       </c>
       <c r="I258">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="J258" t="inlineStr">
         <is>
@@ -26534,7 +26534,7 @@
         <v>45486</v>
       </c>
       <c r="I259">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="J259" t="inlineStr">
         <is>
@@ -26626,13 +26626,13 @@
         <v>45073</v>
       </c>
       <c r="G260">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="H260" s="2">
         <v>45439</v>
       </c>
       <c r="I260">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="J260" t="inlineStr">
         <is>
@@ -26724,7 +26724,7 @@
         <v>45323</v>
       </c>
       <c r="I261">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="J261" t="inlineStr">
         <is>
@@ -26816,7 +26816,7 @@
         <v>45303</v>
       </c>
       <c r="I262">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="J262" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
Bond dates update Fri Sep 22 23:08:12 UTC 2023
</commit_message>
<xml_diff>
--- a/Data/obligacje_screener.xlsx
+++ b/Data/obligacje_screener.xlsx
@@ -512,7 +512,7 @@
         <v>45340</v>
       </c>
       <c r="I2">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="J2" t="inlineStr">
         <is>
@@ -600,13 +600,13 @@
         <v>45121</v>
       </c>
       <c r="G3">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="H3" s="2">
         <v>45305</v>
       </c>
       <c r="I3">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="J3" t="inlineStr">
         <is>
@@ -703,13 +703,13 @@
         <v>45039</v>
       </c>
       <c r="G4">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="H4" s="2">
         <v>45222</v>
       </c>
       <c r="I4">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="J4" t="inlineStr">
         <is>
@@ -806,13 +806,13 @@
         <v>45039</v>
       </c>
       <c r="G5">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="H5" s="2">
         <v>45222</v>
       </c>
       <c r="I5">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="J5" t="inlineStr">
         <is>
@@ -909,13 +909,13 @@
         <v>45129</v>
       </c>
       <c r="G6">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="H6" s="2">
         <v>45221</v>
       </c>
       <c r="I6">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="J6" t="inlineStr">
         <is>
@@ -1012,13 +1012,13 @@
         <v>45162</v>
       </c>
       <c r="G7">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="H7" s="2">
         <v>45254</v>
       </c>
       <c r="I7">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="J7" t="inlineStr">
         <is>
@@ -1110,13 +1110,13 @@
         <v>45156</v>
       </c>
       <c r="G8">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="H8" s="2">
         <v>45248</v>
       </c>
       <c r="I8">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="J8" t="inlineStr">
         <is>
@@ -1213,13 +1213,13 @@
         <v>45141</v>
       </c>
       <c r="G9">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="H9" s="2">
         <v>45233</v>
       </c>
       <c r="I9">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="J9" t="inlineStr">
         <is>
@@ -1316,13 +1316,13 @@
         <v>45062</v>
       </c>
       <c r="G10">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="H10" s="2">
         <v>45246</v>
       </c>
       <c r="I10">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="J10" t="inlineStr">
         <is>
@@ -1419,7 +1419,7 @@
         <v>45286</v>
       </c>
       <c r="I11">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="J11" t="inlineStr">
         <is>
@@ -1516,13 +1516,13 @@
         <v>45011</v>
       </c>
       <c r="G12">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="H12" s="2">
         <v>45195</v>
       </c>
       <c r="I12">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="J12" t="inlineStr">
         <is>
@@ -1614,13 +1614,13 @@
         <v>45036</v>
       </c>
       <c r="G13">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="H13" s="2">
         <v>45219</v>
       </c>
       <c r="I13">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="J13" t="inlineStr">
         <is>
@@ -1717,13 +1717,13 @@
         <v>45036</v>
       </c>
       <c r="G14">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="H14" s="2">
         <v>45219</v>
       </c>
       <c r="I14">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="J14" t="inlineStr">
         <is>
@@ -1820,13 +1820,13 @@
         <v>45106</v>
       </c>
       <c r="G15">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="H15" s="2">
         <v>45289</v>
       </c>
       <c r="I15">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="J15" t="inlineStr">
         <is>
@@ -1923,13 +1923,13 @@
         <v>45094</v>
       </c>
       <c r="G16">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="H16" s="2">
         <v>45186</v>
       </c>
       <c r="I16">
-        <v>-4</v>
+        <v>-5</v>
       </c>
       <c r="J16" t="inlineStr">
         <is>
@@ -2026,13 +2026,13 @@
         <v>45094</v>
       </c>
       <c r="G17">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="H17" s="2">
         <v>45186</v>
       </c>
       <c r="I17">
-        <v>-4</v>
+        <v>-5</v>
       </c>
       <c r="J17" t="inlineStr">
         <is>
@@ -2129,13 +2129,13 @@
         <v>45132</v>
       </c>
       <c r="G18">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="H18" s="2">
         <v>45224</v>
       </c>
       <c r="I18">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="J18" t="inlineStr">
         <is>
@@ -2232,13 +2232,13 @@
         <v>45137</v>
       </c>
       <c r="G19">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="H19" s="2">
         <v>45229</v>
       </c>
       <c r="I19">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="J19" t="inlineStr">
         <is>
@@ -2330,13 +2330,13 @@
         <v>45183</v>
       </c>
       <c r="G20">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="H20" s="2">
         <v>45274</v>
       </c>
       <c r="I20">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="J20" t="inlineStr">
         <is>
@@ -2433,13 +2433,13 @@
         <v>45093</v>
       </c>
       <c r="G21">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="H21" s="2">
         <v>45187</v>
       </c>
       <c r="I21">
-        <v>-3</v>
+        <v>-4</v>
       </c>
       <c r="J21" t="inlineStr">
         <is>
@@ -2536,13 +2536,13 @@
         <v>45096</v>
       </c>
       <c r="G22">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="H22" s="2">
         <v>45187</v>
       </c>
       <c r="I22">
-        <v>-3</v>
+        <v>-4</v>
       </c>
       <c r="J22" t="inlineStr">
         <is>
@@ -2639,7 +2639,7 @@
         <v>45245</v>
       </c>
       <c r="I23">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="J23" t="inlineStr">
         <is>
@@ -2736,7 +2736,7 @@
         <v>45245</v>
       </c>
       <c r="I24">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="J24" t="inlineStr">
         <is>
@@ -2833,13 +2833,13 @@
         <v>45021</v>
       </c>
       <c r="G25">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="H25" s="2">
         <v>45204</v>
       </c>
       <c r="I25">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="J25" t="inlineStr">
         <is>
@@ -2936,13 +2936,13 @@
         <v>45160</v>
       </c>
       <c r="G26">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="H26" s="2">
         <v>45344</v>
       </c>
       <c r="I26">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="J26" t="inlineStr">
         <is>
@@ -3039,13 +3039,13 @@
         <v>45118</v>
       </c>
       <c r="G27">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="H27" s="2">
         <v>45302</v>
       </c>
       <c r="I27">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="J27" t="inlineStr">
         <is>
@@ -3142,13 +3142,13 @@
         <v>45085</v>
       </c>
       <c r="G28">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="H28" s="2">
         <v>45268</v>
       </c>
       <c r="I28">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="J28" t="inlineStr">
         <is>
@@ -3245,13 +3245,13 @@
         <v>45183</v>
       </c>
       <c r="G29">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="H29" s="2">
         <v>45274</v>
       </c>
       <c r="I29">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="J29" t="inlineStr">
         <is>
@@ -3348,7 +3348,7 @@
         <v>45224</v>
       </c>
       <c r="I30">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="J30" t="inlineStr">
         <is>
@@ -3445,13 +3445,13 @@
         <v>45153</v>
       </c>
       <c r="G31">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="H31" s="2">
         <v>45245</v>
       </c>
       <c r="I31">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="J31" t="inlineStr">
         <is>
@@ -3548,13 +3548,13 @@
         <v>45155</v>
       </c>
       <c r="G32">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="H32" s="2">
         <v>45247</v>
       </c>
       <c r="I32">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="J32" t="inlineStr">
         <is>
@@ -3651,7 +3651,7 @@
         <v>45255</v>
       </c>
       <c r="I33">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="J33" t="inlineStr">
         <is>
@@ -3739,13 +3739,13 @@
         <v>45176</v>
       </c>
       <c r="G34">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="H34" s="2">
         <v>45267</v>
       </c>
       <c r="I34">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="J34" t="inlineStr">
         <is>
@@ -3842,13 +3842,13 @@
         <v>45130</v>
       </c>
       <c r="G35">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="H35" s="2">
         <v>45222</v>
       </c>
       <c r="I35">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="J35" t="inlineStr">
         <is>
@@ -3940,13 +3940,13 @@
         <v>45115</v>
       </c>
       <c r="G36">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="H36" s="2">
         <v>45207</v>
       </c>
       <c r="I36">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="J36" t="inlineStr">
         <is>
@@ -4043,13 +4043,13 @@
         <v>45097</v>
       </c>
       <c r="G37">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="H37" s="2">
         <v>45189</v>
       </c>
       <c r="I37">
-        <v>-1</v>
+        <v>-2</v>
       </c>
       <c r="J37" t="inlineStr">
         <is>
@@ -4141,13 +4141,13 @@
         <v>45107</v>
       </c>
       <c r="G38">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="H38" s="2">
         <v>45290</v>
       </c>
       <c r="I38">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="J38" t="inlineStr">
         <is>
@@ -4244,13 +4244,13 @@
         <v>45063</v>
       </c>
       <c r="G39">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="H39" s="2">
         <v>45247</v>
       </c>
       <c r="I39">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="J39" t="inlineStr">
         <is>
@@ -4347,13 +4347,13 @@
         <v>45177</v>
       </c>
       <c r="G40">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="H40" s="2">
         <v>45359</v>
       </c>
       <c r="I40">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="J40" t="inlineStr">
         <is>
@@ -4450,13 +4450,13 @@
         <v>45107</v>
       </c>
       <c r="G41">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="H41" s="2">
         <v>45290</v>
       </c>
       <c r="I41">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="J41" t="inlineStr">
         <is>
@@ -4553,7 +4553,7 @@
         <v>45265</v>
       </c>
       <c r="I42">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="J42" t="inlineStr">
         <is>
@@ -4650,13 +4650,13 @@
         <v>45098</v>
       </c>
       <c r="G43">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="H43" s="2">
         <v>45281</v>
       </c>
       <c r="I43">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="J43" t="inlineStr">
         <is>
@@ -4753,13 +4753,13 @@
         <v>45099</v>
       </c>
       <c r="G44">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="H44" s="2">
         <v>45282</v>
       </c>
       <c r="I44">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="J44" t="inlineStr">
         <is>
@@ -4856,13 +4856,13 @@
         <v>45106</v>
       </c>
       <c r="G45">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="H45" s="2">
         <v>45289</v>
       </c>
       <c r="I45">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="J45" t="inlineStr">
         <is>
@@ -4959,13 +4959,13 @@
         <v>45106</v>
       </c>
       <c r="G46">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="H46" s="2">
         <v>45289</v>
       </c>
       <c r="I46">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="J46" t="inlineStr">
         <is>
@@ -5062,13 +5062,13 @@
         <v>45120</v>
       </c>
       <c r="G47">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="H47" s="2">
         <v>45304</v>
       </c>
       <c r="I47">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="J47" t="inlineStr">
         <is>
@@ -5165,13 +5165,13 @@
         <v>45118</v>
       </c>
       <c r="G48">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="H48" s="2">
         <v>45302</v>
       </c>
       <c r="I48">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="J48" t="inlineStr">
         <is>
@@ -5268,13 +5268,13 @@
         <v>45152</v>
       </c>
       <c r="G49">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="H49" s="2">
         <v>45336</v>
       </c>
       <c r="I49">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="J49" t="inlineStr">
         <is>
@@ -5371,13 +5371,13 @@
         <v>45042</v>
       </c>
       <c r="G50">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="H50" s="2">
         <v>45225</v>
       </c>
       <c r="I50">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="J50" t="inlineStr">
         <is>
@@ -5474,13 +5474,13 @@
         <v>45122</v>
       </c>
       <c r="G51">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="H51" s="2">
         <v>45306</v>
       </c>
       <c r="I51">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="J51" t="inlineStr">
         <is>
@@ -5577,13 +5577,13 @@
         <v>45139</v>
       </c>
       <c r="G52">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="H52" s="2">
         <v>45323</v>
       </c>
       <c r="I52">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="J52" t="inlineStr">
         <is>
@@ -5671,13 +5671,13 @@
         <v>45099</v>
       </c>
       <c r="G53">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="H53" s="2">
         <v>45282</v>
       </c>
       <c r="I53">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="J53" t="inlineStr">
         <is>
@@ -5774,7 +5774,7 @@
         <v>45196</v>
       </c>
       <c r="I54">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="J54" t="inlineStr">
         <is>
@@ -5871,13 +5871,13 @@
         <v>45044</v>
       </c>
       <c r="G55">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="H55" s="2">
         <v>45227</v>
       </c>
       <c r="I55">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="J55" t="inlineStr">
         <is>
@@ -5974,13 +5974,13 @@
         <v>45151</v>
       </c>
       <c r="G56">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="H56" s="2">
         <v>45243</v>
       </c>
       <c r="I56">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="J56" t="inlineStr">
         <is>
@@ -6072,7 +6072,7 @@
         <v>45196</v>
       </c>
       <c r="I57">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="J57" t="inlineStr">
         <is>
@@ -6169,13 +6169,13 @@
         <v>45069</v>
       </c>
       <c r="G58">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="H58" s="2">
         <v>45253</v>
       </c>
       <c r="I58">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="J58" t="inlineStr">
         <is>
@@ -6272,13 +6272,13 @@
         <v>45099</v>
       </c>
       <c r="G59">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="H59" s="2">
         <v>45191</v>
       </c>
       <c r="I59">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J59" t="inlineStr">
         <is>
@@ -6370,13 +6370,13 @@
         <v>45113</v>
       </c>
       <c r="G60">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="H60" s="2">
         <v>45205</v>
       </c>
       <c r="I60">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="J60" t="inlineStr">
         <is>
@@ -6473,13 +6473,13 @@
         <v>45127</v>
       </c>
       <c r="G61">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="H61" s="2">
         <v>45219</v>
       </c>
       <c r="I61">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="J61" t="inlineStr">
         <is>
@@ -6576,13 +6576,13 @@
         <v>45058</v>
       </c>
       <c r="G62">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="H62" s="2">
         <v>45242</v>
       </c>
       <c r="I62">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="J62" t="inlineStr">
         <is>
@@ -6679,13 +6679,13 @@
         <v>45010</v>
       </c>
       <c r="G63">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="H63" s="2">
         <v>45194</v>
       </c>
       <c r="I63">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="J63" t="inlineStr">
         <is>
@@ -6777,13 +6777,13 @@
         <v>45025</v>
       </c>
       <c r="G64">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="H64" s="2">
         <v>45208</v>
       </c>
       <c r="I64">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="J64" t="inlineStr">
         <is>
@@ -6880,13 +6880,13 @@
         <v>45025</v>
       </c>
       <c r="G65">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="H65" s="2">
         <v>45208</v>
       </c>
       <c r="I65">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="J65" t="inlineStr">
         <is>
@@ -6983,13 +6983,13 @@
         <v>45089</v>
       </c>
       <c r="G66">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="H66" s="2">
         <v>45272</v>
       </c>
       <c r="I66">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="J66" t="inlineStr">
         <is>
@@ -7086,13 +7086,13 @@
         <v>45178</v>
       </c>
       <c r="G67">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="H67" s="2">
         <v>45269</v>
       </c>
       <c r="I67">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="J67" t="inlineStr">
         <is>
@@ -7184,13 +7184,13 @@
         <v>45104</v>
       </c>
       <c r="G68">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="H68" s="2">
         <v>45196</v>
       </c>
       <c r="I68">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="J68" t="inlineStr">
         <is>
@@ -7287,13 +7287,13 @@
         <v>45149</v>
       </c>
       <c r="G69">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="H69" s="2">
         <v>45241</v>
       </c>
       <c r="I69">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="J69" t="inlineStr">
         <is>
@@ -7390,7 +7390,7 @@
         <v>45205</v>
       </c>
       <c r="I70">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="J70" t="inlineStr">
         <is>
@@ -7487,13 +7487,13 @@
         <v>45114</v>
       </c>
       <c r="G71">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="H71" s="2">
         <v>45205</v>
       </c>
       <c r="I71">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="J71" t="inlineStr">
         <is>
@@ -7590,13 +7590,13 @@
         <v>45115</v>
       </c>
       <c r="G72">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="H72" s="2">
         <v>45207</v>
       </c>
       <c r="I72">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="J72" t="inlineStr">
         <is>
@@ -7693,13 +7693,13 @@
         <v>45097</v>
       </c>
       <c r="G73">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="H73" s="2">
         <v>45189</v>
       </c>
       <c r="I73">
-        <v>-1</v>
+        <v>-2</v>
       </c>
       <c r="J73" t="inlineStr">
         <is>
@@ -7791,13 +7791,13 @@
         <v>45038</v>
       </c>
       <c r="G74">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="H74" s="2">
         <v>45221</v>
       </c>
       <c r="I74">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="J74" t="inlineStr">
         <is>
@@ -7889,13 +7889,13 @@
         <v>45117</v>
       </c>
       <c r="G75">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="H75" s="2">
         <v>45301</v>
       </c>
       <c r="I75">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="J75" t="inlineStr">
         <is>
@@ -7992,13 +7992,13 @@
         <v>45160</v>
       </c>
       <c r="G76">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="H76" s="2">
         <v>45344</v>
       </c>
       <c r="I76">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="J76" t="inlineStr">
         <is>
@@ -8095,13 +8095,13 @@
         <v>45002</v>
       </c>
       <c r="G77">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="H77" s="2">
         <v>45186</v>
       </c>
       <c r="I77">
-        <v>-4</v>
+        <v>-5</v>
       </c>
       <c r="J77" t="inlineStr">
         <is>
@@ -8198,13 +8198,13 @@
         <v>45043</v>
       </c>
       <c r="G78">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="H78" s="2">
         <v>45226</v>
       </c>
       <c r="I78">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="J78" t="inlineStr">
         <is>
@@ -8301,13 +8301,13 @@
         <v>45079</v>
       </c>
       <c r="G79">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="H79" s="2">
         <v>45262</v>
       </c>
       <c r="I79">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="J79" t="inlineStr">
         <is>
@@ -8404,7 +8404,7 @@
         <v>45254</v>
       </c>
       <c r="I80">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="J80" t="inlineStr">
         <is>
@@ -8501,13 +8501,13 @@
         <v>45104</v>
       </c>
       <c r="G81">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="H81" s="2">
         <v>45287</v>
       </c>
       <c r="I81">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="J81" t="inlineStr">
         <is>
@@ -8604,7 +8604,7 @@
         <v>45288</v>
       </c>
       <c r="I82">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="J82" t="inlineStr">
         <is>
@@ -8696,13 +8696,13 @@
         <v>45175</v>
       </c>
       <c r="G83">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H83" s="2">
         <v>45357</v>
       </c>
       <c r="I83">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="J83" t="inlineStr">
         <is>
@@ -8799,13 +8799,13 @@
         <v>45054</v>
       </c>
       <c r="G84">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="H84" s="2">
         <v>45238</v>
       </c>
       <c r="I84">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="J84" t="inlineStr">
         <is>
@@ -8902,13 +8902,13 @@
         <v>45056</v>
       </c>
       <c r="G85">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="H85" s="2">
         <v>45240</v>
       </c>
       <c r="I85">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="J85" t="inlineStr">
         <is>
@@ -9005,13 +9005,13 @@
         <v>45085</v>
       </c>
       <c r="G86">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="H86" s="2">
         <v>45268</v>
       </c>
       <c r="I86">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="J86" t="inlineStr">
         <is>
@@ -9108,7 +9108,7 @@
         <v>45194</v>
       </c>
       <c r="I87">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="J87" t="inlineStr">
         <is>
@@ -9195,13 +9195,13 @@
         <v>45103</v>
       </c>
       <c r="G88">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="H88" s="2">
         <v>45286</v>
       </c>
       <c r="I88">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="J88" t="inlineStr">
         <is>
@@ -9298,13 +9298,13 @@
         <v>45103</v>
       </c>
       <c r="G89">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="H89" s="2">
         <v>45286</v>
       </c>
       <c r="I89">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="J89" t="inlineStr">
         <is>
@@ -9401,13 +9401,13 @@
         <v>45008</v>
       </c>
       <c r="G90">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="H90" s="2">
         <v>45192</v>
       </c>
       <c r="I90">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J90" t="inlineStr">
         <is>
@@ -9499,13 +9499,13 @@
         <v>45100</v>
       </c>
       <c r="G91">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="H91" s="2">
         <v>45287</v>
       </c>
       <c r="I91">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="J91" t="inlineStr">
         <is>
@@ -9602,13 +9602,13 @@
         <v>45003</v>
       </c>
       <c r="G92">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="H92" s="2">
         <v>45187</v>
       </c>
       <c r="I92">
-        <v>-3</v>
+        <v>-4</v>
       </c>
       <c r="J92" t="inlineStr">
         <is>
@@ -9705,13 +9705,13 @@
         <v>45104</v>
       </c>
       <c r="G93">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="H93" s="2">
         <v>45287</v>
       </c>
       <c r="I93">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="J93" t="inlineStr">
         <is>
@@ -9808,13 +9808,13 @@
         <v>45104</v>
       </c>
       <c r="G94">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="H94" s="2">
         <v>45287</v>
       </c>
       <c r="I94">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="J94" t="inlineStr">
         <is>
@@ -9911,13 +9911,13 @@
         <v>45049</v>
       </c>
       <c r="G95">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="H95" s="2">
         <v>45233</v>
       </c>
       <c r="I95">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="J95" t="inlineStr">
         <is>
@@ -10014,13 +10014,13 @@
         <v>45122</v>
       </c>
       <c r="G96">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="H96" s="2">
         <v>45306</v>
       </c>
       <c r="I96">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="J96" t="inlineStr">
         <is>
@@ -10112,13 +10112,13 @@
         <v>45141</v>
       </c>
       <c r="G97">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="H97" s="2">
         <v>45325</v>
       </c>
       <c r="I97">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="J97" t="inlineStr">
         <is>
@@ -10215,13 +10215,13 @@
         <v>45010</v>
       </c>
       <c r="G98">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="H98" s="2">
         <v>45194</v>
       </c>
       <c r="I98">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="J98" t="inlineStr">
         <is>
@@ -10313,13 +10313,13 @@
         <v>45093</v>
       </c>
       <c r="G99">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="H99" s="2">
         <v>45276</v>
       </c>
       <c r="I99">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="J99" t="inlineStr">
         <is>
@@ -10416,13 +10416,13 @@
         <v>45123</v>
       </c>
       <c r="G100">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="H100" s="2">
         <v>45307</v>
       </c>
       <c r="I100">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="J100" t="inlineStr">
         <is>
@@ -10519,13 +10519,13 @@
         <v>45014</v>
       </c>
       <c r="G101">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="H101" s="2">
         <v>45198</v>
       </c>
       <c r="I101">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="J101" t="inlineStr">
         <is>
@@ -10622,13 +10622,13 @@
         <v>45093</v>
       </c>
       <c r="G102">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="H102" s="2">
         <v>45276</v>
       </c>
       <c r="I102">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="J102" t="inlineStr">
         <is>
@@ -10725,13 +10725,13 @@
         <v>45122</v>
       </c>
       <c r="G103">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="H103" s="2">
         <v>45306</v>
       </c>
       <c r="I103">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="J103" t="inlineStr">
         <is>
@@ -10828,13 +10828,13 @@
         <v>45122</v>
       </c>
       <c r="G104">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="H104" s="2">
         <v>45306</v>
       </c>
       <c r="I104">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="J104" t="inlineStr">
         <is>
@@ -10926,13 +10926,13 @@
         <v>45050</v>
       </c>
       <c r="G105">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="H105" s="2">
         <v>45234</v>
       </c>
       <c r="I105">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="J105" t="inlineStr">
         <is>
@@ -11029,13 +11029,13 @@
         <v>45085</v>
       </c>
       <c r="G106">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="H106" s="2">
         <v>45268</v>
       </c>
       <c r="I106">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="J106" t="inlineStr">
         <is>
@@ -11132,13 +11132,13 @@
         <v>45093</v>
       </c>
       <c r="G107">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="H107" s="2">
         <v>45185</v>
       </c>
       <c r="I107">
-        <v>-5</v>
+        <v>-6</v>
       </c>
       <c r="J107" t="inlineStr">
         <is>
@@ -11230,13 +11230,13 @@
         <v>45093</v>
       </c>
       <c r="G108">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="H108" s="2">
         <v>45185</v>
       </c>
       <c r="I108">
-        <v>-5</v>
+        <v>-6</v>
       </c>
       <c r="J108" t="inlineStr">
         <is>
@@ -11328,13 +11328,13 @@
         <v>45093</v>
       </c>
       <c r="G109">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="H109" s="2">
         <v>45185</v>
       </c>
       <c r="I109">
-        <v>-5</v>
+        <v>-6</v>
       </c>
       <c r="J109" t="inlineStr">
         <is>
@@ -11431,13 +11431,13 @@
         <v>45148</v>
       </c>
       <c r="G110">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="H110" s="2">
         <v>45240</v>
       </c>
       <c r="I110">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="J110" t="inlineStr">
         <is>
@@ -11534,13 +11534,13 @@
         <v>45119</v>
       </c>
       <c r="G111">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="H111" s="2">
         <v>45211</v>
       </c>
       <c r="I111">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="J111" t="inlineStr">
         <is>
@@ -11637,13 +11637,13 @@
         <v>45172</v>
       </c>
       <c r="G112">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="H112" s="2">
         <v>45263</v>
       </c>
       <c r="I112">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="J112" t="inlineStr">
         <is>
@@ -11740,13 +11740,13 @@
         <v>45023</v>
       </c>
       <c r="G113">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="H113" s="2">
         <v>45206</v>
       </c>
       <c r="I113">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="J113" t="inlineStr">
         <is>
@@ -11843,13 +11843,13 @@
         <v>45111</v>
       </c>
       <c r="G114">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="H114" s="2">
         <v>45203</v>
       </c>
       <c r="I114">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="J114" t="inlineStr">
         <is>
@@ -11946,7 +11946,7 @@
         <v>45218</v>
       </c>
       <c r="I115">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="J115" t="inlineStr">
         <is>
@@ -12043,13 +12043,13 @@
         <v>45161</v>
       </c>
       <c r="G116">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="H116" s="2">
         <v>45253</v>
       </c>
       <c r="I116">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="J116" t="inlineStr">
         <is>
@@ -12146,13 +12146,13 @@
         <v>45115</v>
       </c>
       <c r="G117">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="H117" s="2">
         <v>45299</v>
       </c>
       <c r="I117">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="J117" t="inlineStr">
         <is>
@@ -12244,13 +12244,13 @@
         <v>45094</v>
       </c>
       <c r="G118">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="H118" s="2">
         <v>45277</v>
       </c>
       <c r="I118">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="J118" t="inlineStr">
         <is>
@@ -12347,13 +12347,13 @@
         <v>45104</v>
       </c>
       <c r="G119">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="H119" s="2">
         <v>45287</v>
       </c>
       <c r="I119">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="J119" t="inlineStr">
         <is>
@@ -12450,13 +12450,13 @@
         <v>45104</v>
       </c>
       <c r="G120">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="H120" s="2">
         <v>45287</v>
       </c>
       <c r="I120">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="J120" t="inlineStr">
         <is>
@@ -12553,13 +12553,13 @@
         <v>45104</v>
       </c>
       <c r="G121">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="H121" s="2">
         <v>45287</v>
       </c>
       <c r="I121">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="J121" t="inlineStr">
         <is>
@@ -12656,13 +12656,13 @@
         <v>45104</v>
       </c>
       <c r="G122">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="H122" s="2">
         <v>45287</v>
       </c>
       <c r="I122">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="J122" t="inlineStr">
         <is>
@@ -12759,13 +12759,13 @@
         <v>45107</v>
       </c>
       <c r="G123">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="H123" s="2">
         <v>45199</v>
       </c>
       <c r="I123">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="J123" t="inlineStr">
         <is>
@@ -12862,13 +12862,13 @@
         <v>45013</v>
       </c>
       <c r="G124">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="H124" s="2">
         <v>45197</v>
       </c>
       <c r="I124">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="J124" t="inlineStr">
         <is>
@@ -12965,13 +12965,13 @@
         <v>45121</v>
       </c>
       <c r="G125">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="H125" s="2">
         <v>45213</v>
       </c>
       <c r="I125">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="J125" t="inlineStr">
         <is>
@@ -13068,13 +13068,13 @@
         <v>45134</v>
       </c>
       <c r="G126">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="H126" s="2">
         <v>45226</v>
       </c>
       <c r="I126">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="J126" t="inlineStr">
         <is>
@@ -13171,7 +13171,7 @@
         <v>45212</v>
       </c>
       <c r="I127">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="J127" t="inlineStr">
         <is>
@@ -13268,13 +13268,13 @@
         <v>45126</v>
       </c>
       <c r="G128">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="H128" s="2">
         <v>45218</v>
       </c>
       <c r="I128">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="J128" t="inlineStr">
         <is>
@@ -13366,13 +13366,13 @@
         <v>45158</v>
       </c>
       <c r="G129">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="H129" s="2">
         <v>45250</v>
       </c>
       <c r="I129">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="J129" t="inlineStr">
         <is>
@@ -13469,13 +13469,13 @@
         <v>45171</v>
       </c>
       <c r="G130">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="H130" s="2">
         <v>45262</v>
       </c>
       <c r="I130">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="J130" t="inlineStr">
         <is>
@@ -13572,13 +13572,13 @@
         <v>45111</v>
       </c>
       <c r="G131">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="H131" s="2">
         <v>45203</v>
       </c>
       <c r="I131">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="J131" t="inlineStr">
         <is>
@@ -13675,13 +13675,13 @@
         <v>45144</v>
       </c>
       <c r="G132">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="H132" s="2">
         <v>45236</v>
       </c>
       <c r="I132">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="J132" t="inlineStr">
         <is>
@@ -13778,13 +13778,13 @@
         <v>45156</v>
       </c>
       <c r="G133">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="H133" s="2">
         <v>45248</v>
       </c>
       <c r="I133">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="J133" t="inlineStr">
         <is>
@@ -13876,13 +13876,13 @@
         <v>45146</v>
       </c>
       <c r="G134">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="H134" s="2">
         <v>45238</v>
       </c>
       <c r="I134">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="J134" t="inlineStr">
         <is>
@@ -13979,13 +13979,13 @@
         <v>45140</v>
       </c>
       <c r="G135">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="H135" s="2">
         <v>45232</v>
       </c>
       <c r="I135">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="J135" t="inlineStr">
         <is>
@@ -14082,13 +14082,13 @@
         <v>45104</v>
       </c>
       <c r="G136">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="H136" s="2">
         <v>45196</v>
       </c>
       <c r="I136">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="J136" t="inlineStr">
         <is>
@@ -14185,13 +14185,13 @@
         <v>45105</v>
       </c>
       <c r="G137">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="H137" s="2">
         <v>45197</v>
       </c>
       <c r="I137">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="J137" t="inlineStr">
         <is>
@@ -14288,13 +14288,13 @@
         <v>45179</v>
       </c>
       <c r="G138">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="H138" s="2">
         <v>45270</v>
       </c>
       <c r="I138">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="J138" t="inlineStr">
         <is>
@@ -14386,13 +14386,13 @@
         <v>45105</v>
       </c>
       <c r="G139">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="H139" s="2">
         <v>45197</v>
       </c>
       <c r="I139">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="J139" t="inlineStr">
         <is>
@@ -14489,13 +14489,13 @@
         <v>45182</v>
       </c>
       <c r="G140">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="H140" s="2">
         <v>45273</v>
       </c>
       <c r="I140">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="J140" t="inlineStr">
         <is>
@@ -14592,13 +14592,13 @@
         <v>45116</v>
       </c>
       <c r="G141">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="H141" s="2">
         <v>45208</v>
       </c>
       <c r="I141">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="J141" t="inlineStr">
         <is>
@@ -14690,13 +14690,13 @@
         <v>45150</v>
       </c>
       <c r="G142">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="H142" s="2">
         <v>45242</v>
       </c>
       <c r="I142">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="J142" t="inlineStr">
         <is>
@@ -14793,7 +14793,7 @@
         <v>45238</v>
       </c>
       <c r="I143">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="J143" t="inlineStr">
         <is>
@@ -14890,13 +14890,13 @@
         <v>45171</v>
       </c>
       <c r="G144">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="H144" s="2">
         <v>45262</v>
       </c>
       <c r="I144">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="J144" t="inlineStr">
         <is>
@@ -14993,13 +14993,13 @@
         <v>45102</v>
       </c>
       <c r="G145">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="H145" s="2">
         <v>45194</v>
       </c>
       <c r="I145">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="J145" t="inlineStr">
         <is>
@@ -15086,13 +15086,13 @@
         <v>45119</v>
       </c>
       <c r="G146">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="H146" s="2">
         <v>45211</v>
       </c>
       <c r="I146">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="J146" t="inlineStr">
         <is>
@@ -15189,13 +15189,13 @@
         <v>45165</v>
       </c>
       <c r="G147">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="H147" s="2">
         <v>45257</v>
       </c>
       <c r="I147">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="J147" t="inlineStr">
         <is>
@@ -15292,13 +15292,13 @@
         <v>45166</v>
       </c>
       <c r="G148">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="H148" s="2">
         <v>45258</v>
       </c>
       <c r="I148">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="J148" t="inlineStr">
         <is>
@@ -15395,13 +15395,13 @@
         <v>45093</v>
       </c>
       <c r="G149">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="H149" s="2">
         <v>45185</v>
       </c>
       <c r="I149">
-        <v>-5</v>
+        <v>-6</v>
       </c>
       <c r="J149" t="inlineStr">
         <is>
@@ -15498,13 +15498,13 @@
         <v>45035</v>
       </c>
       <c r="G150">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="H150" s="2">
         <v>45218</v>
       </c>
       <c r="I150">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="J150" t="inlineStr">
         <is>
@@ -15601,13 +15601,13 @@
         <v>45174</v>
       </c>
       <c r="G151">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="H151" s="2">
         <v>45356</v>
       </c>
       <c r="I151">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="J151" t="inlineStr">
         <is>
@@ -15704,13 +15704,13 @@
         <v>45089</v>
       </c>
       <c r="G152">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="H152" s="2">
         <v>45272</v>
       </c>
       <c r="I152">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="J152" t="inlineStr">
         <is>
@@ -15807,13 +15807,13 @@
         <v>45124</v>
       </c>
       <c r="G153">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="H153" s="2">
         <v>45308</v>
       </c>
       <c r="I153">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="J153" t="inlineStr">
         <is>
@@ -15910,13 +15910,13 @@
         <v>45124</v>
       </c>
       <c r="G154">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="H154" s="2">
         <v>45308</v>
       </c>
       <c r="I154">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="J154" t="inlineStr">
         <is>
@@ -16013,13 +16013,13 @@
         <v>45026</v>
       </c>
       <c r="G155">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="H155" s="2">
         <v>45209</v>
       </c>
       <c r="I155">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="J155" t="inlineStr">
         <is>
@@ -16116,13 +16116,13 @@
         <v>45026</v>
       </c>
       <c r="G156">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="H156" s="2">
         <v>45209</v>
       </c>
       <c r="I156">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="J156" t="inlineStr">
         <is>
@@ -16219,13 +16219,13 @@
         <v>45026</v>
       </c>
       <c r="G157">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="H157" s="2">
         <v>45209</v>
       </c>
       <c r="I157">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="J157" t="inlineStr">
         <is>
@@ -16322,13 +16322,13 @@
         <v>45026</v>
       </c>
       <c r="G158">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="H158" s="2">
         <v>45209</v>
       </c>
       <c r="I158">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="J158" t="inlineStr">
         <is>
@@ -16425,13 +16425,13 @@
         <v>45156</v>
       </c>
       <c r="G159">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="H159" s="2">
         <v>45247</v>
       </c>
       <c r="I159">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="J159" t="inlineStr">
         <is>
@@ -16528,13 +16528,13 @@
         <v>45153</v>
       </c>
       <c r="G160">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="H160" s="2">
         <v>45245</v>
       </c>
       <c r="I160">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="J160" t="inlineStr">
         <is>
@@ -16631,13 +16631,13 @@
         <v>45135</v>
       </c>
       <c r="G161">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="H161" s="2">
         <v>45319</v>
       </c>
       <c r="I161">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="J161" t="inlineStr">
         <is>
@@ -16734,13 +16734,13 @@
         <v>45091</v>
       </c>
       <c r="G162">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="H162" s="2">
         <v>45274</v>
       </c>
       <c r="I162">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="J162" t="inlineStr">
         <is>
@@ -16832,13 +16832,13 @@
         <v>45091</v>
       </c>
       <c r="G163">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="H163" s="2">
         <v>45274</v>
       </c>
       <c r="I163">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="J163" t="inlineStr">
         <is>
@@ -16930,13 +16930,13 @@
         <v>45138</v>
       </c>
       <c r="G164">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="H164" s="2">
         <v>45322</v>
       </c>
       <c r="I164">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="J164" t="inlineStr">
         <is>
@@ -17033,13 +17033,13 @@
         <v>45138</v>
       </c>
       <c r="G165">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="H165" s="2">
         <v>45322</v>
       </c>
       <c r="I165">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="J165" t="inlineStr">
         <is>
@@ -17136,13 +17136,13 @@
         <v>45085</v>
       </c>
       <c r="G166">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="H166" s="2">
         <v>45268</v>
       </c>
       <c r="I166">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="J166" t="inlineStr">
         <is>
@@ -17239,13 +17239,13 @@
         <v>45085</v>
       </c>
       <c r="G167">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="H167" s="2">
         <v>45268</v>
       </c>
       <c r="I167">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="J167" t="inlineStr">
         <is>
@@ -17342,7 +17342,7 @@
         <v>45326</v>
       </c>
       <c r="I168">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="J168" t="inlineStr">
         <is>
@@ -17439,13 +17439,13 @@
         <v>45173</v>
       </c>
       <c r="G169">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="H169" s="2">
         <v>45355</v>
       </c>
       <c r="I169">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="J169" t="inlineStr">
         <is>
@@ -17542,13 +17542,13 @@
         <v>45056</v>
       </c>
       <c r="G170">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="H170" s="2">
         <v>45240</v>
       </c>
       <c r="I170">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="J170" t="inlineStr">
         <is>
@@ -17645,7 +17645,7 @@
         <v>45238</v>
       </c>
       <c r="I171">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="J171" t="inlineStr">
         <is>
@@ -17742,13 +17742,13 @@
         <v>45141</v>
       </c>
       <c r="G172">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="H172" s="2">
         <v>45325</v>
       </c>
       <c r="I172">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="J172" t="inlineStr">
         <is>
@@ -17845,13 +17845,13 @@
         <v>45037</v>
       </c>
       <c r="G173">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="H173" s="2">
         <v>45220</v>
       </c>
       <c r="I173">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="J173" t="inlineStr">
         <is>
@@ -17948,13 +17948,13 @@
         <v>45171</v>
       </c>
       <c r="G174">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="H174" s="2">
         <v>45262</v>
       </c>
       <c r="I174">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="J174" t="inlineStr">
         <is>
@@ -18051,13 +18051,13 @@
         <v>45105</v>
       </c>
       <c r="G175">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="H175" s="2">
         <v>45197</v>
       </c>
       <c r="I175">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="J175" t="inlineStr">
         <is>
@@ -18154,13 +18154,13 @@
         <v>45162</v>
       </c>
       <c r="G176">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="H176" s="2">
         <v>45254</v>
       </c>
       <c r="I176">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="J176" t="inlineStr">
         <is>
@@ -18257,13 +18257,13 @@
         <v>45061</v>
       </c>
       <c r="G177">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="H177" s="2">
         <v>45245</v>
       </c>
       <c r="I177">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="J177" t="inlineStr">
         <is>
@@ -18360,13 +18360,13 @@
         <v>45120</v>
       </c>
       <c r="G178">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="H178" s="2">
         <v>45212</v>
       </c>
       <c r="I178">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="J178" t="inlineStr">
         <is>
@@ -18463,7 +18463,7 @@
         <v>45191</v>
       </c>
       <c r="I179">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J179" t="inlineStr">
         <is>
@@ -18560,13 +18560,13 @@
         <v>45088</v>
       </c>
       <c r="G180">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="H180" s="2">
         <v>45271</v>
       </c>
       <c r="I180">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="J180" t="inlineStr">
         <is>
@@ -18663,13 +18663,13 @@
         <v>45100</v>
       </c>
       <c r="G181">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="H181" s="2">
         <v>45192</v>
       </c>
       <c r="I181">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J181" t="inlineStr">
         <is>
@@ -18756,13 +18756,13 @@
         <v>45131</v>
       </c>
       <c r="G182">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="H182" s="2">
         <v>45223</v>
       </c>
       <c r="I182">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="J182" t="inlineStr">
         <is>
@@ -18854,13 +18854,13 @@
         <v>45136</v>
       </c>
       <c r="G183">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="H183" s="2">
         <v>45228</v>
       </c>
       <c r="I183">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="J183" t="inlineStr">
         <is>
@@ -18952,13 +18952,13 @@
         <v>45150</v>
       </c>
       <c r="G184">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="H184" s="2">
         <v>45242</v>
       </c>
       <c r="I184">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="J184" t="inlineStr">
         <is>
@@ -19050,13 +19050,13 @@
         <v>45118</v>
       </c>
       <c r="G185">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="H185" s="2">
         <v>45210</v>
       </c>
       <c r="I185">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="J185" t="inlineStr">
         <is>
@@ -19148,13 +19148,13 @@
         <v>45129</v>
       </c>
       <c r="G186">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="H186" s="2">
         <v>45221</v>
       </c>
       <c r="I186">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="J186" t="inlineStr">
         <is>
@@ -19246,13 +19246,13 @@
         <v>45097</v>
       </c>
       <c r="G187">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="H187" s="2">
         <v>45189</v>
       </c>
       <c r="I187">
-        <v>-1</v>
+        <v>-2</v>
       </c>
       <c r="J187" t="inlineStr">
         <is>
@@ -19339,13 +19339,13 @@
         <v>45101</v>
       </c>
       <c r="G188">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="H188" s="2">
         <v>45193</v>
       </c>
       <c r="I188">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="J188" t="inlineStr">
         <is>
@@ -19432,13 +19432,13 @@
         <v>45165</v>
       </c>
       <c r="G189">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="H189" s="2">
         <v>45257</v>
       </c>
       <c r="I189">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="J189" t="inlineStr">
         <is>
@@ -19530,7 +19530,7 @@
         <v>45202</v>
       </c>
       <c r="I190">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="J190" t="inlineStr">
         <is>
@@ -19627,13 +19627,13 @@
         <v>45081</v>
       </c>
       <c r="G191">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="H191" s="2">
         <v>45264</v>
       </c>
       <c r="I191">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="J191" t="inlineStr">
         <is>
@@ -19730,13 +19730,13 @@
         <v>45081</v>
       </c>
       <c r="G192">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="H192" s="2">
         <v>45264</v>
       </c>
       <c r="I192">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="J192" t="inlineStr">
         <is>
@@ -19833,7 +19833,7 @@
         <v>45319</v>
       </c>
       <c r="I193">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="J193" t="inlineStr">
         <is>
@@ -19930,7 +19930,7 @@
         <v>45319</v>
       </c>
       <c r="I194">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="J194" t="inlineStr">
         <is>
@@ -20022,13 +20022,13 @@
         <v>45046</v>
       </c>
       <c r="G195">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="H195" s="2">
         <v>45230</v>
       </c>
       <c r="I195">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="J195" t="inlineStr">
         <is>
@@ -20125,13 +20125,13 @@
         <v>45046</v>
       </c>
       <c r="G196">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="H196" s="2">
         <v>45230</v>
       </c>
       <c r="I196">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="J196" t="inlineStr">
         <is>
@@ -20228,13 +20228,13 @@
         <v>45031</v>
       </c>
       <c r="G197">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="H197" s="2">
         <v>45214</v>
       </c>
       <c r="I197">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="J197" t="inlineStr">
         <is>
@@ -20331,13 +20331,13 @@
         <v>45031</v>
       </c>
       <c r="G198">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="H198" s="2">
         <v>45214</v>
       </c>
       <c r="I198">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="J198" t="inlineStr">
         <is>
@@ -20434,13 +20434,13 @@
         <v>45031</v>
       </c>
       <c r="G199">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="H199" s="2">
         <v>45214</v>
       </c>
       <c r="I199">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="J199" t="inlineStr">
         <is>
@@ -20537,13 +20537,13 @@
         <v>45031</v>
       </c>
       <c r="G200">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="H200" s="2">
         <v>45214</v>
       </c>
       <c r="I200">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="J200" t="inlineStr">
         <is>
@@ -20640,13 +20640,13 @@
         <v>45067</v>
       </c>
       <c r="G201">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="H201" s="2">
         <v>45251</v>
       </c>
       <c r="I201">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="J201" t="inlineStr">
         <is>
@@ -20743,13 +20743,13 @@
         <v>45067</v>
       </c>
       <c r="G202">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="H202" s="2">
         <v>45251</v>
       </c>
       <c r="I202">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="J202" t="inlineStr">
         <is>
@@ -20846,13 +20846,13 @@
         <v>45067</v>
       </c>
       <c r="G203">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="H203" s="2">
         <v>45251</v>
       </c>
       <c r="I203">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="J203" t="inlineStr">
         <is>
@@ -20949,13 +20949,13 @@
         <v>45067</v>
       </c>
       <c r="G204">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="H204" s="2">
         <v>45251</v>
       </c>
       <c r="I204">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="J204" t="inlineStr">
         <is>
@@ -21052,13 +21052,13 @@
         <v>45178</v>
       </c>
       <c r="G205">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="H205" s="2">
         <v>45269</v>
       </c>
       <c r="I205">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="J205" t="inlineStr">
         <is>
@@ -21155,7 +21155,7 @@
         <v>45252</v>
       </c>
       <c r="I206">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="J206" t="inlineStr">
         <is>
@@ -21252,13 +21252,13 @@
         <v>45087</v>
       </c>
       <c r="G207">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="H207" s="2">
         <v>45270</v>
       </c>
       <c r="I207">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="J207" t="inlineStr">
         <is>
@@ -21355,13 +21355,13 @@
         <v>45099</v>
       </c>
       <c r="G208">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="H208" s="2">
         <v>45282</v>
       </c>
       <c r="I208">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="J208" t="inlineStr">
         <is>
@@ -21458,13 +21458,13 @@
         <v>45175</v>
       </c>
       <c r="G209">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H209" s="2">
         <v>45356</v>
       </c>
       <c r="I209">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="J209" t="inlineStr">
         <is>
@@ -21561,13 +21561,13 @@
         <v>45175</v>
       </c>
       <c r="G210">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H210" s="2">
         <v>45356</v>
       </c>
       <c r="I210">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="J210" t="inlineStr">
         <is>
@@ -21664,13 +21664,13 @@
         <v>45166</v>
       </c>
       <c r="G211">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="H211" s="2">
         <v>45350</v>
       </c>
       <c r="I211">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="J211" t="inlineStr">
         <is>
@@ -21767,13 +21767,13 @@
         <v>45166</v>
       </c>
       <c r="G212">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="H212" s="2">
         <v>45350</v>
       </c>
       <c r="I212">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="J212" t="inlineStr">
         <is>
@@ -21870,13 +21870,13 @@
         <v>45090</v>
       </c>
       <c r="G213">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="H213" s="2">
         <v>45273</v>
       </c>
       <c r="I213">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="J213" t="inlineStr">
         <is>
@@ -21973,13 +21973,13 @@
         <v>45106</v>
       </c>
       <c r="G214">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="H214" s="2">
         <v>45289</v>
       </c>
       <c r="I214">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="J214" t="inlineStr">
         <is>
@@ -22076,13 +22076,13 @@
         <v>45134</v>
       </c>
       <c r="G215">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="H215" s="2">
         <v>45226</v>
       </c>
       <c r="I215">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="J215" t="inlineStr">
         <is>
@@ -22179,13 +22179,13 @@
         <v>45132</v>
       </c>
       <c r="G216">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="H216" s="2">
         <v>45224</v>
       </c>
       <c r="I216">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="J216" t="inlineStr">
         <is>
@@ -22282,13 +22282,13 @@
         <v>45150</v>
       </c>
       <c r="G217">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="H217" s="2">
         <v>45242</v>
       </c>
       <c r="I217">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="J217" t="inlineStr">
         <is>
@@ -22385,13 +22385,13 @@
         <v>45095</v>
       </c>
       <c r="G218">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="H218" s="2">
         <v>45187</v>
       </c>
       <c r="I218">
-        <v>-3</v>
+        <v>-4</v>
       </c>
       <c r="J218" t="inlineStr">
         <is>
@@ -22483,13 +22483,13 @@
         <v>45182</v>
       </c>
       <c r="G219">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="H219" s="2">
         <v>45273</v>
       </c>
       <c r="I219">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="J219" t="inlineStr">
         <is>
@@ -22586,7 +22586,7 @@
         <v>45196</v>
       </c>
       <c r="I220">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="J220" t="inlineStr">
         <is>
@@ -22683,13 +22683,13 @@
         <v>45108</v>
       </c>
       <c r="G221">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="H221" s="2">
         <v>45200</v>
       </c>
       <c r="I221">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="J221" t="inlineStr">
         <is>
@@ -22786,13 +22786,13 @@
         <v>45135</v>
       </c>
       <c r="G222">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="H222" s="2">
         <v>45227</v>
       </c>
       <c r="I222">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="J222" t="inlineStr">
         <is>
@@ -22889,13 +22889,13 @@
         <v>45148</v>
       </c>
       <c r="G223">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="H223" s="2">
         <v>45240</v>
       </c>
       <c r="I223">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="J223" t="inlineStr">
         <is>
@@ -22987,13 +22987,13 @@
         <v>45100</v>
       </c>
       <c r="G224">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="H224" s="2">
         <v>45192</v>
       </c>
       <c r="I224">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J224" t="inlineStr">
         <is>
@@ -23085,13 +23085,13 @@
         <v>45136</v>
       </c>
       <c r="G225">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="H225" s="2">
         <v>45320</v>
       </c>
       <c r="I225">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="J225" t="inlineStr">
         <is>
@@ -23188,13 +23188,13 @@
         <v>45136</v>
       </c>
       <c r="G226">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="H226" s="2">
         <v>45320</v>
       </c>
       <c r="I226">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="J226" t="inlineStr">
         <is>
@@ -23291,13 +23291,13 @@
         <v>45094</v>
       </c>
       <c r="G227">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="H227" s="2">
         <v>45277</v>
       </c>
       <c r="I227">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="J227" t="inlineStr">
         <is>
@@ -23394,13 +23394,13 @@
         <v>45081</v>
       </c>
       <c r="G228">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="H228" s="2">
         <v>45264</v>
       </c>
       <c r="I228">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="J228" t="inlineStr">
         <is>
@@ -23497,13 +23497,13 @@
         <v>45099</v>
       </c>
       <c r="G229">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="H229" s="2">
         <v>45282</v>
       </c>
       <c r="I229">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="J229" t="inlineStr">
         <is>
@@ -23600,13 +23600,13 @@
         <v>45018</v>
       </c>
       <c r="G230">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="H230" s="2">
         <v>45201</v>
       </c>
       <c r="I230">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="J230" t="inlineStr">
         <is>
@@ -23703,13 +23703,13 @@
         <v>45031</v>
       </c>
       <c r="G231">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="H231" s="2">
         <v>45214</v>
       </c>
       <c r="I231">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="J231" t="inlineStr">
         <is>
@@ -23806,7 +23806,7 @@
         <v>45294</v>
       </c>
       <c r="I232">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="J232" t="inlineStr">
         <is>
@@ -23903,13 +23903,13 @@
         <v>45079</v>
       </c>
       <c r="G233">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="H233" s="2">
         <v>45262</v>
       </c>
       <c r="I233">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="J233" t="inlineStr">
         <is>
@@ -24006,7 +24006,7 @@
         <v>45199</v>
       </c>
       <c r="I234">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="J234" t="inlineStr">
         <is>
@@ -24103,13 +24103,13 @@
         <v>45021</v>
       </c>
       <c r="G235">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="H235" s="2">
         <v>45204</v>
       </c>
       <c r="I235">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="J235" t="inlineStr">
         <is>
@@ -24206,13 +24206,13 @@
         <v>45021</v>
       </c>
       <c r="G236">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="H236" s="2">
         <v>45204</v>
       </c>
       <c r="I236">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="J236" t="inlineStr">
         <is>
@@ -24309,13 +24309,13 @@
         <v>45080</v>
       </c>
       <c r="G237">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="H237" s="2">
         <v>45263</v>
       </c>
       <c r="I237">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="J237" t="inlineStr">
         <is>
@@ -24412,13 +24412,13 @@
         <v>45046</v>
       </c>
       <c r="G238">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="H238" s="2">
         <v>45229</v>
       </c>
       <c r="I238">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="J238" t="inlineStr">
         <is>
@@ -24515,13 +24515,13 @@
         <v>45112</v>
       </c>
       <c r="G239">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="H239" s="2">
         <v>45204</v>
       </c>
       <c r="I239">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="J239" t="inlineStr">
         <is>
@@ -24609,13 +24609,13 @@
         <v>45112</v>
       </c>
       <c r="G240">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="H240" s="2">
         <v>45204</v>
       </c>
       <c r="I240">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="J240" t="inlineStr">
         <is>
@@ -24703,13 +24703,13 @@
         <v>45016</v>
       </c>
       <c r="G241">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="H241" s="2">
         <v>45199</v>
       </c>
       <c r="I241">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="J241" t="inlineStr">
         <is>
@@ -24806,13 +24806,13 @@
         <v>45070</v>
       </c>
       <c r="G242">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="H242" s="2">
         <v>45254</v>
       </c>
       <c r="I242">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="J242" t="inlineStr">
         <is>
@@ -24909,13 +24909,13 @@
         <v>45168</v>
       </c>
       <c r="G243">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="H243" s="2">
         <v>45260</v>
       </c>
       <c r="I243">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="J243" t="inlineStr">
         <is>
@@ -25012,13 +25012,13 @@
         <v>45027</v>
       </c>
       <c r="G244">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="H244" s="2">
         <v>45210</v>
       </c>
       <c r="I244">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="J244" t="inlineStr">
         <is>
@@ -25115,13 +25115,13 @@
         <v>45077</v>
       </c>
       <c r="G245">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="H245" s="2">
         <v>45260</v>
       </c>
       <c r="I245">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="J245" t="inlineStr">
         <is>
@@ -25218,13 +25218,13 @@
         <v>45100</v>
       </c>
       <c r="G246">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="H246" s="2">
         <v>45283</v>
       </c>
       <c r="I246">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="J246" t="inlineStr">
         <is>
@@ -25321,7 +25321,7 @@
         <v>45281</v>
       </c>
       <c r="I247">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="J247" t="inlineStr">
         <is>
@@ -25418,13 +25418,13 @@
         <v>45044</v>
       </c>
       <c r="G248">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="H248" s="2">
         <v>45227</v>
       </c>
       <c r="I248">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="J248" t="inlineStr">
         <is>
@@ -25521,13 +25521,13 @@
         <v>45101</v>
       </c>
       <c r="G249">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="H249" s="2">
         <v>45283</v>
       </c>
       <c r="I249">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="J249" t="inlineStr">
         <is>
@@ -25624,13 +25624,13 @@
         <v>45134</v>
       </c>
       <c r="G250">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="H250" s="2">
         <v>45226</v>
       </c>
       <c r="I250">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="J250" t="inlineStr">
         <is>
@@ -25727,13 +25727,13 @@
         <v>45158</v>
       </c>
       <c r="G251">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="H251" s="2">
         <v>45250</v>
       </c>
       <c r="I251">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="J251" t="inlineStr">
         <is>
@@ -25830,13 +25830,13 @@
         <v>45108</v>
       </c>
       <c r="G252">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="H252" s="2">
         <v>45200</v>
       </c>
       <c r="I252">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="J252" t="inlineStr">
         <is>
@@ -25933,7 +25933,7 @@
         <v>45317</v>
       </c>
       <c r="I253">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="J253" t="inlineStr">
         <is>
@@ -26030,13 +26030,13 @@
         <v>45039</v>
       </c>
       <c r="G254">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="H254" s="2">
         <v>45222</v>
       </c>
       <c r="I254">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="J254" t="inlineStr">
         <is>
@@ -26128,13 +26128,13 @@
         <v>45129</v>
       </c>
       <c r="G255">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="H255" s="2">
         <v>45221</v>
       </c>
       <c r="I255">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="J255" t="inlineStr">
         <is>
@@ -26231,13 +26231,13 @@
         <v>45157</v>
       </c>
       <c r="G256">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="H256" s="2">
         <v>45341</v>
       </c>
       <c r="I256">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="J256" t="inlineStr">
         <is>
@@ -26334,13 +26334,13 @@
         <v>45063</v>
       </c>
       <c r="G257">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="H257" s="2">
         <v>45247</v>
       </c>
       <c r="I257">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="J257" t="inlineStr">
         <is>
@@ -26437,7 +26437,7 @@
         <v>45254</v>
       </c>
       <c r="I258">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="J258" t="inlineStr">
         <is>
@@ -26534,7 +26534,7 @@
         <v>45486</v>
       </c>
       <c r="I259">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="J259" t="inlineStr">
         <is>
@@ -26626,13 +26626,13 @@
         <v>45073</v>
       </c>
       <c r="G260">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="H260" s="2">
         <v>45439</v>
       </c>
       <c r="I260">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="J260" t="inlineStr">
         <is>
@@ -26724,7 +26724,7 @@
         <v>45323</v>
       </c>
       <c r="I261">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="J261" t="inlineStr">
         <is>
@@ -26816,7 +26816,7 @@
         <v>45303</v>
       </c>
       <c r="I262">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="J262" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
Bond dates update Sat Sep 23 23:08:06 UTC 2023
</commit_message>
<xml_diff>
--- a/Data/obligacje_screener.xlsx
+++ b/Data/obligacje_screener.xlsx
@@ -512,7 +512,7 @@
         <v>45340</v>
       </c>
       <c r="I2">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="J2" t="inlineStr">
         <is>
@@ -600,13 +600,13 @@
         <v>45121</v>
       </c>
       <c r="G3">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="H3" s="2">
         <v>45305</v>
       </c>
       <c r="I3">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="J3" t="inlineStr">
         <is>
@@ -703,13 +703,13 @@
         <v>45039</v>
       </c>
       <c r="G4">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="H4" s="2">
         <v>45222</v>
       </c>
       <c r="I4">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="J4" t="inlineStr">
         <is>
@@ -806,13 +806,13 @@
         <v>45039</v>
       </c>
       <c r="G5">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="H5" s="2">
         <v>45222</v>
       </c>
       <c r="I5">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="J5" t="inlineStr">
         <is>
@@ -909,13 +909,13 @@
         <v>45129</v>
       </c>
       <c r="G6">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="H6" s="2">
         <v>45221</v>
       </c>
       <c r="I6">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="J6" t="inlineStr">
         <is>
@@ -1012,13 +1012,13 @@
         <v>45162</v>
       </c>
       <c r="G7">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="H7" s="2">
         <v>45254</v>
       </c>
       <c r="I7">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="J7" t="inlineStr">
         <is>
@@ -1110,13 +1110,13 @@
         <v>45156</v>
       </c>
       <c r="G8">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="H8" s="2">
         <v>45248</v>
       </c>
       <c r="I8">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="J8" t="inlineStr">
         <is>
@@ -1213,13 +1213,13 @@
         <v>45141</v>
       </c>
       <c r="G9">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="H9" s="2">
         <v>45233</v>
       </c>
       <c r="I9">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="J9" t="inlineStr">
         <is>
@@ -1316,13 +1316,13 @@
         <v>45062</v>
       </c>
       <c r="G10">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="H10" s="2">
         <v>45246</v>
       </c>
       <c r="I10">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="J10" t="inlineStr">
         <is>
@@ -1419,7 +1419,7 @@
         <v>45286</v>
       </c>
       <c r="I11">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="J11" t="inlineStr">
         <is>
@@ -1516,13 +1516,13 @@
         <v>45011</v>
       </c>
       <c r="G12">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="H12" s="2">
         <v>45195</v>
       </c>
       <c r="I12">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="J12" t="inlineStr">
         <is>
@@ -1614,13 +1614,13 @@
         <v>45036</v>
       </c>
       <c r="G13">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="H13" s="2">
         <v>45219</v>
       </c>
       <c r="I13">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="J13" t="inlineStr">
         <is>
@@ -1717,13 +1717,13 @@
         <v>45036</v>
       </c>
       <c r="G14">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="H14" s="2">
         <v>45219</v>
       </c>
       <c r="I14">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="J14" t="inlineStr">
         <is>
@@ -1820,13 +1820,13 @@
         <v>45106</v>
       </c>
       <c r="G15">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="H15" s="2">
         <v>45289</v>
       </c>
       <c r="I15">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="J15" t="inlineStr">
         <is>
@@ -1923,13 +1923,13 @@
         <v>45094</v>
       </c>
       <c r="G16">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="H16" s="2">
         <v>45186</v>
       </c>
       <c r="I16">
-        <v>-5</v>
+        <v>-6</v>
       </c>
       <c r="J16" t="inlineStr">
         <is>
@@ -2026,13 +2026,13 @@
         <v>45094</v>
       </c>
       <c r="G17">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="H17" s="2">
         <v>45186</v>
       </c>
       <c r="I17">
-        <v>-5</v>
+        <v>-6</v>
       </c>
       <c r="J17" t="inlineStr">
         <is>
@@ -2129,13 +2129,13 @@
         <v>45132</v>
       </c>
       <c r="G18">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="H18" s="2">
         <v>45224</v>
       </c>
       <c r="I18">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="J18" t="inlineStr">
         <is>
@@ -2232,13 +2232,13 @@
         <v>45137</v>
       </c>
       <c r="G19">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="H19" s="2">
         <v>45229</v>
       </c>
       <c r="I19">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="J19" t="inlineStr">
         <is>
@@ -2330,13 +2330,13 @@
         <v>45183</v>
       </c>
       <c r="G20">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="H20" s="2">
         <v>45274</v>
       </c>
       <c r="I20">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="J20" t="inlineStr">
         <is>
@@ -2433,13 +2433,13 @@
         <v>45093</v>
       </c>
       <c r="G21">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="H21" s="2">
         <v>45187</v>
       </c>
       <c r="I21">
-        <v>-4</v>
+        <v>-5</v>
       </c>
       <c r="J21" t="inlineStr">
         <is>
@@ -2536,13 +2536,13 @@
         <v>45096</v>
       </c>
       <c r="G22">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="H22" s="2">
         <v>45187</v>
       </c>
       <c r="I22">
-        <v>-4</v>
+        <v>-5</v>
       </c>
       <c r="J22" t="inlineStr">
         <is>
@@ -2639,7 +2639,7 @@
         <v>45245</v>
       </c>
       <c r="I23">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="J23" t="inlineStr">
         <is>
@@ -2736,7 +2736,7 @@
         <v>45245</v>
       </c>
       <c r="I24">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="J24" t="inlineStr">
         <is>
@@ -2833,13 +2833,13 @@
         <v>45021</v>
       </c>
       <c r="G25">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="H25" s="2">
         <v>45204</v>
       </c>
       <c r="I25">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="J25" t="inlineStr">
         <is>
@@ -2936,13 +2936,13 @@
         <v>45160</v>
       </c>
       <c r="G26">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="H26" s="2">
         <v>45344</v>
       </c>
       <c r="I26">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="J26" t="inlineStr">
         <is>
@@ -3039,13 +3039,13 @@
         <v>45118</v>
       </c>
       <c r="G27">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="H27" s="2">
         <v>45302</v>
       </c>
       <c r="I27">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="J27" t="inlineStr">
         <is>
@@ -3142,13 +3142,13 @@
         <v>45085</v>
       </c>
       <c r="G28">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="H28" s="2">
         <v>45268</v>
       </c>
       <c r="I28">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="J28" t="inlineStr">
         <is>
@@ -3245,13 +3245,13 @@
         <v>45183</v>
       </c>
       <c r="G29">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="H29" s="2">
         <v>45274</v>
       </c>
       <c r="I29">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="J29" t="inlineStr">
         <is>
@@ -3348,7 +3348,7 @@
         <v>45224</v>
       </c>
       <c r="I30">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="J30" t="inlineStr">
         <is>
@@ -3445,13 +3445,13 @@
         <v>45153</v>
       </c>
       <c r="G31">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="H31" s="2">
         <v>45245</v>
       </c>
       <c r="I31">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="J31" t="inlineStr">
         <is>
@@ -3548,13 +3548,13 @@
         <v>45155</v>
       </c>
       <c r="G32">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="H32" s="2">
         <v>45247</v>
       </c>
       <c r="I32">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="J32" t="inlineStr">
         <is>
@@ -3651,7 +3651,7 @@
         <v>45255</v>
       </c>
       <c r="I33">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="J33" t="inlineStr">
         <is>
@@ -3739,13 +3739,13 @@
         <v>45176</v>
       </c>
       <c r="G34">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H34" s="2">
         <v>45267</v>
       </c>
       <c r="I34">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="J34" t="inlineStr">
         <is>
@@ -3842,13 +3842,13 @@
         <v>45130</v>
       </c>
       <c r="G35">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="H35" s="2">
         <v>45222</v>
       </c>
       <c r="I35">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="J35" t="inlineStr">
         <is>
@@ -3940,13 +3940,13 @@
         <v>45115</v>
       </c>
       <c r="G36">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="H36" s="2">
         <v>45207</v>
       </c>
       <c r="I36">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="J36" t="inlineStr">
         <is>
@@ -4043,13 +4043,13 @@
         <v>45097</v>
       </c>
       <c r="G37">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="H37" s="2">
         <v>45189</v>
       </c>
       <c r="I37">
-        <v>-2</v>
+        <v>-3</v>
       </c>
       <c r="J37" t="inlineStr">
         <is>
@@ -4141,13 +4141,13 @@
         <v>45107</v>
       </c>
       <c r="G38">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="H38" s="2">
         <v>45290</v>
       </c>
       <c r="I38">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="J38" t="inlineStr">
         <is>
@@ -4244,13 +4244,13 @@
         <v>45063</v>
       </c>
       <c r="G39">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="H39" s="2">
         <v>45247</v>
       </c>
       <c r="I39">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="J39" t="inlineStr">
         <is>
@@ -4347,13 +4347,13 @@
         <v>45177</v>
       </c>
       <c r="G40">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="H40" s="2">
         <v>45359</v>
       </c>
       <c r="I40">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="J40" t="inlineStr">
         <is>
@@ -4450,13 +4450,13 @@
         <v>45107</v>
       </c>
       <c r="G41">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="H41" s="2">
         <v>45290</v>
       </c>
       <c r="I41">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="J41" t="inlineStr">
         <is>
@@ -4553,7 +4553,7 @@
         <v>45265</v>
       </c>
       <c r="I42">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="J42" t="inlineStr">
         <is>
@@ -4650,13 +4650,13 @@
         <v>45098</v>
       </c>
       <c r="G43">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="H43" s="2">
         <v>45281</v>
       </c>
       <c r="I43">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="J43" t="inlineStr">
         <is>
@@ -4753,13 +4753,13 @@
         <v>45099</v>
       </c>
       <c r="G44">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="H44" s="2">
         <v>45282</v>
       </c>
       <c r="I44">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="J44" t="inlineStr">
         <is>
@@ -4856,13 +4856,13 @@
         <v>45106</v>
       </c>
       <c r="G45">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="H45" s="2">
         <v>45289</v>
       </c>
       <c r="I45">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="J45" t="inlineStr">
         <is>
@@ -4959,13 +4959,13 @@
         <v>45106</v>
       </c>
       <c r="G46">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="H46" s="2">
         <v>45289</v>
       </c>
       <c r="I46">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="J46" t="inlineStr">
         <is>
@@ -5062,13 +5062,13 @@
         <v>45120</v>
       </c>
       <c r="G47">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="H47" s="2">
         <v>45304</v>
       </c>
       <c r="I47">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="J47" t="inlineStr">
         <is>
@@ -5165,13 +5165,13 @@
         <v>45118</v>
       </c>
       <c r="G48">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="H48" s="2">
         <v>45302</v>
       </c>
       <c r="I48">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="J48" t="inlineStr">
         <is>
@@ -5268,13 +5268,13 @@
         <v>45152</v>
       </c>
       <c r="G49">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="H49" s="2">
         <v>45336</v>
       </c>
       <c r="I49">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="J49" t="inlineStr">
         <is>
@@ -5371,13 +5371,13 @@
         <v>45042</v>
       </c>
       <c r="G50">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="H50" s="2">
         <v>45225</v>
       </c>
       <c r="I50">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="J50" t="inlineStr">
         <is>
@@ -5474,13 +5474,13 @@
         <v>45122</v>
       </c>
       <c r="G51">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="H51" s="2">
         <v>45306</v>
       </c>
       <c r="I51">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="J51" t="inlineStr">
         <is>
@@ -5577,13 +5577,13 @@
         <v>45139</v>
       </c>
       <c r="G52">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="H52" s="2">
         <v>45323</v>
       </c>
       <c r="I52">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="J52" t="inlineStr">
         <is>
@@ -5671,13 +5671,13 @@
         <v>45099</v>
       </c>
       <c r="G53">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="H53" s="2">
         <v>45282</v>
       </c>
       <c r="I53">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="J53" t="inlineStr">
         <is>
@@ -5774,7 +5774,7 @@
         <v>45196</v>
       </c>
       <c r="I54">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="J54" t="inlineStr">
         <is>
@@ -5871,13 +5871,13 @@
         <v>45044</v>
       </c>
       <c r="G55">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="H55" s="2">
         <v>45227</v>
       </c>
       <c r="I55">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="J55" t="inlineStr">
         <is>
@@ -5974,13 +5974,13 @@
         <v>45151</v>
       </c>
       <c r="G56">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="H56" s="2">
         <v>45243</v>
       </c>
       <c r="I56">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="J56" t="inlineStr">
         <is>
@@ -6072,7 +6072,7 @@
         <v>45196</v>
       </c>
       <c r="I57">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="J57" t="inlineStr">
         <is>
@@ -6169,13 +6169,13 @@
         <v>45069</v>
       </c>
       <c r="G58">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="H58" s="2">
         <v>45253</v>
       </c>
       <c r="I58">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="J58" t="inlineStr">
         <is>
@@ -6272,13 +6272,13 @@
         <v>45099</v>
       </c>
       <c r="G59">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="H59" s="2">
         <v>45191</v>
       </c>
       <c r="I59">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="J59" t="inlineStr">
         <is>
@@ -6370,13 +6370,13 @@
         <v>45113</v>
       </c>
       <c r="G60">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="H60" s="2">
         <v>45205</v>
       </c>
       <c r="I60">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="J60" t="inlineStr">
         <is>
@@ -6473,13 +6473,13 @@
         <v>45127</v>
       </c>
       <c r="G61">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="H61" s="2">
         <v>45219</v>
       </c>
       <c r="I61">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="J61" t="inlineStr">
         <is>
@@ -6576,13 +6576,13 @@
         <v>45058</v>
       </c>
       <c r="G62">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="H62" s="2">
         <v>45242</v>
       </c>
       <c r="I62">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="J62" t="inlineStr">
         <is>
@@ -6679,13 +6679,13 @@
         <v>45010</v>
       </c>
       <c r="G63">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="H63" s="2">
         <v>45194</v>
       </c>
       <c r="I63">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="J63" t="inlineStr">
         <is>
@@ -6777,13 +6777,13 @@
         <v>45025</v>
       </c>
       <c r="G64">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="H64" s="2">
         <v>45208</v>
       </c>
       <c r="I64">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="J64" t="inlineStr">
         <is>
@@ -6880,13 +6880,13 @@
         <v>45025</v>
       </c>
       <c r="G65">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="H65" s="2">
         <v>45208</v>
       </c>
       <c r="I65">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="J65" t="inlineStr">
         <is>
@@ -6983,13 +6983,13 @@
         <v>45089</v>
       </c>
       <c r="G66">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="H66" s="2">
         <v>45272</v>
       </c>
       <c r="I66">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="J66" t="inlineStr">
         <is>
@@ -7086,13 +7086,13 @@
         <v>45178</v>
       </c>
       <c r="G67">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="H67" s="2">
         <v>45269</v>
       </c>
       <c r="I67">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="J67" t="inlineStr">
         <is>
@@ -7184,13 +7184,13 @@
         <v>45104</v>
       </c>
       <c r="G68">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="H68" s="2">
         <v>45196</v>
       </c>
       <c r="I68">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="J68" t="inlineStr">
         <is>
@@ -7287,13 +7287,13 @@
         <v>45149</v>
       </c>
       <c r="G69">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="H69" s="2">
         <v>45241</v>
       </c>
       <c r="I69">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="J69" t="inlineStr">
         <is>
@@ -7390,7 +7390,7 @@
         <v>45205</v>
       </c>
       <c r="I70">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="J70" t="inlineStr">
         <is>
@@ -7487,13 +7487,13 @@
         <v>45114</v>
       </c>
       <c r="G71">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="H71" s="2">
         <v>45205</v>
       </c>
       <c r="I71">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="J71" t="inlineStr">
         <is>
@@ -7590,13 +7590,13 @@
         <v>45115</v>
       </c>
       <c r="G72">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="H72" s="2">
         <v>45207</v>
       </c>
       <c r="I72">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="J72" t="inlineStr">
         <is>
@@ -7693,13 +7693,13 @@
         <v>45097</v>
       </c>
       <c r="G73">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="H73" s="2">
         <v>45189</v>
       </c>
       <c r="I73">
-        <v>-2</v>
+        <v>-3</v>
       </c>
       <c r="J73" t="inlineStr">
         <is>
@@ -7791,13 +7791,13 @@
         <v>45038</v>
       </c>
       <c r="G74">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="H74" s="2">
         <v>45221</v>
       </c>
       <c r="I74">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="J74" t="inlineStr">
         <is>
@@ -7889,13 +7889,13 @@
         <v>45117</v>
       </c>
       <c r="G75">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="H75" s="2">
         <v>45301</v>
       </c>
       <c r="I75">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="J75" t="inlineStr">
         <is>
@@ -7992,13 +7992,13 @@
         <v>45160</v>
       </c>
       <c r="G76">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="H76" s="2">
         <v>45344</v>
       </c>
       <c r="I76">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="J76" t="inlineStr">
         <is>
@@ -8095,13 +8095,13 @@
         <v>45002</v>
       </c>
       <c r="G77">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="H77" s="2">
         <v>45186</v>
       </c>
       <c r="I77">
-        <v>-5</v>
+        <v>-6</v>
       </c>
       <c r="J77" t="inlineStr">
         <is>
@@ -8198,13 +8198,13 @@
         <v>45043</v>
       </c>
       <c r="G78">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="H78" s="2">
         <v>45226</v>
       </c>
       <c r="I78">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="J78" t="inlineStr">
         <is>
@@ -8301,13 +8301,13 @@
         <v>45079</v>
       </c>
       <c r="G79">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="H79" s="2">
         <v>45262</v>
       </c>
       <c r="I79">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="J79" t="inlineStr">
         <is>
@@ -8404,7 +8404,7 @@
         <v>45254</v>
       </c>
       <c r="I80">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="J80" t="inlineStr">
         <is>
@@ -8501,13 +8501,13 @@
         <v>45104</v>
       </c>
       <c r="G81">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="H81" s="2">
         <v>45287</v>
       </c>
       <c r="I81">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="J81" t="inlineStr">
         <is>
@@ -8604,7 +8604,7 @@
         <v>45288</v>
       </c>
       <c r="I82">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="J82" t="inlineStr">
         <is>
@@ -8696,13 +8696,13 @@
         <v>45175</v>
       </c>
       <c r="G83">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="H83" s="2">
         <v>45357</v>
       </c>
       <c r="I83">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="J83" t="inlineStr">
         <is>
@@ -8799,13 +8799,13 @@
         <v>45054</v>
       </c>
       <c r="G84">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="H84" s="2">
         <v>45238</v>
       </c>
       <c r="I84">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="J84" t="inlineStr">
         <is>
@@ -8902,13 +8902,13 @@
         <v>45056</v>
       </c>
       <c r="G85">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="H85" s="2">
         <v>45240</v>
       </c>
       <c r="I85">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="J85" t="inlineStr">
         <is>
@@ -9005,13 +9005,13 @@
         <v>45085</v>
       </c>
       <c r="G86">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="H86" s="2">
         <v>45268</v>
       </c>
       <c r="I86">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="J86" t="inlineStr">
         <is>
@@ -9108,7 +9108,7 @@
         <v>45194</v>
       </c>
       <c r="I87">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="J87" t="inlineStr">
         <is>
@@ -9195,13 +9195,13 @@
         <v>45103</v>
       </c>
       <c r="G88">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="H88" s="2">
         <v>45286</v>
       </c>
       <c r="I88">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="J88" t="inlineStr">
         <is>
@@ -9298,13 +9298,13 @@
         <v>45103</v>
       </c>
       <c r="G89">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="H89" s="2">
         <v>45286</v>
       </c>
       <c r="I89">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="J89" t="inlineStr">
         <is>
@@ -9401,13 +9401,13 @@
         <v>45008</v>
       </c>
       <c r="G90">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="H90" s="2">
         <v>45192</v>
       </c>
       <c r="I90">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J90" t="inlineStr">
         <is>
@@ -9499,13 +9499,13 @@
         <v>45100</v>
       </c>
       <c r="G91">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="H91" s="2">
         <v>45287</v>
       </c>
       <c r="I91">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="J91" t="inlineStr">
         <is>
@@ -9602,13 +9602,13 @@
         <v>45003</v>
       </c>
       <c r="G92">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="H92" s="2">
         <v>45187</v>
       </c>
       <c r="I92">
-        <v>-4</v>
+        <v>-5</v>
       </c>
       <c r="J92" t="inlineStr">
         <is>
@@ -9705,13 +9705,13 @@
         <v>45104</v>
       </c>
       <c r="G93">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="H93" s="2">
         <v>45287</v>
       </c>
       <c r="I93">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="J93" t="inlineStr">
         <is>
@@ -9808,13 +9808,13 @@
         <v>45104</v>
       </c>
       <c r="G94">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="H94" s="2">
         <v>45287</v>
       </c>
       <c r="I94">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="J94" t="inlineStr">
         <is>
@@ -9911,13 +9911,13 @@
         <v>45049</v>
       </c>
       <c r="G95">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="H95" s="2">
         <v>45233</v>
       </c>
       <c r="I95">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="J95" t="inlineStr">
         <is>
@@ -10014,13 +10014,13 @@
         <v>45122</v>
       </c>
       <c r="G96">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="H96" s="2">
         <v>45306</v>
       </c>
       <c r="I96">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="J96" t="inlineStr">
         <is>
@@ -10112,13 +10112,13 @@
         <v>45141</v>
       </c>
       <c r="G97">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="H97" s="2">
         <v>45325</v>
       </c>
       <c r="I97">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="J97" t="inlineStr">
         <is>
@@ -10215,13 +10215,13 @@
         <v>45010</v>
       </c>
       <c r="G98">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="H98" s="2">
         <v>45194</v>
       </c>
       <c r="I98">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="J98" t="inlineStr">
         <is>
@@ -10313,13 +10313,13 @@
         <v>45093</v>
       </c>
       <c r="G99">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="H99" s="2">
         <v>45276</v>
       </c>
       <c r="I99">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="J99" t="inlineStr">
         <is>
@@ -10416,13 +10416,13 @@
         <v>45123</v>
       </c>
       <c r="G100">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="H100" s="2">
         <v>45307</v>
       </c>
       <c r="I100">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="J100" t="inlineStr">
         <is>
@@ -10519,13 +10519,13 @@
         <v>45014</v>
       </c>
       <c r="G101">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="H101" s="2">
         <v>45198</v>
       </c>
       <c r="I101">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="J101" t="inlineStr">
         <is>
@@ -10622,13 +10622,13 @@
         <v>45093</v>
       </c>
       <c r="G102">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="H102" s="2">
         <v>45276</v>
       </c>
       <c r="I102">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="J102" t="inlineStr">
         <is>
@@ -10725,13 +10725,13 @@
         <v>45122</v>
       </c>
       <c r="G103">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="H103" s="2">
         <v>45306</v>
       </c>
       <c r="I103">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="J103" t="inlineStr">
         <is>
@@ -10828,13 +10828,13 @@
         <v>45122</v>
       </c>
       <c r="G104">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="H104" s="2">
         <v>45306</v>
       </c>
       <c r="I104">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="J104" t="inlineStr">
         <is>
@@ -10926,13 +10926,13 @@
         <v>45050</v>
       </c>
       <c r="G105">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="H105" s="2">
         <v>45234</v>
       </c>
       <c r="I105">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="J105" t="inlineStr">
         <is>
@@ -11029,13 +11029,13 @@
         <v>45085</v>
       </c>
       <c r="G106">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="H106" s="2">
         <v>45268</v>
       </c>
       <c r="I106">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="J106" t="inlineStr">
         <is>
@@ -11132,13 +11132,13 @@
         <v>45093</v>
       </c>
       <c r="G107">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="H107" s="2">
         <v>45185</v>
       </c>
       <c r="I107">
-        <v>-6</v>
+        <v>-7</v>
       </c>
       <c r="J107" t="inlineStr">
         <is>
@@ -11230,13 +11230,13 @@
         <v>45093</v>
       </c>
       <c r="G108">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="H108" s="2">
         <v>45185</v>
       </c>
       <c r="I108">
-        <v>-6</v>
+        <v>-7</v>
       </c>
       <c r="J108" t="inlineStr">
         <is>
@@ -11328,13 +11328,13 @@
         <v>45093</v>
       </c>
       <c r="G109">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="H109" s="2">
         <v>45185</v>
       </c>
       <c r="I109">
-        <v>-6</v>
+        <v>-7</v>
       </c>
       <c r="J109" t="inlineStr">
         <is>
@@ -11431,13 +11431,13 @@
         <v>45148</v>
       </c>
       <c r="G110">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="H110" s="2">
         <v>45240</v>
       </c>
       <c r="I110">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="J110" t="inlineStr">
         <is>
@@ -11534,13 +11534,13 @@
         <v>45119</v>
       </c>
       <c r="G111">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="H111" s="2">
         <v>45211</v>
       </c>
       <c r="I111">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="J111" t="inlineStr">
         <is>
@@ -11637,13 +11637,13 @@
         <v>45172</v>
       </c>
       <c r="G112">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="H112" s="2">
         <v>45263</v>
       </c>
       <c r="I112">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="J112" t="inlineStr">
         <is>
@@ -11740,13 +11740,13 @@
         <v>45023</v>
       </c>
       <c r="G113">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="H113" s="2">
         <v>45206</v>
       </c>
       <c r="I113">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="J113" t="inlineStr">
         <is>
@@ -11843,13 +11843,13 @@
         <v>45111</v>
       </c>
       <c r="G114">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="H114" s="2">
         <v>45203</v>
       </c>
       <c r="I114">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="J114" t="inlineStr">
         <is>
@@ -11946,7 +11946,7 @@
         <v>45218</v>
       </c>
       <c r="I115">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="J115" t="inlineStr">
         <is>
@@ -12043,13 +12043,13 @@
         <v>45161</v>
       </c>
       <c r="G116">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="H116" s="2">
         <v>45253</v>
       </c>
       <c r="I116">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="J116" t="inlineStr">
         <is>
@@ -12146,13 +12146,13 @@
         <v>45115</v>
       </c>
       <c r="G117">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="H117" s="2">
         <v>45299</v>
       </c>
       <c r="I117">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="J117" t="inlineStr">
         <is>
@@ -12244,13 +12244,13 @@
         <v>45094</v>
       </c>
       <c r="G118">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="H118" s="2">
         <v>45277</v>
       </c>
       <c r="I118">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="J118" t="inlineStr">
         <is>
@@ -12347,13 +12347,13 @@
         <v>45104</v>
       </c>
       <c r="G119">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="H119" s="2">
         <v>45287</v>
       </c>
       <c r="I119">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="J119" t="inlineStr">
         <is>
@@ -12450,13 +12450,13 @@
         <v>45104</v>
       </c>
       <c r="G120">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="H120" s="2">
         <v>45287</v>
       </c>
       <c r="I120">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="J120" t="inlineStr">
         <is>
@@ -12553,13 +12553,13 @@
         <v>45104</v>
       </c>
       <c r="G121">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="H121" s="2">
         <v>45287</v>
       </c>
       <c r="I121">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="J121" t="inlineStr">
         <is>
@@ -12656,13 +12656,13 @@
         <v>45104</v>
       </c>
       <c r="G122">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="H122" s="2">
         <v>45287</v>
       </c>
       <c r="I122">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="J122" t="inlineStr">
         <is>
@@ -12759,13 +12759,13 @@
         <v>45107</v>
       </c>
       <c r="G123">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="H123" s="2">
         <v>45199</v>
       </c>
       <c r="I123">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="J123" t="inlineStr">
         <is>
@@ -12862,13 +12862,13 @@
         <v>45013</v>
       </c>
       <c r="G124">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="H124" s="2">
         <v>45197</v>
       </c>
       <c r="I124">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="J124" t="inlineStr">
         <is>
@@ -12965,13 +12965,13 @@
         <v>45121</v>
       </c>
       <c r="G125">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="H125" s="2">
         <v>45213</v>
       </c>
       <c r="I125">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="J125" t="inlineStr">
         <is>
@@ -13068,13 +13068,13 @@
         <v>45134</v>
       </c>
       <c r="G126">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="H126" s="2">
         <v>45226</v>
       </c>
       <c r="I126">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="J126" t="inlineStr">
         <is>
@@ -13171,7 +13171,7 @@
         <v>45212</v>
       </c>
       <c r="I127">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="J127" t="inlineStr">
         <is>
@@ -13268,13 +13268,13 @@
         <v>45126</v>
       </c>
       <c r="G128">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="H128" s="2">
         <v>45218</v>
       </c>
       <c r="I128">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="J128" t="inlineStr">
         <is>
@@ -13366,13 +13366,13 @@
         <v>45158</v>
       </c>
       <c r="G129">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="H129" s="2">
         <v>45250</v>
       </c>
       <c r="I129">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="J129" t="inlineStr">
         <is>
@@ -13469,13 +13469,13 @@
         <v>45171</v>
       </c>
       <c r="G130">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="H130" s="2">
         <v>45262</v>
       </c>
       <c r="I130">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="J130" t="inlineStr">
         <is>
@@ -13572,13 +13572,13 @@
         <v>45111</v>
       </c>
       <c r="G131">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="H131" s="2">
         <v>45203</v>
       </c>
       <c r="I131">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="J131" t="inlineStr">
         <is>
@@ -13675,13 +13675,13 @@
         <v>45144</v>
       </c>
       <c r="G132">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="H132" s="2">
         <v>45236</v>
       </c>
       <c r="I132">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="J132" t="inlineStr">
         <is>
@@ -13778,13 +13778,13 @@
         <v>45156</v>
       </c>
       <c r="G133">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="H133" s="2">
         <v>45248</v>
       </c>
       <c r="I133">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="J133" t="inlineStr">
         <is>
@@ -13876,13 +13876,13 @@
         <v>45146</v>
       </c>
       <c r="G134">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="H134" s="2">
         <v>45238</v>
       </c>
       <c r="I134">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="J134" t="inlineStr">
         <is>
@@ -13979,13 +13979,13 @@
         <v>45140</v>
       </c>
       <c r="G135">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="H135" s="2">
         <v>45232</v>
       </c>
       <c r="I135">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="J135" t="inlineStr">
         <is>
@@ -14082,13 +14082,13 @@
         <v>45104</v>
       </c>
       <c r="G136">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="H136" s="2">
         <v>45196</v>
       </c>
       <c r="I136">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="J136" t="inlineStr">
         <is>
@@ -14185,13 +14185,13 @@
         <v>45105</v>
       </c>
       <c r="G137">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="H137" s="2">
         <v>45197</v>
       </c>
       <c r="I137">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="J137" t="inlineStr">
         <is>
@@ -14288,13 +14288,13 @@
         <v>45179</v>
       </c>
       <c r="G138">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="H138" s="2">
         <v>45270</v>
       </c>
       <c r="I138">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="J138" t="inlineStr">
         <is>
@@ -14386,13 +14386,13 @@
         <v>45105</v>
       </c>
       <c r="G139">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="H139" s="2">
         <v>45197</v>
       </c>
       <c r="I139">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="J139" t="inlineStr">
         <is>
@@ -14489,13 +14489,13 @@
         <v>45182</v>
       </c>
       <c r="G140">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="H140" s="2">
         <v>45273</v>
       </c>
       <c r="I140">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="J140" t="inlineStr">
         <is>
@@ -14592,13 +14592,13 @@
         <v>45116</v>
       </c>
       <c r="G141">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="H141" s="2">
         <v>45208</v>
       </c>
       <c r="I141">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="J141" t="inlineStr">
         <is>
@@ -14690,13 +14690,13 @@
         <v>45150</v>
       </c>
       <c r="G142">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="H142" s="2">
         <v>45242</v>
       </c>
       <c r="I142">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="J142" t="inlineStr">
         <is>
@@ -14793,7 +14793,7 @@
         <v>45238</v>
       </c>
       <c r="I143">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="J143" t="inlineStr">
         <is>
@@ -14890,13 +14890,13 @@
         <v>45171</v>
       </c>
       <c r="G144">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="H144" s="2">
         <v>45262</v>
       </c>
       <c r="I144">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="J144" t="inlineStr">
         <is>
@@ -14993,13 +14993,13 @@
         <v>45102</v>
       </c>
       <c r="G145">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="H145" s="2">
         <v>45194</v>
       </c>
       <c r="I145">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="J145" t="inlineStr">
         <is>
@@ -15086,13 +15086,13 @@
         <v>45119</v>
       </c>
       <c r="G146">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="H146" s="2">
         <v>45211</v>
       </c>
       <c r="I146">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="J146" t="inlineStr">
         <is>
@@ -15189,13 +15189,13 @@
         <v>45165</v>
       </c>
       <c r="G147">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="H147" s="2">
         <v>45257</v>
       </c>
       <c r="I147">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="J147" t="inlineStr">
         <is>
@@ -15292,13 +15292,13 @@
         <v>45166</v>
       </c>
       <c r="G148">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="H148" s="2">
         <v>45258</v>
       </c>
       <c r="I148">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="J148" t="inlineStr">
         <is>
@@ -15395,13 +15395,13 @@
         <v>45093</v>
       </c>
       <c r="G149">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="H149" s="2">
         <v>45185</v>
       </c>
       <c r="I149">
-        <v>-6</v>
+        <v>-7</v>
       </c>
       <c r="J149" t="inlineStr">
         <is>
@@ -15498,13 +15498,13 @@
         <v>45035</v>
       </c>
       <c r="G150">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="H150" s="2">
         <v>45218</v>
       </c>
       <c r="I150">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="J150" t="inlineStr">
         <is>
@@ -15601,13 +15601,13 @@
         <v>45174</v>
       </c>
       <c r="G151">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="H151" s="2">
         <v>45356</v>
       </c>
       <c r="I151">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="J151" t="inlineStr">
         <is>
@@ -15704,13 +15704,13 @@
         <v>45089</v>
       </c>
       <c r="G152">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="H152" s="2">
         <v>45272</v>
       </c>
       <c r="I152">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="J152" t="inlineStr">
         <is>
@@ -15807,13 +15807,13 @@
         <v>45124</v>
       </c>
       <c r="G153">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="H153" s="2">
         <v>45308</v>
       </c>
       <c r="I153">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="J153" t="inlineStr">
         <is>
@@ -15910,13 +15910,13 @@
         <v>45124</v>
       </c>
       <c r="G154">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="H154" s="2">
         <v>45308</v>
       </c>
       <c r="I154">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="J154" t="inlineStr">
         <is>
@@ -16013,13 +16013,13 @@
         <v>45026</v>
       </c>
       <c r="G155">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="H155" s="2">
         <v>45209</v>
       </c>
       <c r="I155">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="J155" t="inlineStr">
         <is>
@@ -16116,13 +16116,13 @@
         <v>45026</v>
       </c>
       <c r="G156">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="H156" s="2">
         <v>45209</v>
       </c>
       <c r="I156">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="J156" t="inlineStr">
         <is>
@@ -16219,13 +16219,13 @@
         <v>45026</v>
       </c>
       <c r="G157">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="H157" s="2">
         <v>45209</v>
       </c>
       <c r="I157">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="J157" t="inlineStr">
         <is>
@@ -16322,13 +16322,13 @@
         <v>45026</v>
       </c>
       <c r="G158">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="H158" s="2">
         <v>45209</v>
       </c>
       <c r="I158">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="J158" t="inlineStr">
         <is>
@@ -16425,13 +16425,13 @@
         <v>45156</v>
       </c>
       <c r="G159">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="H159" s="2">
         <v>45247</v>
       </c>
       <c r="I159">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="J159" t="inlineStr">
         <is>
@@ -16528,13 +16528,13 @@
         <v>45153</v>
       </c>
       <c r="G160">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="H160" s="2">
         <v>45245</v>
       </c>
       <c r="I160">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="J160" t="inlineStr">
         <is>
@@ -16631,13 +16631,13 @@
         <v>45135</v>
       </c>
       <c r="G161">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="H161" s="2">
         <v>45319</v>
       </c>
       <c r="I161">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="J161" t="inlineStr">
         <is>
@@ -16734,13 +16734,13 @@
         <v>45091</v>
       </c>
       <c r="G162">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="H162" s="2">
         <v>45274</v>
       </c>
       <c r="I162">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="J162" t="inlineStr">
         <is>
@@ -16832,13 +16832,13 @@
         <v>45091</v>
       </c>
       <c r="G163">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="H163" s="2">
         <v>45274</v>
       </c>
       <c r="I163">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="J163" t="inlineStr">
         <is>
@@ -16930,13 +16930,13 @@
         <v>45138</v>
       </c>
       <c r="G164">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="H164" s="2">
         <v>45322</v>
       </c>
       <c r="I164">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="J164" t="inlineStr">
         <is>
@@ -17033,13 +17033,13 @@
         <v>45138</v>
       </c>
       <c r="G165">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="H165" s="2">
         <v>45322</v>
       </c>
       <c r="I165">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="J165" t="inlineStr">
         <is>
@@ -17136,13 +17136,13 @@
         <v>45085</v>
       </c>
       <c r="G166">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="H166" s="2">
         <v>45268</v>
       </c>
       <c r="I166">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="J166" t="inlineStr">
         <is>
@@ -17239,13 +17239,13 @@
         <v>45085</v>
       </c>
       <c r="G167">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="H167" s="2">
         <v>45268</v>
       </c>
       <c r="I167">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="J167" t="inlineStr">
         <is>
@@ -17342,7 +17342,7 @@
         <v>45326</v>
       </c>
       <c r="I168">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="J168" t="inlineStr">
         <is>
@@ -17439,13 +17439,13 @@
         <v>45173</v>
       </c>
       <c r="G169">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="H169" s="2">
         <v>45355</v>
       </c>
       <c r="I169">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="J169" t="inlineStr">
         <is>
@@ -17542,13 +17542,13 @@
         <v>45056</v>
       </c>
       <c r="G170">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="H170" s="2">
         <v>45240</v>
       </c>
       <c r="I170">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="J170" t="inlineStr">
         <is>
@@ -17645,7 +17645,7 @@
         <v>45238</v>
       </c>
       <c r="I171">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="J171" t="inlineStr">
         <is>
@@ -17742,13 +17742,13 @@
         <v>45141</v>
       </c>
       <c r="G172">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="H172" s="2">
         <v>45325</v>
       </c>
       <c r="I172">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="J172" t="inlineStr">
         <is>
@@ -17845,13 +17845,13 @@
         <v>45037</v>
       </c>
       <c r="G173">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="H173" s="2">
         <v>45220</v>
       </c>
       <c r="I173">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="J173" t="inlineStr">
         <is>
@@ -17948,13 +17948,13 @@
         <v>45171</v>
       </c>
       <c r="G174">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="H174" s="2">
         <v>45262</v>
       </c>
       <c r="I174">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="J174" t="inlineStr">
         <is>
@@ -18051,13 +18051,13 @@
         <v>45105</v>
       </c>
       <c r="G175">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="H175" s="2">
         <v>45197</v>
       </c>
       <c r="I175">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="J175" t="inlineStr">
         <is>
@@ -18154,13 +18154,13 @@
         <v>45162</v>
       </c>
       <c r="G176">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="H176" s="2">
         <v>45254</v>
       </c>
       <c r="I176">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="J176" t="inlineStr">
         <is>
@@ -18257,13 +18257,13 @@
         <v>45061</v>
       </c>
       <c r="G177">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="H177" s="2">
         <v>45245</v>
       </c>
       <c r="I177">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="J177" t="inlineStr">
         <is>
@@ -18360,13 +18360,13 @@
         <v>45120</v>
       </c>
       <c r="G178">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="H178" s="2">
         <v>45212</v>
       </c>
       <c r="I178">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="J178" t="inlineStr">
         <is>
@@ -18463,7 +18463,7 @@
         <v>45191</v>
       </c>
       <c r="I179">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="J179" t="inlineStr">
         <is>
@@ -18560,13 +18560,13 @@
         <v>45088</v>
       </c>
       <c r="G180">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="H180" s="2">
         <v>45271</v>
       </c>
       <c r="I180">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="J180" t="inlineStr">
         <is>
@@ -18663,13 +18663,13 @@
         <v>45100</v>
       </c>
       <c r="G181">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="H181" s="2">
         <v>45192</v>
       </c>
       <c r="I181">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J181" t="inlineStr">
         <is>
@@ -18756,13 +18756,13 @@
         <v>45131</v>
       </c>
       <c r="G182">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="H182" s="2">
         <v>45223</v>
       </c>
       <c r="I182">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="J182" t="inlineStr">
         <is>
@@ -18854,13 +18854,13 @@
         <v>45136</v>
       </c>
       <c r="G183">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="H183" s="2">
         <v>45228</v>
       </c>
       <c r="I183">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="J183" t="inlineStr">
         <is>
@@ -18952,13 +18952,13 @@
         <v>45150</v>
       </c>
       <c r="G184">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="H184" s="2">
         <v>45242</v>
       </c>
       <c r="I184">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="J184" t="inlineStr">
         <is>
@@ -19050,13 +19050,13 @@
         <v>45118</v>
       </c>
       <c r="G185">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="H185" s="2">
         <v>45210</v>
       </c>
       <c r="I185">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="J185" t="inlineStr">
         <is>
@@ -19148,13 +19148,13 @@
         <v>45129</v>
       </c>
       <c r="G186">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="H186" s="2">
         <v>45221</v>
       </c>
       <c r="I186">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="J186" t="inlineStr">
         <is>
@@ -19246,13 +19246,13 @@
         <v>45097</v>
       </c>
       <c r="G187">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="H187" s="2">
         <v>45189</v>
       </c>
       <c r="I187">
-        <v>-2</v>
+        <v>-3</v>
       </c>
       <c r="J187" t="inlineStr">
         <is>
@@ -19339,13 +19339,13 @@
         <v>45101</v>
       </c>
       <c r="G188">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="H188" s="2">
         <v>45193</v>
       </c>
       <c r="I188">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J188" t="inlineStr">
         <is>
@@ -19432,13 +19432,13 @@
         <v>45165</v>
       </c>
       <c r="G189">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="H189" s="2">
         <v>45257</v>
       </c>
       <c r="I189">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="J189" t="inlineStr">
         <is>
@@ -19530,7 +19530,7 @@
         <v>45202</v>
       </c>
       <c r="I190">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="J190" t="inlineStr">
         <is>
@@ -19627,13 +19627,13 @@
         <v>45081</v>
       </c>
       <c r="G191">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="H191" s="2">
         <v>45264</v>
       </c>
       <c r="I191">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="J191" t="inlineStr">
         <is>
@@ -19730,13 +19730,13 @@
         <v>45081</v>
       </c>
       <c r="G192">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="H192" s="2">
         <v>45264</v>
       </c>
       <c r="I192">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="J192" t="inlineStr">
         <is>
@@ -19833,7 +19833,7 @@
         <v>45319</v>
       </c>
       <c r="I193">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="J193" t="inlineStr">
         <is>
@@ -19930,7 +19930,7 @@
         <v>45319</v>
       </c>
       <c r="I194">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="J194" t="inlineStr">
         <is>
@@ -20022,13 +20022,13 @@
         <v>45046</v>
       </c>
       <c r="G195">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="H195" s="2">
         <v>45230</v>
       </c>
       <c r="I195">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="J195" t="inlineStr">
         <is>
@@ -20125,13 +20125,13 @@
         <v>45046</v>
       </c>
       <c r="G196">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="H196" s="2">
         <v>45230</v>
       </c>
       <c r="I196">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="J196" t="inlineStr">
         <is>
@@ -20228,13 +20228,13 @@
         <v>45031</v>
       </c>
       <c r="G197">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="H197" s="2">
         <v>45214</v>
       </c>
       <c r="I197">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="J197" t="inlineStr">
         <is>
@@ -20331,13 +20331,13 @@
         <v>45031</v>
       </c>
       <c r="G198">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="H198" s="2">
         <v>45214</v>
       </c>
       <c r="I198">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="J198" t="inlineStr">
         <is>
@@ -20434,13 +20434,13 @@
         <v>45031</v>
       </c>
       <c r="G199">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="H199" s="2">
         <v>45214</v>
       </c>
       <c r="I199">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="J199" t="inlineStr">
         <is>
@@ -20537,13 +20537,13 @@
         <v>45031</v>
       </c>
       <c r="G200">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="H200" s="2">
         <v>45214</v>
       </c>
       <c r="I200">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="J200" t="inlineStr">
         <is>
@@ -20640,13 +20640,13 @@
         <v>45067</v>
       </c>
       <c r="G201">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="H201" s="2">
         <v>45251</v>
       </c>
       <c r="I201">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="J201" t="inlineStr">
         <is>
@@ -20743,13 +20743,13 @@
         <v>45067</v>
       </c>
       <c r="G202">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="H202" s="2">
         <v>45251</v>
       </c>
       <c r="I202">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="J202" t="inlineStr">
         <is>
@@ -20846,13 +20846,13 @@
         <v>45067</v>
       </c>
       <c r="G203">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="H203" s="2">
         <v>45251</v>
       </c>
       <c r="I203">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="J203" t="inlineStr">
         <is>
@@ -20949,13 +20949,13 @@
         <v>45067</v>
       </c>
       <c r="G204">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="H204" s="2">
         <v>45251</v>
       </c>
       <c r="I204">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="J204" t="inlineStr">
         <is>
@@ -21052,13 +21052,13 @@
         <v>45178</v>
       </c>
       <c r="G205">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="H205" s="2">
         <v>45269</v>
       </c>
       <c r="I205">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="J205" t="inlineStr">
         <is>
@@ -21155,7 +21155,7 @@
         <v>45252</v>
       </c>
       <c r="I206">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="J206" t="inlineStr">
         <is>
@@ -21252,13 +21252,13 @@
         <v>45087</v>
       </c>
       <c r="G207">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="H207" s="2">
         <v>45270</v>
       </c>
       <c r="I207">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="J207" t="inlineStr">
         <is>
@@ -21355,13 +21355,13 @@
         <v>45099</v>
       </c>
       <c r="G208">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="H208" s="2">
         <v>45282</v>
       </c>
       <c r="I208">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="J208" t="inlineStr">
         <is>
@@ -21458,13 +21458,13 @@
         <v>45175</v>
       </c>
       <c r="G209">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="H209" s="2">
         <v>45356</v>
       </c>
       <c r="I209">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="J209" t="inlineStr">
         <is>
@@ -21561,13 +21561,13 @@
         <v>45175</v>
       </c>
       <c r="G210">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="H210" s="2">
         <v>45356</v>
       </c>
       <c r="I210">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="J210" t="inlineStr">
         <is>
@@ -21664,13 +21664,13 @@
         <v>45166</v>
       </c>
       <c r="G211">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="H211" s="2">
         <v>45350</v>
       </c>
       <c r="I211">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="J211" t="inlineStr">
         <is>
@@ -21767,13 +21767,13 @@
         <v>45166</v>
       </c>
       <c r="G212">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="H212" s="2">
         <v>45350</v>
       </c>
       <c r="I212">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="J212" t="inlineStr">
         <is>
@@ -21870,13 +21870,13 @@
         <v>45090</v>
       </c>
       <c r="G213">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="H213" s="2">
         <v>45273</v>
       </c>
       <c r="I213">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="J213" t="inlineStr">
         <is>
@@ -21973,13 +21973,13 @@
         <v>45106</v>
       </c>
       <c r="G214">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="H214" s="2">
         <v>45289</v>
       </c>
       <c r="I214">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="J214" t="inlineStr">
         <is>
@@ -22076,13 +22076,13 @@
         <v>45134</v>
       </c>
       <c r="G215">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="H215" s="2">
         <v>45226</v>
       </c>
       <c r="I215">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="J215" t="inlineStr">
         <is>
@@ -22179,13 +22179,13 @@
         <v>45132</v>
       </c>
       <c r="G216">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="H216" s="2">
         <v>45224</v>
       </c>
       <c r="I216">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="J216" t="inlineStr">
         <is>
@@ -22282,13 +22282,13 @@
         <v>45150</v>
       </c>
       <c r="G217">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="H217" s="2">
         <v>45242</v>
       </c>
       <c r="I217">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="J217" t="inlineStr">
         <is>
@@ -22385,13 +22385,13 @@
         <v>45095</v>
       </c>
       <c r="G218">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="H218" s="2">
         <v>45187</v>
       </c>
       <c r="I218">
-        <v>-4</v>
+        <v>-5</v>
       </c>
       <c r="J218" t="inlineStr">
         <is>
@@ -22483,13 +22483,13 @@
         <v>45182</v>
       </c>
       <c r="G219">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="H219" s="2">
         <v>45273</v>
       </c>
       <c r="I219">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="J219" t="inlineStr">
         <is>
@@ -22586,7 +22586,7 @@
         <v>45196</v>
       </c>
       <c r="I220">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="J220" t="inlineStr">
         <is>
@@ -22683,13 +22683,13 @@
         <v>45108</v>
       </c>
       <c r="G221">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="H221" s="2">
         <v>45200</v>
       </c>
       <c r="I221">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="J221" t="inlineStr">
         <is>
@@ -22786,13 +22786,13 @@
         <v>45135</v>
       </c>
       <c r="G222">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="H222" s="2">
         <v>45227</v>
       </c>
       <c r="I222">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="J222" t="inlineStr">
         <is>
@@ -22889,13 +22889,13 @@
         <v>45148</v>
       </c>
       <c r="G223">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="H223" s="2">
         <v>45240</v>
       </c>
       <c r="I223">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="J223" t="inlineStr">
         <is>
@@ -22987,13 +22987,13 @@
         <v>45100</v>
       </c>
       <c r="G224">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="H224" s="2">
         <v>45192</v>
       </c>
       <c r="I224">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J224" t="inlineStr">
         <is>
@@ -23085,13 +23085,13 @@
         <v>45136</v>
       </c>
       <c r="G225">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="H225" s="2">
         <v>45320</v>
       </c>
       <c r="I225">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="J225" t="inlineStr">
         <is>
@@ -23188,13 +23188,13 @@
         <v>45136</v>
       </c>
       <c r="G226">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="H226" s="2">
         <v>45320</v>
       </c>
       <c r="I226">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="J226" t="inlineStr">
         <is>
@@ -23291,13 +23291,13 @@
         <v>45094</v>
       </c>
       <c r="G227">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="H227" s="2">
         <v>45277</v>
       </c>
       <c r="I227">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="J227" t="inlineStr">
         <is>
@@ -23394,13 +23394,13 @@
         <v>45081</v>
       </c>
       <c r="G228">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="H228" s="2">
         <v>45264</v>
       </c>
       <c r="I228">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="J228" t="inlineStr">
         <is>
@@ -23497,13 +23497,13 @@
         <v>45099</v>
       </c>
       <c r="G229">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="H229" s="2">
         <v>45282</v>
       </c>
       <c r="I229">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="J229" t="inlineStr">
         <is>
@@ -23600,13 +23600,13 @@
         <v>45018</v>
       </c>
       <c r="G230">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="H230" s="2">
         <v>45201</v>
       </c>
       <c r="I230">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="J230" t="inlineStr">
         <is>
@@ -23703,13 +23703,13 @@
         <v>45031</v>
       </c>
       <c r="G231">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="H231" s="2">
         <v>45214</v>
       </c>
       <c r="I231">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="J231" t="inlineStr">
         <is>
@@ -23806,7 +23806,7 @@
         <v>45294</v>
       </c>
       <c r="I232">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="J232" t="inlineStr">
         <is>
@@ -23903,13 +23903,13 @@
         <v>45079</v>
       </c>
       <c r="G233">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="H233" s="2">
         <v>45262</v>
       </c>
       <c r="I233">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="J233" t="inlineStr">
         <is>
@@ -24006,7 +24006,7 @@
         <v>45199</v>
       </c>
       <c r="I234">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="J234" t="inlineStr">
         <is>
@@ -24103,13 +24103,13 @@
         <v>45021</v>
       </c>
       <c r="G235">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="H235" s="2">
         <v>45204</v>
       </c>
       <c r="I235">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="J235" t="inlineStr">
         <is>
@@ -24206,13 +24206,13 @@
         <v>45021</v>
       </c>
       <c r="G236">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="H236" s="2">
         <v>45204</v>
       </c>
       <c r="I236">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="J236" t="inlineStr">
         <is>
@@ -24309,13 +24309,13 @@
         <v>45080</v>
       </c>
       <c r="G237">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="H237" s="2">
         <v>45263</v>
       </c>
       <c r="I237">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="J237" t="inlineStr">
         <is>
@@ -24412,13 +24412,13 @@
         <v>45046</v>
       </c>
       <c r="G238">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="H238" s="2">
         <v>45229</v>
       </c>
       <c r="I238">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="J238" t="inlineStr">
         <is>
@@ -24515,13 +24515,13 @@
         <v>45112</v>
       </c>
       <c r="G239">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="H239" s="2">
         <v>45204</v>
       </c>
       <c r="I239">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="J239" t="inlineStr">
         <is>
@@ -24609,13 +24609,13 @@
         <v>45112</v>
       </c>
       <c r="G240">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="H240" s="2">
         <v>45204</v>
       </c>
       <c r="I240">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="J240" t="inlineStr">
         <is>
@@ -24703,13 +24703,13 @@
         <v>45016</v>
       </c>
       <c r="G241">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="H241" s="2">
         <v>45199</v>
       </c>
       <c r="I241">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="J241" t="inlineStr">
         <is>
@@ -24806,13 +24806,13 @@
         <v>45070</v>
       </c>
       <c r="G242">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="H242" s="2">
         <v>45254</v>
       </c>
       <c r="I242">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="J242" t="inlineStr">
         <is>
@@ -24909,13 +24909,13 @@
         <v>45168</v>
       </c>
       <c r="G243">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="H243" s="2">
         <v>45260</v>
       </c>
       <c r="I243">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="J243" t="inlineStr">
         <is>
@@ -25012,13 +25012,13 @@
         <v>45027</v>
       </c>
       <c r="G244">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="H244" s="2">
         <v>45210</v>
       </c>
       <c r="I244">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="J244" t="inlineStr">
         <is>
@@ -25115,13 +25115,13 @@
         <v>45077</v>
       </c>
       <c r="G245">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="H245" s="2">
         <v>45260</v>
       </c>
       <c r="I245">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="J245" t="inlineStr">
         <is>
@@ -25218,13 +25218,13 @@
         <v>45100</v>
       </c>
       <c r="G246">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="H246" s="2">
         <v>45283</v>
       </c>
       <c r="I246">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="J246" t="inlineStr">
         <is>
@@ -25321,7 +25321,7 @@
         <v>45281</v>
       </c>
       <c r="I247">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="J247" t="inlineStr">
         <is>
@@ -25418,13 +25418,13 @@
         <v>45044</v>
       </c>
       <c r="G248">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="H248" s="2">
         <v>45227</v>
       </c>
       <c r="I248">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="J248" t="inlineStr">
         <is>
@@ -25521,13 +25521,13 @@
         <v>45101</v>
       </c>
       <c r="G249">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="H249" s="2">
         <v>45283</v>
       </c>
       <c r="I249">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="J249" t="inlineStr">
         <is>
@@ -25624,13 +25624,13 @@
         <v>45134</v>
       </c>
       <c r="G250">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="H250" s="2">
         <v>45226</v>
       </c>
       <c r="I250">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="J250" t="inlineStr">
         <is>
@@ -25727,13 +25727,13 @@
         <v>45158</v>
       </c>
       <c r="G251">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="H251" s="2">
         <v>45250</v>
       </c>
       <c r="I251">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="J251" t="inlineStr">
         <is>
@@ -25830,13 +25830,13 @@
         <v>45108</v>
       </c>
       <c r="G252">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="H252" s="2">
         <v>45200</v>
       </c>
       <c r="I252">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="J252" t="inlineStr">
         <is>
@@ -25933,7 +25933,7 @@
         <v>45317</v>
       </c>
       <c r="I253">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="J253" t="inlineStr">
         <is>
@@ -26030,13 +26030,13 @@
         <v>45039</v>
       </c>
       <c r="G254">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="H254" s="2">
         <v>45222</v>
       </c>
       <c r="I254">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="J254" t="inlineStr">
         <is>
@@ -26128,13 +26128,13 @@
         <v>45129</v>
       </c>
       <c r="G255">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="H255" s="2">
         <v>45221</v>
       </c>
       <c r="I255">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="J255" t="inlineStr">
         <is>
@@ -26231,13 +26231,13 @@
         <v>45157</v>
       </c>
       <c r="G256">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="H256" s="2">
         <v>45341</v>
       </c>
       <c r="I256">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="J256" t="inlineStr">
         <is>
@@ -26334,13 +26334,13 @@
         <v>45063</v>
       </c>
       <c r="G257">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="H257" s="2">
         <v>45247</v>
       </c>
       <c r="I257">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="J257" t="inlineStr">
         <is>
@@ -26437,7 +26437,7 @@
         <v>45254</v>
       </c>
       <c r="I258">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="J258" t="inlineStr">
         <is>
@@ -26534,7 +26534,7 @@
         <v>45486</v>
       </c>
       <c r="I259">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="J259" t="inlineStr">
         <is>
@@ -26626,13 +26626,13 @@
         <v>45073</v>
       </c>
       <c r="G260">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="H260" s="2">
         <v>45439</v>
       </c>
       <c r="I260">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="J260" t="inlineStr">
         <is>
@@ -26724,7 +26724,7 @@
         <v>45323</v>
       </c>
       <c r="I261">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="J261" t="inlineStr">
         <is>
@@ -26816,7 +26816,7 @@
         <v>45303</v>
       </c>
       <c r="I262">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="J262" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
Bond dates update Sun Sep 24 23:08:30 UTC 2023
</commit_message>
<xml_diff>
--- a/Data/obligacje_screener.xlsx
+++ b/Data/obligacje_screener.xlsx
@@ -512,7 +512,7 @@
         <v>45340</v>
       </c>
       <c r="I2">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="J2" t="inlineStr">
         <is>
@@ -600,13 +600,13 @@
         <v>45121</v>
       </c>
       <c r="G3">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="H3" s="2">
         <v>45305</v>
       </c>
       <c r="I3">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="J3" t="inlineStr">
         <is>
@@ -703,13 +703,13 @@
         <v>45039</v>
       </c>
       <c r="G4">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="H4" s="2">
         <v>45222</v>
       </c>
       <c r="I4">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="J4" t="inlineStr">
         <is>
@@ -806,13 +806,13 @@
         <v>45039</v>
       </c>
       <c r="G5">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="H5" s="2">
         <v>45222</v>
       </c>
       <c r="I5">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="J5" t="inlineStr">
         <is>
@@ -909,13 +909,13 @@
         <v>45129</v>
       </c>
       <c r="G6">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="H6" s="2">
         <v>45221</v>
       </c>
       <c r="I6">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="J6" t="inlineStr">
         <is>
@@ -1012,13 +1012,13 @@
         <v>45162</v>
       </c>
       <c r="G7">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="H7" s="2">
         <v>45254</v>
       </c>
       <c r="I7">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="J7" t="inlineStr">
         <is>
@@ -1110,13 +1110,13 @@
         <v>45156</v>
       </c>
       <c r="G8">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="H8" s="2">
         <v>45248</v>
       </c>
       <c r="I8">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="J8" t="inlineStr">
         <is>
@@ -1213,13 +1213,13 @@
         <v>45141</v>
       </c>
       <c r="G9">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="H9" s="2">
         <v>45233</v>
       </c>
       <c r="I9">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="J9" t="inlineStr">
         <is>
@@ -1316,13 +1316,13 @@
         <v>45062</v>
       </c>
       <c r="G10">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="H10" s="2">
         <v>45246</v>
       </c>
       <c r="I10">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="J10" t="inlineStr">
         <is>
@@ -1419,7 +1419,7 @@
         <v>45286</v>
       </c>
       <c r="I11">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="J11" t="inlineStr">
         <is>
@@ -1516,13 +1516,13 @@
         <v>45011</v>
       </c>
       <c r="G12">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="H12" s="2">
         <v>45195</v>
       </c>
       <c r="I12">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="J12" t="inlineStr">
         <is>
@@ -1614,13 +1614,13 @@
         <v>45036</v>
       </c>
       <c r="G13">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="H13" s="2">
         <v>45219</v>
       </c>
       <c r="I13">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="J13" t="inlineStr">
         <is>
@@ -1717,13 +1717,13 @@
         <v>45036</v>
       </c>
       <c r="G14">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="H14" s="2">
         <v>45219</v>
       </c>
       <c r="I14">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="J14" t="inlineStr">
         <is>
@@ -1820,13 +1820,13 @@
         <v>45106</v>
       </c>
       <c r="G15">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="H15" s="2">
         <v>45289</v>
       </c>
       <c r="I15">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="J15" t="inlineStr">
         <is>
@@ -1923,13 +1923,13 @@
         <v>45094</v>
       </c>
       <c r="G16">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="H16" s="2">
         <v>45186</v>
       </c>
       <c r="I16">
-        <v>-6</v>
+        <v>-7</v>
       </c>
       <c r="J16" t="inlineStr">
         <is>
@@ -2026,13 +2026,13 @@
         <v>45094</v>
       </c>
       <c r="G17">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="H17" s="2">
         <v>45186</v>
       </c>
       <c r="I17">
-        <v>-6</v>
+        <v>-7</v>
       </c>
       <c r="J17" t="inlineStr">
         <is>
@@ -2129,13 +2129,13 @@
         <v>45132</v>
       </c>
       <c r="G18">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="H18" s="2">
         <v>45224</v>
       </c>
       <c r="I18">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="J18" t="inlineStr">
         <is>
@@ -2232,13 +2232,13 @@
         <v>45137</v>
       </c>
       <c r="G19">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="H19" s="2">
         <v>45229</v>
       </c>
       <c r="I19">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="J19" t="inlineStr">
         <is>
@@ -2330,13 +2330,13 @@
         <v>45183</v>
       </c>
       <c r="G20">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="H20" s="2">
         <v>45274</v>
       </c>
       <c r="I20">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="J20" t="inlineStr">
         <is>
@@ -2433,13 +2433,13 @@
         <v>45093</v>
       </c>
       <c r="G21">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="H21" s="2">
         <v>45187</v>
       </c>
       <c r="I21">
-        <v>-5</v>
+        <v>-6</v>
       </c>
       <c r="J21" t="inlineStr">
         <is>
@@ -2536,13 +2536,13 @@
         <v>45096</v>
       </c>
       <c r="G22">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="H22" s="2">
         <v>45187</v>
       </c>
       <c r="I22">
-        <v>-5</v>
+        <v>-6</v>
       </c>
       <c r="J22" t="inlineStr">
         <is>
@@ -2639,7 +2639,7 @@
         <v>45245</v>
       </c>
       <c r="I23">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="J23" t="inlineStr">
         <is>
@@ -2736,7 +2736,7 @@
         <v>45245</v>
       </c>
       <c r="I24">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="J24" t="inlineStr">
         <is>
@@ -2833,13 +2833,13 @@
         <v>45021</v>
       </c>
       <c r="G25">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="H25" s="2">
         <v>45204</v>
       </c>
       <c r="I25">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="J25" t="inlineStr">
         <is>
@@ -2936,13 +2936,13 @@
         <v>45160</v>
       </c>
       <c r="G26">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="H26" s="2">
         <v>45344</v>
       </c>
       <c r="I26">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="J26" t="inlineStr">
         <is>
@@ -3039,13 +3039,13 @@
         <v>45118</v>
       </c>
       <c r="G27">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="H27" s="2">
         <v>45302</v>
       </c>
       <c r="I27">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="J27" t="inlineStr">
         <is>
@@ -3142,13 +3142,13 @@
         <v>45085</v>
       </c>
       <c r="G28">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="H28" s="2">
         <v>45268</v>
       </c>
       <c r="I28">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="J28" t="inlineStr">
         <is>
@@ -3245,13 +3245,13 @@
         <v>45183</v>
       </c>
       <c r="G29">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="H29" s="2">
         <v>45274</v>
       </c>
       <c r="I29">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="J29" t="inlineStr">
         <is>
@@ -3348,7 +3348,7 @@
         <v>45224</v>
       </c>
       <c r="I30">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="J30" t="inlineStr">
         <is>
@@ -3445,13 +3445,13 @@
         <v>45153</v>
       </c>
       <c r="G31">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="H31" s="2">
         <v>45245</v>
       </c>
       <c r="I31">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="J31" t="inlineStr">
         <is>
@@ -3548,13 +3548,13 @@
         <v>45155</v>
       </c>
       <c r="G32">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="H32" s="2">
         <v>45247</v>
       </c>
       <c r="I32">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="J32" t="inlineStr">
         <is>
@@ -3651,7 +3651,7 @@
         <v>45255</v>
       </c>
       <c r="I33">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="J33" t="inlineStr">
         <is>
@@ -3739,13 +3739,13 @@
         <v>45176</v>
       </c>
       <c r="G34">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="H34" s="2">
         <v>45267</v>
       </c>
       <c r="I34">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="J34" t="inlineStr">
         <is>
@@ -3842,13 +3842,13 @@
         <v>45130</v>
       </c>
       <c r="G35">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="H35" s="2">
         <v>45222</v>
       </c>
       <c r="I35">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="J35" t="inlineStr">
         <is>
@@ -3940,13 +3940,13 @@
         <v>45115</v>
       </c>
       <c r="G36">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="H36" s="2">
         <v>45207</v>
       </c>
       <c r="I36">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="J36" t="inlineStr">
         <is>
@@ -4043,13 +4043,13 @@
         <v>45097</v>
       </c>
       <c r="G37">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="H37" s="2">
         <v>45189</v>
       </c>
       <c r="I37">
-        <v>-3</v>
+        <v>-4</v>
       </c>
       <c r="J37" t="inlineStr">
         <is>
@@ -4141,13 +4141,13 @@
         <v>45107</v>
       </c>
       <c r="G38">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="H38" s="2">
         <v>45290</v>
       </c>
       <c r="I38">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="J38" t="inlineStr">
         <is>
@@ -4244,13 +4244,13 @@
         <v>45063</v>
       </c>
       <c r="G39">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="H39" s="2">
         <v>45247</v>
       </c>
       <c r="I39">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="J39" t="inlineStr">
         <is>
@@ -4347,13 +4347,13 @@
         <v>45177</v>
       </c>
       <c r="G40">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H40" s="2">
         <v>45359</v>
       </c>
       <c r="I40">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="J40" t="inlineStr">
         <is>
@@ -4450,13 +4450,13 @@
         <v>45107</v>
       </c>
       <c r="G41">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="H41" s="2">
         <v>45290</v>
       </c>
       <c r="I41">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="J41" t="inlineStr">
         <is>
@@ -4553,7 +4553,7 @@
         <v>45265</v>
       </c>
       <c r="I42">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="J42" t="inlineStr">
         <is>
@@ -4650,13 +4650,13 @@
         <v>45098</v>
       </c>
       <c r="G43">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="H43" s="2">
         <v>45281</v>
       </c>
       <c r="I43">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="J43" t="inlineStr">
         <is>
@@ -4753,13 +4753,13 @@
         <v>45099</v>
       </c>
       <c r="G44">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="H44" s="2">
         <v>45282</v>
       </c>
       <c r="I44">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="J44" t="inlineStr">
         <is>
@@ -4856,13 +4856,13 @@
         <v>45106</v>
       </c>
       <c r="G45">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="H45" s="2">
         <v>45289</v>
       </c>
       <c r="I45">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="J45" t="inlineStr">
         <is>
@@ -4959,13 +4959,13 @@
         <v>45106</v>
       </c>
       <c r="G46">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="H46" s="2">
         <v>45289</v>
       </c>
       <c r="I46">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="J46" t="inlineStr">
         <is>
@@ -5062,13 +5062,13 @@
         <v>45120</v>
       </c>
       <c r="G47">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="H47" s="2">
         <v>45304</v>
       </c>
       <c r="I47">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="J47" t="inlineStr">
         <is>
@@ -5165,13 +5165,13 @@
         <v>45118</v>
       </c>
       <c r="G48">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="H48" s="2">
         <v>45302</v>
       </c>
       <c r="I48">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="J48" t="inlineStr">
         <is>
@@ -5268,13 +5268,13 @@
         <v>45152</v>
       </c>
       <c r="G49">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="H49" s="2">
         <v>45336</v>
       </c>
       <c r="I49">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="J49" t="inlineStr">
         <is>
@@ -5371,13 +5371,13 @@
         <v>45042</v>
       </c>
       <c r="G50">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="H50" s="2">
         <v>45225</v>
       </c>
       <c r="I50">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="J50" t="inlineStr">
         <is>
@@ -5474,13 +5474,13 @@
         <v>45122</v>
       </c>
       <c r="G51">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="H51" s="2">
         <v>45306</v>
       </c>
       <c r="I51">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="J51" t="inlineStr">
         <is>
@@ -5577,13 +5577,13 @@
         <v>45139</v>
       </c>
       <c r="G52">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="H52" s="2">
         <v>45323</v>
       </c>
       <c r="I52">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="J52" t="inlineStr">
         <is>
@@ -5671,13 +5671,13 @@
         <v>45099</v>
       </c>
       <c r="G53">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="H53" s="2">
         <v>45282</v>
       </c>
       <c r="I53">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="J53" t="inlineStr">
         <is>
@@ -5774,7 +5774,7 @@
         <v>45196</v>
       </c>
       <c r="I54">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="J54" t="inlineStr">
         <is>
@@ -5871,13 +5871,13 @@
         <v>45044</v>
       </c>
       <c r="G55">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="H55" s="2">
         <v>45227</v>
       </c>
       <c r="I55">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="J55" t="inlineStr">
         <is>
@@ -5974,13 +5974,13 @@
         <v>45151</v>
       </c>
       <c r="G56">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="H56" s="2">
         <v>45243</v>
       </c>
       <c r="I56">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="J56" t="inlineStr">
         <is>
@@ -6072,7 +6072,7 @@
         <v>45196</v>
       </c>
       <c r="I57">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="J57" t="inlineStr">
         <is>
@@ -6169,13 +6169,13 @@
         <v>45069</v>
       </c>
       <c r="G58">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="H58" s="2">
         <v>45253</v>
       </c>
       <c r="I58">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="J58" t="inlineStr">
         <is>
@@ -6272,13 +6272,13 @@
         <v>45099</v>
       </c>
       <c r="G59">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="H59" s="2">
         <v>45191</v>
       </c>
       <c r="I59">
-        <v>-1</v>
+        <v>-2</v>
       </c>
       <c r="J59" t="inlineStr">
         <is>
@@ -6370,13 +6370,13 @@
         <v>45113</v>
       </c>
       <c r="G60">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="H60" s="2">
         <v>45205</v>
       </c>
       <c r="I60">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="J60" t="inlineStr">
         <is>
@@ -6473,13 +6473,13 @@
         <v>45127</v>
       </c>
       <c r="G61">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="H61" s="2">
         <v>45219</v>
       </c>
       <c r="I61">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="J61" t="inlineStr">
         <is>
@@ -6576,13 +6576,13 @@
         <v>45058</v>
       </c>
       <c r="G62">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="H62" s="2">
         <v>45242</v>
       </c>
       <c r="I62">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="J62" t="inlineStr">
         <is>
@@ -6679,13 +6679,13 @@
         <v>45010</v>
       </c>
       <c r="G63">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="H63" s="2">
         <v>45194</v>
       </c>
       <c r="I63">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J63" t="inlineStr">
         <is>
@@ -6777,13 +6777,13 @@
         <v>45025</v>
       </c>
       <c r="G64">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="H64" s="2">
         <v>45208</v>
       </c>
       <c r="I64">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="J64" t="inlineStr">
         <is>
@@ -6880,13 +6880,13 @@
         <v>45025</v>
       </c>
       <c r="G65">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="H65" s="2">
         <v>45208</v>
       </c>
       <c r="I65">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="J65" t="inlineStr">
         <is>
@@ -6983,13 +6983,13 @@
         <v>45089</v>
       </c>
       <c r="G66">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="H66" s="2">
         <v>45272</v>
       </c>
       <c r="I66">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="J66" t="inlineStr">
         <is>
@@ -7086,13 +7086,13 @@
         <v>45178</v>
       </c>
       <c r="G67">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="H67" s="2">
         <v>45269</v>
       </c>
       <c r="I67">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="J67" t="inlineStr">
         <is>
@@ -7184,13 +7184,13 @@
         <v>45104</v>
       </c>
       <c r="G68">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="H68" s="2">
         <v>45196</v>
       </c>
       <c r="I68">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="J68" t="inlineStr">
         <is>
@@ -7287,13 +7287,13 @@
         <v>45149</v>
       </c>
       <c r="G69">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="H69" s="2">
         <v>45241</v>
       </c>
       <c r="I69">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="J69" t="inlineStr">
         <is>
@@ -7390,7 +7390,7 @@
         <v>45205</v>
       </c>
       <c r="I70">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="J70" t="inlineStr">
         <is>
@@ -7487,13 +7487,13 @@
         <v>45114</v>
       </c>
       <c r="G71">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="H71" s="2">
         <v>45205</v>
       </c>
       <c r="I71">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="J71" t="inlineStr">
         <is>
@@ -7590,13 +7590,13 @@
         <v>45115</v>
       </c>
       <c r="G72">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="H72" s="2">
         <v>45207</v>
       </c>
       <c r="I72">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="J72" t="inlineStr">
         <is>
@@ -7693,13 +7693,13 @@
         <v>45097</v>
       </c>
       <c r="G73">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="H73" s="2">
         <v>45189</v>
       </c>
       <c r="I73">
-        <v>-3</v>
+        <v>-4</v>
       </c>
       <c r="J73" t="inlineStr">
         <is>
@@ -7791,13 +7791,13 @@
         <v>45038</v>
       </c>
       <c r="G74">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="H74" s="2">
         <v>45221</v>
       </c>
       <c r="I74">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="J74" t="inlineStr">
         <is>
@@ -7889,13 +7889,13 @@
         <v>45117</v>
       </c>
       <c r="G75">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="H75" s="2">
         <v>45301</v>
       </c>
       <c r="I75">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="J75" t="inlineStr">
         <is>
@@ -7992,13 +7992,13 @@
         <v>45160</v>
       </c>
       <c r="G76">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="H76" s="2">
         <v>45344</v>
       </c>
       <c r="I76">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="J76" t="inlineStr">
         <is>
@@ -8095,13 +8095,13 @@
         <v>45002</v>
       </c>
       <c r="G77">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="H77" s="2">
         <v>45186</v>
       </c>
       <c r="I77">
-        <v>-6</v>
+        <v>-7</v>
       </c>
       <c r="J77" t="inlineStr">
         <is>
@@ -8198,13 +8198,13 @@
         <v>45043</v>
       </c>
       <c r="G78">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="H78" s="2">
         <v>45226</v>
       </c>
       <c r="I78">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="J78" t="inlineStr">
         <is>
@@ -8301,13 +8301,13 @@
         <v>45079</v>
       </c>
       <c r="G79">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="H79" s="2">
         <v>45262</v>
       </c>
       <c r="I79">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="J79" t="inlineStr">
         <is>
@@ -8404,7 +8404,7 @@
         <v>45254</v>
       </c>
       <c r="I80">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="J80" t="inlineStr">
         <is>
@@ -8501,13 +8501,13 @@
         <v>45104</v>
       </c>
       <c r="G81">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="H81" s="2">
         <v>45287</v>
       </c>
       <c r="I81">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="J81" t="inlineStr">
         <is>
@@ -8604,7 +8604,7 @@
         <v>45288</v>
       </c>
       <c r="I82">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="J82" t="inlineStr">
         <is>
@@ -8696,13 +8696,13 @@
         <v>45175</v>
       </c>
       <c r="G83">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="H83" s="2">
         <v>45357</v>
       </c>
       <c r="I83">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="J83" t="inlineStr">
         <is>
@@ -8799,13 +8799,13 @@
         <v>45054</v>
       </c>
       <c r="G84">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="H84" s="2">
         <v>45238</v>
       </c>
       <c r="I84">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="J84" t="inlineStr">
         <is>
@@ -8902,13 +8902,13 @@
         <v>45056</v>
       </c>
       <c r="G85">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="H85" s="2">
         <v>45240</v>
       </c>
       <c r="I85">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="J85" t="inlineStr">
         <is>
@@ -9005,13 +9005,13 @@
         <v>45085</v>
       </c>
       <c r="G86">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="H86" s="2">
         <v>45268</v>
       </c>
       <c r="I86">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="J86" t="inlineStr">
         <is>
@@ -9108,7 +9108,7 @@
         <v>45194</v>
       </c>
       <c r="I87">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J87" t="inlineStr">
         <is>
@@ -9195,13 +9195,13 @@
         <v>45103</v>
       </c>
       <c r="G88">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="H88" s="2">
         <v>45286</v>
       </c>
       <c r="I88">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="J88" t="inlineStr">
         <is>
@@ -9298,13 +9298,13 @@
         <v>45103</v>
       </c>
       <c r="G89">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="H89" s="2">
         <v>45286</v>
       </c>
       <c r="I89">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="J89" t="inlineStr">
         <is>
@@ -9401,13 +9401,13 @@
         <v>45008</v>
       </c>
       <c r="G90">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="H90" s="2">
         <v>45192</v>
       </c>
       <c r="I90">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="J90" t="inlineStr">
         <is>
@@ -9499,13 +9499,13 @@
         <v>45100</v>
       </c>
       <c r="G91">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="H91" s="2">
         <v>45287</v>
       </c>
       <c r="I91">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="J91" t="inlineStr">
         <is>
@@ -9602,13 +9602,13 @@
         <v>45003</v>
       </c>
       <c r="G92">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="H92" s="2">
         <v>45187</v>
       </c>
       <c r="I92">
-        <v>-5</v>
+        <v>-6</v>
       </c>
       <c r="J92" t="inlineStr">
         <is>
@@ -9705,13 +9705,13 @@
         <v>45104</v>
       </c>
       <c r="G93">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="H93" s="2">
         <v>45287</v>
       </c>
       <c r="I93">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="J93" t="inlineStr">
         <is>
@@ -9808,13 +9808,13 @@
         <v>45104</v>
       </c>
       <c r="G94">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="H94" s="2">
         <v>45287</v>
       </c>
       <c r="I94">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="J94" t="inlineStr">
         <is>
@@ -9911,13 +9911,13 @@
         <v>45049</v>
       </c>
       <c r="G95">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="H95" s="2">
         <v>45233</v>
       </c>
       <c r="I95">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="J95" t="inlineStr">
         <is>
@@ -10014,13 +10014,13 @@
         <v>45122</v>
       </c>
       <c r="G96">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="H96" s="2">
         <v>45306</v>
       </c>
       <c r="I96">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="J96" t="inlineStr">
         <is>
@@ -10112,13 +10112,13 @@
         <v>45141</v>
       </c>
       <c r="G97">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="H97" s="2">
         <v>45325</v>
       </c>
       <c r="I97">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="J97" t="inlineStr">
         <is>
@@ -10215,13 +10215,13 @@
         <v>45010</v>
       </c>
       <c r="G98">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="H98" s="2">
         <v>45194</v>
       </c>
       <c r="I98">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J98" t="inlineStr">
         <is>
@@ -10313,13 +10313,13 @@
         <v>45093</v>
       </c>
       <c r="G99">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="H99" s="2">
         <v>45276</v>
       </c>
       <c r="I99">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="J99" t="inlineStr">
         <is>
@@ -10416,13 +10416,13 @@
         <v>45123</v>
       </c>
       <c r="G100">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="H100" s="2">
         <v>45307</v>
       </c>
       <c r="I100">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="J100" t="inlineStr">
         <is>
@@ -10519,13 +10519,13 @@
         <v>45014</v>
       </c>
       <c r="G101">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="H101" s="2">
         <v>45198</v>
       </c>
       <c r="I101">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="J101" t="inlineStr">
         <is>
@@ -10622,13 +10622,13 @@
         <v>45093</v>
       </c>
       <c r="G102">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="H102" s="2">
         <v>45276</v>
       </c>
       <c r="I102">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="J102" t="inlineStr">
         <is>
@@ -10725,13 +10725,13 @@
         <v>45122</v>
       </c>
       <c r="G103">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="H103" s="2">
         <v>45306</v>
       </c>
       <c r="I103">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="J103" t="inlineStr">
         <is>
@@ -10828,13 +10828,13 @@
         <v>45122</v>
       </c>
       <c r="G104">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="H104" s="2">
         <v>45306</v>
       </c>
       <c r="I104">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="J104" t="inlineStr">
         <is>
@@ -10926,13 +10926,13 @@
         <v>45050</v>
       </c>
       <c r="G105">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="H105" s="2">
         <v>45234</v>
       </c>
       <c r="I105">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="J105" t="inlineStr">
         <is>
@@ -11029,13 +11029,13 @@
         <v>45085</v>
       </c>
       <c r="G106">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="H106" s="2">
         <v>45268</v>
       </c>
       <c r="I106">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="J106" t="inlineStr">
         <is>
@@ -11132,13 +11132,13 @@
         <v>45093</v>
       </c>
       <c r="G107">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="H107" s="2">
         <v>45185</v>
       </c>
       <c r="I107">
-        <v>-7</v>
+        <v>-8</v>
       </c>
       <c r="J107" t="inlineStr">
         <is>
@@ -11230,13 +11230,13 @@
         <v>45093</v>
       </c>
       <c r="G108">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="H108" s="2">
         <v>45185</v>
       </c>
       <c r="I108">
-        <v>-7</v>
+        <v>-8</v>
       </c>
       <c r="J108" t="inlineStr">
         <is>
@@ -11328,13 +11328,13 @@
         <v>45093</v>
       </c>
       <c r="G109">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="H109" s="2">
         <v>45185</v>
       </c>
       <c r="I109">
-        <v>-7</v>
+        <v>-8</v>
       </c>
       <c r="J109" t="inlineStr">
         <is>
@@ -11431,13 +11431,13 @@
         <v>45148</v>
       </c>
       <c r="G110">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="H110" s="2">
         <v>45240</v>
       </c>
       <c r="I110">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="J110" t="inlineStr">
         <is>
@@ -11534,13 +11534,13 @@
         <v>45119</v>
       </c>
       <c r="G111">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="H111" s="2">
         <v>45211</v>
       </c>
       <c r="I111">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="J111" t="inlineStr">
         <is>
@@ -11637,13 +11637,13 @@
         <v>45172</v>
       </c>
       <c r="G112">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="H112" s="2">
         <v>45263</v>
       </c>
       <c r="I112">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="J112" t="inlineStr">
         <is>
@@ -11740,13 +11740,13 @@
         <v>45023</v>
       </c>
       <c r="G113">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="H113" s="2">
         <v>45206</v>
       </c>
       <c r="I113">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="J113" t="inlineStr">
         <is>
@@ -11843,13 +11843,13 @@
         <v>45111</v>
       </c>
       <c r="G114">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="H114" s="2">
         <v>45203</v>
       </c>
       <c r="I114">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="J114" t="inlineStr">
         <is>
@@ -11946,7 +11946,7 @@
         <v>45218</v>
       </c>
       <c r="I115">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="J115" t="inlineStr">
         <is>
@@ -12043,13 +12043,13 @@
         <v>45161</v>
       </c>
       <c r="G116">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="H116" s="2">
         <v>45253</v>
       </c>
       <c r="I116">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="J116" t="inlineStr">
         <is>
@@ -12146,13 +12146,13 @@
         <v>45115</v>
       </c>
       <c r="G117">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="H117" s="2">
         <v>45299</v>
       </c>
       <c r="I117">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="J117" t="inlineStr">
         <is>
@@ -12244,13 +12244,13 @@
         <v>45094</v>
       </c>
       <c r="G118">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="H118" s="2">
         <v>45277</v>
       </c>
       <c r="I118">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="J118" t="inlineStr">
         <is>
@@ -12347,13 +12347,13 @@
         <v>45104</v>
       </c>
       <c r="G119">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="H119" s="2">
         <v>45287</v>
       </c>
       <c r="I119">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="J119" t="inlineStr">
         <is>
@@ -12450,13 +12450,13 @@
         <v>45104</v>
       </c>
       <c r="G120">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="H120" s="2">
         <v>45287</v>
       </c>
       <c r="I120">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="J120" t="inlineStr">
         <is>
@@ -12553,13 +12553,13 @@
         <v>45104</v>
       </c>
       <c r="G121">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="H121" s="2">
         <v>45287</v>
       </c>
       <c r="I121">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="J121" t="inlineStr">
         <is>
@@ -12656,13 +12656,13 @@
         <v>45104</v>
       </c>
       <c r="G122">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="H122" s="2">
         <v>45287</v>
       </c>
       <c r="I122">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="J122" t="inlineStr">
         <is>
@@ -12759,13 +12759,13 @@
         <v>45107</v>
       </c>
       <c r="G123">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="H123" s="2">
         <v>45199</v>
       </c>
       <c r="I123">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="J123" t="inlineStr">
         <is>
@@ -12862,13 +12862,13 @@
         <v>45013</v>
       </c>
       <c r="G124">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="H124" s="2">
         <v>45197</v>
       </c>
       <c r="I124">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="J124" t="inlineStr">
         <is>
@@ -12965,13 +12965,13 @@
         <v>45121</v>
       </c>
       <c r="G125">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="H125" s="2">
         <v>45213</v>
       </c>
       <c r="I125">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="J125" t="inlineStr">
         <is>
@@ -13068,13 +13068,13 @@
         <v>45134</v>
       </c>
       <c r="G126">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="H126" s="2">
         <v>45226</v>
       </c>
       <c r="I126">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="J126" t="inlineStr">
         <is>
@@ -13171,7 +13171,7 @@
         <v>45212</v>
       </c>
       <c r="I127">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="J127" t="inlineStr">
         <is>
@@ -13268,13 +13268,13 @@
         <v>45126</v>
       </c>
       <c r="G128">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="H128" s="2">
         <v>45218</v>
       </c>
       <c r="I128">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="J128" t="inlineStr">
         <is>
@@ -13366,13 +13366,13 @@
         <v>45158</v>
       </c>
       <c r="G129">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="H129" s="2">
         <v>45250</v>
       </c>
       <c r="I129">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="J129" t="inlineStr">
         <is>
@@ -13469,13 +13469,13 @@
         <v>45171</v>
       </c>
       <c r="G130">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="H130" s="2">
         <v>45262</v>
       </c>
       <c r="I130">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="J130" t="inlineStr">
         <is>
@@ -13572,13 +13572,13 @@
         <v>45111</v>
       </c>
       <c r="G131">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="H131" s="2">
         <v>45203</v>
       </c>
       <c r="I131">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="J131" t="inlineStr">
         <is>
@@ -13675,13 +13675,13 @@
         <v>45144</v>
       </c>
       <c r="G132">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="H132" s="2">
         <v>45236</v>
       </c>
       <c r="I132">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="J132" t="inlineStr">
         <is>
@@ -13778,13 +13778,13 @@
         <v>45156</v>
       </c>
       <c r="G133">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="H133" s="2">
         <v>45248</v>
       </c>
       <c r="I133">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="J133" t="inlineStr">
         <is>
@@ -13876,13 +13876,13 @@
         <v>45146</v>
       </c>
       <c r="G134">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="H134" s="2">
         <v>45238</v>
       </c>
       <c r="I134">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="J134" t="inlineStr">
         <is>
@@ -13979,13 +13979,13 @@
         <v>45140</v>
       </c>
       <c r="G135">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="H135" s="2">
         <v>45232</v>
       </c>
       <c r="I135">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="J135" t="inlineStr">
         <is>
@@ -14082,13 +14082,13 @@
         <v>45104</v>
       </c>
       <c r="G136">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="H136" s="2">
         <v>45196</v>
       </c>
       <c r="I136">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="J136" t="inlineStr">
         <is>
@@ -14185,13 +14185,13 @@
         <v>45105</v>
       </c>
       <c r="G137">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="H137" s="2">
         <v>45197</v>
       </c>
       <c r="I137">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="J137" t="inlineStr">
         <is>
@@ -14288,13 +14288,13 @@
         <v>45179</v>
       </c>
       <c r="G138">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="H138" s="2">
         <v>45270</v>
       </c>
       <c r="I138">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="J138" t="inlineStr">
         <is>
@@ -14386,13 +14386,13 @@
         <v>45105</v>
       </c>
       <c r="G139">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="H139" s="2">
         <v>45197</v>
       </c>
       <c r="I139">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="J139" t="inlineStr">
         <is>
@@ -14489,13 +14489,13 @@
         <v>45182</v>
       </c>
       <c r="G140">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="H140" s="2">
         <v>45273</v>
       </c>
       <c r="I140">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="J140" t="inlineStr">
         <is>
@@ -14592,13 +14592,13 @@
         <v>45116</v>
       </c>
       <c r="G141">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="H141" s="2">
         <v>45208</v>
       </c>
       <c r="I141">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="J141" t="inlineStr">
         <is>
@@ -14690,13 +14690,13 @@
         <v>45150</v>
       </c>
       <c r="G142">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="H142" s="2">
         <v>45242</v>
       </c>
       <c r="I142">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="J142" t="inlineStr">
         <is>
@@ -14793,7 +14793,7 @@
         <v>45238</v>
       </c>
       <c r="I143">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="J143" t="inlineStr">
         <is>
@@ -14890,13 +14890,13 @@
         <v>45171</v>
       </c>
       <c r="G144">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="H144" s="2">
         <v>45262</v>
       </c>
       <c r="I144">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="J144" t="inlineStr">
         <is>
@@ -14993,13 +14993,13 @@
         <v>45102</v>
       </c>
       <c r="G145">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="H145" s="2">
         <v>45194</v>
       </c>
       <c r="I145">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J145" t="inlineStr">
         <is>
@@ -15086,13 +15086,13 @@
         <v>45119</v>
       </c>
       <c r="G146">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="H146" s="2">
         <v>45211</v>
       </c>
       <c r="I146">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="J146" t="inlineStr">
         <is>
@@ -15189,13 +15189,13 @@
         <v>45165</v>
       </c>
       <c r="G147">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="H147" s="2">
         <v>45257</v>
       </c>
       <c r="I147">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="J147" t="inlineStr">
         <is>
@@ -15292,13 +15292,13 @@
         <v>45166</v>
       </c>
       <c r="G148">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="H148" s="2">
         <v>45258</v>
       </c>
       <c r="I148">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="J148" t="inlineStr">
         <is>
@@ -15395,13 +15395,13 @@
         <v>45093</v>
       </c>
       <c r="G149">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="H149" s="2">
         <v>45185</v>
       </c>
       <c r="I149">
-        <v>-7</v>
+        <v>-8</v>
       </c>
       <c r="J149" t="inlineStr">
         <is>
@@ -15498,13 +15498,13 @@
         <v>45035</v>
       </c>
       <c r="G150">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="H150" s="2">
         <v>45218</v>
       </c>
       <c r="I150">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="J150" t="inlineStr">
         <is>
@@ -15601,13 +15601,13 @@
         <v>45174</v>
       </c>
       <c r="G151">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="H151" s="2">
         <v>45356</v>
       </c>
       <c r="I151">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="J151" t="inlineStr">
         <is>
@@ -15704,13 +15704,13 @@
         <v>45089</v>
       </c>
       <c r="G152">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="H152" s="2">
         <v>45272</v>
       </c>
       <c r="I152">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="J152" t="inlineStr">
         <is>
@@ -15807,13 +15807,13 @@
         <v>45124</v>
       </c>
       <c r="G153">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="H153" s="2">
         <v>45308</v>
       </c>
       <c r="I153">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="J153" t="inlineStr">
         <is>
@@ -15910,13 +15910,13 @@
         <v>45124</v>
       </c>
       <c r="G154">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="H154" s="2">
         <v>45308</v>
       </c>
       <c r="I154">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="J154" t="inlineStr">
         <is>
@@ -16013,13 +16013,13 @@
         <v>45026</v>
       </c>
       <c r="G155">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="H155" s="2">
         <v>45209</v>
       </c>
       <c r="I155">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="J155" t="inlineStr">
         <is>
@@ -16116,13 +16116,13 @@
         <v>45026</v>
       </c>
       <c r="G156">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="H156" s="2">
         <v>45209</v>
       </c>
       <c r="I156">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="J156" t="inlineStr">
         <is>
@@ -16219,13 +16219,13 @@
         <v>45026</v>
       </c>
       <c r="G157">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="H157" s="2">
         <v>45209</v>
       </c>
       <c r="I157">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="J157" t="inlineStr">
         <is>
@@ -16322,13 +16322,13 @@
         <v>45026</v>
       </c>
       <c r="G158">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="H158" s="2">
         <v>45209</v>
       </c>
       <c r="I158">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="J158" t="inlineStr">
         <is>
@@ -16425,13 +16425,13 @@
         <v>45156</v>
       </c>
       <c r="G159">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="H159" s="2">
         <v>45247</v>
       </c>
       <c r="I159">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="J159" t="inlineStr">
         <is>
@@ -16528,13 +16528,13 @@
         <v>45153</v>
       </c>
       <c r="G160">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="H160" s="2">
         <v>45245</v>
       </c>
       <c r="I160">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="J160" t="inlineStr">
         <is>
@@ -16631,13 +16631,13 @@
         <v>45135</v>
       </c>
       <c r="G161">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="H161" s="2">
         <v>45319</v>
       </c>
       <c r="I161">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="J161" t="inlineStr">
         <is>
@@ -16734,13 +16734,13 @@
         <v>45091</v>
       </c>
       <c r="G162">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="H162" s="2">
         <v>45274</v>
       </c>
       <c r="I162">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="J162" t="inlineStr">
         <is>
@@ -16832,13 +16832,13 @@
         <v>45091</v>
       </c>
       <c r="G163">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="H163" s="2">
         <v>45274</v>
       </c>
       <c r="I163">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="J163" t="inlineStr">
         <is>
@@ -16930,13 +16930,13 @@
         <v>45138</v>
       </c>
       <c r="G164">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="H164" s="2">
         <v>45322</v>
       </c>
       <c r="I164">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="J164" t="inlineStr">
         <is>
@@ -17033,13 +17033,13 @@
         <v>45138</v>
       </c>
       <c r="G165">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="H165" s="2">
         <v>45322</v>
       </c>
       <c r="I165">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="J165" t="inlineStr">
         <is>
@@ -17136,13 +17136,13 @@
         <v>45085</v>
       </c>
       <c r="G166">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="H166" s="2">
         <v>45268</v>
       </c>
       <c r="I166">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="J166" t="inlineStr">
         <is>
@@ -17239,13 +17239,13 @@
         <v>45085</v>
       </c>
       <c r="G167">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="H167" s="2">
         <v>45268</v>
       </c>
       <c r="I167">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="J167" t="inlineStr">
         <is>
@@ -17342,7 +17342,7 @@
         <v>45326</v>
       </c>
       <c r="I168">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="J168" t="inlineStr">
         <is>
@@ -17439,13 +17439,13 @@
         <v>45173</v>
       </c>
       <c r="G169">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="H169" s="2">
         <v>45355</v>
       </c>
       <c r="I169">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="J169" t="inlineStr">
         <is>
@@ -17542,13 +17542,13 @@
         <v>45056</v>
       </c>
       <c r="G170">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="H170" s="2">
         <v>45240</v>
       </c>
       <c r="I170">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="J170" t="inlineStr">
         <is>
@@ -17645,7 +17645,7 @@
         <v>45238</v>
       </c>
       <c r="I171">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="J171" t="inlineStr">
         <is>
@@ -17742,13 +17742,13 @@
         <v>45141</v>
       </c>
       <c r="G172">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="H172" s="2">
         <v>45325</v>
       </c>
       <c r="I172">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="J172" t="inlineStr">
         <is>
@@ -17845,13 +17845,13 @@
         <v>45037</v>
       </c>
       <c r="G173">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="H173" s="2">
         <v>45220</v>
       </c>
       <c r="I173">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="J173" t="inlineStr">
         <is>
@@ -17948,13 +17948,13 @@
         <v>45171</v>
       </c>
       <c r="G174">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="H174" s="2">
         <v>45262</v>
       </c>
       <c r="I174">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="J174" t="inlineStr">
         <is>
@@ -18051,13 +18051,13 @@
         <v>45105</v>
       </c>
       <c r="G175">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="H175" s="2">
         <v>45197</v>
       </c>
       <c r="I175">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="J175" t="inlineStr">
         <is>
@@ -18154,13 +18154,13 @@
         <v>45162</v>
       </c>
       <c r="G176">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="H176" s="2">
         <v>45254</v>
       </c>
       <c r="I176">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="J176" t="inlineStr">
         <is>
@@ -18257,13 +18257,13 @@
         <v>45061</v>
       </c>
       <c r="G177">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="H177" s="2">
         <v>45245</v>
       </c>
       <c r="I177">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="J177" t="inlineStr">
         <is>
@@ -18360,13 +18360,13 @@
         <v>45120</v>
       </c>
       <c r="G178">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="H178" s="2">
         <v>45212</v>
       </c>
       <c r="I178">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="J178" t="inlineStr">
         <is>
@@ -18463,7 +18463,7 @@
         <v>45191</v>
       </c>
       <c r="I179">
-        <v>-1</v>
+        <v>-2</v>
       </c>
       <c r="J179" t="inlineStr">
         <is>
@@ -18560,13 +18560,13 @@
         <v>45088</v>
       </c>
       <c r="G180">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="H180" s="2">
         <v>45271</v>
       </c>
       <c r="I180">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="J180" t="inlineStr">
         <is>
@@ -18663,13 +18663,13 @@
         <v>45100</v>
       </c>
       <c r="G181">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="H181" s="2">
         <v>45192</v>
       </c>
       <c r="I181">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="J181" t="inlineStr">
         <is>
@@ -18756,13 +18756,13 @@
         <v>45131</v>
       </c>
       <c r="G182">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="H182" s="2">
         <v>45223</v>
       </c>
       <c r="I182">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="J182" t="inlineStr">
         <is>
@@ -18854,13 +18854,13 @@
         <v>45136</v>
       </c>
       <c r="G183">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="H183" s="2">
         <v>45228</v>
       </c>
       <c r="I183">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="J183" t="inlineStr">
         <is>
@@ -18952,13 +18952,13 @@
         <v>45150</v>
       </c>
       <c r="G184">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="H184" s="2">
         <v>45242</v>
       </c>
       <c r="I184">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="J184" t="inlineStr">
         <is>
@@ -19050,13 +19050,13 @@
         <v>45118</v>
       </c>
       <c r="G185">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="H185" s="2">
         <v>45210</v>
       </c>
       <c r="I185">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="J185" t="inlineStr">
         <is>
@@ -19148,13 +19148,13 @@
         <v>45129</v>
       </c>
       <c r="G186">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="H186" s="2">
         <v>45221</v>
       </c>
       <c r="I186">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="J186" t="inlineStr">
         <is>
@@ -19246,13 +19246,13 @@
         <v>45097</v>
       </c>
       <c r="G187">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="H187" s="2">
         <v>45189</v>
       </c>
       <c r="I187">
-        <v>-3</v>
+        <v>-4</v>
       </c>
       <c r="J187" t="inlineStr">
         <is>
@@ -19339,13 +19339,13 @@
         <v>45101</v>
       </c>
       <c r="G188">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="H188" s="2">
         <v>45193</v>
       </c>
       <c r="I188">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J188" t="inlineStr">
         <is>
@@ -19432,13 +19432,13 @@
         <v>45165</v>
       </c>
       <c r="G189">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="H189" s="2">
         <v>45257</v>
       </c>
       <c r="I189">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="J189" t="inlineStr">
         <is>
@@ -19530,7 +19530,7 @@
         <v>45202</v>
       </c>
       <c r="I190">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="J190" t="inlineStr">
         <is>
@@ -19627,13 +19627,13 @@
         <v>45081</v>
       </c>
       <c r="G191">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="H191" s="2">
         <v>45264</v>
       </c>
       <c r="I191">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="J191" t="inlineStr">
         <is>
@@ -19730,13 +19730,13 @@
         <v>45081</v>
       </c>
       <c r="G192">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="H192" s="2">
         <v>45264</v>
       </c>
       <c r="I192">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="J192" t="inlineStr">
         <is>
@@ -19833,7 +19833,7 @@
         <v>45319</v>
       </c>
       <c r="I193">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="J193" t="inlineStr">
         <is>
@@ -19930,7 +19930,7 @@
         <v>45319</v>
       </c>
       <c r="I194">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="J194" t="inlineStr">
         <is>
@@ -20022,13 +20022,13 @@
         <v>45046</v>
       </c>
       <c r="G195">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="H195" s="2">
         <v>45230</v>
       </c>
       <c r="I195">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="J195" t="inlineStr">
         <is>
@@ -20125,13 +20125,13 @@
         <v>45046</v>
       </c>
       <c r="G196">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="H196" s="2">
         <v>45230</v>
       </c>
       <c r="I196">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="J196" t="inlineStr">
         <is>
@@ -20228,13 +20228,13 @@
         <v>45031</v>
       </c>
       <c r="G197">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="H197" s="2">
         <v>45214</v>
       </c>
       <c r="I197">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="J197" t="inlineStr">
         <is>
@@ -20331,13 +20331,13 @@
         <v>45031</v>
       </c>
       <c r="G198">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="H198" s="2">
         <v>45214</v>
       </c>
       <c r="I198">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="J198" t="inlineStr">
         <is>
@@ -20434,13 +20434,13 @@
         <v>45031</v>
       </c>
       <c r="G199">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="H199" s="2">
         <v>45214</v>
       </c>
       <c r="I199">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="J199" t="inlineStr">
         <is>
@@ -20537,13 +20537,13 @@
         <v>45031</v>
       </c>
       <c r="G200">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="H200" s="2">
         <v>45214</v>
       </c>
       <c r="I200">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="J200" t="inlineStr">
         <is>
@@ -20640,13 +20640,13 @@
         <v>45067</v>
       </c>
       <c r="G201">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="H201" s="2">
         <v>45251</v>
       </c>
       <c r="I201">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="J201" t="inlineStr">
         <is>
@@ -20743,13 +20743,13 @@
         <v>45067</v>
       </c>
       <c r="G202">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="H202" s="2">
         <v>45251</v>
       </c>
       <c r="I202">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="J202" t="inlineStr">
         <is>
@@ -20846,13 +20846,13 @@
         <v>45067</v>
       </c>
       <c r="G203">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="H203" s="2">
         <v>45251</v>
       </c>
       <c r="I203">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="J203" t="inlineStr">
         <is>
@@ -20949,13 +20949,13 @@
         <v>45067</v>
       </c>
       <c r="G204">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="H204" s="2">
         <v>45251</v>
       </c>
       <c r="I204">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="J204" t="inlineStr">
         <is>
@@ -21052,13 +21052,13 @@
         <v>45178</v>
       </c>
       <c r="G205">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="H205" s="2">
         <v>45269</v>
       </c>
       <c r="I205">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="J205" t="inlineStr">
         <is>
@@ -21155,7 +21155,7 @@
         <v>45252</v>
       </c>
       <c r="I206">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="J206" t="inlineStr">
         <is>
@@ -21252,13 +21252,13 @@
         <v>45087</v>
       </c>
       <c r="G207">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="H207" s="2">
         <v>45270</v>
       </c>
       <c r="I207">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="J207" t="inlineStr">
         <is>
@@ -21355,13 +21355,13 @@
         <v>45099</v>
       </c>
       <c r="G208">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="H208" s="2">
         <v>45282</v>
       </c>
       <c r="I208">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="J208" t="inlineStr">
         <is>
@@ -21458,13 +21458,13 @@
         <v>45175</v>
       </c>
       <c r="G209">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="H209" s="2">
         <v>45356</v>
       </c>
       <c r="I209">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="J209" t="inlineStr">
         <is>
@@ -21561,13 +21561,13 @@
         <v>45175</v>
       </c>
       <c r="G210">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="H210" s="2">
         <v>45356</v>
       </c>
       <c r="I210">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="J210" t="inlineStr">
         <is>
@@ -21664,13 +21664,13 @@
         <v>45166</v>
       </c>
       <c r="G211">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="H211" s="2">
         <v>45350</v>
       </c>
       <c r="I211">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="J211" t="inlineStr">
         <is>
@@ -21767,13 +21767,13 @@
         <v>45166</v>
       </c>
       <c r="G212">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="H212" s="2">
         <v>45350</v>
       </c>
       <c r="I212">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="J212" t="inlineStr">
         <is>
@@ -21870,13 +21870,13 @@
         <v>45090</v>
       </c>
       <c r="G213">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="H213" s="2">
         <v>45273</v>
       </c>
       <c r="I213">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="J213" t="inlineStr">
         <is>
@@ -21973,13 +21973,13 @@
         <v>45106</v>
       </c>
       <c r="G214">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="H214" s="2">
         <v>45289</v>
       </c>
       <c r="I214">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="J214" t="inlineStr">
         <is>
@@ -22076,13 +22076,13 @@
         <v>45134</v>
       </c>
       <c r="G215">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="H215" s="2">
         <v>45226</v>
       </c>
       <c r="I215">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="J215" t="inlineStr">
         <is>
@@ -22179,13 +22179,13 @@
         <v>45132</v>
       </c>
       <c r="G216">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="H216" s="2">
         <v>45224</v>
       </c>
       <c r="I216">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="J216" t="inlineStr">
         <is>
@@ -22282,13 +22282,13 @@
         <v>45150</v>
       </c>
       <c r="G217">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="H217" s="2">
         <v>45242</v>
       </c>
       <c r="I217">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="J217" t="inlineStr">
         <is>
@@ -22385,13 +22385,13 @@
         <v>45095</v>
       </c>
       <c r="G218">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="H218" s="2">
         <v>45187</v>
       </c>
       <c r="I218">
-        <v>-5</v>
+        <v>-6</v>
       </c>
       <c r="J218" t="inlineStr">
         <is>
@@ -22483,13 +22483,13 @@
         <v>45182</v>
       </c>
       <c r="G219">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="H219" s="2">
         <v>45273</v>
       </c>
       <c r="I219">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="J219" t="inlineStr">
         <is>
@@ -22586,7 +22586,7 @@
         <v>45196</v>
       </c>
       <c r="I220">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="J220" t="inlineStr">
         <is>
@@ -22683,13 +22683,13 @@
         <v>45108</v>
       </c>
       <c r="G221">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="H221" s="2">
         <v>45200</v>
       </c>
       <c r="I221">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="J221" t="inlineStr">
         <is>
@@ -22786,13 +22786,13 @@
         <v>45135</v>
       </c>
       <c r="G222">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="H222" s="2">
         <v>45227</v>
       </c>
       <c r="I222">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="J222" t="inlineStr">
         <is>
@@ -22889,13 +22889,13 @@
         <v>45148</v>
       </c>
       <c r="G223">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="H223" s="2">
         <v>45240</v>
       </c>
       <c r="I223">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="J223" t="inlineStr">
         <is>
@@ -22987,13 +22987,13 @@
         <v>45100</v>
       </c>
       <c r="G224">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="H224" s="2">
         <v>45192</v>
       </c>
       <c r="I224">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="J224" t="inlineStr">
         <is>
@@ -23085,13 +23085,13 @@
         <v>45136</v>
       </c>
       <c r="G225">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="H225" s="2">
         <v>45320</v>
       </c>
       <c r="I225">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="J225" t="inlineStr">
         <is>
@@ -23188,13 +23188,13 @@
         <v>45136</v>
       </c>
       <c r="G226">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="H226" s="2">
         <v>45320</v>
       </c>
       <c r="I226">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="J226" t="inlineStr">
         <is>
@@ -23291,13 +23291,13 @@
         <v>45094</v>
       </c>
       <c r="G227">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="H227" s="2">
         <v>45277</v>
       </c>
       <c r="I227">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="J227" t="inlineStr">
         <is>
@@ -23394,13 +23394,13 @@
         <v>45081</v>
       </c>
       <c r="G228">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="H228" s="2">
         <v>45264</v>
       </c>
       <c r="I228">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="J228" t="inlineStr">
         <is>
@@ -23497,13 +23497,13 @@
         <v>45099</v>
       </c>
       <c r="G229">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="H229" s="2">
         <v>45282</v>
       </c>
       <c r="I229">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="J229" t="inlineStr">
         <is>
@@ -23600,13 +23600,13 @@
         <v>45018</v>
       </c>
       <c r="G230">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="H230" s="2">
         <v>45201</v>
       </c>
       <c r="I230">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="J230" t="inlineStr">
         <is>
@@ -23703,13 +23703,13 @@
         <v>45031</v>
       </c>
       <c r="G231">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="H231" s="2">
         <v>45214</v>
       </c>
       <c r="I231">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="J231" t="inlineStr">
         <is>
@@ -23806,7 +23806,7 @@
         <v>45294</v>
       </c>
       <c r="I232">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="J232" t="inlineStr">
         <is>
@@ -23903,13 +23903,13 @@
         <v>45079</v>
       </c>
       <c r="G233">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="H233" s="2">
         <v>45262</v>
       </c>
       <c r="I233">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="J233" t="inlineStr">
         <is>
@@ -24006,7 +24006,7 @@
         <v>45199</v>
       </c>
       <c r="I234">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="J234" t="inlineStr">
         <is>
@@ -24103,13 +24103,13 @@
         <v>45021</v>
       </c>
       <c r="G235">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="H235" s="2">
         <v>45204</v>
       </c>
       <c r="I235">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="J235" t="inlineStr">
         <is>
@@ -24206,13 +24206,13 @@
         <v>45021</v>
       </c>
       <c r="G236">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="H236" s="2">
         <v>45204</v>
       </c>
       <c r="I236">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="J236" t="inlineStr">
         <is>
@@ -24309,13 +24309,13 @@
         <v>45080</v>
       </c>
       <c r="G237">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="H237" s="2">
         <v>45263</v>
       </c>
       <c r="I237">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="J237" t="inlineStr">
         <is>
@@ -24412,13 +24412,13 @@
         <v>45046</v>
       </c>
       <c r="G238">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="H238" s="2">
         <v>45229</v>
       </c>
       <c r="I238">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="J238" t="inlineStr">
         <is>
@@ -24515,13 +24515,13 @@
         <v>45112</v>
       </c>
       <c r="G239">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="H239" s="2">
         <v>45204</v>
       </c>
       <c r="I239">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="J239" t="inlineStr">
         <is>
@@ -24609,13 +24609,13 @@
         <v>45112</v>
       </c>
       <c r="G240">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="H240" s="2">
         <v>45204</v>
       </c>
       <c r="I240">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="J240" t="inlineStr">
         <is>
@@ -24703,13 +24703,13 @@
         <v>45016</v>
       </c>
       <c r="G241">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="H241" s="2">
         <v>45199</v>
       </c>
       <c r="I241">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="J241" t="inlineStr">
         <is>
@@ -24806,13 +24806,13 @@
         <v>45070</v>
       </c>
       <c r="G242">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="H242" s="2">
         <v>45254</v>
       </c>
       <c r="I242">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="J242" t="inlineStr">
         <is>
@@ -24909,13 +24909,13 @@
         <v>45168</v>
       </c>
       <c r="G243">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="H243" s="2">
         <v>45260</v>
       </c>
       <c r="I243">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="J243" t="inlineStr">
         <is>
@@ -25012,13 +25012,13 @@
         <v>45027</v>
       </c>
       <c r="G244">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="H244" s="2">
         <v>45210</v>
       </c>
       <c r="I244">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="J244" t="inlineStr">
         <is>
@@ -25115,13 +25115,13 @@
         <v>45077</v>
       </c>
       <c r="G245">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="H245" s="2">
         <v>45260</v>
       </c>
       <c r="I245">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="J245" t="inlineStr">
         <is>
@@ -25218,13 +25218,13 @@
         <v>45100</v>
       </c>
       <c r="G246">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="H246" s="2">
         <v>45283</v>
       </c>
       <c r="I246">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="J246" t="inlineStr">
         <is>
@@ -25321,7 +25321,7 @@
         <v>45281</v>
       </c>
       <c r="I247">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="J247" t="inlineStr">
         <is>
@@ -25418,13 +25418,13 @@
         <v>45044</v>
       </c>
       <c r="G248">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="H248" s="2">
         <v>45227</v>
       </c>
       <c r="I248">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="J248" t="inlineStr">
         <is>
@@ -25521,13 +25521,13 @@
         <v>45101</v>
       </c>
       <c r="G249">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="H249" s="2">
         <v>45283</v>
       </c>
       <c r="I249">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="J249" t="inlineStr">
         <is>
@@ -25624,13 +25624,13 @@
         <v>45134</v>
       </c>
       <c r="G250">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="H250" s="2">
         <v>45226</v>
       </c>
       <c r="I250">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="J250" t="inlineStr">
         <is>
@@ -25727,13 +25727,13 @@
         <v>45158</v>
       </c>
       <c r="G251">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="H251" s="2">
         <v>45250</v>
       </c>
       <c r="I251">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="J251" t="inlineStr">
         <is>
@@ -25830,13 +25830,13 @@
         <v>45108</v>
       </c>
       <c r="G252">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="H252" s="2">
         <v>45200</v>
       </c>
       <c r="I252">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="J252" t="inlineStr">
         <is>
@@ -25933,7 +25933,7 @@
         <v>45317</v>
       </c>
       <c r="I253">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="J253" t="inlineStr">
         <is>
@@ -26030,13 +26030,13 @@
         <v>45039</v>
       </c>
       <c r="G254">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="H254" s="2">
         <v>45222</v>
       </c>
       <c r="I254">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="J254" t="inlineStr">
         <is>
@@ -26128,13 +26128,13 @@
         <v>45129</v>
       </c>
       <c r="G255">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="H255" s="2">
         <v>45221</v>
       </c>
       <c r="I255">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="J255" t="inlineStr">
         <is>
@@ -26231,13 +26231,13 @@
         <v>45157</v>
       </c>
       <c r="G256">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="H256" s="2">
         <v>45341</v>
       </c>
       <c r="I256">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="J256" t="inlineStr">
         <is>
@@ -26334,13 +26334,13 @@
         <v>45063</v>
       </c>
       <c r="G257">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="H257" s="2">
         <v>45247</v>
       </c>
       <c r="I257">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="J257" t="inlineStr">
         <is>
@@ -26437,7 +26437,7 @@
         <v>45254</v>
       </c>
       <c r="I258">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="J258" t="inlineStr">
         <is>
@@ -26534,7 +26534,7 @@
         <v>45486</v>
       </c>
       <c r="I259">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="J259" t="inlineStr">
         <is>
@@ -26626,13 +26626,13 @@
         <v>45073</v>
       </c>
       <c r="G260">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="H260" s="2">
         <v>45439</v>
       </c>
       <c r="I260">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="J260" t="inlineStr">
         <is>
@@ -26724,7 +26724,7 @@
         <v>45323</v>
       </c>
       <c r="I261">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="J261" t="inlineStr">
         <is>
@@ -26816,7 +26816,7 @@
         <v>45303</v>
       </c>
       <c r="I262">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="J262" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
Bond dates update Mon Sep 25 23:09:02 UTC 2023
</commit_message>
<xml_diff>
--- a/Data/obligacje_screener.xlsx
+++ b/Data/obligacje_screener.xlsx
@@ -512,7 +512,7 @@
         <v>45340</v>
       </c>
       <c r="I2">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="J2" t="inlineStr">
         <is>
@@ -600,13 +600,13 @@
         <v>45121</v>
       </c>
       <c r="G3">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="H3" s="2">
         <v>45305</v>
       </c>
       <c r="I3">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="J3" t="inlineStr">
         <is>
@@ -703,13 +703,13 @@
         <v>45039</v>
       </c>
       <c r="G4">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="H4" s="2">
         <v>45222</v>
       </c>
       <c r="I4">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="J4" t="inlineStr">
         <is>
@@ -806,13 +806,13 @@
         <v>45039</v>
       </c>
       <c r="G5">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="H5" s="2">
         <v>45222</v>
       </c>
       <c r="I5">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="J5" t="inlineStr">
         <is>
@@ -909,13 +909,13 @@
         <v>45129</v>
       </c>
       <c r="G6">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="H6" s="2">
         <v>45221</v>
       </c>
       <c r="I6">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="J6" t="inlineStr">
         <is>
@@ -1012,13 +1012,13 @@
         <v>45162</v>
       </c>
       <c r="G7">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="H7" s="2">
         <v>45254</v>
       </c>
       <c r="I7">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="J7" t="inlineStr">
         <is>
@@ -1110,13 +1110,13 @@
         <v>45156</v>
       </c>
       <c r="G8">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="H8" s="2">
         <v>45248</v>
       </c>
       <c r="I8">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="J8" t="inlineStr">
         <is>
@@ -1213,13 +1213,13 @@
         <v>45141</v>
       </c>
       <c r="G9">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="H9" s="2">
         <v>45233</v>
       </c>
       <c r="I9">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="J9" t="inlineStr">
         <is>
@@ -1316,13 +1316,13 @@
         <v>45062</v>
       </c>
       <c r="G10">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="H10" s="2">
         <v>45246</v>
       </c>
       <c r="I10">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="J10" t="inlineStr">
         <is>
@@ -1419,7 +1419,7 @@
         <v>45286</v>
       </c>
       <c r="I11">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="J11" t="inlineStr">
         <is>
@@ -1516,13 +1516,13 @@
         <v>45011</v>
       </c>
       <c r="G12">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="H12" s="2">
         <v>45195</v>
       </c>
       <c r="I12">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J12" t="inlineStr">
         <is>
@@ -1614,13 +1614,13 @@
         <v>45036</v>
       </c>
       <c r="G13">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="H13" s="2">
         <v>45219</v>
       </c>
       <c r="I13">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="J13" t="inlineStr">
         <is>
@@ -1717,13 +1717,13 @@
         <v>45036</v>
       </c>
       <c r="G14">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="H14" s="2">
         <v>45219</v>
       </c>
       <c r="I14">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="J14" t="inlineStr">
         <is>
@@ -1820,13 +1820,13 @@
         <v>45106</v>
       </c>
       <c r="G15">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="H15" s="2">
         <v>45289</v>
       </c>
       <c r="I15">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="J15" t="inlineStr">
         <is>
@@ -1923,13 +1923,13 @@
         <v>45094</v>
       </c>
       <c r="G16">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="H16" s="2">
         <v>45186</v>
       </c>
       <c r="I16">
-        <v>-7</v>
+        <v>-8</v>
       </c>
       <c r="J16" t="inlineStr">
         <is>
@@ -2026,13 +2026,13 @@
         <v>45094</v>
       </c>
       <c r="G17">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="H17" s="2">
         <v>45186</v>
       </c>
       <c r="I17">
-        <v>-7</v>
+        <v>-8</v>
       </c>
       <c r="J17" t="inlineStr">
         <is>
@@ -2129,13 +2129,13 @@
         <v>45132</v>
       </c>
       <c r="G18">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="H18" s="2">
         <v>45224</v>
       </c>
       <c r="I18">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="J18" t="inlineStr">
         <is>
@@ -2232,13 +2232,13 @@
         <v>45137</v>
       </c>
       <c r="G19">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="H19" s="2">
         <v>45229</v>
       </c>
       <c r="I19">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="J19" t="inlineStr">
         <is>
@@ -2330,13 +2330,13 @@
         <v>45183</v>
       </c>
       <c r="G20">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="H20" s="2">
         <v>45274</v>
       </c>
       <c r="I20">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="J20" t="inlineStr">
         <is>
@@ -2433,13 +2433,13 @@
         <v>45093</v>
       </c>
       <c r="G21">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="H21" s="2">
         <v>45187</v>
       </c>
       <c r="I21">
-        <v>-6</v>
+        <v>-7</v>
       </c>
       <c r="J21" t="inlineStr">
         <is>
@@ -2536,13 +2536,13 @@
         <v>45096</v>
       </c>
       <c r="G22">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="H22" s="2">
         <v>45187</v>
       </c>
       <c r="I22">
-        <v>-6</v>
+        <v>-7</v>
       </c>
       <c r="J22" t="inlineStr">
         <is>
@@ -2639,7 +2639,7 @@
         <v>45245</v>
       </c>
       <c r="I23">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="J23" t="inlineStr">
         <is>
@@ -2736,7 +2736,7 @@
         <v>45245</v>
       </c>
       <c r="I24">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="J24" t="inlineStr">
         <is>
@@ -2833,13 +2833,13 @@
         <v>45021</v>
       </c>
       <c r="G25">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="H25" s="2">
         <v>45204</v>
       </c>
       <c r="I25">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="J25" t="inlineStr">
         <is>
@@ -2936,13 +2936,13 @@
         <v>45160</v>
       </c>
       <c r="G26">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="H26" s="2">
         <v>45344</v>
       </c>
       <c r="I26">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="J26" t="inlineStr">
         <is>
@@ -3039,13 +3039,13 @@
         <v>45118</v>
       </c>
       <c r="G27">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="H27" s="2">
         <v>45302</v>
       </c>
       <c r="I27">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="J27" t="inlineStr">
         <is>
@@ -3142,13 +3142,13 @@
         <v>45085</v>
       </c>
       <c r="G28">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="H28" s="2">
         <v>45268</v>
       </c>
       <c r="I28">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="J28" t="inlineStr">
         <is>
@@ -3245,13 +3245,13 @@
         <v>45183</v>
       </c>
       <c r="G29">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="H29" s="2">
         <v>45274</v>
       </c>
       <c r="I29">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="J29" t="inlineStr">
         <is>
@@ -3348,7 +3348,7 @@
         <v>45224</v>
       </c>
       <c r="I30">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="J30" t="inlineStr">
         <is>
@@ -3445,13 +3445,13 @@
         <v>45153</v>
       </c>
       <c r="G31">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="H31" s="2">
         <v>45245</v>
       </c>
       <c r="I31">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="J31" t="inlineStr">
         <is>
@@ -3548,13 +3548,13 @@
         <v>45155</v>
       </c>
       <c r="G32">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="H32" s="2">
         <v>45247</v>
       </c>
       <c r="I32">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="J32" t="inlineStr">
         <is>
@@ -3651,7 +3651,7 @@
         <v>45255</v>
       </c>
       <c r="I33">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="J33" t="inlineStr">
         <is>
@@ -3739,13 +3739,13 @@
         <v>45176</v>
       </c>
       <c r="G34">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="H34" s="2">
         <v>45267</v>
       </c>
       <c r="I34">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="J34" t="inlineStr">
         <is>
@@ -3842,13 +3842,13 @@
         <v>45130</v>
       </c>
       <c r="G35">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="H35" s="2">
         <v>45222</v>
       </c>
       <c r="I35">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="J35" t="inlineStr">
         <is>
@@ -3940,13 +3940,13 @@
         <v>45115</v>
       </c>
       <c r="G36">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="H36" s="2">
         <v>45207</v>
       </c>
       <c r="I36">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="J36" t="inlineStr">
         <is>
@@ -4043,13 +4043,13 @@
         <v>45097</v>
       </c>
       <c r="G37">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="H37" s="2">
         <v>45189</v>
       </c>
       <c r="I37">
-        <v>-4</v>
+        <v>-5</v>
       </c>
       <c r="J37" t="inlineStr">
         <is>
@@ -4141,13 +4141,13 @@
         <v>45107</v>
       </c>
       <c r="G38">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="H38" s="2">
         <v>45290</v>
       </c>
       <c r="I38">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="J38" t="inlineStr">
         <is>
@@ -4244,13 +4244,13 @@
         <v>45063</v>
       </c>
       <c r="G39">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="H39" s="2">
         <v>45247</v>
       </c>
       <c r="I39">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="J39" t="inlineStr">
         <is>
@@ -4347,13 +4347,13 @@
         <v>45177</v>
       </c>
       <c r="G40">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="H40" s="2">
         <v>45359</v>
       </c>
       <c r="I40">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="J40" t="inlineStr">
         <is>
@@ -4450,13 +4450,13 @@
         <v>45107</v>
       </c>
       <c r="G41">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="H41" s="2">
         <v>45290</v>
       </c>
       <c r="I41">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="J41" t="inlineStr">
         <is>
@@ -4553,7 +4553,7 @@
         <v>45265</v>
       </c>
       <c r="I42">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="J42" t="inlineStr">
         <is>
@@ -4650,13 +4650,13 @@
         <v>45098</v>
       </c>
       <c r="G43">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="H43" s="2">
         <v>45281</v>
       </c>
       <c r="I43">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="J43" t="inlineStr">
         <is>
@@ -4753,13 +4753,13 @@
         <v>45099</v>
       </c>
       <c r="G44">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="H44" s="2">
         <v>45282</v>
       </c>
       <c r="I44">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="J44" t="inlineStr">
         <is>
@@ -4856,13 +4856,13 @@
         <v>45106</v>
       </c>
       <c r="G45">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="H45" s="2">
         <v>45289</v>
       </c>
       <c r="I45">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="J45" t="inlineStr">
         <is>
@@ -4959,13 +4959,13 @@
         <v>45106</v>
       </c>
       <c r="G46">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="H46" s="2">
         <v>45289</v>
       </c>
       <c r="I46">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="J46" t="inlineStr">
         <is>
@@ -5062,13 +5062,13 @@
         <v>45120</v>
       </c>
       <c r="G47">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="H47" s="2">
         <v>45304</v>
       </c>
       <c r="I47">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="J47" t="inlineStr">
         <is>
@@ -5165,13 +5165,13 @@
         <v>45118</v>
       </c>
       <c r="G48">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="H48" s="2">
         <v>45302</v>
       </c>
       <c r="I48">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="J48" t="inlineStr">
         <is>
@@ -5268,13 +5268,13 @@
         <v>45152</v>
       </c>
       <c r="G49">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="H49" s="2">
         <v>45336</v>
       </c>
       <c r="I49">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="J49" t="inlineStr">
         <is>
@@ -5371,13 +5371,13 @@
         <v>45042</v>
       </c>
       <c r="G50">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="H50" s="2">
         <v>45225</v>
       </c>
       <c r="I50">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="J50" t="inlineStr">
         <is>
@@ -5474,13 +5474,13 @@
         <v>45122</v>
       </c>
       <c r="G51">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="H51" s="2">
         <v>45306</v>
       </c>
       <c r="I51">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="J51" t="inlineStr">
         <is>
@@ -5577,13 +5577,13 @@
         <v>45139</v>
       </c>
       <c r="G52">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="H52" s="2">
         <v>45323</v>
       </c>
       <c r="I52">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="J52" t="inlineStr">
         <is>
@@ -5671,13 +5671,13 @@
         <v>45099</v>
       </c>
       <c r="G53">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="H53" s="2">
         <v>45282</v>
       </c>
       <c r="I53">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="J53" t="inlineStr">
         <is>
@@ -5774,7 +5774,7 @@
         <v>45196</v>
       </c>
       <c r="I54">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="J54" t="inlineStr">
         <is>
@@ -5871,13 +5871,13 @@
         <v>45044</v>
       </c>
       <c r="G55">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="H55" s="2">
         <v>45227</v>
       </c>
       <c r="I55">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="J55" t="inlineStr">
         <is>
@@ -5974,13 +5974,13 @@
         <v>45151</v>
       </c>
       <c r="G56">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="H56" s="2">
         <v>45243</v>
       </c>
       <c r="I56">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="J56" t="inlineStr">
         <is>
@@ -6072,7 +6072,7 @@
         <v>45196</v>
       </c>
       <c r="I57">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="J57" t="inlineStr">
         <is>
@@ -6169,13 +6169,13 @@
         <v>45069</v>
       </c>
       <c r="G58">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="H58" s="2">
         <v>45253</v>
       </c>
       <c r="I58">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="J58" t="inlineStr">
         <is>
@@ -6272,13 +6272,13 @@
         <v>45099</v>
       </c>
       <c r="G59">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="H59" s="2">
         <v>45191</v>
       </c>
       <c r="I59">
-        <v>-2</v>
+        <v>-3</v>
       </c>
       <c r="J59" t="inlineStr">
         <is>
@@ -6370,13 +6370,13 @@
         <v>45113</v>
       </c>
       <c r="G60">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="H60" s="2">
         <v>45205</v>
       </c>
       <c r="I60">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="J60" t="inlineStr">
         <is>
@@ -6473,13 +6473,13 @@
         <v>45127</v>
       </c>
       <c r="G61">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="H61" s="2">
         <v>45219</v>
       </c>
       <c r="I61">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="J61" t="inlineStr">
         <is>
@@ -6576,13 +6576,13 @@
         <v>45058</v>
       </c>
       <c r="G62">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="H62" s="2">
         <v>45242</v>
       </c>
       <c r="I62">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="J62" t="inlineStr">
         <is>
@@ -6679,13 +6679,13 @@
         <v>45010</v>
       </c>
       <c r="G63">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="H63" s="2">
         <v>45194</v>
       </c>
       <c r="I63">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J63" t="inlineStr">
         <is>
@@ -6777,13 +6777,13 @@
         <v>45025</v>
       </c>
       <c r="G64">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="H64" s="2">
         <v>45208</v>
       </c>
       <c r="I64">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="J64" t="inlineStr">
         <is>
@@ -6880,13 +6880,13 @@
         <v>45025</v>
       </c>
       <c r="G65">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="H65" s="2">
         <v>45208</v>
       </c>
       <c r="I65">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="J65" t="inlineStr">
         <is>
@@ -6983,13 +6983,13 @@
         <v>45089</v>
       </c>
       <c r="G66">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="H66" s="2">
         <v>45272</v>
       </c>
       <c r="I66">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="J66" t="inlineStr">
         <is>
@@ -7086,13 +7086,13 @@
         <v>45178</v>
       </c>
       <c r="G67">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H67" s="2">
         <v>45269</v>
       </c>
       <c r="I67">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="J67" t="inlineStr">
         <is>
@@ -7184,13 +7184,13 @@
         <v>45104</v>
       </c>
       <c r="G68">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="H68" s="2">
         <v>45196</v>
       </c>
       <c r="I68">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="J68" t="inlineStr">
         <is>
@@ -7287,13 +7287,13 @@
         <v>45149</v>
       </c>
       <c r="G69">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="H69" s="2">
         <v>45241</v>
       </c>
       <c r="I69">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="J69" t="inlineStr">
         <is>
@@ -7390,7 +7390,7 @@
         <v>45205</v>
       </c>
       <c r="I70">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="J70" t="inlineStr">
         <is>
@@ -7487,13 +7487,13 @@
         <v>45114</v>
       </c>
       <c r="G71">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="H71" s="2">
         <v>45205</v>
       </c>
       <c r="I71">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="J71" t="inlineStr">
         <is>
@@ -7590,13 +7590,13 @@
         <v>45115</v>
       </c>
       <c r="G72">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="H72" s="2">
         <v>45207</v>
       </c>
       <c r="I72">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="J72" t="inlineStr">
         <is>
@@ -7693,13 +7693,13 @@
         <v>45097</v>
       </c>
       <c r="G73">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="H73" s="2">
         <v>45189</v>
       </c>
       <c r="I73">
-        <v>-4</v>
+        <v>-5</v>
       </c>
       <c r="J73" t="inlineStr">
         <is>
@@ -7791,13 +7791,13 @@
         <v>45038</v>
       </c>
       <c r="G74">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="H74" s="2">
         <v>45221</v>
       </c>
       <c r="I74">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="J74" t="inlineStr">
         <is>
@@ -7889,13 +7889,13 @@
         <v>45117</v>
       </c>
       <c r="G75">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="H75" s="2">
         <v>45301</v>
       </c>
       <c r="I75">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="J75" t="inlineStr">
         <is>
@@ -7992,13 +7992,13 @@
         <v>45160</v>
       </c>
       <c r="G76">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="H76" s="2">
         <v>45344</v>
       </c>
       <c r="I76">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="J76" t="inlineStr">
         <is>
@@ -8095,13 +8095,13 @@
         <v>45002</v>
       </c>
       <c r="G77">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="H77" s="2">
         <v>45186</v>
       </c>
       <c r="I77">
-        <v>-7</v>
+        <v>-8</v>
       </c>
       <c r="J77" t="inlineStr">
         <is>
@@ -8198,13 +8198,13 @@
         <v>45043</v>
       </c>
       <c r="G78">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="H78" s="2">
         <v>45226</v>
       </c>
       <c r="I78">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="J78" t="inlineStr">
         <is>
@@ -8301,13 +8301,13 @@
         <v>45079</v>
       </c>
       <c r="G79">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="H79" s="2">
         <v>45262</v>
       </c>
       <c r="I79">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="J79" t="inlineStr">
         <is>
@@ -8404,7 +8404,7 @@
         <v>45254</v>
       </c>
       <c r="I80">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="J80" t="inlineStr">
         <is>
@@ -8501,13 +8501,13 @@
         <v>45104</v>
       </c>
       <c r="G81">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="H81" s="2">
         <v>45287</v>
       </c>
       <c r="I81">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="J81" t="inlineStr">
         <is>
@@ -8604,7 +8604,7 @@
         <v>45288</v>
       </c>
       <c r="I82">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="J82" t="inlineStr">
         <is>
@@ -8696,13 +8696,13 @@
         <v>45175</v>
       </c>
       <c r="G83">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="H83" s="2">
         <v>45357</v>
       </c>
       <c r="I83">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="J83" t="inlineStr">
         <is>
@@ -8799,13 +8799,13 @@
         <v>45054</v>
       </c>
       <c r="G84">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="H84" s="2">
         <v>45238</v>
       </c>
       <c r="I84">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="J84" t="inlineStr">
         <is>
@@ -8902,13 +8902,13 @@
         <v>45056</v>
       </c>
       <c r="G85">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="H85" s="2">
         <v>45240</v>
       </c>
       <c r="I85">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="J85" t="inlineStr">
         <is>
@@ -9005,13 +9005,13 @@
         <v>45085</v>
       </c>
       <c r="G86">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="H86" s="2">
         <v>45268</v>
       </c>
       <c r="I86">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="J86" t="inlineStr">
         <is>
@@ -9108,7 +9108,7 @@
         <v>45194</v>
       </c>
       <c r="I87">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J87" t="inlineStr">
         <is>
@@ -9195,13 +9195,13 @@
         <v>45103</v>
       </c>
       <c r="G88">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="H88" s="2">
         <v>45286</v>
       </c>
       <c r="I88">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="J88" t="inlineStr">
         <is>
@@ -9298,13 +9298,13 @@
         <v>45103</v>
       </c>
       <c r="G89">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="H89" s="2">
         <v>45286</v>
       </c>
       <c r="I89">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="J89" t="inlineStr">
         <is>
@@ -9401,13 +9401,13 @@
         <v>45008</v>
       </c>
       <c r="G90">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="H90" s="2">
         <v>45192</v>
       </c>
       <c r="I90">
-        <v>-1</v>
+        <v>-2</v>
       </c>
       <c r="J90" t="inlineStr">
         <is>
@@ -9499,13 +9499,13 @@
         <v>45100</v>
       </c>
       <c r="G91">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="H91" s="2">
         <v>45287</v>
       </c>
       <c r="I91">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="J91" t="inlineStr">
         <is>
@@ -9602,13 +9602,13 @@
         <v>45003</v>
       </c>
       <c r="G92">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="H92" s="2">
         <v>45187</v>
       </c>
       <c r="I92">
-        <v>-6</v>
+        <v>-7</v>
       </c>
       <c r="J92" t="inlineStr">
         <is>
@@ -9705,13 +9705,13 @@
         <v>45104</v>
       </c>
       <c r="G93">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="H93" s="2">
         <v>45287</v>
       </c>
       <c r="I93">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="J93" t="inlineStr">
         <is>
@@ -9808,13 +9808,13 @@
         <v>45104</v>
       </c>
       <c r="G94">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="H94" s="2">
         <v>45287</v>
       </c>
       <c r="I94">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="J94" t="inlineStr">
         <is>
@@ -9911,13 +9911,13 @@
         <v>45049</v>
       </c>
       <c r="G95">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="H95" s="2">
         <v>45233</v>
       </c>
       <c r="I95">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="J95" t="inlineStr">
         <is>
@@ -10014,13 +10014,13 @@
         <v>45122</v>
       </c>
       <c r="G96">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="H96" s="2">
         <v>45306</v>
       </c>
       <c r="I96">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="J96" t="inlineStr">
         <is>
@@ -10112,13 +10112,13 @@
         <v>45141</v>
       </c>
       <c r="G97">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="H97" s="2">
         <v>45325</v>
       </c>
       <c r="I97">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="J97" t="inlineStr">
         <is>
@@ -10215,13 +10215,13 @@
         <v>45010</v>
       </c>
       <c r="G98">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="H98" s="2">
         <v>45194</v>
       </c>
       <c r="I98">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J98" t="inlineStr">
         <is>
@@ -10313,13 +10313,13 @@
         <v>45093</v>
       </c>
       <c r="G99">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="H99" s="2">
         <v>45276</v>
       </c>
       <c r="I99">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="J99" t="inlineStr">
         <is>
@@ -10416,13 +10416,13 @@
         <v>45123</v>
       </c>
       <c r="G100">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="H100" s="2">
         <v>45307</v>
       </c>
       <c r="I100">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="J100" t="inlineStr">
         <is>
@@ -10519,13 +10519,13 @@
         <v>45014</v>
       </c>
       <c r="G101">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="H101" s="2">
         <v>45198</v>
       </c>
       <c r="I101">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="J101" t="inlineStr">
         <is>
@@ -10622,13 +10622,13 @@
         <v>45093</v>
       </c>
       <c r="G102">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="H102" s="2">
         <v>45276</v>
       </c>
       <c r="I102">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="J102" t="inlineStr">
         <is>
@@ -10725,13 +10725,13 @@
         <v>45122</v>
       </c>
       <c r="G103">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="H103" s="2">
         <v>45306</v>
       </c>
       <c r="I103">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="J103" t="inlineStr">
         <is>
@@ -10828,13 +10828,13 @@
         <v>45122</v>
       </c>
       <c r="G104">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="H104" s="2">
         <v>45306</v>
       </c>
       <c r="I104">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="J104" t="inlineStr">
         <is>
@@ -10926,13 +10926,13 @@
         <v>45050</v>
       </c>
       <c r="G105">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="H105" s="2">
         <v>45234</v>
       </c>
       <c r="I105">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="J105" t="inlineStr">
         <is>
@@ -11029,13 +11029,13 @@
         <v>45085</v>
       </c>
       <c r="G106">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="H106" s="2">
         <v>45268</v>
       </c>
       <c r="I106">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="J106" t="inlineStr">
         <is>
@@ -11132,13 +11132,13 @@
         <v>45093</v>
       </c>
       <c r="G107">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="H107" s="2">
         <v>45185</v>
       </c>
       <c r="I107">
-        <v>-8</v>
+        <v>-9</v>
       </c>
       <c r="J107" t="inlineStr">
         <is>
@@ -11230,13 +11230,13 @@
         <v>45093</v>
       </c>
       <c r="G108">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="H108" s="2">
         <v>45185</v>
       </c>
       <c r="I108">
-        <v>-8</v>
+        <v>-9</v>
       </c>
       <c r="J108" t="inlineStr">
         <is>
@@ -11328,13 +11328,13 @@
         <v>45093</v>
       </c>
       <c r="G109">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="H109" s="2">
         <v>45185</v>
       </c>
       <c r="I109">
-        <v>-8</v>
+        <v>-9</v>
       </c>
       <c r="J109" t="inlineStr">
         <is>
@@ -11431,13 +11431,13 @@
         <v>45148</v>
       </c>
       <c r="G110">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="H110" s="2">
         <v>45240</v>
       </c>
       <c r="I110">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="J110" t="inlineStr">
         <is>
@@ -11534,13 +11534,13 @@
         <v>45119</v>
       </c>
       <c r="G111">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="H111" s="2">
         <v>45211</v>
       </c>
       <c r="I111">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="J111" t="inlineStr">
         <is>
@@ -11637,13 +11637,13 @@
         <v>45172</v>
       </c>
       <c r="G112">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="H112" s="2">
         <v>45263</v>
       </c>
       <c r="I112">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="J112" t="inlineStr">
         <is>
@@ -11740,13 +11740,13 @@
         <v>45023</v>
       </c>
       <c r="G113">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="H113" s="2">
         <v>45206</v>
       </c>
       <c r="I113">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="J113" t="inlineStr">
         <is>
@@ -11843,13 +11843,13 @@
         <v>45111</v>
       </c>
       <c r="G114">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="H114" s="2">
         <v>45203</v>
       </c>
       <c r="I114">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="J114" t="inlineStr">
         <is>
@@ -11946,7 +11946,7 @@
         <v>45218</v>
       </c>
       <c r="I115">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="J115" t="inlineStr">
         <is>
@@ -12043,13 +12043,13 @@
         <v>45161</v>
       </c>
       <c r="G116">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="H116" s="2">
         <v>45253</v>
       </c>
       <c r="I116">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="J116" t="inlineStr">
         <is>
@@ -12146,13 +12146,13 @@
         <v>45115</v>
       </c>
       <c r="G117">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="H117" s="2">
         <v>45299</v>
       </c>
       <c r="I117">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="J117" t="inlineStr">
         <is>
@@ -12244,13 +12244,13 @@
         <v>45094</v>
       </c>
       <c r="G118">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="H118" s="2">
         <v>45277</v>
       </c>
       <c r="I118">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="J118" t="inlineStr">
         <is>
@@ -12347,13 +12347,13 @@
         <v>45104</v>
       </c>
       <c r="G119">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="H119" s="2">
         <v>45287</v>
       </c>
       <c r="I119">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="J119" t="inlineStr">
         <is>
@@ -12450,13 +12450,13 @@
         <v>45104</v>
       </c>
       <c r="G120">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="H120" s="2">
         <v>45287</v>
       </c>
       <c r="I120">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="J120" t="inlineStr">
         <is>
@@ -12553,13 +12553,13 @@
         <v>45104</v>
       </c>
       <c r="G121">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="H121" s="2">
         <v>45287</v>
       </c>
       <c r="I121">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="J121" t="inlineStr">
         <is>
@@ -12656,13 +12656,13 @@
         <v>45104</v>
       </c>
       <c r="G122">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="H122" s="2">
         <v>45287</v>
       </c>
       <c r="I122">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="J122" t="inlineStr">
         <is>
@@ -12759,13 +12759,13 @@
         <v>45107</v>
       </c>
       <c r="G123">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="H123" s="2">
         <v>45199</v>
       </c>
       <c r="I123">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="J123" t="inlineStr">
         <is>
@@ -12862,13 +12862,13 @@
         <v>45013</v>
       </c>
       <c r="G124">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="H124" s="2">
         <v>45197</v>
       </c>
       <c r="I124">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="J124" t="inlineStr">
         <is>
@@ -12965,13 +12965,13 @@
         <v>45121</v>
       </c>
       <c r="G125">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="H125" s="2">
         <v>45213</v>
       </c>
       <c r="I125">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="J125" t="inlineStr">
         <is>
@@ -13068,13 +13068,13 @@
         <v>45134</v>
       </c>
       <c r="G126">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="H126" s="2">
         <v>45226</v>
       </c>
       <c r="I126">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="J126" t="inlineStr">
         <is>
@@ -13171,7 +13171,7 @@
         <v>45212</v>
       </c>
       <c r="I127">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="J127" t="inlineStr">
         <is>
@@ -13268,13 +13268,13 @@
         <v>45126</v>
       </c>
       <c r="G128">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="H128" s="2">
         <v>45218</v>
       </c>
       <c r="I128">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="J128" t="inlineStr">
         <is>
@@ -13366,13 +13366,13 @@
         <v>45158</v>
       </c>
       <c r="G129">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="H129" s="2">
         <v>45250</v>
       </c>
       <c r="I129">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="J129" t="inlineStr">
         <is>
@@ -13469,13 +13469,13 @@
         <v>45171</v>
       </c>
       <c r="G130">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="H130" s="2">
         <v>45262</v>
       </c>
       <c r="I130">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="J130" t="inlineStr">
         <is>
@@ -13572,13 +13572,13 @@
         <v>45111</v>
       </c>
       <c r="G131">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="H131" s="2">
         <v>45203</v>
       </c>
       <c r="I131">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="J131" t="inlineStr">
         <is>
@@ -13675,13 +13675,13 @@
         <v>45144</v>
       </c>
       <c r="G132">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="H132" s="2">
         <v>45236</v>
       </c>
       <c r="I132">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="J132" t="inlineStr">
         <is>
@@ -13778,13 +13778,13 @@
         <v>45156</v>
       </c>
       <c r="G133">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="H133" s="2">
         <v>45248</v>
       </c>
       <c r="I133">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="J133" t="inlineStr">
         <is>
@@ -13876,13 +13876,13 @@
         <v>45146</v>
       </c>
       <c r="G134">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="H134" s="2">
         <v>45238</v>
       </c>
       <c r="I134">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="J134" t="inlineStr">
         <is>
@@ -13979,13 +13979,13 @@
         <v>45140</v>
       </c>
       <c r="G135">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="H135" s="2">
         <v>45232</v>
       </c>
       <c r="I135">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="J135" t="inlineStr">
         <is>
@@ -14082,13 +14082,13 @@
         <v>45104</v>
       </c>
       <c r="G136">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="H136" s="2">
         <v>45196</v>
       </c>
       <c r="I136">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="J136" t="inlineStr">
         <is>
@@ -14185,13 +14185,13 @@
         <v>45105</v>
       </c>
       <c r="G137">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="H137" s="2">
         <v>45197</v>
       </c>
       <c r="I137">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="J137" t="inlineStr">
         <is>
@@ -14288,13 +14288,13 @@
         <v>45179</v>
       </c>
       <c r="G138">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="H138" s="2">
         <v>45270</v>
       </c>
       <c r="I138">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="J138" t="inlineStr">
         <is>
@@ -14386,13 +14386,13 @@
         <v>45105</v>
       </c>
       <c r="G139">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="H139" s="2">
         <v>45197</v>
       </c>
       <c r="I139">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="J139" t="inlineStr">
         <is>
@@ -14489,13 +14489,13 @@
         <v>45182</v>
       </c>
       <c r="G140">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="H140" s="2">
         <v>45273</v>
       </c>
       <c r="I140">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="J140" t="inlineStr">
         <is>
@@ -14592,13 +14592,13 @@
         <v>45116</v>
       </c>
       <c r="G141">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="H141" s="2">
         <v>45208</v>
       </c>
       <c r="I141">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="J141" t="inlineStr">
         <is>
@@ -14690,13 +14690,13 @@
         <v>45150</v>
       </c>
       <c r="G142">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="H142" s="2">
         <v>45242</v>
       </c>
       <c r="I142">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="J142" t="inlineStr">
         <is>
@@ -14793,7 +14793,7 @@
         <v>45238</v>
       </c>
       <c r="I143">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="J143" t="inlineStr">
         <is>
@@ -14890,13 +14890,13 @@
         <v>45171</v>
       </c>
       <c r="G144">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="H144" s="2">
         <v>45262</v>
       </c>
       <c r="I144">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="J144" t="inlineStr">
         <is>
@@ -14993,13 +14993,13 @@
         <v>45102</v>
       </c>
       <c r="G145">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="H145" s="2">
         <v>45194</v>
       </c>
       <c r="I145">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J145" t="inlineStr">
         <is>
@@ -15086,13 +15086,13 @@
         <v>45119</v>
       </c>
       <c r="G146">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="H146" s="2">
         <v>45211</v>
       </c>
       <c r="I146">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="J146" t="inlineStr">
         <is>
@@ -15189,13 +15189,13 @@
         <v>45165</v>
       </c>
       <c r="G147">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="H147" s="2">
         <v>45257</v>
       </c>
       <c r="I147">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="J147" t="inlineStr">
         <is>
@@ -15292,13 +15292,13 @@
         <v>45166</v>
       </c>
       <c r="G148">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="H148" s="2">
         <v>45258</v>
       </c>
       <c r="I148">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="J148" t="inlineStr">
         <is>
@@ -15395,13 +15395,13 @@
         <v>45093</v>
       </c>
       <c r="G149">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="H149" s="2">
         <v>45185</v>
       </c>
       <c r="I149">
-        <v>-8</v>
+        <v>-9</v>
       </c>
       <c r="J149" t="inlineStr">
         <is>
@@ -15498,13 +15498,13 @@
         <v>45035</v>
       </c>
       <c r="G150">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="H150" s="2">
         <v>45218</v>
       </c>
       <c r="I150">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="J150" t="inlineStr">
         <is>
@@ -15601,13 +15601,13 @@
         <v>45174</v>
       </c>
       <c r="G151">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="H151" s="2">
         <v>45356</v>
       </c>
       <c r="I151">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="J151" t="inlineStr">
         <is>
@@ -15704,13 +15704,13 @@
         <v>45089</v>
       </c>
       <c r="G152">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="H152" s="2">
         <v>45272</v>
       </c>
       <c r="I152">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="J152" t="inlineStr">
         <is>
@@ -15807,13 +15807,13 @@
         <v>45124</v>
       </c>
       <c r="G153">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="H153" s="2">
         <v>45308</v>
       </c>
       <c r="I153">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="J153" t="inlineStr">
         <is>
@@ -15910,13 +15910,13 @@
         <v>45124</v>
       </c>
       <c r="G154">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="H154" s="2">
         <v>45308</v>
       </c>
       <c r="I154">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="J154" t="inlineStr">
         <is>
@@ -16013,13 +16013,13 @@
         <v>45026</v>
       </c>
       <c r="G155">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="H155" s="2">
         <v>45209</v>
       </c>
       <c r="I155">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="J155" t="inlineStr">
         <is>
@@ -16116,13 +16116,13 @@
         <v>45026</v>
       </c>
       <c r="G156">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="H156" s="2">
         <v>45209</v>
       </c>
       <c r="I156">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="J156" t="inlineStr">
         <is>
@@ -16219,13 +16219,13 @@
         <v>45026</v>
       </c>
       <c r="G157">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="H157" s="2">
         <v>45209</v>
       </c>
       <c r="I157">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="J157" t="inlineStr">
         <is>
@@ -16322,13 +16322,13 @@
         <v>45026</v>
       </c>
       <c r="G158">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="H158" s="2">
         <v>45209</v>
       </c>
       <c r="I158">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="J158" t="inlineStr">
         <is>
@@ -16425,13 +16425,13 @@
         <v>45156</v>
       </c>
       <c r="G159">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="H159" s="2">
         <v>45247</v>
       </c>
       <c r="I159">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="J159" t="inlineStr">
         <is>
@@ -16528,13 +16528,13 @@
         <v>45153</v>
       </c>
       <c r="G160">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="H160" s="2">
         <v>45245</v>
       </c>
       <c r="I160">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="J160" t="inlineStr">
         <is>
@@ -16631,13 +16631,13 @@
         <v>45135</v>
       </c>
       <c r="G161">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="H161" s="2">
         <v>45319</v>
       </c>
       <c r="I161">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="J161" t="inlineStr">
         <is>
@@ -16734,13 +16734,13 @@
         <v>45091</v>
       </c>
       <c r="G162">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="H162" s="2">
         <v>45274</v>
       </c>
       <c r="I162">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="J162" t="inlineStr">
         <is>
@@ -16832,13 +16832,13 @@
         <v>45091</v>
       </c>
       <c r="G163">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="H163" s="2">
         <v>45274</v>
       </c>
       <c r="I163">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="J163" t="inlineStr">
         <is>
@@ -16930,13 +16930,13 @@
         <v>45138</v>
       </c>
       <c r="G164">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="H164" s="2">
         <v>45322</v>
       </c>
       <c r="I164">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="J164" t="inlineStr">
         <is>
@@ -17033,13 +17033,13 @@
         <v>45138</v>
       </c>
       <c r="G165">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="H165" s="2">
         <v>45322</v>
       </c>
       <c r="I165">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="J165" t="inlineStr">
         <is>
@@ -17136,13 +17136,13 @@
         <v>45085</v>
       </c>
       <c r="G166">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="H166" s="2">
         <v>45268</v>
       </c>
       <c r="I166">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="J166" t="inlineStr">
         <is>
@@ -17239,13 +17239,13 @@
         <v>45085</v>
       </c>
       <c r="G167">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="H167" s="2">
         <v>45268</v>
       </c>
       <c r="I167">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="J167" t="inlineStr">
         <is>
@@ -17342,7 +17342,7 @@
         <v>45326</v>
       </c>
       <c r="I168">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="J168" t="inlineStr">
         <is>
@@ -17439,13 +17439,13 @@
         <v>45173</v>
       </c>
       <c r="G169">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="H169" s="2">
         <v>45355</v>
       </c>
       <c r="I169">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="J169" t="inlineStr">
         <is>
@@ -17542,13 +17542,13 @@
         <v>45056</v>
       </c>
       <c r="G170">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="H170" s="2">
         <v>45240</v>
       </c>
       <c r="I170">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="J170" t="inlineStr">
         <is>
@@ -17645,7 +17645,7 @@
         <v>45238</v>
       </c>
       <c r="I171">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="J171" t="inlineStr">
         <is>
@@ -17742,13 +17742,13 @@
         <v>45141</v>
       </c>
       <c r="G172">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="H172" s="2">
         <v>45325</v>
       </c>
       <c r="I172">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="J172" t="inlineStr">
         <is>
@@ -17845,13 +17845,13 @@
         <v>45037</v>
       </c>
       <c r="G173">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="H173" s="2">
         <v>45220</v>
       </c>
       <c r="I173">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="J173" t="inlineStr">
         <is>
@@ -17948,13 +17948,13 @@
         <v>45171</v>
       </c>
       <c r="G174">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="H174" s="2">
         <v>45262</v>
       </c>
       <c r="I174">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="J174" t="inlineStr">
         <is>
@@ -18051,13 +18051,13 @@
         <v>45105</v>
       </c>
       <c r="G175">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="H175" s="2">
         <v>45197</v>
       </c>
       <c r="I175">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="J175" t="inlineStr">
         <is>
@@ -18154,13 +18154,13 @@
         <v>45162</v>
       </c>
       <c r="G176">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="H176" s="2">
         <v>45254</v>
       </c>
       <c r="I176">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="J176" t="inlineStr">
         <is>
@@ -18257,13 +18257,13 @@
         <v>45061</v>
       </c>
       <c r="G177">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="H177" s="2">
         <v>45245</v>
       </c>
       <c r="I177">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="J177" t="inlineStr">
         <is>
@@ -18360,13 +18360,13 @@
         <v>45120</v>
       </c>
       <c r="G178">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="H178" s="2">
         <v>45212</v>
       </c>
       <c r="I178">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="J178" t="inlineStr">
         <is>
@@ -18463,7 +18463,7 @@
         <v>45191</v>
       </c>
       <c r="I179">
-        <v>-2</v>
+        <v>-3</v>
       </c>
       <c r="J179" t="inlineStr">
         <is>
@@ -18560,13 +18560,13 @@
         <v>45088</v>
       </c>
       <c r="G180">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="H180" s="2">
         <v>45271</v>
       </c>
       <c r="I180">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="J180" t="inlineStr">
         <is>
@@ -18663,13 +18663,13 @@
         <v>45100</v>
       </c>
       <c r="G181">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="H181" s="2">
         <v>45192</v>
       </c>
       <c r="I181">
-        <v>-1</v>
+        <v>-2</v>
       </c>
       <c r="J181" t="inlineStr">
         <is>
@@ -18756,13 +18756,13 @@
         <v>45131</v>
       </c>
       <c r="G182">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="H182" s="2">
         <v>45223</v>
       </c>
       <c r="I182">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="J182" t="inlineStr">
         <is>
@@ -18854,13 +18854,13 @@
         <v>45136</v>
       </c>
       <c r="G183">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="H183" s="2">
         <v>45228</v>
       </c>
       <c r="I183">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="J183" t="inlineStr">
         <is>
@@ -18952,13 +18952,13 @@
         <v>45150</v>
       </c>
       <c r="G184">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="H184" s="2">
         <v>45242</v>
       </c>
       <c r="I184">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="J184" t="inlineStr">
         <is>
@@ -19050,13 +19050,13 @@
         <v>45118</v>
       </c>
       <c r="G185">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="H185" s="2">
         <v>45210</v>
       </c>
       <c r="I185">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="J185" t="inlineStr">
         <is>
@@ -19148,13 +19148,13 @@
         <v>45129</v>
       </c>
       <c r="G186">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="H186" s="2">
         <v>45221</v>
       </c>
       <c r="I186">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="J186" t="inlineStr">
         <is>
@@ -19246,13 +19246,13 @@
         <v>45097</v>
       </c>
       <c r="G187">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="H187" s="2">
         <v>45189</v>
       </c>
       <c r="I187">
-        <v>-4</v>
+        <v>-5</v>
       </c>
       <c r="J187" t="inlineStr">
         <is>
@@ -19339,13 +19339,13 @@
         <v>45101</v>
       </c>
       <c r="G188">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="H188" s="2">
         <v>45193</v>
       </c>
       <c r="I188">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="J188" t="inlineStr">
         <is>
@@ -19432,13 +19432,13 @@
         <v>45165</v>
       </c>
       <c r="G189">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="H189" s="2">
         <v>45257</v>
       </c>
       <c r="I189">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="J189" t="inlineStr">
         <is>
@@ -19530,7 +19530,7 @@
         <v>45202</v>
       </c>
       <c r="I190">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="J190" t="inlineStr">
         <is>
@@ -19627,13 +19627,13 @@
         <v>45081</v>
       </c>
       <c r="G191">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="H191" s="2">
         <v>45264</v>
       </c>
       <c r="I191">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="J191" t="inlineStr">
         <is>
@@ -19730,13 +19730,13 @@
         <v>45081</v>
       </c>
       <c r="G192">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="H192" s="2">
         <v>45264</v>
       </c>
       <c r="I192">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="J192" t="inlineStr">
         <is>
@@ -19833,7 +19833,7 @@
         <v>45319</v>
       </c>
       <c r="I193">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="J193" t="inlineStr">
         <is>
@@ -19930,7 +19930,7 @@
         <v>45319</v>
       </c>
       <c r="I194">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="J194" t="inlineStr">
         <is>
@@ -20022,13 +20022,13 @@
         <v>45046</v>
       </c>
       <c r="G195">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="H195" s="2">
         <v>45230</v>
       </c>
       <c r="I195">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="J195" t="inlineStr">
         <is>
@@ -20125,13 +20125,13 @@
         <v>45046</v>
       </c>
       <c r="G196">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="H196" s="2">
         <v>45230</v>
       </c>
       <c r="I196">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="J196" t="inlineStr">
         <is>
@@ -20228,13 +20228,13 @@
         <v>45031</v>
       </c>
       <c r="G197">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="H197" s="2">
         <v>45214</v>
       </c>
       <c r="I197">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="J197" t="inlineStr">
         <is>
@@ -20331,13 +20331,13 @@
         <v>45031</v>
       </c>
       <c r="G198">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="H198" s="2">
         <v>45214</v>
       </c>
       <c r="I198">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="J198" t="inlineStr">
         <is>
@@ -20434,13 +20434,13 @@
         <v>45031</v>
       </c>
       <c r="G199">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="H199" s="2">
         <v>45214</v>
       </c>
       <c r="I199">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="J199" t="inlineStr">
         <is>
@@ -20537,13 +20537,13 @@
         <v>45031</v>
       </c>
       <c r="G200">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="H200" s="2">
         <v>45214</v>
       </c>
       <c r="I200">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="J200" t="inlineStr">
         <is>
@@ -20640,13 +20640,13 @@
         <v>45067</v>
       </c>
       <c r="G201">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="H201" s="2">
         <v>45251</v>
       </c>
       <c r="I201">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="J201" t="inlineStr">
         <is>
@@ -20743,13 +20743,13 @@
         <v>45067</v>
       </c>
       <c r="G202">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="H202" s="2">
         <v>45251</v>
       </c>
       <c r="I202">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="J202" t="inlineStr">
         <is>
@@ -20846,13 +20846,13 @@
         <v>45067</v>
       </c>
       <c r="G203">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="H203" s="2">
         <v>45251</v>
       </c>
       <c r="I203">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="J203" t="inlineStr">
         <is>
@@ -20949,13 +20949,13 @@
         <v>45067</v>
       </c>
       <c r="G204">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="H204" s="2">
         <v>45251</v>
       </c>
       <c r="I204">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="J204" t="inlineStr">
         <is>
@@ -21052,13 +21052,13 @@
         <v>45178</v>
       </c>
       <c r="G205">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H205" s="2">
         <v>45269</v>
       </c>
       <c r="I205">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="J205" t="inlineStr">
         <is>
@@ -21155,7 +21155,7 @@
         <v>45252</v>
       </c>
       <c r="I206">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="J206" t="inlineStr">
         <is>
@@ -21252,13 +21252,13 @@
         <v>45087</v>
       </c>
       <c r="G207">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="H207" s="2">
         <v>45270</v>
       </c>
       <c r="I207">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="J207" t="inlineStr">
         <is>
@@ -21355,13 +21355,13 @@
         <v>45099</v>
       </c>
       <c r="G208">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="H208" s="2">
         <v>45282</v>
       </c>
       <c r="I208">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="J208" t="inlineStr">
         <is>
@@ -21458,13 +21458,13 @@
         <v>45175</v>
       </c>
       <c r="G209">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="H209" s="2">
         <v>45356</v>
       </c>
       <c r="I209">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="J209" t="inlineStr">
         <is>
@@ -21561,13 +21561,13 @@
         <v>45175</v>
       </c>
       <c r="G210">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="H210" s="2">
         <v>45356</v>
       </c>
       <c r="I210">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="J210" t="inlineStr">
         <is>
@@ -21664,13 +21664,13 @@
         <v>45166</v>
       </c>
       <c r="G211">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="H211" s="2">
         <v>45350</v>
       </c>
       <c r="I211">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="J211" t="inlineStr">
         <is>
@@ -21767,13 +21767,13 @@
         <v>45166</v>
       </c>
       <c r="G212">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="H212" s="2">
         <v>45350</v>
       </c>
       <c r="I212">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="J212" t="inlineStr">
         <is>
@@ -21870,13 +21870,13 @@
         <v>45090</v>
       </c>
       <c r="G213">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="H213" s="2">
         <v>45273</v>
       </c>
       <c r="I213">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="J213" t="inlineStr">
         <is>
@@ -21973,13 +21973,13 @@
         <v>45106</v>
       </c>
       <c r="G214">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="H214" s="2">
         <v>45289</v>
       </c>
       <c r="I214">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="J214" t="inlineStr">
         <is>
@@ -22076,13 +22076,13 @@
         <v>45134</v>
       </c>
       <c r="G215">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="H215" s="2">
         <v>45226</v>
       </c>
       <c r="I215">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="J215" t="inlineStr">
         <is>
@@ -22179,13 +22179,13 @@
         <v>45132</v>
       </c>
       <c r="G216">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="H216" s="2">
         <v>45224</v>
       </c>
       <c r="I216">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="J216" t="inlineStr">
         <is>
@@ -22282,13 +22282,13 @@
         <v>45150</v>
       </c>
       <c r="G217">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="H217" s="2">
         <v>45242</v>
       </c>
       <c r="I217">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="J217" t="inlineStr">
         <is>
@@ -22385,13 +22385,13 @@
         <v>45095</v>
       </c>
       <c r="G218">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="H218" s="2">
         <v>45187</v>
       </c>
       <c r="I218">
-        <v>-6</v>
+        <v>-7</v>
       </c>
       <c r="J218" t="inlineStr">
         <is>
@@ -22483,13 +22483,13 @@
         <v>45182</v>
       </c>
       <c r="G219">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="H219" s="2">
         <v>45273</v>
       </c>
       <c r="I219">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="J219" t="inlineStr">
         <is>
@@ -22586,7 +22586,7 @@
         <v>45196</v>
       </c>
       <c r="I220">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="J220" t="inlineStr">
         <is>
@@ -22683,13 +22683,13 @@
         <v>45108</v>
       </c>
       <c r="G221">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="H221" s="2">
         <v>45200</v>
       </c>
       <c r="I221">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="J221" t="inlineStr">
         <is>
@@ -22786,13 +22786,13 @@
         <v>45135</v>
       </c>
       <c r="G222">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="H222" s="2">
         <v>45227</v>
       </c>
       <c r="I222">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="J222" t="inlineStr">
         <is>
@@ -22889,13 +22889,13 @@
         <v>45148</v>
       </c>
       <c r="G223">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="H223" s="2">
         <v>45240</v>
       </c>
       <c r="I223">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="J223" t="inlineStr">
         <is>
@@ -22987,13 +22987,13 @@
         <v>45100</v>
       </c>
       <c r="G224">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="H224" s="2">
         <v>45192</v>
       </c>
       <c r="I224">
-        <v>-1</v>
+        <v>-2</v>
       </c>
       <c r="J224" t="inlineStr">
         <is>
@@ -23085,13 +23085,13 @@
         <v>45136</v>
       </c>
       <c r="G225">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="H225" s="2">
         <v>45320</v>
       </c>
       <c r="I225">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="J225" t="inlineStr">
         <is>
@@ -23188,13 +23188,13 @@
         <v>45136</v>
       </c>
       <c r="G226">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="H226" s="2">
         <v>45320</v>
       </c>
       <c r="I226">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="J226" t="inlineStr">
         <is>
@@ -23291,13 +23291,13 @@
         <v>45094</v>
       </c>
       <c r="G227">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="H227" s="2">
         <v>45277</v>
       </c>
       <c r="I227">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="J227" t="inlineStr">
         <is>
@@ -23394,13 +23394,13 @@
         <v>45081</v>
       </c>
       <c r="G228">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="H228" s="2">
         <v>45264</v>
       </c>
       <c r="I228">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="J228" t="inlineStr">
         <is>
@@ -23497,13 +23497,13 @@
         <v>45099</v>
       </c>
       <c r="G229">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="H229" s="2">
         <v>45282</v>
       </c>
       <c r="I229">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="J229" t="inlineStr">
         <is>
@@ -23600,13 +23600,13 @@
         <v>45018</v>
       </c>
       <c r="G230">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="H230" s="2">
         <v>45201</v>
       </c>
       <c r="I230">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="J230" t="inlineStr">
         <is>
@@ -23703,13 +23703,13 @@
         <v>45031</v>
       </c>
       <c r="G231">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="H231" s="2">
         <v>45214</v>
       </c>
       <c r="I231">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="J231" t="inlineStr">
         <is>
@@ -23806,7 +23806,7 @@
         <v>45294</v>
       </c>
       <c r="I232">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="J232" t="inlineStr">
         <is>
@@ -23903,13 +23903,13 @@
         <v>45079</v>
       </c>
       <c r="G233">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="H233" s="2">
         <v>45262</v>
       </c>
       <c r="I233">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="J233" t="inlineStr">
         <is>
@@ -24006,7 +24006,7 @@
         <v>45199</v>
       </c>
       <c r="I234">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="J234" t="inlineStr">
         <is>
@@ -24103,13 +24103,13 @@
         <v>45021</v>
       </c>
       <c r="G235">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="H235" s="2">
         <v>45204</v>
       </c>
       <c r="I235">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="J235" t="inlineStr">
         <is>
@@ -24206,13 +24206,13 @@
         <v>45021</v>
       </c>
       <c r="G236">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="H236" s="2">
         <v>45204</v>
       </c>
       <c r="I236">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="J236" t="inlineStr">
         <is>
@@ -24309,13 +24309,13 @@
         <v>45080</v>
       </c>
       <c r="G237">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="H237" s="2">
         <v>45263</v>
       </c>
       <c r="I237">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="J237" t="inlineStr">
         <is>
@@ -24412,13 +24412,13 @@
         <v>45046</v>
       </c>
       <c r="G238">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="H238" s="2">
         <v>45229</v>
       </c>
       <c r="I238">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="J238" t="inlineStr">
         <is>
@@ -24515,13 +24515,13 @@
         <v>45112</v>
       </c>
       <c r="G239">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="H239" s="2">
         <v>45204</v>
       </c>
       <c r="I239">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="J239" t="inlineStr">
         <is>
@@ -24609,13 +24609,13 @@
         <v>45112</v>
       </c>
       <c r="G240">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="H240" s="2">
         <v>45204</v>
       </c>
       <c r="I240">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="J240" t="inlineStr">
         <is>
@@ -24703,13 +24703,13 @@
         <v>45016</v>
       </c>
       <c r="G241">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="H241" s="2">
         <v>45199</v>
       </c>
       <c r="I241">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="J241" t="inlineStr">
         <is>
@@ -24806,13 +24806,13 @@
         <v>45070</v>
       </c>
       <c r="G242">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="H242" s="2">
         <v>45254</v>
       </c>
       <c r="I242">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="J242" t="inlineStr">
         <is>
@@ -24909,13 +24909,13 @@
         <v>45168</v>
       </c>
       <c r="G243">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="H243" s="2">
         <v>45260</v>
       </c>
       <c r="I243">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="J243" t="inlineStr">
         <is>
@@ -25012,13 +25012,13 @@
         <v>45027</v>
       </c>
       <c r="G244">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="H244" s="2">
         <v>45210</v>
       </c>
       <c r="I244">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="J244" t="inlineStr">
         <is>
@@ -25115,13 +25115,13 @@
         <v>45077</v>
       </c>
       <c r="G245">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="H245" s="2">
         <v>45260</v>
       </c>
       <c r="I245">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="J245" t="inlineStr">
         <is>
@@ -25218,13 +25218,13 @@
         <v>45100</v>
       </c>
       <c r="G246">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="H246" s="2">
         <v>45283</v>
       </c>
       <c r="I246">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="J246" t="inlineStr">
         <is>
@@ -25321,7 +25321,7 @@
         <v>45281</v>
       </c>
       <c r="I247">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="J247" t="inlineStr">
         <is>
@@ -25418,13 +25418,13 @@
         <v>45044</v>
       </c>
       <c r="G248">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="H248" s="2">
         <v>45227</v>
       </c>
       <c r="I248">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="J248" t="inlineStr">
         <is>
@@ -25521,13 +25521,13 @@
         <v>45101</v>
       </c>
       <c r="G249">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="H249" s="2">
         <v>45283</v>
       </c>
       <c r="I249">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="J249" t="inlineStr">
         <is>
@@ -25624,13 +25624,13 @@
         <v>45134</v>
       </c>
       <c r="G250">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="H250" s="2">
         <v>45226</v>
       </c>
       <c r="I250">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="J250" t="inlineStr">
         <is>
@@ -25727,13 +25727,13 @@
         <v>45158</v>
       </c>
       <c r="G251">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="H251" s="2">
         <v>45250</v>
       </c>
       <c r="I251">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="J251" t="inlineStr">
         <is>
@@ -25830,13 +25830,13 @@
         <v>45108</v>
       </c>
       <c r="G252">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="H252" s="2">
         <v>45200</v>
       </c>
       <c r="I252">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="J252" t="inlineStr">
         <is>
@@ -25933,7 +25933,7 @@
         <v>45317</v>
       </c>
       <c r="I253">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="J253" t="inlineStr">
         <is>
@@ -26030,13 +26030,13 @@
         <v>45039</v>
       </c>
       <c r="G254">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="H254" s="2">
         <v>45222</v>
       </c>
       <c r="I254">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="J254" t="inlineStr">
         <is>
@@ -26128,13 +26128,13 @@
         <v>45129</v>
       </c>
       <c r="G255">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="H255" s="2">
         <v>45221</v>
       </c>
       <c r="I255">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="J255" t="inlineStr">
         <is>
@@ -26231,13 +26231,13 @@
         <v>45157</v>
       </c>
       <c r="G256">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="H256" s="2">
         <v>45341</v>
       </c>
       <c r="I256">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="J256" t="inlineStr">
         <is>
@@ -26334,13 +26334,13 @@
         <v>45063</v>
       </c>
       <c r="G257">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="H257" s="2">
         <v>45247</v>
       </c>
       <c r="I257">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="J257" t="inlineStr">
         <is>
@@ -26437,7 +26437,7 @@
         <v>45254</v>
       </c>
       <c r="I258">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="J258" t="inlineStr">
         <is>
@@ -26534,7 +26534,7 @@
         <v>45486</v>
       </c>
       <c r="I259">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="J259" t="inlineStr">
         <is>
@@ -26626,13 +26626,13 @@
         <v>45073</v>
       </c>
       <c r="G260">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="H260" s="2">
         <v>45439</v>
       </c>
       <c r="I260">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="J260" t="inlineStr">
         <is>
@@ -26724,7 +26724,7 @@
         <v>45323</v>
       </c>
       <c r="I261">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="J261" t="inlineStr">
         <is>
@@ -26816,7 +26816,7 @@
         <v>45303</v>
       </c>
       <c r="I262">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="J262" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
Bond dates update Tue Sep 26 23:08:24 UTC 2023
</commit_message>
<xml_diff>
--- a/Data/obligacje_screener.xlsx
+++ b/Data/obligacje_screener.xlsx
@@ -512,7 +512,7 @@
         <v>45340</v>
       </c>
       <c r="I2">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="J2" t="inlineStr">
         <is>
@@ -600,13 +600,13 @@
         <v>45121</v>
       </c>
       <c r="G3">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="H3" s="2">
         <v>45305</v>
       </c>
       <c r="I3">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="J3" t="inlineStr">
         <is>
@@ -703,13 +703,13 @@
         <v>45039</v>
       </c>
       <c r="G4">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="H4" s="2">
         <v>45222</v>
       </c>
       <c r="I4">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="J4" t="inlineStr">
         <is>
@@ -806,13 +806,13 @@
         <v>45039</v>
       </c>
       <c r="G5">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="H5" s="2">
         <v>45222</v>
       </c>
       <c r="I5">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="J5" t="inlineStr">
         <is>
@@ -909,13 +909,13 @@
         <v>45129</v>
       </c>
       <c r="G6">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="H6" s="2">
         <v>45221</v>
       </c>
       <c r="I6">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="J6" t="inlineStr">
         <is>
@@ -1012,13 +1012,13 @@
         <v>45162</v>
       </c>
       <c r="G7">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="H7" s="2">
         <v>45254</v>
       </c>
       <c r="I7">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="J7" t="inlineStr">
         <is>
@@ -1110,13 +1110,13 @@
         <v>45156</v>
       </c>
       <c r="G8">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="H8" s="2">
         <v>45248</v>
       </c>
       <c r="I8">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="J8" t="inlineStr">
         <is>
@@ -1213,13 +1213,13 @@
         <v>45141</v>
       </c>
       <c r="G9">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="H9" s="2">
         <v>45233</v>
       </c>
       <c r="I9">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="J9" t="inlineStr">
         <is>
@@ -1316,13 +1316,13 @@
         <v>45062</v>
       </c>
       <c r="G10">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="H10" s="2">
         <v>45246</v>
       </c>
       <c r="I10">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="J10" t="inlineStr">
         <is>
@@ -1419,7 +1419,7 @@
         <v>45286</v>
       </c>
       <c r="I11">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="J11" t="inlineStr">
         <is>
@@ -1516,13 +1516,13 @@
         <v>45011</v>
       </c>
       <c r="G12">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="H12" s="2">
         <v>45195</v>
       </c>
       <c r="I12">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J12" t="inlineStr">
         <is>
@@ -1614,13 +1614,13 @@
         <v>45036</v>
       </c>
       <c r="G13">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="H13" s="2">
         <v>45219</v>
       </c>
       <c r="I13">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="J13" t="inlineStr">
         <is>
@@ -1717,13 +1717,13 @@
         <v>45036</v>
       </c>
       <c r="G14">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="H14" s="2">
         <v>45219</v>
       </c>
       <c r="I14">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="J14" t="inlineStr">
         <is>
@@ -1820,13 +1820,13 @@
         <v>45106</v>
       </c>
       <c r="G15">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="H15" s="2">
         <v>45289</v>
       </c>
       <c r="I15">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="J15" t="inlineStr">
         <is>
@@ -1923,13 +1923,13 @@
         <v>45094</v>
       </c>
       <c r="G16">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="H16" s="2">
         <v>45186</v>
       </c>
       <c r="I16">
-        <v>-8</v>
+        <v>-9</v>
       </c>
       <c r="J16" t="inlineStr">
         <is>
@@ -2026,13 +2026,13 @@
         <v>45094</v>
       </c>
       <c r="G17">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="H17" s="2">
         <v>45186</v>
       </c>
       <c r="I17">
-        <v>-8</v>
+        <v>-9</v>
       </c>
       <c r="J17" t="inlineStr">
         <is>
@@ -2129,13 +2129,13 @@
         <v>45132</v>
       </c>
       <c r="G18">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="H18" s="2">
         <v>45224</v>
       </c>
       <c r="I18">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="J18" t="inlineStr">
         <is>
@@ -2232,13 +2232,13 @@
         <v>45137</v>
       </c>
       <c r="G19">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="H19" s="2">
         <v>45229</v>
       </c>
       <c r="I19">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="J19" t="inlineStr">
         <is>
@@ -2330,13 +2330,13 @@
         <v>45183</v>
       </c>
       <c r="G20">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="H20" s="2">
         <v>45274</v>
       </c>
       <c r="I20">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="J20" t="inlineStr">
         <is>
@@ -2433,13 +2433,13 @@
         <v>45093</v>
       </c>
       <c r="G21">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="H21" s="2">
         <v>45187</v>
       </c>
       <c r="I21">
-        <v>-7</v>
+        <v>-8</v>
       </c>
       <c r="J21" t="inlineStr">
         <is>
@@ -2536,13 +2536,13 @@
         <v>45096</v>
       </c>
       <c r="G22">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="H22" s="2">
         <v>45187</v>
       </c>
       <c r="I22">
-        <v>-7</v>
+        <v>-8</v>
       </c>
       <c r="J22" t="inlineStr">
         <is>
@@ -2639,7 +2639,7 @@
         <v>45245</v>
       </c>
       <c r="I23">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="J23" t="inlineStr">
         <is>
@@ -2736,7 +2736,7 @@
         <v>45245</v>
       </c>
       <c r="I24">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="J24" t="inlineStr">
         <is>
@@ -2833,13 +2833,13 @@
         <v>45021</v>
       </c>
       <c r="G25">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="H25" s="2">
         <v>45204</v>
       </c>
       <c r="I25">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="J25" t="inlineStr">
         <is>
@@ -2936,13 +2936,13 @@
         <v>45160</v>
       </c>
       <c r="G26">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="H26" s="2">
         <v>45344</v>
       </c>
       <c r="I26">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="J26" t="inlineStr">
         <is>
@@ -3039,13 +3039,13 @@
         <v>45118</v>
       </c>
       <c r="G27">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="H27" s="2">
         <v>45302</v>
       </c>
       <c r="I27">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="J27" t="inlineStr">
         <is>
@@ -3142,13 +3142,13 @@
         <v>45085</v>
       </c>
       <c r="G28">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="H28" s="2">
         <v>45268</v>
       </c>
       <c r="I28">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="J28" t="inlineStr">
         <is>
@@ -3245,13 +3245,13 @@
         <v>45183</v>
       </c>
       <c r="G29">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="H29" s="2">
         <v>45274</v>
       </c>
       <c r="I29">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="J29" t="inlineStr">
         <is>
@@ -3348,7 +3348,7 @@
         <v>45224</v>
       </c>
       <c r="I30">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="J30" t="inlineStr">
         <is>
@@ -3445,13 +3445,13 @@
         <v>45153</v>
       </c>
       <c r="G31">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="H31" s="2">
         <v>45245</v>
       </c>
       <c r="I31">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="J31" t="inlineStr">
         <is>
@@ -3548,13 +3548,13 @@
         <v>45155</v>
       </c>
       <c r="G32">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="H32" s="2">
         <v>45247</v>
       </c>
       <c r="I32">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="J32" t="inlineStr">
         <is>
@@ -3651,7 +3651,7 @@
         <v>45255</v>
       </c>
       <c r="I33">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="J33" t="inlineStr">
         <is>
@@ -3739,13 +3739,13 @@
         <v>45176</v>
       </c>
       <c r="G34">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="H34" s="2">
         <v>45267</v>
       </c>
       <c r="I34">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="J34" t="inlineStr">
         <is>
@@ -3842,13 +3842,13 @@
         <v>45130</v>
       </c>
       <c r="G35">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="H35" s="2">
         <v>45222</v>
       </c>
       <c r="I35">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="J35" t="inlineStr">
         <is>
@@ -3940,13 +3940,13 @@
         <v>45115</v>
       </c>
       <c r="G36">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="H36" s="2">
         <v>45207</v>
       </c>
       <c r="I36">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="J36" t="inlineStr">
         <is>
@@ -4043,13 +4043,13 @@
         <v>45097</v>
       </c>
       <c r="G37">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="H37" s="2">
         <v>45189</v>
       </c>
       <c r="I37">
-        <v>-5</v>
+        <v>-6</v>
       </c>
       <c r="J37" t="inlineStr">
         <is>
@@ -4141,13 +4141,13 @@
         <v>45107</v>
       </c>
       <c r="G38">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="H38" s="2">
         <v>45290</v>
       </c>
       <c r="I38">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="J38" t="inlineStr">
         <is>
@@ -4244,13 +4244,13 @@
         <v>45063</v>
       </c>
       <c r="G39">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="H39" s="2">
         <v>45247</v>
       </c>
       <c r="I39">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="J39" t="inlineStr">
         <is>
@@ -4347,13 +4347,13 @@
         <v>45177</v>
       </c>
       <c r="G40">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="H40" s="2">
         <v>45359</v>
       </c>
       <c r="I40">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="J40" t="inlineStr">
         <is>
@@ -4450,13 +4450,13 @@
         <v>45107</v>
       </c>
       <c r="G41">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="H41" s="2">
         <v>45290</v>
       </c>
       <c r="I41">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="J41" t="inlineStr">
         <is>
@@ -4553,7 +4553,7 @@
         <v>45265</v>
       </c>
       <c r="I42">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="J42" t="inlineStr">
         <is>
@@ -4650,13 +4650,13 @@
         <v>45098</v>
       </c>
       <c r="G43">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="H43" s="2">
         <v>45281</v>
       </c>
       <c r="I43">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="J43" t="inlineStr">
         <is>
@@ -4753,13 +4753,13 @@
         <v>45099</v>
       </c>
       <c r="G44">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="H44" s="2">
         <v>45282</v>
       </c>
       <c r="I44">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="J44" t="inlineStr">
         <is>
@@ -4856,13 +4856,13 @@
         <v>45106</v>
       </c>
       <c r="G45">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="H45" s="2">
         <v>45289</v>
       </c>
       <c r="I45">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="J45" t="inlineStr">
         <is>
@@ -4959,13 +4959,13 @@
         <v>45106</v>
       </c>
       <c r="G46">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="H46" s="2">
         <v>45289</v>
       </c>
       <c r="I46">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="J46" t="inlineStr">
         <is>
@@ -5062,13 +5062,13 @@
         <v>45120</v>
       </c>
       <c r="G47">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="H47" s="2">
         <v>45304</v>
       </c>
       <c r="I47">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="J47" t="inlineStr">
         <is>
@@ -5165,13 +5165,13 @@
         <v>45118</v>
       </c>
       <c r="G48">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="H48" s="2">
         <v>45302</v>
       </c>
       <c r="I48">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="J48" t="inlineStr">
         <is>
@@ -5268,13 +5268,13 @@
         <v>45152</v>
       </c>
       <c r="G49">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="H49" s="2">
         <v>45336</v>
       </c>
       <c r="I49">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="J49" t="inlineStr">
         <is>
@@ -5371,13 +5371,13 @@
         <v>45042</v>
       </c>
       <c r="G50">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="H50" s="2">
         <v>45225</v>
       </c>
       <c r="I50">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="J50" t="inlineStr">
         <is>
@@ -5474,13 +5474,13 @@
         <v>45122</v>
       </c>
       <c r="G51">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="H51" s="2">
         <v>45306</v>
       </c>
       <c r="I51">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="J51" t="inlineStr">
         <is>
@@ -5577,13 +5577,13 @@
         <v>45139</v>
       </c>
       <c r="G52">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="H52" s="2">
         <v>45323</v>
       </c>
       <c r="I52">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="J52" t="inlineStr">
         <is>
@@ -5671,13 +5671,13 @@
         <v>45099</v>
       </c>
       <c r="G53">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="H53" s="2">
         <v>45282</v>
       </c>
       <c r="I53">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="J53" t="inlineStr">
         <is>
@@ -5774,7 +5774,7 @@
         <v>45196</v>
       </c>
       <c r="I54">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J54" t="inlineStr">
         <is>
@@ -5871,13 +5871,13 @@
         <v>45044</v>
       </c>
       <c r="G55">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="H55" s="2">
         <v>45227</v>
       </c>
       <c r="I55">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="J55" t="inlineStr">
         <is>
@@ -5974,13 +5974,13 @@
         <v>45151</v>
       </c>
       <c r="G56">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="H56" s="2">
         <v>45243</v>
       </c>
       <c r="I56">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="J56" t="inlineStr">
         <is>
@@ -6072,7 +6072,7 @@
         <v>45196</v>
       </c>
       <c r="I57">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J57" t="inlineStr">
         <is>
@@ -6169,13 +6169,13 @@
         <v>45069</v>
       </c>
       <c r="G58">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="H58" s="2">
         <v>45253</v>
       </c>
       <c r="I58">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="J58" t="inlineStr">
         <is>
@@ -6272,13 +6272,13 @@
         <v>45099</v>
       </c>
       <c r="G59">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="H59" s="2">
         <v>45191</v>
       </c>
       <c r="I59">
-        <v>-3</v>
+        <v>-4</v>
       </c>
       <c r="J59" t="inlineStr">
         <is>
@@ -6370,13 +6370,13 @@
         <v>45113</v>
       </c>
       <c r="G60">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="H60" s="2">
         <v>45205</v>
       </c>
       <c r="I60">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="J60" t="inlineStr">
         <is>
@@ -6473,13 +6473,13 @@
         <v>45127</v>
       </c>
       <c r="G61">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="H61" s="2">
         <v>45219</v>
       </c>
       <c r="I61">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="J61" t="inlineStr">
         <is>
@@ -6576,13 +6576,13 @@
         <v>45058</v>
       </c>
       <c r="G62">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="H62" s="2">
         <v>45242</v>
       </c>
       <c r="I62">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="J62" t="inlineStr">
         <is>
@@ -6679,13 +6679,13 @@
         <v>45010</v>
       </c>
       <c r="G63">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="H63" s="2">
         <v>45194</v>
       </c>
       <c r="I63">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="J63" t="inlineStr">
         <is>
@@ -6777,13 +6777,13 @@
         <v>45025</v>
       </c>
       <c r="G64">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="H64" s="2">
         <v>45208</v>
       </c>
       <c r="I64">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="J64" t="inlineStr">
         <is>
@@ -6880,13 +6880,13 @@
         <v>45025</v>
       </c>
       <c r="G65">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="H65" s="2">
         <v>45208</v>
       </c>
       <c r="I65">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="J65" t="inlineStr">
         <is>
@@ -6983,13 +6983,13 @@
         <v>45089</v>
       </c>
       <c r="G66">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="H66" s="2">
         <v>45272</v>
       </c>
       <c r="I66">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="J66" t="inlineStr">
         <is>
@@ -7086,13 +7086,13 @@
         <v>45178</v>
       </c>
       <c r="G67">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="H67" s="2">
         <v>45269</v>
       </c>
       <c r="I67">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="J67" t="inlineStr">
         <is>
@@ -7184,13 +7184,13 @@
         <v>45104</v>
       </c>
       <c r="G68">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="H68" s="2">
         <v>45196</v>
       </c>
       <c r="I68">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J68" t="inlineStr">
         <is>
@@ -7287,13 +7287,13 @@
         <v>45149</v>
       </c>
       <c r="G69">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="H69" s="2">
         <v>45241</v>
       </c>
       <c r="I69">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="J69" t="inlineStr">
         <is>
@@ -7390,7 +7390,7 @@
         <v>45205</v>
       </c>
       <c r="I70">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="J70" t="inlineStr">
         <is>
@@ -7487,13 +7487,13 @@
         <v>45114</v>
       </c>
       <c r="G71">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="H71" s="2">
         <v>45205</v>
       </c>
       <c r="I71">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="J71" t="inlineStr">
         <is>
@@ -7590,13 +7590,13 @@
         <v>45115</v>
       </c>
       <c r="G72">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="H72" s="2">
         <v>45207</v>
       </c>
       <c r="I72">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="J72" t="inlineStr">
         <is>
@@ -7693,13 +7693,13 @@
         <v>45097</v>
       </c>
       <c r="G73">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="H73" s="2">
         <v>45189</v>
       </c>
       <c r="I73">
-        <v>-5</v>
+        <v>-6</v>
       </c>
       <c r="J73" t="inlineStr">
         <is>
@@ -7791,13 +7791,13 @@
         <v>45038</v>
       </c>
       <c r="G74">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="H74" s="2">
         <v>45221</v>
       </c>
       <c r="I74">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="J74" t="inlineStr">
         <is>
@@ -7889,13 +7889,13 @@
         <v>45117</v>
       </c>
       <c r="G75">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="H75" s="2">
         <v>45301</v>
       </c>
       <c r="I75">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="J75" t="inlineStr">
         <is>
@@ -7992,13 +7992,13 @@
         <v>45160</v>
       </c>
       <c r="G76">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="H76" s="2">
         <v>45344</v>
       </c>
       <c r="I76">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="J76" t="inlineStr">
         <is>
@@ -8095,13 +8095,13 @@
         <v>45002</v>
       </c>
       <c r="G77">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="H77" s="2">
         <v>45186</v>
       </c>
       <c r="I77">
-        <v>-8</v>
+        <v>-9</v>
       </c>
       <c r="J77" t="inlineStr">
         <is>
@@ -8198,13 +8198,13 @@
         <v>45043</v>
       </c>
       <c r="G78">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="H78" s="2">
         <v>45226</v>
       </c>
       <c r="I78">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="J78" t="inlineStr">
         <is>
@@ -8301,13 +8301,13 @@
         <v>45079</v>
       </c>
       <c r="G79">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="H79" s="2">
         <v>45262</v>
       </c>
       <c r="I79">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="J79" t="inlineStr">
         <is>
@@ -8404,7 +8404,7 @@
         <v>45254</v>
       </c>
       <c r="I80">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="J80" t="inlineStr">
         <is>
@@ -8501,13 +8501,13 @@
         <v>45104</v>
       </c>
       <c r="G81">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="H81" s="2">
         <v>45287</v>
       </c>
       <c r="I81">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="J81" t="inlineStr">
         <is>
@@ -8604,7 +8604,7 @@
         <v>45288</v>
       </c>
       <c r="I82">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="J82" t="inlineStr">
         <is>
@@ -8696,13 +8696,13 @@
         <v>45175</v>
       </c>
       <c r="G83">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="H83" s="2">
         <v>45357</v>
       </c>
       <c r="I83">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="J83" t="inlineStr">
         <is>
@@ -8799,13 +8799,13 @@
         <v>45054</v>
       </c>
       <c r="G84">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="H84" s="2">
         <v>45238</v>
       </c>
       <c r="I84">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="J84" t="inlineStr">
         <is>
@@ -8902,13 +8902,13 @@
         <v>45056</v>
       </c>
       <c r="G85">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="H85" s="2">
         <v>45240</v>
       </c>
       <c r="I85">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="J85" t="inlineStr">
         <is>
@@ -9005,13 +9005,13 @@
         <v>45085</v>
       </c>
       <c r="G86">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="H86" s="2">
         <v>45268</v>
       </c>
       <c r="I86">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="J86" t="inlineStr">
         <is>
@@ -9108,7 +9108,7 @@
         <v>45194</v>
       </c>
       <c r="I87">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="J87" t="inlineStr">
         <is>
@@ -9195,13 +9195,13 @@
         <v>45103</v>
       </c>
       <c r="G88">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="H88" s="2">
         <v>45286</v>
       </c>
       <c r="I88">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="J88" t="inlineStr">
         <is>
@@ -9298,13 +9298,13 @@
         <v>45103</v>
       </c>
       <c r="G89">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="H89" s="2">
         <v>45286</v>
       </c>
       <c r="I89">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="J89" t="inlineStr">
         <is>
@@ -9401,13 +9401,13 @@
         <v>45008</v>
       </c>
       <c r="G90">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="H90" s="2">
         <v>45192</v>
       </c>
       <c r="I90">
-        <v>-2</v>
+        <v>-3</v>
       </c>
       <c r="J90" t="inlineStr">
         <is>
@@ -9499,13 +9499,13 @@
         <v>45100</v>
       </c>
       <c r="G91">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="H91" s="2">
         <v>45287</v>
       </c>
       <c r="I91">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="J91" t="inlineStr">
         <is>
@@ -9602,13 +9602,13 @@
         <v>45003</v>
       </c>
       <c r="G92">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="H92" s="2">
         <v>45187</v>
       </c>
       <c r="I92">
-        <v>-7</v>
+        <v>-8</v>
       </c>
       <c r="J92" t="inlineStr">
         <is>
@@ -9705,13 +9705,13 @@
         <v>45104</v>
       </c>
       <c r="G93">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="H93" s="2">
         <v>45287</v>
       </c>
       <c r="I93">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="J93" t="inlineStr">
         <is>
@@ -9808,13 +9808,13 @@
         <v>45104</v>
       </c>
       <c r="G94">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="H94" s="2">
         <v>45287</v>
       </c>
       <c r="I94">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="J94" t="inlineStr">
         <is>
@@ -9911,13 +9911,13 @@
         <v>45049</v>
       </c>
       <c r="G95">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="H95" s="2">
         <v>45233</v>
       </c>
       <c r="I95">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="J95" t="inlineStr">
         <is>
@@ -10014,13 +10014,13 @@
         <v>45122</v>
       </c>
       <c r="G96">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="H96" s="2">
         <v>45306</v>
       </c>
       <c r="I96">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="J96" t="inlineStr">
         <is>
@@ -10112,13 +10112,13 @@
         <v>45141</v>
       </c>
       <c r="G97">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="H97" s="2">
         <v>45325</v>
       </c>
       <c r="I97">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="J97" t="inlineStr">
         <is>
@@ -10215,13 +10215,13 @@
         <v>45010</v>
       </c>
       <c r="G98">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="H98" s="2">
         <v>45194</v>
       </c>
       <c r="I98">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="J98" t="inlineStr">
         <is>
@@ -10313,13 +10313,13 @@
         <v>45093</v>
       </c>
       <c r="G99">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="H99" s="2">
         <v>45276</v>
       </c>
       <c r="I99">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="J99" t="inlineStr">
         <is>
@@ -10416,13 +10416,13 @@
         <v>45123</v>
       </c>
       <c r="G100">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="H100" s="2">
         <v>45307</v>
       </c>
       <c r="I100">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="J100" t="inlineStr">
         <is>
@@ -10519,13 +10519,13 @@
         <v>45014</v>
       </c>
       <c r="G101">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="H101" s="2">
         <v>45198</v>
       </c>
       <c r="I101">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="J101" t="inlineStr">
         <is>
@@ -10622,13 +10622,13 @@
         <v>45093</v>
       </c>
       <c r="G102">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="H102" s="2">
         <v>45276</v>
       </c>
       <c r="I102">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="J102" t="inlineStr">
         <is>
@@ -10725,13 +10725,13 @@
         <v>45122</v>
       </c>
       <c r="G103">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="H103" s="2">
         <v>45306</v>
       </c>
       <c r="I103">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="J103" t="inlineStr">
         <is>
@@ -10828,13 +10828,13 @@
         <v>45122</v>
       </c>
       <c r="G104">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="H104" s="2">
         <v>45306</v>
       </c>
       <c r="I104">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="J104" t="inlineStr">
         <is>
@@ -10926,13 +10926,13 @@
         <v>45050</v>
       </c>
       <c r="G105">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="H105" s="2">
         <v>45234</v>
       </c>
       <c r="I105">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="J105" t="inlineStr">
         <is>
@@ -11029,13 +11029,13 @@
         <v>45085</v>
       </c>
       <c r="G106">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="H106" s="2">
         <v>45268</v>
       </c>
       <c r="I106">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="J106" t="inlineStr">
         <is>
@@ -11132,13 +11132,13 @@
         <v>45093</v>
       </c>
       <c r="G107">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="H107" s="2">
         <v>45185</v>
       </c>
       <c r="I107">
-        <v>-9</v>
+        <v>-10</v>
       </c>
       <c r="J107" t="inlineStr">
         <is>
@@ -11230,13 +11230,13 @@
         <v>45093</v>
       </c>
       <c r="G108">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="H108" s="2">
         <v>45185</v>
       </c>
       <c r="I108">
-        <v>-9</v>
+        <v>-10</v>
       </c>
       <c r="J108" t="inlineStr">
         <is>
@@ -11328,13 +11328,13 @@
         <v>45093</v>
       </c>
       <c r="G109">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="H109" s="2">
         <v>45185</v>
       </c>
       <c r="I109">
-        <v>-9</v>
+        <v>-10</v>
       </c>
       <c r="J109" t="inlineStr">
         <is>
@@ -11431,13 +11431,13 @@
         <v>45148</v>
       </c>
       <c r="G110">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="H110" s="2">
         <v>45240</v>
       </c>
       <c r="I110">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="J110" t="inlineStr">
         <is>
@@ -11534,13 +11534,13 @@
         <v>45119</v>
       </c>
       <c r="G111">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="H111" s="2">
         <v>45211</v>
       </c>
       <c r="I111">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="J111" t="inlineStr">
         <is>
@@ -11637,13 +11637,13 @@
         <v>45172</v>
       </c>
       <c r="G112">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="H112" s="2">
         <v>45263</v>
       </c>
       <c r="I112">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="J112" t="inlineStr">
         <is>
@@ -11740,13 +11740,13 @@
         <v>45023</v>
       </c>
       <c r="G113">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="H113" s="2">
         <v>45206</v>
       </c>
       <c r="I113">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="J113" t="inlineStr">
         <is>
@@ -11843,13 +11843,13 @@
         <v>45111</v>
       </c>
       <c r="G114">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="H114" s="2">
         <v>45203</v>
       </c>
       <c r="I114">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="J114" t="inlineStr">
         <is>
@@ -11946,7 +11946,7 @@
         <v>45218</v>
       </c>
       <c r="I115">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="J115" t="inlineStr">
         <is>
@@ -12043,13 +12043,13 @@
         <v>45161</v>
       </c>
       <c r="G116">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="H116" s="2">
         <v>45253</v>
       </c>
       <c r="I116">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="J116" t="inlineStr">
         <is>
@@ -12146,13 +12146,13 @@
         <v>45115</v>
       </c>
       <c r="G117">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="H117" s="2">
         <v>45299</v>
       </c>
       <c r="I117">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="J117" t="inlineStr">
         <is>
@@ -12244,13 +12244,13 @@
         <v>45094</v>
       </c>
       <c r="G118">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="H118" s="2">
         <v>45277</v>
       </c>
       <c r="I118">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="J118" t="inlineStr">
         <is>
@@ -12347,13 +12347,13 @@
         <v>45104</v>
       </c>
       <c r="G119">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="H119" s="2">
         <v>45287</v>
       </c>
       <c r="I119">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="J119" t="inlineStr">
         <is>
@@ -12450,13 +12450,13 @@
         <v>45104</v>
       </c>
       <c r="G120">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="H120" s="2">
         <v>45287</v>
       </c>
       <c r="I120">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="J120" t="inlineStr">
         <is>
@@ -12553,13 +12553,13 @@
         <v>45104</v>
       </c>
       <c r="G121">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="H121" s="2">
         <v>45287</v>
       </c>
       <c r="I121">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="J121" t="inlineStr">
         <is>
@@ -12656,13 +12656,13 @@
         <v>45104</v>
       </c>
       <c r="G122">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="H122" s="2">
         <v>45287</v>
       </c>
       <c r="I122">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="J122" t="inlineStr">
         <is>
@@ -12759,13 +12759,13 @@
         <v>45107</v>
       </c>
       <c r="G123">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="H123" s="2">
         <v>45199</v>
       </c>
       <c r="I123">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="J123" t="inlineStr">
         <is>
@@ -12862,13 +12862,13 @@
         <v>45013</v>
       </c>
       <c r="G124">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="H124" s="2">
         <v>45197</v>
       </c>
       <c r="I124">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="J124" t="inlineStr">
         <is>
@@ -12965,13 +12965,13 @@
         <v>45121</v>
       </c>
       <c r="G125">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="H125" s="2">
         <v>45213</v>
       </c>
       <c r="I125">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="J125" t="inlineStr">
         <is>
@@ -13068,13 +13068,13 @@
         <v>45134</v>
       </c>
       <c r="G126">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="H126" s="2">
         <v>45226</v>
       </c>
       <c r="I126">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="J126" t="inlineStr">
         <is>
@@ -13171,7 +13171,7 @@
         <v>45212</v>
       </c>
       <c r="I127">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="J127" t="inlineStr">
         <is>
@@ -13268,13 +13268,13 @@
         <v>45126</v>
       </c>
       <c r="G128">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="H128" s="2">
         <v>45218</v>
       </c>
       <c r="I128">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="J128" t="inlineStr">
         <is>
@@ -13366,13 +13366,13 @@
         <v>45158</v>
       </c>
       <c r="G129">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="H129" s="2">
         <v>45250</v>
       </c>
       <c r="I129">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="J129" t="inlineStr">
         <is>
@@ -13469,13 +13469,13 @@
         <v>45171</v>
       </c>
       <c r="G130">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="H130" s="2">
         <v>45262</v>
       </c>
       <c r="I130">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="J130" t="inlineStr">
         <is>
@@ -13572,13 +13572,13 @@
         <v>45111</v>
       </c>
       <c r="G131">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="H131" s="2">
         <v>45203</v>
       </c>
       <c r="I131">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="J131" t="inlineStr">
         <is>
@@ -13675,13 +13675,13 @@
         <v>45144</v>
       </c>
       <c r="G132">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="H132" s="2">
         <v>45236</v>
       </c>
       <c r="I132">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="J132" t="inlineStr">
         <is>
@@ -13778,13 +13778,13 @@
         <v>45156</v>
       </c>
       <c r="G133">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="H133" s="2">
         <v>45248</v>
       </c>
       <c r="I133">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="J133" t="inlineStr">
         <is>
@@ -13876,13 +13876,13 @@
         <v>45146</v>
       </c>
       <c r="G134">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="H134" s="2">
         <v>45238</v>
       </c>
       <c r="I134">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="J134" t="inlineStr">
         <is>
@@ -13979,13 +13979,13 @@
         <v>45140</v>
       </c>
       <c r="G135">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="H135" s="2">
         <v>45232</v>
       </c>
       <c r="I135">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="J135" t="inlineStr">
         <is>
@@ -14082,13 +14082,13 @@
         <v>45104</v>
       </c>
       <c r="G136">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="H136" s="2">
         <v>45196</v>
       </c>
       <c r="I136">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J136" t="inlineStr">
         <is>
@@ -14185,13 +14185,13 @@
         <v>45105</v>
       </c>
       <c r="G137">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="H137" s="2">
         <v>45197</v>
       </c>
       <c r="I137">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="J137" t="inlineStr">
         <is>
@@ -14288,13 +14288,13 @@
         <v>45179</v>
       </c>
       <c r="G138">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H138" s="2">
         <v>45270</v>
       </c>
       <c r="I138">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="J138" t="inlineStr">
         <is>
@@ -14386,13 +14386,13 @@
         <v>45105</v>
       </c>
       <c r="G139">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="H139" s="2">
         <v>45197</v>
       </c>
       <c r="I139">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="J139" t="inlineStr">
         <is>
@@ -14489,13 +14489,13 @@
         <v>45182</v>
       </c>
       <c r="G140">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="H140" s="2">
         <v>45273</v>
       </c>
       <c r="I140">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="J140" t="inlineStr">
         <is>
@@ -14592,13 +14592,13 @@
         <v>45116</v>
       </c>
       <c r="G141">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="H141" s="2">
         <v>45208</v>
       </c>
       <c r="I141">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="J141" t="inlineStr">
         <is>
@@ -14690,13 +14690,13 @@
         <v>45150</v>
       </c>
       <c r="G142">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="H142" s="2">
         <v>45242</v>
       </c>
       <c r="I142">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="J142" t="inlineStr">
         <is>
@@ -14793,7 +14793,7 @@
         <v>45238</v>
       </c>
       <c r="I143">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="J143" t="inlineStr">
         <is>
@@ -14890,13 +14890,13 @@
         <v>45171</v>
       </c>
       <c r="G144">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="H144" s="2">
         <v>45262</v>
       </c>
       <c r="I144">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="J144" t="inlineStr">
         <is>
@@ -14993,13 +14993,13 @@
         <v>45102</v>
       </c>
       <c r="G145">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="H145" s="2">
         <v>45194</v>
       </c>
       <c r="I145">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="J145" t="inlineStr">
         <is>
@@ -15086,13 +15086,13 @@
         <v>45119</v>
       </c>
       <c r="G146">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="H146" s="2">
         <v>45211</v>
       </c>
       <c r="I146">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="J146" t="inlineStr">
         <is>
@@ -15189,13 +15189,13 @@
         <v>45165</v>
       </c>
       <c r="G147">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="H147" s="2">
         <v>45257</v>
       </c>
       <c r="I147">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="J147" t="inlineStr">
         <is>
@@ -15292,13 +15292,13 @@
         <v>45166</v>
       </c>
       <c r="G148">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="H148" s="2">
         <v>45258</v>
       </c>
       <c r="I148">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="J148" t="inlineStr">
         <is>
@@ -15395,13 +15395,13 @@
         <v>45093</v>
       </c>
       <c r="G149">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="H149" s="2">
         <v>45185</v>
       </c>
       <c r="I149">
-        <v>-9</v>
+        <v>-10</v>
       </c>
       <c r="J149" t="inlineStr">
         <is>
@@ -15498,13 +15498,13 @@
         <v>45035</v>
       </c>
       <c r="G150">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="H150" s="2">
         <v>45218</v>
       </c>
       <c r="I150">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="J150" t="inlineStr">
         <is>
@@ -15601,13 +15601,13 @@
         <v>45174</v>
       </c>
       <c r="G151">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="H151" s="2">
         <v>45356</v>
       </c>
       <c r="I151">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="J151" t="inlineStr">
         <is>
@@ -15704,13 +15704,13 @@
         <v>45089</v>
       </c>
       <c r="G152">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="H152" s="2">
         <v>45272</v>
       </c>
       <c r="I152">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="J152" t="inlineStr">
         <is>
@@ -15807,13 +15807,13 @@
         <v>45124</v>
       </c>
       <c r="G153">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="H153" s="2">
         <v>45308</v>
       </c>
       <c r="I153">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="J153" t="inlineStr">
         <is>
@@ -15910,13 +15910,13 @@
         <v>45124</v>
       </c>
       <c r="G154">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="H154" s="2">
         <v>45308</v>
       </c>
       <c r="I154">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="J154" t="inlineStr">
         <is>
@@ -16013,13 +16013,13 @@
         <v>45026</v>
       </c>
       <c r="G155">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="H155" s="2">
         <v>45209</v>
       </c>
       <c r="I155">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="J155" t="inlineStr">
         <is>
@@ -16116,13 +16116,13 @@
         <v>45026</v>
       </c>
       <c r="G156">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="H156" s="2">
         <v>45209</v>
       </c>
       <c r="I156">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="J156" t="inlineStr">
         <is>
@@ -16219,13 +16219,13 @@
         <v>45026</v>
       </c>
       <c r="G157">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="H157" s="2">
         <v>45209</v>
       </c>
       <c r="I157">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="J157" t="inlineStr">
         <is>
@@ -16322,13 +16322,13 @@
         <v>45026</v>
       </c>
       <c r="G158">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="H158" s="2">
         <v>45209</v>
       </c>
       <c r="I158">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="J158" t="inlineStr">
         <is>
@@ -16425,13 +16425,13 @@
         <v>45156</v>
       </c>
       <c r="G159">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="H159" s="2">
         <v>45247</v>
       </c>
       <c r="I159">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="J159" t="inlineStr">
         <is>
@@ -16528,13 +16528,13 @@
         <v>45153</v>
       </c>
       <c r="G160">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="H160" s="2">
         <v>45245</v>
       </c>
       <c r="I160">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="J160" t="inlineStr">
         <is>
@@ -16631,13 +16631,13 @@
         <v>45135</v>
       </c>
       <c r="G161">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="H161" s="2">
         <v>45319</v>
       </c>
       <c r="I161">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="J161" t="inlineStr">
         <is>
@@ -16734,13 +16734,13 @@
         <v>45091</v>
       </c>
       <c r="G162">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="H162" s="2">
         <v>45274</v>
       </c>
       <c r="I162">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="J162" t="inlineStr">
         <is>
@@ -16832,13 +16832,13 @@
         <v>45091</v>
       </c>
       <c r="G163">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="H163" s="2">
         <v>45274</v>
       </c>
       <c r="I163">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="J163" t="inlineStr">
         <is>
@@ -16930,13 +16930,13 @@
         <v>45138</v>
       </c>
       <c r="G164">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="H164" s="2">
         <v>45322</v>
       </c>
       <c r="I164">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="J164" t="inlineStr">
         <is>
@@ -17033,13 +17033,13 @@
         <v>45138</v>
       </c>
       <c r="G165">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="H165" s="2">
         <v>45322</v>
       </c>
       <c r="I165">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="J165" t="inlineStr">
         <is>
@@ -17136,13 +17136,13 @@
         <v>45085</v>
       </c>
       <c r="G166">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="H166" s="2">
         <v>45268</v>
       </c>
       <c r="I166">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="J166" t="inlineStr">
         <is>
@@ -17239,13 +17239,13 @@
         <v>45085</v>
       </c>
       <c r="G167">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="H167" s="2">
         <v>45268</v>
       </c>
       <c r="I167">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="J167" t="inlineStr">
         <is>
@@ -17342,7 +17342,7 @@
         <v>45326</v>
       </c>
       <c r="I168">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="J168" t="inlineStr">
         <is>
@@ -17439,13 +17439,13 @@
         <v>45173</v>
       </c>
       <c r="G169">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="H169" s="2">
         <v>45355</v>
       </c>
       <c r="I169">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="J169" t="inlineStr">
         <is>
@@ -17542,13 +17542,13 @@
         <v>45056</v>
       </c>
       <c r="G170">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="H170" s="2">
         <v>45240</v>
       </c>
       <c r="I170">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="J170" t="inlineStr">
         <is>
@@ -17645,7 +17645,7 @@
         <v>45238</v>
       </c>
       <c r="I171">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="J171" t="inlineStr">
         <is>
@@ -17742,13 +17742,13 @@
         <v>45141</v>
       </c>
       <c r="G172">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="H172" s="2">
         <v>45325</v>
       </c>
       <c r="I172">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="J172" t="inlineStr">
         <is>
@@ -17845,13 +17845,13 @@
         <v>45037</v>
       </c>
       <c r="G173">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="H173" s="2">
         <v>45220</v>
       </c>
       <c r="I173">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="J173" t="inlineStr">
         <is>
@@ -17948,13 +17948,13 @@
         <v>45171</v>
       </c>
       <c r="G174">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="H174" s="2">
         <v>45262</v>
       </c>
       <c r="I174">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="J174" t="inlineStr">
         <is>
@@ -18051,13 +18051,13 @@
         <v>45105</v>
       </c>
       <c r="G175">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="H175" s="2">
         <v>45197</v>
       </c>
       <c r="I175">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="J175" t="inlineStr">
         <is>
@@ -18154,13 +18154,13 @@
         <v>45162</v>
       </c>
       <c r="G176">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="H176" s="2">
         <v>45254</v>
       </c>
       <c r="I176">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="J176" t="inlineStr">
         <is>
@@ -18257,13 +18257,13 @@
         <v>45061</v>
       </c>
       <c r="G177">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="H177" s="2">
         <v>45245</v>
       </c>
       <c r="I177">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="J177" t="inlineStr">
         <is>
@@ -18360,13 +18360,13 @@
         <v>45120</v>
       </c>
       <c r="G178">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="H178" s="2">
         <v>45212</v>
       </c>
       <c r="I178">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="J178" t="inlineStr">
         <is>
@@ -18463,7 +18463,7 @@
         <v>45191</v>
       </c>
       <c r="I179">
-        <v>-3</v>
+        <v>-4</v>
       </c>
       <c r="J179" t="inlineStr">
         <is>
@@ -18560,13 +18560,13 @@
         <v>45088</v>
       </c>
       <c r="G180">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="H180" s="2">
         <v>45271</v>
       </c>
       <c r="I180">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="J180" t="inlineStr">
         <is>
@@ -18663,13 +18663,13 @@
         <v>45100</v>
       </c>
       <c r="G181">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="H181" s="2">
         <v>45192</v>
       </c>
       <c r="I181">
-        <v>-2</v>
+        <v>-3</v>
       </c>
       <c r="J181" t="inlineStr">
         <is>
@@ -18756,13 +18756,13 @@
         <v>45131</v>
       </c>
       <c r="G182">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="H182" s="2">
         <v>45223</v>
       </c>
       <c r="I182">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="J182" t="inlineStr">
         <is>
@@ -18854,13 +18854,13 @@
         <v>45136</v>
       </c>
       <c r="G183">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="H183" s="2">
         <v>45228</v>
       </c>
       <c r="I183">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="J183" t="inlineStr">
         <is>
@@ -18952,13 +18952,13 @@
         <v>45150</v>
       </c>
       <c r="G184">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="H184" s="2">
         <v>45242</v>
       </c>
       <c r="I184">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="J184" t="inlineStr">
         <is>
@@ -19050,13 +19050,13 @@
         <v>45118</v>
       </c>
       <c r="G185">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="H185" s="2">
         <v>45210</v>
       </c>
       <c r="I185">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="J185" t="inlineStr">
         <is>
@@ -19148,13 +19148,13 @@
         <v>45129</v>
       </c>
       <c r="G186">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="H186" s="2">
         <v>45221</v>
       </c>
       <c r="I186">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="J186" t="inlineStr">
         <is>
@@ -19246,13 +19246,13 @@
         <v>45097</v>
       </c>
       <c r="G187">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="H187" s="2">
         <v>45189</v>
       </c>
       <c r="I187">
-        <v>-5</v>
+        <v>-6</v>
       </c>
       <c r="J187" t="inlineStr">
         <is>
@@ -19339,13 +19339,13 @@
         <v>45101</v>
       </c>
       <c r="G188">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="H188" s="2">
         <v>45193</v>
       </c>
       <c r="I188">
-        <v>-1</v>
+        <v>-2</v>
       </c>
       <c r="J188" t="inlineStr">
         <is>
@@ -19432,13 +19432,13 @@
         <v>45165</v>
       </c>
       <c r="G189">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="H189" s="2">
         <v>45257</v>
       </c>
       <c r="I189">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="J189" t="inlineStr">
         <is>
@@ -19530,7 +19530,7 @@
         <v>45202</v>
       </c>
       <c r="I190">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="J190" t="inlineStr">
         <is>
@@ -19627,13 +19627,13 @@
         <v>45081</v>
       </c>
       <c r="G191">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="H191" s="2">
         <v>45264</v>
       </c>
       <c r="I191">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="J191" t="inlineStr">
         <is>
@@ -19730,13 +19730,13 @@
         <v>45081</v>
       </c>
       <c r="G192">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="H192" s="2">
         <v>45264</v>
       </c>
       <c r="I192">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="J192" t="inlineStr">
         <is>
@@ -19833,7 +19833,7 @@
         <v>45319</v>
       </c>
       <c r="I193">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="J193" t="inlineStr">
         <is>
@@ -19930,7 +19930,7 @@
         <v>45319</v>
       </c>
       <c r="I194">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="J194" t="inlineStr">
         <is>
@@ -20022,13 +20022,13 @@
         <v>45046</v>
       </c>
       <c r="G195">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="H195" s="2">
         <v>45230</v>
       </c>
       <c r="I195">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="J195" t="inlineStr">
         <is>
@@ -20125,13 +20125,13 @@
         <v>45046</v>
       </c>
       <c r="G196">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="H196" s="2">
         <v>45230</v>
       </c>
       <c r="I196">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="J196" t="inlineStr">
         <is>
@@ -20228,13 +20228,13 @@
         <v>45031</v>
       </c>
       <c r="G197">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="H197" s="2">
         <v>45214</v>
       </c>
       <c r="I197">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="J197" t="inlineStr">
         <is>
@@ -20331,13 +20331,13 @@
         <v>45031</v>
       </c>
       <c r="G198">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="H198" s="2">
         <v>45214</v>
       </c>
       <c r="I198">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="J198" t="inlineStr">
         <is>
@@ -20434,13 +20434,13 @@
         <v>45031</v>
       </c>
       <c r="G199">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="H199" s="2">
         <v>45214</v>
       </c>
       <c r="I199">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="J199" t="inlineStr">
         <is>
@@ -20537,13 +20537,13 @@
         <v>45031</v>
       </c>
       <c r="G200">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="H200" s="2">
         <v>45214</v>
       </c>
       <c r="I200">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="J200" t="inlineStr">
         <is>
@@ -20640,13 +20640,13 @@
         <v>45067</v>
       </c>
       <c r="G201">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="H201" s="2">
         <v>45251</v>
       </c>
       <c r="I201">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="J201" t="inlineStr">
         <is>
@@ -20743,13 +20743,13 @@
         <v>45067</v>
       </c>
       <c r="G202">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="H202" s="2">
         <v>45251</v>
       </c>
       <c r="I202">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="J202" t="inlineStr">
         <is>
@@ -20846,13 +20846,13 @@
         <v>45067</v>
       </c>
       <c r="G203">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="H203" s="2">
         <v>45251</v>
       </c>
       <c r="I203">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="J203" t="inlineStr">
         <is>
@@ -20949,13 +20949,13 @@
         <v>45067</v>
       </c>
       <c r="G204">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="H204" s="2">
         <v>45251</v>
       </c>
       <c r="I204">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="J204" t="inlineStr">
         <is>
@@ -21052,13 +21052,13 @@
         <v>45178</v>
       </c>
       <c r="G205">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="H205" s="2">
         <v>45269</v>
       </c>
       <c r="I205">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="J205" t="inlineStr">
         <is>
@@ -21155,7 +21155,7 @@
         <v>45252</v>
       </c>
       <c r="I206">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="J206" t="inlineStr">
         <is>
@@ -21252,13 +21252,13 @@
         <v>45087</v>
       </c>
       <c r="G207">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="H207" s="2">
         <v>45270</v>
       </c>
       <c r="I207">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="J207" t="inlineStr">
         <is>
@@ -21355,13 +21355,13 @@
         <v>45099</v>
       </c>
       <c r="G208">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="H208" s="2">
         <v>45282</v>
       </c>
       <c r="I208">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="J208" t="inlineStr">
         <is>
@@ -21458,13 +21458,13 @@
         <v>45175</v>
       </c>
       <c r="G209">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="H209" s="2">
         <v>45356</v>
       </c>
       <c r="I209">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="J209" t="inlineStr">
         <is>
@@ -21561,13 +21561,13 @@
         <v>45175</v>
       </c>
       <c r="G210">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="H210" s="2">
         <v>45356</v>
       </c>
       <c r="I210">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="J210" t="inlineStr">
         <is>
@@ -21664,13 +21664,13 @@
         <v>45166</v>
       </c>
       <c r="G211">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="H211" s="2">
         <v>45350</v>
       </c>
       <c r="I211">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="J211" t="inlineStr">
         <is>
@@ -21767,13 +21767,13 @@
         <v>45166</v>
       </c>
       <c r="G212">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="H212" s="2">
         <v>45350</v>
       </c>
       <c r="I212">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="J212" t="inlineStr">
         <is>
@@ -21870,13 +21870,13 @@
         <v>45090</v>
       </c>
       <c r="G213">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="H213" s="2">
         <v>45273</v>
       </c>
       <c r="I213">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="J213" t="inlineStr">
         <is>
@@ -21973,13 +21973,13 @@
         <v>45106</v>
       </c>
       <c r="G214">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="H214" s="2">
         <v>45289</v>
       </c>
       <c r="I214">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="J214" t="inlineStr">
         <is>
@@ -22076,13 +22076,13 @@
         <v>45134</v>
       </c>
       <c r="G215">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="H215" s="2">
         <v>45226</v>
       </c>
       <c r="I215">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="J215" t="inlineStr">
         <is>
@@ -22179,13 +22179,13 @@
         <v>45132</v>
       </c>
       <c r="G216">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="H216" s="2">
         <v>45224</v>
       </c>
       <c r="I216">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="J216" t="inlineStr">
         <is>
@@ -22282,13 +22282,13 @@
         <v>45150</v>
       </c>
       <c r="G217">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="H217" s="2">
         <v>45242</v>
       </c>
       <c r="I217">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="J217" t="inlineStr">
         <is>
@@ -22385,13 +22385,13 @@
         <v>45095</v>
       </c>
       <c r="G218">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="H218" s="2">
         <v>45187</v>
       </c>
       <c r="I218">
-        <v>-7</v>
+        <v>-8</v>
       </c>
       <c r="J218" t="inlineStr">
         <is>
@@ -22483,13 +22483,13 @@
         <v>45182</v>
       </c>
       <c r="G219">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="H219" s="2">
         <v>45273</v>
       </c>
       <c r="I219">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="J219" t="inlineStr">
         <is>
@@ -22586,7 +22586,7 @@
         <v>45196</v>
       </c>
       <c r="I220">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J220" t="inlineStr">
         <is>
@@ -22683,13 +22683,13 @@
         <v>45108</v>
       </c>
       <c r="G221">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="H221" s="2">
         <v>45200</v>
       </c>
       <c r="I221">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="J221" t="inlineStr">
         <is>
@@ -22786,13 +22786,13 @@
         <v>45135</v>
       </c>
       <c r="G222">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="H222" s="2">
         <v>45227</v>
       </c>
       <c r="I222">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="J222" t="inlineStr">
         <is>
@@ -22889,13 +22889,13 @@
         <v>45148</v>
       </c>
       <c r="G223">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="H223" s="2">
         <v>45240</v>
       </c>
       <c r="I223">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="J223" t="inlineStr">
         <is>
@@ -22987,13 +22987,13 @@
         <v>45100</v>
       </c>
       <c r="G224">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="H224" s="2">
         <v>45192</v>
       </c>
       <c r="I224">
-        <v>-2</v>
+        <v>-3</v>
       </c>
       <c r="J224" t="inlineStr">
         <is>
@@ -23085,13 +23085,13 @@
         <v>45136</v>
       </c>
       <c r="G225">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="H225" s="2">
         <v>45320</v>
       </c>
       <c r="I225">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="J225" t="inlineStr">
         <is>
@@ -23188,13 +23188,13 @@
         <v>45136</v>
       </c>
       <c r="G226">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="H226" s="2">
         <v>45320</v>
       </c>
       <c r="I226">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="J226" t="inlineStr">
         <is>
@@ -23291,13 +23291,13 @@
         <v>45094</v>
       </c>
       <c r="G227">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="H227" s="2">
         <v>45277</v>
       </c>
       <c r="I227">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="J227" t="inlineStr">
         <is>
@@ -23394,13 +23394,13 @@
         <v>45081</v>
       </c>
       <c r="G228">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="H228" s="2">
         <v>45264</v>
       </c>
       <c r="I228">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="J228" t="inlineStr">
         <is>
@@ -23497,13 +23497,13 @@
         <v>45099</v>
       </c>
       <c r="G229">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="H229" s="2">
         <v>45282</v>
       </c>
       <c r="I229">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="J229" t="inlineStr">
         <is>
@@ -23600,13 +23600,13 @@
         <v>45018</v>
       </c>
       <c r="G230">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="H230" s="2">
         <v>45201</v>
       </c>
       <c r="I230">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="J230" t="inlineStr">
         <is>
@@ -23703,13 +23703,13 @@
         <v>45031</v>
       </c>
       <c r="G231">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="H231" s="2">
         <v>45214</v>
       </c>
       <c r="I231">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="J231" t="inlineStr">
         <is>
@@ -23806,7 +23806,7 @@
         <v>45294</v>
       </c>
       <c r="I232">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="J232" t="inlineStr">
         <is>
@@ -23903,13 +23903,13 @@
         <v>45079</v>
       </c>
       <c r="G233">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="H233" s="2">
         <v>45262</v>
       </c>
       <c r="I233">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="J233" t="inlineStr">
         <is>
@@ -24006,7 +24006,7 @@
         <v>45199</v>
       </c>
       <c r="I234">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="J234" t="inlineStr">
         <is>
@@ -24103,13 +24103,13 @@
         <v>45021</v>
       </c>
       <c r="G235">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="H235" s="2">
         <v>45204</v>
       </c>
       <c r="I235">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="J235" t="inlineStr">
         <is>
@@ -24206,13 +24206,13 @@
         <v>45021</v>
       </c>
       <c r="G236">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="H236" s="2">
         <v>45204</v>
       </c>
       <c r="I236">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="J236" t="inlineStr">
         <is>
@@ -24309,13 +24309,13 @@
         <v>45080</v>
       </c>
       <c r="G237">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="H237" s="2">
         <v>45263</v>
       </c>
       <c r="I237">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="J237" t="inlineStr">
         <is>
@@ -24412,13 +24412,13 @@
         <v>45046</v>
       </c>
       <c r="G238">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="H238" s="2">
         <v>45229</v>
       </c>
       <c r="I238">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="J238" t="inlineStr">
         <is>
@@ -24515,13 +24515,13 @@
         <v>45112</v>
       </c>
       <c r="G239">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="H239" s="2">
         <v>45204</v>
       </c>
       <c r="I239">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="J239" t="inlineStr">
         <is>
@@ -24609,13 +24609,13 @@
         <v>45112</v>
       </c>
       <c r="G240">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="H240" s="2">
         <v>45204</v>
       </c>
       <c r="I240">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="J240" t="inlineStr">
         <is>
@@ -24703,13 +24703,13 @@
         <v>45016</v>
       </c>
       <c r="G241">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="H241" s="2">
         <v>45199</v>
       </c>
       <c r="I241">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="J241" t="inlineStr">
         <is>
@@ -24806,13 +24806,13 @@
         <v>45070</v>
       </c>
       <c r="G242">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="H242" s="2">
         <v>45254</v>
       </c>
       <c r="I242">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="J242" t="inlineStr">
         <is>
@@ -24909,13 +24909,13 @@
         <v>45168</v>
       </c>
       <c r="G243">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="H243" s="2">
         <v>45260</v>
       </c>
       <c r="I243">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="J243" t="inlineStr">
         <is>
@@ -25012,13 +25012,13 @@
         <v>45027</v>
       </c>
       <c r="G244">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="H244" s="2">
         <v>45210</v>
       </c>
       <c r="I244">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="J244" t="inlineStr">
         <is>
@@ -25115,13 +25115,13 @@
         <v>45077</v>
       </c>
       <c r="G245">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="H245" s="2">
         <v>45260</v>
       </c>
       <c r="I245">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="J245" t="inlineStr">
         <is>
@@ -25218,13 +25218,13 @@
         <v>45100</v>
       </c>
       <c r="G246">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="H246" s="2">
         <v>45283</v>
       </c>
       <c r="I246">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="J246" t="inlineStr">
         <is>
@@ -25321,7 +25321,7 @@
         <v>45281</v>
       </c>
       <c r="I247">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="J247" t="inlineStr">
         <is>
@@ -25418,13 +25418,13 @@
         <v>45044</v>
       </c>
       <c r="G248">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="H248" s="2">
         <v>45227</v>
       </c>
       <c r="I248">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="J248" t="inlineStr">
         <is>
@@ -25521,13 +25521,13 @@
         <v>45101</v>
       </c>
       <c r="G249">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="H249" s="2">
         <v>45283</v>
       </c>
       <c r="I249">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="J249" t="inlineStr">
         <is>
@@ -25624,13 +25624,13 @@
         <v>45134</v>
       </c>
       <c r="G250">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="H250" s="2">
         <v>45226</v>
       </c>
       <c r="I250">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="J250" t="inlineStr">
         <is>
@@ -25727,13 +25727,13 @@
         <v>45158</v>
       </c>
       <c r="G251">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="H251" s="2">
         <v>45250</v>
       </c>
       <c r="I251">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="J251" t="inlineStr">
         <is>
@@ -25830,13 +25830,13 @@
         <v>45108</v>
       </c>
       <c r="G252">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="H252" s="2">
         <v>45200</v>
       </c>
       <c r="I252">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="J252" t="inlineStr">
         <is>
@@ -25933,7 +25933,7 @@
         <v>45317</v>
       </c>
       <c r="I253">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="J253" t="inlineStr">
         <is>
@@ -26030,13 +26030,13 @@
         <v>45039</v>
       </c>
       <c r="G254">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="H254" s="2">
         <v>45222</v>
       </c>
       <c r="I254">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="J254" t="inlineStr">
         <is>
@@ -26128,13 +26128,13 @@
         <v>45129</v>
       </c>
       <c r="G255">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="H255" s="2">
         <v>45221</v>
       </c>
       <c r="I255">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="J255" t="inlineStr">
         <is>
@@ -26231,13 +26231,13 @@
         <v>45157</v>
       </c>
       <c r="G256">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="H256" s="2">
         <v>45341</v>
       </c>
       <c r="I256">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="J256" t="inlineStr">
         <is>
@@ -26334,13 +26334,13 @@
         <v>45063</v>
       </c>
       <c r="G257">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="H257" s="2">
         <v>45247</v>
       </c>
       <c r="I257">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="J257" t="inlineStr">
         <is>
@@ -26437,7 +26437,7 @@
         <v>45254</v>
       </c>
       <c r="I258">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="J258" t="inlineStr">
         <is>
@@ -26534,7 +26534,7 @@
         <v>45486</v>
       </c>
       <c r="I259">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="J259" t="inlineStr">
         <is>
@@ -26626,13 +26626,13 @@
         <v>45073</v>
       </c>
       <c r="G260">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="H260" s="2">
         <v>45439</v>
       </c>
       <c r="I260">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="J260" t="inlineStr">
         <is>
@@ -26724,7 +26724,7 @@
         <v>45323</v>
       </c>
       <c r="I261">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="J261" t="inlineStr">
         <is>
@@ -26816,7 +26816,7 @@
         <v>45303</v>
       </c>
       <c r="I262">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="J262" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
Bond dates update Wed Sep 27 23:09:16 UTC 2023
</commit_message>
<xml_diff>
--- a/Data/obligacje_screener.xlsx
+++ b/Data/obligacje_screener.xlsx
@@ -512,7 +512,7 @@
         <v>45340</v>
       </c>
       <c r="I2">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="J2" t="inlineStr">
         <is>
@@ -600,13 +600,13 @@
         <v>45121</v>
       </c>
       <c r="G3">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="H3" s="2">
         <v>45305</v>
       </c>
       <c r="I3">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="J3" t="inlineStr">
         <is>
@@ -703,13 +703,13 @@
         <v>45039</v>
       </c>
       <c r="G4">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="H4" s="2">
         <v>45222</v>
       </c>
       <c r="I4">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="J4" t="inlineStr">
         <is>
@@ -806,13 +806,13 @@
         <v>45039</v>
       </c>
       <c r="G5">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="H5" s="2">
         <v>45222</v>
       </c>
       <c r="I5">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="J5" t="inlineStr">
         <is>
@@ -909,13 +909,13 @@
         <v>45129</v>
       </c>
       <c r="G6">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="H6" s="2">
         <v>45221</v>
       </c>
       <c r="I6">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="J6" t="inlineStr">
         <is>
@@ -1012,13 +1012,13 @@
         <v>45162</v>
       </c>
       <c r="G7">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="H7" s="2">
         <v>45254</v>
       </c>
       <c r="I7">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="J7" t="inlineStr">
         <is>
@@ -1110,13 +1110,13 @@
         <v>45156</v>
       </c>
       <c r="G8">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="H8" s="2">
         <v>45248</v>
       </c>
       <c r="I8">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="J8" t="inlineStr">
         <is>
@@ -1213,13 +1213,13 @@
         <v>45141</v>
       </c>
       <c r="G9">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="H9" s="2">
         <v>45233</v>
       </c>
       <c r="I9">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="J9" t="inlineStr">
         <is>
@@ -1316,13 +1316,13 @@
         <v>45062</v>
       </c>
       <c r="G10">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="H10" s="2">
         <v>45246</v>
       </c>
       <c r="I10">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="J10" t="inlineStr">
         <is>
@@ -1419,7 +1419,7 @@
         <v>45286</v>
       </c>
       <c r="I11">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="J11" t="inlineStr">
         <is>
@@ -1516,13 +1516,13 @@
         <v>45011</v>
       </c>
       <c r="G12">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="H12" s="2">
         <v>45195</v>
       </c>
       <c r="I12">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="J12" t="inlineStr">
         <is>
@@ -1614,13 +1614,13 @@
         <v>45036</v>
       </c>
       <c r="G13">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="H13" s="2">
         <v>45219</v>
       </c>
       <c r="I13">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="J13" t="inlineStr">
         <is>
@@ -1717,13 +1717,13 @@
         <v>45036</v>
       </c>
       <c r="G14">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="H14" s="2">
         <v>45219</v>
       </c>
       <c r="I14">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="J14" t="inlineStr">
         <is>
@@ -1820,13 +1820,13 @@
         <v>45106</v>
       </c>
       <c r="G15">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="H15" s="2">
         <v>45289</v>
       </c>
       <c r="I15">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="J15" t="inlineStr">
         <is>
@@ -1923,13 +1923,13 @@
         <v>45094</v>
       </c>
       <c r="G16">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="H16" s="2">
         <v>45186</v>
       </c>
       <c r="I16">
-        <v>-9</v>
+        <v>-10</v>
       </c>
       <c r="J16" t="inlineStr">
         <is>
@@ -2026,13 +2026,13 @@
         <v>45094</v>
       </c>
       <c r="G17">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="H17" s="2">
         <v>45186</v>
       </c>
       <c r="I17">
-        <v>-9</v>
+        <v>-10</v>
       </c>
       <c r="J17" t="inlineStr">
         <is>
@@ -2129,13 +2129,13 @@
         <v>45132</v>
       </c>
       <c r="G18">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="H18" s="2">
         <v>45224</v>
       </c>
       <c r="I18">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="J18" t="inlineStr">
         <is>
@@ -2232,13 +2232,13 @@
         <v>45137</v>
       </c>
       <c r="G19">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="H19" s="2">
         <v>45229</v>
       </c>
       <c r="I19">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="J19" t="inlineStr">
         <is>
@@ -2330,13 +2330,13 @@
         <v>45183</v>
       </c>
       <c r="G20">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="H20" s="2">
         <v>45274</v>
       </c>
       <c r="I20">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="J20" t="inlineStr">
         <is>
@@ -2433,13 +2433,13 @@
         <v>45093</v>
       </c>
       <c r="G21">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="H21" s="2">
         <v>45187</v>
       </c>
       <c r="I21">
-        <v>-8</v>
+        <v>-9</v>
       </c>
       <c r="J21" t="inlineStr">
         <is>
@@ -2536,13 +2536,13 @@
         <v>45096</v>
       </c>
       <c r="G22">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="H22" s="2">
         <v>45187</v>
       </c>
       <c r="I22">
-        <v>-8</v>
+        <v>-9</v>
       </c>
       <c r="J22" t="inlineStr">
         <is>
@@ -2639,7 +2639,7 @@
         <v>45245</v>
       </c>
       <c r="I23">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="J23" t="inlineStr">
         <is>
@@ -2736,7 +2736,7 @@
         <v>45245</v>
       </c>
       <c r="I24">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="J24" t="inlineStr">
         <is>
@@ -2833,13 +2833,13 @@
         <v>45021</v>
       </c>
       <c r="G25">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="H25" s="2">
         <v>45204</v>
       </c>
       <c r="I25">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="J25" t="inlineStr">
         <is>
@@ -2936,13 +2936,13 @@
         <v>45160</v>
       </c>
       <c r="G26">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="H26" s="2">
         <v>45344</v>
       </c>
       <c r="I26">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="J26" t="inlineStr">
         <is>
@@ -3039,13 +3039,13 @@
         <v>45118</v>
       </c>
       <c r="G27">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="H27" s="2">
         <v>45302</v>
       </c>
       <c r="I27">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="J27" t="inlineStr">
         <is>
@@ -3142,13 +3142,13 @@
         <v>45085</v>
       </c>
       <c r="G28">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="H28" s="2">
         <v>45268</v>
       </c>
       <c r="I28">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="J28" t="inlineStr">
         <is>
@@ -3245,13 +3245,13 @@
         <v>45183</v>
       </c>
       <c r="G29">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="H29" s="2">
         <v>45274</v>
       </c>
       <c r="I29">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="J29" t="inlineStr">
         <is>
@@ -3348,7 +3348,7 @@
         <v>45224</v>
       </c>
       <c r="I30">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="J30" t="inlineStr">
         <is>
@@ -3445,13 +3445,13 @@
         <v>45153</v>
       </c>
       <c r="G31">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="H31" s="2">
         <v>45245</v>
       </c>
       <c r="I31">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="J31" t="inlineStr">
         <is>
@@ -3548,13 +3548,13 @@
         <v>45155</v>
       </c>
       <c r="G32">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="H32" s="2">
         <v>45247</v>
       </c>
       <c r="I32">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="J32" t="inlineStr">
         <is>
@@ -3651,7 +3651,7 @@
         <v>45255</v>
       </c>
       <c r="I33">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="J33" t="inlineStr">
         <is>
@@ -3739,13 +3739,13 @@
         <v>45176</v>
       </c>
       <c r="G34">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="H34" s="2">
         <v>45267</v>
       </c>
       <c r="I34">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="J34" t="inlineStr">
         <is>
@@ -3842,13 +3842,13 @@
         <v>45130</v>
       </c>
       <c r="G35">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="H35" s="2">
         <v>45222</v>
       </c>
       <c r="I35">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="J35" t="inlineStr">
         <is>
@@ -3940,13 +3940,13 @@
         <v>45115</v>
       </c>
       <c r="G36">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="H36" s="2">
         <v>45207</v>
       </c>
       <c r="I36">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="J36" t="inlineStr">
         <is>
@@ -4043,13 +4043,13 @@
         <v>45097</v>
       </c>
       <c r="G37">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="H37" s="2">
         <v>45189</v>
       </c>
       <c r="I37">
-        <v>-6</v>
+        <v>-7</v>
       </c>
       <c r="J37" t="inlineStr">
         <is>
@@ -4141,13 +4141,13 @@
         <v>45107</v>
       </c>
       <c r="G38">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="H38" s="2">
         <v>45290</v>
       </c>
       <c r="I38">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="J38" t="inlineStr">
         <is>
@@ -4244,13 +4244,13 @@
         <v>45063</v>
       </c>
       <c r="G39">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="H39" s="2">
         <v>45247</v>
       </c>
       <c r="I39">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="J39" t="inlineStr">
         <is>
@@ -4347,13 +4347,13 @@
         <v>45177</v>
       </c>
       <c r="G40">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="H40" s="2">
         <v>45359</v>
       </c>
       <c r="I40">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="J40" t="inlineStr">
         <is>
@@ -4450,13 +4450,13 @@
         <v>45107</v>
       </c>
       <c r="G41">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="H41" s="2">
         <v>45290</v>
       </c>
       <c r="I41">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="J41" t="inlineStr">
         <is>
@@ -4553,7 +4553,7 @@
         <v>45265</v>
       </c>
       <c r="I42">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="J42" t="inlineStr">
         <is>
@@ -4650,13 +4650,13 @@
         <v>45098</v>
       </c>
       <c r="G43">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="H43" s="2">
         <v>45281</v>
       </c>
       <c r="I43">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="J43" t="inlineStr">
         <is>
@@ -4753,13 +4753,13 @@
         <v>45099</v>
       </c>
       <c r="G44">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="H44" s="2">
         <v>45282</v>
       </c>
       <c r="I44">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="J44" t="inlineStr">
         <is>
@@ -4856,13 +4856,13 @@
         <v>45106</v>
       </c>
       <c r="G45">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="H45" s="2">
         <v>45289</v>
       </c>
       <c r="I45">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="J45" t="inlineStr">
         <is>
@@ -4959,13 +4959,13 @@
         <v>45106</v>
       </c>
       <c r="G46">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="H46" s="2">
         <v>45289</v>
       </c>
       <c r="I46">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="J46" t="inlineStr">
         <is>
@@ -5062,13 +5062,13 @@
         <v>45120</v>
       </c>
       <c r="G47">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="H47" s="2">
         <v>45304</v>
       </c>
       <c r="I47">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="J47" t="inlineStr">
         <is>
@@ -5165,13 +5165,13 @@
         <v>45118</v>
       </c>
       <c r="G48">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="H48" s="2">
         <v>45302</v>
       </c>
       <c r="I48">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="J48" t="inlineStr">
         <is>
@@ -5268,13 +5268,13 @@
         <v>45152</v>
       </c>
       <c r="G49">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="H49" s="2">
         <v>45336</v>
       </c>
       <c r="I49">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="J49" t="inlineStr">
         <is>
@@ -5371,13 +5371,13 @@
         <v>45042</v>
       </c>
       <c r="G50">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="H50" s="2">
         <v>45225</v>
       </c>
       <c r="I50">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="J50" t="inlineStr">
         <is>
@@ -5474,13 +5474,13 @@
         <v>45122</v>
       </c>
       <c r="G51">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="H51" s="2">
         <v>45306</v>
       </c>
       <c r="I51">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="J51" t="inlineStr">
         <is>
@@ -5577,13 +5577,13 @@
         <v>45139</v>
       </c>
       <c r="G52">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="H52" s="2">
         <v>45323</v>
       </c>
       <c r="I52">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="J52" t="inlineStr">
         <is>
@@ -5671,13 +5671,13 @@
         <v>45099</v>
       </c>
       <c r="G53">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="H53" s="2">
         <v>45282</v>
       </c>
       <c r="I53">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="J53" t="inlineStr">
         <is>
@@ -5774,7 +5774,7 @@
         <v>45196</v>
       </c>
       <c r="I54">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J54" t="inlineStr">
         <is>
@@ -5871,13 +5871,13 @@
         <v>45044</v>
       </c>
       <c r="G55">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="H55" s="2">
         <v>45227</v>
       </c>
       <c r="I55">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="J55" t="inlineStr">
         <is>
@@ -5974,13 +5974,13 @@
         <v>45151</v>
       </c>
       <c r="G56">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="H56" s="2">
         <v>45243</v>
       </c>
       <c r="I56">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="J56" t="inlineStr">
         <is>
@@ -6072,7 +6072,7 @@
         <v>45196</v>
       </c>
       <c r="I57">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J57" t="inlineStr">
         <is>
@@ -6169,13 +6169,13 @@
         <v>45069</v>
       </c>
       <c r="G58">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="H58" s="2">
         <v>45253</v>
       </c>
       <c r="I58">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="J58" t="inlineStr">
         <is>
@@ -6272,13 +6272,13 @@
         <v>45099</v>
       </c>
       <c r="G59">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="H59" s="2">
         <v>45191</v>
       </c>
       <c r="I59">
-        <v>-4</v>
+        <v>-5</v>
       </c>
       <c r="J59" t="inlineStr">
         <is>
@@ -6370,13 +6370,13 @@
         <v>45113</v>
       </c>
       <c r="G60">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="H60" s="2">
         <v>45205</v>
       </c>
       <c r="I60">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="J60" t="inlineStr">
         <is>
@@ -6473,13 +6473,13 @@
         <v>45127</v>
       </c>
       <c r="G61">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="H61" s="2">
         <v>45219</v>
       </c>
       <c r="I61">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="J61" t="inlineStr">
         <is>
@@ -6576,13 +6576,13 @@
         <v>45058</v>
       </c>
       <c r="G62">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="H62" s="2">
         <v>45242</v>
       </c>
       <c r="I62">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="J62" t="inlineStr">
         <is>
@@ -6679,13 +6679,13 @@
         <v>45010</v>
       </c>
       <c r="G63">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="H63" s="2">
         <v>45194</v>
       </c>
       <c r="I63">
-        <v>-1</v>
+        <v>-2</v>
       </c>
       <c r="J63" t="inlineStr">
         <is>
@@ -6777,13 +6777,13 @@
         <v>45025</v>
       </c>
       <c r="G64">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="H64" s="2">
         <v>45208</v>
       </c>
       <c r="I64">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="J64" t="inlineStr">
         <is>
@@ -6880,13 +6880,13 @@
         <v>45025</v>
       </c>
       <c r="G65">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="H65" s="2">
         <v>45208</v>
       </c>
       <c r="I65">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="J65" t="inlineStr">
         <is>
@@ -6983,13 +6983,13 @@
         <v>45089</v>
       </c>
       <c r="G66">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="H66" s="2">
         <v>45272</v>
       </c>
       <c r="I66">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="J66" t="inlineStr">
         <is>
@@ -7086,13 +7086,13 @@
         <v>45178</v>
       </c>
       <c r="G67">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="H67" s="2">
         <v>45269</v>
       </c>
       <c r="I67">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="J67" t="inlineStr">
         <is>
@@ -7184,13 +7184,13 @@
         <v>45104</v>
       </c>
       <c r="G68">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="H68" s="2">
         <v>45196</v>
       </c>
       <c r="I68">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J68" t="inlineStr">
         <is>
@@ -7287,13 +7287,13 @@
         <v>45149</v>
       </c>
       <c r="G69">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="H69" s="2">
         <v>45241</v>
       </c>
       <c r="I69">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="J69" t="inlineStr">
         <is>
@@ -7390,7 +7390,7 @@
         <v>45205</v>
       </c>
       <c r="I70">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="J70" t="inlineStr">
         <is>
@@ -7487,13 +7487,13 @@
         <v>45114</v>
       </c>
       <c r="G71">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="H71" s="2">
         <v>45205</v>
       </c>
       <c r="I71">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="J71" t="inlineStr">
         <is>
@@ -7590,13 +7590,13 @@
         <v>45115</v>
       </c>
       <c r="G72">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="H72" s="2">
         <v>45207</v>
       </c>
       <c r="I72">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="J72" t="inlineStr">
         <is>
@@ -7693,13 +7693,13 @@
         <v>45097</v>
       </c>
       <c r="G73">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="H73" s="2">
         <v>45189</v>
       </c>
       <c r="I73">
-        <v>-6</v>
+        <v>-7</v>
       </c>
       <c r="J73" t="inlineStr">
         <is>
@@ -7791,13 +7791,13 @@
         <v>45038</v>
       </c>
       <c r="G74">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="H74" s="2">
         <v>45221</v>
       </c>
       <c r="I74">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="J74" t="inlineStr">
         <is>
@@ -7889,13 +7889,13 @@
         <v>45117</v>
       </c>
       <c r="G75">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="H75" s="2">
         <v>45301</v>
       </c>
       <c r="I75">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="J75" t="inlineStr">
         <is>
@@ -7992,13 +7992,13 @@
         <v>45160</v>
       </c>
       <c r="G76">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="H76" s="2">
         <v>45344</v>
       </c>
       <c r="I76">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="J76" t="inlineStr">
         <is>
@@ -8095,13 +8095,13 @@
         <v>45002</v>
       </c>
       <c r="G77">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="H77" s="2">
         <v>45186</v>
       </c>
       <c r="I77">
-        <v>-9</v>
+        <v>-10</v>
       </c>
       <c r="J77" t="inlineStr">
         <is>
@@ -8198,13 +8198,13 @@
         <v>45043</v>
       </c>
       <c r="G78">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="H78" s="2">
         <v>45226</v>
       </c>
       <c r="I78">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="J78" t="inlineStr">
         <is>
@@ -8301,13 +8301,13 @@
         <v>45079</v>
       </c>
       <c r="G79">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="H79" s="2">
         <v>45262</v>
       </c>
       <c r="I79">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="J79" t="inlineStr">
         <is>
@@ -8404,7 +8404,7 @@
         <v>45254</v>
       </c>
       <c r="I80">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="J80" t="inlineStr">
         <is>
@@ -8501,13 +8501,13 @@
         <v>45104</v>
       </c>
       <c r="G81">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="H81" s="2">
         <v>45287</v>
       </c>
       <c r="I81">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="J81" t="inlineStr">
         <is>
@@ -8604,7 +8604,7 @@
         <v>45288</v>
       </c>
       <c r="I82">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="J82" t="inlineStr">
         <is>
@@ -8696,13 +8696,13 @@
         <v>45175</v>
       </c>
       <c r="G83">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="H83" s="2">
         <v>45357</v>
       </c>
       <c r="I83">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="J83" t="inlineStr">
         <is>
@@ -8799,13 +8799,13 @@
         <v>45054</v>
       </c>
       <c r="G84">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="H84" s="2">
         <v>45238</v>
       </c>
       <c r="I84">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="J84" t="inlineStr">
         <is>
@@ -8902,13 +8902,13 @@
         <v>45056</v>
       </c>
       <c r="G85">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="H85" s="2">
         <v>45240</v>
       </c>
       <c r="I85">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="J85" t="inlineStr">
         <is>
@@ -9005,13 +9005,13 @@
         <v>45085</v>
       </c>
       <c r="G86">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="H86" s="2">
         <v>45268</v>
       </c>
       <c r="I86">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="J86" t="inlineStr">
         <is>
@@ -9108,7 +9108,7 @@
         <v>45194</v>
       </c>
       <c r="I87">
-        <v>-1</v>
+        <v>-2</v>
       </c>
       <c r="J87" t="inlineStr">
         <is>
@@ -9195,13 +9195,13 @@
         <v>45103</v>
       </c>
       <c r="G88">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="H88" s="2">
         <v>45286</v>
       </c>
       <c r="I88">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="J88" t="inlineStr">
         <is>
@@ -9298,13 +9298,13 @@
         <v>45103</v>
       </c>
       <c r="G89">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="H89" s="2">
         <v>45286</v>
       </c>
       <c r="I89">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="J89" t="inlineStr">
         <is>
@@ -9401,13 +9401,13 @@
         <v>45008</v>
       </c>
       <c r="G90">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="H90" s="2">
         <v>45192</v>
       </c>
       <c r="I90">
-        <v>-3</v>
+        <v>-4</v>
       </c>
       <c r="J90" t="inlineStr">
         <is>
@@ -9499,13 +9499,13 @@
         <v>45100</v>
       </c>
       <c r="G91">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="H91" s="2">
         <v>45287</v>
       </c>
       <c r="I91">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="J91" t="inlineStr">
         <is>
@@ -9602,13 +9602,13 @@
         <v>45003</v>
       </c>
       <c r="G92">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="H92" s="2">
         <v>45187</v>
       </c>
       <c r="I92">
-        <v>-8</v>
+        <v>-9</v>
       </c>
       <c r="J92" t="inlineStr">
         <is>
@@ -9705,13 +9705,13 @@
         <v>45104</v>
       </c>
       <c r="G93">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="H93" s="2">
         <v>45287</v>
       </c>
       <c r="I93">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="J93" t="inlineStr">
         <is>
@@ -9808,13 +9808,13 @@
         <v>45104</v>
       </c>
       <c r="G94">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="H94" s="2">
         <v>45287</v>
       </c>
       <c r="I94">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="J94" t="inlineStr">
         <is>
@@ -9911,13 +9911,13 @@
         <v>45049</v>
       </c>
       <c r="G95">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="H95" s="2">
         <v>45233</v>
       </c>
       <c r="I95">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="J95" t="inlineStr">
         <is>
@@ -10014,13 +10014,13 @@
         <v>45122</v>
       </c>
       <c r="G96">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="H96" s="2">
         <v>45306</v>
       </c>
       <c r="I96">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="J96" t="inlineStr">
         <is>
@@ -10112,13 +10112,13 @@
         <v>45141</v>
       </c>
       <c r="G97">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="H97" s="2">
         <v>45325</v>
       </c>
       <c r="I97">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="J97" t="inlineStr">
         <is>
@@ -10215,13 +10215,13 @@
         <v>45010</v>
       </c>
       <c r="G98">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="H98" s="2">
         <v>45194</v>
       </c>
       <c r="I98">
-        <v>-1</v>
+        <v>-2</v>
       </c>
       <c r="J98" t="inlineStr">
         <is>
@@ -10313,13 +10313,13 @@
         <v>45093</v>
       </c>
       <c r="G99">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="H99" s="2">
         <v>45276</v>
       </c>
       <c r="I99">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="J99" t="inlineStr">
         <is>
@@ -10416,13 +10416,13 @@
         <v>45123</v>
       </c>
       <c r="G100">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="H100" s="2">
         <v>45307</v>
       </c>
       <c r="I100">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="J100" t="inlineStr">
         <is>
@@ -10519,13 +10519,13 @@
         <v>45014</v>
       </c>
       <c r="G101">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="H101" s="2">
         <v>45198</v>
       </c>
       <c r="I101">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="J101" t="inlineStr">
         <is>
@@ -10622,13 +10622,13 @@
         <v>45093</v>
       </c>
       <c r="G102">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="H102" s="2">
         <v>45276</v>
       </c>
       <c r="I102">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="J102" t="inlineStr">
         <is>
@@ -10725,13 +10725,13 @@
         <v>45122</v>
       </c>
       <c r="G103">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="H103" s="2">
         <v>45306</v>
       </c>
       <c r="I103">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="J103" t="inlineStr">
         <is>
@@ -10828,13 +10828,13 @@
         <v>45122</v>
       </c>
       <c r="G104">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="H104" s="2">
         <v>45306</v>
       </c>
       <c r="I104">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="J104" t="inlineStr">
         <is>
@@ -10926,13 +10926,13 @@
         <v>45050</v>
       </c>
       <c r="G105">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="H105" s="2">
         <v>45234</v>
       </c>
       <c r="I105">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="J105" t="inlineStr">
         <is>
@@ -11029,13 +11029,13 @@
         <v>45085</v>
       </c>
       <c r="G106">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="H106" s="2">
         <v>45268</v>
       </c>
       <c r="I106">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="J106" t="inlineStr">
         <is>
@@ -11132,13 +11132,13 @@
         <v>45093</v>
       </c>
       <c r="G107">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="H107" s="2">
         <v>45185</v>
       </c>
       <c r="I107">
-        <v>-10</v>
+        <v>-11</v>
       </c>
       <c r="J107" t="inlineStr">
         <is>
@@ -11230,13 +11230,13 @@
         <v>45093</v>
       </c>
       <c r="G108">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="H108" s="2">
         <v>45185</v>
       </c>
       <c r="I108">
-        <v>-10</v>
+        <v>-11</v>
       </c>
       <c r="J108" t="inlineStr">
         <is>
@@ -11328,13 +11328,13 @@
         <v>45093</v>
       </c>
       <c r="G109">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="H109" s="2">
         <v>45185</v>
       </c>
       <c r="I109">
-        <v>-10</v>
+        <v>-11</v>
       </c>
       <c r="J109" t="inlineStr">
         <is>
@@ -11431,13 +11431,13 @@
         <v>45148</v>
       </c>
       <c r="G110">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="H110" s="2">
         <v>45240</v>
       </c>
       <c r="I110">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="J110" t="inlineStr">
         <is>
@@ -11534,13 +11534,13 @@
         <v>45119</v>
       </c>
       <c r="G111">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="H111" s="2">
         <v>45211</v>
       </c>
       <c r="I111">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="J111" t="inlineStr">
         <is>
@@ -11637,13 +11637,13 @@
         <v>45172</v>
       </c>
       <c r="G112">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="H112" s="2">
         <v>45263</v>
       </c>
       <c r="I112">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="J112" t="inlineStr">
         <is>
@@ -11740,13 +11740,13 @@
         <v>45023</v>
       </c>
       <c r="G113">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="H113" s="2">
         <v>45206</v>
       </c>
       <c r="I113">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="J113" t="inlineStr">
         <is>
@@ -11843,13 +11843,13 @@
         <v>45111</v>
       </c>
       <c r="G114">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="H114" s="2">
         <v>45203</v>
       </c>
       <c r="I114">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="J114" t="inlineStr">
         <is>
@@ -11946,7 +11946,7 @@
         <v>45218</v>
       </c>
       <c r="I115">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="J115" t="inlineStr">
         <is>
@@ -12043,13 +12043,13 @@
         <v>45161</v>
       </c>
       <c r="G116">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="H116" s="2">
         <v>45253</v>
       </c>
       <c r="I116">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="J116" t="inlineStr">
         <is>
@@ -12146,13 +12146,13 @@
         <v>45115</v>
       </c>
       <c r="G117">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="H117" s="2">
         <v>45299</v>
       </c>
       <c r="I117">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="J117" t="inlineStr">
         <is>
@@ -12244,13 +12244,13 @@
         <v>45094</v>
       </c>
       <c r="G118">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="H118" s="2">
         <v>45277</v>
       </c>
       <c r="I118">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="J118" t="inlineStr">
         <is>
@@ -12347,13 +12347,13 @@
         <v>45104</v>
       </c>
       <c r="G119">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="H119" s="2">
         <v>45287</v>
       </c>
       <c r="I119">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="J119" t="inlineStr">
         <is>
@@ -12450,13 +12450,13 @@
         <v>45104</v>
       </c>
       <c r="G120">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="H120" s="2">
         <v>45287</v>
       </c>
       <c r="I120">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="J120" t="inlineStr">
         <is>
@@ -12553,13 +12553,13 @@
         <v>45104</v>
       </c>
       <c r="G121">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="H121" s="2">
         <v>45287</v>
       </c>
       <c r="I121">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="J121" t="inlineStr">
         <is>
@@ -12656,13 +12656,13 @@
         <v>45104</v>
       </c>
       <c r="G122">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="H122" s="2">
         <v>45287</v>
       </c>
       <c r="I122">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="J122" t="inlineStr">
         <is>
@@ -12759,13 +12759,13 @@
         <v>45107</v>
       </c>
       <c r="G123">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="H123" s="2">
         <v>45199</v>
       </c>
       <c r="I123">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="J123" t="inlineStr">
         <is>
@@ -12862,13 +12862,13 @@
         <v>45013</v>
       </c>
       <c r="G124">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="H124" s="2">
         <v>45197</v>
       </c>
       <c r="I124">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J124" t="inlineStr">
         <is>
@@ -12965,13 +12965,13 @@
         <v>45121</v>
       </c>
       <c r="G125">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="H125" s="2">
         <v>45213</v>
       </c>
       <c r="I125">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="J125" t="inlineStr">
         <is>
@@ -13068,13 +13068,13 @@
         <v>45134</v>
       </c>
       <c r="G126">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="H126" s="2">
         <v>45226</v>
       </c>
       <c r="I126">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="J126" t="inlineStr">
         <is>
@@ -13171,7 +13171,7 @@
         <v>45212</v>
       </c>
       <c r="I127">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="J127" t="inlineStr">
         <is>
@@ -13268,13 +13268,13 @@
         <v>45126</v>
       </c>
       <c r="G128">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="H128" s="2">
         <v>45218</v>
       </c>
       <c r="I128">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="J128" t="inlineStr">
         <is>
@@ -13366,13 +13366,13 @@
         <v>45158</v>
       </c>
       <c r="G129">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="H129" s="2">
         <v>45250</v>
       </c>
       <c r="I129">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="J129" t="inlineStr">
         <is>
@@ -13469,13 +13469,13 @@
         <v>45171</v>
       </c>
       <c r="G130">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="H130" s="2">
         <v>45262</v>
       </c>
       <c r="I130">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="J130" t="inlineStr">
         <is>
@@ -13572,13 +13572,13 @@
         <v>45111</v>
       </c>
       <c r="G131">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="H131" s="2">
         <v>45203</v>
       </c>
       <c r="I131">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="J131" t="inlineStr">
         <is>
@@ -13675,13 +13675,13 @@
         <v>45144</v>
       </c>
       <c r="G132">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="H132" s="2">
         <v>45236</v>
       </c>
       <c r="I132">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="J132" t="inlineStr">
         <is>
@@ -13778,13 +13778,13 @@
         <v>45156</v>
       </c>
       <c r="G133">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="H133" s="2">
         <v>45248</v>
       </c>
       <c r="I133">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="J133" t="inlineStr">
         <is>
@@ -13876,13 +13876,13 @@
         <v>45146</v>
       </c>
       <c r="G134">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="H134" s="2">
         <v>45238</v>
       </c>
       <c r="I134">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="J134" t="inlineStr">
         <is>
@@ -13979,13 +13979,13 @@
         <v>45140</v>
       </c>
       <c r="G135">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="H135" s="2">
         <v>45232</v>
       </c>
       <c r="I135">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="J135" t="inlineStr">
         <is>
@@ -14082,13 +14082,13 @@
         <v>45104</v>
       </c>
       <c r="G136">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="H136" s="2">
         <v>45196</v>
       </c>
       <c r="I136">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J136" t="inlineStr">
         <is>
@@ -14185,13 +14185,13 @@
         <v>45105</v>
       </c>
       <c r="G137">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="H137" s="2">
         <v>45197</v>
       </c>
       <c r="I137">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J137" t="inlineStr">
         <is>
@@ -14288,13 +14288,13 @@
         <v>45179</v>
       </c>
       <c r="G138">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="H138" s="2">
         <v>45270</v>
       </c>
       <c r="I138">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="J138" t="inlineStr">
         <is>
@@ -14386,13 +14386,13 @@
         <v>45105</v>
       </c>
       <c r="G139">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="H139" s="2">
         <v>45197</v>
       </c>
       <c r="I139">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J139" t="inlineStr">
         <is>
@@ -14489,13 +14489,13 @@
         <v>45182</v>
       </c>
       <c r="G140">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="H140" s="2">
         <v>45273</v>
       </c>
       <c r="I140">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="J140" t="inlineStr">
         <is>
@@ -14592,13 +14592,13 @@
         <v>45116</v>
       </c>
       <c r="G141">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="H141" s="2">
         <v>45208</v>
       </c>
       <c r="I141">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="J141" t="inlineStr">
         <is>
@@ -14690,13 +14690,13 @@
         <v>45150</v>
       </c>
       <c r="G142">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="H142" s="2">
         <v>45242</v>
       </c>
       <c r="I142">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="J142" t="inlineStr">
         <is>
@@ -14793,7 +14793,7 @@
         <v>45238</v>
       </c>
       <c r="I143">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="J143" t="inlineStr">
         <is>
@@ -14890,13 +14890,13 @@
         <v>45171</v>
       </c>
       <c r="G144">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="H144" s="2">
         <v>45262</v>
       </c>
       <c r="I144">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="J144" t="inlineStr">
         <is>
@@ -14993,13 +14993,13 @@
         <v>45102</v>
       </c>
       <c r="G145">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="H145" s="2">
         <v>45194</v>
       </c>
       <c r="I145">
-        <v>-1</v>
+        <v>-2</v>
       </c>
       <c r="J145" t="inlineStr">
         <is>
@@ -15086,13 +15086,13 @@
         <v>45119</v>
       </c>
       <c r="G146">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="H146" s="2">
         <v>45211</v>
       </c>
       <c r="I146">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="J146" t="inlineStr">
         <is>
@@ -15189,13 +15189,13 @@
         <v>45165</v>
       </c>
       <c r="G147">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="H147" s="2">
         <v>45257</v>
       </c>
       <c r="I147">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="J147" t="inlineStr">
         <is>
@@ -15292,13 +15292,13 @@
         <v>45166</v>
       </c>
       <c r="G148">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="H148" s="2">
         <v>45258</v>
       </c>
       <c r="I148">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="J148" t="inlineStr">
         <is>
@@ -15395,13 +15395,13 @@
         <v>45093</v>
       </c>
       <c r="G149">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="H149" s="2">
         <v>45185</v>
       </c>
       <c r="I149">
-        <v>-10</v>
+        <v>-11</v>
       </c>
       <c r="J149" t="inlineStr">
         <is>
@@ -15498,13 +15498,13 @@
         <v>45035</v>
       </c>
       <c r="G150">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="H150" s="2">
         <v>45218</v>
       </c>
       <c r="I150">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="J150" t="inlineStr">
         <is>
@@ -15601,13 +15601,13 @@
         <v>45174</v>
       </c>
       <c r="G151">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="H151" s="2">
         <v>45356</v>
       </c>
       <c r="I151">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="J151" t="inlineStr">
         <is>
@@ -15704,13 +15704,13 @@
         <v>45089</v>
       </c>
       <c r="G152">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="H152" s="2">
         <v>45272</v>
       </c>
       <c r="I152">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="J152" t="inlineStr">
         <is>
@@ -15807,13 +15807,13 @@
         <v>45124</v>
       </c>
       <c r="G153">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="H153" s="2">
         <v>45308</v>
       </c>
       <c r="I153">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="J153" t="inlineStr">
         <is>
@@ -15910,13 +15910,13 @@
         <v>45124</v>
       </c>
       <c r="G154">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="H154" s="2">
         <v>45308</v>
       </c>
       <c r="I154">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="J154" t="inlineStr">
         <is>
@@ -16013,13 +16013,13 @@
         <v>45026</v>
       </c>
       <c r="G155">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="H155" s="2">
         <v>45209</v>
       </c>
       <c r="I155">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="J155" t="inlineStr">
         <is>
@@ -16116,13 +16116,13 @@
         <v>45026</v>
       </c>
       <c r="G156">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="H156" s="2">
         <v>45209</v>
       </c>
       <c r="I156">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="J156" t="inlineStr">
         <is>
@@ -16219,13 +16219,13 @@
         <v>45026</v>
       </c>
       <c r="G157">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="H157" s="2">
         <v>45209</v>
       </c>
       <c r="I157">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="J157" t="inlineStr">
         <is>
@@ -16322,13 +16322,13 @@
         <v>45026</v>
       </c>
       <c r="G158">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="H158" s="2">
         <v>45209</v>
       </c>
       <c r="I158">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="J158" t="inlineStr">
         <is>
@@ -16425,13 +16425,13 @@
         <v>45156</v>
       </c>
       <c r="G159">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="H159" s="2">
         <v>45247</v>
       </c>
       <c r="I159">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="J159" t="inlineStr">
         <is>
@@ -16528,13 +16528,13 @@
         <v>45153</v>
       </c>
       <c r="G160">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="H160" s="2">
         <v>45245</v>
       </c>
       <c r="I160">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="J160" t="inlineStr">
         <is>
@@ -16631,13 +16631,13 @@
         <v>45135</v>
       </c>
       <c r="G161">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="H161" s="2">
         <v>45319</v>
       </c>
       <c r="I161">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="J161" t="inlineStr">
         <is>
@@ -16734,13 +16734,13 @@
         <v>45091</v>
       </c>
       <c r="G162">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="H162" s="2">
         <v>45274</v>
       </c>
       <c r="I162">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="J162" t="inlineStr">
         <is>
@@ -16832,13 +16832,13 @@
         <v>45091</v>
       </c>
       <c r="G163">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="H163" s="2">
         <v>45274</v>
       </c>
       <c r="I163">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="J163" t="inlineStr">
         <is>
@@ -16930,13 +16930,13 @@
         <v>45138</v>
       </c>
       <c r="G164">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="H164" s="2">
         <v>45322</v>
       </c>
       <c r="I164">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="J164" t="inlineStr">
         <is>
@@ -17033,13 +17033,13 @@
         <v>45138</v>
       </c>
       <c r="G165">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="H165" s="2">
         <v>45322</v>
       </c>
       <c r="I165">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="J165" t="inlineStr">
         <is>
@@ -17136,13 +17136,13 @@
         <v>45085</v>
       </c>
       <c r="G166">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="H166" s="2">
         <v>45268</v>
       </c>
       <c r="I166">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="J166" t="inlineStr">
         <is>
@@ -17239,13 +17239,13 @@
         <v>45085</v>
       </c>
       <c r="G167">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="H167" s="2">
         <v>45268</v>
       </c>
       <c r="I167">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="J167" t="inlineStr">
         <is>
@@ -17342,7 +17342,7 @@
         <v>45326</v>
       </c>
       <c r="I168">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="J168" t="inlineStr">
         <is>
@@ -17439,13 +17439,13 @@
         <v>45173</v>
       </c>
       <c r="G169">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="H169" s="2">
         <v>45355</v>
       </c>
       <c r="I169">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="J169" t="inlineStr">
         <is>
@@ -17542,13 +17542,13 @@
         <v>45056</v>
       </c>
       <c r="G170">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="H170" s="2">
         <v>45240</v>
       </c>
       <c r="I170">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="J170" t="inlineStr">
         <is>
@@ -17645,7 +17645,7 @@
         <v>45238</v>
       </c>
       <c r="I171">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="J171" t="inlineStr">
         <is>
@@ -17742,13 +17742,13 @@
         <v>45141</v>
       </c>
       <c r="G172">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="H172" s="2">
         <v>45325</v>
       </c>
       <c r="I172">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="J172" t="inlineStr">
         <is>
@@ -17845,13 +17845,13 @@
         <v>45037</v>
       </c>
       <c r="G173">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="H173" s="2">
         <v>45220</v>
       </c>
       <c r="I173">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="J173" t="inlineStr">
         <is>
@@ -17948,13 +17948,13 @@
         <v>45171</v>
       </c>
       <c r="G174">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="H174" s="2">
         <v>45262</v>
       </c>
       <c r="I174">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="J174" t="inlineStr">
         <is>
@@ -18051,13 +18051,13 @@
         <v>45105</v>
       </c>
       <c r="G175">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="H175" s="2">
         <v>45197</v>
       </c>
       <c r="I175">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J175" t="inlineStr">
         <is>
@@ -18154,13 +18154,13 @@
         <v>45162</v>
       </c>
       <c r="G176">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="H176" s="2">
         <v>45254</v>
       </c>
       <c r="I176">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="J176" t="inlineStr">
         <is>
@@ -18257,13 +18257,13 @@
         <v>45061</v>
       </c>
       <c r="G177">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="H177" s="2">
         <v>45245</v>
       </c>
       <c r="I177">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="J177" t="inlineStr">
         <is>
@@ -18360,13 +18360,13 @@
         <v>45120</v>
       </c>
       <c r="G178">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="H178" s="2">
         <v>45212</v>
       </c>
       <c r="I178">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="J178" t="inlineStr">
         <is>
@@ -18463,7 +18463,7 @@
         <v>45191</v>
       </c>
       <c r="I179">
-        <v>-4</v>
+        <v>-5</v>
       </c>
       <c r="J179" t="inlineStr">
         <is>
@@ -18560,13 +18560,13 @@
         <v>45088</v>
       </c>
       <c r="G180">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="H180" s="2">
         <v>45271</v>
       </c>
       <c r="I180">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="J180" t="inlineStr">
         <is>
@@ -18663,13 +18663,13 @@
         <v>45100</v>
       </c>
       <c r="G181">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="H181" s="2">
         <v>45192</v>
       </c>
       <c r="I181">
-        <v>-3</v>
+        <v>-4</v>
       </c>
       <c r="J181" t="inlineStr">
         <is>
@@ -18756,13 +18756,13 @@
         <v>45131</v>
       </c>
       <c r="G182">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="H182" s="2">
         <v>45223</v>
       </c>
       <c r="I182">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="J182" t="inlineStr">
         <is>
@@ -18854,13 +18854,13 @@
         <v>45136</v>
       </c>
       <c r="G183">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="H183" s="2">
         <v>45228</v>
       </c>
       <c r="I183">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="J183" t="inlineStr">
         <is>
@@ -18952,13 +18952,13 @@
         <v>45150</v>
       </c>
       <c r="G184">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="H184" s="2">
         <v>45242</v>
       </c>
       <c r="I184">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="J184" t="inlineStr">
         <is>
@@ -19050,13 +19050,13 @@
         <v>45118</v>
       </c>
       <c r="G185">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="H185" s="2">
         <v>45210</v>
       </c>
       <c r="I185">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="J185" t="inlineStr">
         <is>
@@ -19148,13 +19148,13 @@
         <v>45129</v>
       </c>
       <c r="G186">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="H186" s="2">
         <v>45221</v>
       </c>
       <c r="I186">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="J186" t="inlineStr">
         <is>
@@ -19246,13 +19246,13 @@
         <v>45097</v>
       </c>
       <c r="G187">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="H187" s="2">
         <v>45189</v>
       </c>
       <c r="I187">
-        <v>-6</v>
+        <v>-7</v>
       </c>
       <c r="J187" t="inlineStr">
         <is>
@@ -19339,13 +19339,13 @@
         <v>45101</v>
       </c>
       <c r="G188">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="H188" s="2">
         <v>45193</v>
       </c>
       <c r="I188">
-        <v>-2</v>
+        <v>-3</v>
       </c>
       <c r="J188" t="inlineStr">
         <is>
@@ -19432,13 +19432,13 @@
         <v>45165</v>
       </c>
       <c r="G189">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="H189" s="2">
         <v>45257</v>
       </c>
       <c r="I189">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="J189" t="inlineStr">
         <is>
@@ -19530,7 +19530,7 @@
         <v>45202</v>
       </c>
       <c r="I190">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="J190" t="inlineStr">
         <is>
@@ -19627,13 +19627,13 @@
         <v>45081</v>
       </c>
       <c r="G191">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="H191" s="2">
         <v>45264</v>
       </c>
       <c r="I191">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="J191" t="inlineStr">
         <is>
@@ -19730,13 +19730,13 @@
         <v>45081</v>
       </c>
       <c r="G192">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="H192" s="2">
         <v>45264</v>
       </c>
       <c r="I192">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="J192" t="inlineStr">
         <is>
@@ -19833,7 +19833,7 @@
         <v>45319</v>
       </c>
       <c r="I193">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="J193" t="inlineStr">
         <is>
@@ -19930,7 +19930,7 @@
         <v>45319</v>
       </c>
       <c r="I194">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="J194" t="inlineStr">
         <is>
@@ -20022,13 +20022,13 @@
         <v>45046</v>
       </c>
       <c r="G195">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="H195" s="2">
         <v>45230</v>
       </c>
       <c r="I195">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="J195" t="inlineStr">
         <is>
@@ -20125,13 +20125,13 @@
         <v>45046</v>
       </c>
       <c r="G196">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="H196" s="2">
         <v>45230</v>
       </c>
       <c r="I196">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="J196" t="inlineStr">
         <is>
@@ -20228,13 +20228,13 @@
         <v>45031</v>
       </c>
       <c r="G197">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="H197" s="2">
         <v>45214</v>
       </c>
       <c r="I197">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="J197" t="inlineStr">
         <is>
@@ -20331,13 +20331,13 @@
         <v>45031</v>
       </c>
       <c r="G198">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="H198" s="2">
         <v>45214</v>
       </c>
       <c r="I198">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="J198" t="inlineStr">
         <is>
@@ -20434,13 +20434,13 @@
         <v>45031</v>
       </c>
       <c r="G199">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="H199" s="2">
         <v>45214</v>
       </c>
       <c r="I199">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="J199" t="inlineStr">
         <is>
@@ -20537,13 +20537,13 @@
         <v>45031</v>
       </c>
       <c r="G200">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="H200" s="2">
         <v>45214</v>
       </c>
       <c r="I200">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="J200" t="inlineStr">
         <is>
@@ -20640,13 +20640,13 @@
         <v>45067</v>
       </c>
       <c r="G201">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="H201" s="2">
         <v>45251</v>
       </c>
       <c r="I201">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="J201" t="inlineStr">
         <is>
@@ -20743,13 +20743,13 @@
         <v>45067</v>
       </c>
       <c r="G202">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="H202" s="2">
         <v>45251</v>
       </c>
       <c r="I202">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="J202" t="inlineStr">
         <is>
@@ -20846,13 +20846,13 @@
         <v>45067</v>
       </c>
       <c r="G203">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="H203" s="2">
         <v>45251</v>
       </c>
       <c r="I203">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="J203" t="inlineStr">
         <is>
@@ -20949,13 +20949,13 @@
         <v>45067</v>
       </c>
       <c r="G204">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="H204" s="2">
         <v>45251</v>
       </c>
       <c r="I204">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="J204" t="inlineStr">
         <is>
@@ -21052,13 +21052,13 @@
         <v>45178</v>
       </c>
       <c r="G205">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="H205" s="2">
         <v>45269</v>
       </c>
       <c r="I205">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="J205" t="inlineStr">
         <is>
@@ -21155,7 +21155,7 @@
         <v>45252</v>
       </c>
       <c r="I206">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="J206" t="inlineStr">
         <is>
@@ -21252,13 +21252,13 @@
         <v>45087</v>
       </c>
       <c r="G207">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="H207" s="2">
         <v>45270</v>
       </c>
       <c r="I207">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="J207" t="inlineStr">
         <is>
@@ -21355,13 +21355,13 @@
         <v>45099</v>
       </c>
       <c r="G208">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="H208" s="2">
         <v>45282</v>
       </c>
       <c r="I208">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="J208" t="inlineStr">
         <is>
@@ -21458,13 +21458,13 @@
         <v>45175</v>
       </c>
       <c r="G209">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="H209" s="2">
         <v>45356</v>
       </c>
       <c r="I209">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="J209" t="inlineStr">
         <is>
@@ -21561,13 +21561,13 @@
         <v>45175</v>
       </c>
       <c r="G210">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="H210" s="2">
         <v>45356</v>
       </c>
       <c r="I210">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="J210" t="inlineStr">
         <is>
@@ -21664,13 +21664,13 @@
         <v>45166</v>
       </c>
       <c r="G211">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="H211" s="2">
         <v>45350</v>
       </c>
       <c r="I211">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="J211" t="inlineStr">
         <is>
@@ -21767,13 +21767,13 @@
         <v>45166</v>
       </c>
       <c r="G212">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="H212" s="2">
         <v>45350</v>
       </c>
       <c r="I212">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="J212" t="inlineStr">
         <is>
@@ -21870,13 +21870,13 @@
         <v>45090</v>
       </c>
       <c r="G213">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="H213" s="2">
         <v>45273</v>
       </c>
       <c r="I213">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="J213" t="inlineStr">
         <is>
@@ -21973,13 +21973,13 @@
         <v>45106</v>
       </c>
       <c r="G214">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="H214" s="2">
         <v>45289</v>
       </c>
       <c r="I214">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="J214" t="inlineStr">
         <is>
@@ -22076,13 +22076,13 @@
         <v>45134</v>
       </c>
       <c r="G215">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="H215" s="2">
         <v>45226</v>
       </c>
       <c r="I215">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="J215" t="inlineStr">
         <is>
@@ -22179,13 +22179,13 @@
         <v>45132</v>
       </c>
       <c r="G216">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="H216" s="2">
         <v>45224</v>
       </c>
       <c r="I216">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="J216" t="inlineStr">
         <is>
@@ -22282,13 +22282,13 @@
         <v>45150</v>
       </c>
       <c r="G217">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="H217" s="2">
         <v>45242</v>
       </c>
       <c r="I217">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="J217" t="inlineStr">
         <is>
@@ -22385,13 +22385,13 @@
         <v>45095</v>
       </c>
       <c r="G218">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="H218" s="2">
         <v>45187</v>
       </c>
       <c r="I218">
-        <v>-8</v>
+        <v>-9</v>
       </c>
       <c r="J218" t="inlineStr">
         <is>
@@ -22483,13 +22483,13 @@
         <v>45182</v>
       </c>
       <c r="G219">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="H219" s="2">
         <v>45273</v>
       </c>
       <c r="I219">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="J219" t="inlineStr">
         <is>
@@ -22586,7 +22586,7 @@
         <v>45196</v>
       </c>
       <c r="I220">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J220" t="inlineStr">
         <is>
@@ -22683,13 +22683,13 @@
         <v>45108</v>
       </c>
       <c r="G221">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="H221" s="2">
         <v>45200</v>
       </c>
       <c r="I221">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="J221" t="inlineStr">
         <is>
@@ -22786,13 +22786,13 @@
         <v>45135</v>
       </c>
       <c r="G222">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="H222" s="2">
         <v>45227</v>
       </c>
       <c r="I222">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="J222" t="inlineStr">
         <is>
@@ -22889,13 +22889,13 @@
         <v>45148</v>
       </c>
       <c r="G223">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="H223" s="2">
         <v>45240</v>
       </c>
       <c r="I223">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="J223" t="inlineStr">
         <is>
@@ -22987,13 +22987,13 @@
         <v>45100</v>
       </c>
       <c r="G224">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="H224" s="2">
         <v>45192</v>
       </c>
       <c r="I224">
-        <v>-3</v>
+        <v>-4</v>
       </c>
       <c r="J224" t="inlineStr">
         <is>
@@ -23085,13 +23085,13 @@
         <v>45136</v>
       </c>
       <c r="G225">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="H225" s="2">
         <v>45320</v>
       </c>
       <c r="I225">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="J225" t="inlineStr">
         <is>
@@ -23188,13 +23188,13 @@
         <v>45136</v>
       </c>
       <c r="G226">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="H226" s="2">
         <v>45320</v>
       </c>
       <c r="I226">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="J226" t="inlineStr">
         <is>
@@ -23291,13 +23291,13 @@
         <v>45094</v>
       </c>
       <c r="G227">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="H227" s="2">
         <v>45277</v>
       </c>
       <c r="I227">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="J227" t="inlineStr">
         <is>
@@ -23394,13 +23394,13 @@
         <v>45081</v>
       </c>
       <c r="G228">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="H228" s="2">
         <v>45264</v>
       </c>
       <c r="I228">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="J228" t="inlineStr">
         <is>
@@ -23497,13 +23497,13 @@
         <v>45099</v>
       </c>
       <c r="G229">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="H229" s="2">
         <v>45282</v>
       </c>
       <c r="I229">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="J229" t="inlineStr">
         <is>
@@ -23600,13 +23600,13 @@
         <v>45018</v>
       </c>
       <c r="G230">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="H230" s="2">
         <v>45201</v>
       </c>
       <c r="I230">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="J230" t="inlineStr">
         <is>
@@ -23703,13 +23703,13 @@
         <v>45031</v>
       </c>
       <c r="G231">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="H231" s="2">
         <v>45214</v>
       </c>
       <c r="I231">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="J231" t="inlineStr">
         <is>
@@ -23806,7 +23806,7 @@
         <v>45294</v>
       </c>
       <c r="I232">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="J232" t="inlineStr">
         <is>
@@ -23903,13 +23903,13 @@
         <v>45079</v>
       </c>
       <c r="G233">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="H233" s="2">
         <v>45262</v>
       </c>
       <c r="I233">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="J233" t="inlineStr">
         <is>
@@ -24006,7 +24006,7 @@
         <v>45199</v>
       </c>
       <c r="I234">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="J234" t="inlineStr">
         <is>
@@ -24103,13 +24103,13 @@
         <v>45021</v>
       </c>
       <c r="G235">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="H235" s="2">
         <v>45204</v>
       </c>
       <c r="I235">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="J235" t="inlineStr">
         <is>
@@ -24206,13 +24206,13 @@
         <v>45021</v>
       </c>
       <c r="G236">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="H236" s="2">
         <v>45204</v>
       </c>
       <c r="I236">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="J236" t="inlineStr">
         <is>
@@ -24309,13 +24309,13 @@
         <v>45080</v>
       </c>
       <c r="G237">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="H237" s="2">
         <v>45263</v>
       </c>
       <c r="I237">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="J237" t="inlineStr">
         <is>
@@ -24412,13 +24412,13 @@
         <v>45046</v>
       </c>
       <c r="G238">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="H238" s="2">
         <v>45229</v>
       </c>
       <c r="I238">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="J238" t="inlineStr">
         <is>
@@ -24515,13 +24515,13 @@
         <v>45112</v>
       </c>
       <c r="G239">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="H239" s="2">
         <v>45204</v>
       </c>
       <c r="I239">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="J239" t="inlineStr">
         <is>
@@ -24609,13 +24609,13 @@
         <v>45112</v>
       </c>
       <c r="G240">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="H240" s="2">
         <v>45204</v>
       </c>
       <c r="I240">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="J240" t="inlineStr">
         <is>
@@ -24703,13 +24703,13 @@
         <v>45016</v>
       </c>
       <c r="G241">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="H241" s="2">
         <v>45199</v>
       </c>
       <c r="I241">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="J241" t="inlineStr">
         <is>
@@ -24806,13 +24806,13 @@
         <v>45070</v>
       </c>
       <c r="G242">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="H242" s="2">
         <v>45254</v>
       </c>
       <c r="I242">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="J242" t="inlineStr">
         <is>
@@ -24909,13 +24909,13 @@
         <v>45168</v>
       </c>
       <c r="G243">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="H243" s="2">
         <v>45260</v>
       </c>
       <c r="I243">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="J243" t="inlineStr">
         <is>
@@ -25012,13 +25012,13 @@
         <v>45027</v>
       </c>
       <c r="G244">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="H244" s="2">
         <v>45210</v>
       </c>
       <c r="I244">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="J244" t="inlineStr">
         <is>
@@ -25115,13 +25115,13 @@
         <v>45077</v>
       </c>
       <c r="G245">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="H245" s="2">
         <v>45260</v>
       </c>
       <c r="I245">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="J245" t="inlineStr">
         <is>
@@ -25218,13 +25218,13 @@
         <v>45100</v>
       </c>
       <c r="G246">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="H246" s="2">
         <v>45283</v>
       </c>
       <c r="I246">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="J246" t="inlineStr">
         <is>
@@ -25321,7 +25321,7 @@
         <v>45281</v>
       </c>
       <c r="I247">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="J247" t="inlineStr">
         <is>
@@ -25418,13 +25418,13 @@
         <v>45044</v>
       </c>
       <c r="G248">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="H248" s="2">
         <v>45227</v>
       </c>
       <c r="I248">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="J248" t="inlineStr">
         <is>
@@ -25521,13 +25521,13 @@
         <v>45101</v>
       </c>
       <c r="G249">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="H249" s="2">
         <v>45283</v>
       </c>
       <c r="I249">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="J249" t="inlineStr">
         <is>
@@ -25624,13 +25624,13 @@
         <v>45134</v>
       </c>
       <c r="G250">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="H250" s="2">
         <v>45226</v>
       </c>
       <c r="I250">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="J250" t="inlineStr">
         <is>
@@ -25727,13 +25727,13 @@
         <v>45158</v>
       </c>
       <c r="G251">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="H251" s="2">
         <v>45250</v>
       </c>
       <c r="I251">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="J251" t="inlineStr">
         <is>
@@ -25830,13 +25830,13 @@
         <v>45108</v>
       </c>
       <c r="G252">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="H252" s="2">
         <v>45200</v>
       </c>
       <c r="I252">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="J252" t="inlineStr">
         <is>
@@ -25933,7 +25933,7 @@
         <v>45317</v>
       </c>
       <c r="I253">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="J253" t="inlineStr">
         <is>
@@ -26030,13 +26030,13 @@
         <v>45039</v>
       </c>
       <c r="G254">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="H254" s="2">
         <v>45222</v>
       </c>
       <c r="I254">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="J254" t="inlineStr">
         <is>
@@ -26128,13 +26128,13 @@
         <v>45129</v>
       </c>
       <c r="G255">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="H255" s="2">
         <v>45221</v>
       </c>
       <c r="I255">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="J255" t="inlineStr">
         <is>
@@ -26231,13 +26231,13 @@
         <v>45157</v>
       </c>
       <c r="G256">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="H256" s="2">
         <v>45341</v>
       </c>
       <c r="I256">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="J256" t="inlineStr">
         <is>
@@ -26334,13 +26334,13 @@
         <v>45063</v>
       </c>
       <c r="G257">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="H257" s="2">
         <v>45247</v>
       </c>
       <c r="I257">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="J257" t="inlineStr">
         <is>
@@ -26437,7 +26437,7 @@
         <v>45254</v>
       </c>
       <c r="I258">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="J258" t="inlineStr">
         <is>
@@ -26534,7 +26534,7 @@
         <v>45486</v>
       </c>
       <c r="I259">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="J259" t="inlineStr">
         <is>
@@ -26626,13 +26626,13 @@
         <v>45073</v>
       </c>
       <c r="G260">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="H260" s="2">
         <v>45439</v>
       </c>
       <c r="I260">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="J260" t="inlineStr">
         <is>
@@ -26724,7 +26724,7 @@
         <v>45323</v>
       </c>
       <c r="I261">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="J261" t="inlineStr">
         <is>
@@ -26816,7 +26816,7 @@
         <v>45303</v>
       </c>
       <c r="I262">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="J262" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
Bond dates update Thu Sep 28 23:11:33 UTC 2023
</commit_message>
<xml_diff>
--- a/Data/obligacje_screener.xlsx
+++ b/Data/obligacje_screener.xlsx
@@ -512,7 +512,7 @@
         <v>45340</v>
       </c>
       <c r="I2">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="J2" t="inlineStr">
         <is>
@@ -600,13 +600,13 @@
         <v>45121</v>
       </c>
       <c r="G3">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="H3" s="2">
         <v>45305</v>
       </c>
       <c r="I3">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="J3" t="inlineStr">
         <is>
@@ -703,13 +703,13 @@
         <v>45039</v>
       </c>
       <c r="G4">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="H4" s="2">
         <v>45222</v>
       </c>
       <c r="I4">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="J4" t="inlineStr">
         <is>
@@ -806,13 +806,13 @@
         <v>45039</v>
       </c>
       <c r="G5">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="H5" s="2">
         <v>45222</v>
       </c>
       <c r="I5">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="J5" t="inlineStr">
         <is>
@@ -909,13 +909,13 @@
         <v>45129</v>
       </c>
       <c r="G6">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="H6" s="2">
         <v>45221</v>
       </c>
       <c r="I6">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="J6" t="inlineStr">
         <is>
@@ -1012,13 +1012,13 @@
         <v>45162</v>
       </c>
       <c r="G7">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="H7" s="2">
         <v>45254</v>
       </c>
       <c r="I7">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="J7" t="inlineStr">
         <is>
@@ -1110,13 +1110,13 @@
         <v>45156</v>
       </c>
       <c r="G8">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="H8" s="2">
         <v>45248</v>
       </c>
       <c r="I8">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="J8" t="inlineStr">
         <is>
@@ -1213,13 +1213,13 @@
         <v>45141</v>
       </c>
       <c r="G9">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="H9" s="2">
         <v>45233</v>
       </c>
       <c r="I9">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="J9" t="inlineStr">
         <is>
@@ -1316,13 +1316,13 @@
         <v>45062</v>
       </c>
       <c r="G10">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="H10" s="2">
         <v>45246</v>
       </c>
       <c r="I10">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="J10" t="inlineStr">
         <is>
@@ -1419,7 +1419,7 @@
         <v>45286</v>
       </c>
       <c r="I11">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="J11" t="inlineStr">
         <is>
@@ -1516,13 +1516,13 @@
         <v>45011</v>
       </c>
       <c r="G12">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="H12" s="2">
         <v>45195</v>
       </c>
       <c r="I12">
-        <v>-1</v>
+        <v>-2</v>
       </c>
       <c r="J12" t="inlineStr">
         <is>
@@ -1614,13 +1614,13 @@
         <v>45036</v>
       </c>
       <c r="G13">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="H13" s="2">
         <v>45219</v>
       </c>
       <c r="I13">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="J13" t="inlineStr">
         <is>
@@ -1717,13 +1717,13 @@
         <v>45036</v>
       </c>
       <c r="G14">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="H14" s="2">
         <v>45219</v>
       </c>
       <c r="I14">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="J14" t="inlineStr">
         <is>
@@ -1820,13 +1820,13 @@
         <v>45106</v>
       </c>
       <c r="G15">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="H15" s="2">
         <v>45289</v>
       </c>
       <c r="I15">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="J15" t="inlineStr">
         <is>
@@ -1923,13 +1923,13 @@
         <v>45094</v>
       </c>
       <c r="G16">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="H16" s="2">
         <v>45186</v>
       </c>
       <c r="I16">
-        <v>-10</v>
+        <v>-11</v>
       </c>
       <c r="J16" t="inlineStr">
         <is>
@@ -2026,13 +2026,13 @@
         <v>45094</v>
       </c>
       <c r="G17">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="H17" s="2">
         <v>45186</v>
       </c>
       <c r="I17">
-        <v>-10</v>
+        <v>-11</v>
       </c>
       <c r="J17" t="inlineStr">
         <is>
@@ -2129,13 +2129,13 @@
         <v>45132</v>
       </c>
       <c r="G18">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="H18" s="2">
         <v>45224</v>
       </c>
       <c r="I18">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="J18" t="inlineStr">
         <is>
@@ -2232,13 +2232,13 @@
         <v>45137</v>
       </c>
       <c r="G19">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="H19" s="2">
         <v>45229</v>
       </c>
       <c r="I19">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="J19" t="inlineStr">
         <is>
@@ -2330,13 +2330,13 @@
         <v>45183</v>
       </c>
       <c r="G20">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="H20" s="2">
         <v>45274</v>
       </c>
       <c r="I20">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="J20" t="inlineStr">
         <is>
@@ -2433,13 +2433,13 @@
         <v>45093</v>
       </c>
       <c r="G21">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="H21" s="2">
         <v>45187</v>
       </c>
       <c r="I21">
-        <v>-9</v>
+        <v>-10</v>
       </c>
       <c r="J21" t="inlineStr">
         <is>
@@ -2536,13 +2536,13 @@
         <v>45096</v>
       </c>
       <c r="G22">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="H22" s="2">
         <v>45187</v>
       </c>
       <c r="I22">
-        <v>-9</v>
+        <v>-10</v>
       </c>
       <c r="J22" t="inlineStr">
         <is>
@@ -2639,7 +2639,7 @@
         <v>45245</v>
       </c>
       <c r="I23">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="J23" t="inlineStr">
         <is>
@@ -2736,7 +2736,7 @@
         <v>45245</v>
       </c>
       <c r="I24">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="J24" t="inlineStr">
         <is>
@@ -2833,13 +2833,13 @@
         <v>45021</v>
       </c>
       <c r="G25">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="H25" s="2">
         <v>45204</v>
       </c>
       <c r="I25">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="J25" t="inlineStr">
         <is>
@@ -2936,13 +2936,13 @@
         <v>45160</v>
       </c>
       <c r="G26">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="H26" s="2">
         <v>45344</v>
       </c>
       <c r="I26">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="J26" t="inlineStr">
         <is>
@@ -3039,13 +3039,13 @@
         <v>45118</v>
       </c>
       <c r="G27">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="H27" s="2">
         <v>45302</v>
       </c>
       <c r="I27">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="J27" t="inlineStr">
         <is>
@@ -3142,13 +3142,13 @@
         <v>45085</v>
       </c>
       <c r="G28">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="H28" s="2">
         <v>45268</v>
       </c>
       <c r="I28">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="J28" t="inlineStr">
         <is>
@@ -3245,13 +3245,13 @@
         <v>45183</v>
       </c>
       <c r="G29">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="H29" s="2">
         <v>45274</v>
       </c>
       <c r="I29">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="J29" t="inlineStr">
         <is>
@@ -3348,7 +3348,7 @@
         <v>45224</v>
       </c>
       <c r="I30">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="J30" t="inlineStr">
         <is>
@@ -3445,13 +3445,13 @@
         <v>45153</v>
       </c>
       <c r="G31">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="H31" s="2">
         <v>45245</v>
       </c>
       <c r="I31">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="J31" t="inlineStr">
         <is>
@@ -3548,13 +3548,13 @@
         <v>45155</v>
       </c>
       <c r="G32">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="H32" s="2">
         <v>45247</v>
       </c>
       <c r="I32">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="J32" t="inlineStr">
         <is>
@@ -3651,7 +3651,7 @@
         <v>45255</v>
       </c>
       <c r="I33">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="J33" t="inlineStr">
         <is>
@@ -3739,13 +3739,13 @@
         <v>45176</v>
       </c>
       <c r="G34">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="H34" s="2">
         <v>45267</v>
       </c>
       <c r="I34">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="J34" t="inlineStr">
         <is>
@@ -3842,13 +3842,13 @@
         <v>45130</v>
       </c>
       <c r="G35">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="H35" s="2">
         <v>45222</v>
       </c>
       <c r="I35">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="J35" t="inlineStr">
         <is>
@@ -3940,13 +3940,13 @@
         <v>45115</v>
       </c>
       <c r="G36">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="H36" s="2">
         <v>45207</v>
       </c>
       <c r="I36">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="J36" t="inlineStr">
         <is>
@@ -4043,13 +4043,13 @@
         <v>45097</v>
       </c>
       <c r="G37">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="H37" s="2">
         <v>45189</v>
       </c>
       <c r="I37">
-        <v>-7</v>
+        <v>-8</v>
       </c>
       <c r="J37" t="inlineStr">
         <is>
@@ -4141,13 +4141,13 @@
         <v>45107</v>
       </c>
       <c r="G38">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="H38" s="2">
         <v>45290</v>
       </c>
       <c r="I38">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="J38" t="inlineStr">
         <is>
@@ -4244,13 +4244,13 @@
         <v>45063</v>
       </c>
       <c r="G39">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="H39" s="2">
         <v>45247</v>
       </c>
       <c r="I39">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="J39" t="inlineStr">
         <is>
@@ -4347,13 +4347,13 @@
         <v>45177</v>
       </c>
       <c r="G40">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="H40" s="2">
         <v>45359</v>
       </c>
       <c r="I40">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="J40" t="inlineStr">
         <is>
@@ -4450,13 +4450,13 @@
         <v>45107</v>
       </c>
       <c r="G41">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="H41" s="2">
         <v>45290</v>
       </c>
       <c r="I41">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="J41" t="inlineStr">
         <is>
@@ -4553,7 +4553,7 @@
         <v>45265</v>
       </c>
       <c r="I42">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="J42" t="inlineStr">
         <is>
@@ -4650,13 +4650,13 @@
         <v>45098</v>
       </c>
       <c r="G43">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="H43" s="2">
         <v>45281</v>
       </c>
       <c r="I43">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="J43" t="inlineStr">
         <is>
@@ -4753,13 +4753,13 @@
         <v>45099</v>
       </c>
       <c r="G44">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="H44" s="2">
         <v>45282</v>
       </c>
       <c r="I44">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="J44" t="inlineStr">
         <is>
@@ -4856,13 +4856,13 @@
         <v>45106</v>
       </c>
       <c r="G45">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="H45" s="2">
         <v>45289</v>
       </c>
       <c r="I45">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="J45" t="inlineStr">
         <is>
@@ -4959,13 +4959,13 @@
         <v>45106</v>
       </c>
       <c r="G46">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="H46" s="2">
         <v>45289</v>
       </c>
       <c r="I46">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="J46" t="inlineStr">
         <is>
@@ -5062,13 +5062,13 @@
         <v>45120</v>
       </c>
       <c r="G47">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="H47" s="2">
         <v>45304</v>
       </c>
       <c r="I47">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="J47" t="inlineStr">
         <is>
@@ -5165,13 +5165,13 @@
         <v>45118</v>
       </c>
       <c r="G48">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="H48" s="2">
         <v>45302</v>
       </c>
       <c r="I48">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="J48" t="inlineStr">
         <is>
@@ -5268,13 +5268,13 @@
         <v>45152</v>
       </c>
       <c r="G49">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="H49" s="2">
         <v>45336</v>
       </c>
       <c r="I49">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="J49" t="inlineStr">
         <is>
@@ -5371,13 +5371,13 @@
         <v>45042</v>
       </c>
       <c r="G50">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="H50" s="2">
         <v>45225</v>
       </c>
       <c r="I50">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="J50" t="inlineStr">
         <is>
@@ -5474,13 +5474,13 @@
         <v>45122</v>
       </c>
       <c r="G51">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="H51" s="2">
         <v>45306</v>
       </c>
       <c r="I51">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="J51" t="inlineStr">
         <is>
@@ -5577,13 +5577,13 @@
         <v>45139</v>
       </c>
       <c r="G52">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="H52" s="2">
         <v>45323</v>
       </c>
       <c r="I52">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="J52" t="inlineStr">
         <is>
@@ -5671,13 +5671,13 @@
         <v>45099</v>
       </c>
       <c r="G53">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="H53" s="2">
         <v>45282</v>
       </c>
       <c r="I53">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="J53" t="inlineStr">
         <is>
@@ -5774,7 +5774,7 @@
         <v>45196</v>
       </c>
       <c r="I54">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="J54" t="inlineStr">
         <is>
@@ -5871,13 +5871,13 @@
         <v>45044</v>
       </c>
       <c r="G55">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="H55" s="2">
         <v>45227</v>
       </c>
       <c r="I55">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="J55" t="inlineStr">
         <is>
@@ -5974,13 +5974,13 @@
         <v>45151</v>
       </c>
       <c r="G56">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="H56" s="2">
         <v>45243</v>
       </c>
       <c r="I56">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="J56" t="inlineStr">
         <is>
@@ -6072,7 +6072,7 @@
         <v>45196</v>
       </c>
       <c r="I57">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="J57" t="inlineStr">
         <is>
@@ -6169,13 +6169,13 @@
         <v>45069</v>
       </c>
       <c r="G58">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="H58" s="2">
         <v>45253</v>
       </c>
       <c r="I58">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="J58" t="inlineStr">
         <is>
@@ -6272,13 +6272,13 @@
         <v>45099</v>
       </c>
       <c r="G59">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="H59" s="2">
         <v>45191</v>
       </c>
       <c r="I59">
-        <v>-5</v>
+        <v>-6</v>
       </c>
       <c r="J59" t="inlineStr">
         <is>
@@ -6370,13 +6370,13 @@
         <v>45113</v>
       </c>
       <c r="G60">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="H60" s="2">
         <v>45205</v>
       </c>
       <c r="I60">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="J60" t="inlineStr">
         <is>
@@ -6473,13 +6473,13 @@
         <v>45127</v>
       </c>
       <c r="G61">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="H61" s="2">
         <v>45219</v>
       </c>
       <c r="I61">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="J61" t="inlineStr">
         <is>
@@ -6576,13 +6576,13 @@
         <v>45058</v>
       </c>
       <c r="G62">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="H62" s="2">
         <v>45242</v>
       </c>
       <c r="I62">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="J62" t="inlineStr">
         <is>
@@ -6679,13 +6679,13 @@
         <v>45010</v>
       </c>
       <c r="G63">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="H63" s="2">
         <v>45194</v>
       </c>
       <c r="I63">
-        <v>-2</v>
+        <v>-3</v>
       </c>
       <c r="J63" t="inlineStr">
         <is>
@@ -6777,13 +6777,13 @@
         <v>45025</v>
       </c>
       <c r="G64">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="H64" s="2">
         <v>45208</v>
       </c>
       <c r="I64">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="J64" t="inlineStr">
         <is>
@@ -6880,13 +6880,13 @@
         <v>45025</v>
       </c>
       <c r="G65">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="H65" s="2">
         <v>45208</v>
       </c>
       <c r="I65">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="J65" t="inlineStr">
         <is>
@@ -6983,13 +6983,13 @@
         <v>45089</v>
       </c>
       <c r="G66">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="H66" s="2">
         <v>45272</v>
       </c>
       <c r="I66">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="J66" t="inlineStr">
         <is>
@@ -7086,13 +7086,13 @@
         <v>45178</v>
       </c>
       <c r="G67">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="H67" s="2">
         <v>45269</v>
       </c>
       <c r="I67">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="J67" t="inlineStr">
         <is>
@@ -7184,13 +7184,13 @@
         <v>45104</v>
       </c>
       <c r="G68">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="H68" s="2">
         <v>45196</v>
       </c>
       <c r="I68">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="J68" t="inlineStr">
         <is>
@@ -7287,13 +7287,13 @@
         <v>45149</v>
       </c>
       <c r="G69">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="H69" s="2">
         <v>45241</v>
       </c>
       <c r="I69">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="J69" t="inlineStr">
         <is>
@@ -7390,7 +7390,7 @@
         <v>45205</v>
       </c>
       <c r="I70">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="J70" t="inlineStr">
         <is>
@@ -7487,13 +7487,13 @@
         <v>45114</v>
       </c>
       <c r="G71">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="H71" s="2">
         <v>45205</v>
       </c>
       <c r="I71">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="J71" t="inlineStr">
         <is>
@@ -7590,13 +7590,13 @@
         <v>45115</v>
       </c>
       <c r="G72">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="H72" s="2">
         <v>45207</v>
       </c>
       <c r="I72">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="J72" t="inlineStr">
         <is>
@@ -7693,13 +7693,13 @@
         <v>45097</v>
       </c>
       <c r="G73">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="H73" s="2">
         <v>45189</v>
       </c>
       <c r="I73">
-        <v>-7</v>
+        <v>-8</v>
       </c>
       <c r="J73" t="inlineStr">
         <is>
@@ -7791,13 +7791,13 @@
         <v>45038</v>
       </c>
       <c r="G74">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="H74" s="2">
         <v>45221</v>
       </c>
       <c r="I74">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="J74" t="inlineStr">
         <is>
@@ -7889,13 +7889,13 @@
         <v>45117</v>
       </c>
       <c r="G75">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="H75" s="2">
         <v>45301</v>
       </c>
       <c r="I75">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="J75" t="inlineStr">
         <is>
@@ -7992,13 +7992,13 @@
         <v>45160</v>
       </c>
       <c r="G76">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="H76" s="2">
         <v>45344</v>
       </c>
       <c r="I76">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="J76" t="inlineStr">
         <is>
@@ -8095,13 +8095,13 @@
         <v>45002</v>
       </c>
       <c r="G77">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="H77" s="2">
         <v>45186</v>
       </c>
       <c r="I77">
-        <v>-10</v>
+        <v>-11</v>
       </c>
       <c r="J77" t="inlineStr">
         <is>
@@ -8198,13 +8198,13 @@
         <v>45043</v>
       </c>
       <c r="G78">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="H78" s="2">
         <v>45226</v>
       </c>
       <c r="I78">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="J78" t="inlineStr">
         <is>
@@ -8301,13 +8301,13 @@
         <v>45079</v>
       </c>
       <c r="G79">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="H79" s="2">
         <v>45262</v>
       </c>
       <c r="I79">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="J79" t="inlineStr">
         <is>
@@ -8404,7 +8404,7 @@
         <v>45254</v>
       </c>
       <c r="I80">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="J80" t="inlineStr">
         <is>
@@ -8501,13 +8501,13 @@
         <v>45104</v>
       </c>
       <c r="G81">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="H81" s="2">
         <v>45287</v>
       </c>
       <c r="I81">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="J81" t="inlineStr">
         <is>
@@ -8604,7 +8604,7 @@
         <v>45288</v>
       </c>
       <c r="I82">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="J82" t="inlineStr">
         <is>
@@ -8696,13 +8696,13 @@
         <v>45175</v>
       </c>
       <c r="G83">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="H83" s="2">
         <v>45357</v>
       </c>
       <c r="I83">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="J83" t="inlineStr">
         <is>
@@ -8799,13 +8799,13 @@
         <v>45054</v>
       </c>
       <c r="G84">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="H84" s="2">
         <v>45238</v>
       </c>
       <c r="I84">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="J84" t="inlineStr">
         <is>
@@ -8902,13 +8902,13 @@
         <v>45056</v>
       </c>
       <c r="G85">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="H85" s="2">
         <v>45240</v>
       </c>
       <c r="I85">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="J85" t="inlineStr">
         <is>
@@ -9005,13 +9005,13 @@
         <v>45085</v>
       </c>
       <c r="G86">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="H86" s="2">
         <v>45268</v>
       </c>
       <c r="I86">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="J86" t="inlineStr">
         <is>
@@ -9108,7 +9108,7 @@
         <v>45194</v>
       </c>
       <c r="I87">
-        <v>-2</v>
+        <v>-3</v>
       </c>
       <c r="J87" t="inlineStr">
         <is>
@@ -9195,13 +9195,13 @@
         <v>45103</v>
       </c>
       <c r="G88">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="H88" s="2">
         <v>45286</v>
       </c>
       <c r="I88">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="J88" t="inlineStr">
         <is>
@@ -9298,13 +9298,13 @@
         <v>45103</v>
       </c>
       <c r="G89">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="H89" s="2">
         <v>45286</v>
       </c>
       <c r="I89">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="J89" t="inlineStr">
         <is>
@@ -9401,13 +9401,13 @@
         <v>45008</v>
       </c>
       <c r="G90">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="H90" s="2">
         <v>45192</v>
       </c>
       <c r="I90">
-        <v>-4</v>
+        <v>-5</v>
       </c>
       <c r="J90" t="inlineStr">
         <is>
@@ -9499,13 +9499,13 @@
         <v>45100</v>
       </c>
       <c r="G91">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="H91" s="2">
         <v>45287</v>
       </c>
       <c r="I91">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="J91" t="inlineStr">
         <is>
@@ -9602,13 +9602,13 @@
         <v>45003</v>
       </c>
       <c r="G92">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="H92" s="2">
         <v>45187</v>
       </c>
       <c r="I92">
-        <v>-9</v>
+        <v>-10</v>
       </c>
       <c r="J92" t="inlineStr">
         <is>
@@ -9705,13 +9705,13 @@
         <v>45104</v>
       </c>
       <c r="G93">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="H93" s="2">
         <v>45287</v>
       </c>
       <c r="I93">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="J93" t="inlineStr">
         <is>
@@ -9808,13 +9808,13 @@
         <v>45104</v>
       </c>
       <c r="G94">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="H94" s="2">
         <v>45287</v>
       </c>
       <c r="I94">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="J94" t="inlineStr">
         <is>
@@ -9911,13 +9911,13 @@
         <v>45049</v>
       </c>
       <c r="G95">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="H95" s="2">
         <v>45233</v>
       </c>
       <c r="I95">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="J95" t="inlineStr">
         <is>
@@ -10014,13 +10014,13 @@
         <v>45122</v>
       </c>
       <c r="G96">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="H96" s="2">
         <v>45306</v>
       </c>
       <c r="I96">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="J96" t="inlineStr">
         <is>
@@ -10112,13 +10112,13 @@
         <v>45141</v>
       </c>
       <c r="G97">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="H97" s="2">
         <v>45325</v>
       </c>
       <c r="I97">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="J97" t="inlineStr">
         <is>
@@ -10215,13 +10215,13 @@
         <v>45010</v>
       </c>
       <c r="G98">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="H98" s="2">
         <v>45194</v>
       </c>
       <c r="I98">
-        <v>-2</v>
+        <v>-3</v>
       </c>
       <c r="J98" t="inlineStr">
         <is>
@@ -10313,13 +10313,13 @@
         <v>45093</v>
       </c>
       <c r="G99">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="H99" s="2">
         <v>45276</v>
       </c>
       <c r="I99">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="J99" t="inlineStr">
         <is>
@@ -10416,13 +10416,13 @@
         <v>45123</v>
       </c>
       <c r="G100">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="H100" s="2">
         <v>45307</v>
       </c>
       <c r="I100">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="J100" t="inlineStr">
         <is>
@@ -10519,13 +10519,13 @@
         <v>45014</v>
       </c>
       <c r="G101">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="H101" s="2">
         <v>45198</v>
       </c>
       <c r="I101">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J101" t="inlineStr">
         <is>
@@ -10622,13 +10622,13 @@
         <v>45093</v>
       </c>
       <c r="G102">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="H102" s="2">
         <v>45276</v>
       </c>
       <c r="I102">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="J102" t="inlineStr">
         <is>
@@ -10725,13 +10725,13 @@
         <v>45122</v>
       </c>
       <c r="G103">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="H103" s="2">
         <v>45306</v>
       </c>
       <c r="I103">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="J103" t="inlineStr">
         <is>
@@ -10828,13 +10828,13 @@
         <v>45122</v>
       </c>
       <c r="G104">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="H104" s="2">
         <v>45306</v>
       </c>
       <c r="I104">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="J104" t="inlineStr">
         <is>
@@ -10926,13 +10926,13 @@
         <v>45050</v>
       </c>
       <c r="G105">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="H105" s="2">
         <v>45234</v>
       </c>
       <c r="I105">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="J105" t="inlineStr">
         <is>
@@ -11029,13 +11029,13 @@
         <v>45085</v>
       </c>
       <c r="G106">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="H106" s="2">
         <v>45268</v>
       </c>
       <c r="I106">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="J106" t="inlineStr">
         <is>
@@ -11132,13 +11132,13 @@
         <v>45093</v>
       </c>
       <c r="G107">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="H107" s="2">
         <v>45185</v>
       </c>
       <c r="I107">
-        <v>-11</v>
+        <v>-12</v>
       </c>
       <c r="J107" t="inlineStr">
         <is>
@@ -11230,13 +11230,13 @@
         <v>45093</v>
       </c>
       <c r="G108">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="H108" s="2">
         <v>45185</v>
       </c>
       <c r="I108">
-        <v>-11</v>
+        <v>-12</v>
       </c>
       <c r="J108" t="inlineStr">
         <is>
@@ -11328,13 +11328,13 @@
         <v>45093</v>
       </c>
       <c r="G109">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="H109" s="2">
         <v>45185</v>
       </c>
       <c r="I109">
-        <v>-11</v>
+        <v>-12</v>
       </c>
       <c r="J109" t="inlineStr">
         <is>
@@ -11431,13 +11431,13 @@
         <v>45148</v>
       </c>
       <c r="G110">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="H110" s="2">
         <v>45240</v>
       </c>
       <c r="I110">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="J110" t="inlineStr">
         <is>
@@ -11534,13 +11534,13 @@
         <v>45119</v>
       </c>
       <c r="G111">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="H111" s="2">
         <v>45211</v>
       </c>
       <c r="I111">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="J111" t="inlineStr">
         <is>
@@ -11637,13 +11637,13 @@
         <v>45172</v>
       </c>
       <c r="G112">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="H112" s="2">
         <v>45263</v>
       </c>
       <c r="I112">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="J112" t="inlineStr">
         <is>
@@ -11740,13 +11740,13 @@
         <v>45023</v>
       </c>
       <c r="G113">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="H113" s="2">
         <v>45206</v>
       </c>
       <c r="I113">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="J113" t="inlineStr">
         <is>
@@ -11843,13 +11843,13 @@
         <v>45111</v>
       </c>
       <c r="G114">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="H114" s="2">
         <v>45203</v>
       </c>
       <c r="I114">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="J114" t="inlineStr">
         <is>
@@ -11946,7 +11946,7 @@
         <v>45218</v>
       </c>
       <c r="I115">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="J115" t="inlineStr">
         <is>
@@ -12043,13 +12043,13 @@
         <v>45161</v>
       </c>
       <c r="G116">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="H116" s="2">
         <v>45253</v>
       </c>
       <c r="I116">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="J116" t="inlineStr">
         <is>
@@ -12146,13 +12146,13 @@
         <v>45115</v>
       </c>
       <c r="G117">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="H117" s="2">
         <v>45299</v>
       </c>
       <c r="I117">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="J117" t="inlineStr">
         <is>
@@ -12244,13 +12244,13 @@
         <v>45094</v>
       </c>
       <c r="G118">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="H118" s="2">
         <v>45277</v>
       </c>
       <c r="I118">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="J118" t="inlineStr">
         <is>
@@ -12347,13 +12347,13 @@
         <v>45104</v>
       </c>
       <c r="G119">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="H119" s="2">
         <v>45287</v>
       </c>
       <c r="I119">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="J119" t="inlineStr">
         <is>
@@ -12450,13 +12450,13 @@
         <v>45104</v>
       </c>
       <c r="G120">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="H120" s="2">
         <v>45287</v>
       </c>
       <c r="I120">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="J120" t="inlineStr">
         <is>
@@ -12553,13 +12553,13 @@
         <v>45104</v>
       </c>
       <c r="G121">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="H121" s="2">
         <v>45287</v>
       </c>
       <c r="I121">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="J121" t="inlineStr">
         <is>
@@ -12656,13 +12656,13 @@
         <v>45104</v>
       </c>
       <c r="G122">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="H122" s="2">
         <v>45287</v>
       </c>
       <c r="I122">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="J122" t="inlineStr">
         <is>
@@ -12759,13 +12759,13 @@
         <v>45107</v>
       </c>
       <c r="G123">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="H123" s="2">
         <v>45199</v>
       </c>
       <c r="I123">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="J123" t="inlineStr">
         <is>
@@ -12862,13 +12862,13 @@
         <v>45013</v>
       </c>
       <c r="G124">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="H124" s="2">
         <v>45197</v>
       </c>
       <c r="I124">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J124" t="inlineStr">
         <is>
@@ -12965,13 +12965,13 @@
         <v>45121</v>
       </c>
       <c r="G125">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="H125" s="2">
         <v>45213</v>
       </c>
       <c r="I125">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="J125" t="inlineStr">
         <is>
@@ -13068,13 +13068,13 @@
         <v>45134</v>
       </c>
       <c r="G126">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="H126" s="2">
         <v>45226</v>
       </c>
       <c r="I126">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="J126" t="inlineStr">
         <is>
@@ -13171,7 +13171,7 @@
         <v>45212</v>
       </c>
       <c r="I127">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="J127" t="inlineStr">
         <is>
@@ -13268,13 +13268,13 @@
         <v>45126</v>
       </c>
       <c r="G128">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="H128" s="2">
         <v>45218</v>
       </c>
       <c r="I128">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="J128" t="inlineStr">
         <is>
@@ -13366,13 +13366,13 @@
         <v>45158</v>
       </c>
       <c r="G129">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="H129" s="2">
         <v>45250</v>
       </c>
       <c r="I129">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="J129" t="inlineStr">
         <is>
@@ -13469,13 +13469,13 @@
         <v>45171</v>
       </c>
       <c r="G130">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="H130" s="2">
         <v>45262</v>
       </c>
       <c r="I130">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="J130" t="inlineStr">
         <is>
@@ -13572,13 +13572,13 @@
         <v>45111</v>
       </c>
       <c r="G131">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="H131" s="2">
         <v>45203</v>
       </c>
       <c r="I131">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="J131" t="inlineStr">
         <is>
@@ -13675,13 +13675,13 @@
         <v>45144</v>
       </c>
       <c r="G132">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="H132" s="2">
         <v>45236</v>
       </c>
       <c r="I132">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="J132" t="inlineStr">
         <is>
@@ -13778,13 +13778,13 @@
         <v>45156</v>
       </c>
       <c r="G133">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="H133" s="2">
         <v>45248</v>
       </c>
       <c r="I133">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="J133" t="inlineStr">
         <is>
@@ -13876,13 +13876,13 @@
         <v>45146</v>
       </c>
       <c r="G134">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="H134" s="2">
         <v>45238</v>
       </c>
       <c r="I134">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="J134" t="inlineStr">
         <is>
@@ -13979,13 +13979,13 @@
         <v>45140</v>
       </c>
       <c r="G135">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="H135" s="2">
         <v>45232</v>
       </c>
       <c r="I135">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="J135" t="inlineStr">
         <is>
@@ -14082,13 +14082,13 @@
         <v>45104</v>
       </c>
       <c r="G136">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="H136" s="2">
         <v>45196</v>
       </c>
       <c r="I136">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="J136" t="inlineStr">
         <is>
@@ -14185,13 +14185,13 @@
         <v>45105</v>
       </c>
       <c r="G137">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="H137" s="2">
         <v>45197</v>
       </c>
       <c r="I137">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J137" t="inlineStr">
         <is>
@@ -14288,13 +14288,13 @@
         <v>45179</v>
       </c>
       <c r="G138">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="H138" s="2">
         <v>45270</v>
       </c>
       <c r="I138">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="J138" t="inlineStr">
         <is>
@@ -14386,13 +14386,13 @@
         <v>45105</v>
       </c>
       <c r="G139">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="H139" s="2">
         <v>45197</v>
       </c>
       <c r="I139">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J139" t="inlineStr">
         <is>
@@ -14489,13 +14489,13 @@
         <v>45182</v>
       </c>
       <c r="G140">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="H140" s="2">
         <v>45273</v>
       </c>
       <c r="I140">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="J140" t="inlineStr">
         <is>
@@ -14592,13 +14592,13 @@
         <v>45116</v>
       </c>
       <c r="G141">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="H141" s="2">
         <v>45208</v>
       </c>
       <c r="I141">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="J141" t="inlineStr">
         <is>
@@ -14690,13 +14690,13 @@
         <v>45150</v>
       </c>
       <c r="G142">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="H142" s="2">
         <v>45242</v>
       </c>
       <c r="I142">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="J142" t="inlineStr">
         <is>
@@ -14793,7 +14793,7 @@
         <v>45238</v>
       </c>
       <c r="I143">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="J143" t="inlineStr">
         <is>
@@ -14890,13 +14890,13 @@
         <v>45171</v>
       </c>
       <c r="G144">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="H144" s="2">
         <v>45262</v>
       </c>
       <c r="I144">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="J144" t="inlineStr">
         <is>
@@ -14993,13 +14993,13 @@
         <v>45102</v>
       </c>
       <c r="G145">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="H145" s="2">
         <v>45194</v>
       </c>
       <c r="I145">
-        <v>-2</v>
+        <v>-3</v>
       </c>
       <c r="J145" t="inlineStr">
         <is>
@@ -15086,13 +15086,13 @@
         <v>45119</v>
       </c>
       <c r="G146">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="H146" s="2">
         <v>45211</v>
       </c>
       <c r="I146">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="J146" t="inlineStr">
         <is>
@@ -15189,13 +15189,13 @@
         <v>45165</v>
       </c>
       <c r="G147">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="H147" s="2">
         <v>45257</v>
       </c>
       <c r="I147">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="J147" t="inlineStr">
         <is>
@@ -15292,13 +15292,13 @@
         <v>45166</v>
       </c>
       <c r="G148">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="H148" s="2">
         <v>45258</v>
       </c>
       <c r="I148">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="J148" t="inlineStr">
         <is>
@@ -15395,13 +15395,13 @@
         <v>45093</v>
       </c>
       <c r="G149">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="H149" s="2">
         <v>45185</v>
       </c>
       <c r="I149">
-        <v>-11</v>
+        <v>-12</v>
       </c>
       <c r="J149" t="inlineStr">
         <is>
@@ -15498,13 +15498,13 @@
         <v>45035</v>
       </c>
       <c r="G150">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="H150" s="2">
         <v>45218</v>
       </c>
       <c r="I150">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="J150" t="inlineStr">
         <is>
@@ -15601,13 +15601,13 @@
         <v>45174</v>
       </c>
       <c r="G151">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="H151" s="2">
         <v>45356</v>
       </c>
       <c r="I151">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="J151" t="inlineStr">
         <is>
@@ -15704,13 +15704,13 @@
         <v>45089</v>
       </c>
       <c r="G152">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="H152" s="2">
         <v>45272</v>
       </c>
       <c r="I152">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="J152" t="inlineStr">
         <is>
@@ -15807,13 +15807,13 @@
         <v>45124</v>
       </c>
       <c r="G153">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="H153" s="2">
         <v>45308</v>
       </c>
       <c r="I153">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="J153" t="inlineStr">
         <is>
@@ -15910,13 +15910,13 @@
         <v>45124</v>
       </c>
       <c r="G154">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="H154" s="2">
         <v>45308</v>
       </c>
       <c r="I154">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="J154" t="inlineStr">
         <is>
@@ -16013,13 +16013,13 @@
         <v>45026</v>
       </c>
       <c r="G155">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="H155" s="2">
         <v>45209</v>
       </c>
       <c r="I155">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="J155" t="inlineStr">
         <is>
@@ -16116,13 +16116,13 @@
         <v>45026</v>
       </c>
       <c r="G156">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="H156" s="2">
         <v>45209</v>
       </c>
       <c r="I156">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="J156" t="inlineStr">
         <is>
@@ -16219,13 +16219,13 @@
         <v>45026</v>
       </c>
       <c r="G157">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="H157" s="2">
         <v>45209</v>
       </c>
       <c r="I157">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="J157" t="inlineStr">
         <is>
@@ -16322,13 +16322,13 @@
         <v>45026</v>
       </c>
       <c r="G158">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="H158" s="2">
         <v>45209</v>
       </c>
       <c r="I158">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="J158" t="inlineStr">
         <is>
@@ -16425,13 +16425,13 @@
         <v>45156</v>
       </c>
       <c r="G159">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="H159" s="2">
         <v>45247</v>
       </c>
       <c r="I159">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="J159" t="inlineStr">
         <is>
@@ -16528,13 +16528,13 @@
         <v>45153</v>
       </c>
       <c r="G160">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="H160" s="2">
         <v>45245</v>
       </c>
       <c r="I160">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="J160" t="inlineStr">
         <is>
@@ -16631,13 +16631,13 @@
         <v>45135</v>
       </c>
       <c r="G161">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="H161" s="2">
         <v>45319</v>
       </c>
       <c r="I161">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="J161" t="inlineStr">
         <is>
@@ -16734,13 +16734,13 @@
         <v>45091</v>
       </c>
       <c r="G162">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="H162" s="2">
         <v>45274</v>
       </c>
       <c r="I162">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="J162" t="inlineStr">
         <is>
@@ -16832,13 +16832,13 @@
         <v>45091</v>
       </c>
       <c r="G163">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="H163" s="2">
         <v>45274</v>
       </c>
       <c r="I163">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="J163" t="inlineStr">
         <is>
@@ -16930,13 +16930,13 @@
         <v>45138</v>
       </c>
       <c r="G164">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="H164" s="2">
         <v>45322</v>
       </c>
       <c r="I164">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="J164" t="inlineStr">
         <is>
@@ -17033,13 +17033,13 @@
         <v>45138</v>
       </c>
       <c r="G165">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="H165" s="2">
         <v>45322</v>
       </c>
       <c r="I165">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="J165" t="inlineStr">
         <is>
@@ -17136,13 +17136,13 @@
         <v>45085</v>
       </c>
       <c r="G166">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="H166" s="2">
         <v>45268</v>
       </c>
       <c r="I166">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="J166" t="inlineStr">
         <is>
@@ -17239,13 +17239,13 @@
         <v>45085</v>
       </c>
       <c r="G167">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="H167" s="2">
         <v>45268</v>
       </c>
       <c r="I167">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="J167" t="inlineStr">
         <is>
@@ -17342,7 +17342,7 @@
         <v>45326</v>
       </c>
       <c r="I168">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="J168" t="inlineStr">
         <is>
@@ -17439,13 +17439,13 @@
         <v>45173</v>
       </c>
       <c r="G169">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="H169" s="2">
         <v>45355</v>
       </c>
       <c r="I169">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="J169" t="inlineStr">
         <is>
@@ -17542,13 +17542,13 @@
         <v>45056</v>
       </c>
       <c r="G170">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="H170" s="2">
         <v>45240</v>
       </c>
       <c r="I170">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="J170" t="inlineStr">
         <is>
@@ -17645,7 +17645,7 @@
         <v>45238</v>
       </c>
       <c r="I171">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="J171" t="inlineStr">
         <is>
@@ -17742,13 +17742,13 @@
         <v>45141</v>
       </c>
       <c r="G172">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="H172" s="2">
         <v>45325</v>
       </c>
       <c r="I172">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="J172" t="inlineStr">
         <is>
@@ -17845,13 +17845,13 @@
         <v>45037</v>
       </c>
       <c r="G173">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="H173" s="2">
         <v>45220</v>
       </c>
       <c r="I173">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="J173" t="inlineStr">
         <is>
@@ -17948,13 +17948,13 @@
         <v>45171</v>
       </c>
       <c r="G174">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="H174" s="2">
         <v>45262</v>
       </c>
       <c r="I174">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="J174" t="inlineStr">
         <is>
@@ -18051,13 +18051,13 @@
         <v>45105</v>
       </c>
       <c r="G175">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="H175" s="2">
         <v>45197</v>
       </c>
       <c r="I175">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J175" t="inlineStr">
         <is>
@@ -18154,13 +18154,13 @@
         <v>45162</v>
       </c>
       <c r="G176">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="H176" s="2">
         <v>45254</v>
       </c>
       <c r="I176">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="J176" t="inlineStr">
         <is>
@@ -18257,13 +18257,13 @@
         <v>45061</v>
       </c>
       <c r="G177">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="H177" s="2">
         <v>45245</v>
       </c>
       <c r="I177">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="J177" t="inlineStr">
         <is>
@@ -18360,13 +18360,13 @@
         <v>45120</v>
       </c>
       <c r="G178">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="H178" s="2">
         <v>45212</v>
       </c>
       <c r="I178">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="J178" t="inlineStr">
         <is>
@@ -18463,7 +18463,7 @@
         <v>45191</v>
       </c>
       <c r="I179">
-        <v>-5</v>
+        <v>-6</v>
       </c>
       <c r="J179" t="inlineStr">
         <is>
@@ -18560,13 +18560,13 @@
         <v>45088</v>
       </c>
       <c r="G180">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="H180" s="2">
         <v>45271</v>
       </c>
       <c r="I180">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="J180" t="inlineStr">
         <is>
@@ -18663,13 +18663,13 @@
         <v>45100</v>
       </c>
       <c r="G181">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="H181" s="2">
         <v>45192</v>
       </c>
       <c r="I181">
-        <v>-4</v>
+        <v>-5</v>
       </c>
       <c r="J181" t="inlineStr">
         <is>
@@ -18756,13 +18756,13 @@
         <v>45131</v>
       </c>
       <c r="G182">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="H182" s="2">
         <v>45223</v>
       </c>
       <c r="I182">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="J182" t="inlineStr">
         <is>
@@ -18854,13 +18854,13 @@
         <v>45136</v>
       </c>
       <c r="G183">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="H183" s="2">
         <v>45228</v>
       </c>
       <c r="I183">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="J183" t="inlineStr">
         <is>
@@ -18952,13 +18952,13 @@
         <v>45150</v>
       </c>
       <c r="G184">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="H184" s="2">
         <v>45242</v>
       </c>
       <c r="I184">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="J184" t="inlineStr">
         <is>
@@ -19050,13 +19050,13 @@
         <v>45118</v>
       </c>
       <c r="G185">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="H185" s="2">
         <v>45210</v>
       </c>
       <c r="I185">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="J185" t="inlineStr">
         <is>
@@ -19148,13 +19148,13 @@
         <v>45129</v>
       </c>
       <c r="G186">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="H186" s="2">
         <v>45221</v>
       </c>
       <c r="I186">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="J186" t="inlineStr">
         <is>
@@ -19246,13 +19246,13 @@
         <v>45097</v>
       </c>
       <c r="G187">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="H187" s="2">
         <v>45189</v>
       </c>
       <c r="I187">
-        <v>-7</v>
+        <v>-8</v>
       </c>
       <c r="J187" t="inlineStr">
         <is>
@@ -19339,13 +19339,13 @@
         <v>45101</v>
       </c>
       <c r="G188">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="H188" s="2">
         <v>45193</v>
       </c>
       <c r="I188">
-        <v>-3</v>
+        <v>-4</v>
       </c>
       <c r="J188" t="inlineStr">
         <is>
@@ -19432,13 +19432,13 @@
         <v>45165</v>
       </c>
       <c r="G189">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="H189" s="2">
         <v>45257</v>
       </c>
       <c r="I189">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="J189" t="inlineStr">
         <is>
@@ -19530,7 +19530,7 @@
         <v>45202</v>
       </c>
       <c r="I190">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="J190" t="inlineStr">
         <is>
@@ -19627,13 +19627,13 @@
         <v>45081</v>
       </c>
       <c r="G191">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="H191" s="2">
         <v>45264</v>
       </c>
       <c r="I191">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="J191" t="inlineStr">
         <is>
@@ -19730,13 +19730,13 @@
         <v>45081</v>
       </c>
       <c r="G192">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="H192" s="2">
         <v>45264</v>
       </c>
       <c r="I192">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="J192" t="inlineStr">
         <is>
@@ -19833,7 +19833,7 @@
         <v>45319</v>
       </c>
       <c r="I193">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="J193" t="inlineStr">
         <is>
@@ -19930,7 +19930,7 @@
         <v>45319</v>
       </c>
       <c r="I194">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="J194" t="inlineStr">
         <is>
@@ -20022,13 +20022,13 @@
         <v>45046</v>
       </c>
       <c r="G195">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="H195" s="2">
         <v>45230</v>
       </c>
       <c r="I195">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="J195" t="inlineStr">
         <is>
@@ -20125,13 +20125,13 @@
         <v>45046</v>
       </c>
       <c r="G196">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="H196" s="2">
         <v>45230</v>
       </c>
       <c r="I196">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="J196" t="inlineStr">
         <is>
@@ -20228,13 +20228,13 @@
         <v>45031</v>
       </c>
       <c r="G197">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="H197" s="2">
         <v>45214</v>
       </c>
       <c r="I197">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="J197" t="inlineStr">
         <is>
@@ -20331,13 +20331,13 @@
         <v>45031</v>
       </c>
       <c r="G198">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="H198" s="2">
         <v>45214</v>
       </c>
       <c r="I198">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="J198" t="inlineStr">
         <is>
@@ -20434,13 +20434,13 @@
         <v>45031</v>
       </c>
       <c r="G199">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="H199" s="2">
         <v>45214</v>
       </c>
       <c r="I199">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="J199" t="inlineStr">
         <is>
@@ -20537,13 +20537,13 @@
         <v>45031</v>
       </c>
       <c r="G200">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="H200" s="2">
         <v>45214</v>
       </c>
       <c r="I200">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="J200" t="inlineStr">
         <is>
@@ -20640,13 +20640,13 @@
         <v>45067</v>
       </c>
       <c r="G201">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="H201" s="2">
         <v>45251</v>
       </c>
       <c r="I201">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="J201" t="inlineStr">
         <is>
@@ -20743,13 +20743,13 @@
         <v>45067</v>
       </c>
       <c r="G202">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="H202" s="2">
         <v>45251</v>
       </c>
       <c r="I202">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="J202" t="inlineStr">
         <is>
@@ -20846,13 +20846,13 @@
         <v>45067</v>
       </c>
       <c r="G203">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="H203" s="2">
         <v>45251</v>
       </c>
       <c r="I203">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="J203" t="inlineStr">
         <is>
@@ -20949,13 +20949,13 @@
         <v>45067</v>
       </c>
       <c r="G204">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="H204" s="2">
         <v>45251</v>
       </c>
       <c r="I204">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="J204" t="inlineStr">
         <is>
@@ -21052,13 +21052,13 @@
         <v>45178</v>
       </c>
       <c r="G205">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="H205" s="2">
         <v>45269</v>
       </c>
       <c r="I205">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="J205" t="inlineStr">
         <is>
@@ -21155,7 +21155,7 @@
         <v>45252</v>
       </c>
       <c r="I206">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="J206" t="inlineStr">
         <is>
@@ -21252,13 +21252,13 @@
         <v>45087</v>
       </c>
       <c r="G207">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="H207" s="2">
         <v>45270</v>
       </c>
       <c r="I207">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="J207" t="inlineStr">
         <is>
@@ -21355,13 +21355,13 @@
         <v>45099</v>
       </c>
       <c r="G208">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="H208" s="2">
         <v>45282</v>
       </c>
       <c r="I208">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="J208" t="inlineStr">
         <is>
@@ -21458,13 +21458,13 @@
         <v>45175</v>
       </c>
       <c r="G209">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="H209" s="2">
         <v>45356</v>
       </c>
       <c r="I209">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="J209" t="inlineStr">
         <is>
@@ -21561,13 +21561,13 @@
         <v>45175</v>
       </c>
       <c r="G210">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="H210" s="2">
         <v>45356</v>
       </c>
       <c r="I210">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="J210" t="inlineStr">
         <is>
@@ -21664,13 +21664,13 @@
         <v>45166</v>
       </c>
       <c r="G211">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="H211" s="2">
         <v>45350</v>
       </c>
       <c r="I211">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="J211" t="inlineStr">
         <is>
@@ -21767,13 +21767,13 @@
         <v>45166</v>
       </c>
       <c r="G212">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="H212" s="2">
         <v>45350</v>
       </c>
       <c r="I212">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="J212" t="inlineStr">
         <is>
@@ -21870,13 +21870,13 @@
         <v>45090</v>
       </c>
       <c r="G213">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="H213" s="2">
         <v>45273</v>
       </c>
       <c r="I213">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="J213" t="inlineStr">
         <is>
@@ -21973,13 +21973,13 @@
         <v>45106</v>
       </c>
       <c r="G214">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="H214" s="2">
         <v>45289</v>
       </c>
       <c r="I214">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="J214" t="inlineStr">
         <is>
@@ -22076,13 +22076,13 @@
         <v>45134</v>
       </c>
       <c r="G215">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="H215" s="2">
         <v>45226</v>
       </c>
       <c r="I215">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="J215" t="inlineStr">
         <is>
@@ -22179,13 +22179,13 @@
         <v>45132</v>
       </c>
       <c r="G216">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="H216" s="2">
         <v>45224</v>
       </c>
       <c r="I216">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="J216" t="inlineStr">
         <is>
@@ -22282,13 +22282,13 @@
         <v>45150</v>
       </c>
       <c r="G217">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="H217" s="2">
         <v>45242</v>
       </c>
       <c r="I217">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="J217" t="inlineStr">
         <is>
@@ -22385,13 +22385,13 @@
         <v>45095</v>
       </c>
       <c r="G218">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="H218" s="2">
         <v>45187</v>
       </c>
       <c r="I218">
-        <v>-9</v>
+        <v>-10</v>
       </c>
       <c r="J218" t="inlineStr">
         <is>
@@ -22483,13 +22483,13 @@
         <v>45182</v>
       </c>
       <c r="G219">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="H219" s="2">
         <v>45273</v>
       </c>
       <c r="I219">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="J219" t="inlineStr">
         <is>
@@ -22586,7 +22586,7 @@
         <v>45196</v>
       </c>
       <c r="I220">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="J220" t="inlineStr">
         <is>
@@ -22683,13 +22683,13 @@
         <v>45108</v>
       </c>
       <c r="G221">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="H221" s="2">
         <v>45200</v>
       </c>
       <c r="I221">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="J221" t="inlineStr">
         <is>
@@ -22786,13 +22786,13 @@
         <v>45135</v>
       </c>
       <c r="G222">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="H222" s="2">
         <v>45227</v>
       </c>
       <c r="I222">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="J222" t="inlineStr">
         <is>
@@ -22889,13 +22889,13 @@
         <v>45148</v>
       </c>
       <c r="G223">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="H223" s="2">
         <v>45240</v>
       </c>
       <c r="I223">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="J223" t="inlineStr">
         <is>
@@ -22987,13 +22987,13 @@
         <v>45100</v>
       </c>
       <c r="G224">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="H224" s="2">
         <v>45192</v>
       </c>
       <c r="I224">
-        <v>-4</v>
+        <v>-5</v>
       </c>
       <c r="J224" t="inlineStr">
         <is>
@@ -23085,13 +23085,13 @@
         <v>45136</v>
       </c>
       <c r="G225">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="H225" s="2">
         <v>45320</v>
       </c>
       <c r="I225">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="J225" t="inlineStr">
         <is>
@@ -23188,13 +23188,13 @@
         <v>45136</v>
       </c>
       <c r="G226">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="H226" s="2">
         <v>45320</v>
       </c>
       <c r="I226">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="J226" t="inlineStr">
         <is>
@@ -23291,13 +23291,13 @@
         <v>45094</v>
       </c>
       <c r="G227">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="H227" s="2">
         <v>45277</v>
       </c>
       <c r="I227">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="J227" t="inlineStr">
         <is>
@@ -23394,13 +23394,13 @@
         <v>45081</v>
       </c>
       <c r="G228">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="H228" s="2">
         <v>45264</v>
       </c>
       <c r="I228">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="J228" t="inlineStr">
         <is>
@@ -23497,13 +23497,13 @@
         <v>45099</v>
       </c>
       <c r="G229">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="H229" s="2">
         <v>45282</v>
       </c>
       <c r="I229">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="J229" t="inlineStr">
         <is>
@@ -23600,13 +23600,13 @@
         <v>45018</v>
       </c>
       <c r="G230">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="H230" s="2">
         <v>45201</v>
       </c>
       <c r="I230">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="J230" t="inlineStr">
         <is>
@@ -23703,13 +23703,13 @@
         <v>45031</v>
       </c>
       <c r="G231">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="H231" s="2">
         <v>45214</v>
       </c>
       <c r="I231">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="J231" t="inlineStr">
         <is>
@@ -23806,7 +23806,7 @@
         <v>45294</v>
       </c>
       <c r="I232">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="J232" t="inlineStr">
         <is>
@@ -23903,13 +23903,13 @@
         <v>45079</v>
       </c>
       <c r="G233">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="H233" s="2">
         <v>45262</v>
       </c>
       <c r="I233">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="J233" t="inlineStr">
         <is>
@@ -24006,7 +24006,7 @@
         <v>45199</v>
       </c>
       <c r="I234">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="J234" t="inlineStr">
         <is>
@@ -24103,13 +24103,13 @@
         <v>45021</v>
       </c>
       <c r="G235">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="H235" s="2">
         <v>45204</v>
       </c>
       <c r="I235">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="J235" t="inlineStr">
         <is>
@@ -24206,13 +24206,13 @@
         <v>45021</v>
       </c>
       <c r="G236">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="H236" s="2">
         <v>45204</v>
       </c>
       <c r="I236">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="J236" t="inlineStr">
         <is>
@@ -24309,13 +24309,13 @@
         <v>45080</v>
       </c>
       <c r="G237">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="H237" s="2">
         <v>45263</v>
       </c>
       <c r="I237">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="J237" t="inlineStr">
         <is>
@@ -24412,13 +24412,13 @@
         <v>45046</v>
       </c>
       <c r="G238">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="H238" s="2">
         <v>45229</v>
       </c>
       <c r="I238">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="J238" t="inlineStr">
         <is>
@@ -24515,13 +24515,13 @@
         <v>45112</v>
       </c>
       <c r="G239">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="H239" s="2">
         <v>45204</v>
       </c>
       <c r="I239">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="J239" t="inlineStr">
         <is>
@@ -24609,13 +24609,13 @@
         <v>45112</v>
       </c>
       <c r="G240">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="H240" s="2">
         <v>45204</v>
       </c>
       <c r="I240">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="J240" t="inlineStr">
         <is>
@@ -24703,13 +24703,13 @@
         <v>45016</v>
       </c>
       <c r="G241">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="H241" s="2">
         <v>45199</v>
       </c>
       <c r="I241">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="J241" t="inlineStr">
         <is>
@@ -24806,13 +24806,13 @@
         <v>45070</v>
       </c>
       <c r="G242">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="H242" s="2">
         <v>45254</v>
       </c>
       <c r="I242">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="J242" t="inlineStr">
         <is>
@@ -24909,13 +24909,13 @@
         <v>45168</v>
       </c>
       <c r="G243">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="H243" s="2">
         <v>45260</v>
       </c>
       <c r="I243">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="J243" t="inlineStr">
         <is>
@@ -25012,13 +25012,13 @@
         <v>45027</v>
       </c>
       <c r="G244">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="H244" s="2">
         <v>45210</v>
       </c>
       <c r="I244">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="J244" t="inlineStr">
         <is>
@@ -25115,13 +25115,13 @@
         <v>45077</v>
       </c>
       <c r="G245">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="H245" s="2">
         <v>45260</v>
       </c>
       <c r="I245">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="J245" t="inlineStr">
         <is>
@@ -25218,13 +25218,13 @@
         <v>45100</v>
       </c>
       <c r="G246">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="H246" s="2">
         <v>45283</v>
       </c>
       <c r="I246">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="J246" t="inlineStr">
         <is>
@@ -25321,7 +25321,7 @@
         <v>45281</v>
       </c>
       <c r="I247">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="J247" t="inlineStr">
         <is>
@@ -25418,13 +25418,13 @@
         <v>45044</v>
       </c>
       <c r="G248">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="H248" s="2">
         <v>45227</v>
       </c>
       <c r="I248">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="J248" t="inlineStr">
         <is>
@@ -25521,13 +25521,13 @@
         <v>45101</v>
       </c>
       <c r="G249">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="H249" s="2">
         <v>45283</v>
       </c>
       <c r="I249">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="J249" t="inlineStr">
         <is>
@@ -25624,13 +25624,13 @@
         <v>45134</v>
       </c>
       <c r="G250">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="H250" s="2">
         <v>45226</v>
       </c>
       <c r="I250">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="J250" t="inlineStr">
         <is>
@@ -25727,13 +25727,13 @@
         <v>45158</v>
       </c>
       <c r="G251">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="H251" s="2">
         <v>45250</v>
       </c>
       <c r="I251">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="J251" t="inlineStr">
         <is>
@@ -25830,13 +25830,13 @@
         <v>45108</v>
       </c>
       <c r="G252">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="H252" s="2">
         <v>45200</v>
       </c>
       <c r="I252">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="J252" t="inlineStr">
         <is>
@@ -25933,7 +25933,7 @@
         <v>45317</v>
       </c>
       <c r="I253">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="J253" t="inlineStr">
         <is>
@@ -26030,13 +26030,13 @@
         <v>45039</v>
       </c>
       <c r="G254">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="H254" s="2">
         <v>45222</v>
       </c>
       <c r="I254">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="J254" t="inlineStr">
         <is>
@@ -26128,13 +26128,13 @@
         <v>45129</v>
       </c>
       <c r="G255">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="H255" s="2">
         <v>45221</v>
       </c>
       <c r="I255">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="J255" t="inlineStr">
         <is>
@@ -26231,13 +26231,13 @@
         <v>45157</v>
       </c>
       <c r="G256">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="H256" s="2">
         <v>45341</v>
       </c>
       <c r="I256">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="J256" t="inlineStr">
         <is>
@@ -26334,13 +26334,13 @@
         <v>45063</v>
       </c>
       <c r="G257">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="H257" s="2">
         <v>45247</v>
       </c>
       <c r="I257">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="J257" t="inlineStr">
         <is>
@@ -26437,7 +26437,7 @@
         <v>45254</v>
       </c>
       <c r="I258">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="J258" t="inlineStr">
         <is>
@@ -26534,7 +26534,7 @@
         <v>45486</v>
       </c>
       <c r="I259">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="J259" t="inlineStr">
         <is>
@@ -26626,13 +26626,13 @@
         <v>45073</v>
       </c>
       <c r="G260">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="H260" s="2">
         <v>45439</v>
       </c>
       <c r="I260">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="J260" t="inlineStr">
         <is>
@@ -26724,7 +26724,7 @@
         <v>45323</v>
       </c>
       <c r="I261">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="J261" t="inlineStr">
         <is>
@@ -26816,7 +26816,7 @@
         <v>45303</v>
       </c>
       <c r="I262">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="J262" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
Bond dates update Fri Sep 29 23:08:08 UTC 2023
</commit_message>
<xml_diff>
--- a/Data/obligacje_screener.xlsx
+++ b/Data/obligacje_screener.xlsx
@@ -512,7 +512,7 @@
         <v>45340</v>
       </c>
       <c r="I2">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="J2" t="inlineStr">
         <is>
@@ -600,13 +600,13 @@
         <v>45121</v>
       </c>
       <c r="G3">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="H3" s="2">
         <v>45305</v>
       </c>
       <c r="I3">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="J3" t="inlineStr">
         <is>
@@ -703,13 +703,13 @@
         <v>45039</v>
       </c>
       <c r="G4">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="H4" s="2">
         <v>45222</v>
       </c>
       <c r="I4">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="J4" t="inlineStr">
         <is>
@@ -806,13 +806,13 @@
         <v>45039</v>
       </c>
       <c r="G5">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="H5" s="2">
         <v>45222</v>
       </c>
       <c r="I5">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="J5" t="inlineStr">
         <is>
@@ -909,13 +909,13 @@
         <v>45129</v>
       </c>
       <c r="G6">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="H6" s="2">
         <v>45221</v>
       </c>
       <c r="I6">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="J6" t="inlineStr">
         <is>
@@ -1012,13 +1012,13 @@
         <v>45162</v>
       </c>
       <c r="G7">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="H7" s="2">
         <v>45254</v>
       </c>
       <c r="I7">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="J7" t="inlineStr">
         <is>
@@ -1110,13 +1110,13 @@
         <v>45156</v>
       </c>
       <c r="G8">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="H8" s="2">
         <v>45248</v>
       </c>
       <c r="I8">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="J8" t="inlineStr">
         <is>
@@ -1213,13 +1213,13 @@
         <v>45141</v>
       </c>
       <c r="G9">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="H9" s="2">
         <v>45233</v>
       </c>
       <c r="I9">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="J9" t="inlineStr">
         <is>
@@ -1316,13 +1316,13 @@
         <v>45062</v>
       </c>
       <c r="G10">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="H10" s="2">
         <v>45246</v>
       </c>
       <c r="I10">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="J10" t="inlineStr">
         <is>
@@ -1419,7 +1419,7 @@
         <v>45286</v>
       </c>
       <c r="I11">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="J11" t="inlineStr">
         <is>
@@ -1516,13 +1516,13 @@
         <v>45011</v>
       </c>
       <c r="G12">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="H12" s="2">
         <v>45195</v>
       </c>
       <c r="I12">
-        <v>-2</v>
+        <v>-3</v>
       </c>
       <c r="J12" t="inlineStr">
         <is>
@@ -1614,13 +1614,13 @@
         <v>45036</v>
       </c>
       <c r="G13">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="H13" s="2">
         <v>45219</v>
       </c>
       <c r="I13">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="J13" t="inlineStr">
         <is>
@@ -1717,13 +1717,13 @@
         <v>45036</v>
       </c>
       <c r="G14">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="H14" s="2">
         <v>45219</v>
       </c>
       <c r="I14">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="J14" t="inlineStr">
         <is>
@@ -1820,13 +1820,13 @@
         <v>45106</v>
       </c>
       <c r="G15">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="H15" s="2">
         <v>45289</v>
       </c>
       <c r="I15">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="J15" t="inlineStr">
         <is>
@@ -1923,13 +1923,13 @@
         <v>45094</v>
       </c>
       <c r="G16">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="H16" s="2">
         <v>45186</v>
       </c>
       <c r="I16">
-        <v>-11</v>
+        <v>-12</v>
       </c>
       <c r="J16" t="inlineStr">
         <is>
@@ -2026,13 +2026,13 @@
         <v>45094</v>
       </c>
       <c r="G17">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="H17" s="2">
         <v>45186</v>
       </c>
       <c r="I17">
-        <v>-11</v>
+        <v>-12</v>
       </c>
       <c r="J17" t="inlineStr">
         <is>
@@ -2129,13 +2129,13 @@
         <v>45132</v>
       </c>
       <c r="G18">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="H18" s="2">
         <v>45224</v>
       </c>
       <c r="I18">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="J18" t="inlineStr">
         <is>
@@ -2232,13 +2232,13 @@
         <v>45137</v>
       </c>
       <c r="G19">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="H19" s="2">
         <v>45229</v>
       </c>
       <c r="I19">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="J19" t="inlineStr">
         <is>
@@ -2330,13 +2330,13 @@
         <v>45183</v>
       </c>
       <c r="G20">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="H20" s="2">
         <v>45274</v>
       </c>
       <c r="I20">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="J20" t="inlineStr">
         <is>
@@ -2433,13 +2433,13 @@
         <v>45093</v>
       </c>
       <c r="G21">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="H21" s="2">
         <v>45187</v>
       </c>
       <c r="I21">
-        <v>-10</v>
+        <v>-11</v>
       </c>
       <c r="J21" t="inlineStr">
         <is>
@@ -2536,13 +2536,13 @@
         <v>45096</v>
       </c>
       <c r="G22">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="H22" s="2">
         <v>45187</v>
       </c>
       <c r="I22">
-        <v>-10</v>
+        <v>-11</v>
       </c>
       <c r="J22" t="inlineStr">
         <is>
@@ -2639,7 +2639,7 @@
         <v>45245</v>
       </c>
       <c r="I23">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="J23" t="inlineStr">
         <is>
@@ -2736,7 +2736,7 @@
         <v>45245</v>
       </c>
       <c r="I24">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="J24" t="inlineStr">
         <is>
@@ -2833,13 +2833,13 @@
         <v>45021</v>
       </c>
       <c r="G25">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="H25" s="2">
         <v>45204</v>
       </c>
       <c r="I25">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="J25" t="inlineStr">
         <is>
@@ -2936,13 +2936,13 @@
         <v>45160</v>
       </c>
       <c r="G26">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="H26" s="2">
         <v>45344</v>
       </c>
       <c r="I26">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="J26" t="inlineStr">
         <is>
@@ -3039,13 +3039,13 @@
         <v>45118</v>
       </c>
       <c r="G27">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="H27" s="2">
         <v>45302</v>
       </c>
       <c r="I27">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="J27" t="inlineStr">
         <is>
@@ -3142,13 +3142,13 @@
         <v>45085</v>
       </c>
       <c r="G28">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="H28" s="2">
         <v>45268</v>
       </c>
       <c r="I28">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="J28" t="inlineStr">
         <is>
@@ -3245,13 +3245,13 @@
         <v>45183</v>
       </c>
       <c r="G29">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="H29" s="2">
         <v>45274</v>
       </c>
       <c r="I29">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="J29" t="inlineStr">
         <is>
@@ -3348,7 +3348,7 @@
         <v>45224</v>
       </c>
       <c r="I30">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="J30" t="inlineStr">
         <is>
@@ -3445,13 +3445,13 @@
         <v>45153</v>
       </c>
       <c r="G31">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="H31" s="2">
         <v>45245</v>
       </c>
       <c r="I31">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="J31" t="inlineStr">
         <is>
@@ -3548,13 +3548,13 @@
         <v>45155</v>
       </c>
       <c r="G32">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="H32" s="2">
         <v>45247</v>
       </c>
       <c r="I32">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="J32" t="inlineStr">
         <is>
@@ -3651,7 +3651,7 @@
         <v>45255</v>
       </c>
       <c r="I33">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="J33" t="inlineStr">
         <is>
@@ -3739,13 +3739,13 @@
         <v>45176</v>
       </c>
       <c r="G34">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="H34" s="2">
         <v>45267</v>
       </c>
       <c r="I34">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="J34" t="inlineStr">
         <is>
@@ -3842,13 +3842,13 @@
         <v>45130</v>
       </c>
       <c r="G35">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="H35" s="2">
         <v>45222</v>
       </c>
       <c r="I35">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="J35" t="inlineStr">
         <is>
@@ -3940,13 +3940,13 @@
         <v>45115</v>
       </c>
       <c r="G36">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="H36" s="2">
         <v>45207</v>
       </c>
       <c r="I36">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="J36" t="inlineStr">
         <is>
@@ -4043,13 +4043,13 @@
         <v>45097</v>
       </c>
       <c r="G37">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="H37" s="2">
         <v>45189</v>
       </c>
       <c r="I37">
-        <v>-8</v>
+        <v>-9</v>
       </c>
       <c r="J37" t="inlineStr">
         <is>
@@ -4141,13 +4141,13 @@
         <v>45107</v>
       </c>
       <c r="G38">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="H38" s="2">
         <v>45290</v>
       </c>
       <c r="I38">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="J38" t="inlineStr">
         <is>
@@ -4244,13 +4244,13 @@
         <v>45063</v>
       </c>
       <c r="G39">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="H39" s="2">
         <v>45247</v>
       </c>
       <c r="I39">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="J39" t="inlineStr">
         <is>
@@ -4347,13 +4347,13 @@
         <v>45177</v>
       </c>
       <c r="G40">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="H40" s="2">
         <v>45359</v>
       </c>
       <c r="I40">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="J40" t="inlineStr">
         <is>
@@ -4450,13 +4450,13 @@
         <v>45107</v>
       </c>
       <c r="G41">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="H41" s="2">
         <v>45290</v>
       </c>
       <c r="I41">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="J41" t="inlineStr">
         <is>
@@ -4553,7 +4553,7 @@
         <v>45265</v>
       </c>
       <c r="I42">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="J42" t="inlineStr">
         <is>
@@ -4650,13 +4650,13 @@
         <v>45098</v>
       </c>
       <c r="G43">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="H43" s="2">
         <v>45281</v>
       </c>
       <c r="I43">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="J43" t="inlineStr">
         <is>
@@ -4753,13 +4753,13 @@
         <v>45099</v>
       </c>
       <c r="G44">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="H44" s="2">
         <v>45282</v>
       </c>
       <c r="I44">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="J44" t="inlineStr">
         <is>
@@ -4856,13 +4856,13 @@
         <v>45106</v>
       </c>
       <c r="G45">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="H45" s="2">
         <v>45289</v>
       </c>
       <c r="I45">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="J45" t="inlineStr">
         <is>
@@ -4959,13 +4959,13 @@
         <v>45106</v>
       </c>
       <c r="G46">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="H46" s="2">
         <v>45289</v>
       </c>
       <c r="I46">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="J46" t="inlineStr">
         <is>
@@ -5062,13 +5062,13 @@
         <v>45120</v>
       </c>
       <c r="G47">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="H47" s="2">
         <v>45304</v>
       </c>
       <c r="I47">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="J47" t="inlineStr">
         <is>
@@ -5165,13 +5165,13 @@
         <v>45118</v>
       </c>
       <c r="G48">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="H48" s="2">
         <v>45302</v>
       </c>
       <c r="I48">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="J48" t="inlineStr">
         <is>
@@ -5268,13 +5268,13 @@
         <v>45152</v>
       </c>
       <c r="G49">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="H49" s="2">
         <v>45336</v>
       </c>
       <c r="I49">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="J49" t="inlineStr">
         <is>
@@ -5371,13 +5371,13 @@
         <v>45042</v>
       </c>
       <c r="G50">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="H50" s="2">
         <v>45225</v>
       </c>
       <c r="I50">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="J50" t="inlineStr">
         <is>
@@ -5474,13 +5474,13 @@
         <v>45122</v>
       </c>
       <c r="G51">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="H51" s="2">
         <v>45306</v>
       </c>
       <c r="I51">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="J51" t="inlineStr">
         <is>
@@ -5577,13 +5577,13 @@
         <v>45139</v>
       </c>
       <c r="G52">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="H52" s="2">
         <v>45323</v>
       </c>
       <c r="I52">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="J52" t="inlineStr">
         <is>
@@ -5671,13 +5671,13 @@
         <v>45099</v>
       </c>
       <c r="G53">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="H53" s="2">
         <v>45282</v>
       </c>
       <c r="I53">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="J53" t="inlineStr">
         <is>
@@ -5774,7 +5774,7 @@
         <v>45196</v>
       </c>
       <c r="I54">
-        <v>-1</v>
+        <v>-2</v>
       </c>
       <c r="J54" t="inlineStr">
         <is>
@@ -5871,13 +5871,13 @@
         <v>45044</v>
       </c>
       <c r="G55">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="H55" s="2">
         <v>45227</v>
       </c>
       <c r="I55">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="J55" t="inlineStr">
         <is>
@@ -5974,13 +5974,13 @@
         <v>45151</v>
       </c>
       <c r="G56">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="H56" s="2">
         <v>45243</v>
       </c>
       <c r="I56">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="J56" t="inlineStr">
         <is>
@@ -6072,7 +6072,7 @@
         <v>45196</v>
       </c>
       <c r="I57">
-        <v>-1</v>
+        <v>-2</v>
       </c>
       <c r="J57" t="inlineStr">
         <is>
@@ -6169,13 +6169,13 @@
         <v>45069</v>
       </c>
       <c r="G58">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="H58" s="2">
         <v>45253</v>
       </c>
       <c r="I58">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="J58" t="inlineStr">
         <is>
@@ -6272,13 +6272,13 @@
         <v>45099</v>
       </c>
       <c r="G59">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="H59" s="2">
         <v>45191</v>
       </c>
       <c r="I59">
-        <v>-6</v>
+        <v>-7</v>
       </c>
       <c r="J59" t="inlineStr">
         <is>
@@ -6370,13 +6370,13 @@
         <v>45113</v>
       </c>
       <c r="G60">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="H60" s="2">
         <v>45205</v>
       </c>
       <c r="I60">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="J60" t="inlineStr">
         <is>
@@ -6473,13 +6473,13 @@
         <v>45127</v>
       </c>
       <c r="G61">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="H61" s="2">
         <v>45219</v>
       </c>
       <c r="I61">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="J61" t="inlineStr">
         <is>
@@ -6576,13 +6576,13 @@
         <v>45058</v>
       </c>
       <c r="G62">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="H62" s="2">
         <v>45242</v>
       </c>
       <c r="I62">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="J62" t="inlineStr">
         <is>
@@ -6679,13 +6679,13 @@
         <v>45010</v>
       </c>
       <c r="G63">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="H63" s="2">
         <v>45194</v>
       </c>
       <c r="I63">
-        <v>-3</v>
+        <v>-4</v>
       </c>
       <c r="J63" t="inlineStr">
         <is>
@@ -6777,13 +6777,13 @@
         <v>45025</v>
       </c>
       <c r="G64">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="H64" s="2">
         <v>45208</v>
       </c>
       <c r="I64">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="J64" t="inlineStr">
         <is>
@@ -6880,13 +6880,13 @@
         <v>45025</v>
       </c>
       <c r="G65">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="H65" s="2">
         <v>45208</v>
       </c>
       <c r="I65">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="J65" t="inlineStr">
         <is>
@@ -6983,13 +6983,13 @@
         <v>45089</v>
       </c>
       <c r="G66">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="H66" s="2">
         <v>45272</v>
       </c>
       <c r="I66">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="J66" t="inlineStr">
         <is>
@@ -7086,13 +7086,13 @@
         <v>45178</v>
       </c>
       <c r="G67">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="H67" s="2">
         <v>45269</v>
       </c>
       <c r="I67">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="J67" t="inlineStr">
         <is>
@@ -7184,13 +7184,13 @@
         <v>45104</v>
       </c>
       <c r="G68">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="H68" s="2">
         <v>45196</v>
       </c>
       <c r="I68">
-        <v>-1</v>
+        <v>-2</v>
       </c>
       <c r="J68" t="inlineStr">
         <is>
@@ -7287,13 +7287,13 @@
         <v>45149</v>
       </c>
       <c r="G69">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="H69" s="2">
         <v>45241</v>
       </c>
       <c r="I69">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="J69" t="inlineStr">
         <is>
@@ -7390,7 +7390,7 @@
         <v>45205</v>
       </c>
       <c r="I70">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="J70" t="inlineStr">
         <is>
@@ -7487,13 +7487,13 @@
         <v>45114</v>
       </c>
       <c r="G71">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="H71" s="2">
         <v>45205</v>
       </c>
       <c r="I71">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="J71" t="inlineStr">
         <is>
@@ -7590,13 +7590,13 @@
         <v>45115</v>
       </c>
       <c r="G72">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="H72" s="2">
         <v>45207</v>
       </c>
       <c r="I72">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="J72" t="inlineStr">
         <is>
@@ -7693,13 +7693,13 @@
         <v>45097</v>
       </c>
       <c r="G73">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="H73" s="2">
         <v>45189</v>
       </c>
       <c r="I73">
-        <v>-8</v>
+        <v>-9</v>
       </c>
       <c r="J73" t="inlineStr">
         <is>
@@ -7791,13 +7791,13 @@
         <v>45038</v>
       </c>
       <c r="G74">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="H74" s="2">
         <v>45221</v>
       </c>
       <c r="I74">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="J74" t="inlineStr">
         <is>
@@ -7889,13 +7889,13 @@
         <v>45117</v>
       </c>
       <c r="G75">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="H75" s="2">
         <v>45301</v>
       </c>
       <c r="I75">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="J75" t="inlineStr">
         <is>
@@ -7992,13 +7992,13 @@
         <v>45160</v>
       </c>
       <c r="G76">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="H76" s="2">
         <v>45344</v>
       </c>
       <c r="I76">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="J76" t="inlineStr">
         <is>
@@ -8095,13 +8095,13 @@
         <v>45002</v>
       </c>
       <c r="G77">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="H77" s="2">
         <v>45186</v>
       </c>
       <c r="I77">
-        <v>-11</v>
+        <v>-12</v>
       </c>
       <c r="J77" t="inlineStr">
         <is>
@@ -8198,13 +8198,13 @@
         <v>45043</v>
       </c>
       <c r="G78">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="H78" s="2">
         <v>45226</v>
       </c>
       <c r="I78">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="J78" t="inlineStr">
         <is>
@@ -8301,13 +8301,13 @@
         <v>45079</v>
       </c>
       <c r="G79">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="H79" s="2">
         <v>45262</v>
       </c>
       <c r="I79">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="J79" t="inlineStr">
         <is>
@@ -8404,7 +8404,7 @@
         <v>45254</v>
       </c>
       <c r="I80">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="J80" t="inlineStr">
         <is>
@@ -8501,13 +8501,13 @@
         <v>45104</v>
       </c>
       <c r="G81">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="H81" s="2">
         <v>45287</v>
       </c>
       <c r="I81">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="J81" t="inlineStr">
         <is>
@@ -8604,7 +8604,7 @@
         <v>45288</v>
       </c>
       <c r="I82">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="J82" t="inlineStr">
         <is>
@@ -8696,13 +8696,13 @@
         <v>45175</v>
       </c>
       <c r="G83">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="H83" s="2">
         <v>45357</v>
       </c>
       <c r="I83">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="J83" t="inlineStr">
         <is>
@@ -8799,13 +8799,13 @@
         <v>45054</v>
       </c>
       <c r="G84">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="H84" s="2">
         <v>45238</v>
       </c>
       <c r="I84">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="J84" t="inlineStr">
         <is>
@@ -8902,13 +8902,13 @@
         <v>45056</v>
       </c>
       <c r="G85">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="H85" s="2">
         <v>45240</v>
       </c>
       <c r="I85">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="J85" t="inlineStr">
         <is>
@@ -9005,13 +9005,13 @@
         <v>45085</v>
       </c>
       <c r="G86">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="H86" s="2">
         <v>45268</v>
       </c>
       <c r="I86">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="J86" t="inlineStr">
         <is>
@@ -9108,7 +9108,7 @@
         <v>45194</v>
       </c>
       <c r="I87">
-        <v>-3</v>
+        <v>-4</v>
       </c>
       <c r="J87" t="inlineStr">
         <is>
@@ -9195,13 +9195,13 @@
         <v>45103</v>
       </c>
       <c r="G88">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="H88" s="2">
         <v>45286</v>
       </c>
       <c r="I88">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="J88" t="inlineStr">
         <is>
@@ -9298,13 +9298,13 @@
         <v>45103</v>
       </c>
       <c r="G89">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="H89" s="2">
         <v>45286</v>
       </c>
       <c r="I89">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="J89" t="inlineStr">
         <is>
@@ -9401,13 +9401,13 @@
         <v>45008</v>
       </c>
       <c r="G90">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="H90" s="2">
         <v>45192</v>
       </c>
       <c r="I90">
-        <v>-5</v>
+        <v>-6</v>
       </c>
       <c r="J90" t="inlineStr">
         <is>
@@ -9499,13 +9499,13 @@
         <v>45100</v>
       </c>
       <c r="G91">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="H91" s="2">
         <v>45287</v>
       </c>
       <c r="I91">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="J91" t="inlineStr">
         <is>
@@ -9602,13 +9602,13 @@
         <v>45003</v>
       </c>
       <c r="G92">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="H92" s="2">
         <v>45187</v>
       </c>
       <c r="I92">
-        <v>-10</v>
+        <v>-11</v>
       </c>
       <c r="J92" t="inlineStr">
         <is>
@@ -9705,13 +9705,13 @@
         <v>45104</v>
       </c>
       <c r="G93">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="H93" s="2">
         <v>45287</v>
       </c>
       <c r="I93">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="J93" t="inlineStr">
         <is>
@@ -9808,13 +9808,13 @@
         <v>45104</v>
       </c>
       <c r="G94">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="H94" s="2">
         <v>45287</v>
       </c>
       <c r="I94">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="J94" t="inlineStr">
         <is>
@@ -9911,13 +9911,13 @@
         <v>45049</v>
       </c>
       <c r="G95">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="H95" s="2">
         <v>45233</v>
       </c>
       <c r="I95">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="J95" t="inlineStr">
         <is>
@@ -10014,13 +10014,13 @@
         <v>45122</v>
       </c>
       <c r="G96">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="H96" s="2">
         <v>45306</v>
       </c>
       <c r="I96">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="J96" t="inlineStr">
         <is>
@@ -10112,13 +10112,13 @@
         <v>45141</v>
       </c>
       <c r="G97">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="H97" s="2">
         <v>45325</v>
       </c>
       <c r="I97">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="J97" t="inlineStr">
         <is>
@@ -10215,13 +10215,13 @@
         <v>45010</v>
       </c>
       <c r="G98">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="H98" s="2">
         <v>45194</v>
       </c>
       <c r="I98">
-        <v>-3</v>
+        <v>-4</v>
       </c>
       <c r="J98" t="inlineStr">
         <is>
@@ -10313,13 +10313,13 @@
         <v>45093</v>
       </c>
       <c r="G99">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="H99" s="2">
         <v>45276</v>
       </c>
       <c r="I99">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="J99" t="inlineStr">
         <is>
@@ -10416,13 +10416,13 @@
         <v>45123</v>
       </c>
       <c r="G100">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="H100" s="2">
         <v>45307</v>
       </c>
       <c r="I100">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="J100" t="inlineStr">
         <is>
@@ -10519,13 +10519,13 @@
         <v>45014</v>
       </c>
       <c r="G101">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="H101" s="2">
         <v>45198</v>
       </c>
       <c r="I101">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J101" t="inlineStr">
         <is>
@@ -10622,13 +10622,13 @@
         <v>45093</v>
       </c>
       <c r="G102">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="H102" s="2">
         <v>45276</v>
       </c>
       <c r="I102">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="J102" t="inlineStr">
         <is>
@@ -10725,13 +10725,13 @@
         <v>45122</v>
       </c>
       <c r="G103">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="H103" s="2">
         <v>45306</v>
       </c>
       <c r="I103">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="J103" t="inlineStr">
         <is>
@@ -10828,13 +10828,13 @@
         <v>45122</v>
       </c>
       <c r="G104">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="H104" s="2">
         <v>45306</v>
       </c>
       <c r="I104">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="J104" t="inlineStr">
         <is>
@@ -10926,13 +10926,13 @@
         <v>45050</v>
       </c>
       <c r="G105">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="H105" s="2">
         <v>45234</v>
       </c>
       <c r="I105">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="J105" t="inlineStr">
         <is>
@@ -11029,13 +11029,13 @@
         <v>45085</v>
       </c>
       <c r="G106">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="H106" s="2">
         <v>45268</v>
       </c>
       <c r="I106">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="J106" t="inlineStr">
         <is>
@@ -11132,13 +11132,13 @@
         <v>45093</v>
       </c>
       <c r="G107">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="H107" s="2">
         <v>45185</v>
       </c>
       <c r="I107">
-        <v>-12</v>
+        <v>-13</v>
       </c>
       <c r="J107" t="inlineStr">
         <is>
@@ -11230,13 +11230,13 @@
         <v>45093</v>
       </c>
       <c r="G108">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="H108" s="2">
         <v>45185</v>
       </c>
       <c r="I108">
-        <v>-12</v>
+        <v>-13</v>
       </c>
       <c r="J108" t="inlineStr">
         <is>
@@ -11328,13 +11328,13 @@
         <v>45093</v>
       </c>
       <c r="G109">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="H109" s="2">
         <v>45185</v>
       </c>
       <c r="I109">
-        <v>-12</v>
+        <v>-13</v>
       </c>
       <c r="J109" t="inlineStr">
         <is>
@@ -11431,13 +11431,13 @@
         <v>45148</v>
       </c>
       <c r="G110">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="H110" s="2">
         <v>45240</v>
       </c>
       <c r="I110">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="J110" t="inlineStr">
         <is>
@@ -11534,13 +11534,13 @@
         <v>45119</v>
       </c>
       <c r="G111">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="H111" s="2">
         <v>45211</v>
       </c>
       <c r="I111">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="J111" t="inlineStr">
         <is>
@@ -11637,13 +11637,13 @@
         <v>45172</v>
       </c>
       <c r="G112">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="H112" s="2">
         <v>45263</v>
       </c>
       <c r="I112">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="J112" t="inlineStr">
         <is>
@@ -11740,13 +11740,13 @@
         <v>45023</v>
       </c>
       <c r="G113">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="H113" s="2">
         <v>45206</v>
       </c>
       <c r="I113">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="J113" t="inlineStr">
         <is>
@@ -11843,13 +11843,13 @@
         <v>45111</v>
       </c>
       <c r="G114">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="H114" s="2">
         <v>45203</v>
       </c>
       <c r="I114">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="J114" t="inlineStr">
         <is>
@@ -11946,7 +11946,7 @@
         <v>45218</v>
       </c>
       <c r="I115">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="J115" t="inlineStr">
         <is>
@@ -12043,13 +12043,13 @@
         <v>45161</v>
       </c>
       <c r="G116">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="H116" s="2">
         <v>45253</v>
       </c>
       <c r="I116">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="J116" t="inlineStr">
         <is>
@@ -12146,13 +12146,13 @@
         <v>45115</v>
       </c>
       <c r="G117">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="H117" s="2">
         <v>45299</v>
       </c>
       <c r="I117">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="J117" t="inlineStr">
         <is>
@@ -12244,13 +12244,13 @@
         <v>45094</v>
       </c>
       <c r="G118">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="H118" s="2">
         <v>45277</v>
       </c>
       <c r="I118">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="J118" t="inlineStr">
         <is>
@@ -12347,13 +12347,13 @@
         <v>45104</v>
       </c>
       <c r="G119">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="H119" s="2">
         <v>45287</v>
       </c>
       <c r="I119">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="J119" t="inlineStr">
         <is>
@@ -12450,13 +12450,13 @@
         <v>45104</v>
       </c>
       <c r="G120">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="H120" s="2">
         <v>45287</v>
       </c>
       <c r="I120">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="J120" t="inlineStr">
         <is>
@@ -12553,13 +12553,13 @@
         <v>45104</v>
       </c>
       <c r="G121">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="H121" s="2">
         <v>45287</v>
       </c>
       <c r="I121">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="J121" t="inlineStr">
         <is>
@@ -12656,13 +12656,13 @@
         <v>45104</v>
       </c>
       <c r="G122">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="H122" s="2">
         <v>45287</v>
       </c>
       <c r="I122">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="J122" t="inlineStr">
         <is>
@@ -12759,13 +12759,13 @@
         <v>45107</v>
       </c>
       <c r="G123">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="H123" s="2">
         <v>45199</v>
       </c>
       <c r="I123">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J123" t="inlineStr">
         <is>
@@ -12862,13 +12862,13 @@
         <v>45013</v>
       </c>
       <c r="G124">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="H124" s="2">
         <v>45197</v>
       </c>
       <c r="I124">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="J124" t="inlineStr">
         <is>
@@ -12965,13 +12965,13 @@
         <v>45121</v>
       </c>
       <c r="G125">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="H125" s="2">
         <v>45213</v>
       </c>
       <c r="I125">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="J125" t="inlineStr">
         <is>
@@ -13068,13 +13068,13 @@
         <v>45134</v>
       </c>
       <c r="G126">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="H126" s="2">
         <v>45226</v>
       </c>
       <c r="I126">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="J126" t="inlineStr">
         <is>
@@ -13171,7 +13171,7 @@
         <v>45212</v>
       </c>
       <c r="I127">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="J127" t="inlineStr">
         <is>
@@ -13268,13 +13268,13 @@
         <v>45126</v>
       </c>
       <c r="G128">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="H128" s="2">
         <v>45218</v>
       </c>
       <c r="I128">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="J128" t="inlineStr">
         <is>
@@ -13366,13 +13366,13 @@
         <v>45158</v>
       </c>
       <c r="G129">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="H129" s="2">
         <v>45250</v>
       </c>
       <c r="I129">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="J129" t="inlineStr">
         <is>
@@ -13469,13 +13469,13 @@
         <v>45171</v>
       </c>
       <c r="G130">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="H130" s="2">
         <v>45262</v>
       </c>
       <c r="I130">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="J130" t="inlineStr">
         <is>
@@ -13572,13 +13572,13 @@
         <v>45111</v>
       </c>
       <c r="G131">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="H131" s="2">
         <v>45203</v>
       </c>
       <c r="I131">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="J131" t="inlineStr">
         <is>
@@ -13675,13 +13675,13 @@
         <v>45144</v>
       </c>
       <c r="G132">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="H132" s="2">
         <v>45236</v>
       </c>
       <c r="I132">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="J132" t="inlineStr">
         <is>
@@ -13778,13 +13778,13 @@
         <v>45156</v>
       </c>
       <c r="G133">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="H133" s="2">
         <v>45248</v>
       </c>
       <c r="I133">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="J133" t="inlineStr">
         <is>
@@ -13876,13 +13876,13 @@
         <v>45146</v>
       </c>
       <c r="G134">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="H134" s="2">
         <v>45238</v>
       </c>
       <c r="I134">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="J134" t="inlineStr">
         <is>
@@ -13979,13 +13979,13 @@
         <v>45140</v>
       </c>
       <c r="G135">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="H135" s="2">
         <v>45232</v>
       </c>
       <c r="I135">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="J135" t="inlineStr">
         <is>
@@ -14082,13 +14082,13 @@
         <v>45104</v>
       </c>
       <c r="G136">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="H136" s="2">
         <v>45196</v>
       </c>
       <c r="I136">
-        <v>-1</v>
+        <v>-2</v>
       </c>
       <c r="J136" t="inlineStr">
         <is>
@@ -14185,13 +14185,13 @@
         <v>45105</v>
       </c>
       <c r="G137">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="H137" s="2">
         <v>45197</v>
       </c>
       <c r="I137">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="J137" t="inlineStr">
         <is>
@@ -14288,13 +14288,13 @@
         <v>45179</v>
       </c>
       <c r="G138">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="H138" s="2">
         <v>45270</v>
       </c>
       <c r="I138">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="J138" t="inlineStr">
         <is>
@@ -14386,13 +14386,13 @@
         <v>45105</v>
       </c>
       <c r="G139">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="H139" s="2">
         <v>45197</v>
       </c>
       <c r="I139">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="J139" t="inlineStr">
         <is>
@@ -14489,13 +14489,13 @@
         <v>45182</v>
       </c>
       <c r="G140">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H140" s="2">
         <v>45273</v>
       </c>
       <c r="I140">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="J140" t="inlineStr">
         <is>
@@ -14592,13 +14592,13 @@
         <v>45116</v>
       </c>
       <c r="G141">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="H141" s="2">
         <v>45208</v>
       </c>
       <c r="I141">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="J141" t="inlineStr">
         <is>
@@ -14690,13 +14690,13 @@
         <v>45150</v>
       </c>
       <c r="G142">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="H142" s="2">
         <v>45242</v>
       </c>
       <c r="I142">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="J142" t="inlineStr">
         <is>
@@ -14793,7 +14793,7 @@
         <v>45238</v>
       </c>
       <c r="I143">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="J143" t="inlineStr">
         <is>
@@ -14890,13 +14890,13 @@
         <v>45171</v>
       </c>
       <c r="G144">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="H144" s="2">
         <v>45262</v>
       </c>
       <c r="I144">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="J144" t="inlineStr">
         <is>
@@ -14993,13 +14993,13 @@
         <v>45102</v>
       </c>
       <c r="G145">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="H145" s="2">
         <v>45194</v>
       </c>
       <c r="I145">
-        <v>-3</v>
+        <v>-4</v>
       </c>
       <c r="J145" t="inlineStr">
         <is>
@@ -15086,13 +15086,13 @@
         <v>45119</v>
       </c>
       <c r="G146">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="H146" s="2">
         <v>45211</v>
       </c>
       <c r="I146">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="J146" t="inlineStr">
         <is>
@@ -15189,13 +15189,13 @@
         <v>45165</v>
       </c>
       <c r="G147">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="H147" s="2">
         <v>45257</v>
       </c>
       <c r="I147">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="J147" t="inlineStr">
         <is>
@@ -15292,13 +15292,13 @@
         <v>45166</v>
       </c>
       <c r="G148">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="H148" s="2">
         <v>45258</v>
       </c>
       <c r="I148">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="J148" t="inlineStr">
         <is>
@@ -15395,13 +15395,13 @@
         <v>45093</v>
       </c>
       <c r="G149">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="H149" s="2">
         <v>45185</v>
       </c>
       <c r="I149">
-        <v>-12</v>
+        <v>-13</v>
       </c>
       <c r="J149" t="inlineStr">
         <is>
@@ -15498,13 +15498,13 @@
         <v>45035</v>
       </c>
       <c r="G150">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="H150" s="2">
         <v>45218</v>
       </c>
       <c r="I150">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="J150" t="inlineStr">
         <is>
@@ -15601,13 +15601,13 @@
         <v>45174</v>
       </c>
       <c r="G151">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="H151" s="2">
         <v>45356</v>
       </c>
       <c r="I151">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="J151" t="inlineStr">
         <is>
@@ -15704,13 +15704,13 @@
         <v>45089</v>
       </c>
       <c r="G152">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="H152" s="2">
         <v>45272</v>
       </c>
       <c r="I152">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="J152" t="inlineStr">
         <is>
@@ -15807,13 +15807,13 @@
         <v>45124</v>
       </c>
       <c r="G153">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="H153" s="2">
         <v>45308</v>
       </c>
       <c r="I153">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="J153" t="inlineStr">
         <is>
@@ -15910,13 +15910,13 @@
         <v>45124</v>
       </c>
       <c r="G154">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="H154" s="2">
         <v>45308</v>
       </c>
       <c r="I154">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="J154" t="inlineStr">
         <is>
@@ -16013,13 +16013,13 @@
         <v>45026</v>
       </c>
       <c r="G155">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="H155" s="2">
         <v>45209</v>
       </c>
       <c r="I155">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="J155" t="inlineStr">
         <is>
@@ -16116,13 +16116,13 @@
         <v>45026</v>
       </c>
       <c r="G156">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="H156" s="2">
         <v>45209</v>
       </c>
       <c r="I156">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="J156" t="inlineStr">
         <is>
@@ -16219,13 +16219,13 @@
         <v>45026</v>
       </c>
       <c r="G157">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="H157" s="2">
         <v>45209</v>
       </c>
       <c r="I157">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="J157" t="inlineStr">
         <is>
@@ -16322,13 +16322,13 @@
         <v>45026</v>
       </c>
       <c r="G158">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="H158" s="2">
         <v>45209</v>
       </c>
       <c r="I158">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="J158" t="inlineStr">
         <is>
@@ -16425,13 +16425,13 @@
         <v>45156</v>
       </c>
       <c r="G159">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="H159" s="2">
         <v>45247</v>
       </c>
       <c r="I159">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="J159" t="inlineStr">
         <is>
@@ -16528,13 +16528,13 @@
         <v>45153</v>
       </c>
       <c r="G160">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="H160" s="2">
         <v>45245</v>
       </c>
       <c r="I160">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="J160" t="inlineStr">
         <is>
@@ -16631,13 +16631,13 @@
         <v>45135</v>
       </c>
       <c r="G161">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="H161" s="2">
         <v>45319</v>
       </c>
       <c r="I161">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="J161" t="inlineStr">
         <is>
@@ -16734,13 +16734,13 @@
         <v>45091</v>
       </c>
       <c r="G162">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="H162" s="2">
         <v>45274</v>
       </c>
       <c r="I162">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="J162" t="inlineStr">
         <is>
@@ -16832,13 +16832,13 @@
         <v>45091</v>
       </c>
       <c r="G163">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="H163" s="2">
         <v>45274</v>
       </c>
       <c r="I163">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="J163" t="inlineStr">
         <is>
@@ -16930,13 +16930,13 @@
         <v>45138</v>
       </c>
       <c r="G164">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="H164" s="2">
         <v>45322</v>
       </c>
       <c r="I164">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="J164" t="inlineStr">
         <is>
@@ -17033,13 +17033,13 @@
         <v>45138</v>
       </c>
       <c r="G165">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="H165" s="2">
         <v>45322</v>
       </c>
       <c r="I165">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="J165" t="inlineStr">
         <is>
@@ -17136,13 +17136,13 @@
         <v>45085</v>
       </c>
       <c r="G166">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="H166" s="2">
         <v>45268</v>
       </c>
       <c r="I166">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="J166" t="inlineStr">
         <is>
@@ -17239,13 +17239,13 @@
         <v>45085</v>
       </c>
       <c r="G167">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="H167" s="2">
         <v>45268</v>
       </c>
       <c r="I167">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="J167" t="inlineStr">
         <is>
@@ -17342,7 +17342,7 @@
         <v>45326</v>
       </c>
       <c r="I168">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="J168" t="inlineStr">
         <is>
@@ -17439,13 +17439,13 @@
         <v>45173</v>
       </c>
       <c r="G169">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="H169" s="2">
         <v>45355</v>
       </c>
       <c r="I169">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="J169" t="inlineStr">
         <is>
@@ -17542,13 +17542,13 @@
         <v>45056</v>
       </c>
       <c r="G170">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="H170" s="2">
         <v>45240</v>
       </c>
       <c r="I170">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="J170" t="inlineStr">
         <is>
@@ -17645,7 +17645,7 @@
         <v>45238</v>
       </c>
       <c r="I171">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="J171" t="inlineStr">
         <is>
@@ -17742,13 +17742,13 @@
         <v>45141</v>
       </c>
       <c r="G172">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="H172" s="2">
         <v>45325</v>
       </c>
       <c r="I172">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="J172" t="inlineStr">
         <is>
@@ -17845,13 +17845,13 @@
         <v>45037</v>
       </c>
       <c r="G173">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="H173" s="2">
         <v>45220</v>
       </c>
       <c r="I173">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="J173" t="inlineStr">
         <is>
@@ -17948,13 +17948,13 @@
         <v>45171</v>
       </c>
       <c r="G174">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="H174" s="2">
         <v>45262</v>
       </c>
       <c r="I174">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="J174" t="inlineStr">
         <is>
@@ -18051,13 +18051,13 @@
         <v>45105</v>
       </c>
       <c r="G175">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="H175" s="2">
         <v>45197</v>
       </c>
       <c r="I175">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="J175" t="inlineStr">
         <is>
@@ -18154,13 +18154,13 @@
         <v>45162</v>
       </c>
       <c r="G176">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="H176" s="2">
         <v>45254</v>
       </c>
       <c r="I176">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="J176" t="inlineStr">
         <is>
@@ -18257,13 +18257,13 @@
         <v>45061</v>
       </c>
       <c r="G177">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="H177" s="2">
         <v>45245</v>
       </c>
       <c r="I177">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="J177" t="inlineStr">
         <is>
@@ -18360,13 +18360,13 @@
         <v>45120</v>
       </c>
       <c r="G178">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="H178" s="2">
         <v>45212</v>
       </c>
       <c r="I178">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="J178" t="inlineStr">
         <is>
@@ -18463,7 +18463,7 @@
         <v>45191</v>
       </c>
       <c r="I179">
-        <v>-6</v>
+        <v>-7</v>
       </c>
       <c r="J179" t="inlineStr">
         <is>
@@ -18560,13 +18560,13 @@
         <v>45088</v>
       </c>
       <c r="G180">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="H180" s="2">
         <v>45271</v>
       </c>
       <c r="I180">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="J180" t="inlineStr">
         <is>
@@ -18663,13 +18663,13 @@
         <v>45100</v>
       </c>
       <c r="G181">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="H181" s="2">
         <v>45192</v>
       </c>
       <c r="I181">
-        <v>-5</v>
+        <v>-6</v>
       </c>
       <c r="J181" t="inlineStr">
         <is>
@@ -18756,13 +18756,13 @@
         <v>45131</v>
       </c>
       <c r="G182">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="H182" s="2">
         <v>45223</v>
       </c>
       <c r="I182">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="J182" t="inlineStr">
         <is>
@@ -18854,13 +18854,13 @@
         <v>45136</v>
       </c>
       <c r="G183">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="H183" s="2">
         <v>45228</v>
       </c>
       <c r="I183">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="J183" t="inlineStr">
         <is>
@@ -18952,13 +18952,13 @@
         <v>45150</v>
       </c>
       <c r="G184">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="H184" s="2">
         <v>45242</v>
       </c>
       <c r="I184">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="J184" t="inlineStr">
         <is>
@@ -19050,13 +19050,13 @@
         <v>45118</v>
       </c>
       <c r="G185">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="H185" s="2">
         <v>45210</v>
       </c>
       <c r="I185">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="J185" t="inlineStr">
         <is>
@@ -19148,13 +19148,13 @@
         <v>45129</v>
       </c>
       <c r="G186">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="H186" s="2">
         <v>45221</v>
       </c>
       <c r="I186">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="J186" t="inlineStr">
         <is>
@@ -19246,13 +19246,13 @@
         <v>45097</v>
       </c>
       <c r="G187">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="H187" s="2">
         <v>45189</v>
       </c>
       <c r="I187">
-        <v>-8</v>
+        <v>-9</v>
       </c>
       <c r="J187" t="inlineStr">
         <is>
@@ -19339,13 +19339,13 @@
         <v>45101</v>
       </c>
       <c r="G188">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="H188" s="2">
         <v>45193</v>
       </c>
       <c r="I188">
-        <v>-4</v>
+        <v>-5</v>
       </c>
       <c r="J188" t="inlineStr">
         <is>
@@ -19432,13 +19432,13 @@
         <v>45165</v>
       </c>
       <c r="G189">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="H189" s="2">
         <v>45257</v>
       </c>
       <c r="I189">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="J189" t="inlineStr">
         <is>
@@ -19530,7 +19530,7 @@
         <v>45202</v>
       </c>
       <c r="I190">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="J190" t="inlineStr">
         <is>
@@ -19627,13 +19627,13 @@
         <v>45081</v>
       </c>
       <c r="G191">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="H191" s="2">
         <v>45264</v>
       </c>
       <c r="I191">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="J191" t="inlineStr">
         <is>
@@ -19730,13 +19730,13 @@
         <v>45081</v>
       </c>
       <c r="G192">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="H192" s="2">
         <v>45264</v>
       </c>
       <c r="I192">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="J192" t="inlineStr">
         <is>
@@ -19833,7 +19833,7 @@
         <v>45319</v>
       </c>
       <c r="I193">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="J193" t="inlineStr">
         <is>
@@ -19930,7 +19930,7 @@
         <v>45319</v>
       </c>
       <c r="I194">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="J194" t="inlineStr">
         <is>
@@ -20022,13 +20022,13 @@
         <v>45046</v>
       </c>
       <c r="G195">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="H195" s="2">
         <v>45230</v>
       </c>
       <c r="I195">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="J195" t="inlineStr">
         <is>
@@ -20125,13 +20125,13 @@
         <v>45046</v>
       </c>
       <c r="G196">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="H196" s="2">
         <v>45230</v>
       </c>
       <c r="I196">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="J196" t="inlineStr">
         <is>
@@ -20228,13 +20228,13 @@
         <v>45031</v>
       </c>
       <c r="G197">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="H197" s="2">
         <v>45214</v>
       </c>
       <c r="I197">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="J197" t="inlineStr">
         <is>
@@ -20331,13 +20331,13 @@
         <v>45031</v>
       </c>
       <c r="G198">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="H198" s="2">
         <v>45214</v>
       </c>
       <c r="I198">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="J198" t="inlineStr">
         <is>
@@ -20434,13 +20434,13 @@
         <v>45031</v>
       </c>
       <c r="G199">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="H199" s="2">
         <v>45214</v>
       </c>
       <c r="I199">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="J199" t="inlineStr">
         <is>
@@ -20537,13 +20537,13 @@
         <v>45031</v>
       </c>
       <c r="G200">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="H200" s="2">
         <v>45214</v>
       </c>
       <c r="I200">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="J200" t="inlineStr">
         <is>
@@ -20640,13 +20640,13 @@
         <v>45067</v>
       </c>
       <c r="G201">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="H201" s="2">
         <v>45251</v>
       </c>
       <c r="I201">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="J201" t="inlineStr">
         <is>
@@ -20743,13 +20743,13 @@
         <v>45067</v>
       </c>
       <c r="G202">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="H202" s="2">
         <v>45251</v>
       </c>
       <c r="I202">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="J202" t="inlineStr">
         <is>
@@ -20846,13 +20846,13 @@
         <v>45067</v>
       </c>
       <c r="G203">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="H203" s="2">
         <v>45251</v>
       </c>
       <c r="I203">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="J203" t="inlineStr">
         <is>
@@ -20949,13 +20949,13 @@
         <v>45067</v>
       </c>
       <c r="G204">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="H204" s="2">
         <v>45251</v>
       </c>
       <c r="I204">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="J204" t="inlineStr">
         <is>
@@ -21052,13 +21052,13 @@
         <v>45178</v>
       </c>
       <c r="G205">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="H205" s="2">
         <v>45269</v>
       </c>
       <c r="I205">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="J205" t="inlineStr">
         <is>
@@ -21155,7 +21155,7 @@
         <v>45252</v>
       </c>
       <c r="I206">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="J206" t="inlineStr">
         <is>
@@ -21252,13 +21252,13 @@
         <v>45087</v>
       </c>
       <c r="G207">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="H207" s="2">
         <v>45270</v>
       </c>
       <c r="I207">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="J207" t="inlineStr">
         <is>
@@ -21355,13 +21355,13 @@
         <v>45099</v>
       </c>
       <c r="G208">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="H208" s="2">
         <v>45282</v>
       </c>
       <c r="I208">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="J208" t="inlineStr">
         <is>
@@ -21458,13 +21458,13 @@
         <v>45175</v>
       </c>
       <c r="G209">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="H209" s="2">
         <v>45356</v>
       </c>
       <c r="I209">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="J209" t="inlineStr">
         <is>
@@ -21561,13 +21561,13 @@
         <v>45175</v>
       </c>
       <c r="G210">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="H210" s="2">
         <v>45356</v>
       </c>
       <c r="I210">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="J210" t="inlineStr">
         <is>
@@ -21664,13 +21664,13 @@
         <v>45166</v>
       </c>
       <c r="G211">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="H211" s="2">
         <v>45350</v>
       </c>
       <c r="I211">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="J211" t="inlineStr">
         <is>
@@ -21767,13 +21767,13 @@
         <v>45166</v>
       </c>
       <c r="G212">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="H212" s="2">
         <v>45350</v>
       </c>
       <c r="I212">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="J212" t="inlineStr">
         <is>
@@ -21870,13 +21870,13 @@
         <v>45090</v>
       </c>
       <c r="G213">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="H213" s="2">
         <v>45273</v>
       </c>
       <c r="I213">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="J213" t="inlineStr">
         <is>
@@ -21973,13 +21973,13 @@
         <v>45106</v>
       </c>
       <c r="G214">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="H214" s="2">
         <v>45289</v>
       </c>
       <c r="I214">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="J214" t="inlineStr">
         <is>
@@ -22076,13 +22076,13 @@
         <v>45134</v>
       </c>
       <c r="G215">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="H215" s="2">
         <v>45226</v>
       </c>
       <c r="I215">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="J215" t="inlineStr">
         <is>
@@ -22179,13 +22179,13 @@
         <v>45132</v>
       </c>
       <c r="G216">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="H216" s="2">
         <v>45224</v>
       </c>
       <c r="I216">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="J216" t="inlineStr">
         <is>
@@ -22282,13 +22282,13 @@
         <v>45150</v>
       </c>
       <c r="G217">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="H217" s="2">
         <v>45242</v>
       </c>
       <c r="I217">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="J217" t="inlineStr">
         <is>
@@ -22385,13 +22385,13 @@
         <v>45095</v>
       </c>
       <c r="G218">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="H218" s="2">
         <v>45187</v>
       </c>
       <c r="I218">
-        <v>-10</v>
+        <v>-11</v>
       </c>
       <c r="J218" t="inlineStr">
         <is>
@@ -22483,13 +22483,13 @@
         <v>45182</v>
       </c>
       <c r="G219">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H219" s="2">
         <v>45273</v>
       </c>
       <c r="I219">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="J219" t="inlineStr">
         <is>
@@ -22586,7 +22586,7 @@
         <v>45196</v>
       </c>
       <c r="I220">
-        <v>-1</v>
+        <v>-2</v>
       </c>
       <c r="J220" t="inlineStr">
         <is>
@@ -22683,13 +22683,13 @@
         <v>45108</v>
       </c>
       <c r="G221">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="H221" s="2">
         <v>45200</v>
       </c>
       <c r="I221">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="J221" t="inlineStr">
         <is>
@@ -22786,13 +22786,13 @@
         <v>45135</v>
       </c>
       <c r="G222">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="H222" s="2">
         <v>45227</v>
       </c>
       <c r="I222">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="J222" t="inlineStr">
         <is>
@@ -22889,13 +22889,13 @@
         <v>45148</v>
       </c>
       <c r="G223">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="H223" s="2">
         <v>45240</v>
       </c>
       <c r="I223">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="J223" t="inlineStr">
         <is>
@@ -22987,13 +22987,13 @@
         <v>45100</v>
       </c>
       <c r="G224">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="H224" s="2">
         <v>45192</v>
       </c>
       <c r="I224">
-        <v>-5</v>
+        <v>-6</v>
       </c>
       <c r="J224" t="inlineStr">
         <is>
@@ -23085,13 +23085,13 @@
         <v>45136</v>
       </c>
       <c r="G225">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="H225" s="2">
         <v>45320</v>
       </c>
       <c r="I225">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="J225" t="inlineStr">
         <is>
@@ -23188,13 +23188,13 @@
         <v>45136</v>
       </c>
       <c r="G226">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="H226" s="2">
         <v>45320</v>
       </c>
       <c r="I226">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="J226" t="inlineStr">
         <is>
@@ -23291,13 +23291,13 @@
         <v>45094</v>
       </c>
       <c r="G227">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="H227" s="2">
         <v>45277</v>
       </c>
       <c r="I227">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="J227" t="inlineStr">
         <is>
@@ -23394,13 +23394,13 @@
         <v>45081</v>
       </c>
       <c r="G228">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="H228" s="2">
         <v>45264</v>
       </c>
       <c r="I228">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="J228" t="inlineStr">
         <is>
@@ -23497,13 +23497,13 @@
         <v>45099</v>
       </c>
       <c r="G229">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="H229" s="2">
         <v>45282</v>
       </c>
       <c r="I229">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="J229" t="inlineStr">
         <is>
@@ -23600,13 +23600,13 @@
         <v>45018</v>
       </c>
       <c r="G230">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="H230" s="2">
         <v>45201</v>
       </c>
       <c r="I230">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="J230" t="inlineStr">
         <is>
@@ -23703,13 +23703,13 @@
         <v>45031</v>
       </c>
       <c r="G231">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="H231" s="2">
         <v>45214</v>
       </c>
       <c r="I231">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="J231" t="inlineStr">
         <is>
@@ -23806,7 +23806,7 @@
         <v>45294</v>
       </c>
       <c r="I232">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="J232" t="inlineStr">
         <is>
@@ -23903,13 +23903,13 @@
         <v>45079</v>
       </c>
       <c r="G233">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="H233" s="2">
         <v>45262</v>
       </c>
       <c r="I233">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="J233" t="inlineStr">
         <is>
@@ -24006,7 +24006,7 @@
         <v>45199</v>
       </c>
       <c r="I234">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J234" t="inlineStr">
         <is>
@@ -24103,13 +24103,13 @@
         <v>45021</v>
       </c>
       <c r="G235">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="H235" s="2">
         <v>45204</v>
       </c>
       <c r="I235">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="J235" t="inlineStr">
         <is>
@@ -24206,13 +24206,13 @@
         <v>45021</v>
       </c>
       <c r="G236">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="H236" s="2">
         <v>45204</v>
       </c>
       <c r="I236">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="J236" t="inlineStr">
         <is>
@@ -24309,13 +24309,13 @@
         <v>45080</v>
       </c>
       <c r="G237">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="H237" s="2">
         <v>45263</v>
       </c>
       <c r="I237">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="J237" t="inlineStr">
         <is>
@@ -24412,13 +24412,13 @@
         <v>45046</v>
       </c>
       <c r="G238">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="H238" s="2">
         <v>45229</v>
       </c>
       <c r="I238">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="J238" t="inlineStr">
         <is>
@@ -24515,13 +24515,13 @@
         <v>45112</v>
       </c>
       <c r="G239">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="H239" s="2">
         <v>45204</v>
       </c>
       <c r="I239">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="J239" t="inlineStr">
         <is>
@@ -24609,13 +24609,13 @@
         <v>45112</v>
       </c>
       <c r="G240">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="H240" s="2">
         <v>45204</v>
       </c>
       <c r="I240">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="J240" t="inlineStr">
         <is>
@@ -24703,13 +24703,13 @@
         <v>45016</v>
       </c>
       <c r="G241">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="H241" s="2">
         <v>45199</v>
       </c>
       <c r="I241">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J241" t="inlineStr">
         <is>
@@ -24806,13 +24806,13 @@
         <v>45070</v>
       </c>
       <c r="G242">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="H242" s="2">
         <v>45254</v>
       </c>
       <c r="I242">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="J242" t="inlineStr">
         <is>
@@ -24909,13 +24909,13 @@
         <v>45168</v>
       </c>
       <c r="G243">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="H243" s="2">
         <v>45260</v>
       </c>
       <c r="I243">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="J243" t="inlineStr">
         <is>
@@ -25012,13 +25012,13 @@
         <v>45027</v>
       </c>
       <c r="G244">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="H244" s="2">
         <v>45210</v>
       </c>
       <c r="I244">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="J244" t="inlineStr">
         <is>
@@ -25115,13 +25115,13 @@
         <v>45077</v>
       </c>
       <c r="G245">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="H245" s="2">
         <v>45260</v>
       </c>
       <c r="I245">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="J245" t="inlineStr">
         <is>
@@ -25218,13 +25218,13 @@
         <v>45100</v>
       </c>
       <c r="G246">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="H246" s="2">
         <v>45283</v>
       </c>
       <c r="I246">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="J246" t="inlineStr">
         <is>
@@ -25321,7 +25321,7 @@
         <v>45281</v>
       </c>
       <c r="I247">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="J247" t="inlineStr">
         <is>
@@ -25418,13 +25418,13 @@
         <v>45044</v>
       </c>
       <c r="G248">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="H248" s="2">
         <v>45227</v>
       </c>
       <c r="I248">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="J248" t="inlineStr">
         <is>
@@ -25521,13 +25521,13 @@
         <v>45101</v>
       </c>
       <c r="G249">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="H249" s="2">
         <v>45283</v>
       </c>
       <c r="I249">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="J249" t="inlineStr">
         <is>
@@ -25624,13 +25624,13 @@
         <v>45134</v>
       </c>
       <c r="G250">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="H250" s="2">
         <v>45226</v>
       </c>
       <c r="I250">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="J250" t="inlineStr">
         <is>
@@ -25727,13 +25727,13 @@
         <v>45158</v>
       </c>
       <c r="G251">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="H251" s="2">
         <v>45250</v>
       </c>
       <c r="I251">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="J251" t="inlineStr">
         <is>
@@ -25830,13 +25830,13 @@
         <v>45108</v>
       </c>
       <c r="G252">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="H252" s="2">
         <v>45200</v>
       </c>
       <c r="I252">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="J252" t="inlineStr">
         <is>
@@ -25933,7 +25933,7 @@
         <v>45317</v>
       </c>
       <c r="I253">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="J253" t="inlineStr">
         <is>
@@ -26030,13 +26030,13 @@
         <v>45039</v>
       </c>
       <c r="G254">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="H254" s="2">
         <v>45222</v>
       </c>
       <c r="I254">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="J254" t="inlineStr">
         <is>
@@ -26128,13 +26128,13 @@
         <v>45129</v>
       </c>
       <c r="G255">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="H255" s="2">
         <v>45221</v>
       </c>
       <c r="I255">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="J255" t="inlineStr">
         <is>
@@ -26231,13 +26231,13 @@
         <v>45157</v>
       </c>
       <c r="G256">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="H256" s="2">
         <v>45341</v>
       </c>
       <c r="I256">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="J256" t="inlineStr">
         <is>
@@ -26334,13 +26334,13 @@
         <v>45063</v>
       </c>
       <c r="G257">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="H257" s="2">
         <v>45247</v>
       </c>
       <c r="I257">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="J257" t="inlineStr">
         <is>
@@ -26437,7 +26437,7 @@
         <v>45254</v>
       </c>
       <c r="I258">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="J258" t="inlineStr">
         <is>
@@ -26534,7 +26534,7 @@
         <v>45486</v>
       </c>
       <c r="I259">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="J259" t="inlineStr">
         <is>
@@ -26626,13 +26626,13 @@
         <v>45073</v>
       </c>
       <c r="G260">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="H260" s="2">
         <v>45439</v>
       </c>
       <c r="I260">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="J260" t="inlineStr">
         <is>
@@ -26724,7 +26724,7 @@
         <v>45323</v>
       </c>
       <c r="I261">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="J261" t="inlineStr">
         <is>
@@ -26816,7 +26816,7 @@
         <v>45303</v>
       </c>
       <c r="I262">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="J262" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
Bond dates update Sat Sep 30 23:09:13 UTC 2023
</commit_message>
<xml_diff>
--- a/Data/obligacje_screener.xlsx
+++ b/Data/obligacje_screener.xlsx
@@ -512,7 +512,7 @@
         <v>45340</v>
       </c>
       <c r="I2">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="J2" t="inlineStr">
         <is>
@@ -600,13 +600,13 @@
         <v>45121</v>
       </c>
       <c r="G3">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="H3" s="2">
         <v>45305</v>
       </c>
       <c r="I3">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="J3" t="inlineStr">
         <is>
@@ -703,13 +703,13 @@
         <v>45039</v>
       </c>
       <c r="G4">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="H4" s="2">
         <v>45222</v>
       </c>
       <c r="I4">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="J4" t="inlineStr">
         <is>
@@ -806,13 +806,13 @@
         <v>45039</v>
       </c>
       <c r="G5">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="H5" s="2">
         <v>45222</v>
       </c>
       <c r="I5">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="J5" t="inlineStr">
         <is>
@@ -909,13 +909,13 @@
         <v>45129</v>
       </c>
       <c r="G6">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="H6" s="2">
         <v>45221</v>
       </c>
       <c r="I6">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="J6" t="inlineStr">
         <is>
@@ -1012,13 +1012,13 @@
         <v>45162</v>
       </c>
       <c r="G7">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="H7" s="2">
         <v>45254</v>
       </c>
       <c r="I7">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="J7" t="inlineStr">
         <is>
@@ -1110,13 +1110,13 @@
         <v>45156</v>
       </c>
       <c r="G8">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="H8" s="2">
         <v>45248</v>
       </c>
       <c r="I8">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="J8" t="inlineStr">
         <is>
@@ -1213,13 +1213,13 @@
         <v>45141</v>
       </c>
       <c r="G9">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="H9" s="2">
         <v>45233</v>
       </c>
       <c r="I9">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="J9" t="inlineStr">
         <is>
@@ -1316,13 +1316,13 @@
         <v>45062</v>
       </c>
       <c r="G10">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="H10" s="2">
         <v>45246</v>
       </c>
       <c r="I10">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="J10" t="inlineStr">
         <is>
@@ -1419,7 +1419,7 @@
         <v>45286</v>
       </c>
       <c r="I11">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="J11" t="inlineStr">
         <is>
@@ -1516,13 +1516,13 @@
         <v>45011</v>
       </c>
       <c r="G12">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="H12" s="2">
         <v>45195</v>
       </c>
       <c r="I12">
-        <v>-3</v>
+        <v>-4</v>
       </c>
       <c r="J12" t="inlineStr">
         <is>
@@ -1614,13 +1614,13 @@
         <v>45036</v>
       </c>
       <c r="G13">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="H13" s="2">
         <v>45219</v>
       </c>
       <c r="I13">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="J13" t="inlineStr">
         <is>
@@ -1717,13 +1717,13 @@
         <v>45036</v>
       </c>
       <c r="G14">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="H14" s="2">
         <v>45219</v>
       </c>
       <c r="I14">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="J14" t="inlineStr">
         <is>
@@ -1820,13 +1820,13 @@
         <v>45106</v>
       </c>
       <c r="G15">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="H15" s="2">
         <v>45289</v>
       </c>
       <c r="I15">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="J15" t="inlineStr">
         <is>
@@ -1923,13 +1923,13 @@
         <v>45094</v>
       </c>
       <c r="G16">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="H16" s="2">
         <v>45186</v>
       </c>
       <c r="I16">
-        <v>-12</v>
+        <v>-13</v>
       </c>
       <c r="J16" t="inlineStr">
         <is>
@@ -2026,13 +2026,13 @@
         <v>45094</v>
       </c>
       <c r="G17">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="H17" s="2">
         <v>45186</v>
       </c>
       <c r="I17">
-        <v>-12</v>
+        <v>-13</v>
       </c>
       <c r="J17" t="inlineStr">
         <is>
@@ -2129,13 +2129,13 @@
         <v>45132</v>
       </c>
       <c r="G18">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="H18" s="2">
         <v>45224</v>
       </c>
       <c r="I18">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="J18" t="inlineStr">
         <is>
@@ -2232,13 +2232,13 @@
         <v>45137</v>
       </c>
       <c r="G19">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="H19" s="2">
         <v>45229</v>
       </c>
       <c r="I19">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="J19" t="inlineStr">
         <is>
@@ -2330,13 +2330,13 @@
         <v>45183</v>
       </c>
       <c r="G20">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H20" s="2">
         <v>45274</v>
       </c>
       <c r="I20">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="J20" t="inlineStr">
         <is>
@@ -2433,13 +2433,13 @@
         <v>45093</v>
       </c>
       <c r="G21">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="H21" s="2">
         <v>45187</v>
       </c>
       <c r="I21">
-        <v>-11</v>
+        <v>-12</v>
       </c>
       <c r="J21" t="inlineStr">
         <is>
@@ -2536,13 +2536,13 @@
         <v>45096</v>
       </c>
       <c r="G22">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="H22" s="2">
         <v>45187</v>
       </c>
       <c r="I22">
-        <v>-11</v>
+        <v>-12</v>
       </c>
       <c r="J22" t="inlineStr">
         <is>
@@ -2639,7 +2639,7 @@
         <v>45245</v>
       </c>
       <c r="I23">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="J23" t="inlineStr">
         <is>
@@ -2736,7 +2736,7 @@
         <v>45245</v>
       </c>
       <c r="I24">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="J24" t="inlineStr">
         <is>
@@ -2833,13 +2833,13 @@
         <v>45021</v>
       </c>
       <c r="G25">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="H25" s="2">
         <v>45204</v>
       </c>
       <c r="I25">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="J25" t="inlineStr">
         <is>
@@ -2936,13 +2936,13 @@
         <v>45160</v>
       </c>
       <c r="G26">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="H26" s="2">
         <v>45344</v>
       </c>
       <c r="I26">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="J26" t="inlineStr">
         <is>
@@ -3039,13 +3039,13 @@
         <v>45118</v>
       </c>
       <c r="G27">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="H27" s="2">
         <v>45302</v>
       </c>
       <c r="I27">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="J27" t="inlineStr">
         <is>
@@ -3142,13 +3142,13 @@
         <v>45085</v>
       </c>
       <c r="G28">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="H28" s="2">
         <v>45268</v>
       </c>
       <c r="I28">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="J28" t="inlineStr">
         <is>
@@ -3245,13 +3245,13 @@
         <v>45183</v>
       </c>
       <c r="G29">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H29" s="2">
         <v>45274</v>
       </c>
       <c r="I29">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="J29" t="inlineStr">
         <is>
@@ -3348,7 +3348,7 @@
         <v>45224</v>
       </c>
       <c r="I30">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="J30" t="inlineStr">
         <is>
@@ -3445,13 +3445,13 @@
         <v>45153</v>
       </c>
       <c r="G31">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="H31" s="2">
         <v>45245</v>
       </c>
       <c r="I31">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="J31" t="inlineStr">
         <is>
@@ -3548,13 +3548,13 @@
         <v>45155</v>
       </c>
       <c r="G32">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="H32" s="2">
         <v>45247</v>
       </c>
       <c r="I32">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="J32" t="inlineStr">
         <is>
@@ -3651,7 +3651,7 @@
         <v>45255</v>
       </c>
       <c r="I33">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="J33" t="inlineStr">
         <is>
@@ -3739,13 +3739,13 @@
         <v>45176</v>
       </c>
       <c r="G34">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="H34" s="2">
         <v>45267</v>
       </c>
       <c r="I34">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="J34" t="inlineStr">
         <is>
@@ -3842,13 +3842,13 @@
         <v>45130</v>
       </c>
       <c r="G35">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="H35" s="2">
         <v>45222</v>
       </c>
       <c r="I35">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="J35" t="inlineStr">
         <is>
@@ -3940,13 +3940,13 @@
         <v>45115</v>
       </c>
       <c r="G36">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="H36" s="2">
         <v>45207</v>
       </c>
       <c r="I36">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="J36" t="inlineStr">
         <is>
@@ -4043,13 +4043,13 @@
         <v>45097</v>
       </c>
       <c r="G37">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="H37" s="2">
         <v>45189</v>
       </c>
       <c r="I37">
-        <v>-9</v>
+        <v>-10</v>
       </c>
       <c r="J37" t="inlineStr">
         <is>
@@ -4141,13 +4141,13 @@
         <v>45107</v>
       </c>
       <c r="G38">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="H38" s="2">
         <v>45290</v>
       </c>
       <c r="I38">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="J38" t="inlineStr">
         <is>
@@ -4244,13 +4244,13 @@
         <v>45063</v>
       </c>
       <c r="G39">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="H39" s="2">
         <v>45247</v>
       </c>
       <c r="I39">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="J39" t="inlineStr">
         <is>
@@ -4347,13 +4347,13 @@
         <v>45177</v>
       </c>
       <c r="G40">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="H40" s="2">
         <v>45359</v>
       </c>
       <c r="I40">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="J40" t="inlineStr">
         <is>
@@ -4450,13 +4450,13 @@
         <v>45107</v>
       </c>
       <c r="G41">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="H41" s="2">
         <v>45290</v>
       </c>
       <c r="I41">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="J41" t="inlineStr">
         <is>
@@ -4553,7 +4553,7 @@
         <v>45265</v>
       </c>
       <c r="I42">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="J42" t="inlineStr">
         <is>
@@ -4650,13 +4650,13 @@
         <v>45098</v>
       </c>
       <c r="G43">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="H43" s="2">
         <v>45281</v>
       </c>
       <c r="I43">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="J43" t="inlineStr">
         <is>
@@ -4753,13 +4753,13 @@
         <v>45099</v>
       </c>
       <c r="G44">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="H44" s="2">
         <v>45282</v>
       </c>
       <c r="I44">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="J44" t="inlineStr">
         <is>
@@ -4856,13 +4856,13 @@
         <v>45106</v>
       </c>
       <c r="G45">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="H45" s="2">
         <v>45289</v>
       </c>
       <c r="I45">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="J45" t="inlineStr">
         <is>
@@ -4959,13 +4959,13 @@
         <v>45106</v>
       </c>
       <c r="G46">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="H46" s="2">
         <v>45289</v>
       </c>
       <c r="I46">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="J46" t="inlineStr">
         <is>
@@ -5062,13 +5062,13 @@
         <v>45120</v>
       </c>
       <c r="G47">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="H47" s="2">
         <v>45304</v>
       </c>
       <c r="I47">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="J47" t="inlineStr">
         <is>
@@ -5165,13 +5165,13 @@
         <v>45118</v>
       </c>
       <c r="G48">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="H48" s="2">
         <v>45302</v>
       </c>
       <c r="I48">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="J48" t="inlineStr">
         <is>
@@ -5268,13 +5268,13 @@
         <v>45152</v>
       </c>
       <c r="G49">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="H49" s="2">
         <v>45336</v>
       </c>
       <c r="I49">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="J49" t="inlineStr">
         <is>
@@ -5371,13 +5371,13 @@
         <v>45042</v>
       </c>
       <c r="G50">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="H50" s="2">
         <v>45225</v>
       </c>
       <c r="I50">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="J50" t="inlineStr">
         <is>
@@ -5474,13 +5474,13 @@
         <v>45122</v>
       </c>
       <c r="G51">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="H51" s="2">
         <v>45306</v>
       </c>
       <c r="I51">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="J51" t="inlineStr">
         <is>
@@ -5577,13 +5577,13 @@
         <v>45139</v>
       </c>
       <c r="G52">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="H52" s="2">
         <v>45323</v>
       </c>
       <c r="I52">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="J52" t="inlineStr">
         <is>
@@ -5671,13 +5671,13 @@
         <v>45099</v>
       </c>
       <c r="G53">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="H53" s="2">
         <v>45282</v>
       </c>
       <c r="I53">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="J53" t="inlineStr">
         <is>
@@ -5774,7 +5774,7 @@
         <v>45196</v>
       </c>
       <c r="I54">
-        <v>-2</v>
+        <v>-3</v>
       </c>
       <c r="J54" t="inlineStr">
         <is>
@@ -5871,13 +5871,13 @@
         <v>45044</v>
       </c>
       <c r="G55">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="H55" s="2">
         <v>45227</v>
       </c>
       <c r="I55">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="J55" t="inlineStr">
         <is>
@@ -5974,13 +5974,13 @@
         <v>45151</v>
       </c>
       <c r="G56">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="H56" s="2">
         <v>45243</v>
       </c>
       <c r="I56">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="J56" t="inlineStr">
         <is>
@@ -6072,7 +6072,7 @@
         <v>45196</v>
       </c>
       <c r="I57">
-        <v>-2</v>
+        <v>-3</v>
       </c>
       <c r="J57" t="inlineStr">
         <is>
@@ -6169,13 +6169,13 @@
         <v>45069</v>
       </c>
       <c r="G58">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="H58" s="2">
         <v>45253</v>
       </c>
       <c r="I58">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="J58" t="inlineStr">
         <is>
@@ -6272,13 +6272,13 @@
         <v>45099</v>
       </c>
       <c r="G59">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="H59" s="2">
         <v>45191</v>
       </c>
       <c r="I59">
-        <v>-7</v>
+        <v>-8</v>
       </c>
       <c r="J59" t="inlineStr">
         <is>
@@ -6370,13 +6370,13 @@
         <v>45113</v>
       </c>
       <c r="G60">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="H60" s="2">
         <v>45205</v>
       </c>
       <c r="I60">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="J60" t="inlineStr">
         <is>
@@ -6473,13 +6473,13 @@
         <v>45127</v>
       </c>
       <c r="G61">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="H61" s="2">
         <v>45219</v>
       </c>
       <c r="I61">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="J61" t="inlineStr">
         <is>
@@ -6576,13 +6576,13 @@
         <v>45058</v>
       </c>
       <c r="G62">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="H62" s="2">
         <v>45242</v>
       </c>
       <c r="I62">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="J62" t="inlineStr">
         <is>
@@ -6679,13 +6679,13 @@
         <v>45010</v>
       </c>
       <c r="G63">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="H63" s="2">
         <v>45194</v>
       </c>
       <c r="I63">
-        <v>-4</v>
+        <v>-5</v>
       </c>
       <c r="J63" t="inlineStr">
         <is>
@@ -6777,13 +6777,13 @@
         <v>45025</v>
       </c>
       <c r="G64">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="H64" s="2">
         <v>45208</v>
       </c>
       <c r="I64">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="J64" t="inlineStr">
         <is>
@@ -6880,13 +6880,13 @@
         <v>45025</v>
       </c>
       <c r="G65">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="H65" s="2">
         <v>45208</v>
       </c>
       <c r="I65">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="J65" t="inlineStr">
         <is>
@@ -6983,13 +6983,13 @@
         <v>45089</v>
       </c>
       <c r="G66">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="H66" s="2">
         <v>45272</v>
       </c>
       <c r="I66">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="J66" t="inlineStr">
         <is>
@@ -7086,13 +7086,13 @@
         <v>45178</v>
       </c>
       <c r="G67">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="H67" s="2">
         <v>45269</v>
       </c>
       <c r="I67">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="J67" t="inlineStr">
         <is>
@@ -7184,13 +7184,13 @@
         <v>45104</v>
       </c>
       <c r="G68">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="H68" s="2">
         <v>45196</v>
       </c>
       <c r="I68">
-        <v>-2</v>
+        <v>-3</v>
       </c>
       <c r="J68" t="inlineStr">
         <is>
@@ -7287,13 +7287,13 @@
         <v>45149</v>
       </c>
       <c r="G69">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="H69" s="2">
         <v>45241</v>
       </c>
       <c r="I69">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="J69" t="inlineStr">
         <is>
@@ -7390,7 +7390,7 @@
         <v>45205</v>
       </c>
       <c r="I70">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="J70" t="inlineStr">
         <is>
@@ -7487,13 +7487,13 @@
         <v>45114</v>
       </c>
       <c r="G71">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="H71" s="2">
         <v>45205</v>
       </c>
       <c r="I71">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="J71" t="inlineStr">
         <is>
@@ -7590,13 +7590,13 @@
         <v>45115</v>
       </c>
       <c r="G72">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="H72" s="2">
         <v>45207</v>
       </c>
       <c r="I72">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="J72" t="inlineStr">
         <is>
@@ -7693,13 +7693,13 @@
         <v>45097</v>
       </c>
       <c r="G73">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="H73" s="2">
         <v>45189</v>
       </c>
       <c r="I73">
-        <v>-9</v>
+        <v>-10</v>
       </c>
       <c r="J73" t="inlineStr">
         <is>
@@ -7791,13 +7791,13 @@
         <v>45038</v>
       </c>
       <c r="G74">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="H74" s="2">
         <v>45221</v>
       </c>
       <c r="I74">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="J74" t="inlineStr">
         <is>
@@ -7889,13 +7889,13 @@
         <v>45117</v>
       </c>
       <c r="G75">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="H75" s="2">
         <v>45301</v>
       </c>
       <c r="I75">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="J75" t="inlineStr">
         <is>
@@ -7992,13 +7992,13 @@
         <v>45160</v>
       </c>
       <c r="G76">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="H76" s="2">
         <v>45344</v>
       </c>
       <c r="I76">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="J76" t="inlineStr">
         <is>
@@ -8095,13 +8095,13 @@
         <v>45002</v>
       </c>
       <c r="G77">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="H77" s="2">
         <v>45186</v>
       </c>
       <c r="I77">
-        <v>-12</v>
+        <v>-13</v>
       </c>
       <c r="J77" t="inlineStr">
         <is>
@@ -8198,13 +8198,13 @@
         <v>45043</v>
       </c>
       <c r="G78">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="H78" s="2">
         <v>45226</v>
       </c>
       <c r="I78">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="J78" t="inlineStr">
         <is>
@@ -8301,13 +8301,13 @@
         <v>45079</v>
       </c>
       <c r="G79">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="H79" s="2">
         <v>45262</v>
       </c>
       <c r="I79">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="J79" t="inlineStr">
         <is>
@@ -8404,7 +8404,7 @@
         <v>45254</v>
       </c>
       <c r="I80">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="J80" t="inlineStr">
         <is>
@@ -8501,13 +8501,13 @@
         <v>45104</v>
       </c>
       <c r="G81">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="H81" s="2">
         <v>45287</v>
       </c>
       <c r="I81">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="J81" t="inlineStr">
         <is>
@@ -8604,7 +8604,7 @@
         <v>45288</v>
       </c>
       <c r="I82">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="J82" t="inlineStr">
         <is>
@@ -8696,13 +8696,13 @@
         <v>45175</v>
       </c>
       <c r="G83">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="H83" s="2">
         <v>45357</v>
       </c>
       <c r="I83">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="J83" t="inlineStr">
         <is>
@@ -8799,13 +8799,13 @@
         <v>45054</v>
       </c>
       <c r="G84">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="H84" s="2">
         <v>45238</v>
       </c>
       <c r="I84">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="J84" t="inlineStr">
         <is>
@@ -8902,13 +8902,13 @@
         <v>45056</v>
       </c>
       <c r="G85">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="H85" s="2">
         <v>45240</v>
       </c>
       <c r="I85">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="J85" t="inlineStr">
         <is>
@@ -9005,13 +9005,13 @@
         <v>45085</v>
       </c>
       <c r="G86">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="H86" s="2">
         <v>45268</v>
       </c>
       <c r="I86">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="J86" t="inlineStr">
         <is>
@@ -9108,7 +9108,7 @@
         <v>45194</v>
       </c>
       <c r="I87">
-        <v>-4</v>
+        <v>-5</v>
       </c>
       <c r="J87" t="inlineStr">
         <is>
@@ -9195,13 +9195,13 @@
         <v>45103</v>
       </c>
       <c r="G88">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="H88" s="2">
         <v>45286</v>
       </c>
       <c r="I88">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="J88" t="inlineStr">
         <is>
@@ -9298,13 +9298,13 @@
         <v>45103</v>
       </c>
       <c r="G89">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="H89" s="2">
         <v>45286</v>
       </c>
       <c r="I89">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="J89" t="inlineStr">
         <is>
@@ -9401,13 +9401,13 @@
         <v>45008</v>
       </c>
       <c r="G90">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="H90" s="2">
         <v>45192</v>
       </c>
       <c r="I90">
-        <v>-6</v>
+        <v>-7</v>
       </c>
       <c r="J90" t="inlineStr">
         <is>
@@ -9499,13 +9499,13 @@
         <v>45100</v>
       </c>
       <c r="G91">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="H91" s="2">
         <v>45287</v>
       </c>
       <c r="I91">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="J91" t="inlineStr">
         <is>
@@ -9602,13 +9602,13 @@
         <v>45003</v>
       </c>
       <c r="G92">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="H92" s="2">
         <v>45187</v>
       </c>
       <c r="I92">
-        <v>-11</v>
+        <v>-12</v>
       </c>
       <c r="J92" t="inlineStr">
         <is>
@@ -9705,13 +9705,13 @@
         <v>45104</v>
       </c>
       <c r="G93">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="H93" s="2">
         <v>45287</v>
       </c>
       <c r="I93">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="J93" t="inlineStr">
         <is>
@@ -9808,13 +9808,13 @@
         <v>45104</v>
       </c>
       <c r="G94">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="H94" s="2">
         <v>45287</v>
       </c>
       <c r="I94">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="J94" t="inlineStr">
         <is>
@@ -9911,13 +9911,13 @@
         <v>45049</v>
       </c>
       <c r="G95">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="H95" s="2">
         <v>45233</v>
       </c>
       <c r="I95">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="J95" t="inlineStr">
         <is>
@@ -10014,13 +10014,13 @@
         <v>45122</v>
       </c>
       <c r="G96">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="H96" s="2">
         <v>45306</v>
       </c>
       <c r="I96">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="J96" t="inlineStr">
         <is>
@@ -10112,13 +10112,13 @@
         <v>45141</v>
       </c>
       <c r="G97">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="H97" s="2">
         <v>45325</v>
       </c>
       <c r="I97">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="J97" t="inlineStr">
         <is>
@@ -10215,13 +10215,13 @@
         <v>45010</v>
       </c>
       <c r="G98">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="H98" s="2">
         <v>45194</v>
       </c>
       <c r="I98">
-        <v>-4</v>
+        <v>-5</v>
       </c>
       <c r="J98" t="inlineStr">
         <is>
@@ -10313,13 +10313,13 @@
         <v>45093</v>
       </c>
       <c r="G99">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="H99" s="2">
         <v>45276</v>
       </c>
       <c r="I99">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="J99" t="inlineStr">
         <is>
@@ -10416,13 +10416,13 @@
         <v>45123</v>
       </c>
       <c r="G100">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="H100" s="2">
         <v>45307</v>
       </c>
       <c r="I100">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="J100" t="inlineStr">
         <is>
@@ -10519,13 +10519,13 @@
         <v>45014</v>
       </c>
       <c r="G101">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="H101" s="2">
         <v>45198</v>
       </c>
       <c r="I101">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="J101" t="inlineStr">
         <is>
@@ -10622,13 +10622,13 @@
         <v>45093</v>
       </c>
       <c r="G102">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="H102" s="2">
         <v>45276</v>
       </c>
       <c r="I102">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="J102" t="inlineStr">
         <is>
@@ -10725,13 +10725,13 @@
         <v>45122</v>
       </c>
       <c r="G103">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="H103" s="2">
         <v>45306</v>
       </c>
       <c r="I103">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="J103" t="inlineStr">
         <is>
@@ -10828,13 +10828,13 @@
         <v>45122</v>
       </c>
       <c r="G104">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="H104" s="2">
         <v>45306</v>
       </c>
       <c r="I104">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="J104" t="inlineStr">
         <is>
@@ -10926,13 +10926,13 @@
         <v>45050</v>
       </c>
       <c r="G105">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="H105" s="2">
         <v>45234</v>
       </c>
       <c r="I105">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="J105" t="inlineStr">
         <is>
@@ -11029,13 +11029,13 @@
         <v>45085</v>
       </c>
       <c r="G106">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="H106" s="2">
         <v>45268</v>
       </c>
       <c r="I106">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="J106" t="inlineStr">
         <is>
@@ -11132,13 +11132,13 @@
         <v>45093</v>
       </c>
       <c r="G107">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="H107" s="2">
         <v>45185</v>
       </c>
       <c r="I107">
-        <v>-13</v>
+        <v>-14</v>
       </c>
       <c r="J107" t="inlineStr">
         <is>
@@ -11230,13 +11230,13 @@
         <v>45093</v>
       </c>
       <c r="G108">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="H108" s="2">
         <v>45185</v>
       </c>
       <c r="I108">
-        <v>-13</v>
+        <v>-14</v>
       </c>
       <c r="J108" t="inlineStr">
         <is>
@@ -11328,13 +11328,13 @@
         <v>45093</v>
       </c>
       <c r="G109">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="H109" s="2">
         <v>45185</v>
       </c>
       <c r="I109">
-        <v>-13</v>
+        <v>-14</v>
       </c>
       <c r="J109" t="inlineStr">
         <is>
@@ -11431,13 +11431,13 @@
         <v>45148</v>
       </c>
       <c r="G110">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="H110" s="2">
         <v>45240</v>
       </c>
       <c r="I110">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="J110" t="inlineStr">
         <is>
@@ -11534,13 +11534,13 @@
         <v>45119</v>
       </c>
       <c r="G111">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="H111" s="2">
         <v>45211</v>
       </c>
       <c r="I111">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="J111" t="inlineStr">
         <is>
@@ -11637,13 +11637,13 @@
         <v>45172</v>
       </c>
       <c r="G112">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="H112" s="2">
         <v>45263</v>
       </c>
       <c r="I112">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="J112" t="inlineStr">
         <is>
@@ -11740,13 +11740,13 @@
         <v>45023</v>
       </c>
       <c r="G113">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="H113" s="2">
         <v>45206</v>
       </c>
       <c r="I113">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="J113" t="inlineStr">
         <is>
@@ -11843,13 +11843,13 @@
         <v>45111</v>
       </c>
       <c r="G114">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="H114" s="2">
         <v>45203</v>
       </c>
       <c r="I114">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="J114" t="inlineStr">
         <is>
@@ -11946,7 +11946,7 @@
         <v>45218</v>
       </c>
       <c r="I115">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="J115" t="inlineStr">
         <is>
@@ -12043,13 +12043,13 @@
         <v>45161</v>
       </c>
       <c r="G116">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="H116" s="2">
         <v>45253</v>
       </c>
       <c r="I116">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="J116" t="inlineStr">
         <is>
@@ -12146,13 +12146,13 @@
         <v>45115</v>
       </c>
       <c r="G117">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="H117" s="2">
         <v>45299</v>
       </c>
       <c r="I117">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="J117" t="inlineStr">
         <is>
@@ -12244,13 +12244,13 @@
         <v>45094</v>
       </c>
       <c r="G118">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="H118" s="2">
         <v>45277</v>
       </c>
       <c r="I118">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="J118" t="inlineStr">
         <is>
@@ -12347,13 +12347,13 @@
         <v>45104</v>
       </c>
       <c r="G119">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="H119" s="2">
         <v>45287</v>
       </c>
       <c r="I119">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="J119" t="inlineStr">
         <is>
@@ -12450,13 +12450,13 @@
         <v>45104</v>
       </c>
       <c r="G120">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="H120" s="2">
         <v>45287</v>
       </c>
       <c r="I120">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="J120" t="inlineStr">
         <is>
@@ -12553,13 +12553,13 @@
         <v>45104</v>
       </c>
       <c r="G121">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="H121" s="2">
         <v>45287</v>
       </c>
       <c r="I121">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="J121" t="inlineStr">
         <is>
@@ -12656,13 +12656,13 @@
         <v>45104</v>
       </c>
       <c r="G122">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="H122" s="2">
         <v>45287</v>
       </c>
       <c r="I122">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="J122" t="inlineStr">
         <is>
@@ -12759,13 +12759,13 @@
         <v>45107</v>
       </c>
       <c r="G123">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="H123" s="2">
         <v>45199</v>
       </c>
       <c r="I123">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J123" t="inlineStr">
         <is>
@@ -12862,13 +12862,13 @@
         <v>45013</v>
       </c>
       <c r="G124">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="H124" s="2">
         <v>45197</v>
       </c>
       <c r="I124">
-        <v>-1</v>
+        <v>-2</v>
       </c>
       <c r="J124" t="inlineStr">
         <is>
@@ -12965,13 +12965,13 @@
         <v>45121</v>
       </c>
       <c r="G125">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="H125" s="2">
         <v>45213</v>
       </c>
       <c r="I125">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="J125" t="inlineStr">
         <is>
@@ -13068,13 +13068,13 @@
         <v>45134</v>
       </c>
       <c r="G126">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="H126" s="2">
         <v>45226</v>
       </c>
       <c r="I126">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="J126" t="inlineStr">
         <is>
@@ -13171,7 +13171,7 @@
         <v>45212</v>
       </c>
       <c r="I127">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="J127" t="inlineStr">
         <is>
@@ -13268,13 +13268,13 @@
         <v>45126</v>
       </c>
       <c r="G128">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="H128" s="2">
         <v>45218</v>
       </c>
       <c r="I128">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="J128" t="inlineStr">
         <is>
@@ -13366,13 +13366,13 @@
         <v>45158</v>
       </c>
       <c r="G129">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="H129" s="2">
         <v>45250</v>
       </c>
       <c r="I129">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="J129" t="inlineStr">
         <is>
@@ -13469,13 +13469,13 @@
         <v>45171</v>
       </c>
       <c r="G130">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="H130" s="2">
         <v>45262</v>
       </c>
       <c r="I130">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="J130" t="inlineStr">
         <is>
@@ -13572,13 +13572,13 @@
         <v>45111</v>
       </c>
       <c r="G131">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="H131" s="2">
         <v>45203</v>
       </c>
       <c r="I131">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="J131" t="inlineStr">
         <is>
@@ -13675,13 +13675,13 @@
         <v>45144</v>
       </c>
       <c r="G132">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="H132" s="2">
         <v>45236</v>
       </c>
       <c r="I132">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="J132" t="inlineStr">
         <is>
@@ -13778,13 +13778,13 @@
         <v>45156</v>
       </c>
       <c r="G133">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="H133" s="2">
         <v>45248</v>
       </c>
       <c r="I133">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="J133" t="inlineStr">
         <is>
@@ -13876,13 +13876,13 @@
         <v>45146</v>
       </c>
       <c r="G134">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="H134" s="2">
         <v>45238</v>
       </c>
       <c r="I134">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="J134" t="inlineStr">
         <is>
@@ -13979,13 +13979,13 @@
         <v>45140</v>
       </c>
       <c r="G135">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="H135" s="2">
         <v>45232</v>
       </c>
       <c r="I135">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="J135" t="inlineStr">
         <is>
@@ -14082,13 +14082,13 @@
         <v>45104</v>
       </c>
       <c r="G136">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="H136" s="2">
         <v>45196</v>
       </c>
       <c r="I136">
-        <v>-2</v>
+        <v>-3</v>
       </c>
       <c r="J136" t="inlineStr">
         <is>
@@ -14185,13 +14185,13 @@
         <v>45105</v>
       </c>
       <c r="G137">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="H137" s="2">
         <v>45197</v>
       </c>
       <c r="I137">
-        <v>-1</v>
+        <v>-2</v>
       </c>
       <c r="J137" t="inlineStr">
         <is>
@@ -14288,13 +14288,13 @@
         <v>45179</v>
       </c>
       <c r="G138">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="H138" s="2">
         <v>45270</v>
       </c>
       <c r="I138">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="J138" t="inlineStr">
         <is>
@@ -14386,13 +14386,13 @@
         <v>45105</v>
       </c>
       <c r="G139">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="H139" s="2">
         <v>45197</v>
       </c>
       <c r="I139">
-        <v>-1</v>
+        <v>-2</v>
       </c>
       <c r="J139" t="inlineStr">
         <is>
@@ -14489,13 +14489,13 @@
         <v>45182</v>
       </c>
       <c r="G140">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="H140" s="2">
         <v>45273</v>
       </c>
       <c r="I140">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="J140" t="inlineStr">
         <is>
@@ -14592,13 +14592,13 @@
         <v>45116</v>
       </c>
       <c r="G141">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="H141" s="2">
         <v>45208</v>
       </c>
       <c r="I141">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="J141" t="inlineStr">
         <is>
@@ -14690,13 +14690,13 @@
         <v>45150</v>
       </c>
       <c r="G142">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="H142" s="2">
         <v>45242</v>
       </c>
       <c r="I142">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="J142" t="inlineStr">
         <is>
@@ -14793,7 +14793,7 @@
         <v>45238</v>
       </c>
       <c r="I143">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="J143" t="inlineStr">
         <is>
@@ -14890,13 +14890,13 @@
         <v>45171</v>
       </c>
       <c r="G144">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="H144" s="2">
         <v>45262</v>
       </c>
       <c r="I144">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="J144" t="inlineStr">
         <is>
@@ -14993,13 +14993,13 @@
         <v>45102</v>
       </c>
       <c r="G145">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="H145" s="2">
         <v>45194</v>
       </c>
       <c r="I145">
-        <v>-4</v>
+        <v>-5</v>
       </c>
       <c r="J145" t="inlineStr">
         <is>
@@ -15086,13 +15086,13 @@
         <v>45119</v>
       </c>
       <c r="G146">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="H146" s="2">
         <v>45211</v>
       </c>
       <c r="I146">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="J146" t="inlineStr">
         <is>
@@ -15189,13 +15189,13 @@
         <v>45165</v>
       </c>
       <c r="G147">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="H147" s="2">
         <v>45257</v>
       </c>
       <c r="I147">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="J147" t="inlineStr">
         <is>
@@ -15292,13 +15292,13 @@
         <v>45166</v>
       </c>
       <c r="G148">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="H148" s="2">
         <v>45258</v>
       </c>
       <c r="I148">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="J148" t="inlineStr">
         <is>
@@ -15395,13 +15395,13 @@
         <v>45093</v>
       </c>
       <c r="G149">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="H149" s="2">
         <v>45185</v>
       </c>
       <c r="I149">
-        <v>-13</v>
+        <v>-14</v>
       </c>
       <c r="J149" t="inlineStr">
         <is>
@@ -15498,13 +15498,13 @@
         <v>45035</v>
       </c>
       <c r="G150">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="H150" s="2">
         <v>45218</v>
       </c>
       <c r="I150">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="J150" t="inlineStr">
         <is>
@@ -15601,13 +15601,13 @@
         <v>45174</v>
       </c>
       <c r="G151">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="H151" s="2">
         <v>45356</v>
       </c>
       <c r="I151">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="J151" t="inlineStr">
         <is>
@@ -15704,13 +15704,13 @@
         <v>45089</v>
       </c>
       <c r="G152">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="H152" s="2">
         <v>45272</v>
       </c>
       <c r="I152">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="J152" t="inlineStr">
         <is>
@@ -15807,13 +15807,13 @@
         <v>45124</v>
       </c>
       <c r="G153">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="H153" s="2">
         <v>45308</v>
       </c>
       <c r="I153">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="J153" t="inlineStr">
         <is>
@@ -15910,13 +15910,13 @@
         <v>45124</v>
       </c>
       <c r="G154">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="H154" s="2">
         <v>45308</v>
       </c>
       <c r="I154">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="J154" t="inlineStr">
         <is>
@@ -16013,13 +16013,13 @@
         <v>45026</v>
       </c>
       <c r="G155">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="H155" s="2">
         <v>45209</v>
       </c>
       <c r="I155">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="J155" t="inlineStr">
         <is>
@@ -16116,13 +16116,13 @@
         <v>45026</v>
       </c>
       <c r="G156">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="H156" s="2">
         <v>45209</v>
       </c>
       <c r="I156">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="J156" t="inlineStr">
         <is>
@@ -16219,13 +16219,13 @@
         <v>45026</v>
       </c>
       <c r="G157">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="H157" s="2">
         <v>45209</v>
       </c>
       <c r="I157">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="J157" t="inlineStr">
         <is>
@@ -16322,13 +16322,13 @@
         <v>45026</v>
       </c>
       <c r="G158">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="H158" s="2">
         <v>45209</v>
       </c>
       <c r="I158">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="J158" t="inlineStr">
         <is>
@@ -16425,13 +16425,13 @@
         <v>45156</v>
       </c>
       <c r="G159">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="H159" s="2">
         <v>45247</v>
       </c>
       <c r="I159">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="J159" t="inlineStr">
         <is>
@@ -16528,13 +16528,13 @@
         <v>45153</v>
       </c>
       <c r="G160">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="H160" s="2">
         <v>45245</v>
       </c>
       <c r="I160">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="J160" t="inlineStr">
         <is>
@@ -16631,13 +16631,13 @@
         <v>45135</v>
       </c>
       <c r="G161">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="H161" s="2">
         <v>45319</v>
       </c>
       <c r="I161">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="J161" t="inlineStr">
         <is>
@@ -16734,13 +16734,13 @@
         <v>45091</v>
       </c>
       <c r="G162">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="H162" s="2">
         <v>45274</v>
       </c>
       <c r="I162">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="J162" t="inlineStr">
         <is>
@@ -16832,13 +16832,13 @@
         <v>45091</v>
       </c>
       <c r="G163">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="H163" s="2">
         <v>45274</v>
       </c>
       <c r="I163">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="J163" t="inlineStr">
         <is>
@@ -16930,13 +16930,13 @@
         <v>45138</v>
       </c>
       <c r="G164">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="H164" s="2">
         <v>45322</v>
       </c>
       <c r="I164">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="J164" t="inlineStr">
         <is>
@@ -17033,13 +17033,13 @@
         <v>45138</v>
       </c>
       <c r="G165">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="H165" s="2">
         <v>45322</v>
       </c>
       <c r="I165">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="J165" t="inlineStr">
         <is>
@@ -17136,13 +17136,13 @@
         <v>45085</v>
       </c>
       <c r="G166">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="H166" s="2">
         <v>45268</v>
       </c>
       <c r="I166">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="J166" t="inlineStr">
         <is>
@@ -17239,13 +17239,13 @@
         <v>45085</v>
       </c>
       <c r="G167">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="H167" s="2">
         <v>45268</v>
       </c>
       <c r="I167">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="J167" t="inlineStr">
         <is>
@@ -17342,7 +17342,7 @@
         <v>45326</v>
       </c>
       <c r="I168">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="J168" t="inlineStr">
         <is>
@@ -17439,13 +17439,13 @@
         <v>45173</v>
       </c>
       <c r="G169">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="H169" s="2">
         <v>45355</v>
       </c>
       <c r="I169">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="J169" t="inlineStr">
         <is>
@@ -17542,13 +17542,13 @@
         <v>45056</v>
       </c>
       <c r="G170">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="H170" s="2">
         <v>45240</v>
       </c>
       <c r="I170">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="J170" t="inlineStr">
         <is>
@@ -17645,7 +17645,7 @@
         <v>45238</v>
       </c>
       <c r="I171">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="J171" t="inlineStr">
         <is>
@@ -17742,13 +17742,13 @@
         <v>45141</v>
       </c>
       <c r="G172">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="H172" s="2">
         <v>45325</v>
       </c>
       <c r="I172">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="J172" t="inlineStr">
         <is>
@@ -17845,13 +17845,13 @@
         <v>45037</v>
       </c>
       <c r="G173">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="H173" s="2">
         <v>45220</v>
       </c>
       <c r="I173">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="J173" t="inlineStr">
         <is>
@@ -17948,13 +17948,13 @@
         <v>45171</v>
       </c>
       <c r="G174">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="H174" s="2">
         <v>45262</v>
       </c>
       <c r="I174">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="J174" t="inlineStr">
         <is>
@@ -18051,13 +18051,13 @@
         <v>45105</v>
       </c>
       <c r="G175">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="H175" s="2">
         <v>45197</v>
       </c>
       <c r="I175">
-        <v>-1</v>
+        <v>-2</v>
       </c>
       <c r="J175" t="inlineStr">
         <is>
@@ -18154,13 +18154,13 @@
         <v>45162</v>
       </c>
       <c r="G176">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="H176" s="2">
         <v>45254</v>
       </c>
       <c r="I176">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="J176" t="inlineStr">
         <is>
@@ -18257,13 +18257,13 @@
         <v>45061</v>
       </c>
       <c r="G177">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="H177" s="2">
         <v>45245</v>
       </c>
       <c r="I177">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="J177" t="inlineStr">
         <is>
@@ -18360,13 +18360,13 @@
         <v>45120</v>
       </c>
       <c r="G178">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="H178" s="2">
         <v>45212</v>
       </c>
       <c r="I178">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="J178" t="inlineStr">
         <is>
@@ -18463,7 +18463,7 @@
         <v>45191</v>
       </c>
       <c r="I179">
-        <v>-7</v>
+        <v>-8</v>
       </c>
       <c r="J179" t="inlineStr">
         <is>
@@ -18560,13 +18560,13 @@
         <v>45088</v>
       </c>
       <c r="G180">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="H180" s="2">
         <v>45271</v>
       </c>
       <c r="I180">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="J180" t="inlineStr">
         <is>
@@ -18663,13 +18663,13 @@
         <v>45100</v>
       </c>
       <c r="G181">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="H181" s="2">
         <v>45192</v>
       </c>
       <c r="I181">
-        <v>-6</v>
+        <v>-7</v>
       </c>
       <c r="J181" t="inlineStr">
         <is>
@@ -18756,13 +18756,13 @@
         <v>45131</v>
       </c>
       <c r="G182">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="H182" s="2">
         <v>45223</v>
       </c>
       <c r="I182">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="J182" t="inlineStr">
         <is>
@@ -18854,13 +18854,13 @@
         <v>45136</v>
       </c>
       <c r="G183">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="H183" s="2">
         <v>45228</v>
       </c>
       <c r="I183">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="J183" t="inlineStr">
         <is>
@@ -18952,13 +18952,13 @@
         <v>45150</v>
       </c>
       <c r="G184">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="H184" s="2">
         <v>45242</v>
       </c>
       <c r="I184">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="J184" t="inlineStr">
         <is>
@@ -19050,13 +19050,13 @@
         <v>45118</v>
       </c>
       <c r="G185">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="H185" s="2">
         <v>45210</v>
       </c>
       <c r="I185">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="J185" t="inlineStr">
         <is>
@@ -19148,13 +19148,13 @@
         <v>45129</v>
       </c>
       <c r="G186">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="H186" s="2">
         <v>45221</v>
       </c>
       <c r="I186">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="J186" t="inlineStr">
         <is>
@@ -19246,13 +19246,13 @@
         <v>45097</v>
       </c>
       <c r="G187">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="H187" s="2">
         <v>45189</v>
       </c>
       <c r="I187">
-        <v>-9</v>
+        <v>-10</v>
       </c>
       <c r="J187" t="inlineStr">
         <is>
@@ -19339,13 +19339,13 @@
         <v>45101</v>
       </c>
       <c r="G188">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="H188" s="2">
         <v>45193</v>
       </c>
       <c r="I188">
-        <v>-5</v>
+        <v>-6</v>
       </c>
       <c r="J188" t="inlineStr">
         <is>
@@ -19432,13 +19432,13 @@
         <v>45165</v>
       </c>
       <c r="G189">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="H189" s="2">
         <v>45257</v>
       </c>
       <c r="I189">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="J189" t="inlineStr">
         <is>
@@ -19530,7 +19530,7 @@
         <v>45202</v>
       </c>
       <c r="I190">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="J190" t="inlineStr">
         <is>
@@ -19627,13 +19627,13 @@
         <v>45081</v>
       </c>
       <c r="G191">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="H191" s="2">
         <v>45264</v>
       </c>
       <c r="I191">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="J191" t="inlineStr">
         <is>
@@ -19730,13 +19730,13 @@
         <v>45081</v>
       </c>
       <c r="G192">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="H192" s="2">
         <v>45264</v>
       </c>
       <c r="I192">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="J192" t="inlineStr">
         <is>
@@ -19833,7 +19833,7 @@
         <v>45319</v>
       </c>
       <c r="I193">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="J193" t="inlineStr">
         <is>
@@ -19930,7 +19930,7 @@
         <v>45319</v>
       </c>
       <c r="I194">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="J194" t="inlineStr">
         <is>
@@ -20022,13 +20022,13 @@
         <v>45046</v>
       </c>
       <c r="G195">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="H195" s="2">
         <v>45230</v>
       </c>
       <c r="I195">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="J195" t="inlineStr">
         <is>
@@ -20125,13 +20125,13 @@
         <v>45046</v>
       </c>
       <c r="G196">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="H196" s="2">
         <v>45230</v>
       </c>
       <c r="I196">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="J196" t="inlineStr">
         <is>
@@ -20228,13 +20228,13 @@
         <v>45031</v>
       </c>
       <c r="G197">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="H197" s="2">
         <v>45214</v>
       </c>
       <c r="I197">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="J197" t="inlineStr">
         <is>
@@ -20331,13 +20331,13 @@
         <v>45031</v>
       </c>
       <c r="G198">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="H198" s="2">
         <v>45214</v>
       </c>
       <c r="I198">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="J198" t="inlineStr">
         <is>
@@ -20434,13 +20434,13 @@
         <v>45031</v>
       </c>
       <c r="G199">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="H199" s="2">
         <v>45214</v>
       </c>
       <c r="I199">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="J199" t="inlineStr">
         <is>
@@ -20537,13 +20537,13 @@
         <v>45031</v>
       </c>
       <c r="G200">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="H200" s="2">
         <v>45214</v>
       </c>
       <c r="I200">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="J200" t="inlineStr">
         <is>
@@ -20640,13 +20640,13 @@
         <v>45067</v>
       </c>
       <c r="G201">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="H201" s="2">
         <v>45251</v>
       </c>
       <c r="I201">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="J201" t="inlineStr">
         <is>
@@ -20743,13 +20743,13 @@
         <v>45067</v>
       </c>
       <c r="G202">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="H202" s="2">
         <v>45251</v>
       </c>
       <c r="I202">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="J202" t="inlineStr">
         <is>
@@ -20846,13 +20846,13 @@
         <v>45067</v>
       </c>
       <c r="G203">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="H203" s="2">
         <v>45251</v>
       </c>
       <c r="I203">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="J203" t="inlineStr">
         <is>
@@ -20949,13 +20949,13 @@
         <v>45067</v>
       </c>
       <c r="G204">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="H204" s="2">
         <v>45251</v>
       </c>
       <c r="I204">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="J204" t="inlineStr">
         <is>
@@ -21052,13 +21052,13 @@
         <v>45178</v>
       </c>
       <c r="G205">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="H205" s="2">
         <v>45269</v>
       </c>
       <c r="I205">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="J205" t="inlineStr">
         <is>
@@ -21155,7 +21155,7 @@
         <v>45252</v>
       </c>
       <c r="I206">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="J206" t="inlineStr">
         <is>
@@ -21252,13 +21252,13 @@
         <v>45087</v>
       </c>
       <c r="G207">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="H207" s="2">
         <v>45270</v>
       </c>
       <c r="I207">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="J207" t="inlineStr">
         <is>
@@ -21355,13 +21355,13 @@
         <v>45099</v>
       </c>
       <c r="G208">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="H208" s="2">
         <v>45282</v>
       </c>
       <c r="I208">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="J208" t="inlineStr">
         <is>
@@ -21458,13 +21458,13 @@
         <v>45175</v>
       </c>
       <c r="G209">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="H209" s="2">
         <v>45356</v>
       </c>
       <c r="I209">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="J209" t="inlineStr">
         <is>
@@ -21561,13 +21561,13 @@
         <v>45175</v>
       </c>
       <c r="G210">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="H210" s="2">
         <v>45356</v>
       </c>
       <c r="I210">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="J210" t="inlineStr">
         <is>
@@ -21664,13 +21664,13 @@
         <v>45166</v>
       </c>
       <c r="G211">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="H211" s="2">
         <v>45350</v>
       </c>
       <c r="I211">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="J211" t="inlineStr">
         <is>
@@ -21767,13 +21767,13 @@
         <v>45166</v>
       </c>
       <c r="G212">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="H212" s="2">
         <v>45350</v>
       </c>
       <c r="I212">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="J212" t="inlineStr">
         <is>
@@ -21870,13 +21870,13 @@
         <v>45090</v>
       </c>
       <c r="G213">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="H213" s="2">
         <v>45273</v>
       </c>
       <c r="I213">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="J213" t="inlineStr">
         <is>
@@ -21973,13 +21973,13 @@
         <v>45106</v>
       </c>
       <c r="G214">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="H214" s="2">
         <v>45289</v>
       </c>
       <c r="I214">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="J214" t="inlineStr">
         <is>
@@ -22076,13 +22076,13 @@
         <v>45134</v>
       </c>
       <c r="G215">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="H215" s="2">
         <v>45226</v>
       </c>
       <c r="I215">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="J215" t="inlineStr">
         <is>
@@ -22179,13 +22179,13 @@
         <v>45132</v>
       </c>
       <c r="G216">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="H216" s="2">
         <v>45224</v>
       </c>
       <c r="I216">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="J216" t="inlineStr">
         <is>
@@ -22282,13 +22282,13 @@
         <v>45150</v>
       </c>
       <c r="G217">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="H217" s="2">
         <v>45242</v>
       </c>
       <c r="I217">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="J217" t="inlineStr">
         <is>
@@ -22385,13 +22385,13 @@
         <v>45095</v>
       </c>
       <c r="G218">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="H218" s="2">
         <v>45187</v>
       </c>
       <c r="I218">
-        <v>-11</v>
+        <v>-12</v>
       </c>
       <c r="J218" t="inlineStr">
         <is>
@@ -22483,13 +22483,13 @@
         <v>45182</v>
       </c>
       <c r="G219">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="H219" s="2">
         <v>45273</v>
       </c>
       <c r="I219">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="J219" t="inlineStr">
         <is>
@@ -22586,7 +22586,7 @@
         <v>45196</v>
       </c>
       <c r="I220">
-        <v>-2</v>
+        <v>-3</v>
       </c>
       <c r="J220" t="inlineStr">
         <is>
@@ -22683,13 +22683,13 @@
         <v>45108</v>
       </c>
       <c r="G221">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="H221" s="2">
         <v>45200</v>
       </c>
       <c r="I221">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J221" t="inlineStr">
         <is>
@@ -22786,13 +22786,13 @@
         <v>45135</v>
       </c>
       <c r="G222">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="H222" s="2">
         <v>45227</v>
       </c>
       <c r="I222">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="J222" t="inlineStr">
         <is>
@@ -22889,13 +22889,13 @@
         <v>45148</v>
       </c>
       <c r="G223">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="H223" s="2">
         <v>45240</v>
       </c>
       <c r="I223">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="J223" t="inlineStr">
         <is>
@@ -22987,13 +22987,13 @@
         <v>45100</v>
       </c>
       <c r="G224">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="H224" s="2">
         <v>45192</v>
       </c>
       <c r="I224">
-        <v>-6</v>
+        <v>-7</v>
       </c>
       <c r="J224" t="inlineStr">
         <is>
@@ -23085,13 +23085,13 @@
         <v>45136</v>
       </c>
       <c r="G225">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="H225" s="2">
         <v>45320</v>
       </c>
       <c r="I225">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="J225" t="inlineStr">
         <is>
@@ -23188,13 +23188,13 @@
         <v>45136</v>
       </c>
       <c r="G226">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="H226" s="2">
         <v>45320</v>
       </c>
       <c r="I226">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="J226" t="inlineStr">
         <is>
@@ -23291,13 +23291,13 @@
         <v>45094</v>
       </c>
       <c r="G227">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="H227" s="2">
         <v>45277</v>
       </c>
       <c r="I227">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="J227" t="inlineStr">
         <is>
@@ -23394,13 +23394,13 @@
         <v>45081</v>
       </c>
       <c r="G228">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="H228" s="2">
         <v>45264</v>
       </c>
       <c r="I228">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="J228" t="inlineStr">
         <is>
@@ -23497,13 +23497,13 @@
         <v>45099</v>
       </c>
       <c r="G229">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="H229" s="2">
         <v>45282</v>
       </c>
       <c r="I229">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="J229" t="inlineStr">
         <is>
@@ -23600,13 +23600,13 @@
         <v>45018</v>
       </c>
       <c r="G230">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="H230" s="2">
         <v>45201</v>
       </c>
       <c r="I230">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="J230" t="inlineStr">
         <is>
@@ -23703,13 +23703,13 @@
         <v>45031</v>
       </c>
       <c r="G231">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="H231" s="2">
         <v>45214</v>
       </c>
       <c r="I231">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="J231" t="inlineStr">
         <is>
@@ -23806,7 +23806,7 @@
         <v>45294</v>
       </c>
       <c r="I232">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="J232" t="inlineStr">
         <is>
@@ -23903,13 +23903,13 @@
         <v>45079</v>
       </c>
       <c r="G233">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="H233" s="2">
         <v>45262</v>
       </c>
       <c r="I233">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="J233" t="inlineStr">
         <is>
@@ -24006,7 +24006,7 @@
         <v>45199</v>
       </c>
       <c r="I234">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J234" t="inlineStr">
         <is>
@@ -24103,13 +24103,13 @@
         <v>45021</v>
       </c>
       <c r="G235">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="H235" s="2">
         <v>45204</v>
       </c>
       <c r="I235">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="J235" t="inlineStr">
         <is>
@@ -24206,13 +24206,13 @@
         <v>45021</v>
       </c>
       <c r="G236">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="H236" s="2">
         <v>45204</v>
       </c>
       <c r="I236">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="J236" t="inlineStr">
         <is>
@@ -24309,13 +24309,13 @@
         <v>45080</v>
       </c>
       <c r="G237">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="H237" s="2">
         <v>45263</v>
       </c>
       <c r="I237">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="J237" t="inlineStr">
         <is>
@@ -24412,13 +24412,13 @@
         <v>45046</v>
       </c>
       <c r="G238">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="H238" s="2">
         <v>45229</v>
       </c>
       <c r="I238">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="J238" t="inlineStr">
         <is>
@@ -24515,13 +24515,13 @@
         <v>45112</v>
       </c>
       <c r="G239">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="H239" s="2">
         <v>45204</v>
       </c>
       <c r="I239">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="J239" t="inlineStr">
         <is>
@@ -24609,13 +24609,13 @@
         <v>45112</v>
       </c>
       <c r="G240">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="H240" s="2">
         <v>45204</v>
       </c>
       <c r="I240">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="J240" t="inlineStr">
         <is>
@@ -24703,13 +24703,13 @@
         <v>45016</v>
       </c>
       <c r="G241">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="H241" s="2">
         <v>45199</v>
       </c>
       <c r="I241">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J241" t="inlineStr">
         <is>
@@ -24806,13 +24806,13 @@
         <v>45070</v>
       </c>
       <c r="G242">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="H242" s="2">
         <v>45254</v>
       </c>
       <c r="I242">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="J242" t="inlineStr">
         <is>
@@ -24909,13 +24909,13 @@
         <v>45168</v>
       </c>
       <c r="G243">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="H243" s="2">
         <v>45260</v>
       </c>
       <c r="I243">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="J243" t="inlineStr">
         <is>
@@ -25012,13 +25012,13 @@
         <v>45027</v>
       </c>
       <c r="G244">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="H244" s="2">
         <v>45210</v>
       </c>
       <c r="I244">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="J244" t="inlineStr">
         <is>
@@ -25115,13 +25115,13 @@
         <v>45077</v>
       </c>
       <c r="G245">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="H245" s="2">
         <v>45260</v>
       </c>
       <c r="I245">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="J245" t="inlineStr">
         <is>
@@ -25218,13 +25218,13 @@
         <v>45100</v>
       </c>
       <c r="G246">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="H246" s="2">
         <v>45283</v>
       </c>
       <c r="I246">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="J246" t="inlineStr">
         <is>
@@ -25321,7 +25321,7 @@
         <v>45281</v>
       </c>
       <c r="I247">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="J247" t="inlineStr">
         <is>
@@ -25418,13 +25418,13 @@
         <v>45044</v>
       </c>
       <c r="G248">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="H248" s="2">
         <v>45227</v>
       </c>
       <c r="I248">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="J248" t="inlineStr">
         <is>
@@ -25521,13 +25521,13 @@
         <v>45101</v>
       </c>
       <c r="G249">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="H249" s="2">
         <v>45283</v>
       </c>
       <c r="I249">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="J249" t="inlineStr">
         <is>
@@ -25624,13 +25624,13 @@
         <v>45134</v>
       </c>
       <c r="G250">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="H250" s="2">
         <v>45226</v>
       </c>
       <c r="I250">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="J250" t="inlineStr">
         <is>
@@ -25727,13 +25727,13 @@
         <v>45158</v>
       </c>
       <c r="G251">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="H251" s="2">
         <v>45250</v>
       </c>
       <c r="I251">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="J251" t="inlineStr">
         <is>
@@ -25830,13 +25830,13 @@
         <v>45108</v>
       </c>
       <c r="G252">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="H252" s="2">
         <v>45200</v>
       </c>
       <c r="I252">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J252" t="inlineStr">
         <is>
@@ -25933,7 +25933,7 @@
         <v>45317</v>
       </c>
       <c r="I253">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="J253" t="inlineStr">
         <is>
@@ -26030,13 +26030,13 @@
         <v>45039</v>
       </c>
       <c r="G254">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="H254" s="2">
         <v>45222</v>
       </c>
       <c r="I254">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="J254" t="inlineStr">
         <is>
@@ -26128,13 +26128,13 @@
         <v>45129</v>
       </c>
       <c r="G255">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="H255" s="2">
         <v>45221</v>
       </c>
       <c r="I255">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="J255" t="inlineStr">
         <is>
@@ -26231,13 +26231,13 @@
         <v>45157</v>
       </c>
       <c r="G256">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="H256" s="2">
         <v>45341</v>
       </c>
       <c r="I256">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="J256" t="inlineStr">
         <is>
@@ -26334,13 +26334,13 @@
         <v>45063</v>
       </c>
       <c r="G257">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="H257" s="2">
         <v>45247</v>
       </c>
       <c r="I257">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="J257" t="inlineStr">
         <is>
@@ -26437,7 +26437,7 @@
         <v>45254</v>
       </c>
       <c r="I258">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="J258" t="inlineStr">
         <is>
@@ -26534,7 +26534,7 @@
         <v>45486</v>
       </c>
       <c r="I259">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="J259" t="inlineStr">
         <is>
@@ -26626,13 +26626,13 @@
         <v>45073</v>
       </c>
       <c r="G260">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="H260" s="2">
         <v>45439</v>
       </c>
       <c r="I260">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="J260" t="inlineStr">
         <is>
@@ -26724,7 +26724,7 @@
         <v>45323</v>
       </c>
       <c r="I261">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="J261" t="inlineStr">
         <is>
@@ -26816,7 +26816,7 @@
         <v>45303</v>
       </c>
       <c r="I262">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="J262" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
Bond dates update Sun Oct  1 23:10:51 UTC 2023
</commit_message>
<xml_diff>
--- a/Data/obligacje_screener.xlsx
+++ b/Data/obligacje_screener.xlsx
@@ -512,7 +512,7 @@
         <v>45340</v>
       </c>
       <c r="I2">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="J2" t="inlineStr">
         <is>
@@ -600,13 +600,13 @@
         <v>45121</v>
       </c>
       <c r="G3">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="H3" s="2">
         <v>45305</v>
       </c>
       <c r="I3">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="J3" t="inlineStr">
         <is>
@@ -703,13 +703,13 @@
         <v>45039</v>
       </c>
       <c r="G4">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="H4" s="2">
         <v>45222</v>
       </c>
       <c r="I4">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="J4" t="inlineStr">
         <is>
@@ -806,13 +806,13 @@
         <v>45039</v>
       </c>
       <c r="G5">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="H5" s="2">
         <v>45222</v>
       </c>
       <c r="I5">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="J5" t="inlineStr">
         <is>
@@ -909,13 +909,13 @@
         <v>45129</v>
       </c>
       <c r="G6">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="H6" s="2">
         <v>45221</v>
       </c>
       <c r="I6">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="J6" t="inlineStr">
         <is>
@@ -1012,13 +1012,13 @@
         <v>45162</v>
       </c>
       <c r="G7">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="H7" s="2">
         <v>45254</v>
       </c>
       <c r="I7">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="J7" t="inlineStr">
         <is>
@@ -1110,13 +1110,13 @@
         <v>45156</v>
       </c>
       <c r="G8">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="H8" s="2">
         <v>45248</v>
       </c>
       <c r="I8">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="J8" t="inlineStr">
         <is>
@@ -1213,13 +1213,13 @@
         <v>45141</v>
       </c>
       <c r="G9">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="H9" s="2">
         <v>45233</v>
       </c>
       <c r="I9">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="J9" t="inlineStr">
         <is>
@@ -1316,13 +1316,13 @@
         <v>45062</v>
       </c>
       <c r="G10">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="H10" s="2">
         <v>45246</v>
       </c>
       <c r="I10">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="J10" t="inlineStr">
         <is>
@@ -1419,7 +1419,7 @@
         <v>45286</v>
       </c>
       <c r="I11">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="J11" t="inlineStr">
         <is>
@@ -1516,13 +1516,13 @@
         <v>45011</v>
       </c>
       <c r="G12">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="H12" s="2">
         <v>45195</v>
       </c>
       <c r="I12">
-        <v>-4</v>
+        <v>-5</v>
       </c>
       <c r="J12" t="inlineStr">
         <is>
@@ -1614,13 +1614,13 @@
         <v>45036</v>
       </c>
       <c r="G13">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="H13" s="2">
         <v>45219</v>
       </c>
       <c r="I13">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="J13" t="inlineStr">
         <is>
@@ -1717,13 +1717,13 @@
         <v>45036</v>
       </c>
       <c r="G14">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="H14" s="2">
         <v>45219</v>
       </c>
       <c r="I14">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="J14" t="inlineStr">
         <is>
@@ -1820,13 +1820,13 @@
         <v>45106</v>
       </c>
       <c r="G15">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="H15" s="2">
         <v>45289</v>
       </c>
       <c r="I15">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="J15" t="inlineStr">
         <is>
@@ -1923,13 +1923,13 @@
         <v>45094</v>
       </c>
       <c r="G16">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="H16" s="2">
         <v>45186</v>
       </c>
       <c r="I16">
-        <v>-13</v>
+        <v>-14</v>
       </c>
       <c r="J16" t="inlineStr">
         <is>
@@ -2026,13 +2026,13 @@
         <v>45094</v>
       </c>
       <c r="G17">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="H17" s="2">
         <v>45186</v>
       </c>
       <c r="I17">
-        <v>-13</v>
+        <v>-14</v>
       </c>
       <c r="J17" t="inlineStr">
         <is>
@@ -2129,13 +2129,13 @@
         <v>45132</v>
       </c>
       <c r="G18">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="H18" s="2">
         <v>45224</v>
       </c>
       <c r="I18">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="J18" t="inlineStr">
         <is>
@@ -2232,13 +2232,13 @@
         <v>45137</v>
       </c>
       <c r="G19">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="H19" s="2">
         <v>45229</v>
       </c>
       <c r="I19">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="J19" t="inlineStr">
         <is>
@@ -2330,13 +2330,13 @@
         <v>45183</v>
       </c>
       <c r="G20">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="H20" s="2">
         <v>45274</v>
       </c>
       <c r="I20">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="J20" t="inlineStr">
         <is>
@@ -2433,13 +2433,13 @@
         <v>45093</v>
       </c>
       <c r="G21">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="H21" s="2">
         <v>45187</v>
       </c>
       <c r="I21">
-        <v>-12</v>
+        <v>-13</v>
       </c>
       <c r="J21" t="inlineStr">
         <is>
@@ -2536,13 +2536,13 @@
         <v>45096</v>
       </c>
       <c r="G22">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="H22" s="2">
         <v>45187</v>
       </c>
       <c r="I22">
-        <v>-12</v>
+        <v>-13</v>
       </c>
       <c r="J22" t="inlineStr">
         <is>
@@ -2639,7 +2639,7 @@
         <v>45245</v>
       </c>
       <c r="I23">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="J23" t="inlineStr">
         <is>
@@ -2736,7 +2736,7 @@
         <v>45245</v>
       </c>
       <c r="I24">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="J24" t="inlineStr">
         <is>
@@ -2833,13 +2833,13 @@
         <v>45021</v>
       </c>
       <c r="G25">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="H25" s="2">
         <v>45204</v>
       </c>
       <c r="I25">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="J25" t="inlineStr">
         <is>
@@ -2936,13 +2936,13 @@
         <v>45160</v>
       </c>
       <c r="G26">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="H26" s="2">
         <v>45344</v>
       </c>
       <c r="I26">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="J26" t="inlineStr">
         <is>
@@ -3039,13 +3039,13 @@
         <v>45118</v>
       </c>
       <c r="G27">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="H27" s="2">
         <v>45302</v>
       </c>
       <c r="I27">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="J27" t="inlineStr">
         <is>
@@ -3142,13 +3142,13 @@
         <v>45085</v>
       </c>
       <c r="G28">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="H28" s="2">
         <v>45268</v>
       </c>
       <c r="I28">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="J28" t="inlineStr">
         <is>
@@ -3245,13 +3245,13 @@
         <v>45183</v>
       </c>
       <c r="G29">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="H29" s="2">
         <v>45274</v>
       </c>
       <c r="I29">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="J29" t="inlineStr">
         <is>
@@ -3348,7 +3348,7 @@
         <v>45224</v>
       </c>
       <c r="I30">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="J30" t="inlineStr">
         <is>
@@ -3445,13 +3445,13 @@
         <v>45153</v>
       </c>
       <c r="G31">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="H31" s="2">
         <v>45245</v>
       </c>
       <c r="I31">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="J31" t="inlineStr">
         <is>
@@ -3548,13 +3548,13 @@
         <v>45155</v>
       </c>
       <c r="G32">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="H32" s="2">
         <v>45247</v>
       </c>
       <c r="I32">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="J32" t="inlineStr">
         <is>
@@ -3651,7 +3651,7 @@
         <v>45255</v>
       </c>
       <c r="I33">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="J33" t="inlineStr">
         <is>
@@ -3739,13 +3739,13 @@
         <v>45176</v>
       </c>
       <c r="G34">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="H34" s="2">
         <v>45267</v>
       </c>
       <c r="I34">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="J34" t="inlineStr">
         <is>
@@ -3842,13 +3842,13 @@
         <v>45130</v>
       </c>
       <c r="G35">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="H35" s="2">
         <v>45222</v>
       </c>
       <c r="I35">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="J35" t="inlineStr">
         <is>
@@ -3940,13 +3940,13 @@
         <v>45115</v>
       </c>
       <c r="G36">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="H36" s="2">
         <v>45207</v>
       </c>
       <c r="I36">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="J36" t="inlineStr">
         <is>
@@ -4043,13 +4043,13 @@
         <v>45097</v>
       </c>
       <c r="G37">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="H37" s="2">
         <v>45189</v>
       </c>
       <c r="I37">
-        <v>-10</v>
+        <v>-11</v>
       </c>
       <c r="J37" t="inlineStr">
         <is>
@@ -4141,13 +4141,13 @@
         <v>45107</v>
       </c>
       <c r="G38">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="H38" s="2">
         <v>45290</v>
       </c>
       <c r="I38">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="J38" t="inlineStr">
         <is>
@@ -4244,13 +4244,13 @@
         <v>45063</v>
       </c>
       <c r="G39">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="H39" s="2">
         <v>45247</v>
       </c>
       <c r="I39">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="J39" t="inlineStr">
         <is>
@@ -4347,13 +4347,13 @@
         <v>45177</v>
       </c>
       <c r="G40">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="H40" s="2">
         <v>45359</v>
       </c>
       <c r="I40">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="J40" t="inlineStr">
         <is>
@@ -4450,13 +4450,13 @@
         <v>45107</v>
       </c>
       <c r="G41">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="H41" s="2">
         <v>45290</v>
       </c>
       <c r="I41">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="J41" t="inlineStr">
         <is>
@@ -4553,7 +4553,7 @@
         <v>45265</v>
       </c>
       <c r="I42">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="J42" t="inlineStr">
         <is>
@@ -4650,13 +4650,13 @@
         <v>45098</v>
       </c>
       <c r="G43">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="H43" s="2">
         <v>45281</v>
       </c>
       <c r="I43">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="J43" t="inlineStr">
         <is>
@@ -4753,13 +4753,13 @@
         <v>45099</v>
       </c>
       <c r="G44">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="H44" s="2">
         <v>45282</v>
       </c>
       <c r="I44">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="J44" t="inlineStr">
         <is>
@@ -4856,13 +4856,13 @@
         <v>45106</v>
       </c>
       <c r="G45">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="H45" s="2">
         <v>45289</v>
       </c>
       <c r="I45">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="J45" t="inlineStr">
         <is>
@@ -4959,13 +4959,13 @@
         <v>45106</v>
       </c>
       <c r="G46">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="H46" s="2">
         <v>45289</v>
       </c>
       <c r="I46">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="J46" t="inlineStr">
         <is>
@@ -5062,13 +5062,13 @@
         <v>45120</v>
       </c>
       <c r="G47">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="H47" s="2">
         <v>45304</v>
       </c>
       <c r="I47">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="J47" t="inlineStr">
         <is>
@@ -5165,13 +5165,13 @@
         <v>45118</v>
       </c>
       <c r="G48">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="H48" s="2">
         <v>45302</v>
       </c>
       <c r="I48">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="J48" t="inlineStr">
         <is>
@@ -5268,13 +5268,13 @@
         <v>45152</v>
       </c>
       <c r="G49">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="H49" s="2">
         <v>45336</v>
       </c>
       <c r="I49">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="J49" t="inlineStr">
         <is>
@@ -5371,13 +5371,13 @@
         <v>45042</v>
       </c>
       <c r="G50">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="H50" s="2">
         <v>45225</v>
       </c>
       <c r="I50">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="J50" t="inlineStr">
         <is>
@@ -5474,13 +5474,13 @@
         <v>45122</v>
       </c>
       <c r="G51">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="H51" s="2">
         <v>45306</v>
       </c>
       <c r="I51">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="J51" t="inlineStr">
         <is>
@@ -5577,13 +5577,13 @@
         <v>45139</v>
       </c>
       <c r="G52">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="H52" s="2">
         <v>45323</v>
       </c>
       <c r="I52">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="J52" t="inlineStr">
         <is>
@@ -5671,13 +5671,13 @@
         <v>45099</v>
       </c>
       <c r="G53">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="H53" s="2">
         <v>45282</v>
       </c>
       <c r="I53">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="J53" t="inlineStr">
         <is>
@@ -5774,7 +5774,7 @@
         <v>45196</v>
       </c>
       <c r="I54">
-        <v>-3</v>
+        <v>-4</v>
       </c>
       <c r="J54" t="inlineStr">
         <is>
@@ -5871,13 +5871,13 @@
         <v>45044</v>
       </c>
       <c r="G55">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="H55" s="2">
         <v>45227</v>
       </c>
       <c r="I55">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="J55" t="inlineStr">
         <is>
@@ -5974,13 +5974,13 @@
         <v>45151</v>
       </c>
       <c r="G56">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="H56" s="2">
         <v>45243</v>
       </c>
       <c r="I56">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="J56" t="inlineStr">
         <is>
@@ -6072,7 +6072,7 @@
         <v>45196</v>
       </c>
       <c r="I57">
-        <v>-3</v>
+        <v>-4</v>
       </c>
       <c r="J57" t="inlineStr">
         <is>
@@ -6169,13 +6169,13 @@
         <v>45069</v>
       </c>
       <c r="G58">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="H58" s="2">
         <v>45253</v>
       </c>
       <c r="I58">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="J58" t="inlineStr">
         <is>
@@ -6272,13 +6272,13 @@
         <v>45099</v>
       </c>
       <c r="G59">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="H59" s="2">
         <v>45191</v>
       </c>
       <c r="I59">
-        <v>-8</v>
+        <v>-9</v>
       </c>
       <c r="J59" t="inlineStr">
         <is>
@@ -6370,13 +6370,13 @@
         <v>45113</v>
       </c>
       <c r="G60">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="H60" s="2">
         <v>45205</v>
       </c>
       <c r="I60">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="J60" t="inlineStr">
         <is>
@@ -6473,13 +6473,13 @@
         <v>45127</v>
       </c>
       <c r="G61">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="H61" s="2">
         <v>45219</v>
       </c>
       <c r="I61">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="J61" t="inlineStr">
         <is>
@@ -6576,13 +6576,13 @@
         <v>45058</v>
       </c>
       <c r="G62">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="H62" s="2">
         <v>45242</v>
       </c>
       <c r="I62">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="J62" t="inlineStr">
         <is>
@@ -6679,13 +6679,13 @@
         <v>45010</v>
       </c>
       <c r="G63">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="H63" s="2">
         <v>45194</v>
       </c>
       <c r="I63">
-        <v>-5</v>
+        <v>-6</v>
       </c>
       <c r="J63" t="inlineStr">
         <is>
@@ -6777,13 +6777,13 @@
         <v>45025</v>
       </c>
       <c r="G64">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="H64" s="2">
         <v>45208</v>
       </c>
       <c r="I64">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="J64" t="inlineStr">
         <is>
@@ -6880,13 +6880,13 @@
         <v>45025</v>
       </c>
       <c r="G65">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="H65" s="2">
         <v>45208</v>
       </c>
       <c r="I65">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="J65" t="inlineStr">
         <is>
@@ -6983,13 +6983,13 @@
         <v>45089</v>
       </c>
       <c r="G66">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="H66" s="2">
         <v>45272</v>
       </c>
       <c r="I66">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="J66" t="inlineStr">
         <is>
@@ -7086,13 +7086,13 @@
         <v>45178</v>
       </c>
       <c r="G67">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="H67" s="2">
         <v>45269</v>
       </c>
       <c r="I67">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="J67" t="inlineStr">
         <is>
@@ -7184,13 +7184,13 @@
         <v>45104</v>
       </c>
       <c r="G68">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="H68" s="2">
         <v>45196</v>
       </c>
       <c r="I68">
-        <v>-3</v>
+        <v>-4</v>
       </c>
       <c r="J68" t="inlineStr">
         <is>
@@ -7287,13 +7287,13 @@
         <v>45149</v>
       </c>
       <c r="G69">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="H69" s="2">
         <v>45241</v>
       </c>
       <c r="I69">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="J69" t="inlineStr">
         <is>
@@ -7390,7 +7390,7 @@
         <v>45205</v>
       </c>
       <c r="I70">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="J70" t="inlineStr">
         <is>
@@ -7487,13 +7487,13 @@
         <v>45114</v>
       </c>
       <c r="G71">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="H71" s="2">
         <v>45205</v>
       </c>
       <c r="I71">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="J71" t="inlineStr">
         <is>
@@ -7590,13 +7590,13 @@
         <v>45115</v>
       </c>
       <c r="G72">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="H72" s="2">
         <v>45207</v>
       </c>
       <c r="I72">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="J72" t="inlineStr">
         <is>
@@ -7693,13 +7693,13 @@
         <v>45097</v>
       </c>
       <c r="G73">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="H73" s="2">
         <v>45189</v>
       </c>
       <c r="I73">
-        <v>-10</v>
+        <v>-11</v>
       </c>
       <c r="J73" t="inlineStr">
         <is>
@@ -7791,13 +7791,13 @@
         <v>45038</v>
       </c>
       <c r="G74">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="H74" s="2">
         <v>45221</v>
       </c>
       <c r="I74">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="J74" t="inlineStr">
         <is>
@@ -7889,13 +7889,13 @@
         <v>45117</v>
       </c>
       <c r="G75">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="H75" s="2">
         <v>45301</v>
       </c>
       <c r="I75">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="J75" t="inlineStr">
         <is>
@@ -7992,13 +7992,13 @@
         <v>45160</v>
       </c>
       <c r="G76">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="H76" s="2">
         <v>45344</v>
       </c>
       <c r="I76">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="J76" t="inlineStr">
         <is>
@@ -8095,13 +8095,13 @@
         <v>45002</v>
       </c>
       <c r="G77">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="H77" s="2">
         <v>45186</v>
       </c>
       <c r="I77">
-        <v>-13</v>
+        <v>-14</v>
       </c>
       <c r="J77" t="inlineStr">
         <is>
@@ -8198,13 +8198,13 @@
         <v>45043</v>
       </c>
       <c r="G78">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="H78" s="2">
         <v>45226</v>
       </c>
       <c r="I78">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="J78" t="inlineStr">
         <is>
@@ -8301,13 +8301,13 @@
         <v>45079</v>
       </c>
       <c r="G79">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="H79" s="2">
         <v>45262</v>
       </c>
       <c r="I79">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="J79" t="inlineStr">
         <is>
@@ -8404,7 +8404,7 @@
         <v>45254</v>
       </c>
       <c r="I80">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="J80" t="inlineStr">
         <is>
@@ -8501,13 +8501,13 @@
         <v>45104</v>
       </c>
       <c r="G81">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="H81" s="2">
         <v>45287</v>
       </c>
       <c r="I81">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="J81" t="inlineStr">
         <is>
@@ -8604,7 +8604,7 @@
         <v>45288</v>
       </c>
       <c r="I82">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="J82" t="inlineStr">
         <is>
@@ -8696,13 +8696,13 @@
         <v>45175</v>
       </c>
       <c r="G83">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="H83" s="2">
         <v>45357</v>
       </c>
       <c r="I83">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="J83" t="inlineStr">
         <is>
@@ -8799,13 +8799,13 @@
         <v>45054</v>
       </c>
       <c r="G84">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="H84" s="2">
         <v>45238</v>
       </c>
       <c r="I84">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="J84" t="inlineStr">
         <is>
@@ -8902,13 +8902,13 @@
         <v>45056</v>
       </c>
       <c r="G85">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="H85" s="2">
         <v>45240</v>
       </c>
       <c r="I85">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="J85" t="inlineStr">
         <is>
@@ -9005,13 +9005,13 @@
         <v>45085</v>
       </c>
       <c r="G86">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="H86" s="2">
         <v>45268</v>
       </c>
       <c r="I86">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="J86" t="inlineStr">
         <is>
@@ -9108,7 +9108,7 @@
         <v>45194</v>
       </c>
       <c r="I87">
-        <v>-5</v>
+        <v>-6</v>
       </c>
       <c r="J87" t="inlineStr">
         <is>
@@ -9195,13 +9195,13 @@
         <v>45103</v>
       </c>
       <c r="G88">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="H88" s="2">
         <v>45286</v>
       </c>
       <c r="I88">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="J88" t="inlineStr">
         <is>
@@ -9298,13 +9298,13 @@
         <v>45103</v>
       </c>
       <c r="G89">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="H89" s="2">
         <v>45286</v>
       </c>
       <c r="I89">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="J89" t="inlineStr">
         <is>
@@ -9401,13 +9401,13 @@
         <v>45008</v>
       </c>
       <c r="G90">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="H90" s="2">
         <v>45192</v>
       </c>
       <c r="I90">
-        <v>-7</v>
+        <v>-8</v>
       </c>
       <c r="J90" t="inlineStr">
         <is>
@@ -9499,13 +9499,13 @@
         <v>45100</v>
       </c>
       <c r="G91">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="H91" s="2">
         <v>45287</v>
       </c>
       <c r="I91">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="J91" t="inlineStr">
         <is>
@@ -9602,13 +9602,13 @@
         <v>45003</v>
       </c>
       <c r="G92">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="H92" s="2">
         <v>45187</v>
       </c>
       <c r="I92">
-        <v>-12</v>
+        <v>-13</v>
       </c>
       <c r="J92" t="inlineStr">
         <is>
@@ -9705,13 +9705,13 @@
         <v>45104</v>
       </c>
       <c r="G93">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="H93" s="2">
         <v>45287</v>
       </c>
       <c r="I93">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="J93" t="inlineStr">
         <is>
@@ -9808,13 +9808,13 @@
         <v>45104</v>
       </c>
       <c r="G94">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="H94" s="2">
         <v>45287</v>
       </c>
       <c r="I94">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="J94" t="inlineStr">
         <is>
@@ -9911,13 +9911,13 @@
         <v>45049</v>
       </c>
       <c r="G95">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="H95" s="2">
         <v>45233</v>
       </c>
       <c r="I95">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="J95" t="inlineStr">
         <is>
@@ -10014,13 +10014,13 @@
         <v>45122</v>
       </c>
       <c r="G96">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="H96" s="2">
         <v>45306</v>
       </c>
       <c r="I96">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="J96" t="inlineStr">
         <is>
@@ -10112,13 +10112,13 @@
         <v>45141</v>
       </c>
       <c r="G97">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="H97" s="2">
         <v>45325</v>
       </c>
       <c r="I97">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="J97" t="inlineStr">
         <is>
@@ -10215,13 +10215,13 @@
         <v>45010</v>
       </c>
       <c r="G98">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="H98" s="2">
         <v>45194</v>
       </c>
       <c r="I98">
-        <v>-5</v>
+        <v>-6</v>
       </c>
       <c r="J98" t="inlineStr">
         <is>
@@ -10313,13 +10313,13 @@
         <v>45093</v>
       </c>
       <c r="G99">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="H99" s="2">
         <v>45276</v>
       </c>
       <c r="I99">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="J99" t="inlineStr">
         <is>
@@ -10416,13 +10416,13 @@
         <v>45123</v>
       </c>
       <c r="G100">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="H100" s="2">
         <v>45307</v>
       </c>
       <c r="I100">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="J100" t="inlineStr">
         <is>
@@ -10519,13 +10519,13 @@
         <v>45014</v>
       </c>
       <c r="G101">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="H101" s="2">
         <v>45198</v>
       </c>
       <c r="I101">
-        <v>-1</v>
+        <v>-2</v>
       </c>
       <c r="J101" t="inlineStr">
         <is>
@@ -10622,13 +10622,13 @@
         <v>45093</v>
       </c>
       <c r="G102">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="H102" s="2">
         <v>45276</v>
       </c>
       <c r="I102">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="J102" t="inlineStr">
         <is>
@@ -10725,13 +10725,13 @@
         <v>45122</v>
       </c>
       <c r="G103">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="H103" s="2">
         <v>45306</v>
       </c>
       <c r="I103">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="J103" t="inlineStr">
         <is>
@@ -10828,13 +10828,13 @@
         <v>45122</v>
       </c>
       <c r="G104">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="H104" s="2">
         <v>45306</v>
       </c>
       <c r="I104">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="J104" t="inlineStr">
         <is>
@@ -10926,13 +10926,13 @@
         <v>45050</v>
       </c>
       <c r="G105">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="H105" s="2">
         <v>45234</v>
       </c>
       <c r="I105">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="J105" t="inlineStr">
         <is>
@@ -11029,13 +11029,13 @@
         <v>45085</v>
       </c>
       <c r="G106">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="H106" s="2">
         <v>45268</v>
       </c>
       <c r="I106">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="J106" t="inlineStr">
         <is>
@@ -11132,13 +11132,13 @@
         <v>45093</v>
       </c>
       <c r="G107">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="H107" s="2">
         <v>45185</v>
       </c>
       <c r="I107">
-        <v>-14</v>
+        <v>-15</v>
       </c>
       <c r="J107" t="inlineStr">
         <is>
@@ -11230,13 +11230,13 @@
         <v>45093</v>
       </c>
       <c r="G108">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="H108" s="2">
         <v>45185</v>
       </c>
       <c r="I108">
-        <v>-14</v>
+        <v>-15</v>
       </c>
       <c r="J108" t="inlineStr">
         <is>
@@ -11328,13 +11328,13 @@
         <v>45093</v>
       </c>
       <c r="G109">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="H109" s="2">
         <v>45185</v>
       </c>
       <c r="I109">
-        <v>-14</v>
+        <v>-15</v>
       </c>
       <c r="J109" t="inlineStr">
         <is>
@@ -11431,13 +11431,13 @@
         <v>45148</v>
       </c>
       <c r="G110">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="H110" s="2">
         <v>45240</v>
       </c>
       <c r="I110">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="J110" t="inlineStr">
         <is>
@@ -11534,13 +11534,13 @@
         <v>45119</v>
       </c>
       <c r="G111">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="H111" s="2">
         <v>45211</v>
       </c>
       <c r="I111">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="J111" t="inlineStr">
         <is>
@@ -11637,13 +11637,13 @@
         <v>45172</v>
       </c>
       <c r="G112">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="H112" s="2">
         <v>45263</v>
       </c>
       <c r="I112">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="J112" t="inlineStr">
         <is>
@@ -11740,13 +11740,13 @@
         <v>45023</v>
       </c>
       <c r="G113">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="H113" s="2">
         <v>45206</v>
       </c>
       <c r="I113">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="J113" t="inlineStr">
         <is>
@@ -11843,13 +11843,13 @@
         <v>45111</v>
       </c>
       <c r="G114">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="H114" s="2">
         <v>45203</v>
       </c>
       <c r="I114">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="J114" t="inlineStr">
         <is>
@@ -11946,7 +11946,7 @@
         <v>45218</v>
       </c>
       <c r="I115">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="J115" t="inlineStr">
         <is>
@@ -12043,13 +12043,13 @@
         <v>45161</v>
       </c>
       <c r="G116">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="H116" s="2">
         <v>45253</v>
       </c>
       <c r="I116">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="J116" t="inlineStr">
         <is>
@@ -12146,13 +12146,13 @@
         <v>45115</v>
       </c>
       <c r="G117">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="H117" s="2">
         <v>45299</v>
       </c>
       <c r="I117">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="J117" t="inlineStr">
         <is>
@@ -12244,13 +12244,13 @@
         <v>45094</v>
       </c>
       <c r="G118">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="H118" s="2">
         <v>45277</v>
       </c>
       <c r="I118">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="J118" t="inlineStr">
         <is>
@@ -12347,13 +12347,13 @@
         <v>45104</v>
       </c>
       <c r="G119">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="H119" s="2">
         <v>45287</v>
       </c>
       <c r="I119">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="J119" t="inlineStr">
         <is>
@@ -12450,13 +12450,13 @@
         <v>45104</v>
       </c>
       <c r="G120">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="H120" s="2">
         <v>45287</v>
       </c>
       <c r="I120">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="J120" t="inlineStr">
         <is>
@@ -12553,13 +12553,13 @@
         <v>45104</v>
       </c>
       <c r="G121">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="H121" s="2">
         <v>45287</v>
       </c>
       <c r="I121">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="J121" t="inlineStr">
         <is>
@@ -12656,13 +12656,13 @@
         <v>45104</v>
       </c>
       <c r="G122">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="H122" s="2">
         <v>45287</v>
       </c>
       <c r="I122">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="J122" t="inlineStr">
         <is>
@@ -12759,13 +12759,13 @@
         <v>45107</v>
       </c>
       <c r="G123">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="H123" s="2">
         <v>45199</v>
       </c>
       <c r="I123">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="J123" t="inlineStr">
         <is>
@@ -12862,13 +12862,13 @@
         <v>45013</v>
       </c>
       <c r="G124">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="H124" s="2">
         <v>45197</v>
       </c>
       <c r="I124">
-        <v>-2</v>
+        <v>-3</v>
       </c>
       <c r="J124" t="inlineStr">
         <is>
@@ -12965,13 +12965,13 @@
         <v>45121</v>
       </c>
       <c r="G125">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="H125" s="2">
         <v>45213</v>
       </c>
       <c r="I125">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="J125" t="inlineStr">
         <is>
@@ -13068,13 +13068,13 @@
         <v>45134</v>
       </c>
       <c r="G126">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="H126" s="2">
         <v>45226</v>
       </c>
       <c r="I126">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="J126" t="inlineStr">
         <is>
@@ -13171,7 +13171,7 @@
         <v>45212</v>
       </c>
       <c r="I127">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="J127" t="inlineStr">
         <is>
@@ -13268,13 +13268,13 @@
         <v>45126</v>
       </c>
       <c r="G128">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="H128" s="2">
         <v>45218</v>
       </c>
       <c r="I128">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="J128" t="inlineStr">
         <is>
@@ -13366,13 +13366,13 @@
         <v>45158</v>
       </c>
       <c r="G129">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="H129" s="2">
         <v>45250</v>
       </c>
       <c r="I129">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="J129" t="inlineStr">
         <is>
@@ -13469,13 +13469,13 @@
         <v>45171</v>
       </c>
       <c r="G130">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="H130" s="2">
         <v>45262</v>
       </c>
       <c r="I130">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="J130" t="inlineStr">
         <is>
@@ -13572,13 +13572,13 @@
         <v>45111</v>
       </c>
       <c r="G131">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="H131" s="2">
         <v>45203</v>
       </c>
       <c r="I131">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="J131" t="inlineStr">
         <is>
@@ -13675,13 +13675,13 @@
         <v>45144</v>
       </c>
       <c r="G132">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="H132" s="2">
         <v>45236</v>
       </c>
       <c r="I132">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="J132" t="inlineStr">
         <is>
@@ -13778,13 +13778,13 @@
         <v>45156</v>
       </c>
       <c r="G133">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="H133" s="2">
         <v>45248</v>
       </c>
       <c r="I133">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="J133" t="inlineStr">
         <is>
@@ -13876,13 +13876,13 @@
         <v>45146</v>
       </c>
       <c r="G134">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="H134" s="2">
         <v>45238</v>
       </c>
       <c r="I134">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="J134" t="inlineStr">
         <is>
@@ -13979,13 +13979,13 @@
         <v>45140</v>
       </c>
       <c r="G135">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="H135" s="2">
         <v>45232</v>
       </c>
       <c r="I135">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="J135" t="inlineStr">
         <is>
@@ -14082,13 +14082,13 @@
         <v>45104</v>
       </c>
       <c r="G136">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="H136" s="2">
         <v>45196</v>
       </c>
       <c r="I136">
-        <v>-3</v>
+        <v>-4</v>
       </c>
       <c r="J136" t="inlineStr">
         <is>
@@ -14185,13 +14185,13 @@
         <v>45105</v>
       </c>
       <c r="G137">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="H137" s="2">
         <v>45197</v>
       </c>
       <c r="I137">
-        <v>-2</v>
+        <v>-3</v>
       </c>
       <c r="J137" t="inlineStr">
         <is>
@@ -14288,13 +14288,13 @@
         <v>45179</v>
       </c>
       <c r="G138">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="H138" s="2">
         <v>45270</v>
       </c>
       <c r="I138">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="J138" t="inlineStr">
         <is>
@@ -14386,13 +14386,13 @@
         <v>45105</v>
       </c>
       <c r="G139">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="H139" s="2">
         <v>45197</v>
       </c>
       <c r="I139">
-        <v>-2</v>
+        <v>-3</v>
       </c>
       <c r="J139" t="inlineStr">
         <is>
@@ -14489,13 +14489,13 @@
         <v>45182</v>
       </c>
       <c r="G140">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="H140" s="2">
         <v>45273</v>
       </c>
       <c r="I140">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="J140" t="inlineStr">
         <is>
@@ -14592,13 +14592,13 @@
         <v>45116</v>
       </c>
       <c r="G141">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="H141" s="2">
         <v>45208</v>
       </c>
       <c r="I141">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="J141" t="inlineStr">
         <is>
@@ -14690,13 +14690,13 @@
         <v>45150</v>
       </c>
       <c r="G142">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="H142" s="2">
         <v>45242</v>
       </c>
       <c r="I142">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="J142" t="inlineStr">
         <is>
@@ -14793,7 +14793,7 @@
         <v>45238</v>
       </c>
       <c r="I143">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="J143" t="inlineStr">
         <is>
@@ -14890,13 +14890,13 @@
         <v>45171</v>
       </c>
       <c r="G144">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="H144" s="2">
         <v>45262</v>
       </c>
       <c r="I144">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="J144" t="inlineStr">
         <is>
@@ -14993,13 +14993,13 @@
         <v>45102</v>
       </c>
       <c r="G145">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="H145" s="2">
         <v>45194</v>
       </c>
       <c r="I145">
-        <v>-5</v>
+        <v>-6</v>
       </c>
       <c r="J145" t="inlineStr">
         <is>
@@ -15086,13 +15086,13 @@
         <v>45119</v>
       </c>
       <c r="G146">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="H146" s="2">
         <v>45211</v>
       </c>
       <c r="I146">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="J146" t="inlineStr">
         <is>
@@ -15189,13 +15189,13 @@
         <v>45165</v>
       </c>
       <c r="G147">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="H147" s="2">
         <v>45257</v>
       </c>
       <c r="I147">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="J147" t="inlineStr">
         <is>
@@ -15292,13 +15292,13 @@
         <v>45166</v>
       </c>
       <c r="G148">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="H148" s="2">
         <v>45258</v>
       </c>
       <c r="I148">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="J148" t="inlineStr">
         <is>
@@ -15395,13 +15395,13 @@
         <v>45093</v>
       </c>
       <c r="G149">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="H149" s="2">
         <v>45185</v>
       </c>
       <c r="I149">
-        <v>-14</v>
+        <v>-15</v>
       </c>
       <c r="J149" t="inlineStr">
         <is>
@@ -15498,13 +15498,13 @@
         <v>45035</v>
       </c>
       <c r="G150">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="H150" s="2">
         <v>45218</v>
       </c>
       <c r="I150">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="J150" t="inlineStr">
         <is>
@@ -15601,13 +15601,13 @@
         <v>45174</v>
       </c>
       <c r="G151">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="H151" s="2">
         <v>45356</v>
       </c>
       <c r="I151">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="J151" t="inlineStr">
         <is>
@@ -15704,13 +15704,13 @@
         <v>45089</v>
       </c>
       <c r="G152">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="H152" s="2">
         <v>45272</v>
       </c>
       <c r="I152">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="J152" t="inlineStr">
         <is>
@@ -15807,13 +15807,13 @@
         <v>45124</v>
       </c>
       <c r="G153">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="H153" s="2">
         <v>45308</v>
       </c>
       <c r="I153">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="J153" t="inlineStr">
         <is>
@@ -15910,13 +15910,13 @@
         <v>45124</v>
       </c>
       <c r="G154">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="H154" s="2">
         <v>45308</v>
       </c>
       <c r="I154">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="J154" t="inlineStr">
         <is>
@@ -16013,13 +16013,13 @@
         <v>45026</v>
       </c>
       <c r="G155">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="H155" s="2">
         <v>45209</v>
       </c>
       <c r="I155">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="J155" t="inlineStr">
         <is>
@@ -16116,13 +16116,13 @@
         <v>45026</v>
       </c>
       <c r="G156">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="H156" s="2">
         <v>45209</v>
       </c>
       <c r="I156">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="J156" t="inlineStr">
         <is>
@@ -16219,13 +16219,13 @@
         <v>45026</v>
       </c>
       <c r="G157">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="H157" s="2">
         <v>45209</v>
       </c>
       <c r="I157">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="J157" t="inlineStr">
         <is>
@@ -16322,13 +16322,13 @@
         <v>45026</v>
       </c>
       <c r="G158">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="H158" s="2">
         <v>45209</v>
       </c>
       <c r="I158">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="J158" t="inlineStr">
         <is>
@@ -16425,13 +16425,13 @@
         <v>45156</v>
       </c>
       <c r="G159">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="H159" s="2">
         <v>45247</v>
       </c>
       <c r="I159">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="J159" t="inlineStr">
         <is>
@@ -16528,13 +16528,13 @@
         <v>45153</v>
       </c>
       <c r="G160">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="H160" s="2">
         <v>45245</v>
       </c>
       <c r="I160">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="J160" t="inlineStr">
         <is>
@@ -16631,13 +16631,13 @@
         <v>45135</v>
       </c>
       <c r="G161">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="H161" s="2">
         <v>45319</v>
       </c>
       <c r="I161">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="J161" t="inlineStr">
         <is>
@@ -16734,13 +16734,13 @@
         <v>45091</v>
       </c>
       <c r="G162">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="H162" s="2">
         <v>45274</v>
       </c>
       <c r="I162">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="J162" t="inlineStr">
         <is>
@@ -16832,13 +16832,13 @@
         <v>45091</v>
       </c>
       <c r="G163">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="H163" s="2">
         <v>45274</v>
       </c>
       <c r="I163">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="J163" t="inlineStr">
         <is>
@@ -16930,13 +16930,13 @@
         <v>45138</v>
       </c>
       <c r="G164">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="H164" s="2">
         <v>45322</v>
       </c>
       <c r="I164">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="J164" t="inlineStr">
         <is>
@@ -17033,13 +17033,13 @@
         <v>45138</v>
       </c>
       <c r="G165">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="H165" s="2">
         <v>45322</v>
       </c>
       <c r="I165">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="J165" t="inlineStr">
         <is>
@@ -17136,13 +17136,13 @@
         <v>45085</v>
       </c>
       <c r="G166">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="H166" s="2">
         <v>45268</v>
       </c>
       <c r="I166">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="J166" t="inlineStr">
         <is>
@@ -17239,13 +17239,13 @@
         <v>45085</v>
       </c>
       <c r="G167">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="H167" s="2">
         <v>45268</v>
       </c>
       <c r="I167">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="J167" t="inlineStr">
         <is>
@@ -17342,7 +17342,7 @@
         <v>45326</v>
       </c>
       <c r="I168">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="J168" t="inlineStr">
         <is>
@@ -17439,13 +17439,13 @@
         <v>45173</v>
       </c>
       <c r="G169">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="H169" s="2">
         <v>45355</v>
       </c>
       <c r="I169">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="J169" t="inlineStr">
         <is>
@@ -17542,13 +17542,13 @@
         <v>45056</v>
       </c>
       <c r="G170">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="H170" s="2">
         <v>45240</v>
       </c>
       <c r="I170">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="J170" t="inlineStr">
         <is>
@@ -17645,7 +17645,7 @@
         <v>45238</v>
       </c>
       <c r="I171">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="J171" t="inlineStr">
         <is>
@@ -17742,13 +17742,13 @@
         <v>45141</v>
       </c>
       <c r="G172">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="H172" s="2">
         <v>45325</v>
       </c>
       <c r="I172">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="J172" t="inlineStr">
         <is>
@@ -17845,13 +17845,13 @@
         <v>45037</v>
       </c>
       <c r="G173">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="H173" s="2">
         <v>45220</v>
       </c>
       <c r="I173">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="J173" t="inlineStr">
         <is>
@@ -17948,13 +17948,13 @@
         <v>45171</v>
       </c>
       <c r="G174">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="H174" s="2">
         <v>45262</v>
       </c>
       <c r="I174">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="J174" t="inlineStr">
         <is>
@@ -18051,13 +18051,13 @@
         <v>45105</v>
       </c>
       <c r="G175">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="H175" s="2">
         <v>45197</v>
       </c>
       <c r="I175">
-        <v>-2</v>
+        <v>-3</v>
       </c>
       <c r="J175" t="inlineStr">
         <is>
@@ -18154,13 +18154,13 @@
         <v>45162</v>
       </c>
       <c r="G176">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="H176" s="2">
         <v>45254</v>
       </c>
       <c r="I176">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="J176" t="inlineStr">
         <is>
@@ -18257,13 +18257,13 @@
         <v>45061</v>
       </c>
       <c r="G177">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="H177" s="2">
         <v>45245</v>
       </c>
       <c r="I177">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="J177" t="inlineStr">
         <is>
@@ -18360,13 +18360,13 @@
         <v>45120</v>
       </c>
       <c r="G178">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="H178" s="2">
         <v>45212</v>
       </c>
       <c r="I178">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="J178" t="inlineStr">
         <is>
@@ -18463,7 +18463,7 @@
         <v>45191</v>
       </c>
       <c r="I179">
-        <v>-8</v>
+        <v>-9</v>
       </c>
       <c r="J179" t="inlineStr">
         <is>
@@ -18560,13 +18560,13 @@
         <v>45088</v>
       </c>
       <c r="G180">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="H180" s="2">
         <v>45271</v>
       </c>
       <c r="I180">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="J180" t="inlineStr">
         <is>
@@ -18663,13 +18663,13 @@
         <v>45100</v>
       </c>
       <c r="G181">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="H181" s="2">
         <v>45192</v>
       </c>
       <c r="I181">
-        <v>-7</v>
+        <v>-8</v>
       </c>
       <c r="J181" t="inlineStr">
         <is>
@@ -18756,13 +18756,13 @@
         <v>45131</v>
       </c>
       <c r="G182">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="H182" s="2">
         <v>45223</v>
       </c>
       <c r="I182">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="J182" t="inlineStr">
         <is>
@@ -18854,13 +18854,13 @@
         <v>45136</v>
       </c>
       <c r="G183">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="H183" s="2">
         <v>45228</v>
       </c>
       <c r="I183">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="J183" t="inlineStr">
         <is>
@@ -18952,13 +18952,13 @@
         <v>45150</v>
       </c>
       <c r="G184">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="H184" s="2">
         <v>45242</v>
       </c>
       <c r="I184">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="J184" t="inlineStr">
         <is>
@@ -19050,13 +19050,13 @@
         <v>45118</v>
       </c>
       <c r="G185">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="H185" s="2">
         <v>45210</v>
       </c>
       <c r="I185">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="J185" t="inlineStr">
         <is>
@@ -19148,13 +19148,13 @@
         <v>45129</v>
       </c>
       <c r="G186">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="H186" s="2">
         <v>45221</v>
       </c>
       <c r="I186">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="J186" t="inlineStr">
         <is>
@@ -19246,13 +19246,13 @@
         <v>45097</v>
       </c>
       <c r="G187">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="H187" s="2">
         <v>45189</v>
       </c>
       <c r="I187">
-        <v>-10</v>
+        <v>-11</v>
       </c>
       <c r="J187" t="inlineStr">
         <is>
@@ -19339,13 +19339,13 @@
         <v>45101</v>
       </c>
       <c r="G188">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="H188" s="2">
         <v>45193</v>
       </c>
       <c r="I188">
-        <v>-6</v>
+        <v>-7</v>
       </c>
       <c r="J188" t="inlineStr">
         <is>
@@ -19432,13 +19432,13 @@
         <v>45165</v>
       </c>
       <c r="G189">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="H189" s="2">
         <v>45257</v>
       </c>
       <c r="I189">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="J189" t="inlineStr">
         <is>
@@ -19530,7 +19530,7 @@
         <v>45202</v>
       </c>
       <c r="I190">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="J190" t="inlineStr">
         <is>
@@ -19627,13 +19627,13 @@
         <v>45081</v>
       </c>
       <c r="G191">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="H191" s="2">
         <v>45264</v>
       </c>
       <c r="I191">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="J191" t="inlineStr">
         <is>
@@ -19730,13 +19730,13 @@
         <v>45081</v>
       </c>
       <c r="G192">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="H192" s="2">
         <v>45264</v>
       </c>
       <c r="I192">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="J192" t="inlineStr">
         <is>
@@ -19833,7 +19833,7 @@
         <v>45319</v>
       </c>
       <c r="I193">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="J193" t="inlineStr">
         <is>
@@ -19930,7 +19930,7 @@
         <v>45319</v>
       </c>
       <c r="I194">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="J194" t="inlineStr">
         <is>
@@ -20022,13 +20022,13 @@
         <v>45046</v>
       </c>
       <c r="G195">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="H195" s="2">
         <v>45230</v>
       </c>
       <c r="I195">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="J195" t="inlineStr">
         <is>
@@ -20125,13 +20125,13 @@
         <v>45046</v>
       </c>
       <c r="G196">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="H196" s="2">
         <v>45230</v>
       </c>
       <c r="I196">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="J196" t="inlineStr">
         <is>
@@ -20228,13 +20228,13 @@
         <v>45031</v>
       </c>
       <c r="G197">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="H197" s="2">
         <v>45214</v>
       </c>
       <c r="I197">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="J197" t="inlineStr">
         <is>
@@ -20331,13 +20331,13 @@
         <v>45031</v>
       </c>
       <c r="G198">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="H198" s="2">
         <v>45214</v>
       </c>
       <c r="I198">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="J198" t="inlineStr">
         <is>
@@ -20434,13 +20434,13 @@
         <v>45031</v>
       </c>
       <c r="G199">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="H199" s="2">
         <v>45214</v>
       </c>
       <c r="I199">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="J199" t="inlineStr">
         <is>
@@ -20537,13 +20537,13 @@
         <v>45031</v>
       </c>
       <c r="G200">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="H200" s="2">
         <v>45214</v>
       </c>
       <c r="I200">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="J200" t="inlineStr">
         <is>
@@ -20640,13 +20640,13 @@
         <v>45067</v>
       </c>
       <c r="G201">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="H201" s="2">
         <v>45251</v>
       </c>
       <c r="I201">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="J201" t="inlineStr">
         <is>
@@ -20743,13 +20743,13 @@
         <v>45067</v>
       </c>
       <c r="G202">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="H202" s="2">
         <v>45251</v>
       </c>
       <c r="I202">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="J202" t="inlineStr">
         <is>
@@ -20846,13 +20846,13 @@
         <v>45067</v>
       </c>
       <c r="G203">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="H203" s="2">
         <v>45251</v>
       </c>
       <c r="I203">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="J203" t="inlineStr">
         <is>
@@ -20949,13 +20949,13 @@
         <v>45067</v>
       </c>
       <c r="G204">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="H204" s="2">
         <v>45251</v>
       </c>
       <c r="I204">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="J204" t="inlineStr">
         <is>
@@ -21052,13 +21052,13 @@
         <v>45178</v>
       </c>
       <c r="G205">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="H205" s="2">
         <v>45269</v>
       </c>
       <c r="I205">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="J205" t="inlineStr">
         <is>
@@ -21155,7 +21155,7 @@
         <v>45252</v>
       </c>
       <c r="I206">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="J206" t="inlineStr">
         <is>
@@ -21252,13 +21252,13 @@
         <v>45087</v>
       </c>
       <c r="G207">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="H207" s="2">
         <v>45270</v>
       </c>
       <c r="I207">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="J207" t="inlineStr">
         <is>
@@ -21355,13 +21355,13 @@
         <v>45099</v>
       </c>
       <c r="G208">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="H208" s="2">
         <v>45282</v>
       </c>
       <c r="I208">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="J208" t="inlineStr">
         <is>
@@ -21458,13 +21458,13 @@
         <v>45175</v>
       </c>
       <c r="G209">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="H209" s="2">
         <v>45356</v>
       </c>
       <c r="I209">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="J209" t="inlineStr">
         <is>
@@ -21561,13 +21561,13 @@
         <v>45175</v>
       </c>
       <c r="G210">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="H210" s="2">
         <v>45356</v>
       </c>
       <c r="I210">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="J210" t="inlineStr">
         <is>
@@ -21664,13 +21664,13 @@
         <v>45166</v>
       </c>
       <c r="G211">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="H211" s="2">
         <v>45350</v>
       </c>
       <c r="I211">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="J211" t="inlineStr">
         <is>
@@ -21767,13 +21767,13 @@
         <v>45166</v>
       </c>
       <c r="G212">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="H212" s="2">
         <v>45350</v>
       </c>
       <c r="I212">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="J212" t="inlineStr">
         <is>
@@ -21870,13 +21870,13 @@
         <v>45090</v>
       </c>
       <c r="G213">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="H213" s="2">
         <v>45273</v>
       </c>
       <c r="I213">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="J213" t="inlineStr">
         <is>
@@ -21973,13 +21973,13 @@
         <v>45106</v>
       </c>
       <c r="G214">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="H214" s="2">
         <v>45289</v>
       </c>
       <c r="I214">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="J214" t="inlineStr">
         <is>
@@ -22076,13 +22076,13 @@
         <v>45134</v>
       </c>
       <c r="G215">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="H215" s="2">
         <v>45226</v>
       </c>
       <c r="I215">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="J215" t="inlineStr">
         <is>
@@ -22179,13 +22179,13 @@
         <v>45132</v>
       </c>
       <c r="G216">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="H216" s="2">
         <v>45224</v>
       </c>
       <c r="I216">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="J216" t="inlineStr">
         <is>
@@ -22282,13 +22282,13 @@
         <v>45150</v>
       </c>
       <c r="G217">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="H217" s="2">
         <v>45242</v>
       </c>
       <c r="I217">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="J217" t="inlineStr">
         <is>
@@ -22385,13 +22385,13 @@
         <v>45095</v>
       </c>
       <c r="G218">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="H218" s="2">
         <v>45187</v>
       </c>
       <c r="I218">
-        <v>-12</v>
+        <v>-13</v>
       </c>
       <c r="J218" t="inlineStr">
         <is>
@@ -22483,13 +22483,13 @@
         <v>45182</v>
       </c>
       <c r="G219">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="H219" s="2">
         <v>45273</v>
       </c>
       <c r="I219">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="J219" t="inlineStr">
         <is>
@@ -22586,7 +22586,7 @@
         <v>45196</v>
       </c>
       <c r="I220">
-        <v>-3</v>
+        <v>-4</v>
       </c>
       <c r="J220" t="inlineStr">
         <is>
@@ -22683,13 +22683,13 @@
         <v>45108</v>
       </c>
       <c r="G221">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="H221" s="2">
         <v>45200</v>
       </c>
       <c r="I221">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J221" t="inlineStr">
         <is>
@@ -22786,13 +22786,13 @@
         <v>45135</v>
       </c>
       <c r="G222">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="H222" s="2">
         <v>45227</v>
       </c>
       <c r="I222">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="J222" t="inlineStr">
         <is>
@@ -22889,13 +22889,13 @@
         <v>45148</v>
       </c>
       <c r="G223">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="H223" s="2">
         <v>45240</v>
       </c>
       <c r="I223">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="J223" t="inlineStr">
         <is>
@@ -22987,13 +22987,13 @@
         <v>45100</v>
       </c>
       <c r="G224">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="H224" s="2">
         <v>45192</v>
       </c>
       <c r="I224">
-        <v>-7</v>
+        <v>-8</v>
       </c>
       <c r="J224" t="inlineStr">
         <is>
@@ -23085,13 +23085,13 @@
         <v>45136</v>
       </c>
       <c r="G225">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="H225" s="2">
         <v>45320</v>
       </c>
       <c r="I225">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="J225" t="inlineStr">
         <is>
@@ -23188,13 +23188,13 @@
         <v>45136</v>
       </c>
       <c r="G226">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="H226" s="2">
         <v>45320</v>
       </c>
       <c r="I226">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="J226" t="inlineStr">
         <is>
@@ -23291,13 +23291,13 @@
         <v>45094</v>
       </c>
       <c r="G227">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="H227" s="2">
         <v>45277</v>
       </c>
       <c r="I227">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="J227" t="inlineStr">
         <is>
@@ -23394,13 +23394,13 @@
         <v>45081</v>
       </c>
       <c r="G228">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="H228" s="2">
         <v>45264</v>
       </c>
       <c r="I228">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="J228" t="inlineStr">
         <is>
@@ -23497,13 +23497,13 @@
         <v>45099</v>
       </c>
       <c r="G229">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="H229" s="2">
         <v>45282</v>
       </c>
       <c r="I229">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="J229" t="inlineStr">
         <is>
@@ -23600,13 +23600,13 @@
         <v>45018</v>
       </c>
       <c r="G230">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="H230" s="2">
         <v>45201</v>
       </c>
       <c r="I230">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J230" t="inlineStr">
         <is>
@@ -23703,13 +23703,13 @@
         <v>45031</v>
       </c>
       <c r="G231">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="H231" s="2">
         <v>45214</v>
       </c>
       <c r="I231">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="J231" t="inlineStr">
         <is>
@@ -23806,7 +23806,7 @@
         <v>45294</v>
       </c>
       <c r="I232">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="J232" t="inlineStr">
         <is>
@@ -23903,13 +23903,13 @@
         <v>45079</v>
       </c>
       <c r="G233">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="H233" s="2">
         <v>45262</v>
       </c>
       <c r="I233">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="J233" t="inlineStr">
         <is>
@@ -24006,7 +24006,7 @@
         <v>45199</v>
       </c>
       <c r="I234">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="J234" t="inlineStr">
         <is>
@@ -24103,13 +24103,13 @@
         <v>45021</v>
       </c>
       <c r="G235">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="H235" s="2">
         <v>45204</v>
       </c>
       <c r="I235">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="J235" t="inlineStr">
         <is>
@@ -24206,13 +24206,13 @@
         <v>45021</v>
       </c>
       <c r="G236">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="H236" s="2">
         <v>45204</v>
       </c>
       <c r="I236">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="J236" t="inlineStr">
         <is>
@@ -24309,13 +24309,13 @@
         <v>45080</v>
       </c>
       <c r="G237">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="H237" s="2">
         <v>45263</v>
       </c>
       <c r="I237">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="J237" t="inlineStr">
         <is>
@@ -24412,13 +24412,13 @@
         <v>45046</v>
       </c>
       <c r="G238">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="H238" s="2">
         <v>45229</v>
       </c>
       <c r="I238">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="J238" t="inlineStr">
         <is>
@@ -24515,13 +24515,13 @@
         <v>45112</v>
       </c>
       <c r="G239">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="H239" s="2">
         <v>45204</v>
       </c>
       <c r="I239">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="J239" t="inlineStr">
         <is>
@@ -24609,13 +24609,13 @@
         <v>45112</v>
       </c>
       <c r="G240">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="H240" s="2">
         <v>45204</v>
       </c>
       <c r="I240">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="J240" t="inlineStr">
         <is>
@@ -24703,13 +24703,13 @@
         <v>45016</v>
       </c>
       <c r="G241">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="H241" s="2">
         <v>45199</v>
       </c>
       <c r="I241">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="J241" t="inlineStr">
         <is>
@@ -24806,13 +24806,13 @@
         <v>45070</v>
       </c>
       <c r="G242">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="H242" s="2">
         <v>45254</v>
       </c>
       <c r="I242">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="J242" t="inlineStr">
         <is>
@@ -24909,13 +24909,13 @@
         <v>45168</v>
       </c>
       <c r="G243">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="H243" s="2">
         <v>45260</v>
       </c>
       <c r="I243">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="J243" t="inlineStr">
         <is>
@@ -25012,13 +25012,13 @@
         <v>45027</v>
       </c>
       <c r="G244">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="H244" s="2">
         <v>45210</v>
       </c>
       <c r="I244">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="J244" t="inlineStr">
         <is>
@@ -25115,13 +25115,13 @@
         <v>45077</v>
       </c>
       <c r="G245">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="H245" s="2">
         <v>45260</v>
       </c>
       <c r="I245">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="J245" t="inlineStr">
         <is>
@@ -25218,13 +25218,13 @@
         <v>45100</v>
       </c>
       <c r="G246">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="H246" s="2">
         <v>45283</v>
       </c>
       <c r="I246">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="J246" t="inlineStr">
         <is>
@@ -25321,7 +25321,7 @@
         <v>45281</v>
       </c>
       <c r="I247">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="J247" t="inlineStr">
         <is>
@@ -25418,13 +25418,13 @@
         <v>45044</v>
       </c>
       <c r="G248">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="H248" s="2">
         <v>45227</v>
       </c>
       <c r="I248">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="J248" t="inlineStr">
         <is>
@@ -25521,13 +25521,13 @@
         <v>45101</v>
       </c>
       <c r="G249">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="H249" s="2">
         <v>45283</v>
       </c>
       <c r="I249">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="J249" t="inlineStr">
         <is>
@@ -25624,13 +25624,13 @@
         <v>45134</v>
       </c>
       <c r="G250">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="H250" s="2">
         <v>45226</v>
       </c>
       <c r="I250">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="J250" t="inlineStr">
         <is>
@@ -25727,13 +25727,13 @@
         <v>45158</v>
       </c>
       <c r="G251">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="H251" s="2">
         <v>45250</v>
       </c>
       <c r="I251">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="J251" t="inlineStr">
         <is>
@@ -25830,13 +25830,13 @@
         <v>45108</v>
       </c>
       <c r="G252">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="H252" s="2">
         <v>45200</v>
       </c>
       <c r="I252">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J252" t="inlineStr">
         <is>
@@ -25933,7 +25933,7 @@
         <v>45317</v>
       </c>
       <c r="I253">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="J253" t="inlineStr">
         <is>
@@ -26030,13 +26030,13 @@
         <v>45039</v>
       </c>
       <c r="G254">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="H254" s="2">
         <v>45222</v>
       </c>
       <c r="I254">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="J254" t="inlineStr">
         <is>
@@ -26128,13 +26128,13 @@
         <v>45129</v>
       </c>
       <c r="G255">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="H255" s="2">
         <v>45221</v>
       </c>
       <c r="I255">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="J255" t="inlineStr">
         <is>
@@ -26231,13 +26231,13 @@
         <v>45157</v>
       </c>
       <c r="G256">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="H256" s="2">
         <v>45341</v>
       </c>
       <c r="I256">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="J256" t="inlineStr">
         <is>
@@ -26334,13 +26334,13 @@
         <v>45063</v>
       </c>
       <c r="G257">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="H257" s="2">
         <v>45247</v>
       </c>
       <c r="I257">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="J257" t="inlineStr">
         <is>
@@ -26437,7 +26437,7 @@
         <v>45254</v>
       </c>
       <c r="I258">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="J258" t="inlineStr">
         <is>
@@ -26534,7 +26534,7 @@
         <v>45486</v>
       </c>
       <c r="I259">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="J259" t="inlineStr">
         <is>
@@ -26626,13 +26626,13 @@
         <v>45073</v>
       </c>
       <c r="G260">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="H260" s="2">
         <v>45439</v>
       </c>
       <c r="I260">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="J260" t="inlineStr">
         <is>
@@ -26724,7 +26724,7 @@
         <v>45323</v>
       </c>
       <c r="I261">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="J261" t="inlineStr">
         <is>
@@ -26816,7 +26816,7 @@
         <v>45303</v>
       </c>
       <c r="I262">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="J262" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
Bond dates update Tue Oct  3 20:22:12 UTC 2023
</commit_message>
<xml_diff>
--- a/Data/obligacje_screener.xlsx
+++ b/Data/obligacje_screener.xlsx
@@ -512,7 +512,7 @@
         <v>45340</v>
       </c>
       <c r="I2">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="J2" t="inlineStr">
         <is>
@@ -600,13 +600,13 @@
         <v>45121</v>
       </c>
       <c r="G3">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="H3" s="2">
         <v>45305</v>
       </c>
       <c r="I3">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="J3" t="inlineStr">
         <is>
@@ -703,13 +703,13 @@
         <v>45039</v>
       </c>
       <c r="G4">
-        <v>161</v>
+        <v>163</v>
       </c>
       <c r="H4" s="2">
         <v>45222</v>
       </c>
       <c r="I4">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="J4" t="inlineStr">
         <is>
@@ -806,13 +806,13 @@
         <v>45039</v>
       </c>
       <c r="G5">
-        <v>161</v>
+        <v>163</v>
       </c>
       <c r="H5" s="2">
         <v>45222</v>
       </c>
       <c r="I5">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="J5" t="inlineStr">
         <is>
@@ -909,13 +909,13 @@
         <v>45129</v>
       </c>
       <c r="G6">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="H6" s="2">
         <v>45221</v>
       </c>
       <c r="I6">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="J6" t="inlineStr">
         <is>
@@ -1012,13 +1012,13 @@
         <v>45162</v>
       </c>
       <c r="G7">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="H7" s="2">
         <v>45254</v>
       </c>
       <c r="I7">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="J7" t="inlineStr">
         <is>
@@ -1110,13 +1110,13 @@
         <v>45156</v>
       </c>
       <c r="G8">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="H8" s="2">
         <v>45248</v>
       </c>
       <c r="I8">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="J8" t="inlineStr">
         <is>
@@ -1213,13 +1213,13 @@
         <v>45141</v>
       </c>
       <c r="G9">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="H9" s="2">
         <v>45233</v>
       </c>
       <c r="I9">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="J9" t="inlineStr">
         <is>
@@ -1316,13 +1316,13 @@
         <v>45062</v>
       </c>
       <c r="G10">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="H10" s="2">
         <v>45246</v>
       </c>
       <c r="I10">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="J10" t="inlineStr">
         <is>
@@ -1419,7 +1419,7 @@
         <v>45286</v>
       </c>
       <c r="I11">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="J11" t="inlineStr">
         <is>
@@ -1516,13 +1516,13 @@
         <v>45011</v>
       </c>
       <c r="G12">
-        <v>189</v>
+        <v>191</v>
       </c>
       <c r="H12" s="2">
         <v>45195</v>
       </c>
       <c r="I12">
-        <v>-5</v>
+        <v>-7</v>
       </c>
       <c r="J12" t="inlineStr">
         <is>
@@ -1614,13 +1614,13 @@
         <v>45036</v>
       </c>
       <c r="G13">
-        <v>164</v>
+        <v>166</v>
       </c>
       <c r="H13" s="2">
         <v>45219</v>
       </c>
       <c r="I13">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="J13" t="inlineStr">
         <is>
@@ -1717,13 +1717,13 @@
         <v>45036</v>
       </c>
       <c r="G14">
-        <v>164</v>
+        <v>166</v>
       </c>
       <c r="H14" s="2">
         <v>45219</v>
       </c>
       <c r="I14">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="J14" t="inlineStr">
         <is>
@@ -1820,13 +1820,13 @@
         <v>45106</v>
       </c>
       <c r="G15">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="H15" s="2">
         <v>45289</v>
       </c>
       <c r="I15">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="J15" t="inlineStr">
         <is>
@@ -1923,13 +1923,13 @@
         <v>45094</v>
       </c>
       <c r="G16">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="H16" s="2">
         <v>45186</v>
       </c>
       <c r="I16">
-        <v>-14</v>
+        <v>-16</v>
       </c>
       <c r="J16" t="inlineStr">
         <is>
@@ -2026,13 +2026,13 @@
         <v>45094</v>
       </c>
       <c r="G17">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="H17" s="2">
         <v>45186</v>
       </c>
       <c r="I17">
-        <v>-14</v>
+        <v>-16</v>
       </c>
       <c r="J17" t="inlineStr">
         <is>
@@ -2129,13 +2129,13 @@
         <v>45132</v>
       </c>
       <c r="G18">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="H18" s="2">
         <v>45224</v>
       </c>
       <c r="I18">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="J18" t="inlineStr">
         <is>
@@ -2232,13 +2232,13 @@
         <v>45137</v>
       </c>
       <c r="G19">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="H19" s="2">
         <v>45229</v>
       </c>
       <c r="I19">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="J19" t="inlineStr">
         <is>
@@ -2330,13 +2330,13 @@
         <v>45183</v>
       </c>
       <c r="G20">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="H20" s="2">
         <v>45274</v>
       </c>
       <c r="I20">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="J20" t="inlineStr">
         <is>
@@ -2433,13 +2433,13 @@
         <v>45093</v>
       </c>
       <c r="G21">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="H21" s="2">
         <v>45187</v>
       </c>
       <c r="I21">
-        <v>-13</v>
+        <v>-15</v>
       </c>
       <c r="J21" t="inlineStr">
         <is>
@@ -2536,13 +2536,13 @@
         <v>45096</v>
       </c>
       <c r="G22">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="H22" s="2">
         <v>45187</v>
       </c>
       <c r="I22">
-        <v>-13</v>
+        <v>-15</v>
       </c>
       <c r="J22" t="inlineStr">
         <is>
@@ -2639,7 +2639,7 @@
         <v>45245</v>
       </c>
       <c r="I23">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="J23" t="inlineStr">
         <is>
@@ -2736,7 +2736,7 @@
         <v>45245</v>
       </c>
       <c r="I24">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="J24" t="inlineStr">
         <is>
@@ -2833,13 +2833,13 @@
         <v>45021</v>
       </c>
       <c r="G25">
-        <v>179</v>
+        <v>181</v>
       </c>
       <c r="H25" s="2">
         <v>45204</v>
       </c>
       <c r="I25">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="J25" t="inlineStr">
         <is>
@@ -2936,13 +2936,13 @@
         <v>45160</v>
       </c>
       <c r="G26">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="H26" s="2">
         <v>45344</v>
       </c>
       <c r="I26">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="J26" t="inlineStr">
         <is>
@@ -3039,13 +3039,13 @@
         <v>45118</v>
       </c>
       <c r="G27">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="H27" s="2">
         <v>45302</v>
       </c>
       <c r="I27">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="J27" t="inlineStr">
         <is>
@@ -3142,13 +3142,13 @@
         <v>45085</v>
       </c>
       <c r="G28">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="H28" s="2">
         <v>45268</v>
       </c>
       <c r="I28">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="J28" t="inlineStr">
         <is>
@@ -3245,13 +3245,13 @@
         <v>45183</v>
       </c>
       <c r="G29">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="H29" s="2">
         <v>45274</v>
       </c>
       <c r="I29">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="J29" t="inlineStr">
         <is>
@@ -3348,7 +3348,7 @@
         <v>45224</v>
       </c>
       <c r="I30">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="J30" t="inlineStr">
         <is>
@@ -3445,13 +3445,13 @@
         <v>45153</v>
       </c>
       <c r="G31">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="H31" s="2">
         <v>45245</v>
       </c>
       <c r="I31">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="J31" t="inlineStr">
         <is>
@@ -3548,13 +3548,13 @@
         <v>45155</v>
       </c>
       <c r="G32">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="H32" s="2">
         <v>45247</v>
       </c>
       <c r="I32">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="J32" t="inlineStr">
         <is>
@@ -3651,7 +3651,7 @@
         <v>45255</v>
       </c>
       <c r="I33">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="J33" t="inlineStr">
         <is>
@@ -3739,13 +3739,13 @@
         <v>45176</v>
       </c>
       <c r="G34">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="H34" s="2">
         <v>45267</v>
       </c>
       <c r="I34">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="J34" t="inlineStr">
         <is>
@@ -3842,13 +3842,13 @@
         <v>45130</v>
       </c>
       <c r="G35">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="H35" s="2">
         <v>45222</v>
       </c>
       <c r="I35">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="J35" t="inlineStr">
         <is>
@@ -3940,13 +3940,13 @@
         <v>45115</v>
       </c>
       <c r="G36">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="H36" s="2">
         <v>45207</v>
       </c>
       <c r="I36">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="J36" t="inlineStr">
         <is>
@@ -4043,13 +4043,13 @@
         <v>45097</v>
       </c>
       <c r="G37">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="H37" s="2">
         <v>45189</v>
       </c>
       <c r="I37">
-        <v>-11</v>
+        <v>-13</v>
       </c>
       <c r="J37" t="inlineStr">
         <is>
@@ -4141,13 +4141,13 @@
         <v>45107</v>
       </c>
       <c r="G38">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="H38" s="2">
         <v>45290</v>
       </c>
       <c r="I38">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="J38" t="inlineStr">
         <is>
@@ -4244,13 +4244,13 @@
         <v>45063</v>
       </c>
       <c r="G39">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="H39" s="2">
         <v>45247</v>
       </c>
       <c r="I39">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="J39" t="inlineStr">
         <is>
@@ -4347,13 +4347,13 @@
         <v>45177</v>
       </c>
       <c r="G40">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="H40" s="2">
         <v>45359</v>
       </c>
       <c r="I40">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="J40" t="inlineStr">
         <is>
@@ -4450,13 +4450,13 @@
         <v>45107</v>
       </c>
       <c r="G41">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="H41" s="2">
         <v>45290</v>
       </c>
       <c r="I41">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="J41" t="inlineStr">
         <is>
@@ -4553,7 +4553,7 @@
         <v>45265</v>
       </c>
       <c r="I42">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="J42" t="inlineStr">
         <is>
@@ -4650,13 +4650,13 @@
         <v>45098</v>
       </c>
       <c r="G43">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="H43" s="2">
         <v>45281</v>
       </c>
       <c r="I43">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="J43" t="inlineStr">
         <is>
@@ -4753,13 +4753,13 @@
         <v>45099</v>
       </c>
       <c r="G44">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="H44" s="2">
         <v>45282</v>
       </c>
       <c r="I44">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="J44" t="inlineStr">
         <is>
@@ -4856,13 +4856,13 @@
         <v>45106</v>
       </c>
       <c r="G45">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="H45" s="2">
         <v>45289</v>
       </c>
       <c r="I45">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="J45" t="inlineStr">
         <is>
@@ -4959,13 +4959,13 @@
         <v>45106</v>
       </c>
       <c r="G46">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="H46" s="2">
         <v>45289</v>
       </c>
       <c r="I46">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="J46" t="inlineStr">
         <is>
@@ -5062,13 +5062,13 @@
         <v>45120</v>
       </c>
       <c r="G47">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="H47" s="2">
         <v>45304</v>
       </c>
       <c r="I47">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="J47" t="inlineStr">
         <is>
@@ -5165,13 +5165,13 @@
         <v>45118</v>
       </c>
       <c r="G48">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="H48" s="2">
         <v>45302</v>
       </c>
       <c r="I48">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="J48" t="inlineStr">
         <is>
@@ -5268,13 +5268,13 @@
         <v>45152</v>
       </c>
       <c r="G49">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="H49" s="2">
         <v>45336</v>
       </c>
       <c r="I49">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="J49" t="inlineStr">
         <is>
@@ -5371,13 +5371,13 @@
         <v>45042</v>
       </c>
       <c r="G50">
-        <v>158</v>
+        <v>160</v>
       </c>
       <c r="H50" s="2">
         <v>45225</v>
       </c>
       <c r="I50">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="J50" t="inlineStr">
         <is>
@@ -5474,13 +5474,13 @@
         <v>45122</v>
       </c>
       <c r="G51">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="H51" s="2">
         <v>45306</v>
       </c>
       <c r="I51">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="J51" t="inlineStr">
         <is>
@@ -5577,13 +5577,13 @@
         <v>45139</v>
       </c>
       <c r="G52">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="H52" s="2">
         <v>45323</v>
       </c>
       <c r="I52">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="J52" t="inlineStr">
         <is>
@@ -5671,13 +5671,13 @@
         <v>45099</v>
       </c>
       <c r="G53">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="H53" s="2">
         <v>45282</v>
       </c>
       <c r="I53">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="J53" t="inlineStr">
         <is>
@@ -5774,7 +5774,7 @@
         <v>45196</v>
       </c>
       <c r="I54">
-        <v>-4</v>
+        <v>-6</v>
       </c>
       <c r="J54" t="inlineStr">
         <is>
@@ -5871,13 +5871,13 @@
         <v>45044</v>
       </c>
       <c r="G55">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="H55" s="2">
         <v>45227</v>
       </c>
       <c r="I55">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="J55" t="inlineStr">
         <is>
@@ -5974,13 +5974,13 @@
         <v>45151</v>
       </c>
       <c r="G56">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="H56" s="2">
         <v>45243</v>
       </c>
       <c r="I56">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="J56" t="inlineStr">
         <is>
@@ -6072,7 +6072,7 @@
         <v>45196</v>
       </c>
       <c r="I57">
-        <v>-4</v>
+        <v>-6</v>
       </c>
       <c r="J57" t="inlineStr">
         <is>
@@ -6169,13 +6169,13 @@
         <v>45069</v>
       </c>
       <c r="G58">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="H58" s="2">
         <v>45253</v>
       </c>
       <c r="I58">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="J58" t="inlineStr">
         <is>
@@ -6272,13 +6272,13 @@
         <v>45099</v>
       </c>
       <c r="G59">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="H59" s="2">
         <v>45191</v>
       </c>
       <c r="I59">
-        <v>-9</v>
+        <v>-11</v>
       </c>
       <c r="J59" t="inlineStr">
         <is>
@@ -6370,13 +6370,13 @@
         <v>45113</v>
       </c>
       <c r="G60">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="H60" s="2">
         <v>45205</v>
       </c>
       <c r="I60">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="J60" t="inlineStr">
         <is>
@@ -6473,13 +6473,13 @@
         <v>45127</v>
       </c>
       <c r="G61">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="H61" s="2">
         <v>45219</v>
       </c>
       <c r="I61">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="J61" t="inlineStr">
         <is>
@@ -6576,13 +6576,13 @@
         <v>45058</v>
       </c>
       <c r="G62">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="H62" s="2">
         <v>45242</v>
       </c>
       <c r="I62">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="J62" t="inlineStr">
         <is>
@@ -6679,13 +6679,13 @@
         <v>45010</v>
       </c>
       <c r="G63">
-        <v>190</v>
+        <v>192</v>
       </c>
       <c r="H63" s="2">
         <v>45194</v>
       </c>
       <c r="I63">
-        <v>-6</v>
+        <v>-8</v>
       </c>
       <c r="J63" t="inlineStr">
         <is>
@@ -6777,13 +6777,13 @@
         <v>45025</v>
       </c>
       <c r="G64">
-        <v>175</v>
+        <v>177</v>
       </c>
       <c r="H64" s="2">
         <v>45208</v>
       </c>
       <c r="I64">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="J64" t="inlineStr">
         <is>
@@ -6880,13 +6880,13 @@
         <v>45025</v>
       </c>
       <c r="G65">
-        <v>175</v>
+        <v>177</v>
       </c>
       <c r="H65" s="2">
         <v>45208</v>
       </c>
       <c r="I65">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="J65" t="inlineStr">
         <is>
@@ -6983,13 +6983,13 @@
         <v>45089</v>
       </c>
       <c r="G66">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="H66" s="2">
         <v>45272</v>
       </c>
       <c r="I66">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="J66" t="inlineStr">
         <is>
@@ -7086,13 +7086,13 @@
         <v>45178</v>
       </c>
       <c r="G67">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="H67" s="2">
         <v>45269</v>
       </c>
       <c r="I67">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="J67" t="inlineStr">
         <is>
@@ -7184,13 +7184,13 @@
         <v>45104</v>
       </c>
       <c r="G68">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="H68" s="2">
         <v>45196</v>
       </c>
       <c r="I68">
-        <v>-4</v>
+        <v>-6</v>
       </c>
       <c r="J68" t="inlineStr">
         <is>
@@ -7287,13 +7287,13 @@
         <v>45149</v>
       </c>
       <c r="G69">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="H69" s="2">
         <v>45241</v>
       </c>
       <c r="I69">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="J69" t="inlineStr">
         <is>
@@ -7390,7 +7390,7 @@
         <v>45205</v>
       </c>
       <c r="I70">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="J70" t="inlineStr">
         <is>
@@ -7487,13 +7487,13 @@
         <v>45114</v>
       </c>
       <c r="G71">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="H71" s="2">
         <v>45205</v>
       </c>
       <c r="I71">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="J71" t="inlineStr">
         <is>
@@ -7590,13 +7590,13 @@
         <v>45115</v>
       </c>
       <c r="G72">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="H72" s="2">
         <v>45207</v>
       </c>
       <c r="I72">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="J72" t="inlineStr">
         <is>
@@ -7693,13 +7693,13 @@
         <v>45097</v>
       </c>
       <c r="G73">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="H73" s="2">
         <v>45189</v>
       </c>
       <c r="I73">
-        <v>-11</v>
+        <v>-13</v>
       </c>
       <c r="J73" t="inlineStr">
         <is>
@@ -7791,13 +7791,13 @@
         <v>45038</v>
       </c>
       <c r="G74">
-        <v>162</v>
+        <v>164</v>
       </c>
       <c r="H74" s="2">
         <v>45221</v>
       </c>
       <c r="I74">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="J74" t="inlineStr">
         <is>
@@ -7889,13 +7889,13 @@
         <v>45117</v>
       </c>
       <c r="G75">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="H75" s="2">
         <v>45301</v>
       </c>
       <c r="I75">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="J75" t="inlineStr">
         <is>
@@ -7992,13 +7992,13 @@
         <v>45160</v>
       </c>
       <c r="G76">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="H76" s="2">
         <v>45344</v>
       </c>
       <c r="I76">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="J76" t="inlineStr">
         <is>
@@ -8095,13 +8095,13 @@
         <v>45002</v>
       </c>
       <c r="G77">
-        <v>198</v>
+        <v>200</v>
       </c>
       <c r="H77" s="2">
         <v>45186</v>
       </c>
       <c r="I77">
-        <v>-14</v>
+        <v>-16</v>
       </c>
       <c r="J77" t="inlineStr">
         <is>
@@ -8198,13 +8198,13 @@
         <v>45043</v>
       </c>
       <c r="G78">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="H78" s="2">
         <v>45226</v>
       </c>
       <c r="I78">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="J78" t="inlineStr">
         <is>
@@ -8301,13 +8301,13 @@
         <v>45079</v>
       </c>
       <c r="G79">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="H79" s="2">
         <v>45262</v>
       </c>
       <c r="I79">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="J79" t="inlineStr">
         <is>
@@ -8404,7 +8404,7 @@
         <v>45254</v>
       </c>
       <c r="I80">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="J80" t="inlineStr">
         <is>
@@ -8501,13 +8501,13 @@
         <v>45104</v>
       </c>
       <c r="G81">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="H81" s="2">
         <v>45287</v>
       </c>
       <c r="I81">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="J81" t="inlineStr">
         <is>
@@ -8604,7 +8604,7 @@
         <v>45288</v>
       </c>
       <c r="I82">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="J82" t="inlineStr">
         <is>
@@ -8696,13 +8696,13 @@
         <v>45175</v>
       </c>
       <c r="G83">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="H83" s="2">
         <v>45357</v>
       </c>
       <c r="I83">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="J83" t="inlineStr">
         <is>
@@ -8799,13 +8799,13 @@
         <v>45054</v>
       </c>
       <c r="G84">
-        <v>146</v>
+        <v>148</v>
       </c>
       <c r="H84" s="2">
         <v>45238</v>
       </c>
       <c r="I84">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="J84" t="inlineStr">
         <is>
@@ -8902,13 +8902,13 @@
         <v>45056</v>
       </c>
       <c r="G85">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="H85" s="2">
         <v>45240</v>
       </c>
       <c r="I85">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="J85" t="inlineStr">
         <is>
@@ -9005,13 +9005,13 @@
         <v>45085</v>
       </c>
       <c r="G86">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="H86" s="2">
         <v>45268</v>
       </c>
       <c r="I86">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="J86" t="inlineStr">
         <is>
@@ -9108,7 +9108,7 @@
         <v>45194</v>
       </c>
       <c r="I87">
-        <v>-6</v>
+        <v>-8</v>
       </c>
       <c r="J87" t="inlineStr">
         <is>
@@ -9195,13 +9195,13 @@
         <v>45103</v>
       </c>
       <c r="G88">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="H88" s="2">
         <v>45286</v>
       </c>
       <c r="I88">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="J88" t="inlineStr">
         <is>
@@ -9298,13 +9298,13 @@
         <v>45103</v>
       </c>
       <c r="G89">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="H89" s="2">
         <v>45286</v>
       </c>
       <c r="I89">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="J89" t="inlineStr">
         <is>
@@ -9401,13 +9401,13 @@
         <v>45008</v>
       </c>
       <c r="G90">
-        <v>192</v>
+        <v>194</v>
       </c>
       <c r="H90" s="2">
         <v>45192</v>
       </c>
       <c r="I90">
-        <v>-8</v>
+        <v>-10</v>
       </c>
       <c r="J90" t="inlineStr">
         <is>
@@ -9499,13 +9499,13 @@
         <v>45100</v>
       </c>
       <c r="G91">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="H91" s="2">
         <v>45287</v>
       </c>
       <c r="I91">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="J91" t="inlineStr">
         <is>
@@ -9602,13 +9602,13 @@
         <v>45003</v>
       </c>
       <c r="G92">
-        <v>197</v>
+        <v>199</v>
       </c>
       <c r="H92" s="2">
         <v>45187</v>
       </c>
       <c r="I92">
-        <v>-13</v>
+        <v>-15</v>
       </c>
       <c r="J92" t="inlineStr">
         <is>
@@ -9705,13 +9705,13 @@
         <v>45104</v>
       </c>
       <c r="G93">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="H93" s="2">
         <v>45287</v>
       </c>
       <c r="I93">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="J93" t="inlineStr">
         <is>
@@ -9808,13 +9808,13 @@
         <v>45104</v>
       </c>
       <c r="G94">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="H94" s="2">
         <v>45287</v>
       </c>
       <c r="I94">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="J94" t="inlineStr">
         <is>
@@ -9911,13 +9911,13 @@
         <v>45049</v>
       </c>
       <c r="G95">
-        <v>151</v>
+        <v>153</v>
       </c>
       <c r="H95" s="2">
         <v>45233</v>
       </c>
       <c r="I95">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="J95" t="inlineStr">
         <is>
@@ -10014,13 +10014,13 @@
         <v>45122</v>
       </c>
       <c r="G96">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="H96" s="2">
         <v>45306</v>
       </c>
       <c r="I96">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="J96" t="inlineStr">
         <is>
@@ -10112,13 +10112,13 @@
         <v>45141</v>
       </c>
       <c r="G97">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="H97" s="2">
         <v>45325</v>
       </c>
       <c r="I97">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="J97" t="inlineStr">
         <is>
@@ -10215,13 +10215,13 @@
         <v>45010</v>
       </c>
       <c r="G98">
-        <v>190</v>
+        <v>192</v>
       </c>
       <c r="H98" s="2">
         <v>45194</v>
       </c>
       <c r="I98">
-        <v>-6</v>
+        <v>-8</v>
       </c>
       <c r="J98" t="inlineStr">
         <is>
@@ -10313,13 +10313,13 @@
         <v>45093</v>
       </c>
       <c r="G99">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="H99" s="2">
         <v>45276</v>
       </c>
       <c r="I99">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="J99" t="inlineStr">
         <is>
@@ -10416,13 +10416,13 @@
         <v>45123</v>
       </c>
       <c r="G100">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="H100" s="2">
         <v>45307</v>
       </c>
       <c r="I100">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="J100" t="inlineStr">
         <is>
@@ -10519,13 +10519,13 @@
         <v>45014</v>
       </c>
       <c r="G101">
-        <v>186</v>
+        <v>188</v>
       </c>
       <c r="H101" s="2">
         <v>45198</v>
       </c>
       <c r="I101">
-        <v>-2</v>
+        <v>-4</v>
       </c>
       <c r="J101" t="inlineStr">
         <is>
@@ -10622,13 +10622,13 @@
         <v>45093</v>
       </c>
       <c r="G102">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="H102" s="2">
         <v>45276</v>
       </c>
       <c r="I102">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="J102" t="inlineStr">
         <is>
@@ -10725,13 +10725,13 @@
         <v>45122</v>
       </c>
       <c r="G103">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="H103" s="2">
         <v>45306</v>
       </c>
       <c r="I103">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="J103" t="inlineStr">
         <is>
@@ -10828,13 +10828,13 @@
         <v>45122</v>
       </c>
       <c r="G104">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="H104" s="2">
         <v>45306</v>
       </c>
       <c r="I104">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="J104" t="inlineStr">
         <is>
@@ -10926,13 +10926,13 @@
         <v>45050</v>
       </c>
       <c r="G105">
-        <v>150</v>
+        <v>152</v>
       </c>
       <c r="H105" s="2">
         <v>45234</v>
       </c>
       <c r="I105">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="J105" t="inlineStr">
         <is>
@@ -11029,13 +11029,13 @@
         <v>45085</v>
       </c>
       <c r="G106">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="H106" s="2">
         <v>45268</v>
       </c>
       <c r="I106">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="J106" t="inlineStr">
         <is>
@@ -11132,13 +11132,13 @@
         <v>45093</v>
       </c>
       <c r="G107">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="H107" s="2">
         <v>45185</v>
       </c>
       <c r="I107">
-        <v>-15</v>
+        <v>-17</v>
       </c>
       <c r="J107" t="inlineStr">
         <is>
@@ -11230,13 +11230,13 @@
         <v>45093</v>
       </c>
       <c r="G108">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="H108" s="2">
         <v>45185</v>
       </c>
       <c r="I108">
-        <v>-15</v>
+        <v>-17</v>
       </c>
       <c r="J108" t="inlineStr">
         <is>
@@ -11328,13 +11328,13 @@
         <v>45093</v>
       </c>
       <c r="G109">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="H109" s="2">
         <v>45185</v>
       </c>
       <c r="I109">
-        <v>-15</v>
+        <v>-17</v>
       </c>
       <c r="J109" t="inlineStr">
         <is>
@@ -11431,13 +11431,13 @@
         <v>45148</v>
       </c>
       <c r="G110">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="H110" s="2">
         <v>45240</v>
       </c>
       <c r="I110">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="J110" t="inlineStr">
         <is>
@@ -11534,13 +11534,13 @@
         <v>45119</v>
       </c>
       <c r="G111">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="H111" s="2">
         <v>45211</v>
       </c>
       <c r="I111">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="J111" t="inlineStr">
         <is>
@@ -11637,13 +11637,13 @@
         <v>45172</v>
       </c>
       <c r="G112">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="H112" s="2">
         <v>45263</v>
       </c>
       <c r="I112">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="J112" t="inlineStr">
         <is>
@@ -11740,13 +11740,13 @@
         <v>45023</v>
       </c>
       <c r="G113">
-        <v>177</v>
+        <v>179</v>
       </c>
       <c r="H113" s="2">
         <v>45206</v>
       </c>
       <c r="I113">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="J113" t="inlineStr">
         <is>
@@ -11843,13 +11843,13 @@
         <v>45111</v>
       </c>
       <c r="G114">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="H114" s="2">
         <v>45203</v>
       </c>
       <c r="I114">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="J114" t="inlineStr">
         <is>
@@ -11946,7 +11946,7 @@
         <v>45218</v>
       </c>
       <c r="I115">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="J115" t="inlineStr">
         <is>
@@ -12043,13 +12043,13 @@
         <v>45161</v>
       </c>
       <c r="G116">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="H116" s="2">
         <v>45253</v>
       </c>
       <c r="I116">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="J116" t="inlineStr">
         <is>
@@ -12146,13 +12146,13 @@
         <v>45115</v>
       </c>
       <c r="G117">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="H117" s="2">
         <v>45299</v>
       </c>
       <c r="I117">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="J117" t="inlineStr">
         <is>
@@ -12244,13 +12244,13 @@
         <v>45094</v>
       </c>
       <c r="G118">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="H118" s="2">
         <v>45277</v>
       </c>
       <c r="I118">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="J118" t="inlineStr">
         <is>
@@ -12347,13 +12347,13 @@
         <v>45104</v>
       </c>
       <c r="G119">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="H119" s="2">
         <v>45287</v>
       </c>
       <c r="I119">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="J119" t="inlineStr">
         <is>
@@ -12450,13 +12450,13 @@
         <v>45104</v>
       </c>
       <c r="G120">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="H120" s="2">
         <v>45287</v>
       </c>
       <c r="I120">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="J120" t="inlineStr">
         <is>
@@ -12553,13 +12553,13 @@
         <v>45104</v>
       </c>
       <c r="G121">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="H121" s="2">
         <v>45287</v>
       </c>
       <c r="I121">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="J121" t="inlineStr">
         <is>
@@ -12656,13 +12656,13 @@
         <v>45104</v>
       </c>
       <c r="G122">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="H122" s="2">
         <v>45287</v>
       </c>
       <c r="I122">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="J122" t="inlineStr">
         <is>
@@ -12759,13 +12759,13 @@
         <v>45107</v>
       </c>
       <c r="G123">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="H123" s="2">
         <v>45199</v>
       </c>
       <c r="I123">
-        <v>-1</v>
+        <v>-3</v>
       </c>
       <c r="J123" t="inlineStr">
         <is>
@@ -12862,13 +12862,13 @@
         <v>45013</v>
       </c>
       <c r="G124">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="H124" s="2">
         <v>45197</v>
       </c>
       <c r="I124">
-        <v>-3</v>
+        <v>-5</v>
       </c>
       <c r="J124" t="inlineStr">
         <is>
@@ -12965,13 +12965,13 @@
         <v>45121</v>
       </c>
       <c r="G125">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="H125" s="2">
         <v>45213</v>
       </c>
       <c r="I125">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="J125" t="inlineStr">
         <is>
@@ -13068,13 +13068,13 @@
         <v>45134</v>
       </c>
       <c r="G126">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="H126" s="2">
         <v>45226</v>
       </c>
       <c r="I126">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="J126" t="inlineStr">
         <is>
@@ -13171,7 +13171,7 @@
         <v>45212</v>
       </c>
       <c r="I127">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="J127" t="inlineStr">
         <is>
@@ -13268,13 +13268,13 @@
         <v>45126</v>
       </c>
       <c r="G128">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="H128" s="2">
         <v>45218</v>
       </c>
       <c r="I128">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="J128" t="inlineStr">
         <is>
@@ -13366,13 +13366,13 @@
         <v>45158</v>
       </c>
       <c r="G129">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="H129" s="2">
         <v>45250</v>
       </c>
       <c r="I129">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="J129" t="inlineStr">
         <is>
@@ -13469,13 +13469,13 @@
         <v>45171</v>
       </c>
       <c r="G130">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="H130" s="2">
         <v>45262</v>
       </c>
       <c r="I130">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="J130" t="inlineStr">
         <is>
@@ -13572,13 +13572,13 @@
         <v>45111</v>
       </c>
       <c r="G131">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="H131" s="2">
         <v>45203</v>
       </c>
       <c r="I131">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="J131" t="inlineStr">
         <is>
@@ -13675,13 +13675,13 @@
         <v>45144</v>
       </c>
       <c r="G132">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="H132" s="2">
         <v>45236</v>
       </c>
       <c r="I132">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="J132" t="inlineStr">
         <is>
@@ -13778,13 +13778,13 @@
         <v>45156</v>
       </c>
       <c r="G133">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="H133" s="2">
         <v>45248</v>
       </c>
       <c r="I133">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="J133" t="inlineStr">
         <is>
@@ -13876,13 +13876,13 @@
         <v>45146</v>
       </c>
       <c r="G134">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="H134" s="2">
         <v>45238</v>
       </c>
       <c r="I134">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="J134" t="inlineStr">
         <is>
@@ -13979,13 +13979,13 @@
         <v>45140</v>
       </c>
       <c r="G135">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="H135" s="2">
         <v>45232</v>
       </c>
       <c r="I135">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="J135" t="inlineStr">
         <is>
@@ -14082,13 +14082,13 @@
         <v>45104</v>
       </c>
       <c r="G136">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="H136" s="2">
         <v>45196</v>
       </c>
       <c r="I136">
-        <v>-4</v>
+        <v>-6</v>
       </c>
       <c r="J136" t="inlineStr">
         <is>
@@ -14185,13 +14185,13 @@
         <v>45105</v>
       </c>
       <c r="G137">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="H137" s="2">
         <v>45197</v>
       </c>
       <c r="I137">
-        <v>-3</v>
+        <v>-5</v>
       </c>
       <c r="J137" t="inlineStr">
         <is>
@@ -14288,13 +14288,13 @@
         <v>45179</v>
       </c>
       <c r="G138">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="H138" s="2">
         <v>45270</v>
       </c>
       <c r="I138">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="J138" t="inlineStr">
         <is>
@@ -14386,13 +14386,13 @@
         <v>45105</v>
       </c>
       <c r="G139">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="H139" s="2">
         <v>45197</v>
       </c>
       <c r="I139">
-        <v>-3</v>
+        <v>-5</v>
       </c>
       <c r="J139" t="inlineStr">
         <is>
@@ -14489,13 +14489,13 @@
         <v>45182</v>
       </c>
       <c r="G140">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="H140" s="2">
         <v>45273</v>
       </c>
       <c r="I140">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="J140" t="inlineStr">
         <is>
@@ -14592,13 +14592,13 @@
         <v>45116</v>
       </c>
       <c r="G141">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="H141" s="2">
         <v>45208</v>
       </c>
       <c r="I141">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="J141" t="inlineStr">
         <is>
@@ -14690,13 +14690,13 @@
         <v>45150</v>
       </c>
       <c r="G142">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="H142" s="2">
         <v>45242</v>
       </c>
       <c r="I142">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="J142" t="inlineStr">
         <is>
@@ -14793,7 +14793,7 @@
         <v>45238</v>
       </c>
       <c r="I143">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="J143" t="inlineStr">
         <is>
@@ -14890,13 +14890,13 @@
         <v>45171</v>
       </c>
       <c r="G144">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="H144" s="2">
         <v>45262</v>
       </c>
       <c r="I144">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="J144" t="inlineStr">
         <is>
@@ -14993,13 +14993,13 @@
         <v>45102</v>
       </c>
       <c r="G145">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="H145" s="2">
         <v>45194</v>
       </c>
       <c r="I145">
-        <v>-6</v>
+        <v>-8</v>
       </c>
       <c r="J145" t="inlineStr">
         <is>
@@ -15086,13 +15086,13 @@
         <v>45119</v>
       </c>
       <c r="G146">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="H146" s="2">
         <v>45211</v>
       </c>
       <c r="I146">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="J146" t="inlineStr">
         <is>
@@ -15189,13 +15189,13 @@
         <v>45165</v>
       </c>
       <c r="G147">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="H147" s="2">
         <v>45257</v>
       </c>
       <c r="I147">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="J147" t="inlineStr">
         <is>
@@ -15292,13 +15292,13 @@
         <v>45166</v>
       </c>
       <c r="G148">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="H148" s="2">
         <v>45258</v>
       </c>
       <c r="I148">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="J148" t="inlineStr">
         <is>
@@ -15395,13 +15395,13 @@
         <v>45093</v>
       </c>
       <c r="G149">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="H149" s="2">
         <v>45185</v>
       </c>
       <c r="I149">
-        <v>-15</v>
+        <v>-17</v>
       </c>
       <c r="J149" t="inlineStr">
         <is>
@@ -15498,13 +15498,13 @@
         <v>45035</v>
       </c>
       <c r="G150">
-        <v>165</v>
+        <v>167</v>
       </c>
       <c r="H150" s="2">
         <v>45218</v>
       </c>
       <c r="I150">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="J150" t="inlineStr">
         <is>
@@ -15601,13 +15601,13 @@
         <v>45174</v>
       </c>
       <c r="G151">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="H151" s="2">
         <v>45356</v>
       </c>
       <c r="I151">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="J151" t="inlineStr">
         <is>
@@ -15704,13 +15704,13 @@
         <v>45089</v>
       </c>
       <c r="G152">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="H152" s="2">
         <v>45272</v>
       </c>
       <c r="I152">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="J152" t="inlineStr">
         <is>
@@ -15807,13 +15807,13 @@
         <v>45124</v>
       </c>
       <c r="G153">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="H153" s="2">
         <v>45308</v>
       </c>
       <c r="I153">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="J153" t="inlineStr">
         <is>
@@ -15910,13 +15910,13 @@
         <v>45124</v>
       </c>
       <c r="G154">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="H154" s="2">
         <v>45308</v>
       </c>
       <c r="I154">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="J154" t="inlineStr">
         <is>
@@ -16013,13 +16013,13 @@
         <v>45026</v>
       </c>
       <c r="G155">
-        <v>174</v>
+        <v>176</v>
       </c>
       <c r="H155" s="2">
         <v>45209</v>
       </c>
       <c r="I155">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="J155" t="inlineStr">
         <is>
@@ -16116,13 +16116,13 @@
         <v>45026</v>
       </c>
       <c r="G156">
-        <v>174</v>
+        <v>176</v>
       </c>
       <c r="H156" s="2">
         <v>45209</v>
       </c>
       <c r="I156">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="J156" t="inlineStr">
         <is>
@@ -16219,13 +16219,13 @@
         <v>45026</v>
       </c>
       <c r="G157">
-        <v>174</v>
+        <v>176</v>
       </c>
       <c r="H157" s="2">
         <v>45209</v>
       </c>
       <c r="I157">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="J157" t="inlineStr">
         <is>
@@ -16322,13 +16322,13 @@
         <v>45026</v>
       </c>
       <c r="G158">
-        <v>174</v>
+        <v>176</v>
       </c>
       <c r="H158" s="2">
         <v>45209</v>
       </c>
       <c r="I158">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="J158" t="inlineStr">
         <is>
@@ -16425,13 +16425,13 @@
         <v>45156</v>
       </c>
       <c r="G159">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="H159" s="2">
         <v>45247</v>
       </c>
       <c r="I159">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="J159" t="inlineStr">
         <is>
@@ -16528,13 +16528,13 @@
         <v>45153</v>
       </c>
       <c r="G160">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="H160" s="2">
         <v>45245</v>
       </c>
       <c r="I160">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="J160" t="inlineStr">
         <is>
@@ -16631,13 +16631,13 @@
         <v>45135</v>
       </c>
       <c r="G161">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="H161" s="2">
         <v>45319</v>
       </c>
       <c r="I161">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="J161" t="inlineStr">
         <is>
@@ -16734,13 +16734,13 @@
         <v>45091</v>
       </c>
       <c r="G162">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="H162" s="2">
         <v>45274</v>
       </c>
       <c r="I162">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="J162" t="inlineStr">
         <is>
@@ -16832,13 +16832,13 @@
         <v>45091</v>
       </c>
       <c r="G163">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="H163" s="2">
         <v>45274</v>
       </c>
       <c r="I163">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="J163" t="inlineStr">
         <is>
@@ -16930,13 +16930,13 @@
         <v>45138</v>
       </c>
       <c r="G164">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="H164" s="2">
         <v>45322</v>
       </c>
       <c r="I164">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="J164" t="inlineStr">
         <is>
@@ -17033,13 +17033,13 @@
         <v>45138</v>
       </c>
       <c r="G165">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="H165" s="2">
         <v>45322</v>
       </c>
       <c r="I165">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="J165" t="inlineStr">
         <is>
@@ -17136,13 +17136,13 @@
         <v>45085</v>
       </c>
       <c r="G166">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="H166" s="2">
         <v>45268</v>
       </c>
       <c r="I166">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="J166" t="inlineStr">
         <is>
@@ -17239,13 +17239,13 @@
         <v>45085</v>
       </c>
       <c r="G167">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="H167" s="2">
         <v>45268</v>
       </c>
       <c r="I167">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="J167" t="inlineStr">
         <is>
@@ -17342,7 +17342,7 @@
         <v>45326</v>
       </c>
       <c r="I168">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="J168" t="inlineStr">
         <is>
@@ -17439,13 +17439,13 @@
         <v>45173</v>
       </c>
       <c r="G169">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="H169" s="2">
         <v>45355</v>
       </c>
       <c r="I169">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="J169" t="inlineStr">
         <is>
@@ -17542,13 +17542,13 @@
         <v>45056</v>
       </c>
       <c r="G170">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="H170" s="2">
         <v>45240</v>
       </c>
       <c r="I170">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="J170" t="inlineStr">
         <is>
@@ -17645,7 +17645,7 @@
         <v>45238</v>
       </c>
       <c r="I171">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="J171" t="inlineStr">
         <is>
@@ -17742,13 +17742,13 @@
         <v>45141</v>
       </c>
       <c r="G172">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="H172" s="2">
         <v>45325</v>
       </c>
       <c r="I172">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="J172" t="inlineStr">
         <is>
@@ -17845,13 +17845,13 @@
         <v>45037</v>
       </c>
       <c r="G173">
-        <v>163</v>
+        <v>165</v>
       </c>
       <c r="H173" s="2">
         <v>45220</v>
       </c>
       <c r="I173">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="J173" t="inlineStr">
         <is>
@@ -17948,13 +17948,13 @@
         <v>45171</v>
       </c>
       <c r="G174">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="H174" s="2">
         <v>45262</v>
       </c>
       <c r="I174">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="J174" t="inlineStr">
         <is>
@@ -18051,13 +18051,13 @@
         <v>45105</v>
       </c>
       <c r="G175">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="H175" s="2">
         <v>45197</v>
       </c>
       <c r="I175">
-        <v>-3</v>
+        <v>-5</v>
       </c>
       <c r="J175" t="inlineStr">
         <is>
@@ -18154,13 +18154,13 @@
         <v>45162</v>
       </c>
       <c r="G176">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="H176" s="2">
         <v>45254</v>
       </c>
       <c r="I176">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="J176" t="inlineStr">
         <is>
@@ -18257,13 +18257,13 @@
         <v>45061</v>
       </c>
       <c r="G177">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="H177" s="2">
         <v>45245</v>
       </c>
       <c r="I177">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="J177" t="inlineStr">
         <is>
@@ -18360,13 +18360,13 @@
         <v>45120</v>
       </c>
       <c r="G178">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="H178" s="2">
         <v>45212</v>
       </c>
       <c r="I178">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="J178" t="inlineStr">
         <is>
@@ -18463,7 +18463,7 @@
         <v>45191</v>
       </c>
       <c r="I179">
-        <v>-9</v>
+        <v>-11</v>
       </c>
       <c r="J179" t="inlineStr">
         <is>
@@ -18560,13 +18560,13 @@
         <v>45088</v>
       </c>
       <c r="G180">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="H180" s="2">
         <v>45271</v>
       </c>
       <c r="I180">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="J180" t="inlineStr">
         <is>
@@ -18663,13 +18663,13 @@
         <v>45100</v>
       </c>
       <c r="G181">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="H181" s="2">
         <v>45192</v>
       </c>
       <c r="I181">
-        <v>-8</v>
+        <v>-10</v>
       </c>
       <c r="J181" t="inlineStr">
         <is>
@@ -18756,13 +18756,13 @@
         <v>45131</v>
       </c>
       <c r="G182">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="H182" s="2">
         <v>45223</v>
       </c>
       <c r="I182">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="J182" t="inlineStr">
         <is>
@@ -18854,13 +18854,13 @@
         <v>45136</v>
       </c>
       <c r="G183">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="H183" s="2">
         <v>45228</v>
       </c>
       <c r="I183">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="J183" t="inlineStr">
         <is>
@@ -18952,13 +18952,13 @@
         <v>45150</v>
       </c>
       <c r="G184">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="H184" s="2">
         <v>45242</v>
       </c>
       <c r="I184">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="J184" t="inlineStr">
         <is>
@@ -19050,13 +19050,13 @@
         <v>45118</v>
       </c>
       <c r="G185">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="H185" s="2">
         <v>45210</v>
       </c>
       <c r="I185">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="J185" t="inlineStr">
         <is>
@@ -19148,13 +19148,13 @@
         <v>45129</v>
       </c>
       <c r="G186">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="H186" s="2">
         <v>45221</v>
       </c>
       <c r="I186">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="J186" t="inlineStr">
         <is>
@@ -19246,13 +19246,13 @@
         <v>45097</v>
       </c>
       <c r="G187">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="H187" s="2">
         <v>45189</v>
       </c>
       <c r="I187">
-        <v>-11</v>
+        <v>-13</v>
       </c>
       <c r="J187" t="inlineStr">
         <is>
@@ -19339,13 +19339,13 @@
         <v>45101</v>
       </c>
       <c r="G188">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="H188" s="2">
         <v>45193</v>
       </c>
       <c r="I188">
-        <v>-7</v>
+        <v>-9</v>
       </c>
       <c r="J188" t="inlineStr">
         <is>
@@ -19432,13 +19432,13 @@
         <v>45165</v>
       </c>
       <c r="G189">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="H189" s="2">
         <v>45257</v>
       </c>
       <c r="I189">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="J189" t="inlineStr">
         <is>
@@ -19530,7 +19530,7 @@
         <v>45202</v>
       </c>
       <c r="I190">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J190" t="inlineStr">
         <is>
@@ -19627,13 +19627,13 @@
         <v>45081</v>
       </c>
       <c r="G191">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="H191" s="2">
         <v>45264</v>
       </c>
       <c r="I191">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="J191" t="inlineStr">
         <is>
@@ -19730,13 +19730,13 @@
         <v>45081</v>
       </c>
       <c r="G192">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="H192" s="2">
         <v>45264</v>
       </c>
       <c r="I192">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="J192" t="inlineStr">
         <is>
@@ -19833,7 +19833,7 @@
         <v>45319</v>
       </c>
       <c r="I193">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="J193" t="inlineStr">
         <is>
@@ -19930,7 +19930,7 @@
         <v>45319</v>
       </c>
       <c r="I194">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="J194" t="inlineStr">
         <is>
@@ -20022,13 +20022,13 @@
         <v>45046</v>
       </c>
       <c r="G195">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="H195" s="2">
         <v>45230</v>
       </c>
       <c r="I195">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="J195" t="inlineStr">
         <is>
@@ -20125,13 +20125,13 @@
         <v>45046</v>
       </c>
       <c r="G196">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="H196" s="2">
         <v>45230</v>
       </c>
       <c r="I196">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="J196" t="inlineStr">
         <is>
@@ -20228,13 +20228,13 @@
         <v>45031</v>
       </c>
       <c r="G197">
-        <v>169</v>
+        <v>171</v>
       </c>
       <c r="H197" s="2">
         <v>45214</v>
       </c>
       <c r="I197">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="J197" t="inlineStr">
         <is>
@@ -20331,13 +20331,13 @@
         <v>45031</v>
       </c>
       <c r="G198">
-        <v>169</v>
+        <v>171</v>
       </c>
       <c r="H198" s="2">
         <v>45214</v>
       </c>
       <c r="I198">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="J198" t="inlineStr">
         <is>
@@ -20434,13 +20434,13 @@
         <v>45031</v>
       </c>
       <c r="G199">
-        <v>169</v>
+        <v>171</v>
       </c>
       <c r="H199" s="2">
         <v>45214</v>
       </c>
       <c r="I199">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="J199" t="inlineStr">
         <is>
@@ -20537,13 +20537,13 @@
         <v>45031</v>
       </c>
       <c r="G200">
-        <v>169</v>
+        <v>171</v>
       </c>
       <c r="H200" s="2">
         <v>45214</v>
       </c>
       <c r="I200">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="J200" t="inlineStr">
         <is>
@@ -20640,13 +20640,13 @@
         <v>45067</v>
       </c>
       <c r="G201">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="H201" s="2">
         <v>45251</v>
       </c>
       <c r="I201">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="J201" t="inlineStr">
         <is>
@@ -20743,13 +20743,13 @@
         <v>45067</v>
       </c>
       <c r="G202">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="H202" s="2">
         <v>45251</v>
       </c>
       <c r="I202">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="J202" t="inlineStr">
         <is>
@@ -20846,13 +20846,13 @@
         <v>45067</v>
       </c>
       <c r="G203">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="H203" s="2">
         <v>45251</v>
       </c>
       <c r="I203">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="J203" t="inlineStr">
         <is>
@@ -20949,13 +20949,13 @@
         <v>45067</v>
       </c>
       <c r="G204">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="H204" s="2">
         <v>45251</v>
       </c>
       <c r="I204">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="J204" t="inlineStr">
         <is>
@@ -21052,13 +21052,13 @@
         <v>45178</v>
       </c>
       <c r="G205">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="H205" s="2">
         <v>45269</v>
       </c>
       <c r="I205">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="J205" t="inlineStr">
         <is>
@@ -21155,7 +21155,7 @@
         <v>45252</v>
       </c>
       <c r="I206">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="J206" t="inlineStr">
         <is>
@@ -21252,13 +21252,13 @@
         <v>45087</v>
       </c>
       <c r="G207">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="H207" s="2">
         <v>45270</v>
       </c>
       <c r="I207">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="J207" t="inlineStr">
         <is>
@@ -21355,13 +21355,13 @@
         <v>45099</v>
       </c>
       <c r="G208">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="H208" s="2">
         <v>45282</v>
       </c>
       <c r="I208">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="J208" t="inlineStr">
         <is>
@@ -21458,13 +21458,13 @@
         <v>45175</v>
       </c>
       <c r="G209">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="H209" s="2">
         <v>45356</v>
       </c>
       <c r="I209">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="J209" t="inlineStr">
         <is>
@@ -21561,13 +21561,13 @@
         <v>45175</v>
       </c>
       <c r="G210">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="H210" s="2">
         <v>45356</v>
       </c>
       <c r="I210">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="J210" t="inlineStr">
         <is>
@@ -21664,13 +21664,13 @@
         <v>45166</v>
       </c>
       <c r="G211">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="H211" s="2">
         <v>45350</v>
       </c>
       <c r="I211">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="J211" t="inlineStr">
         <is>
@@ -21767,13 +21767,13 @@
         <v>45166</v>
       </c>
       <c r="G212">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="H212" s="2">
         <v>45350</v>
       </c>
       <c r="I212">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="J212" t="inlineStr">
         <is>
@@ -21870,13 +21870,13 @@
         <v>45090</v>
       </c>
       <c r="G213">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="H213" s="2">
         <v>45273</v>
       </c>
       <c r="I213">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="J213" t="inlineStr">
         <is>
@@ -21973,13 +21973,13 @@
         <v>45106</v>
       </c>
       <c r="G214">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="H214" s="2">
         <v>45289</v>
       </c>
       <c r="I214">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="J214" t="inlineStr">
         <is>
@@ -22076,13 +22076,13 @@
         <v>45134</v>
       </c>
       <c r="G215">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="H215" s="2">
         <v>45226</v>
       </c>
       <c r="I215">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="J215" t="inlineStr">
         <is>
@@ -22179,13 +22179,13 @@
         <v>45132</v>
       </c>
       <c r="G216">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="H216" s="2">
         <v>45224</v>
       </c>
       <c r="I216">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="J216" t="inlineStr">
         <is>
@@ -22282,13 +22282,13 @@
         <v>45150</v>
       </c>
       <c r="G217">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="H217" s="2">
         <v>45242</v>
       </c>
       <c r="I217">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="J217" t="inlineStr">
         <is>
@@ -22385,13 +22385,13 @@
         <v>45095</v>
       </c>
       <c r="G218">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="H218" s="2">
         <v>45187</v>
       </c>
       <c r="I218">
-        <v>-13</v>
+        <v>-15</v>
       </c>
       <c r="J218" t="inlineStr">
         <is>
@@ -22483,13 +22483,13 @@
         <v>45182</v>
       </c>
       <c r="G219">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="H219" s="2">
         <v>45273</v>
       </c>
       <c r="I219">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="J219" t="inlineStr">
         <is>
@@ -22586,7 +22586,7 @@
         <v>45196</v>
       </c>
       <c r="I220">
-        <v>-4</v>
+        <v>-6</v>
       </c>
       <c r="J220" t="inlineStr">
         <is>
@@ -22683,13 +22683,13 @@
         <v>45108</v>
       </c>
       <c r="G221">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="H221" s="2">
         <v>45200</v>
       </c>
       <c r="I221">
-        <v>0</v>
+        <v>-2</v>
       </c>
       <c r="J221" t="inlineStr">
         <is>
@@ -22786,13 +22786,13 @@
         <v>45135</v>
       </c>
       <c r="G222">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="H222" s="2">
         <v>45227</v>
       </c>
       <c r="I222">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="J222" t="inlineStr">
         <is>
@@ -22889,13 +22889,13 @@
         <v>45148</v>
       </c>
       <c r="G223">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="H223" s="2">
         <v>45240</v>
       </c>
       <c r="I223">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="J223" t="inlineStr">
         <is>
@@ -22987,13 +22987,13 @@
         <v>45100</v>
       </c>
       <c r="G224">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="H224" s="2">
         <v>45192</v>
       </c>
       <c r="I224">
-        <v>-8</v>
+        <v>-10</v>
       </c>
       <c r="J224" t="inlineStr">
         <is>
@@ -23085,13 +23085,13 @@
         <v>45136</v>
       </c>
       <c r="G225">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="H225" s="2">
         <v>45320</v>
       </c>
       <c r="I225">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="J225" t="inlineStr">
         <is>
@@ -23188,13 +23188,13 @@
         <v>45136</v>
       </c>
       <c r="G226">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="H226" s="2">
         <v>45320</v>
       </c>
       <c r="I226">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="J226" t="inlineStr">
         <is>
@@ -23291,13 +23291,13 @@
         <v>45094</v>
       </c>
       <c r="G227">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="H227" s="2">
         <v>45277</v>
       </c>
       <c r="I227">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="J227" t="inlineStr">
         <is>
@@ -23394,13 +23394,13 @@
         <v>45081</v>
       </c>
       <c r="G228">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="H228" s="2">
         <v>45264</v>
       </c>
       <c r="I228">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="J228" t="inlineStr">
         <is>
@@ -23497,13 +23497,13 @@
         <v>45099</v>
       </c>
       <c r="G229">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="H229" s="2">
         <v>45282</v>
       </c>
       <c r="I229">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="J229" t="inlineStr">
         <is>
@@ -23600,13 +23600,13 @@
         <v>45018</v>
       </c>
       <c r="G230">
-        <v>182</v>
+        <v>184</v>
       </c>
       <c r="H230" s="2">
         <v>45201</v>
       </c>
       <c r="I230">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="J230" t="inlineStr">
         <is>
@@ -23703,13 +23703,13 @@
         <v>45031</v>
       </c>
       <c r="G231">
-        <v>169</v>
+        <v>171</v>
       </c>
       <c r="H231" s="2">
         <v>45214</v>
       </c>
       <c r="I231">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="J231" t="inlineStr">
         <is>
@@ -23806,7 +23806,7 @@
         <v>45294</v>
       </c>
       <c r="I232">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="J232" t="inlineStr">
         <is>
@@ -23903,13 +23903,13 @@
         <v>45079</v>
       </c>
       <c r="G233">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="H233" s="2">
         <v>45262</v>
       </c>
       <c r="I233">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="J233" t="inlineStr">
         <is>
@@ -24006,7 +24006,7 @@
         <v>45199</v>
       </c>
       <c r="I234">
-        <v>-1</v>
+        <v>-3</v>
       </c>
       <c r="J234" t="inlineStr">
         <is>
@@ -24103,13 +24103,13 @@
         <v>45021</v>
       </c>
       <c r="G235">
-        <v>179</v>
+        <v>181</v>
       </c>
       <c r="H235" s="2">
         <v>45204</v>
       </c>
       <c r="I235">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="J235" t="inlineStr">
         <is>
@@ -24206,13 +24206,13 @@
         <v>45021</v>
       </c>
       <c r="G236">
-        <v>179</v>
+        <v>181</v>
       </c>
       <c r="H236" s="2">
         <v>45204</v>
       </c>
       <c r="I236">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="J236" t="inlineStr">
         <is>
@@ -24309,13 +24309,13 @@
         <v>45080</v>
       </c>
       <c r="G237">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="H237" s="2">
         <v>45263</v>
       </c>
       <c r="I237">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="J237" t="inlineStr">
         <is>
@@ -24412,13 +24412,13 @@
         <v>45046</v>
       </c>
       <c r="G238">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="H238" s="2">
         <v>45229</v>
       </c>
       <c r="I238">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="J238" t="inlineStr">
         <is>
@@ -24515,13 +24515,13 @@
         <v>45112</v>
       </c>
       <c r="G239">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="H239" s="2">
         <v>45204</v>
       </c>
       <c r="I239">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="J239" t="inlineStr">
         <is>
@@ -24609,13 +24609,13 @@
         <v>45112</v>
       </c>
       <c r="G240">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="H240" s="2">
         <v>45204</v>
       </c>
       <c r="I240">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="J240" t="inlineStr">
         <is>
@@ -24703,13 +24703,13 @@
         <v>45016</v>
       </c>
       <c r="G241">
-        <v>184</v>
+        <v>186</v>
       </c>
       <c r="H241" s="2">
         <v>45199</v>
       </c>
       <c r="I241">
-        <v>-1</v>
+        <v>-3</v>
       </c>
       <c r="J241" t="inlineStr">
         <is>
@@ -24806,13 +24806,13 @@
         <v>45070</v>
       </c>
       <c r="G242">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="H242" s="2">
         <v>45254</v>
       </c>
       <c r="I242">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="J242" t="inlineStr">
         <is>
@@ -24909,13 +24909,13 @@
         <v>45168</v>
       </c>
       <c r="G243">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="H243" s="2">
         <v>45260</v>
       </c>
       <c r="I243">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="J243" t="inlineStr">
         <is>
@@ -25012,13 +25012,13 @@
         <v>45027</v>
       </c>
       <c r="G244">
-        <v>173</v>
+        <v>175</v>
       </c>
       <c r="H244" s="2">
         <v>45210</v>
       </c>
       <c r="I244">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="J244" t="inlineStr">
         <is>
@@ -25115,13 +25115,13 @@
         <v>45077</v>
       </c>
       <c r="G245">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="H245" s="2">
         <v>45260</v>
       </c>
       <c r="I245">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="J245" t="inlineStr">
         <is>
@@ -25218,13 +25218,13 @@
         <v>45100</v>
       </c>
       <c r="G246">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="H246" s="2">
         <v>45283</v>
       </c>
       <c r="I246">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="J246" t="inlineStr">
         <is>
@@ -25321,7 +25321,7 @@
         <v>45281</v>
       </c>
       <c r="I247">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="J247" t="inlineStr">
         <is>
@@ -25418,13 +25418,13 @@
         <v>45044</v>
       </c>
       <c r="G248">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="H248" s="2">
         <v>45227</v>
       </c>
       <c r="I248">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="J248" t="inlineStr">
         <is>
@@ -25521,13 +25521,13 @@
         <v>45101</v>
       </c>
       <c r="G249">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="H249" s="2">
         <v>45283</v>
       </c>
       <c r="I249">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="J249" t="inlineStr">
         <is>
@@ -25624,13 +25624,13 @@
         <v>45134</v>
       </c>
       <c r="G250">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="H250" s="2">
         <v>45226</v>
       </c>
       <c r="I250">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="J250" t="inlineStr">
         <is>
@@ -25727,13 +25727,13 @@
         <v>45158</v>
       </c>
       <c r="G251">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="H251" s="2">
         <v>45250</v>
       </c>
       <c r="I251">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="J251" t="inlineStr">
         <is>
@@ -25830,13 +25830,13 @@
         <v>45108</v>
       </c>
       <c r="G252">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="H252" s="2">
         <v>45200</v>
       </c>
       <c r="I252">
-        <v>0</v>
+        <v>-2</v>
       </c>
       <c r="J252" t="inlineStr">
         <is>
@@ -25933,7 +25933,7 @@
         <v>45317</v>
       </c>
       <c r="I253">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="J253" t="inlineStr">
         <is>
@@ -26030,13 +26030,13 @@
         <v>45039</v>
       </c>
       <c r="G254">
-        <v>161</v>
+        <v>163</v>
       </c>
       <c r="H254" s="2">
         <v>45222</v>
       </c>
       <c r="I254">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="J254" t="inlineStr">
         <is>
@@ -26128,13 +26128,13 @@
         <v>45129</v>
       </c>
       <c r="G255">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="H255" s="2">
         <v>45221</v>
       </c>
       <c r="I255">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="J255" t="inlineStr">
         <is>
@@ -26231,13 +26231,13 @@
         <v>45157</v>
       </c>
       <c r="G256">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="H256" s="2">
         <v>45341</v>
       </c>
       <c r="I256">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="J256" t="inlineStr">
         <is>
@@ -26334,13 +26334,13 @@
         <v>45063</v>
       </c>
       <c r="G257">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="H257" s="2">
         <v>45247</v>
       </c>
       <c r="I257">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="J257" t="inlineStr">
         <is>
@@ -26437,7 +26437,7 @@
         <v>45254</v>
       </c>
       <c r="I258">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="J258" t="inlineStr">
         <is>
@@ -26534,7 +26534,7 @@
         <v>45486</v>
       </c>
       <c r="I259">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="J259" t="inlineStr">
         <is>
@@ -26626,13 +26626,13 @@
         <v>45073</v>
       </c>
       <c r="G260">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="H260" s="2">
         <v>45439</v>
       </c>
       <c r="I260">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="J260" t="inlineStr">
         <is>
@@ -26724,7 +26724,7 @@
         <v>45323</v>
       </c>
       <c r="I261">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="J261" t="inlineStr">
         <is>
@@ -26816,7 +26816,7 @@
         <v>45303</v>
       </c>
       <c r="I262">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="J262" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
Bond dates update Wed Oct  4 23:16:23 UTC 2023
</commit_message>
<xml_diff>
--- a/Data/obligacje_screener.xlsx
+++ b/Data/obligacje_screener.xlsx
@@ -512,7 +512,7 @@
         <v>45340</v>
       </c>
       <c r="I2">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="J2" t="inlineStr">
         <is>
@@ -600,13 +600,13 @@
         <v>45121</v>
       </c>
       <c r="G3">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="H3" s="2">
         <v>45305</v>
       </c>
       <c r="I3">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="J3" t="inlineStr">
         <is>
@@ -703,13 +703,13 @@
         <v>45039</v>
       </c>
       <c r="G4">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="H4" s="2">
         <v>45222</v>
       </c>
       <c r="I4">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="J4" t="inlineStr">
         <is>
@@ -806,13 +806,13 @@
         <v>45039</v>
       </c>
       <c r="G5">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="H5" s="2">
         <v>45222</v>
       </c>
       <c r="I5">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="J5" t="inlineStr">
         <is>
@@ -909,13 +909,13 @@
         <v>45129</v>
       </c>
       <c r="G6">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="H6" s="2">
         <v>45221</v>
       </c>
       <c r="I6">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="J6" t="inlineStr">
         <is>
@@ -1012,13 +1012,13 @@
         <v>45162</v>
       </c>
       <c r="G7">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="H7" s="2">
         <v>45254</v>
       </c>
       <c r="I7">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="J7" t="inlineStr">
         <is>
@@ -1110,13 +1110,13 @@
         <v>45156</v>
       </c>
       <c r="G8">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="H8" s="2">
         <v>45248</v>
       </c>
       <c r="I8">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="J8" t="inlineStr">
         <is>
@@ -1213,13 +1213,13 @@
         <v>45141</v>
       </c>
       <c r="G9">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="H9" s="2">
         <v>45233</v>
       </c>
       <c r="I9">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="J9" t="inlineStr">
         <is>
@@ -1316,13 +1316,13 @@
         <v>45062</v>
       </c>
       <c r="G10">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="H10" s="2">
         <v>45246</v>
       </c>
       <c r="I10">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="J10" t="inlineStr">
         <is>
@@ -1419,7 +1419,7 @@
         <v>45286</v>
       </c>
       <c r="I11">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="J11" t="inlineStr">
         <is>
@@ -1516,13 +1516,13 @@
         <v>45011</v>
       </c>
       <c r="G12">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="H12" s="2">
         <v>45195</v>
       </c>
       <c r="I12">
-        <v>-7</v>
+        <v>-8</v>
       </c>
       <c r="J12" t="inlineStr">
         <is>
@@ -1614,13 +1614,13 @@
         <v>45036</v>
       </c>
       <c r="G13">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="H13" s="2">
         <v>45219</v>
       </c>
       <c r="I13">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="J13" t="inlineStr">
         <is>
@@ -1717,13 +1717,13 @@
         <v>45036</v>
       </c>
       <c r="G14">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="H14" s="2">
         <v>45219</v>
       </c>
       <c r="I14">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="J14" t="inlineStr">
         <is>
@@ -1820,13 +1820,13 @@
         <v>45106</v>
       </c>
       <c r="G15">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="H15" s="2">
         <v>45289</v>
       </c>
       <c r="I15">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="J15" t="inlineStr">
         <is>
@@ -1923,13 +1923,13 @@
         <v>45094</v>
       </c>
       <c r="G16">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="H16" s="2">
         <v>45186</v>
       </c>
       <c r="I16">
-        <v>-16</v>
+        <v>-17</v>
       </c>
       <c r="J16" t="inlineStr">
         <is>
@@ -2026,13 +2026,13 @@
         <v>45094</v>
       </c>
       <c r="G17">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="H17" s="2">
         <v>45186</v>
       </c>
       <c r="I17">
-        <v>-16</v>
+        <v>-17</v>
       </c>
       <c r="J17" t="inlineStr">
         <is>
@@ -2129,13 +2129,13 @@
         <v>45132</v>
       </c>
       <c r="G18">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="H18" s="2">
         <v>45224</v>
       </c>
       <c r="I18">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="J18" t="inlineStr">
         <is>
@@ -2232,13 +2232,13 @@
         <v>45137</v>
       </c>
       <c r="G19">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="H19" s="2">
         <v>45229</v>
       </c>
       <c r="I19">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="J19" t="inlineStr">
         <is>
@@ -2330,13 +2330,13 @@
         <v>45183</v>
       </c>
       <c r="G20">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="H20" s="2">
         <v>45274</v>
       </c>
       <c r="I20">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="J20" t="inlineStr">
         <is>
@@ -2433,13 +2433,13 @@
         <v>45093</v>
       </c>
       <c r="G21">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="H21" s="2">
         <v>45187</v>
       </c>
       <c r="I21">
-        <v>-15</v>
+        <v>-16</v>
       </c>
       <c r="J21" t="inlineStr">
         <is>
@@ -2536,13 +2536,13 @@
         <v>45096</v>
       </c>
       <c r="G22">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="H22" s="2">
         <v>45187</v>
       </c>
       <c r="I22">
-        <v>-15</v>
+        <v>-16</v>
       </c>
       <c r="J22" t="inlineStr">
         <is>
@@ -2639,7 +2639,7 @@
         <v>45245</v>
       </c>
       <c r="I23">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="J23" t="inlineStr">
         <is>
@@ -2736,7 +2736,7 @@
         <v>45245</v>
       </c>
       <c r="I24">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="J24" t="inlineStr">
         <is>
@@ -2833,13 +2833,13 @@
         <v>45021</v>
       </c>
       <c r="G25">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="H25" s="2">
         <v>45204</v>
       </c>
       <c r="I25">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J25" t="inlineStr">
         <is>
@@ -2936,13 +2936,13 @@
         <v>45160</v>
       </c>
       <c r="G26">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="H26" s="2">
         <v>45344</v>
       </c>
       <c r="I26">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="J26" t="inlineStr">
         <is>
@@ -3039,13 +3039,13 @@
         <v>45118</v>
       </c>
       <c r="G27">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="H27" s="2">
         <v>45302</v>
       </c>
       <c r="I27">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="J27" t="inlineStr">
         <is>
@@ -3142,13 +3142,13 @@
         <v>45085</v>
       </c>
       <c r="G28">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="H28" s="2">
         <v>45268</v>
       </c>
       <c r="I28">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="J28" t="inlineStr">
         <is>
@@ -3245,13 +3245,13 @@
         <v>45183</v>
       </c>
       <c r="G29">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="H29" s="2">
         <v>45274</v>
       </c>
       <c r="I29">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="J29" t="inlineStr">
         <is>
@@ -3348,7 +3348,7 @@
         <v>45224</v>
       </c>
       <c r="I30">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="J30" t="inlineStr">
         <is>
@@ -3445,13 +3445,13 @@
         <v>45153</v>
       </c>
       <c r="G31">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="H31" s="2">
         <v>45245</v>
       </c>
       <c r="I31">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="J31" t="inlineStr">
         <is>
@@ -3548,13 +3548,13 @@
         <v>45155</v>
       </c>
       <c r="G32">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="H32" s="2">
         <v>45247</v>
       </c>
       <c r="I32">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="J32" t="inlineStr">
         <is>
@@ -3651,7 +3651,7 @@
         <v>45255</v>
       </c>
       <c r="I33">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="J33" t="inlineStr">
         <is>
@@ -3739,13 +3739,13 @@
         <v>45176</v>
       </c>
       <c r="G34">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="H34" s="2">
         <v>45267</v>
       </c>
       <c r="I34">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="J34" t="inlineStr">
         <is>
@@ -3842,13 +3842,13 @@
         <v>45130</v>
       </c>
       <c r="G35">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="H35" s="2">
         <v>45222</v>
       </c>
       <c r="I35">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="J35" t="inlineStr">
         <is>
@@ -3940,13 +3940,13 @@
         <v>45115</v>
       </c>
       <c r="G36">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="H36" s="2">
         <v>45207</v>
       </c>
       <c r="I36">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="J36" t="inlineStr">
         <is>
@@ -4043,13 +4043,13 @@
         <v>45097</v>
       </c>
       <c r="G37">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="H37" s="2">
         <v>45189</v>
       </c>
       <c r="I37">
-        <v>-13</v>
+        <v>-14</v>
       </c>
       <c r="J37" t="inlineStr">
         <is>
@@ -4141,13 +4141,13 @@
         <v>45107</v>
       </c>
       <c r="G38">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="H38" s="2">
         <v>45290</v>
       </c>
       <c r="I38">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="J38" t="inlineStr">
         <is>
@@ -4244,13 +4244,13 @@
         <v>45063</v>
       </c>
       <c r="G39">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="H39" s="2">
         <v>45247</v>
       </c>
       <c r="I39">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="J39" t="inlineStr">
         <is>
@@ -4347,13 +4347,13 @@
         <v>45177</v>
       </c>
       <c r="G40">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="H40" s="2">
         <v>45359</v>
       </c>
       <c r="I40">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="J40" t="inlineStr">
         <is>
@@ -4450,13 +4450,13 @@
         <v>45107</v>
       </c>
       <c r="G41">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="H41" s="2">
         <v>45290</v>
       </c>
       <c r="I41">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="J41" t="inlineStr">
         <is>
@@ -4553,7 +4553,7 @@
         <v>45265</v>
       </c>
       <c r="I42">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="J42" t="inlineStr">
         <is>
@@ -4650,13 +4650,13 @@
         <v>45098</v>
       </c>
       <c r="G43">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="H43" s="2">
         <v>45281</v>
       </c>
       <c r="I43">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="J43" t="inlineStr">
         <is>
@@ -4753,13 +4753,13 @@
         <v>45099</v>
       </c>
       <c r="G44">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="H44" s="2">
         <v>45282</v>
       </c>
       <c r="I44">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="J44" t="inlineStr">
         <is>
@@ -4856,13 +4856,13 @@
         <v>45106</v>
       </c>
       <c r="G45">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="H45" s="2">
         <v>45289</v>
       </c>
       <c r="I45">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="J45" t="inlineStr">
         <is>
@@ -4959,13 +4959,13 @@
         <v>45106</v>
       </c>
       <c r="G46">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="H46" s="2">
         <v>45289</v>
       </c>
       <c r="I46">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="J46" t="inlineStr">
         <is>
@@ -5062,13 +5062,13 @@
         <v>45120</v>
       </c>
       <c r="G47">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="H47" s="2">
         <v>45304</v>
       </c>
       <c r="I47">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="J47" t="inlineStr">
         <is>
@@ -5165,13 +5165,13 @@
         <v>45118</v>
       </c>
       <c r="G48">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="H48" s="2">
         <v>45302</v>
       </c>
       <c r="I48">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="J48" t="inlineStr">
         <is>
@@ -5268,13 +5268,13 @@
         <v>45152</v>
       </c>
       <c r="G49">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="H49" s="2">
         <v>45336</v>
       </c>
       <c r="I49">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="J49" t="inlineStr">
         <is>
@@ -5371,13 +5371,13 @@
         <v>45042</v>
       </c>
       <c r="G50">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="H50" s="2">
         <v>45225</v>
       </c>
       <c r="I50">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="J50" t="inlineStr">
         <is>
@@ -5474,13 +5474,13 @@
         <v>45122</v>
       </c>
       <c r="G51">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="H51" s="2">
         <v>45306</v>
       </c>
       <c r="I51">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="J51" t="inlineStr">
         <is>
@@ -5577,13 +5577,13 @@
         <v>45139</v>
       </c>
       <c r="G52">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="H52" s="2">
         <v>45323</v>
       </c>
       <c r="I52">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="J52" t="inlineStr">
         <is>
@@ -5671,13 +5671,13 @@
         <v>45099</v>
       </c>
       <c r="G53">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="H53" s="2">
         <v>45282</v>
       </c>
       <c r="I53">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="J53" t="inlineStr">
         <is>
@@ -5774,7 +5774,7 @@
         <v>45196</v>
       </c>
       <c r="I54">
-        <v>-6</v>
+        <v>-7</v>
       </c>
       <c r="J54" t="inlineStr">
         <is>
@@ -5871,13 +5871,13 @@
         <v>45044</v>
       </c>
       <c r="G55">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="H55" s="2">
         <v>45227</v>
       </c>
       <c r="I55">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="J55" t="inlineStr">
         <is>
@@ -5974,13 +5974,13 @@
         <v>45151</v>
       </c>
       <c r="G56">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="H56" s="2">
         <v>45243</v>
       </c>
       <c r="I56">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="J56" t="inlineStr">
         <is>
@@ -6072,7 +6072,7 @@
         <v>45196</v>
       </c>
       <c r="I57">
-        <v>-6</v>
+        <v>-7</v>
       </c>
       <c r="J57" t="inlineStr">
         <is>
@@ -6169,13 +6169,13 @@
         <v>45069</v>
       </c>
       <c r="G58">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="H58" s="2">
         <v>45253</v>
       </c>
       <c r="I58">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="J58" t="inlineStr">
         <is>
@@ -6272,13 +6272,13 @@
         <v>45099</v>
       </c>
       <c r="G59">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="H59" s="2">
         <v>45191</v>
       </c>
       <c r="I59">
-        <v>-11</v>
+        <v>-12</v>
       </c>
       <c r="J59" t="inlineStr">
         <is>
@@ -6370,13 +6370,13 @@
         <v>45113</v>
       </c>
       <c r="G60">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="H60" s="2">
         <v>45205</v>
       </c>
       <c r="I60">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="J60" t="inlineStr">
         <is>
@@ -6473,13 +6473,13 @@
         <v>45127</v>
       </c>
       <c r="G61">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="H61" s="2">
         <v>45219</v>
       </c>
       <c r="I61">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="J61" t="inlineStr">
         <is>
@@ -6576,13 +6576,13 @@
         <v>45058</v>
       </c>
       <c r="G62">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="H62" s="2">
         <v>45242</v>
       </c>
       <c r="I62">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="J62" t="inlineStr">
         <is>
@@ -6679,13 +6679,13 @@
         <v>45010</v>
       </c>
       <c r="G63">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="H63" s="2">
         <v>45194</v>
       </c>
       <c r="I63">
-        <v>-8</v>
+        <v>-9</v>
       </c>
       <c r="J63" t="inlineStr">
         <is>
@@ -6777,13 +6777,13 @@
         <v>45025</v>
       </c>
       <c r="G64">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="H64" s="2">
         <v>45208</v>
       </c>
       <c r="I64">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="J64" t="inlineStr">
         <is>
@@ -6880,13 +6880,13 @@
         <v>45025</v>
       </c>
       <c r="G65">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="H65" s="2">
         <v>45208</v>
       </c>
       <c r="I65">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="J65" t="inlineStr">
         <is>
@@ -6983,13 +6983,13 @@
         <v>45089</v>
       </c>
       <c r="G66">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="H66" s="2">
         <v>45272</v>
       </c>
       <c r="I66">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="J66" t="inlineStr">
         <is>
@@ -7086,13 +7086,13 @@
         <v>45178</v>
       </c>
       <c r="G67">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="H67" s="2">
         <v>45269</v>
       </c>
       <c r="I67">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="J67" t="inlineStr">
         <is>
@@ -7184,13 +7184,13 @@
         <v>45104</v>
       </c>
       <c r="G68">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="H68" s="2">
         <v>45196</v>
       </c>
       <c r="I68">
-        <v>-6</v>
+        <v>-7</v>
       </c>
       <c r="J68" t="inlineStr">
         <is>
@@ -7287,13 +7287,13 @@
         <v>45149</v>
       </c>
       <c r="G69">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="H69" s="2">
         <v>45241</v>
       </c>
       <c r="I69">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="J69" t="inlineStr">
         <is>
@@ -7390,7 +7390,7 @@
         <v>45205</v>
       </c>
       <c r="I70">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="J70" t="inlineStr">
         <is>
@@ -7487,13 +7487,13 @@
         <v>45114</v>
       </c>
       <c r="G71">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="H71" s="2">
         <v>45205</v>
       </c>
       <c r="I71">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="J71" t="inlineStr">
         <is>
@@ -7590,13 +7590,13 @@
         <v>45115</v>
       </c>
       <c r="G72">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="H72" s="2">
         <v>45207</v>
       </c>
       <c r="I72">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="J72" t="inlineStr">
         <is>
@@ -7693,13 +7693,13 @@
         <v>45097</v>
       </c>
       <c r="G73">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="H73" s="2">
         <v>45189</v>
       </c>
       <c r="I73">
-        <v>-13</v>
+        <v>-14</v>
       </c>
       <c r="J73" t="inlineStr">
         <is>
@@ -7791,13 +7791,13 @@
         <v>45038</v>
       </c>
       <c r="G74">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="H74" s="2">
         <v>45221</v>
       </c>
       <c r="I74">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="J74" t="inlineStr">
         <is>
@@ -7889,13 +7889,13 @@
         <v>45117</v>
       </c>
       <c r="G75">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="H75" s="2">
         <v>45301</v>
       </c>
       <c r="I75">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="J75" t="inlineStr">
         <is>
@@ -7992,13 +7992,13 @@
         <v>45160</v>
       </c>
       <c r="G76">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="H76" s="2">
         <v>45344</v>
       </c>
       <c r="I76">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="J76" t="inlineStr">
         <is>
@@ -8095,13 +8095,13 @@
         <v>45002</v>
       </c>
       <c r="G77">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="H77" s="2">
         <v>45186</v>
       </c>
       <c r="I77">
-        <v>-16</v>
+        <v>-17</v>
       </c>
       <c r="J77" t="inlineStr">
         <is>
@@ -8198,13 +8198,13 @@
         <v>45043</v>
       </c>
       <c r="G78">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="H78" s="2">
         <v>45226</v>
       </c>
       <c r="I78">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="J78" t="inlineStr">
         <is>
@@ -8301,13 +8301,13 @@
         <v>45079</v>
       </c>
       <c r="G79">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="H79" s="2">
         <v>45262</v>
       </c>
       <c r="I79">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="J79" t="inlineStr">
         <is>
@@ -8404,7 +8404,7 @@
         <v>45254</v>
       </c>
       <c r="I80">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="J80" t="inlineStr">
         <is>
@@ -8501,13 +8501,13 @@
         <v>45104</v>
       </c>
       <c r="G81">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="H81" s="2">
         <v>45287</v>
       </c>
       <c r="I81">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="J81" t="inlineStr">
         <is>
@@ -8604,7 +8604,7 @@
         <v>45288</v>
       </c>
       <c r="I82">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="J82" t="inlineStr">
         <is>
@@ -8696,13 +8696,13 @@
         <v>45175</v>
       </c>
       <c r="G83">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="H83" s="2">
         <v>45357</v>
       </c>
       <c r="I83">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="J83" t="inlineStr">
         <is>
@@ -8799,13 +8799,13 @@
         <v>45054</v>
       </c>
       <c r="G84">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="H84" s="2">
         <v>45238</v>
       </c>
       <c r="I84">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="J84" t="inlineStr">
         <is>
@@ -8902,13 +8902,13 @@
         <v>45056</v>
       </c>
       <c r="G85">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="H85" s="2">
         <v>45240</v>
       </c>
       <c r="I85">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="J85" t="inlineStr">
         <is>
@@ -9005,13 +9005,13 @@
         <v>45085</v>
       </c>
       <c r="G86">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="H86" s="2">
         <v>45268</v>
       </c>
       <c r="I86">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="J86" t="inlineStr">
         <is>
@@ -9108,7 +9108,7 @@
         <v>45194</v>
       </c>
       <c r="I87">
-        <v>-8</v>
+        <v>-9</v>
       </c>
       <c r="J87" t="inlineStr">
         <is>
@@ -9195,13 +9195,13 @@
         <v>45103</v>
       </c>
       <c r="G88">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="H88" s="2">
         <v>45286</v>
       </c>
       <c r="I88">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="J88" t="inlineStr">
         <is>
@@ -9298,13 +9298,13 @@
         <v>45103</v>
       </c>
       <c r="G89">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="H89" s="2">
         <v>45286</v>
       </c>
       <c r="I89">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="J89" t="inlineStr">
         <is>
@@ -9401,13 +9401,13 @@
         <v>45008</v>
       </c>
       <c r="G90">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="H90" s="2">
         <v>45192</v>
       </c>
       <c r="I90">
-        <v>-10</v>
+        <v>-11</v>
       </c>
       <c r="J90" t="inlineStr">
         <is>
@@ -9499,13 +9499,13 @@
         <v>45100</v>
       </c>
       <c r="G91">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="H91" s="2">
         <v>45287</v>
       </c>
       <c r="I91">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="J91" t="inlineStr">
         <is>
@@ -9602,13 +9602,13 @@
         <v>45003</v>
       </c>
       <c r="G92">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="H92" s="2">
         <v>45187</v>
       </c>
       <c r="I92">
-        <v>-15</v>
+        <v>-16</v>
       </c>
       <c r="J92" t="inlineStr">
         <is>
@@ -9705,13 +9705,13 @@
         <v>45104</v>
       </c>
       <c r="G93">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="H93" s="2">
         <v>45287</v>
       </c>
       <c r="I93">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="J93" t="inlineStr">
         <is>
@@ -9808,13 +9808,13 @@
         <v>45104</v>
       </c>
       <c r="G94">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="H94" s="2">
         <v>45287</v>
       </c>
       <c r="I94">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="J94" t="inlineStr">
         <is>
@@ -9911,13 +9911,13 @@
         <v>45049</v>
       </c>
       <c r="G95">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="H95" s="2">
         <v>45233</v>
       </c>
       <c r="I95">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="J95" t="inlineStr">
         <is>
@@ -10014,13 +10014,13 @@
         <v>45122</v>
       </c>
       <c r="G96">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="H96" s="2">
         <v>45306</v>
       </c>
       <c r="I96">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="J96" t="inlineStr">
         <is>
@@ -10112,13 +10112,13 @@
         <v>45141</v>
       </c>
       <c r="G97">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="H97" s="2">
         <v>45325</v>
       </c>
       <c r="I97">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="J97" t="inlineStr">
         <is>
@@ -10215,13 +10215,13 @@
         <v>45010</v>
       </c>
       <c r="G98">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="H98" s="2">
         <v>45194</v>
       </c>
       <c r="I98">
-        <v>-8</v>
+        <v>-9</v>
       </c>
       <c r="J98" t="inlineStr">
         <is>
@@ -10313,13 +10313,13 @@
         <v>45093</v>
       </c>
       <c r="G99">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="H99" s="2">
         <v>45276</v>
       </c>
       <c r="I99">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="J99" t="inlineStr">
         <is>
@@ -10416,13 +10416,13 @@
         <v>45123</v>
       </c>
       <c r="G100">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="H100" s="2">
         <v>45307</v>
       </c>
       <c r="I100">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="J100" t="inlineStr">
         <is>
@@ -10519,13 +10519,13 @@
         <v>45014</v>
       </c>
       <c r="G101">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="H101" s="2">
         <v>45198</v>
       </c>
       <c r="I101">
-        <v>-4</v>
+        <v>-5</v>
       </c>
       <c r="J101" t="inlineStr">
         <is>
@@ -10622,13 +10622,13 @@
         <v>45093</v>
       </c>
       <c r="G102">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="H102" s="2">
         <v>45276</v>
       </c>
       <c r="I102">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="J102" t="inlineStr">
         <is>
@@ -10725,13 +10725,13 @@
         <v>45122</v>
       </c>
       <c r="G103">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="H103" s="2">
         <v>45306</v>
       </c>
       <c r="I103">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="J103" t="inlineStr">
         <is>
@@ -10828,13 +10828,13 @@
         <v>45122</v>
       </c>
       <c r="G104">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="H104" s="2">
         <v>45306</v>
       </c>
       <c r="I104">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="J104" t="inlineStr">
         <is>
@@ -10926,13 +10926,13 @@
         <v>45050</v>
       </c>
       <c r="G105">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="H105" s="2">
         <v>45234</v>
       </c>
       <c r="I105">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="J105" t="inlineStr">
         <is>
@@ -11029,13 +11029,13 @@
         <v>45085</v>
       </c>
       <c r="G106">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="H106" s="2">
         <v>45268</v>
       </c>
       <c r="I106">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="J106" t="inlineStr">
         <is>
@@ -11132,13 +11132,13 @@
         <v>45093</v>
       </c>
       <c r="G107">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="H107" s="2">
         <v>45185</v>
       </c>
       <c r="I107">
-        <v>-17</v>
+        <v>-18</v>
       </c>
       <c r="J107" t="inlineStr">
         <is>
@@ -11230,13 +11230,13 @@
         <v>45093</v>
       </c>
       <c r="G108">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="H108" s="2">
         <v>45185</v>
       </c>
       <c r="I108">
-        <v>-17</v>
+        <v>-18</v>
       </c>
       <c r="J108" t="inlineStr">
         <is>
@@ -11328,13 +11328,13 @@
         <v>45093</v>
       </c>
       <c r="G109">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="H109" s="2">
         <v>45185</v>
       </c>
       <c r="I109">
-        <v>-17</v>
+        <v>-18</v>
       </c>
       <c r="J109" t="inlineStr">
         <is>
@@ -11431,13 +11431,13 @@
         <v>45148</v>
       </c>
       <c r="G110">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="H110" s="2">
         <v>45240</v>
       </c>
       <c r="I110">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="J110" t="inlineStr">
         <is>
@@ -11534,13 +11534,13 @@
         <v>45119</v>
       </c>
       <c r="G111">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="H111" s="2">
         <v>45211</v>
       </c>
       <c r="I111">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="J111" t="inlineStr">
         <is>
@@ -11637,13 +11637,13 @@
         <v>45172</v>
       </c>
       <c r="G112">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="H112" s="2">
         <v>45263</v>
       </c>
       <c r="I112">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="J112" t="inlineStr">
         <is>
@@ -11740,13 +11740,13 @@
         <v>45023</v>
       </c>
       <c r="G113">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="H113" s="2">
         <v>45206</v>
       </c>
       <c r="I113">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="J113" t="inlineStr">
         <is>
@@ -11843,13 +11843,13 @@
         <v>45111</v>
       </c>
       <c r="G114">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="H114" s="2">
         <v>45203</v>
       </c>
       <c r="I114">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J114" t="inlineStr">
         <is>
@@ -11946,7 +11946,7 @@
         <v>45218</v>
       </c>
       <c r="I115">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="J115" t="inlineStr">
         <is>
@@ -12043,13 +12043,13 @@
         <v>45161</v>
       </c>
       <c r="G116">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="H116" s="2">
         <v>45253</v>
       </c>
       <c r="I116">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="J116" t="inlineStr">
         <is>
@@ -12146,13 +12146,13 @@
         <v>45115</v>
       </c>
       <c r="G117">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="H117" s="2">
         <v>45299</v>
       </c>
       <c r="I117">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="J117" t="inlineStr">
         <is>
@@ -12244,13 +12244,13 @@
         <v>45094</v>
       </c>
       <c r="G118">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="H118" s="2">
         <v>45277</v>
       </c>
       <c r="I118">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="J118" t="inlineStr">
         <is>
@@ -12347,13 +12347,13 @@
         <v>45104</v>
       </c>
       <c r="G119">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="H119" s="2">
         <v>45287</v>
       </c>
       <c r="I119">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="J119" t="inlineStr">
         <is>
@@ -12450,13 +12450,13 @@
         <v>45104</v>
       </c>
       <c r="G120">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="H120" s="2">
         <v>45287</v>
       </c>
       <c r="I120">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="J120" t="inlineStr">
         <is>
@@ -12553,13 +12553,13 @@
         <v>45104</v>
       </c>
       <c r="G121">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="H121" s="2">
         <v>45287</v>
       </c>
       <c r="I121">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="J121" t="inlineStr">
         <is>
@@ -12656,13 +12656,13 @@
         <v>45104</v>
       </c>
       <c r="G122">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="H122" s="2">
         <v>45287</v>
       </c>
       <c r="I122">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="J122" t="inlineStr">
         <is>
@@ -12759,13 +12759,13 @@
         <v>45107</v>
       </c>
       <c r="G123">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="H123" s="2">
         <v>45199</v>
       </c>
       <c r="I123">
-        <v>-3</v>
+        <v>-4</v>
       </c>
       <c r="J123" t="inlineStr">
         <is>
@@ -12862,13 +12862,13 @@
         <v>45013</v>
       </c>
       <c r="G124">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="H124" s="2">
         <v>45197</v>
       </c>
       <c r="I124">
-        <v>-5</v>
+        <v>-6</v>
       </c>
       <c r="J124" t="inlineStr">
         <is>
@@ -12965,13 +12965,13 @@
         <v>45121</v>
       </c>
       <c r="G125">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="H125" s="2">
         <v>45213</v>
       </c>
       <c r="I125">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="J125" t="inlineStr">
         <is>
@@ -13068,13 +13068,13 @@
         <v>45134</v>
       </c>
       <c r="G126">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="H126" s="2">
         <v>45226</v>
       </c>
       <c r="I126">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="J126" t="inlineStr">
         <is>
@@ -13171,7 +13171,7 @@
         <v>45212</v>
       </c>
       <c r="I127">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="J127" t="inlineStr">
         <is>
@@ -13268,13 +13268,13 @@
         <v>45126</v>
       </c>
       <c r="G128">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="H128" s="2">
         <v>45218</v>
       </c>
       <c r="I128">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="J128" t="inlineStr">
         <is>
@@ -13366,13 +13366,13 @@
         <v>45158</v>
       </c>
       <c r="G129">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="H129" s="2">
         <v>45250</v>
       </c>
       <c r="I129">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="J129" t="inlineStr">
         <is>
@@ -13469,13 +13469,13 @@
         <v>45171</v>
       </c>
       <c r="G130">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="H130" s="2">
         <v>45262</v>
       </c>
       <c r="I130">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="J130" t="inlineStr">
         <is>
@@ -13572,13 +13572,13 @@
         <v>45111</v>
       </c>
       <c r="G131">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="H131" s="2">
         <v>45203</v>
       </c>
       <c r="I131">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J131" t="inlineStr">
         <is>
@@ -13675,13 +13675,13 @@
         <v>45144</v>
       </c>
       <c r="G132">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="H132" s="2">
         <v>45236</v>
       </c>
       <c r="I132">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="J132" t="inlineStr">
         <is>
@@ -13778,13 +13778,13 @@
         <v>45156</v>
       </c>
       <c r="G133">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="H133" s="2">
         <v>45248</v>
       </c>
       <c r="I133">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="J133" t="inlineStr">
         <is>
@@ -13876,13 +13876,13 @@
         <v>45146</v>
       </c>
       <c r="G134">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="H134" s="2">
         <v>45238</v>
       </c>
       <c r="I134">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="J134" t="inlineStr">
         <is>
@@ -13979,13 +13979,13 @@
         <v>45140</v>
       </c>
       <c r="G135">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="H135" s="2">
         <v>45232</v>
       </c>
       <c r="I135">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="J135" t="inlineStr">
         <is>
@@ -14082,13 +14082,13 @@
         <v>45104</v>
       </c>
       <c r="G136">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="H136" s="2">
         <v>45196</v>
       </c>
       <c r="I136">
-        <v>-6</v>
+        <v>-7</v>
       </c>
       <c r="J136" t="inlineStr">
         <is>
@@ -14185,13 +14185,13 @@
         <v>45105</v>
       </c>
       <c r="G137">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="H137" s="2">
         <v>45197</v>
       </c>
       <c r="I137">
-        <v>-5</v>
+        <v>-6</v>
       </c>
       <c r="J137" t="inlineStr">
         <is>
@@ -14288,13 +14288,13 @@
         <v>45179</v>
       </c>
       <c r="G138">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="H138" s="2">
         <v>45270</v>
       </c>
       <c r="I138">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="J138" t="inlineStr">
         <is>
@@ -14386,13 +14386,13 @@
         <v>45105</v>
       </c>
       <c r="G139">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="H139" s="2">
         <v>45197</v>
       </c>
       <c r="I139">
-        <v>-5</v>
+        <v>-6</v>
       </c>
       <c r="J139" t="inlineStr">
         <is>
@@ -14489,13 +14489,13 @@
         <v>45182</v>
       </c>
       <c r="G140">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="H140" s="2">
         <v>45273</v>
       </c>
       <c r="I140">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="J140" t="inlineStr">
         <is>
@@ -14592,13 +14592,13 @@
         <v>45116</v>
       </c>
       <c r="G141">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="H141" s="2">
         <v>45208</v>
       </c>
       <c r="I141">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="J141" t="inlineStr">
         <is>
@@ -14690,13 +14690,13 @@
         <v>45150</v>
       </c>
       <c r="G142">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="H142" s="2">
         <v>45242</v>
       </c>
       <c r="I142">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="J142" t="inlineStr">
         <is>
@@ -14793,7 +14793,7 @@
         <v>45238</v>
       </c>
       <c r="I143">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="J143" t="inlineStr">
         <is>
@@ -14890,13 +14890,13 @@
         <v>45171</v>
       </c>
       <c r="G144">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="H144" s="2">
         <v>45262</v>
       </c>
       <c r="I144">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="J144" t="inlineStr">
         <is>
@@ -14993,13 +14993,13 @@
         <v>45102</v>
       </c>
       <c r="G145">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="H145" s="2">
         <v>45194</v>
       </c>
       <c r="I145">
-        <v>-8</v>
+        <v>-9</v>
       </c>
       <c r="J145" t="inlineStr">
         <is>
@@ -15086,13 +15086,13 @@
         <v>45119</v>
       </c>
       <c r="G146">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="H146" s="2">
         <v>45211</v>
       </c>
       <c r="I146">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="J146" t="inlineStr">
         <is>
@@ -15189,13 +15189,13 @@
         <v>45165</v>
       </c>
       <c r="G147">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="H147" s="2">
         <v>45257</v>
       </c>
       <c r="I147">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="J147" t="inlineStr">
         <is>
@@ -15292,13 +15292,13 @@
         <v>45166</v>
       </c>
       <c r="G148">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="H148" s="2">
         <v>45258</v>
       </c>
       <c r="I148">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="J148" t="inlineStr">
         <is>
@@ -15395,13 +15395,13 @@
         <v>45093</v>
       </c>
       <c r="G149">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="H149" s="2">
         <v>45185</v>
       </c>
       <c r="I149">
-        <v>-17</v>
+        <v>-18</v>
       </c>
       <c r="J149" t="inlineStr">
         <is>
@@ -15498,13 +15498,13 @@
         <v>45035</v>
       </c>
       <c r="G150">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="H150" s="2">
         <v>45218</v>
       </c>
       <c r="I150">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="J150" t="inlineStr">
         <is>
@@ -15601,13 +15601,13 @@
         <v>45174</v>
       </c>
       <c r="G151">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="H151" s="2">
         <v>45356</v>
       </c>
       <c r="I151">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="J151" t="inlineStr">
         <is>
@@ -15704,13 +15704,13 @@
         <v>45089</v>
       </c>
       <c r="G152">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="H152" s="2">
         <v>45272</v>
       </c>
       <c r="I152">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="J152" t="inlineStr">
         <is>
@@ -15807,13 +15807,13 @@
         <v>45124</v>
       </c>
       <c r="G153">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="H153" s="2">
         <v>45308</v>
       </c>
       <c r="I153">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="J153" t="inlineStr">
         <is>
@@ -15910,13 +15910,13 @@
         <v>45124</v>
       </c>
       <c r="G154">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="H154" s="2">
         <v>45308</v>
       </c>
       <c r="I154">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="J154" t="inlineStr">
         <is>
@@ -16013,13 +16013,13 @@
         <v>45026</v>
       </c>
       <c r="G155">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="H155" s="2">
         <v>45209</v>
       </c>
       <c r="I155">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="J155" t="inlineStr">
         <is>
@@ -16116,13 +16116,13 @@
         <v>45026</v>
       </c>
       <c r="G156">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="H156" s="2">
         <v>45209</v>
       </c>
       <c r="I156">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="J156" t="inlineStr">
         <is>
@@ -16219,13 +16219,13 @@
         <v>45026</v>
       </c>
       <c r="G157">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="H157" s="2">
         <v>45209</v>
       </c>
       <c r="I157">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="J157" t="inlineStr">
         <is>
@@ -16322,13 +16322,13 @@
         <v>45026</v>
       </c>
       <c r="G158">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="H158" s="2">
         <v>45209</v>
       </c>
       <c r="I158">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="J158" t="inlineStr">
         <is>
@@ -16425,13 +16425,13 @@
         <v>45156</v>
       </c>
       <c r="G159">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="H159" s="2">
         <v>45247</v>
       </c>
       <c r="I159">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="J159" t="inlineStr">
         <is>
@@ -16528,13 +16528,13 @@
         <v>45153</v>
       </c>
       <c r="G160">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="H160" s="2">
         <v>45245</v>
       </c>
       <c r="I160">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="J160" t="inlineStr">
         <is>
@@ -16631,13 +16631,13 @@
         <v>45135</v>
       </c>
       <c r="G161">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="H161" s="2">
         <v>45319</v>
       </c>
       <c r="I161">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="J161" t="inlineStr">
         <is>
@@ -16734,13 +16734,13 @@
         <v>45091</v>
       </c>
       <c r="G162">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="H162" s="2">
         <v>45274</v>
       </c>
       <c r="I162">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="J162" t="inlineStr">
         <is>
@@ -16832,13 +16832,13 @@
         <v>45091</v>
       </c>
       <c r="G163">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="H163" s="2">
         <v>45274</v>
       </c>
       <c r="I163">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="J163" t="inlineStr">
         <is>
@@ -16930,13 +16930,13 @@
         <v>45138</v>
       </c>
       <c r="G164">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="H164" s="2">
         <v>45322</v>
       </c>
       <c r="I164">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="J164" t="inlineStr">
         <is>
@@ -17033,13 +17033,13 @@
         <v>45138</v>
       </c>
       <c r="G165">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="H165" s="2">
         <v>45322</v>
       </c>
       <c r="I165">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="J165" t="inlineStr">
         <is>
@@ -17136,13 +17136,13 @@
         <v>45085</v>
       </c>
       <c r="G166">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="H166" s="2">
         <v>45268</v>
       </c>
       <c r="I166">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="J166" t="inlineStr">
         <is>
@@ -17239,13 +17239,13 @@
         <v>45085</v>
       </c>
       <c r="G167">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="H167" s="2">
         <v>45268</v>
       </c>
       <c r="I167">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="J167" t="inlineStr">
         <is>
@@ -17342,7 +17342,7 @@
         <v>45326</v>
       </c>
       <c r="I168">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="J168" t="inlineStr">
         <is>
@@ -17439,13 +17439,13 @@
         <v>45173</v>
       </c>
       <c r="G169">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="H169" s="2">
         <v>45355</v>
       </c>
       <c r="I169">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="J169" t="inlineStr">
         <is>
@@ -17542,13 +17542,13 @@
         <v>45056</v>
       </c>
       <c r="G170">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="H170" s="2">
         <v>45240</v>
       </c>
       <c r="I170">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="J170" t="inlineStr">
         <is>
@@ -17645,7 +17645,7 @@
         <v>45238</v>
       </c>
       <c r="I171">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="J171" t="inlineStr">
         <is>
@@ -17742,13 +17742,13 @@
         <v>45141</v>
       </c>
       <c r="G172">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="H172" s="2">
         <v>45325</v>
       </c>
       <c r="I172">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="J172" t="inlineStr">
         <is>
@@ -17845,13 +17845,13 @@
         <v>45037</v>
       </c>
       <c r="G173">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="H173" s="2">
         <v>45220</v>
       </c>
       <c r="I173">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="J173" t="inlineStr">
         <is>
@@ -17948,13 +17948,13 @@
         <v>45171</v>
       </c>
       <c r="G174">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="H174" s="2">
         <v>45262</v>
       </c>
       <c r="I174">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="J174" t="inlineStr">
         <is>
@@ -18051,13 +18051,13 @@
         <v>45105</v>
       </c>
       <c r="G175">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="H175" s="2">
         <v>45197</v>
       </c>
       <c r="I175">
-        <v>-5</v>
+        <v>-6</v>
       </c>
       <c r="J175" t="inlineStr">
         <is>
@@ -18154,13 +18154,13 @@
         <v>45162</v>
       </c>
       <c r="G176">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="H176" s="2">
         <v>45254</v>
       </c>
       <c r="I176">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="J176" t="inlineStr">
         <is>
@@ -18257,13 +18257,13 @@
         <v>45061</v>
       </c>
       <c r="G177">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="H177" s="2">
         <v>45245</v>
       </c>
       <c r="I177">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="J177" t="inlineStr">
         <is>
@@ -18360,13 +18360,13 @@
         <v>45120</v>
       </c>
       <c r="G178">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="H178" s="2">
         <v>45212</v>
       </c>
       <c r="I178">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="J178" t="inlineStr">
         <is>
@@ -18463,7 +18463,7 @@
         <v>45191</v>
       </c>
       <c r="I179">
-        <v>-11</v>
+        <v>-12</v>
       </c>
       <c r="J179" t="inlineStr">
         <is>
@@ -18560,13 +18560,13 @@
         <v>45088</v>
       </c>
       <c r="G180">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="H180" s="2">
         <v>45271</v>
       </c>
       <c r="I180">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="J180" t="inlineStr">
         <is>
@@ -18663,13 +18663,13 @@
         <v>45100</v>
       </c>
       <c r="G181">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="H181" s="2">
         <v>45192</v>
       </c>
       <c r="I181">
-        <v>-10</v>
+        <v>-11</v>
       </c>
       <c r="J181" t="inlineStr">
         <is>
@@ -18756,13 +18756,13 @@
         <v>45131</v>
       </c>
       <c r="G182">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="H182" s="2">
         <v>45223</v>
       </c>
       <c r="I182">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="J182" t="inlineStr">
         <is>
@@ -18854,13 +18854,13 @@
         <v>45136</v>
       </c>
       <c r="G183">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="H183" s="2">
         <v>45228</v>
       </c>
       <c r="I183">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="J183" t="inlineStr">
         <is>
@@ -18952,13 +18952,13 @@
         <v>45150</v>
       </c>
       <c r="G184">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="H184" s="2">
         <v>45242</v>
       </c>
       <c r="I184">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="J184" t="inlineStr">
         <is>
@@ -19050,13 +19050,13 @@
         <v>45118</v>
       </c>
       <c r="G185">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="H185" s="2">
         <v>45210</v>
       </c>
       <c r="I185">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="J185" t="inlineStr">
         <is>
@@ -19148,13 +19148,13 @@
         <v>45129</v>
       </c>
       <c r="G186">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="H186" s="2">
         <v>45221</v>
       </c>
       <c r="I186">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="J186" t="inlineStr">
         <is>
@@ -19246,13 +19246,13 @@
         <v>45097</v>
       </c>
       <c r="G187">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="H187" s="2">
         <v>45189</v>
       </c>
       <c r="I187">
-        <v>-13</v>
+        <v>-14</v>
       </c>
       <c r="J187" t="inlineStr">
         <is>
@@ -19339,13 +19339,13 @@
         <v>45101</v>
       </c>
       <c r="G188">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="H188" s="2">
         <v>45193</v>
       </c>
       <c r="I188">
-        <v>-9</v>
+        <v>-10</v>
       </c>
       <c r="J188" t="inlineStr">
         <is>
@@ -19432,13 +19432,13 @@
         <v>45165</v>
       </c>
       <c r="G189">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="H189" s="2">
         <v>45257</v>
       </c>
       <c r="I189">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="J189" t="inlineStr">
         <is>
@@ -19530,7 +19530,7 @@
         <v>45202</v>
       </c>
       <c r="I190">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="J190" t="inlineStr">
         <is>
@@ -19627,13 +19627,13 @@
         <v>45081</v>
       </c>
       <c r="G191">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="H191" s="2">
         <v>45264</v>
       </c>
       <c r="I191">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="J191" t="inlineStr">
         <is>
@@ -19730,13 +19730,13 @@
         <v>45081</v>
       </c>
       <c r="G192">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="H192" s="2">
         <v>45264</v>
       </c>
       <c r="I192">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="J192" t="inlineStr">
         <is>
@@ -19833,7 +19833,7 @@
         <v>45319</v>
       </c>
       <c r="I193">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="J193" t="inlineStr">
         <is>
@@ -19930,7 +19930,7 @@
         <v>45319</v>
       </c>
       <c r="I194">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="J194" t="inlineStr">
         <is>
@@ -20022,13 +20022,13 @@
         <v>45046</v>
       </c>
       <c r="G195">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="H195" s="2">
         <v>45230</v>
       </c>
       <c r="I195">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="J195" t="inlineStr">
         <is>
@@ -20125,13 +20125,13 @@
         <v>45046</v>
       </c>
       <c r="G196">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="H196" s="2">
         <v>45230</v>
       </c>
       <c r="I196">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="J196" t="inlineStr">
         <is>
@@ -20228,13 +20228,13 @@
         <v>45031</v>
       </c>
       <c r="G197">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="H197" s="2">
         <v>45214</v>
       </c>
       <c r="I197">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="J197" t="inlineStr">
         <is>
@@ -20331,13 +20331,13 @@
         <v>45031</v>
       </c>
       <c r="G198">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="H198" s="2">
         <v>45214</v>
       </c>
       <c r="I198">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="J198" t="inlineStr">
         <is>
@@ -20434,13 +20434,13 @@
         <v>45031</v>
       </c>
       <c r="G199">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="H199" s="2">
         <v>45214</v>
       </c>
       <c r="I199">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="J199" t="inlineStr">
         <is>
@@ -20537,13 +20537,13 @@
         <v>45031</v>
       </c>
       <c r="G200">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="H200" s="2">
         <v>45214</v>
       </c>
       <c r="I200">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="J200" t="inlineStr">
         <is>
@@ -20640,13 +20640,13 @@
         <v>45067</v>
       </c>
       <c r="G201">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="H201" s="2">
         <v>45251</v>
       </c>
       <c r="I201">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="J201" t="inlineStr">
         <is>
@@ -20743,13 +20743,13 @@
         <v>45067</v>
       </c>
       <c r="G202">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="H202" s="2">
         <v>45251</v>
       </c>
       <c r="I202">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="J202" t="inlineStr">
         <is>
@@ -20846,13 +20846,13 @@
         <v>45067</v>
       </c>
       <c r="G203">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="H203" s="2">
         <v>45251</v>
       </c>
       <c r="I203">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="J203" t="inlineStr">
         <is>
@@ -20949,13 +20949,13 @@
         <v>45067</v>
       </c>
       <c r="G204">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="H204" s="2">
         <v>45251</v>
       </c>
       <c r="I204">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="J204" t="inlineStr">
         <is>
@@ -21052,13 +21052,13 @@
         <v>45178</v>
       </c>
       <c r="G205">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="H205" s="2">
         <v>45269</v>
       </c>
       <c r="I205">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="J205" t="inlineStr">
         <is>
@@ -21155,7 +21155,7 @@
         <v>45252</v>
       </c>
       <c r="I206">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="J206" t="inlineStr">
         <is>
@@ -21252,13 +21252,13 @@
         <v>45087</v>
       </c>
       <c r="G207">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="H207" s="2">
         <v>45270</v>
       </c>
       <c r="I207">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="J207" t="inlineStr">
         <is>
@@ -21355,13 +21355,13 @@
         <v>45099</v>
       </c>
       <c r="G208">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="H208" s="2">
         <v>45282</v>
       </c>
       <c r="I208">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="J208" t="inlineStr">
         <is>
@@ -21458,13 +21458,13 @@
         <v>45175</v>
       </c>
       <c r="G209">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="H209" s="2">
         <v>45356</v>
       </c>
       <c r="I209">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="J209" t="inlineStr">
         <is>
@@ -21561,13 +21561,13 @@
         <v>45175</v>
       </c>
       <c r="G210">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="H210" s="2">
         <v>45356</v>
       </c>
       <c r="I210">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="J210" t="inlineStr">
         <is>
@@ -21664,13 +21664,13 @@
         <v>45166</v>
       </c>
       <c r="G211">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="H211" s="2">
         <v>45350</v>
       </c>
       <c r="I211">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="J211" t="inlineStr">
         <is>
@@ -21767,13 +21767,13 @@
         <v>45166</v>
       </c>
       <c r="G212">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="H212" s="2">
         <v>45350</v>
       </c>
       <c r="I212">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="J212" t="inlineStr">
         <is>
@@ -21870,13 +21870,13 @@
         <v>45090</v>
       </c>
       <c r="G213">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="H213" s="2">
         <v>45273</v>
       </c>
       <c r="I213">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="J213" t="inlineStr">
         <is>
@@ -21973,13 +21973,13 @@
         <v>45106</v>
       </c>
       <c r="G214">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="H214" s="2">
         <v>45289</v>
       </c>
       <c r="I214">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="J214" t="inlineStr">
         <is>
@@ -22076,13 +22076,13 @@
         <v>45134</v>
       </c>
       <c r="G215">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="H215" s="2">
         <v>45226</v>
       </c>
       <c r="I215">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="J215" t="inlineStr">
         <is>
@@ -22179,13 +22179,13 @@
         <v>45132</v>
       </c>
       <c r="G216">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="H216" s="2">
         <v>45224</v>
       </c>
       <c r="I216">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="J216" t="inlineStr">
         <is>
@@ -22282,13 +22282,13 @@
         <v>45150</v>
       </c>
       <c r="G217">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="H217" s="2">
         <v>45242</v>
       </c>
       <c r="I217">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="J217" t="inlineStr">
         <is>
@@ -22385,13 +22385,13 @@
         <v>45095</v>
       </c>
       <c r="G218">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="H218" s="2">
         <v>45187</v>
       </c>
       <c r="I218">
-        <v>-15</v>
+        <v>-16</v>
       </c>
       <c r="J218" t="inlineStr">
         <is>
@@ -22483,13 +22483,13 @@
         <v>45182</v>
       </c>
       <c r="G219">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="H219" s="2">
         <v>45273</v>
       </c>
       <c r="I219">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="J219" t="inlineStr">
         <is>
@@ -22586,7 +22586,7 @@
         <v>45196</v>
       </c>
       <c r="I220">
-        <v>-6</v>
+        <v>-7</v>
       </c>
       <c r="J220" t="inlineStr">
         <is>
@@ -22683,13 +22683,13 @@
         <v>45108</v>
       </c>
       <c r="G221">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="H221" s="2">
         <v>45200</v>
       </c>
       <c r="I221">
-        <v>-2</v>
+        <v>-3</v>
       </c>
       <c r="J221" t="inlineStr">
         <is>
@@ -22786,13 +22786,13 @@
         <v>45135</v>
       </c>
       <c r="G222">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="H222" s="2">
         <v>45227</v>
       </c>
       <c r="I222">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="J222" t="inlineStr">
         <is>
@@ -22889,13 +22889,13 @@
         <v>45148</v>
       </c>
       <c r="G223">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="H223" s="2">
         <v>45240</v>
       </c>
       <c r="I223">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="J223" t="inlineStr">
         <is>
@@ -22987,13 +22987,13 @@
         <v>45100</v>
       </c>
       <c r="G224">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="H224" s="2">
         <v>45192</v>
       </c>
       <c r="I224">
-        <v>-10</v>
+        <v>-11</v>
       </c>
       <c r="J224" t="inlineStr">
         <is>
@@ -23085,13 +23085,13 @@
         <v>45136</v>
       </c>
       <c r="G225">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="H225" s="2">
         <v>45320</v>
       </c>
       <c r="I225">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="J225" t="inlineStr">
         <is>
@@ -23188,13 +23188,13 @@
         <v>45136</v>
       </c>
       <c r="G226">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="H226" s="2">
         <v>45320</v>
       </c>
       <c r="I226">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="J226" t="inlineStr">
         <is>
@@ -23291,13 +23291,13 @@
         <v>45094</v>
       </c>
       <c r="G227">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="H227" s="2">
         <v>45277</v>
       </c>
       <c r="I227">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="J227" t="inlineStr">
         <is>
@@ -23394,13 +23394,13 @@
         <v>45081</v>
       </c>
       <c r="G228">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="H228" s="2">
         <v>45264</v>
       </c>
       <c r="I228">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="J228" t="inlineStr">
         <is>
@@ -23497,13 +23497,13 @@
         <v>45099</v>
       </c>
       <c r="G229">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="H229" s="2">
         <v>45282</v>
       </c>
       <c r="I229">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="J229" t="inlineStr">
         <is>
@@ -23600,13 +23600,13 @@
         <v>45018</v>
       </c>
       <c r="G230">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="H230" s="2">
         <v>45201</v>
       </c>
       <c r="I230">
-        <v>-1</v>
+        <v>-2</v>
       </c>
       <c r="J230" t="inlineStr">
         <is>
@@ -23703,13 +23703,13 @@
         <v>45031</v>
       </c>
       <c r="G231">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="H231" s="2">
         <v>45214</v>
       </c>
       <c r="I231">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="J231" t="inlineStr">
         <is>
@@ -23806,7 +23806,7 @@
         <v>45294</v>
       </c>
       <c r="I232">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="J232" t="inlineStr">
         <is>
@@ -23903,13 +23903,13 @@
         <v>45079</v>
       </c>
       <c r="G233">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="H233" s="2">
         <v>45262</v>
       </c>
       <c r="I233">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="J233" t="inlineStr">
         <is>
@@ -24006,7 +24006,7 @@
         <v>45199</v>
       </c>
       <c r="I234">
-        <v>-3</v>
+        <v>-4</v>
       </c>
       <c r="J234" t="inlineStr">
         <is>
@@ -24103,13 +24103,13 @@
         <v>45021</v>
       </c>
       <c r="G235">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="H235" s="2">
         <v>45204</v>
       </c>
       <c r="I235">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J235" t="inlineStr">
         <is>
@@ -24206,13 +24206,13 @@
         <v>45021</v>
       </c>
       <c r="G236">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="H236" s="2">
         <v>45204</v>
       </c>
       <c r="I236">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J236" t="inlineStr">
         <is>
@@ -24309,13 +24309,13 @@
         <v>45080</v>
       </c>
       <c r="G237">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="H237" s="2">
         <v>45263</v>
       </c>
       <c r="I237">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="J237" t="inlineStr">
         <is>
@@ -24412,13 +24412,13 @@
         <v>45046</v>
       </c>
       <c r="G238">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="H238" s="2">
         <v>45229</v>
       </c>
       <c r="I238">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="J238" t="inlineStr">
         <is>
@@ -24515,13 +24515,13 @@
         <v>45112</v>
       </c>
       <c r="G239">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="H239" s="2">
         <v>45204</v>
       </c>
       <c r="I239">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J239" t="inlineStr">
         <is>
@@ -24609,13 +24609,13 @@
         <v>45112</v>
       </c>
       <c r="G240">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="H240" s="2">
         <v>45204</v>
       </c>
       <c r="I240">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J240" t="inlineStr">
         <is>
@@ -24703,13 +24703,13 @@
         <v>45016</v>
       </c>
       <c r="G241">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="H241" s="2">
         <v>45199</v>
       </c>
       <c r="I241">
-        <v>-3</v>
+        <v>-4</v>
       </c>
       <c r="J241" t="inlineStr">
         <is>
@@ -24806,13 +24806,13 @@
         <v>45070</v>
       </c>
       <c r="G242">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="H242" s="2">
         <v>45254</v>
       </c>
       <c r="I242">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="J242" t="inlineStr">
         <is>
@@ -24909,13 +24909,13 @@
         <v>45168</v>
       </c>
       <c r="G243">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="H243" s="2">
         <v>45260</v>
       </c>
       <c r="I243">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="J243" t="inlineStr">
         <is>
@@ -25012,13 +25012,13 @@
         <v>45027</v>
       </c>
       <c r="G244">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="H244" s="2">
         <v>45210</v>
       </c>
       <c r="I244">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="J244" t="inlineStr">
         <is>
@@ -25115,13 +25115,13 @@
         <v>45077</v>
       </c>
       <c r="G245">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="H245" s="2">
         <v>45260</v>
       </c>
       <c r="I245">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="J245" t="inlineStr">
         <is>
@@ -25218,13 +25218,13 @@
         <v>45100</v>
       </c>
       <c r="G246">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="H246" s="2">
         <v>45283</v>
       </c>
       <c r="I246">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="J246" t="inlineStr">
         <is>
@@ -25321,7 +25321,7 @@
         <v>45281</v>
       </c>
       <c r="I247">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="J247" t="inlineStr">
         <is>
@@ -25418,13 +25418,13 @@
         <v>45044</v>
       </c>
       <c r="G248">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="H248" s="2">
         <v>45227</v>
       </c>
       <c r="I248">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="J248" t="inlineStr">
         <is>
@@ -25521,13 +25521,13 @@
         <v>45101</v>
       </c>
       <c r="G249">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="H249" s="2">
         <v>45283</v>
       </c>
       <c r="I249">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="J249" t="inlineStr">
         <is>
@@ -25624,13 +25624,13 @@
         <v>45134</v>
       </c>
       <c r="G250">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="H250" s="2">
         <v>45226</v>
       </c>
       <c r="I250">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="J250" t="inlineStr">
         <is>
@@ -25727,13 +25727,13 @@
         <v>45158</v>
       </c>
       <c r="G251">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="H251" s="2">
         <v>45250</v>
       </c>
       <c r="I251">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="J251" t="inlineStr">
         <is>
@@ -25830,13 +25830,13 @@
         <v>45108</v>
       </c>
       <c r="G252">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="H252" s="2">
         <v>45200</v>
       </c>
       <c r="I252">
-        <v>-2</v>
+        <v>-3</v>
       </c>
       <c r="J252" t="inlineStr">
         <is>
@@ -25933,7 +25933,7 @@
         <v>45317</v>
       </c>
       <c r="I253">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="J253" t="inlineStr">
         <is>
@@ -26030,13 +26030,13 @@
         <v>45039</v>
       </c>
       <c r="G254">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="H254" s="2">
         <v>45222</v>
       </c>
       <c r="I254">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="J254" t="inlineStr">
         <is>
@@ -26128,13 +26128,13 @@
         <v>45129</v>
       </c>
       <c r="G255">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="H255" s="2">
         <v>45221</v>
       </c>
       <c r="I255">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="J255" t="inlineStr">
         <is>
@@ -26231,13 +26231,13 @@
         <v>45157</v>
       </c>
       <c r="G256">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="H256" s="2">
         <v>45341</v>
       </c>
       <c r="I256">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="J256" t="inlineStr">
         <is>
@@ -26334,13 +26334,13 @@
         <v>45063</v>
       </c>
       <c r="G257">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="H257" s="2">
         <v>45247</v>
       </c>
       <c r="I257">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="J257" t="inlineStr">
         <is>
@@ -26437,7 +26437,7 @@
         <v>45254</v>
       </c>
       <c r="I258">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="J258" t="inlineStr">
         <is>
@@ -26534,7 +26534,7 @@
         <v>45486</v>
       </c>
       <c r="I259">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="J259" t="inlineStr">
         <is>
@@ -26626,13 +26626,13 @@
         <v>45073</v>
       </c>
       <c r="G260">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="H260" s="2">
         <v>45439</v>
       </c>
       <c r="I260">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="J260" t="inlineStr">
         <is>
@@ -26724,7 +26724,7 @@
         <v>45323</v>
       </c>
       <c r="I261">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="J261" t="inlineStr">
         <is>
@@ -26816,7 +26816,7 @@
         <v>45303</v>
       </c>
       <c r="I262">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="J262" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
Bond dates update Thu Oct  5 15:58:48 UTC 2023
</commit_message>
<xml_diff>
--- a/Data/obligacje_screener.xlsx
+++ b/Data/obligacje_screener.xlsx
@@ -512,7 +512,7 @@
         <v>45340</v>
       </c>
       <c r="I2">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="J2" t="inlineStr">
         <is>
@@ -600,13 +600,13 @@
         <v>45121</v>
       </c>
       <c r="G3">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="H3" s="2">
         <v>45305</v>
       </c>
       <c r="I3">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="J3" t="inlineStr">
         <is>
@@ -703,13 +703,13 @@
         <v>45039</v>
       </c>
       <c r="G4">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="H4" s="2">
         <v>45222</v>
       </c>
       <c r="I4">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="J4" t="inlineStr">
         <is>
@@ -806,13 +806,13 @@
         <v>45039</v>
       </c>
       <c r="G5">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="H5" s="2">
         <v>45222</v>
       </c>
       <c r="I5">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="J5" t="inlineStr">
         <is>
@@ -909,13 +909,13 @@
         <v>45129</v>
       </c>
       <c r="G6">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="H6" s="2">
         <v>45221</v>
       </c>
       <c r="I6">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="J6" t="inlineStr">
         <is>
@@ -1012,13 +1012,13 @@
         <v>45162</v>
       </c>
       <c r="G7">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="H7" s="2">
         <v>45254</v>
       </c>
       <c r="I7">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="J7" t="inlineStr">
         <is>
@@ -1110,13 +1110,13 @@
         <v>45156</v>
       </c>
       <c r="G8">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="H8" s="2">
         <v>45248</v>
       </c>
       <c r="I8">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="J8" t="inlineStr">
         <is>
@@ -1213,13 +1213,13 @@
         <v>45141</v>
       </c>
       <c r="G9">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="H9" s="2">
         <v>45233</v>
       </c>
       <c r="I9">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="J9" t="inlineStr">
         <is>
@@ -1316,13 +1316,13 @@
         <v>45062</v>
       </c>
       <c r="G10">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="H10" s="2">
         <v>45246</v>
       </c>
       <c r="I10">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="J10" t="inlineStr">
         <is>
@@ -1419,7 +1419,7 @@
         <v>45286</v>
       </c>
       <c r="I11">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="J11" t="inlineStr">
         <is>
@@ -1513,16 +1513,16 @@
         </is>
       </c>
       <c r="F12" s="2">
-        <v>45011</v>
+        <v>45195</v>
       </c>
       <c r="G12">
-        <v>192</v>
+        <v>9</v>
       </c>
       <c r="H12" s="2">
-        <v>45195</v>
+        <v>45377</v>
       </c>
       <c r="I12">
-        <v>-8</v>
+        <v>173</v>
       </c>
       <c r="J12" t="inlineStr">
         <is>
@@ -1614,13 +1614,13 @@
         <v>45036</v>
       </c>
       <c r="G13">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="H13" s="2">
         <v>45219</v>
       </c>
       <c r="I13">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="J13" t="inlineStr">
         <is>
@@ -1717,13 +1717,13 @@
         <v>45036</v>
       </c>
       <c r="G14">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="H14" s="2">
         <v>45219</v>
       </c>
       <c r="I14">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="J14" t="inlineStr">
         <is>
@@ -1820,13 +1820,13 @@
         <v>45106</v>
       </c>
       <c r="G15">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="H15" s="2">
         <v>45289</v>
       </c>
       <c r="I15">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="J15" t="inlineStr">
         <is>
@@ -1920,16 +1920,16 @@
         </is>
       </c>
       <c r="F16" s="2">
-        <v>45094</v>
+        <v>45186</v>
       </c>
       <c r="G16">
-        <v>109</v>
+        <v>18</v>
       </c>
       <c r="H16" s="2">
-        <v>45186</v>
+        <v>45278</v>
       </c>
       <c r="I16">
-        <v>-17</v>
+        <v>74</v>
       </c>
       <c r="J16" t="inlineStr">
         <is>
@@ -2023,16 +2023,16 @@
         </is>
       </c>
       <c r="F17" s="2">
-        <v>45094</v>
+        <v>45186</v>
       </c>
       <c r="G17">
-        <v>109</v>
+        <v>18</v>
       </c>
       <c r="H17" s="2">
-        <v>45186</v>
+        <v>45277</v>
       </c>
       <c r="I17">
-        <v>-17</v>
+        <v>73</v>
       </c>
       <c r="J17" t="inlineStr">
         <is>
@@ -2129,13 +2129,13 @@
         <v>45132</v>
       </c>
       <c r="G18">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="H18" s="2">
         <v>45224</v>
       </c>
       <c r="I18">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="J18" t="inlineStr">
         <is>
@@ -2232,13 +2232,13 @@
         <v>45137</v>
       </c>
       <c r="G19">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="H19" s="2">
         <v>45229</v>
       </c>
       <c r="I19">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="J19" t="inlineStr">
         <is>
@@ -2330,13 +2330,13 @@
         <v>45183</v>
       </c>
       <c r="G20">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="H20" s="2">
         <v>45274</v>
       </c>
       <c r="I20">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="J20" t="inlineStr">
         <is>
@@ -2430,16 +2430,16 @@
         </is>
       </c>
       <c r="F21" s="2">
-        <v>45093</v>
+        <v>45187</v>
       </c>
       <c r="G21">
-        <v>110</v>
+        <v>17</v>
       </c>
       <c r="H21" s="2">
-        <v>45187</v>
+        <v>45278</v>
       </c>
       <c r="I21">
-        <v>-16</v>
+        <v>74</v>
       </c>
       <c r="J21" t="inlineStr">
         <is>
@@ -2533,16 +2533,16 @@
         </is>
       </c>
       <c r="F22" s="2">
-        <v>45096</v>
+        <v>45187</v>
       </c>
       <c r="G22">
-        <v>107</v>
+        <v>17</v>
       </c>
       <c r="H22" s="2">
-        <v>45187</v>
+        <v>45278</v>
       </c>
       <c r="I22">
-        <v>-16</v>
+        <v>74</v>
       </c>
       <c r="J22" t="inlineStr">
         <is>
@@ -2639,7 +2639,7 @@
         <v>45245</v>
       </c>
       <c r="I23">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="J23" t="inlineStr">
         <is>
@@ -2736,7 +2736,7 @@
         <v>45245</v>
       </c>
       <c r="I24">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="J24" t="inlineStr">
         <is>
@@ -2833,13 +2833,7 @@
         <v>45021</v>
       </c>
       <c r="G25">
-        <v>182</v>
-      </c>
-      <c r="H25" s="2">
-        <v>45204</v>
-      </c>
-      <c r="I25">
-        <v>1</v>
+        <v>183</v>
       </c>
       <c r="J25" t="inlineStr">
         <is>
@@ -2936,13 +2930,13 @@
         <v>45160</v>
       </c>
       <c r="G26">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="H26" s="2">
         <v>45344</v>
       </c>
       <c r="I26">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="J26" t="inlineStr">
         <is>
@@ -3039,13 +3033,13 @@
         <v>45118</v>
       </c>
       <c r="G27">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="H27" s="2">
         <v>45302</v>
       </c>
       <c r="I27">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="J27" t="inlineStr">
         <is>
@@ -3142,13 +3136,13 @@
         <v>45085</v>
       </c>
       <c r="G28">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="H28" s="2">
         <v>45268</v>
       </c>
       <c r="I28">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="J28" t="inlineStr">
         <is>
@@ -3245,13 +3239,13 @@
         <v>45183</v>
       </c>
       <c r="G29">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="H29" s="2">
         <v>45274</v>
       </c>
       <c r="I29">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="J29" t="inlineStr">
         <is>
@@ -3348,7 +3342,7 @@
         <v>45224</v>
       </c>
       <c r="I30">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="J30" t="inlineStr">
         <is>
@@ -3445,13 +3439,13 @@
         <v>45153</v>
       </c>
       <c r="G31">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="H31" s="2">
         <v>45245</v>
       </c>
       <c r="I31">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="J31" t="inlineStr">
         <is>
@@ -3548,13 +3542,13 @@
         <v>45155</v>
       </c>
       <c r="G32">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="H32" s="2">
         <v>45247</v>
       </c>
       <c r="I32">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="J32" t="inlineStr">
         <is>
@@ -3651,7 +3645,7 @@
         <v>45255</v>
       </c>
       <c r="I33">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="J33" t="inlineStr">
         <is>
@@ -3739,13 +3733,13 @@
         <v>45176</v>
       </c>
       <c r="G34">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="H34" s="2">
         <v>45267</v>
       </c>
       <c r="I34">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="J34" t="inlineStr">
         <is>
@@ -3842,13 +3836,13 @@
         <v>45130</v>
       </c>
       <c r="G35">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="H35" s="2">
         <v>45222</v>
       </c>
       <c r="I35">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="J35" t="inlineStr">
         <is>
@@ -3940,13 +3934,13 @@
         <v>45115</v>
       </c>
       <c r="G36">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="H36" s="2">
         <v>45207</v>
       </c>
       <c r="I36">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="J36" t="inlineStr">
         <is>
@@ -4040,16 +4034,16 @@
         </is>
       </c>
       <c r="F37" s="2">
-        <v>45097</v>
+        <v>45189</v>
       </c>
       <c r="G37">
-        <v>106</v>
+        <v>15</v>
       </c>
       <c r="H37" s="2">
-        <v>45189</v>
+        <v>45280</v>
       </c>
       <c r="I37">
-        <v>-14</v>
+        <v>76</v>
       </c>
       <c r="J37" t="inlineStr">
         <is>
@@ -4141,13 +4135,13 @@
         <v>45107</v>
       </c>
       <c r="G38">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="H38" s="2">
         <v>45290</v>
       </c>
       <c r="I38">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="J38" t="inlineStr">
         <is>
@@ -4244,13 +4238,13 @@
         <v>45063</v>
       </c>
       <c r="G39">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="H39" s="2">
         <v>45247</v>
       </c>
       <c r="I39">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="J39" t="inlineStr">
         <is>
@@ -4347,13 +4341,13 @@
         <v>45177</v>
       </c>
       <c r="G40">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="H40" s="2">
         <v>45359</v>
       </c>
       <c r="I40">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="J40" t="inlineStr">
         <is>
@@ -4450,13 +4444,13 @@
         <v>45107</v>
       </c>
       <c r="G41">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="H41" s="2">
         <v>45290</v>
       </c>
       <c r="I41">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="J41" t="inlineStr">
         <is>
@@ -4553,7 +4547,7 @@
         <v>45265</v>
       </c>
       <c r="I42">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="J42" t="inlineStr">
         <is>
@@ -4650,13 +4644,13 @@
         <v>45098</v>
       </c>
       <c r="G43">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="H43" s="2">
         <v>45281</v>
       </c>
       <c r="I43">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="J43" t="inlineStr">
         <is>
@@ -4753,13 +4747,13 @@
         <v>45099</v>
       </c>
       <c r="G44">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="H44" s="2">
         <v>45282</v>
       </c>
       <c r="I44">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="J44" t="inlineStr">
         <is>
@@ -4856,13 +4850,13 @@
         <v>45106</v>
       </c>
       <c r="G45">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="H45" s="2">
         <v>45289</v>
       </c>
       <c r="I45">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="J45" t="inlineStr">
         <is>
@@ -4959,13 +4953,13 @@
         <v>45106</v>
       </c>
       <c r="G46">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="H46" s="2">
         <v>45289</v>
       </c>
       <c r="I46">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="J46" t="inlineStr">
         <is>
@@ -5062,13 +5056,13 @@
         <v>45120</v>
       </c>
       <c r="G47">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="H47" s="2">
         <v>45304</v>
       </c>
       <c r="I47">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="J47" t="inlineStr">
         <is>
@@ -5165,13 +5159,13 @@
         <v>45118</v>
       </c>
       <c r="G48">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="H48" s="2">
         <v>45302</v>
       </c>
       <c r="I48">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="J48" t="inlineStr">
         <is>
@@ -5268,13 +5262,13 @@
         <v>45152</v>
       </c>
       <c r="G49">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="H49" s="2">
         <v>45336</v>
       </c>
       <c r="I49">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="J49" t="inlineStr">
         <is>
@@ -5371,13 +5365,13 @@
         <v>45042</v>
       </c>
       <c r="G50">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="H50" s="2">
         <v>45225</v>
       </c>
       <c r="I50">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="J50" t="inlineStr">
         <is>
@@ -5474,13 +5468,13 @@
         <v>45122</v>
       </c>
       <c r="G51">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="H51" s="2">
         <v>45306</v>
       </c>
       <c r="I51">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="J51" t="inlineStr">
         <is>
@@ -5577,13 +5571,13 @@
         <v>45139</v>
       </c>
       <c r="G52">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="H52" s="2">
         <v>45323</v>
       </c>
       <c r="I52">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="J52" t="inlineStr">
         <is>
@@ -5671,13 +5665,13 @@
         <v>45099</v>
       </c>
       <c r="G53">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="H53" s="2">
         <v>45282</v>
       </c>
       <c r="I53">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="J53" t="inlineStr">
         <is>
@@ -5770,11 +5764,17 @@
           <t>1 000,00</t>
         </is>
       </c>
+      <c r="F54" s="2">
+        <v>45196</v>
+      </c>
+      <c r="G54">
+        <v>8</v>
+      </c>
       <c r="H54" s="2">
-        <v>45196</v>
+        <v>45287</v>
       </c>
       <c r="I54">
-        <v>-7</v>
+        <v>83</v>
       </c>
       <c r="J54" t="inlineStr">
         <is>
@@ -5871,13 +5871,13 @@
         <v>45044</v>
       </c>
       <c r="G55">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="H55" s="2">
         <v>45227</v>
       </c>
       <c r="I55">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="J55" t="inlineStr">
         <is>
@@ -5974,13 +5974,13 @@
         <v>45151</v>
       </c>
       <c r="G56">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="H56" s="2">
         <v>45243</v>
       </c>
       <c r="I56">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="J56" t="inlineStr">
         <is>
@@ -6068,11 +6068,17 @@
           <t>1 000,00</t>
         </is>
       </c>
+      <c r="F57" s="2">
+        <v>45196</v>
+      </c>
+      <c r="G57">
+        <v>8</v>
+      </c>
       <c r="H57" s="2">
-        <v>45196</v>
+        <v>45287</v>
       </c>
       <c r="I57">
-        <v>-7</v>
+        <v>83</v>
       </c>
       <c r="J57" t="inlineStr">
         <is>
@@ -6169,13 +6175,13 @@
         <v>45069</v>
       </c>
       <c r="G58">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="H58" s="2">
         <v>45253</v>
       </c>
       <c r="I58">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="J58" t="inlineStr">
         <is>
@@ -6269,16 +6275,16 @@
         </is>
       </c>
       <c r="F59" s="2">
-        <v>45099</v>
+        <v>45191</v>
       </c>
       <c r="G59">
-        <v>104</v>
+        <v>13</v>
       </c>
       <c r="H59" s="2">
-        <v>45191</v>
+        <v>45282</v>
       </c>
       <c r="I59">
-        <v>-12</v>
+        <v>78</v>
       </c>
       <c r="J59" t="inlineStr">
         <is>
@@ -6370,13 +6376,13 @@
         <v>45113</v>
       </c>
       <c r="G60">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="H60" s="2">
         <v>45205</v>
       </c>
       <c r="I60">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J60" t="inlineStr">
         <is>
@@ -6473,13 +6479,13 @@
         <v>45127</v>
       </c>
       <c r="G61">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="H61" s="2">
         <v>45219</v>
       </c>
       <c r="I61">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="J61" t="inlineStr">
         <is>
@@ -6576,13 +6582,13 @@
         <v>45058</v>
       </c>
       <c r="G62">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="H62" s="2">
         <v>45242</v>
       </c>
       <c r="I62">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="J62" t="inlineStr">
         <is>
@@ -6676,16 +6682,16 @@
         </is>
       </c>
       <c r="F63" s="2">
-        <v>45010</v>
+        <v>45194</v>
       </c>
       <c r="G63">
-        <v>193</v>
+        <v>10</v>
       </c>
       <c r="H63" s="2">
-        <v>45194</v>
+        <v>45376</v>
       </c>
       <c r="I63">
-        <v>-9</v>
+        <v>172</v>
       </c>
       <c r="J63" t="inlineStr">
         <is>
@@ -6777,13 +6783,13 @@
         <v>45025</v>
       </c>
       <c r="G64">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="H64" s="2">
         <v>45208</v>
       </c>
       <c r="I64">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="J64" t="inlineStr">
         <is>
@@ -6880,13 +6886,13 @@
         <v>45025</v>
       </c>
       <c r="G65">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="H65" s="2">
         <v>45208</v>
       </c>
       <c r="I65">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="J65" t="inlineStr">
         <is>
@@ -6983,13 +6989,13 @@
         <v>45089</v>
       </c>
       <c r="G66">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="H66" s="2">
         <v>45272</v>
       </c>
       <c r="I66">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="J66" t="inlineStr">
         <is>
@@ -7086,13 +7092,13 @@
         <v>45178</v>
       </c>
       <c r="G67">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="H67" s="2">
         <v>45269</v>
       </c>
       <c r="I67">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="J67" t="inlineStr">
         <is>
@@ -7181,16 +7187,16 @@
         </is>
       </c>
       <c r="F68" s="2">
-        <v>45104</v>
+        <v>45196</v>
       </c>
       <c r="G68">
-        <v>99</v>
+        <v>8</v>
       </c>
       <c r="H68" s="2">
-        <v>45196</v>
+        <v>45287</v>
       </c>
       <c r="I68">
-        <v>-7</v>
+        <v>83</v>
       </c>
       <c r="J68" t="inlineStr">
         <is>
@@ -7287,13 +7293,13 @@
         <v>45149</v>
       </c>
       <c r="G69">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="H69" s="2">
         <v>45241</v>
       </c>
       <c r="I69">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="J69" t="inlineStr">
         <is>
@@ -7390,7 +7396,7 @@
         <v>45205</v>
       </c>
       <c r="I70">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J70" t="inlineStr">
         <is>
@@ -7487,13 +7493,13 @@
         <v>45114</v>
       </c>
       <c r="G71">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="H71" s="2">
         <v>45205</v>
       </c>
       <c r="I71">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J71" t="inlineStr">
         <is>
@@ -7590,13 +7596,13 @@
         <v>45115</v>
       </c>
       <c r="G72">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="H72" s="2">
         <v>45207</v>
       </c>
       <c r="I72">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="J72" t="inlineStr">
         <is>
@@ -7690,16 +7696,16 @@
         </is>
       </c>
       <c r="F73" s="2">
-        <v>45097</v>
+        <v>45189</v>
       </c>
       <c r="G73">
-        <v>106</v>
+        <v>15</v>
       </c>
       <c r="H73" s="2">
-        <v>45189</v>
+        <v>45280</v>
       </c>
       <c r="I73">
-        <v>-14</v>
+        <v>76</v>
       </c>
       <c r="J73" t="inlineStr">
         <is>
@@ -7791,13 +7797,13 @@
         <v>45038</v>
       </c>
       <c r="G74">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="H74" s="2">
         <v>45221</v>
       </c>
       <c r="I74">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="J74" t="inlineStr">
         <is>
@@ -7889,13 +7895,13 @@
         <v>45117</v>
       </c>
       <c r="G75">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="H75" s="2">
         <v>45301</v>
       </c>
       <c r="I75">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="J75" t="inlineStr">
         <is>
@@ -7992,13 +7998,13 @@
         <v>45160</v>
       </c>
       <c r="G76">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="H76" s="2">
         <v>45344</v>
       </c>
       <c r="I76">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="J76" t="inlineStr">
         <is>
@@ -8092,16 +8098,16 @@
         </is>
       </c>
       <c r="F77" s="2">
-        <v>45002</v>
+        <v>45186</v>
       </c>
       <c r="G77">
-        <v>201</v>
+        <v>18</v>
       </c>
       <c r="H77" s="2">
-        <v>45186</v>
+        <v>45368</v>
       </c>
       <c r="I77">
-        <v>-17</v>
+        <v>164</v>
       </c>
       <c r="J77" t="inlineStr">
         <is>
@@ -8198,13 +8204,13 @@
         <v>45043</v>
       </c>
       <c r="G78">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="H78" s="2">
         <v>45226</v>
       </c>
       <c r="I78">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="J78" t="inlineStr">
         <is>
@@ -8301,13 +8307,13 @@
         <v>45079</v>
       </c>
       <c r="G79">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="H79" s="2">
         <v>45262</v>
       </c>
       <c r="I79">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="J79" t="inlineStr">
         <is>
@@ -8404,7 +8410,7 @@
         <v>45254</v>
       </c>
       <c r="I80">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="J80" t="inlineStr">
         <is>
@@ -8501,13 +8507,13 @@
         <v>45104</v>
       </c>
       <c r="G81">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="H81" s="2">
         <v>45287</v>
       </c>
       <c r="I81">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="J81" t="inlineStr">
         <is>
@@ -8604,7 +8610,7 @@
         <v>45288</v>
       </c>
       <c r="I82">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="J82" t="inlineStr">
         <is>
@@ -8696,13 +8702,13 @@
         <v>45175</v>
       </c>
       <c r="G83">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="H83" s="2">
         <v>45357</v>
       </c>
       <c r="I83">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="J83" t="inlineStr">
         <is>
@@ -8799,13 +8805,13 @@
         <v>45054</v>
       </c>
       <c r="G84">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="H84" s="2">
         <v>45238</v>
       </c>
       <c r="I84">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="J84" t="inlineStr">
         <is>
@@ -8902,13 +8908,13 @@
         <v>45056</v>
       </c>
       <c r="G85">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="H85" s="2">
         <v>45240</v>
       </c>
       <c r="I85">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="J85" t="inlineStr">
         <is>
@@ -9005,13 +9011,13 @@
         <v>45085</v>
       </c>
       <c r="G86">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="H86" s="2">
         <v>45268</v>
       </c>
       <c r="I86">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="J86" t="inlineStr">
         <is>
@@ -9104,11 +9110,17 @@
           <t>1 000,00</t>
         </is>
       </c>
+      <c r="F87" s="2">
+        <v>45194</v>
+      </c>
+      <c r="G87">
+        <v>10</v>
+      </c>
       <c r="H87" s="2">
-        <v>45194</v>
+        <v>45560</v>
       </c>
       <c r="I87">
-        <v>-9</v>
+        <v>356</v>
       </c>
       <c r="J87" t="inlineStr">
         <is>
@@ -9195,13 +9207,13 @@
         <v>45103</v>
       </c>
       <c r="G88">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="H88" s="2">
         <v>45286</v>
       </c>
       <c r="I88">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="J88" t="inlineStr">
         <is>
@@ -9298,13 +9310,13 @@
         <v>45103</v>
       </c>
       <c r="G89">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="H89" s="2">
         <v>45286</v>
       </c>
       <c r="I89">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="J89" t="inlineStr">
         <is>
@@ -9398,16 +9410,16 @@
         </is>
       </c>
       <c r="F90" s="2">
-        <v>45008</v>
+        <v>45192</v>
       </c>
       <c r="G90">
-        <v>195</v>
+        <v>12</v>
       </c>
       <c r="H90" s="2">
-        <v>45192</v>
+        <v>45374</v>
       </c>
       <c r="I90">
-        <v>-11</v>
+        <v>170</v>
       </c>
       <c r="J90" t="inlineStr">
         <is>
@@ -9499,13 +9511,13 @@
         <v>45100</v>
       </c>
       <c r="G91">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="H91" s="2">
         <v>45287</v>
       </c>
       <c r="I91">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="J91" t="inlineStr">
         <is>
@@ -9599,16 +9611,16 @@
         </is>
       </c>
       <c r="F92" s="2">
-        <v>45003</v>
+        <v>45187</v>
       </c>
       <c r="G92">
-        <v>200</v>
+        <v>17</v>
       </c>
       <c r="H92" s="2">
-        <v>45187</v>
+        <v>45369</v>
       </c>
       <c r="I92">
-        <v>-16</v>
+        <v>165</v>
       </c>
       <c r="J92" t="inlineStr">
         <is>
@@ -9705,13 +9717,13 @@
         <v>45104</v>
       </c>
       <c r="G93">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="H93" s="2">
         <v>45287</v>
       </c>
       <c r="I93">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="J93" t="inlineStr">
         <is>
@@ -9808,13 +9820,13 @@
         <v>45104</v>
       </c>
       <c r="G94">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="H94" s="2">
         <v>45287</v>
       </c>
       <c r="I94">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="J94" t="inlineStr">
         <is>
@@ -9911,13 +9923,13 @@
         <v>45049</v>
       </c>
       <c r="G95">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="H95" s="2">
         <v>45233</v>
       </c>
       <c r="I95">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="J95" t="inlineStr">
         <is>
@@ -10014,13 +10026,13 @@
         <v>45122</v>
       </c>
       <c r="G96">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="H96" s="2">
         <v>45306</v>
       </c>
       <c r="I96">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="J96" t="inlineStr">
         <is>
@@ -10112,13 +10124,13 @@
         <v>45141</v>
       </c>
       <c r="G97">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="H97" s="2">
         <v>45325</v>
       </c>
       <c r="I97">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="J97" t="inlineStr">
         <is>
@@ -10212,16 +10224,16 @@
         </is>
       </c>
       <c r="F98" s="2">
-        <v>45010</v>
+        <v>45194</v>
       </c>
       <c r="G98">
-        <v>193</v>
+        <v>10</v>
       </c>
       <c r="H98" s="2">
-        <v>45194</v>
+        <v>45376</v>
       </c>
       <c r="I98">
-        <v>-9</v>
+        <v>172</v>
       </c>
       <c r="J98" t="inlineStr">
         <is>
@@ -10313,13 +10325,13 @@
         <v>45093</v>
       </c>
       <c r="G99">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="H99" s="2">
         <v>45276</v>
       </c>
       <c r="I99">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="J99" t="inlineStr">
         <is>
@@ -10416,13 +10428,13 @@
         <v>45123</v>
       </c>
       <c r="G100">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="H100" s="2">
         <v>45307</v>
       </c>
       <c r="I100">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="J100" t="inlineStr">
         <is>
@@ -10516,16 +10528,16 @@
         </is>
       </c>
       <c r="F101" s="2">
-        <v>45014</v>
+        <v>45198</v>
       </c>
       <c r="G101">
-        <v>189</v>
+        <v>6</v>
       </c>
       <c r="H101" s="2">
-        <v>45198</v>
+        <v>45380</v>
       </c>
       <c r="I101">
-        <v>-5</v>
+        <v>176</v>
       </c>
       <c r="J101" t="inlineStr">
         <is>
@@ -10622,13 +10634,13 @@
         <v>45093</v>
       </c>
       <c r="G102">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="H102" s="2">
         <v>45276</v>
       </c>
       <c r="I102">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="J102" t="inlineStr">
         <is>
@@ -10725,13 +10737,13 @@
         <v>45122</v>
       </c>
       <c r="G103">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="H103" s="2">
         <v>45306</v>
       </c>
       <c r="I103">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="J103" t="inlineStr">
         <is>
@@ -10828,13 +10840,13 @@
         <v>45122</v>
       </c>
       <c r="G104">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="H104" s="2">
         <v>45306</v>
       </c>
       <c r="I104">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="J104" t="inlineStr">
         <is>
@@ -10926,13 +10938,13 @@
         <v>45050</v>
       </c>
       <c r="G105">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="H105" s="2">
         <v>45234</v>
       </c>
       <c r="I105">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="J105" t="inlineStr">
         <is>
@@ -11029,13 +11041,13 @@
         <v>45085</v>
       </c>
       <c r="G106">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="H106" s="2">
         <v>45268</v>
       </c>
       <c r="I106">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="J106" t="inlineStr">
         <is>
@@ -11129,16 +11141,16 @@
         </is>
       </c>
       <c r="F107" s="2">
-        <v>45093</v>
+        <v>45185</v>
       </c>
       <c r="G107">
-        <v>110</v>
+        <v>19</v>
       </c>
       <c r="H107" s="2">
-        <v>45185</v>
+        <v>45276</v>
       </c>
       <c r="I107">
-        <v>-18</v>
+        <v>72</v>
       </c>
       <c r="J107" t="inlineStr">
         <is>
@@ -11227,16 +11239,16 @@
         </is>
       </c>
       <c r="F108" s="2">
-        <v>45093</v>
+        <v>45185</v>
       </c>
       <c r="G108">
-        <v>110</v>
+        <v>19</v>
       </c>
       <c r="H108" s="2">
-        <v>45185</v>
+        <v>45276</v>
       </c>
       <c r="I108">
-        <v>-18</v>
+        <v>72</v>
       </c>
       <c r="J108" t="inlineStr">
         <is>
@@ -11325,16 +11337,16 @@
         </is>
       </c>
       <c r="F109" s="2">
-        <v>45093</v>
+        <v>45185</v>
       </c>
       <c r="G109">
-        <v>110</v>
+        <v>19</v>
       </c>
       <c r="H109" s="2">
-        <v>45185</v>
+        <v>45276</v>
       </c>
       <c r="I109">
-        <v>-18</v>
+        <v>72</v>
       </c>
       <c r="J109" t="inlineStr">
         <is>
@@ -11431,13 +11443,13 @@
         <v>45148</v>
       </c>
       <c r="G110">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="H110" s="2">
         <v>45240</v>
       </c>
       <c r="I110">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="J110" t="inlineStr">
         <is>
@@ -11534,13 +11546,13 @@
         <v>45119</v>
       </c>
       <c r="G111">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="H111" s="2">
         <v>45211</v>
       </c>
       <c r="I111">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="J111" t="inlineStr">
         <is>
@@ -11637,13 +11649,13 @@
         <v>45172</v>
       </c>
       <c r="G112">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="H112" s="2">
         <v>45263</v>
       </c>
       <c r="I112">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="J112" t="inlineStr">
         <is>
@@ -11740,13 +11752,13 @@
         <v>45023</v>
       </c>
       <c r="G113">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="H113" s="2">
         <v>45206</v>
       </c>
       <c r="I113">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="J113" t="inlineStr">
         <is>
@@ -11840,16 +11852,16 @@
         </is>
       </c>
       <c r="F114" s="2">
-        <v>45111</v>
+        <v>45203</v>
       </c>
       <c r="G114">
-        <v>92</v>
+        <v>1</v>
       </c>
       <c r="H114" s="2">
-        <v>45203</v>
+        <v>45295</v>
       </c>
       <c r="I114">
-        <v>0</v>
+        <v>91</v>
       </c>
       <c r="J114" t="inlineStr">
         <is>
@@ -11946,7 +11958,7 @@
         <v>45218</v>
       </c>
       <c r="I115">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="J115" t="inlineStr">
         <is>
@@ -12043,13 +12055,13 @@
         <v>45161</v>
       </c>
       <c r="G116">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="H116" s="2">
         <v>45253</v>
       </c>
       <c r="I116">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="J116" t="inlineStr">
         <is>
@@ -12146,13 +12158,13 @@
         <v>45115</v>
       </c>
       <c r="G117">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="H117" s="2">
         <v>45299</v>
       </c>
       <c r="I117">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="J117" t="inlineStr">
         <is>
@@ -12244,13 +12256,13 @@
         <v>45094</v>
       </c>
       <c r="G118">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="H118" s="2">
         <v>45277</v>
       </c>
       <c r="I118">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="J118" t="inlineStr">
         <is>
@@ -12347,13 +12359,13 @@
         <v>45104</v>
       </c>
       <c r="G119">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="H119" s="2">
         <v>45287</v>
       </c>
       <c r="I119">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="J119" t="inlineStr">
         <is>
@@ -12450,13 +12462,13 @@
         <v>45104</v>
       </c>
       <c r="G120">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="H120" s="2">
         <v>45287</v>
       </c>
       <c r="I120">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="J120" t="inlineStr">
         <is>
@@ -12553,13 +12565,13 @@
         <v>45104</v>
       </c>
       <c r="G121">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="H121" s="2">
         <v>45287</v>
       </c>
       <c r="I121">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="J121" t="inlineStr">
         <is>
@@ -12656,13 +12668,13 @@
         <v>45104</v>
       </c>
       <c r="G122">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="H122" s="2">
         <v>45287</v>
       </c>
       <c r="I122">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="J122" t="inlineStr">
         <is>
@@ -12756,16 +12768,16 @@
         </is>
       </c>
       <c r="F123" s="2">
-        <v>45107</v>
+        <v>45199</v>
       </c>
       <c r="G123">
-        <v>96</v>
+        <v>5</v>
       </c>
       <c r="H123" s="2">
-        <v>45199</v>
+        <v>45291</v>
       </c>
       <c r="I123">
-        <v>-4</v>
+        <v>87</v>
       </c>
       <c r="J123" t="inlineStr">
         <is>
@@ -12859,16 +12871,16 @@
         </is>
       </c>
       <c r="F124" s="2">
-        <v>45013</v>
+        <v>45197</v>
       </c>
       <c r="G124">
-        <v>190</v>
+        <v>7</v>
       </c>
       <c r="H124" s="2">
-        <v>45197</v>
+        <v>45379</v>
       </c>
       <c r="I124">
-        <v>-6</v>
+        <v>175</v>
       </c>
       <c r="J124" t="inlineStr">
         <is>
@@ -12965,13 +12977,13 @@
         <v>45121</v>
       </c>
       <c r="G125">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="H125" s="2">
         <v>45213</v>
       </c>
       <c r="I125">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="J125" t="inlineStr">
         <is>
@@ -13068,13 +13080,13 @@
         <v>45134</v>
       </c>
       <c r="G126">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="H126" s="2">
         <v>45226</v>
       </c>
       <c r="I126">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="J126" t="inlineStr">
         <is>
@@ -13171,7 +13183,7 @@
         <v>45212</v>
       </c>
       <c r="I127">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="J127" t="inlineStr">
         <is>
@@ -13268,13 +13280,13 @@
         <v>45126</v>
       </c>
       <c r="G128">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="H128" s="2">
         <v>45218</v>
       </c>
       <c r="I128">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="J128" t="inlineStr">
         <is>
@@ -13366,13 +13378,13 @@
         <v>45158</v>
       </c>
       <c r="G129">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="H129" s="2">
         <v>45250</v>
       </c>
       <c r="I129">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="J129" t="inlineStr">
         <is>
@@ -13469,13 +13481,13 @@
         <v>45171</v>
       </c>
       <c r="G130">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="H130" s="2">
         <v>45262</v>
       </c>
       <c r="I130">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="J130" t="inlineStr">
         <is>
@@ -13569,16 +13581,16 @@
         </is>
       </c>
       <c r="F131" s="2">
-        <v>45111</v>
+        <v>45203</v>
       </c>
       <c r="G131">
-        <v>92</v>
+        <v>1</v>
       </c>
       <c r="H131" s="2">
-        <v>45203</v>
+        <v>45295</v>
       </c>
       <c r="I131">
-        <v>0</v>
+        <v>91</v>
       </c>
       <c r="J131" t="inlineStr">
         <is>
@@ -13675,13 +13687,13 @@
         <v>45144</v>
       </c>
       <c r="G132">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="H132" s="2">
         <v>45236</v>
       </c>
       <c r="I132">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="J132" t="inlineStr">
         <is>
@@ -13778,13 +13790,13 @@
         <v>45156</v>
       </c>
       <c r="G133">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="H133" s="2">
         <v>45248</v>
       </c>
       <c r="I133">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="J133" t="inlineStr">
         <is>
@@ -13876,13 +13888,13 @@
         <v>45146</v>
       </c>
       <c r="G134">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="H134" s="2">
         <v>45238</v>
       </c>
       <c r="I134">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="J134" t="inlineStr">
         <is>
@@ -13979,13 +13991,13 @@
         <v>45140</v>
       </c>
       <c r="G135">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="H135" s="2">
         <v>45232</v>
       </c>
       <c r="I135">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="J135" t="inlineStr">
         <is>
@@ -14079,16 +14091,16 @@
         </is>
       </c>
       <c r="F136" s="2">
-        <v>45104</v>
+        <v>45196</v>
       </c>
       <c r="G136">
-        <v>99</v>
+        <v>8</v>
       </c>
       <c r="H136" s="2">
-        <v>45196</v>
+        <v>45287</v>
       </c>
       <c r="I136">
-        <v>-7</v>
+        <v>83</v>
       </c>
       <c r="J136" t="inlineStr">
         <is>
@@ -14182,16 +14194,16 @@
         </is>
       </c>
       <c r="F137" s="2">
-        <v>45105</v>
+        <v>45197</v>
       </c>
       <c r="G137">
-        <v>98</v>
+        <v>7</v>
       </c>
       <c r="H137" s="2">
-        <v>45197</v>
+        <v>45288</v>
       </c>
       <c r="I137">
-        <v>-6</v>
+        <v>84</v>
       </c>
       <c r="J137" t="inlineStr">
         <is>
@@ -14288,13 +14300,13 @@
         <v>45179</v>
       </c>
       <c r="G138">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="H138" s="2">
         <v>45270</v>
       </c>
       <c r="I138">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="J138" t="inlineStr">
         <is>
@@ -14383,16 +14395,16 @@
         </is>
       </c>
       <c r="F139" s="2">
-        <v>45105</v>
+        <v>45197</v>
       </c>
       <c r="G139">
-        <v>98</v>
+        <v>7</v>
       </c>
       <c r="H139" s="2">
-        <v>45197</v>
+        <v>45288</v>
       </c>
       <c r="I139">
-        <v>-6</v>
+        <v>84</v>
       </c>
       <c r="J139" t="inlineStr">
         <is>
@@ -14489,13 +14501,13 @@
         <v>45182</v>
       </c>
       <c r="G140">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="H140" s="2">
         <v>45273</v>
       </c>
       <c r="I140">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="J140" t="inlineStr">
         <is>
@@ -14592,13 +14604,13 @@
         <v>45116</v>
       </c>
       <c r="G141">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="H141" s="2">
         <v>45208</v>
       </c>
       <c r="I141">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="J141" t="inlineStr">
         <is>
@@ -14690,13 +14702,13 @@
         <v>45150</v>
       </c>
       <c r="G142">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="H142" s="2">
         <v>45242</v>
       </c>
       <c r="I142">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="J142" t="inlineStr">
         <is>
@@ -14793,7 +14805,7 @@
         <v>45238</v>
       </c>
       <c r="I143">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="J143" t="inlineStr">
         <is>
@@ -14890,13 +14902,13 @@
         <v>45171</v>
       </c>
       <c r="G144">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="H144" s="2">
         <v>45262</v>
       </c>
       <c r="I144">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="J144" t="inlineStr">
         <is>
@@ -14990,16 +15002,16 @@
         </is>
       </c>
       <c r="F145" s="2">
-        <v>45102</v>
+        <v>45194</v>
       </c>
       <c r="G145">
-        <v>101</v>
+        <v>10</v>
       </c>
       <c r="H145" s="2">
-        <v>45194</v>
+        <v>45285</v>
       </c>
       <c r="I145">
-        <v>-9</v>
+        <v>81</v>
       </c>
       <c r="J145" t="inlineStr">
         <is>
@@ -15086,13 +15098,13 @@
         <v>45119</v>
       </c>
       <c r="G146">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="H146" s="2">
         <v>45211</v>
       </c>
       <c r="I146">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="J146" t="inlineStr">
         <is>
@@ -15189,13 +15201,13 @@
         <v>45165</v>
       </c>
       <c r="G147">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="H147" s="2">
         <v>45257</v>
       </c>
       <c r="I147">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="J147" t="inlineStr">
         <is>
@@ -15292,13 +15304,13 @@
         <v>45166</v>
       </c>
       <c r="G148">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="H148" s="2">
         <v>45258</v>
       </c>
       <c r="I148">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="J148" t="inlineStr">
         <is>
@@ -15392,16 +15404,16 @@
         </is>
       </c>
       <c r="F149" s="2">
-        <v>45093</v>
+        <v>45185</v>
       </c>
       <c r="G149">
-        <v>110</v>
+        <v>19</v>
       </c>
       <c r="H149" s="2">
-        <v>45185</v>
+        <v>45276</v>
       </c>
       <c r="I149">
-        <v>-18</v>
+        <v>72</v>
       </c>
       <c r="J149" t="inlineStr">
         <is>
@@ -15498,13 +15510,13 @@
         <v>45035</v>
       </c>
       <c r="G150">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="H150" s="2">
         <v>45218</v>
       </c>
       <c r="I150">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="J150" t="inlineStr">
         <is>
@@ -15601,13 +15613,13 @@
         <v>45174</v>
       </c>
       <c r="G151">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="H151" s="2">
         <v>45356</v>
       </c>
       <c r="I151">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="J151" t="inlineStr">
         <is>
@@ -15704,13 +15716,13 @@
         <v>45089</v>
       </c>
       <c r="G152">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="H152" s="2">
         <v>45272</v>
       </c>
       <c r="I152">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="J152" t="inlineStr">
         <is>
@@ -15807,13 +15819,13 @@
         <v>45124</v>
       </c>
       <c r="G153">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="H153" s="2">
         <v>45308</v>
       </c>
       <c r="I153">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="J153" t="inlineStr">
         <is>
@@ -15910,13 +15922,13 @@
         <v>45124</v>
       </c>
       <c r="G154">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="H154" s="2">
         <v>45308</v>
       </c>
       <c r="I154">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="J154" t="inlineStr">
         <is>
@@ -16013,13 +16025,13 @@
         <v>45026</v>
       </c>
       <c r="G155">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="H155" s="2">
         <v>45209</v>
       </c>
       <c r="I155">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="J155" t="inlineStr">
         <is>
@@ -16116,13 +16128,13 @@
         <v>45026</v>
       </c>
       <c r="G156">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="H156" s="2">
         <v>45209</v>
       </c>
       <c r="I156">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="J156" t="inlineStr">
         <is>
@@ -16219,13 +16231,13 @@
         <v>45026</v>
       </c>
       <c r="G157">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="H157" s="2">
         <v>45209</v>
       </c>
       <c r="I157">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="J157" t="inlineStr">
         <is>
@@ -16322,13 +16334,13 @@
         <v>45026</v>
       </c>
       <c r="G158">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="H158" s="2">
         <v>45209</v>
       </c>
       <c r="I158">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="J158" t="inlineStr">
         <is>
@@ -16425,13 +16437,13 @@
         <v>45156</v>
       </c>
       <c r="G159">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="H159" s="2">
         <v>45247</v>
       </c>
       <c r="I159">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="J159" t="inlineStr">
         <is>
@@ -16528,13 +16540,13 @@
         <v>45153</v>
       </c>
       <c r="G160">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="H160" s="2">
         <v>45245</v>
       </c>
       <c r="I160">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="J160" t="inlineStr">
         <is>
@@ -16631,13 +16643,13 @@
         <v>45135</v>
       </c>
       <c r="G161">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="H161" s="2">
         <v>45319</v>
       </c>
       <c r="I161">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="J161" t="inlineStr">
         <is>
@@ -16734,13 +16746,13 @@
         <v>45091</v>
       </c>
       <c r="G162">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="H162" s="2">
         <v>45274</v>
       </c>
       <c r="I162">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="J162" t="inlineStr">
         <is>
@@ -16832,13 +16844,13 @@
         <v>45091</v>
       </c>
       <c r="G163">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="H163" s="2">
         <v>45274</v>
       </c>
       <c r="I163">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="J163" t="inlineStr">
         <is>
@@ -16930,13 +16942,13 @@
         <v>45138</v>
       </c>
       <c r="G164">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="H164" s="2">
         <v>45322</v>
       </c>
       <c r="I164">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="J164" t="inlineStr">
         <is>
@@ -17033,13 +17045,13 @@
         <v>45138</v>
       </c>
       <c r="G165">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="H165" s="2">
         <v>45322</v>
       </c>
       <c r="I165">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="J165" t="inlineStr">
         <is>
@@ -17136,13 +17148,13 @@
         <v>45085</v>
       </c>
       <c r="G166">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="H166" s="2">
         <v>45268</v>
       </c>
       <c r="I166">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="J166" t="inlineStr">
         <is>
@@ -17239,13 +17251,13 @@
         <v>45085</v>
       </c>
       <c r="G167">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="H167" s="2">
         <v>45268</v>
       </c>
       <c r="I167">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="J167" t="inlineStr">
         <is>
@@ -17342,7 +17354,7 @@
         <v>45326</v>
       </c>
       <c r="I168">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="J168" t="inlineStr">
         <is>
@@ -17439,13 +17451,13 @@
         <v>45173</v>
       </c>
       <c r="G169">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="H169" s="2">
         <v>45355</v>
       </c>
       <c r="I169">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="J169" t="inlineStr">
         <is>
@@ -17542,13 +17554,13 @@
         <v>45056</v>
       </c>
       <c r="G170">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="H170" s="2">
         <v>45240</v>
       </c>
       <c r="I170">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="J170" t="inlineStr">
         <is>
@@ -17645,7 +17657,7 @@
         <v>45238</v>
       </c>
       <c r="I171">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="J171" t="inlineStr">
         <is>
@@ -17742,13 +17754,13 @@
         <v>45141</v>
       </c>
       <c r="G172">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="H172" s="2">
         <v>45325</v>
       </c>
       <c r="I172">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="J172" t="inlineStr">
         <is>
@@ -17845,13 +17857,13 @@
         <v>45037</v>
       </c>
       <c r="G173">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="H173" s="2">
         <v>45220</v>
       </c>
       <c r="I173">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="J173" t="inlineStr">
         <is>
@@ -17948,13 +17960,13 @@
         <v>45171</v>
       </c>
       <c r="G174">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="H174" s="2">
         <v>45262</v>
       </c>
       <c r="I174">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="J174" t="inlineStr">
         <is>
@@ -18048,16 +18060,16 @@
         </is>
       </c>
       <c r="F175" s="2">
-        <v>45105</v>
+        <v>45197</v>
       </c>
       <c r="G175">
-        <v>98</v>
+        <v>7</v>
       </c>
       <c r="H175" s="2">
-        <v>45197</v>
+        <v>45288</v>
       </c>
       <c r="I175">
-        <v>-6</v>
+        <v>84</v>
       </c>
       <c r="J175" t="inlineStr">
         <is>
@@ -18154,13 +18166,13 @@
         <v>45162</v>
       </c>
       <c r="G176">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="H176" s="2">
         <v>45254</v>
       </c>
       <c r="I176">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="J176" t="inlineStr">
         <is>
@@ -18257,13 +18269,13 @@
         <v>45061</v>
       </c>
       <c r="G177">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="H177" s="2">
         <v>45245</v>
       </c>
       <c r="I177">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="J177" t="inlineStr">
         <is>
@@ -18360,13 +18372,13 @@
         <v>45120</v>
       </c>
       <c r="G178">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="H178" s="2">
         <v>45212</v>
       </c>
       <c r="I178">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="J178" t="inlineStr">
         <is>
@@ -18459,11 +18471,17 @@
           <t>1 000,00</t>
         </is>
       </c>
+      <c r="F179" s="2">
+        <v>45191</v>
+      </c>
+      <c r="G179">
+        <v>13</v>
+      </c>
       <c r="H179" s="2">
-        <v>45191</v>
+        <v>45282</v>
       </c>
       <c r="I179">
-        <v>-12</v>
+        <v>78</v>
       </c>
       <c r="J179" t="inlineStr">
         <is>
@@ -18560,13 +18578,13 @@
         <v>45088</v>
       </c>
       <c r="G180">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="H180" s="2">
         <v>45271</v>
       </c>
       <c r="I180">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="J180" t="inlineStr">
         <is>
@@ -18660,16 +18678,16 @@
         </is>
       </c>
       <c r="F181" s="2">
-        <v>45100</v>
+        <v>45192</v>
       </c>
       <c r="G181">
-        <v>103</v>
+        <v>12</v>
       </c>
       <c r="H181" s="2">
-        <v>45192</v>
+        <v>45283</v>
       </c>
       <c r="I181">
-        <v>-11</v>
+        <v>79</v>
       </c>
       <c r="J181" t="inlineStr">
         <is>
@@ -18756,13 +18774,13 @@
         <v>45131</v>
       </c>
       <c r="G182">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="H182" s="2">
         <v>45223</v>
       </c>
       <c r="I182">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="J182" t="inlineStr">
         <is>
@@ -18854,13 +18872,13 @@
         <v>45136</v>
       </c>
       <c r="G183">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="H183" s="2">
         <v>45228</v>
       </c>
       <c r="I183">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="J183" t="inlineStr">
         <is>
@@ -18952,13 +18970,13 @@
         <v>45150</v>
       </c>
       <c r="G184">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="H184" s="2">
         <v>45242</v>
       </c>
       <c r="I184">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="J184" t="inlineStr">
         <is>
@@ -19050,13 +19068,13 @@
         <v>45118</v>
       </c>
       <c r="G185">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="H185" s="2">
         <v>45210</v>
       </c>
       <c r="I185">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="J185" t="inlineStr">
         <is>
@@ -19148,13 +19166,13 @@
         <v>45129</v>
       </c>
       <c r="G186">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="H186" s="2">
         <v>45221</v>
       </c>
       <c r="I186">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="J186" t="inlineStr">
         <is>
@@ -19243,16 +19261,16 @@
         </is>
       </c>
       <c r="F187" s="2">
-        <v>45097</v>
+        <v>45189</v>
       </c>
       <c r="G187">
-        <v>106</v>
+        <v>15</v>
       </c>
       <c r="H187" s="2">
-        <v>45189</v>
+        <v>45280</v>
       </c>
       <c r="I187">
-        <v>-14</v>
+        <v>76</v>
       </c>
       <c r="J187" t="inlineStr">
         <is>
@@ -19336,16 +19354,16 @@
         </is>
       </c>
       <c r="F188" s="2">
-        <v>45101</v>
+        <v>45193</v>
       </c>
       <c r="G188">
-        <v>102</v>
+        <v>11</v>
       </c>
       <c r="H188" s="2">
-        <v>45193</v>
+        <v>45284</v>
       </c>
       <c r="I188">
-        <v>-10</v>
+        <v>80</v>
       </c>
       <c r="J188" t="inlineStr">
         <is>
@@ -19432,13 +19450,13 @@
         <v>45165</v>
       </c>
       <c r="G189">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="H189" s="2">
         <v>45257</v>
       </c>
       <c r="I189">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="J189" t="inlineStr">
         <is>
@@ -19526,11 +19544,17 @@
           <t>500 000,00</t>
         </is>
       </c>
+      <c r="F190" s="2">
+        <v>45202</v>
+      </c>
+      <c r="G190">
+        <v>2</v>
+      </c>
       <c r="H190" s="2">
-        <v>45202</v>
+        <v>45385</v>
       </c>
       <c r="I190">
-        <v>-1</v>
+        <v>181</v>
       </c>
       <c r="J190" t="inlineStr">
         <is>
@@ -19627,13 +19651,13 @@
         <v>45081</v>
       </c>
       <c r="G191">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="H191" s="2">
         <v>45264</v>
       </c>
       <c r="I191">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="J191" t="inlineStr">
         <is>
@@ -19730,13 +19754,13 @@
         <v>45081</v>
       </c>
       <c r="G192">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="H192" s="2">
         <v>45264</v>
       </c>
       <c r="I192">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="J192" t="inlineStr">
         <is>
@@ -19833,7 +19857,7 @@
         <v>45319</v>
       </c>
       <c r="I193">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="J193" t="inlineStr">
         <is>
@@ -19930,7 +19954,7 @@
         <v>45319</v>
       </c>
       <c r="I194">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="J194" t="inlineStr">
         <is>
@@ -20022,13 +20046,13 @@
         <v>45046</v>
       </c>
       <c r="G195">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="H195" s="2">
         <v>45230</v>
       </c>
       <c r="I195">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="J195" t="inlineStr">
         <is>
@@ -20125,13 +20149,13 @@
         <v>45046</v>
       </c>
       <c r="G196">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="H196" s="2">
         <v>45230</v>
       </c>
       <c r="I196">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="J196" t="inlineStr">
         <is>
@@ -20228,13 +20252,13 @@
         <v>45031</v>
       </c>
       <c r="G197">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="H197" s="2">
         <v>45214</v>
       </c>
       <c r="I197">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="J197" t="inlineStr">
         <is>
@@ -20331,13 +20355,13 @@
         <v>45031</v>
       </c>
       <c r="G198">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="H198" s="2">
         <v>45214</v>
       </c>
       <c r="I198">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="J198" t="inlineStr">
         <is>
@@ -20434,13 +20458,13 @@
         <v>45031</v>
       </c>
       <c r="G199">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="H199" s="2">
         <v>45214</v>
       </c>
       <c r="I199">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="J199" t="inlineStr">
         <is>
@@ -20537,13 +20561,13 @@
         <v>45031</v>
       </c>
       <c r="G200">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="H200" s="2">
         <v>45214</v>
       </c>
       <c r="I200">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="J200" t="inlineStr">
         <is>
@@ -20640,13 +20664,13 @@
         <v>45067</v>
       </c>
       <c r="G201">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="H201" s="2">
         <v>45251</v>
       </c>
       <c r="I201">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="J201" t="inlineStr">
         <is>
@@ -20743,13 +20767,13 @@
         <v>45067</v>
       </c>
       <c r="G202">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="H202" s="2">
         <v>45251</v>
       </c>
       <c r="I202">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="J202" t="inlineStr">
         <is>
@@ -20846,13 +20870,13 @@
         <v>45067</v>
       </c>
       <c r="G203">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="H203" s="2">
         <v>45251</v>
       </c>
       <c r="I203">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="J203" t="inlineStr">
         <is>
@@ -20949,13 +20973,13 @@
         <v>45067</v>
       </c>
       <c r="G204">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="H204" s="2">
         <v>45251</v>
       </c>
       <c r="I204">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="J204" t="inlineStr">
         <is>
@@ -21052,13 +21076,13 @@
         <v>45178</v>
       </c>
       <c r="G205">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="H205" s="2">
         <v>45269</v>
       </c>
       <c r="I205">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="J205" t="inlineStr">
         <is>
@@ -21155,7 +21179,7 @@
         <v>45252</v>
       </c>
       <c r="I206">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="J206" t="inlineStr">
         <is>
@@ -21252,13 +21276,13 @@
         <v>45087</v>
       </c>
       <c r="G207">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="H207" s="2">
         <v>45270</v>
       </c>
       <c r="I207">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="J207" t="inlineStr">
         <is>
@@ -21355,13 +21379,13 @@
         <v>45099</v>
       </c>
       <c r="G208">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="H208" s="2">
         <v>45282</v>
       </c>
       <c r="I208">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="J208" t="inlineStr">
         <is>
@@ -21458,13 +21482,13 @@
         <v>45175</v>
       </c>
       <c r="G209">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="H209" s="2">
         <v>45356</v>
       </c>
       <c r="I209">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="J209" t="inlineStr">
         <is>
@@ -21561,13 +21585,13 @@
         <v>45175</v>
       </c>
       <c r="G210">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="H210" s="2">
         <v>45356</v>
       </c>
       <c r="I210">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="J210" t="inlineStr">
         <is>
@@ -21664,13 +21688,13 @@
         <v>45166</v>
       </c>
       <c r="G211">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="H211" s="2">
         <v>45350</v>
       </c>
       <c r="I211">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="J211" t="inlineStr">
         <is>
@@ -21767,13 +21791,13 @@
         <v>45166</v>
       </c>
       <c r="G212">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="H212" s="2">
         <v>45350</v>
       </c>
       <c r="I212">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="J212" t="inlineStr">
         <is>
@@ -21870,13 +21894,13 @@
         <v>45090</v>
       </c>
       <c r="G213">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="H213" s="2">
         <v>45273</v>
       </c>
       <c r="I213">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="J213" t="inlineStr">
         <is>
@@ -21973,13 +21997,13 @@
         <v>45106</v>
       </c>
       <c r="G214">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="H214" s="2">
         <v>45289</v>
       </c>
       <c r="I214">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="J214" t="inlineStr">
         <is>
@@ -22076,13 +22100,13 @@
         <v>45134</v>
       </c>
       <c r="G215">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="H215" s="2">
         <v>45226</v>
       </c>
       <c r="I215">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="J215" t="inlineStr">
         <is>
@@ -22179,13 +22203,13 @@
         <v>45132</v>
       </c>
       <c r="G216">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="H216" s="2">
         <v>45224</v>
       </c>
       <c r="I216">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="J216" t="inlineStr">
         <is>
@@ -22282,13 +22306,13 @@
         <v>45150</v>
       </c>
       <c r="G217">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="H217" s="2">
         <v>45242</v>
       </c>
       <c r="I217">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="J217" t="inlineStr">
         <is>
@@ -22382,16 +22406,16 @@
         </is>
       </c>
       <c r="F218" s="2">
-        <v>45095</v>
+        <v>45187</v>
       </c>
       <c r="G218">
-        <v>108</v>
+        <v>17</v>
       </c>
       <c r="H218" s="2">
-        <v>45187</v>
+        <v>45278</v>
       </c>
       <c r="I218">
-        <v>-16</v>
+        <v>74</v>
       </c>
       <c r="J218" t="inlineStr">
         <is>
@@ -22483,13 +22507,13 @@
         <v>45182</v>
       </c>
       <c r="G219">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="H219" s="2">
         <v>45273</v>
       </c>
       <c r="I219">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="J219" t="inlineStr">
         <is>
@@ -22582,11 +22606,17 @@
           <t>100,00</t>
         </is>
       </c>
+      <c r="F220" s="2">
+        <v>45196</v>
+      </c>
+      <c r="G220">
+        <v>8</v>
+      </c>
       <c r="H220" s="2">
-        <v>45196</v>
+        <v>45287</v>
       </c>
       <c r="I220">
-        <v>-7</v>
+        <v>83</v>
       </c>
       <c r="J220" t="inlineStr">
         <is>
@@ -22680,16 +22710,16 @@
         </is>
       </c>
       <c r="F221" s="2">
-        <v>45108</v>
+        <v>45200</v>
       </c>
       <c r="G221">
-        <v>95</v>
+        <v>4</v>
       </c>
       <c r="H221" s="2">
-        <v>45200</v>
+        <v>45292</v>
       </c>
       <c r="I221">
-        <v>-3</v>
+        <v>88</v>
       </c>
       <c r="J221" t="inlineStr">
         <is>
@@ -22786,13 +22816,13 @@
         <v>45135</v>
       </c>
       <c r="G222">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="H222" s="2">
         <v>45227</v>
       </c>
       <c r="I222">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="J222" t="inlineStr">
         <is>
@@ -22889,13 +22919,13 @@
         <v>45148</v>
       </c>
       <c r="G223">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="H223" s="2">
         <v>45240</v>
       </c>
       <c r="I223">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="J223" t="inlineStr">
         <is>
@@ -22984,16 +23014,16 @@
         </is>
       </c>
       <c r="F224" s="2">
-        <v>45100</v>
+        <v>45192</v>
       </c>
       <c r="G224">
-        <v>103</v>
+        <v>12</v>
       </c>
       <c r="H224" s="2">
-        <v>45192</v>
+        <v>45283</v>
       </c>
       <c r="I224">
-        <v>-11</v>
+        <v>79</v>
       </c>
       <c r="J224" t="inlineStr">
         <is>
@@ -23085,13 +23115,13 @@
         <v>45136</v>
       </c>
       <c r="G225">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="H225" s="2">
         <v>45320</v>
       </c>
       <c r="I225">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="J225" t="inlineStr">
         <is>
@@ -23188,13 +23218,13 @@
         <v>45136</v>
       </c>
       <c r="G226">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="H226" s="2">
         <v>45320</v>
       </c>
       <c r="I226">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="J226" t="inlineStr">
         <is>
@@ -23291,13 +23321,13 @@
         <v>45094</v>
       </c>
       <c r="G227">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="H227" s="2">
         <v>45277</v>
       </c>
       <c r="I227">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="J227" t="inlineStr">
         <is>
@@ -23394,13 +23424,13 @@
         <v>45081</v>
       </c>
       <c r="G228">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="H228" s="2">
         <v>45264</v>
       </c>
       <c r="I228">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="J228" t="inlineStr">
         <is>
@@ -23497,13 +23527,13 @@
         <v>45099</v>
       </c>
       <c r="G229">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="H229" s="2">
         <v>45282</v>
       </c>
       <c r="I229">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="J229" t="inlineStr">
         <is>
@@ -23597,16 +23627,16 @@
         </is>
       </c>
       <c r="F230" s="2">
-        <v>45018</v>
+        <v>45201</v>
       </c>
       <c r="G230">
-        <v>185</v>
+        <v>3</v>
       </c>
       <c r="H230" s="2">
-        <v>45201</v>
+        <v>45384</v>
       </c>
       <c r="I230">
-        <v>-2</v>
+        <v>180</v>
       </c>
       <c r="J230" t="inlineStr">
         <is>
@@ -23703,13 +23733,13 @@
         <v>45031</v>
       </c>
       <c r="G231">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="H231" s="2">
         <v>45214</v>
       </c>
       <c r="I231">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="J231" t="inlineStr">
         <is>
@@ -23806,7 +23836,7 @@
         <v>45294</v>
       </c>
       <c r="I232">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="J232" t="inlineStr">
         <is>
@@ -23903,13 +23933,13 @@
         <v>45079</v>
       </c>
       <c r="G233">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="H233" s="2">
         <v>45262</v>
       </c>
       <c r="I233">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="J233" t="inlineStr">
         <is>
@@ -24002,11 +24032,17 @@
           <t>500 000,00</t>
         </is>
       </c>
+      <c r="F234" s="2">
+        <v>45199</v>
+      </c>
+      <c r="G234">
+        <v>5</v>
+      </c>
       <c r="H234" s="2">
-        <v>45199</v>
+        <v>45382</v>
       </c>
       <c r="I234">
-        <v>-4</v>
+        <v>178</v>
       </c>
       <c r="J234" t="inlineStr">
         <is>
@@ -24103,13 +24139,13 @@
         <v>45021</v>
       </c>
       <c r="G235">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="H235" s="2">
-        <v>45204</v>
+        <v>45387</v>
       </c>
       <c r="I235">
-        <v>1</v>
+        <v>183</v>
       </c>
       <c r="J235" t="inlineStr">
         <is>
@@ -24206,13 +24242,13 @@
         <v>45021</v>
       </c>
       <c r="G236">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="H236" s="2">
-        <v>45204</v>
+        <v>45387</v>
       </c>
       <c r="I236">
-        <v>1</v>
+        <v>183</v>
       </c>
       <c r="J236" t="inlineStr">
         <is>
@@ -24309,13 +24345,13 @@
         <v>45080</v>
       </c>
       <c r="G237">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="H237" s="2">
         <v>45263</v>
       </c>
       <c r="I237">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="J237" t="inlineStr">
         <is>
@@ -24412,13 +24448,13 @@
         <v>45046</v>
       </c>
       <c r="G238">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="H238" s="2">
         <v>45229</v>
       </c>
       <c r="I238">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="J238" t="inlineStr">
         <is>
@@ -24515,13 +24551,13 @@
         <v>45112</v>
       </c>
       <c r="G239">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="H239" s="2">
-        <v>45204</v>
+        <v>45296</v>
       </c>
       <c r="I239">
-        <v>1</v>
+        <v>92</v>
       </c>
       <c r="J239" t="inlineStr">
         <is>
@@ -24609,13 +24645,13 @@
         <v>45112</v>
       </c>
       <c r="G240">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="H240" s="2">
-        <v>45204</v>
+        <v>45296</v>
       </c>
       <c r="I240">
-        <v>1</v>
+        <v>92</v>
       </c>
       <c r="J240" t="inlineStr">
         <is>
@@ -24700,16 +24736,16 @@
         </is>
       </c>
       <c r="F241" s="2">
-        <v>45016</v>
+        <v>45199</v>
       </c>
       <c r="G241">
-        <v>187</v>
+        <v>5</v>
       </c>
       <c r="H241" s="2">
-        <v>45199</v>
+        <v>45382</v>
       </c>
       <c r="I241">
-        <v>-4</v>
+        <v>178</v>
       </c>
       <c r="J241" t="inlineStr">
         <is>
@@ -24806,13 +24842,13 @@
         <v>45070</v>
       </c>
       <c r="G242">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="H242" s="2">
         <v>45254</v>
       </c>
       <c r="I242">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="J242" t="inlineStr">
         <is>
@@ -24909,13 +24945,13 @@
         <v>45168</v>
       </c>
       <c r="G243">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="H243" s="2">
         <v>45260</v>
       </c>
       <c r="I243">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="J243" t="inlineStr">
         <is>
@@ -25012,13 +25048,13 @@
         <v>45027</v>
       </c>
       <c r="G244">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="H244" s="2">
         <v>45210</v>
       </c>
       <c r="I244">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="J244" t="inlineStr">
         <is>
@@ -25115,13 +25151,13 @@
         <v>45077</v>
       </c>
       <c r="G245">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="H245" s="2">
         <v>45260</v>
       </c>
       <c r="I245">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="J245" t="inlineStr">
         <is>
@@ -25218,13 +25254,13 @@
         <v>45100</v>
       </c>
       <c r="G246">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="H246" s="2">
         <v>45283</v>
       </c>
       <c r="I246">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="J246" t="inlineStr">
         <is>
@@ -25321,7 +25357,7 @@
         <v>45281</v>
       </c>
       <c r="I247">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="J247" t="inlineStr">
         <is>
@@ -25418,13 +25454,13 @@
         <v>45044</v>
       </c>
       <c r="G248">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="H248" s="2">
         <v>45227</v>
       </c>
       <c r="I248">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="J248" t="inlineStr">
         <is>
@@ -25521,13 +25557,13 @@
         <v>45101</v>
       </c>
       <c r="G249">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="H249" s="2">
         <v>45283</v>
       </c>
       <c r="I249">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="J249" t="inlineStr">
         <is>
@@ -25624,13 +25660,13 @@
         <v>45134</v>
       </c>
       <c r="G250">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="H250" s="2">
         <v>45226</v>
       </c>
       <c r="I250">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="J250" t="inlineStr">
         <is>
@@ -25727,13 +25763,13 @@
         <v>45158</v>
       </c>
       <c r="G251">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="H251" s="2">
         <v>45250</v>
       </c>
       <c r="I251">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="J251" t="inlineStr">
         <is>
@@ -25827,16 +25863,16 @@
         </is>
       </c>
       <c r="F252" s="2">
-        <v>45108</v>
+        <v>45200</v>
       </c>
       <c r="G252">
-        <v>95</v>
+        <v>4</v>
       </c>
       <c r="H252" s="2">
-        <v>45200</v>
+        <v>45292</v>
       </c>
       <c r="I252">
-        <v>-3</v>
+        <v>88</v>
       </c>
       <c r="J252" t="inlineStr">
         <is>
@@ -25933,7 +25969,7 @@
         <v>45317</v>
       </c>
       <c r="I253">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="J253" t="inlineStr">
         <is>
@@ -26030,13 +26066,13 @@
         <v>45039</v>
       </c>
       <c r="G254">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="H254" s="2">
         <v>45222</v>
       </c>
       <c r="I254">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="J254" t="inlineStr">
         <is>
@@ -26128,13 +26164,13 @@
         <v>45129</v>
       </c>
       <c r="G255">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="H255" s="2">
         <v>45221</v>
       </c>
       <c r="I255">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="J255" t="inlineStr">
         <is>
@@ -26231,13 +26267,13 @@
         <v>45157</v>
       </c>
       <c r="G256">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="H256" s="2">
         <v>45341</v>
       </c>
       <c r="I256">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="J256" t="inlineStr">
         <is>
@@ -26334,13 +26370,13 @@
         <v>45063</v>
       </c>
       <c r="G257">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="H257" s="2">
         <v>45247</v>
       </c>
       <c r="I257">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="J257" t="inlineStr">
         <is>
@@ -26437,7 +26473,7 @@
         <v>45254</v>
       </c>
       <c r="I258">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="J258" t="inlineStr">
         <is>
@@ -26534,7 +26570,7 @@
         <v>45486</v>
       </c>
       <c r="I259">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="J259" t="inlineStr">
         <is>
@@ -26626,13 +26662,13 @@
         <v>45073</v>
       </c>
       <c r="G260">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="H260" s="2">
         <v>45439</v>
       </c>
       <c r="I260">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="J260" t="inlineStr">
         <is>
@@ -26724,7 +26760,7 @@
         <v>45323</v>
       </c>
       <c r="I261">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="J261" t="inlineStr">
         <is>
@@ -26816,7 +26852,7 @@
         <v>45303</v>
       </c>
       <c r="I262">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="J262" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
Bond dates update Fri Oct  6 23:15:13 UTC 2023
</commit_message>
<xml_diff>
--- a/Data/obligacje_screener.xlsx
+++ b/Data/obligacje_screener.xlsx
@@ -512,7 +512,7 @@
         <v>45340</v>
       </c>
       <c r="I2">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="J2" t="inlineStr">
         <is>
@@ -600,13 +600,13 @@
         <v>45121</v>
       </c>
       <c r="G3">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="H3" s="2">
         <v>45305</v>
       </c>
       <c r="I3">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="J3" t="inlineStr">
         <is>
@@ -703,13 +703,13 @@
         <v>45039</v>
       </c>
       <c r="G4">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="H4" s="2">
         <v>45222</v>
       </c>
       <c r="I4">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="J4" t="inlineStr">
         <is>
@@ -806,13 +806,13 @@
         <v>45039</v>
       </c>
       <c r="G5">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="H5" s="2">
         <v>45222</v>
       </c>
       <c r="I5">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="J5" t="inlineStr">
         <is>
@@ -909,13 +909,13 @@
         <v>45129</v>
       </c>
       <c r="G6">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="H6" s="2">
         <v>45221</v>
       </c>
       <c r="I6">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="J6" t="inlineStr">
         <is>
@@ -1012,13 +1012,13 @@
         <v>45162</v>
       </c>
       <c r="G7">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="H7" s="2">
         <v>45254</v>
       </c>
       <c r="I7">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="J7" t="inlineStr">
         <is>
@@ -1110,13 +1110,13 @@
         <v>45156</v>
       </c>
       <c r="G8">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="H8" s="2">
         <v>45248</v>
       </c>
       <c r="I8">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="J8" t="inlineStr">
         <is>
@@ -1213,13 +1213,13 @@
         <v>45141</v>
       </c>
       <c r="G9">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="H9" s="2">
         <v>45233</v>
       </c>
       <c r="I9">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="J9" t="inlineStr">
         <is>
@@ -1316,13 +1316,13 @@
         <v>45062</v>
       </c>
       <c r="G10">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="H10" s="2">
         <v>45246</v>
       </c>
       <c r="I10">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="J10" t="inlineStr">
         <is>
@@ -1419,7 +1419,7 @@
         <v>45286</v>
       </c>
       <c r="I11">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="J11" t="inlineStr">
         <is>
@@ -1516,13 +1516,13 @@
         <v>45195</v>
       </c>
       <c r="G12">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="H12" s="2">
         <v>45377</v>
       </c>
       <c r="I12">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="J12" t="inlineStr">
         <is>
@@ -1614,13 +1614,13 @@
         <v>45036</v>
       </c>
       <c r="G13">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="H13" s="2">
         <v>45219</v>
       </c>
       <c r="I13">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="J13" t="inlineStr">
         <is>
@@ -1717,13 +1717,13 @@
         <v>45036</v>
       </c>
       <c r="G14">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="H14" s="2">
         <v>45219</v>
       </c>
       <c r="I14">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="J14" t="inlineStr">
         <is>
@@ -1820,13 +1820,13 @@
         <v>45106</v>
       </c>
       <c r="G15">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="H15" s="2">
         <v>45289</v>
       </c>
       <c r="I15">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="J15" t="inlineStr">
         <is>
@@ -1923,13 +1923,13 @@
         <v>45186</v>
       </c>
       <c r="G16">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="H16" s="2">
         <v>45278</v>
       </c>
       <c r="I16">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="J16" t="inlineStr">
         <is>
@@ -2026,13 +2026,13 @@
         <v>45186</v>
       </c>
       <c r="G17">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="H17" s="2">
         <v>45277</v>
       </c>
       <c r="I17">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="J17" t="inlineStr">
         <is>
@@ -2129,13 +2129,13 @@
         <v>45132</v>
       </c>
       <c r="G18">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="H18" s="2">
         <v>45224</v>
       </c>
       <c r="I18">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="J18" t="inlineStr">
         <is>
@@ -2232,13 +2232,13 @@
         <v>45137</v>
       </c>
       <c r="G19">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="H19" s="2">
         <v>45229</v>
       </c>
       <c r="I19">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="J19" t="inlineStr">
         <is>
@@ -2330,13 +2330,13 @@
         <v>45183</v>
       </c>
       <c r="G20">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="H20" s="2">
         <v>45274</v>
       </c>
       <c r="I20">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="J20" t="inlineStr">
         <is>
@@ -2433,13 +2433,13 @@
         <v>45187</v>
       </c>
       <c r="G21">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="H21" s="2">
         <v>45278</v>
       </c>
       <c r="I21">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="J21" t="inlineStr">
         <is>
@@ -2536,13 +2536,13 @@
         <v>45187</v>
       </c>
       <c r="G22">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="H22" s="2">
         <v>45278</v>
       </c>
       <c r="I22">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="J22" t="inlineStr">
         <is>
@@ -2639,7 +2639,7 @@
         <v>45245</v>
       </c>
       <c r="I23">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="J23" t="inlineStr">
         <is>
@@ -2736,7 +2736,7 @@
         <v>45245</v>
       </c>
       <c r="I24">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="J24" t="inlineStr">
         <is>
@@ -2830,10 +2830,10 @@
         </is>
       </c>
       <c r="F25" s="2">
-        <v>45021</v>
+        <v>45204</v>
       </c>
       <c r="G25">
-        <v>183</v>
+        <v>1</v>
       </c>
       <c r="J25" t="inlineStr">
         <is>
@@ -2930,13 +2930,13 @@
         <v>45160</v>
       </c>
       <c r="G26">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="H26" s="2">
         <v>45344</v>
       </c>
       <c r="I26">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="J26" t="inlineStr">
         <is>
@@ -3033,13 +3033,13 @@
         <v>45118</v>
       </c>
       <c r="G27">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="H27" s="2">
         <v>45302</v>
       </c>
       <c r="I27">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="J27" t="inlineStr">
         <is>
@@ -3136,13 +3136,13 @@
         <v>45085</v>
       </c>
       <c r="G28">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="H28" s="2">
         <v>45268</v>
       </c>
       <c r="I28">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="J28" t="inlineStr">
         <is>
@@ -3239,13 +3239,13 @@
         <v>45183</v>
       </c>
       <c r="G29">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="H29" s="2">
         <v>45274</v>
       </c>
       <c r="I29">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="J29" t="inlineStr">
         <is>
@@ -3342,7 +3342,7 @@
         <v>45224</v>
       </c>
       <c r="I30">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="J30" t="inlineStr">
         <is>
@@ -3439,13 +3439,13 @@
         <v>45153</v>
       </c>
       <c r="G31">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="H31" s="2">
         <v>45245</v>
       </c>
       <c r="I31">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="J31" t="inlineStr">
         <is>
@@ -3542,13 +3542,13 @@
         <v>45155</v>
       </c>
       <c r="G32">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="H32" s="2">
         <v>45247</v>
       </c>
       <c r="I32">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="J32" t="inlineStr">
         <is>
@@ -3645,7 +3645,7 @@
         <v>45255</v>
       </c>
       <c r="I33">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="J33" t="inlineStr">
         <is>
@@ -3733,13 +3733,13 @@
         <v>45176</v>
       </c>
       <c r="G34">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="H34" s="2">
         <v>45267</v>
       </c>
       <c r="I34">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="J34" t="inlineStr">
         <is>
@@ -3836,13 +3836,13 @@
         <v>45130</v>
       </c>
       <c r="G35">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="H35" s="2">
         <v>45222</v>
       </c>
       <c r="I35">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="J35" t="inlineStr">
         <is>
@@ -3934,13 +3934,13 @@
         <v>45115</v>
       </c>
       <c r="G36">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="H36" s="2">
         <v>45207</v>
       </c>
       <c r="I36">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="J36" t="inlineStr">
         <is>
@@ -4037,13 +4037,13 @@
         <v>45189</v>
       </c>
       <c r="G37">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H37" s="2">
         <v>45280</v>
       </c>
       <c r="I37">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="J37" t="inlineStr">
         <is>
@@ -4135,13 +4135,13 @@
         <v>45107</v>
       </c>
       <c r="G38">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="H38" s="2">
         <v>45290</v>
       </c>
       <c r="I38">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="J38" t="inlineStr">
         <is>
@@ -4238,13 +4238,13 @@
         <v>45063</v>
       </c>
       <c r="G39">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="H39" s="2">
         <v>45247</v>
       </c>
       <c r="I39">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="J39" t="inlineStr">
         <is>
@@ -4341,13 +4341,13 @@
         <v>45177</v>
       </c>
       <c r="G40">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="H40" s="2">
         <v>45359</v>
       </c>
       <c r="I40">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="J40" t="inlineStr">
         <is>
@@ -4444,13 +4444,13 @@
         <v>45107</v>
       </c>
       <c r="G41">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="H41" s="2">
         <v>45290</v>
       </c>
       <c r="I41">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="J41" t="inlineStr">
         <is>
@@ -4547,7 +4547,7 @@
         <v>45265</v>
       </c>
       <c r="I42">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="J42" t="inlineStr">
         <is>
@@ -4644,13 +4644,13 @@
         <v>45098</v>
       </c>
       <c r="G43">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="H43" s="2">
         <v>45281</v>
       </c>
       <c r="I43">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="J43" t="inlineStr">
         <is>
@@ -4747,13 +4747,13 @@
         <v>45099</v>
       </c>
       <c r="G44">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="H44" s="2">
         <v>45282</v>
       </c>
       <c r="I44">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="J44" t="inlineStr">
         <is>
@@ -4850,13 +4850,13 @@
         <v>45106</v>
       </c>
       <c r="G45">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="H45" s="2">
         <v>45289</v>
       </c>
       <c r="I45">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="J45" t="inlineStr">
         <is>
@@ -4953,13 +4953,13 @@
         <v>45106</v>
       </c>
       <c r="G46">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="H46" s="2">
         <v>45289</v>
       </c>
       <c r="I46">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="J46" t="inlineStr">
         <is>
@@ -5056,13 +5056,13 @@
         <v>45120</v>
       </c>
       <c r="G47">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="H47" s="2">
         <v>45304</v>
       </c>
       <c r="I47">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="J47" t="inlineStr">
         <is>
@@ -5159,13 +5159,13 @@
         <v>45118</v>
       </c>
       <c r="G48">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="H48" s="2">
         <v>45302</v>
       </c>
       <c r="I48">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="J48" t="inlineStr">
         <is>
@@ -5262,13 +5262,13 @@
         <v>45152</v>
       </c>
       <c r="G49">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="H49" s="2">
         <v>45336</v>
       </c>
       <c r="I49">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="J49" t="inlineStr">
         <is>
@@ -5365,13 +5365,13 @@
         <v>45042</v>
       </c>
       <c r="G50">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="H50" s="2">
         <v>45225</v>
       </c>
       <c r="I50">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="J50" t="inlineStr">
         <is>
@@ -5468,13 +5468,13 @@
         <v>45122</v>
       </c>
       <c r="G51">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="H51" s="2">
         <v>45306</v>
       </c>
       <c r="I51">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="J51" t="inlineStr">
         <is>
@@ -5571,13 +5571,13 @@
         <v>45139</v>
       </c>
       <c r="G52">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="H52" s="2">
         <v>45323</v>
       </c>
       <c r="I52">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="J52" t="inlineStr">
         <is>
@@ -5665,13 +5665,13 @@
         <v>45099</v>
       </c>
       <c r="G53">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="H53" s="2">
         <v>45282</v>
       </c>
       <c r="I53">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="J53" t="inlineStr">
         <is>
@@ -5768,13 +5768,13 @@
         <v>45196</v>
       </c>
       <c r="G54">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="H54" s="2">
         <v>45287</v>
       </c>
       <c r="I54">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="J54" t="inlineStr">
         <is>
@@ -5871,13 +5871,13 @@
         <v>45044</v>
       </c>
       <c r="G55">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="H55" s="2">
         <v>45227</v>
       </c>
       <c r="I55">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="J55" t="inlineStr">
         <is>
@@ -5974,13 +5974,13 @@
         <v>45151</v>
       </c>
       <c r="G56">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="H56" s="2">
         <v>45243</v>
       </c>
       <c r="I56">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="J56" t="inlineStr">
         <is>
@@ -6072,13 +6072,13 @@
         <v>45196</v>
       </c>
       <c r="G57">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="H57" s="2">
         <v>45287</v>
       </c>
       <c r="I57">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="J57" t="inlineStr">
         <is>
@@ -6175,13 +6175,13 @@
         <v>45069</v>
       </c>
       <c r="G58">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="H58" s="2">
         <v>45253</v>
       </c>
       <c r="I58">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="J58" t="inlineStr">
         <is>
@@ -6278,13 +6278,13 @@
         <v>45191</v>
       </c>
       <c r="G59">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="H59" s="2">
         <v>45282</v>
       </c>
       <c r="I59">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="J59" t="inlineStr">
         <is>
@@ -6376,13 +6376,7 @@
         <v>45113</v>
       </c>
       <c r="G60">
-        <v>91</v>
-      </c>
-      <c r="H60" s="2">
-        <v>45205</v>
-      </c>
-      <c r="I60">
-        <v>1</v>
+        <v>92</v>
       </c>
       <c r="J60" t="inlineStr">
         <is>
@@ -6479,13 +6473,13 @@
         <v>45127</v>
       </c>
       <c r="G61">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="H61" s="2">
         <v>45219</v>
       </c>
       <c r="I61">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="J61" t="inlineStr">
         <is>
@@ -6582,13 +6576,13 @@
         <v>45058</v>
       </c>
       <c r="G62">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="H62" s="2">
         <v>45242</v>
       </c>
       <c r="I62">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="J62" t="inlineStr">
         <is>
@@ -6685,13 +6679,13 @@
         <v>45194</v>
       </c>
       <c r="G63">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="H63" s="2">
         <v>45376</v>
       </c>
       <c r="I63">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="J63" t="inlineStr">
         <is>
@@ -6783,13 +6777,13 @@
         <v>45025</v>
       </c>
       <c r="G64">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="H64" s="2">
         <v>45208</v>
       </c>
       <c r="I64">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="J64" t="inlineStr">
         <is>
@@ -6886,13 +6880,13 @@
         <v>45025</v>
       </c>
       <c r="G65">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="H65" s="2">
         <v>45208</v>
       </c>
       <c r="I65">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="J65" t="inlineStr">
         <is>
@@ -6989,13 +6983,13 @@
         <v>45089</v>
       </c>
       <c r="G66">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="H66" s="2">
         <v>45272</v>
       </c>
       <c r="I66">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="J66" t="inlineStr">
         <is>
@@ -7092,13 +7086,13 @@
         <v>45178</v>
       </c>
       <c r="G67">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="H67" s="2">
         <v>45269</v>
       </c>
       <c r="I67">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="J67" t="inlineStr">
         <is>
@@ -7190,13 +7184,13 @@
         <v>45196</v>
       </c>
       <c r="G68">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="H68" s="2">
         <v>45287</v>
       </c>
       <c r="I68">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="J68" t="inlineStr">
         <is>
@@ -7293,13 +7287,13 @@
         <v>45149</v>
       </c>
       <c r="G69">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="H69" s="2">
         <v>45241</v>
       </c>
       <c r="I69">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="J69" t="inlineStr">
         <is>
@@ -7393,10 +7387,10 @@
         </is>
       </c>
       <c r="H70" s="2">
-        <v>45205</v>
+        <v>45296</v>
       </c>
       <c r="I70">
-        <v>1</v>
+        <v>91</v>
       </c>
       <c r="J70" t="inlineStr">
         <is>
@@ -7493,13 +7487,7 @@
         <v>45114</v>
       </c>
       <c r="G71">
-        <v>90</v>
-      </c>
-      <c r="H71" s="2">
-        <v>45205</v>
-      </c>
-      <c r="I71">
-        <v>1</v>
+        <v>91</v>
       </c>
       <c r="J71" t="inlineStr">
         <is>
@@ -7596,13 +7584,13 @@
         <v>45115</v>
       </c>
       <c r="G72">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="H72" s="2">
         <v>45207</v>
       </c>
       <c r="I72">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="J72" t="inlineStr">
         <is>
@@ -7699,13 +7687,13 @@
         <v>45189</v>
       </c>
       <c r="G73">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H73" s="2">
         <v>45280</v>
       </c>
       <c r="I73">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="J73" t="inlineStr">
         <is>
@@ -7797,13 +7785,13 @@
         <v>45038</v>
       </c>
       <c r="G74">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="H74" s="2">
         <v>45221</v>
       </c>
       <c r="I74">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="J74" t="inlineStr">
         <is>
@@ -7895,13 +7883,13 @@
         <v>45117</v>
       </c>
       <c r="G75">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="H75" s="2">
         <v>45301</v>
       </c>
       <c r="I75">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="J75" t="inlineStr">
         <is>
@@ -7998,13 +7986,13 @@
         <v>45160</v>
       </c>
       <c r="G76">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="H76" s="2">
         <v>45344</v>
       </c>
       <c r="I76">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="J76" t="inlineStr">
         <is>
@@ -8101,13 +8089,13 @@
         <v>45186</v>
       </c>
       <c r="G77">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="H77" s="2">
         <v>45368</v>
       </c>
       <c r="I77">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="J77" t="inlineStr">
         <is>
@@ -8204,13 +8192,13 @@
         <v>45043</v>
       </c>
       <c r="G78">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="H78" s="2">
         <v>45226</v>
       </c>
       <c r="I78">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="J78" t="inlineStr">
         <is>
@@ -8307,13 +8295,13 @@
         <v>45079</v>
       </c>
       <c r="G79">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="H79" s="2">
         <v>45262</v>
       </c>
       <c r="I79">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="J79" t="inlineStr">
         <is>
@@ -8410,7 +8398,7 @@
         <v>45254</v>
       </c>
       <c r="I80">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="J80" t="inlineStr">
         <is>
@@ -8507,13 +8495,13 @@
         <v>45104</v>
       </c>
       <c r="G81">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="H81" s="2">
         <v>45287</v>
       </c>
       <c r="I81">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="J81" t="inlineStr">
         <is>
@@ -8610,7 +8598,7 @@
         <v>45288</v>
       </c>
       <c r="I82">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="J82" t="inlineStr">
         <is>
@@ -8702,13 +8690,13 @@
         <v>45175</v>
       </c>
       <c r="G83">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="H83" s="2">
         <v>45357</v>
       </c>
       <c r="I83">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="J83" t="inlineStr">
         <is>
@@ -8805,13 +8793,13 @@
         <v>45054</v>
       </c>
       <c r="G84">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="H84" s="2">
         <v>45238</v>
       </c>
       <c r="I84">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="J84" t="inlineStr">
         <is>
@@ -8908,13 +8896,13 @@
         <v>45056</v>
       </c>
       <c r="G85">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="H85" s="2">
         <v>45240</v>
       </c>
       <c r="I85">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="J85" t="inlineStr">
         <is>
@@ -9011,13 +8999,13 @@
         <v>45085</v>
       </c>
       <c r="G86">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="H86" s="2">
         <v>45268</v>
       </c>
       <c r="I86">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="J86" t="inlineStr">
         <is>
@@ -9114,13 +9102,13 @@
         <v>45194</v>
       </c>
       <c r="G87">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="H87" s="2">
         <v>45560</v>
       </c>
       <c r="I87">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="J87" t="inlineStr">
         <is>
@@ -9207,13 +9195,13 @@
         <v>45103</v>
       </c>
       <c r="G88">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="H88" s="2">
         <v>45286</v>
       </c>
       <c r="I88">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="J88" t="inlineStr">
         <is>
@@ -9310,13 +9298,13 @@
         <v>45103</v>
       </c>
       <c r="G89">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="H89" s="2">
         <v>45286</v>
       </c>
       <c r="I89">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="J89" t="inlineStr">
         <is>
@@ -9413,13 +9401,13 @@
         <v>45192</v>
       </c>
       <c r="G90">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="H90" s="2">
         <v>45374</v>
       </c>
       <c r="I90">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="J90" t="inlineStr">
         <is>
@@ -9511,13 +9499,13 @@
         <v>45100</v>
       </c>
       <c r="G91">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="H91" s="2">
         <v>45287</v>
       </c>
       <c r="I91">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="J91" t="inlineStr">
         <is>
@@ -9614,13 +9602,13 @@
         <v>45187</v>
       </c>
       <c r="G92">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="H92" s="2">
         <v>45369</v>
       </c>
       <c r="I92">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="J92" t="inlineStr">
         <is>
@@ -9717,13 +9705,13 @@
         <v>45104</v>
       </c>
       <c r="G93">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="H93" s="2">
         <v>45287</v>
       </c>
       <c r="I93">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="J93" t="inlineStr">
         <is>
@@ -9820,13 +9808,13 @@
         <v>45104</v>
       </c>
       <c r="G94">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="H94" s="2">
         <v>45287</v>
       </c>
       <c r="I94">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="J94" t="inlineStr">
         <is>
@@ -9923,13 +9911,13 @@
         <v>45049</v>
       </c>
       <c r="G95">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="H95" s="2">
         <v>45233</v>
       </c>
       <c r="I95">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="J95" t="inlineStr">
         <is>
@@ -10026,13 +10014,13 @@
         <v>45122</v>
       </c>
       <c r="G96">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="H96" s="2">
         <v>45306</v>
       </c>
       <c r="I96">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="J96" t="inlineStr">
         <is>
@@ -10124,13 +10112,13 @@
         <v>45141</v>
       </c>
       <c r="G97">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="H97" s="2">
         <v>45325</v>
       </c>
       <c r="I97">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="J97" t="inlineStr">
         <is>
@@ -10227,13 +10215,13 @@
         <v>45194</v>
       </c>
       <c r="G98">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="H98" s="2">
         <v>45376</v>
       </c>
       <c r="I98">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="J98" t="inlineStr">
         <is>
@@ -10325,13 +10313,13 @@
         <v>45093</v>
       </c>
       <c r="G99">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="H99" s="2">
         <v>45276</v>
       </c>
       <c r="I99">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="J99" t="inlineStr">
         <is>
@@ -10428,13 +10416,13 @@
         <v>45123</v>
       </c>
       <c r="G100">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="H100" s="2">
         <v>45307</v>
       </c>
       <c r="I100">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="J100" t="inlineStr">
         <is>
@@ -10531,13 +10519,13 @@
         <v>45198</v>
       </c>
       <c r="G101">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="H101" s="2">
         <v>45380</v>
       </c>
       <c r="I101">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="J101" t="inlineStr">
         <is>
@@ -10634,13 +10622,13 @@
         <v>45093</v>
       </c>
       <c r="G102">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="H102" s="2">
         <v>45276</v>
       </c>
       <c r="I102">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="J102" t="inlineStr">
         <is>
@@ -10737,13 +10725,13 @@
         <v>45122</v>
       </c>
       <c r="G103">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="H103" s="2">
         <v>45306</v>
       </c>
       <c r="I103">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="J103" t="inlineStr">
         <is>
@@ -10840,13 +10828,13 @@
         <v>45122</v>
       </c>
       <c r="G104">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="H104" s="2">
         <v>45306</v>
       </c>
       <c r="I104">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="J104" t="inlineStr">
         <is>
@@ -10938,13 +10926,13 @@
         <v>45050</v>
       </c>
       <c r="G105">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="H105" s="2">
         <v>45234</v>
       </c>
       <c r="I105">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="J105" t="inlineStr">
         <is>
@@ -11041,13 +11029,13 @@
         <v>45085</v>
       </c>
       <c r="G106">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="H106" s="2">
         <v>45268</v>
       </c>
       <c r="I106">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="J106" t="inlineStr">
         <is>
@@ -11144,13 +11132,13 @@
         <v>45185</v>
       </c>
       <c r="G107">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="H107" s="2">
         <v>45276</v>
       </c>
       <c r="I107">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="J107" t="inlineStr">
         <is>
@@ -11242,13 +11230,13 @@
         <v>45185</v>
       </c>
       <c r="G108">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="H108" s="2">
         <v>45276</v>
       </c>
       <c r="I108">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="J108" t="inlineStr">
         <is>
@@ -11340,13 +11328,13 @@
         <v>45185</v>
       </c>
       <c r="G109">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="H109" s="2">
         <v>45276</v>
       </c>
       <c r="I109">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="J109" t="inlineStr">
         <is>
@@ -11443,13 +11431,13 @@
         <v>45148</v>
       </c>
       <c r="G110">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="H110" s="2">
         <v>45240</v>
       </c>
       <c r="I110">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="J110" t="inlineStr">
         <is>
@@ -11546,13 +11534,13 @@
         <v>45119</v>
       </c>
       <c r="G111">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="H111" s="2">
         <v>45211</v>
       </c>
       <c r="I111">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="J111" t="inlineStr">
         <is>
@@ -11649,13 +11637,13 @@
         <v>45172</v>
       </c>
       <c r="G112">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="H112" s="2">
         <v>45263</v>
       </c>
       <c r="I112">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="J112" t="inlineStr">
         <is>
@@ -11752,13 +11740,13 @@
         <v>45023</v>
       </c>
       <c r="G113">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="H113" s="2">
         <v>45206</v>
       </c>
       <c r="I113">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J113" t="inlineStr">
         <is>
@@ -11855,13 +11843,13 @@
         <v>45203</v>
       </c>
       <c r="G114">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H114" s="2">
         <v>45295</v>
       </c>
       <c r="I114">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="J114" t="inlineStr">
         <is>
@@ -11958,7 +11946,7 @@
         <v>45218</v>
       </c>
       <c r="I115">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="J115" t="inlineStr">
         <is>
@@ -12055,13 +12043,13 @@
         <v>45161</v>
       </c>
       <c r="G116">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="H116" s="2">
         <v>45253</v>
       </c>
       <c r="I116">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="J116" t="inlineStr">
         <is>
@@ -12158,13 +12146,13 @@
         <v>45115</v>
       </c>
       <c r="G117">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="H117" s="2">
         <v>45299</v>
       </c>
       <c r="I117">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="J117" t="inlineStr">
         <is>
@@ -12256,13 +12244,13 @@
         <v>45094</v>
       </c>
       <c r="G118">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="H118" s="2">
         <v>45277</v>
       </c>
       <c r="I118">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="J118" t="inlineStr">
         <is>
@@ -12359,13 +12347,13 @@
         <v>45104</v>
       </c>
       <c r="G119">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="H119" s="2">
         <v>45287</v>
       </c>
       <c r="I119">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="J119" t="inlineStr">
         <is>
@@ -12462,13 +12450,13 @@
         <v>45104</v>
       </c>
       <c r="G120">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="H120" s="2">
         <v>45287</v>
       </c>
       <c r="I120">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="J120" t="inlineStr">
         <is>
@@ -12565,13 +12553,13 @@
         <v>45104</v>
       </c>
       <c r="G121">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="H121" s="2">
         <v>45287</v>
       </c>
       <c r="I121">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="J121" t="inlineStr">
         <is>
@@ -12668,13 +12656,13 @@
         <v>45104</v>
       </c>
       <c r="G122">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="H122" s="2">
         <v>45287</v>
       </c>
       <c r="I122">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="J122" t="inlineStr">
         <is>
@@ -12771,13 +12759,13 @@
         <v>45199</v>
       </c>
       <c r="G123">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="H123" s="2">
         <v>45291</v>
       </c>
       <c r="I123">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="J123" t="inlineStr">
         <is>
@@ -12874,13 +12862,13 @@
         <v>45197</v>
       </c>
       <c r="G124">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="H124" s="2">
         <v>45379</v>
       </c>
       <c r="I124">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="J124" t="inlineStr">
         <is>
@@ -12977,13 +12965,13 @@
         <v>45121</v>
       </c>
       <c r="G125">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="H125" s="2">
         <v>45213</v>
       </c>
       <c r="I125">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="J125" t="inlineStr">
         <is>
@@ -13080,13 +13068,13 @@
         <v>45134</v>
       </c>
       <c r="G126">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="H126" s="2">
         <v>45226</v>
       </c>
       <c r="I126">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="J126" t="inlineStr">
         <is>
@@ -13183,7 +13171,7 @@
         <v>45212</v>
       </c>
       <c r="I127">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="J127" t="inlineStr">
         <is>
@@ -13280,13 +13268,13 @@
         <v>45126</v>
       </c>
       <c r="G128">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="H128" s="2">
         <v>45218</v>
       </c>
       <c r="I128">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="J128" t="inlineStr">
         <is>
@@ -13378,13 +13366,13 @@
         <v>45158</v>
       </c>
       <c r="G129">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="H129" s="2">
         <v>45250</v>
       </c>
       <c r="I129">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="J129" t="inlineStr">
         <is>
@@ -13481,13 +13469,13 @@
         <v>45171</v>
       </c>
       <c r="G130">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="H130" s="2">
         <v>45262</v>
       </c>
       <c r="I130">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="J130" t="inlineStr">
         <is>
@@ -13584,13 +13572,13 @@
         <v>45203</v>
       </c>
       <c r="G131">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H131" s="2">
         <v>45295</v>
       </c>
       <c r="I131">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="J131" t="inlineStr">
         <is>
@@ -13687,13 +13675,13 @@
         <v>45144</v>
       </c>
       <c r="G132">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="H132" s="2">
         <v>45236</v>
       </c>
       <c r="I132">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="J132" t="inlineStr">
         <is>
@@ -13790,13 +13778,13 @@
         <v>45156</v>
       </c>
       <c r="G133">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="H133" s="2">
         <v>45248</v>
       </c>
       <c r="I133">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="J133" t="inlineStr">
         <is>
@@ -13888,13 +13876,13 @@
         <v>45146</v>
       </c>
       <c r="G134">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="H134" s="2">
         <v>45238</v>
       </c>
       <c r="I134">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="J134" t="inlineStr">
         <is>
@@ -13991,13 +13979,13 @@
         <v>45140</v>
       </c>
       <c r="G135">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="H135" s="2">
         <v>45232</v>
       </c>
       <c r="I135">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="J135" t="inlineStr">
         <is>
@@ -14094,13 +14082,13 @@
         <v>45196</v>
       </c>
       <c r="G136">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="H136" s="2">
         <v>45287</v>
       </c>
       <c r="I136">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="J136" t="inlineStr">
         <is>
@@ -14197,13 +14185,13 @@
         <v>45197</v>
       </c>
       <c r="G137">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="H137" s="2">
         <v>45288</v>
       </c>
       <c r="I137">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="J137" t="inlineStr">
         <is>
@@ -14300,13 +14288,13 @@
         <v>45179</v>
       </c>
       <c r="G138">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="H138" s="2">
         <v>45270</v>
       </c>
       <c r="I138">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="J138" t="inlineStr">
         <is>
@@ -14398,13 +14386,13 @@
         <v>45197</v>
       </c>
       <c r="G139">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="H139" s="2">
         <v>45288</v>
       </c>
       <c r="I139">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="J139" t="inlineStr">
         <is>
@@ -14501,13 +14489,13 @@
         <v>45182</v>
       </c>
       <c r="G140">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="H140" s="2">
         <v>45273</v>
       </c>
       <c r="I140">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="J140" t="inlineStr">
         <is>
@@ -14604,13 +14592,13 @@
         <v>45116</v>
       </c>
       <c r="G141">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="H141" s="2">
         <v>45208</v>
       </c>
       <c r="I141">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="J141" t="inlineStr">
         <is>
@@ -14702,13 +14690,13 @@
         <v>45150</v>
       </c>
       <c r="G142">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="H142" s="2">
         <v>45242</v>
       </c>
       <c r="I142">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="J142" t="inlineStr">
         <is>
@@ -14805,7 +14793,7 @@
         <v>45238</v>
       </c>
       <c r="I143">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="J143" t="inlineStr">
         <is>
@@ -14902,13 +14890,13 @@
         <v>45171</v>
       </c>
       <c r="G144">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="H144" s="2">
         <v>45262</v>
       </c>
       <c r="I144">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="J144" t="inlineStr">
         <is>
@@ -15005,13 +14993,13 @@
         <v>45194</v>
       </c>
       <c r="G145">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="H145" s="2">
         <v>45285</v>
       </c>
       <c r="I145">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="J145" t="inlineStr">
         <is>
@@ -15098,13 +15086,13 @@
         <v>45119</v>
       </c>
       <c r="G146">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="H146" s="2">
         <v>45211</v>
       </c>
       <c r="I146">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="J146" t="inlineStr">
         <is>
@@ -15201,13 +15189,13 @@
         <v>45165</v>
       </c>
       <c r="G147">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="H147" s="2">
         <v>45257</v>
       </c>
       <c r="I147">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="J147" t="inlineStr">
         <is>
@@ -15304,13 +15292,13 @@
         <v>45166</v>
       </c>
       <c r="G148">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="H148" s="2">
         <v>45258</v>
       </c>
       <c r="I148">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="J148" t="inlineStr">
         <is>
@@ -15407,13 +15395,13 @@
         <v>45185</v>
       </c>
       <c r="G149">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="H149" s="2">
         <v>45276</v>
       </c>
       <c r="I149">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="J149" t="inlineStr">
         <is>
@@ -15510,13 +15498,13 @@
         <v>45035</v>
       </c>
       <c r="G150">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="H150" s="2">
         <v>45218</v>
       </c>
       <c r="I150">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="J150" t="inlineStr">
         <is>
@@ -15613,13 +15601,13 @@
         <v>45174</v>
       </c>
       <c r="G151">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="H151" s="2">
         <v>45356</v>
       </c>
       <c r="I151">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="J151" t="inlineStr">
         <is>
@@ -15716,13 +15704,13 @@
         <v>45089</v>
       </c>
       <c r="G152">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="H152" s="2">
         <v>45272</v>
       </c>
       <c r="I152">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="J152" t="inlineStr">
         <is>
@@ -15819,13 +15807,13 @@
         <v>45124</v>
       </c>
       <c r="G153">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="H153" s="2">
         <v>45308</v>
       </c>
       <c r="I153">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="J153" t="inlineStr">
         <is>
@@ -15922,13 +15910,13 @@
         <v>45124</v>
       </c>
       <c r="G154">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="H154" s="2">
         <v>45308</v>
       </c>
       <c r="I154">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="J154" t="inlineStr">
         <is>
@@ -16025,13 +16013,13 @@
         <v>45026</v>
       </c>
       <c r="G155">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="H155" s="2">
         <v>45209</v>
       </c>
       <c r="I155">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="J155" t="inlineStr">
         <is>
@@ -16128,13 +16116,13 @@
         <v>45026</v>
       </c>
       <c r="G156">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="H156" s="2">
         <v>45209</v>
       </c>
       <c r="I156">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="J156" t="inlineStr">
         <is>
@@ -16231,13 +16219,13 @@
         <v>45026</v>
       </c>
       <c r="G157">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="H157" s="2">
         <v>45209</v>
       </c>
       <c r="I157">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="J157" t="inlineStr">
         <is>
@@ -16334,13 +16322,13 @@
         <v>45026</v>
       </c>
       <c r="G158">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="H158" s="2">
         <v>45209</v>
       </c>
       <c r="I158">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="J158" t="inlineStr">
         <is>
@@ -16437,13 +16425,13 @@
         <v>45156</v>
       </c>
       <c r="G159">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="H159" s="2">
         <v>45247</v>
       </c>
       <c r="I159">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="J159" t="inlineStr">
         <is>
@@ -16540,13 +16528,13 @@
         <v>45153</v>
       </c>
       <c r="G160">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="H160" s="2">
         <v>45245</v>
       </c>
       <c r="I160">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="J160" t="inlineStr">
         <is>
@@ -16643,13 +16631,13 @@
         <v>45135</v>
       </c>
       <c r="G161">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="H161" s="2">
         <v>45319</v>
       </c>
       <c r="I161">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="J161" t="inlineStr">
         <is>
@@ -16746,13 +16734,13 @@
         <v>45091</v>
       </c>
       <c r="G162">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="H162" s="2">
         <v>45274</v>
       </c>
       <c r="I162">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="J162" t="inlineStr">
         <is>
@@ -16844,13 +16832,13 @@
         <v>45091</v>
       </c>
       <c r="G163">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="H163" s="2">
         <v>45274</v>
       </c>
       <c r="I163">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="J163" t="inlineStr">
         <is>
@@ -16942,13 +16930,13 @@
         <v>45138</v>
       </c>
       <c r="G164">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="H164" s="2">
         <v>45322</v>
       </c>
       <c r="I164">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="J164" t="inlineStr">
         <is>
@@ -17045,13 +17033,13 @@
         <v>45138</v>
       </c>
       <c r="G165">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="H165" s="2">
         <v>45322</v>
       </c>
       <c r="I165">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="J165" t="inlineStr">
         <is>
@@ -17148,13 +17136,13 @@
         <v>45085</v>
       </c>
       <c r="G166">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="H166" s="2">
         <v>45268</v>
       </c>
       <c r="I166">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="J166" t="inlineStr">
         <is>
@@ -17251,13 +17239,13 @@
         <v>45085</v>
       </c>
       <c r="G167">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="H167" s="2">
         <v>45268</v>
       </c>
       <c r="I167">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="J167" t="inlineStr">
         <is>
@@ -17354,7 +17342,7 @@
         <v>45326</v>
       </c>
       <c r="I168">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="J168" t="inlineStr">
         <is>
@@ -17451,13 +17439,13 @@
         <v>45173</v>
       </c>
       <c r="G169">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="H169" s="2">
         <v>45355</v>
       </c>
       <c r="I169">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="J169" t="inlineStr">
         <is>
@@ -17554,13 +17542,13 @@
         <v>45056</v>
       </c>
       <c r="G170">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="H170" s="2">
         <v>45240</v>
       </c>
       <c r="I170">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="J170" t="inlineStr">
         <is>
@@ -17657,7 +17645,7 @@
         <v>45238</v>
       </c>
       <c r="I171">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="J171" t="inlineStr">
         <is>
@@ -17754,13 +17742,13 @@
         <v>45141</v>
       </c>
       <c r="G172">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="H172" s="2">
         <v>45325</v>
       </c>
       <c r="I172">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="J172" t="inlineStr">
         <is>
@@ -17857,13 +17845,13 @@
         <v>45037</v>
       </c>
       <c r="G173">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="H173" s="2">
         <v>45220</v>
       </c>
       <c r="I173">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="J173" t="inlineStr">
         <is>
@@ -17960,13 +17948,13 @@
         <v>45171</v>
       </c>
       <c r="G174">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="H174" s="2">
         <v>45262</v>
       </c>
       <c r="I174">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="J174" t="inlineStr">
         <is>
@@ -18063,13 +18051,13 @@
         <v>45197</v>
       </c>
       <c r="G175">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="H175" s="2">
         <v>45288</v>
       </c>
       <c r="I175">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="J175" t="inlineStr">
         <is>
@@ -18166,13 +18154,13 @@
         <v>45162</v>
       </c>
       <c r="G176">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="H176" s="2">
         <v>45254</v>
       </c>
       <c r="I176">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="J176" t="inlineStr">
         <is>
@@ -18269,13 +18257,13 @@
         <v>45061</v>
       </c>
       <c r="G177">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="H177" s="2">
         <v>45245</v>
       </c>
       <c r="I177">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="J177" t="inlineStr">
         <is>
@@ -18372,13 +18360,13 @@
         <v>45120</v>
       </c>
       <c r="G178">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="H178" s="2">
         <v>45212</v>
       </c>
       <c r="I178">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="J178" t="inlineStr">
         <is>
@@ -18475,13 +18463,13 @@
         <v>45191</v>
       </c>
       <c r="G179">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="H179" s="2">
         <v>45282</v>
       </c>
       <c r="I179">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="J179" t="inlineStr">
         <is>
@@ -18578,13 +18566,13 @@
         <v>45088</v>
       </c>
       <c r="G180">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="H180" s="2">
         <v>45271</v>
       </c>
       <c r="I180">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="J180" t="inlineStr">
         <is>
@@ -18681,13 +18669,13 @@
         <v>45192</v>
       </c>
       <c r="G181">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="H181" s="2">
         <v>45283</v>
       </c>
       <c r="I181">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="J181" t="inlineStr">
         <is>
@@ -18774,13 +18762,13 @@
         <v>45131</v>
       </c>
       <c r="G182">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="H182" s="2">
         <v>45223</v>
       </c>
       <c r="I182">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="J182" t="inlineStr">
         <is>
@@ -18872,13 +18860,13 @@
         <v>45136</v>
       </c>
       <c r="G183">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="H183" s="2">
         <v>45228</v>
       </c>
       <c r="I183">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="J183" t="inlineStr">
         <is>
@@ -18970,13 +18958,13 @@
         <v>45150</v>
       </c>
       <c r="G184">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="H184" s="2">
         <v>45242</v>
       </c>
       <c r="I184">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="J184" t="inlineStr">
         <is>
@@ -19068,13 +19056,13 @@
         <v>45118</v>
       </c>
       <c r="G185">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="H185" s="2">
         <v>45210</v>
       </c>
       <c r="I185">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="J185" t="inlineStr">
         <is>
@@ -19166,13 +19154,13 @@
         <v>45129</v>
       </c>
       <c r="G186">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="H186" s="2">
         <v>45221</v>
       </c>
       <c r="I186">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="J186" t="inlineStr">
         <is>
@@ -19264,13 +19252,13 @@
         <v>45189</v>
       </c>
       <c r="G187">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H187" s="2">
         <v>45280</v>
       </c>
       <c r="I187">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="J187" t="inlineStr">
         <is>
@@ -19357,13 +19345,13 @@
         <v>45193</v>
       </c>
       <c r="G188">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="H188" s="2">
         <v>45284</v>
       </c>
       <c r="I188">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="J188" t="inlineStr">
         <is>
@@ -19450,13 +19438,13 @@
         <v>45165</v>
       </c>
       <c r="G189">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="H189" s="2">
         <v>45257</v>
       </c>
       <c r="I189">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="J189" t="inlineStr">
         <is>
@@ -19548,13 +19536,13 @@
         <v>45202</v>
       </c>
       <c r="G190">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H190" s="2">
         <v>45385</v>
       </c>
       <c r="I190">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="J190" t="inlineStr">
         <is>
@@ -19651,13 +19639,13 @@
         <v>45081</v>
       </c>
       <c r="G191">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="H191" s="2">
         <v>45264</v>
       </c>
       <c r="I191">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="J191" t="inlineStr">
         <is>
@@ -19754,13 +19742,13 @@
         <v>45081</v>
       </c>
       <c r="G192">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="H192" s="2">
         <v>45264</v>
       </c>
       <c r="I192">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="J192" t="inlineStr">
         <is>
@@ -19857,7 +19845,7 @@
         <v>45319</v>
       </c>
       <c r="I193">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="J193" t="inlineStr">
         <is>
@@ -19954,7 +19942,7 @@
         <v>45319</v>
       </c>
       <c r="I194">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="J194" t="inlineStr">
         <is>
@@ -20046,13 +20034,13 @@
         <v>45046</v>
       </c>
       <c r="G195">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="H195" s="2">
         <v>45230</v>
       </c>
       <c r="I195">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="J195" t="inlineStr">
         <is>
@@ -20149,13 +20137,13 @@
         <v>45046</v>
       </c>
       <c r="G196">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="H196" s="2">
         <v>45230</v>
       </c>
       <c r="I196">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="J196" t="inlineStr">
         <is>
@@ -20252,13 +20240,13 @@
         <v>45031</v>
       </c>
       <c r="G197">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="H197" s="2">
         <v>45214</v>
       </c>
       <c r="I197">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="J197" t="inlineStr">
         <is>
@@ -20355,13 +20343,13 @@
         <v>45031</v>
       </c>
       <c r="G198">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="H198" s="2">
         <v>45214</v>
       </c>
       <c r="I198">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="J198" t="inlineStr">
         <is>
@@ -20458,13 +20446,13 @@
         <v>45031</v>
       </c>
       <c r="G199">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="H199" s="2">
         <v>45214</v>
       </c>
       <c r="I199">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="J199" t="inlineStr">
         <is>
@@ -20561,13 +20549,13 @@
         <v>45031</v>
       </c>
       <c r="G200">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="H200" s="2">
         <v>45214</v>
       </c>
       <c r="I200">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="J200" t="inlineStr">
         <is>
@@ -20664,13 +20652,13 @@
         <v>45067</v>
       </c>
       <c r="G201">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="H201" s="2">
         <v>45251</v>
       </c>
       <c r="I201">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="J201" t="inlineStr">
         <is>
@@ -20767,13 +20755,13 @@
         <v>45067</v>
       </c>
       <c r="G202">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="H202" s="2">
         <v>45251</v>
       </c>
       <c r="I202">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="J202" t="inlineStr">
         <is>
@@ -20870,13 +20858,13 @@
         <v>45067</v>
       </c>
       <c r="G203">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="H203" s="2">
         <v>45251</v>
       </c>
       <c r="I203">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="J203" t="inlineStr">
         <is>
@@ -20973,13 +20961,13 @@
         <v>45067</v>
       </c>
       <c r="G204">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="H204" s="2">
         <v>45251</v>
       </c>
       <c r="I204">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="J204" t="inlineStr">
         <is>
@@ -21076,13 +21064,13 @@
         <v>45178</v>
       </c>
       <c r="G205">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="H205" s="2">
         <v>45269</v>
       </c>
       <c r="I205">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="J205" t="inlineStr">
         <is>
@@ -21179,7 +21167,7 @@
         <v>45252</v>
       </c>
       <c r="I206">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="J206" t="inlineStr">
         <is>
@@ -21276,13 +21264,13 @@
         <v>45087</v>
       </c>
       <c r="G207">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="H207" s="2">
         <v>45270</v>
       </c>
       <c r="I207">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="J207" t="inlineStr">
         <is>
@@ -21379,13 +21367,13 @@
         <v>45099</v>
       </c>
       <c r="G208">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="H208" s="2">
         <v>45282</v>
       </c>
       <c r="I208">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="J208" t="inlineStr">
         <is>
@@ -21482,13 +21470,13 @@
         <v>45175</v>
       </c>
       <c r="G209">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="H209" s="2">
         <v>45356</v>
       </c>
       <c r="I209">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="J209" t="inlineStr">
         <is>
@@ -21585,13 +21573,13 @@
         <v>45175</v>
       </c>
       <c r="G210">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="H210" s="2">
         <v>45356</v>
       </c>
       <c r="I210">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="J210" t="inlineStr">
         <is>
@@ -21688,13 +21676,13 @@
         <v>45166</v>
       </c>
       <c r="G211">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="H211" s="2">
         <v>45350</v>
       </c>
       <c r="I211">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="J211" t="inlineStr">
         <is>
@@ -21791,13 +21779,13 @@
         <v>45166</v>
       </c>
       <c r="G212">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="H212" s="2">
         <v>45350</v>
       </c>
       <c r="I212">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="J212" t="inlineStr">
         <is>
@@ -21894,13 +21882,13 @@
         <v>45090</v>
       </c>
       <c r="G213">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="H213" s="2">
         <v>45273</v>
       </c>
       <c r="I213">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="J213" t="inlineStr">
         <is>
@@ -21997,13 +21985,13 @@
         <v>45106</v>
       </c>
       <c r="G214">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="H214" s="2">
         <v>45289</v>
       </c>
       <c r="I214">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="J214" t="inlineStr">
         <is>
@@ -22100,13 +22088,13 @@
         <v>45134</v>
       </c>
       <c r="G215">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="H215" s="2">
         <v>45226</v>
       </c>
       <c r="I215">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="J215" t="inlineStr">
         <is>
@@ -22203,13 +22191,13 @@
         <v>45132</v>
       </c>
       <c r="G216">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="H216" s="2">
         <v>45224</v>
       </c>
       <c r="I216">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="J216" t="inlineStr">
         <is>
@@ -22306,13 +22294,13 @@
         <v>45150</v>
       </c>
       <c r="G217">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="H217" s="2">
         <v>45242</v>
       </c>
       <c r="I217">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="J217" t="inlineStr">
         <is>
@@ -22409,13 +22397,13 @@
         <v>45187</v>
       </c>
       <c r="G218">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="H218" s="2">
         <v>45278</v>
       </c>
       <c r="I218">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="J218" t="inlineStr">
         <is>
@@ -22507,13 +22495,13 @@
         <v>45182</v>
       </c>
       <c r="G219">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="H219" s="2">
         <v>45273</v>
       </c>
       <c r="I219">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="J219" t="inlineStr">
         <is>
@@ -22610,13 +22598,13 @@
         <v>45196</v>
       </c>
       <c r="G220">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="H220" s="2">
         <v>45287</v>
       </c>
       <c r="I220">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="J220" t="inlineStr">
         <is>
@@ -22713,13 +22701,13 @@
         <v>45200</v>
       </c>
       <c r="G221">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="H221" s="2">
         <v>45292</v>
       </c>
       <c r="I221">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="J221" t="inlineStr">
         <is>
@@ -22816,13 +22804,13 @@
         <v>45135</v>
       </c>
       <c r="G222">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="H222" s="2">
         <v>45227</v>
       </c>
       <c r="I222">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="J222" t="inlineStr">
         <is>
@@ -22919,13 +22907,13 @@
         <v>45148</v>
       </c>
       <c r="G223">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="H223" s="2">
         <v>45240</v>
       </c>
       <c r="I223">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="J223" t="inlineStr">
         <is>
@@ -23017,13 +23005,13 @@
         <v>45192</v>
       </c>
       <c r="G224">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="H224" s="2">
         <v>45283</v>
       </c>
       <c r="I224">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="J224" t="inlineStr">
         <is>
@@ -23115,13 +23103,13 @@
         <v>45136</v>
       </c>
       <c r="G225">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="H225" s="2">
         <v>45320</v>
       </c>
       <c r="I225">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="J225" t="inlineStr">
         <is>
@@ -23218,13 +23206,13 @@
         <v>45136</v>
       </c>
       <c r="G226">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="H226" s="2">
         <v>45320</v>
       </c>
       <c r="I226">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="J226" t="inlineStr">
         <is>
@@ -23321,13 +23309,13 @@
         <v>45094</v>
       </c>
       <c r="G227">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="H227" s="2">
         <v>45277</v>
       </c>
       <c r="I227">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="J227" t="inlineStr">
         <is>
@@ -23424,13 +23412,13 @@
         <v>45081</v>
       </c>
       <c r="G228">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="H228" s="2">
         <v>45264</v>
       </c>
       <c r="I228">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="J228" t="inlineStr">
         <is>
@@ -23527,13 +23515,13 @@
         <v>45099</v>
       </c>
       <c r="G229">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="H229" s="2">
         <v>45282</v>
       </c>
       <c r="I229">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="J229" t="inlineStr">
         <is>
@@ -23630,13 +23618,13 @@
         <v>45201</v>
       </c>
       <c r="G230">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="H230" s="2">
         <v>45384</v>
       </c>
       <c r="I230">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="J230" t="inlineStr">
         <is>
@@ -23733,13 +23721,13 @@
         <v>45031</v>
       </c>
       <c r="G231">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="H231" s="2">
         <v>45214</v>
       </c>
       <c r="I231">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="J231" t="inlineStr">
         <is>
@@ -23836,7 +23824,7 @@
         <v>45294</v>
       </c>
       <c r="I232">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="J232" t="inlineStr">
         <is>
@@ -23933,13 +23921,13 @@
         <v>45079</v>
       </c>
       <c r="G233">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="H233" s="2">
         <v>45262</v>
       </c>
       <c r="I233">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="J233" t="inlineStr">
         <is>
@@ -24036,13 +24024,13 @@
         <v>45199</v>
       </c>
       <c r="G234">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="H234" s="2">
         <v>45382</v>
       </c>
       <c r="I234">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="J234" t="inlineStr">
         <is>
@@ -24136,16 +24124,16 @@
         </is>
       </c>
       <c r="F235" s="2">
-        <v>45021</v>
+        <v>45204</v>
       </c>
       <c r="G235">
-        <v>183</v>
+        <v>1</v>
       </c>
       <c r="H235" s="2">
         <v>45387</v>
       </c>
       <c r="I235">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="J235" t="inlineStr">
         <is>
@@ -24239,16 +24227,16 @@
         </is>
       </c>
       <c r="F236" s="2">
-        <v>45021</v>
+        <v>45204</v>
       </c>
       <c r="G236">
-        <v>183</v>
+        <v>1</v>
       </c>
       <c r="H236" s="2">
         <v>45387</v>
       </c>
       <c r="I236">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="J236" t="inlineStr">
         <is>
@@ -24345,13 +24333,13 @@
         <v>45080</v>
       </c>
       <c r="G237">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="H237" s="2">
         <v>45263</v>
       </c>
       <c r="I237">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="J237" t="inlineStr">
         <is>
@@ -24448,13 +24436,13 @@
         <v>45046</v>
       </c>
       <c r="G238">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="H238" s="2">
         <v>45229</v>
       </c>
       <c r="I238">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="J238" t="inlineStr">
         <is>
@@ -24548,16 +24536,16 @@
         </is>
       </c>
       <c r="F239" s="2">
-        <v>45112</v>
+        <v>45204</v>
       </c>
       <c r="G239">
-        <v>92</v>
+        <v>1</v>
       </c>
       <c r="H239" s="2">
         <v>45296</v>
       </c>
       <c r="I239">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="J239" t="inlineStr">
         <is>
@@ -24642,16 +24630,16 @@
         </is>
       </c>
       <c r="F240" s="2">
-        <v>45112</v>
+        <v>45204</v>
       </c>
       <c r="G240">
-        <v>92</v>
+        <v>1</v>
       </c>
       <c r="H240" s="2">
         <v>45296</v>
       </c>
       <c r="I240">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="J240" t="inlineStr">
         <is>
@@ -24739,13 +24727,13 @@
         <v>45199</v>
       </c>
       <c r="G241">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="H241" s="2">
         <v>45382</v>
       </c>
       <c r="I241">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="J241" t="inlineStr">
         <is>
@@ -24842,13 +24830,13 @@
         <v>45070</v>
       </c>
       <c r="G242">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="H242" s="2">
         <v>45254</v>
       </c>
       <c r="I242">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="J242" t="inlineStr">
         <is>
@@ -24945,13 +24933,13 @@
         <v>45168</v>
       </c>
       <c r="G243">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="H243" s="2">
         <v>45260</v>
       </c>
       <c r="I243">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="J243" t="inlineStr">
         <is>
@@ -25048,13 +25036,13 @@
         <v>45027</v>
       </c>
       <c r="G244">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="H244" s="2">
         <v>45210</v>
       </c>
       <c r="I244">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="J244" t="inlineStr">
         <is>
@@ -25151,13 +25139,13 @@
         <v>45077</v>
       </c>
       <c r="G245">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="H245" s="2">
         <v>45260</v>
       </c>
       <c r="I245">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="J245" t="inlineStr">
         <is>
@@ -25254,13 +25242,13 @@
         <v>45100</v>
       </c>
       <c r="G246">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="H246" s="2">
         <v>45283</v>
       </c>
       <c r="I246">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="J246" t="inlineStr">
         <is>
@@ -25357,7 +25345,7 @@
         <v>45281</v>
       </c>
       <c r="I247">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="J247" t="inlineStr">
         <is>
@@ -25454,13 +25442,13 @@
         <v>45044</v>
       </c>
       <c r="G248">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="H248" s="2">
         <v>45227</v>
       </c>
       <c r="I248">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="J248" t="inlineStr">
         <is>
@@ -25557,13 +25545,13 @@
         <v>45101</v>
       </c>
       <c r="G249">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="H249" s="2">
         <v>45283</v>
       </c>
       <c r="I249">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="J249" t="inlineStr">
         <is>
@@ -25660,13 +25648,13 @@
         <v>45134</v>
       </c>
       <c r="G250">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="H250" s="2">
         <v>45226</v>
       </c>
       <c r="I250">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="J250" t="inlineStr">
         <is>
@@ -25763,13 +25751,13 @@
         <v>45158</v>
       </c>
       <c r="G251">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="H251" s="2">
         <v>45250</v>
       </c>
       <c r="I251">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="J251" t="inlineStr">
         <is>
@@ -25866,13 +25854,13 @@
         <v>45200</v>
       </c>
       <c r="G252">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="H252" s="2">
         <v>45292</v>
       </c>
       <c r="I252">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="J252" t="inlineStr">
         <is>
@@ -25969,7 +25957,7 @@
         <v>45317</v>
       </c>
       <c r="I253">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="J253" t="inlineStr">
         <is>
@@ -26066,13 +26054,13 @@
         <v>45039</v>
       </c>
       <c r="G254">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="H254" s="2">
         <v>45222</v>
       </c>
       <c r="I254">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="J254" t="inlineStr">
         <is>
@@ -26164,13 +26152,13 @@
         <v>45129</v>
       </c>
       <c r="G255">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="H255" s="2">
         <v>45221</v>
       </c>
       <c r="I255">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="J255" t="inlineStr">
         <is>
@@ -26267,13 +26255,13 @@
         <v>45157</v>
       </c>
       <c r="G256">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="H256" s="2">
         <v>45341</v>
       </c>
       <c r="I256">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="J256" t="inlineStr">
         <is>
@@ -26370,13 +26358,13 @@
         <v>45063</v>
       </c>
       <c r="G257">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="H257" s="2">
         <v>45247</v>
       </c>
       <c r="I257">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="J257" t="inlineStr">
         <is>
@@ -26473,7 +26461,7 @@
         <v>45254</v>
       </c>
       <c r="I258">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="J258" t="inlineStr">
         <is>
@@ -26570,7 +26558,7 @@
         <v>45486</v>
       </c>
       <c r="I259">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="J259" t="inlineStr">
         <is>
@@ -26662,13 +26650,13 @@
         <v>45073</v>
       </c>
       <c r="G260">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="H260" s="2">
         <v>45439</v>
       </c>
       <c r="I260">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="J260" t="inlineStr">
         <is>
@@ -26760,7 +26748,7 @@
         <v>45323</v>
       </c>
       <c r="I261">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="J261" t="inlineStr">
         <is>
@@ -26852,7 +26840,7 @@
         <v>45303</v>
       </c>
       <c r="I262">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="J262" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
Bond dates update Sat Oct  7 23:15:24 UTC 2023
</commit_message>
<xml_diff>
--- a/Data/obligacje_screener.xlsx
+++ b/Data/obligacje_screener.xlsx
@@ -512,7 +512,7 @@
         <v>45340</v>
       </c>
       <c r="I2">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="J2" t="inlineStr">
         <is>
@@ -600,13 +600,13 @@
         <v>45121</v>
       </c>
       <c r="G3">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="H3" s="2">
         <v>45305</v>
       </c>
       <c r="I3">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="J3" t="inlineStr">
         <is>
@@ -703,13 +703,13 @@
         <v>45039</v>
       </c>
       <c r="G4">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="H4" s="2">
         <v>45222</v>
       </c>
       <c r="I4">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="J4" t="inlineStr">
         <is>
@@ -806,13 +806,13 @@
         <v>45039</v>
       </c>
       <c r="G5">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="H5" s="2">
         <v>45222</v>
       </c>
       <c r="I5">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="J5" t="inlineStr">
         <is>
@@ -909,13 +909,13 @@
         <v>45129</v>
       </c>
       <c r="G6">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="H6" s="2">
         <v>45221</v>
       </c>
       <c r="I6">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="J6" t="inlineStr">
         <is>
@@ -1012,13 +1012,13 @@
         <v>45162</v>
       </c>
       <c r="G7">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="H7" s="2">
         <v>45254</v>
       </c>
       <c r="I7">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="J7" t="inlineStr">
         <is>
@@ -1110,13 +1110,13 @@
         <v>45156</v>
       </c>
       <c r="G8">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="H8" s="2">
         <v>45248</v>
       </c>
       <c r="I8">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="J8" t="inlineStr">
         <is>
@@ -1213,13 +1213,13 @@
         <v>45141</v>
       </c>
       <c r="G9">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="H9" s="2">
         <v>45233</v>
       </c>
       <c r="I9">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="J9" t="inlineStr">
         <is>
@@ -1316,13 +1316,13 @@
         <v>45062</v>
       </c>
       <c r="G10">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="H10" s="2">
         <v>45246</v>
       </c>
       <c r="I10">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="J10" t="inlineStr">
         <is>
@@ -1419,7 +1419,7 @@
         <v>45286</v>
       </c>
       <c r="I11">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="J11" t="inlineStr">
         <is>
@@ -1516,13 +1516,13 @@
         <v>45195</v>
       </c>
       <c r="G12">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="H12" s="2">
         <v>45377</v>
       </c>
       <c r="I12">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="J12" t="inlineStr">
         <is>
@@ -1614,13 +1614,13 @@
         <v>45036</v>
       </c>
       <c r="G13">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="H13" s="2">
         <v>45219</v>
       </c>
       <c r="I13">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="J13" t="inlineStr">
         <is>
@@ -1717,13 +1717,13 @@
         <v>45036</v>
       </c>
       <c r="G14">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="H14" s="2">
         <v>45219</v>
       </c>
       <c r="I14">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="J14" t="inlineStr">
         <is>
@@ -1820,13 +1820,13 @@
         <v>45106</v>
       </c>
       <c r="G15">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="H15" s="2">
         <v>45289</v>
       </c>
       <c r="I15">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="J15" t="inlineStr">
         <is>
@@ -1923,13 +1923,13 @@
         <v>45186</v>
       </c>
       <c r="G16">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="H16" s="2">
         <v>45278</v>
       </c>
       <c r="I16">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="J16" t="inlineStr">
         <is>
@@ -2026,13 +2026,13 @@
         <v>45186</v>
       </c>
       <c r="G17">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="H17" s="2">
         <v>45277</v>
       </c>
       <c r="I17">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="J17" t="inlineStr">
         <is>
@@ -2129,13 +2129,13 @@
         <v>45132</v>
       </c>
       <c r="G18">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="H18" s="2">
         <v>45224</v>
       </c>
       <c r="I18">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="J18" t="inlineStr">
         <is>
@@ -2232,13 +2232,13 @@
         <v>45137</v>
       </c>
       <c r="G19">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="H19" s="2">
         <v>45229</v>
       </c>
       <c r="I19">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="J19" t="inlineStr">
         <is>
@@ -2330,13 +2330,13 @@
         <v>45183</v>
       </c>
       <c r="G20">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="H20" s="2">
         <v>45274</v>
       </c>
       <c r="I20">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="J20" t="inlineStr">
         <is>
@@ -2433,13 +2433,13 @@
         <v>45187</v>
       </c>
       <c r="G21">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="H21" s="2">
         <v>45278</v>
       </c>
       <c r="I21">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="J21" t="inlineStr">
         <is>
@@ -2536,13 +2536,13 @@
         <v>45187</v>
       </c>
       <c r="G22">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="H22" s="2">
         <v>45278</v>
       </c>
       <c r="I22">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="J22" t="inlineStr">
         <is>
@@ -2639,7 +2639,7 @@
         <v>45245</v>
       </c>
       <c r="I23">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="J23" t="inlineStr">
         <is>
@@ -2736,7 +2736,7 @@
         <v>45245</v>
       </c>
       <c r="I24">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="J24" t="inlineStr">
         <is>
@@ -2833,7 +2833,7 @@
         <v>45204</v>
       </c>
       <c r="G25">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J25" t="inlineStr">
         <is>
@@ -2930,13 +2930,13 @@
         <v>45160</v>
       </c>
       <c r="G26">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="H26" s="2">
         <v>45344</v>
       </c>
       <c r="I26">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="J26" t="inlineStr">
         <is>
@@ -3033,13 +3033,13 @@
         <v>45118</v>
       </c>
       <c r="G27">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="H27" s="2">
         <v>45302</v>
       </c>
       <c r="I27">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="J27" t="inlineStr">
         <is>
@@ -3136,13 +3136,13 @@
         <v>45085</v>
       </c>
       <c r="G28">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="H28" s="2">
         <v>45268</v>
       </c>
       <c r="I28">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="J28" t="inlineStr">
         <is>
@@ -3239,13 +3239,13 @@
         <v>45183</v>
       </c>
       <c r="G29">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="H29" s="2">
         <v>45274</v>
       </c>
       <c r="I29">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="J29" t="inlineStr">
         <is>
@@ -3342,7 +3342,7 @@
         <v>45224</v>
       </c>
       <c r="I30">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="J30" t="inlineStr">
         <is>
@@ -3439,13 +3439,13 @@
         <v>45153</v>
       </c>
       <c r="G31">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="H31" s="2">
         <v>45245</v>
       </c>
       <c r="I31">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="J31" t="inlineStr">
         <is>
@@ -3542,13 +3542,13 @@
         <v>45155</v>
       </c>
       <c r="G32">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="H32" s="2">
         <v>45247</v>
       </c>
       <c r="I32">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="J32" t="inlineStr">
         <is>
@@ -3645,7 +3645,7 @@
         <v>45255</v>
       </c>
       <c r="I33">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="J33" t="inlineStr">
         <is>
@@ -3733,13 +3733,13 @@
         <v>45176</v>
       </c>
       <c r="G34">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="H34" s="2">
         <v>45267</v>
       </c>
       <c r="I34">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="J34" t="inlineStr">
         <is>
@@ -3836,13 +3836,13 @@
         <v>45130</v>
       </c>
       <c r="G35">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="H35" s="2">
         <v>45222</v>
       </c>
       <c r="I35">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="J35" t="inlineStr">
         <is>
@@ -3934,13 +3934,13 @@
         <v>45115</v>
       </c>
       <c r="G36">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="H36" s="2">
         <v>45207</v>
       </c>
       <c r="I36">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J36" t="inlineStr">
         <is>
@@ -4037,13 +4037,13 @@
         <v>45189</v>
       </c>
       <c r="G37">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="H37" s="2">
         <v>45280</v>
       </c>
       <c r="I37">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="J37" t="inlineStr">
         <is>
@@ -4135,13 +4135,13 @@
         <v>45107</v>
       </c>
       <c r="G38">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="H38" s="2">
         <v>45290</v>
       </c>
       <c r="I38">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="J38" t="inlineStr">
         <is>
@@ -4238,13 +4238,13 @@
         <v>45063</v>
       </c>
       <c r="G39">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="H39" s="2">
         <v>45247</v>
       </c>
       <c r="I39">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="J39" t="inlineStr">
         <is>
@@ -4341,13 +4341,13 @@
         <v>45177</v>
       </c>
       <c r="G40">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="H40" s="2">
         <v>45359</v>
       </c>
       <c r="I40">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="J40" t="inlineStr">
         <is>
@@ -4444,13 +4444,13 @@
         <v>45107</v>
       </c>
       <c r="G41">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="H41" s="2">
         <v>45290</v>
       </c>
       <c r="I41">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="J41" t="inlineStr">
         <is>
@@ -4547,7 +4547,7 @@
         <v>45265</v>
       </c>
       <c r="I42">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="J42" t="inlineStr">
         <is>
@@ -4644,13 +4644,13 @@
         <v>45098</v>
       </c>
       <c r="G43">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="H43" s="2">
         <v>45281</v>
       </c>
       <c r="I43">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="J43" t="inlineStr">
         <is>
@@ -4747,13 +4747,13 @@
         <v>45099</v>
       </c>
       <c r="G44">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="H44" s="2">
         <v>45282</v>
       </c>
       <c r="I44">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="J44" t="inlineStr">
         <is>
@@ -4850,13 +4850,13 @@
         <v>45106</v>
       </c>
       <c r="G45">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="H45" s="2">
         <v>45289</v>
       </c>
       <c r="I45">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="J45" t="inlineStr">
         <is>
@@ -4953,13 +4953,13 @@
         <v>45106</v>
       </c>
       <c r="G46">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="H46" s="2">
         <v>45289</v>
       </c>
       <c r="I46">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="J46" t="inlineStr">
         <is>
@@ -5056,13 +5056,13 @@
         <v>45120</v>
       </c>
       <c r="G47">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="H47" s="2">
         <v>45304</v>
       </c>
       <c r="I47">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="J47" t="inlineStr">
         <is>
@@ -5159,13 +5159,13 @@
         <v>45118</v>
       </c>
       <c r="G48">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="H48" s="2">
         <v>45302</v>
       </c>
       <c r="I48">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="J48" t="inlineStr">
         <is>
@@ -5262,13 +5262,13 @@
         <v>45152</v>
       </c>
       <c r="G49">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="H49" s="2">
         <v>45336</v>
       </c>
       <c r="I49">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="J49" t="inlineStr">
         <is>
@@ -5365,13 +5365,13 @@
         <v>45042</v>
       </c>
       <c r="G50">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="H50" s="2">
         <v>45225</v>
       </c>
       <c r="I50">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="J50" t="inlineStr">
         <is>
@@ -5468,13 +5468,13 @@
         <v>45122</v>
       </c>
       <c r="G51">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="H51" s="2">
         <v>45306</v>
       </c>
       <c r="I51">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="J51" t="inlineStr">
         <is>
@@ -5571,13 +5571,13 @@
         <v>45139</v>
       </c>
       <c r="G52">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="H52" s="2">
         <v>45323</v>
       </c>
       <c r="I52">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="J52" t="inlineStr">
         <is>
@@ -5665,13 +5665,13 @@
         <v>45099</v>
       </c>
       <c r="G53">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="H53" s="2">
         <v>45282</v>
       </c>
       <c r="I53">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="J53" t="inlineStr">
         <is>
@@ -5768,13 +5768,13 @@
         <v>45196</v>
       </c>
       <c r="G54">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="H54" s="2">
         <v>45287</v>
       </c>
       <c r="I54">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="J54" t="inlineStr">
         <is>
@@ -5871,13 +5871,13 @@
         <v>45044</v>
       </c>
       <c r="G55">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="H55" s="2">
         <v>45227</v>
       </c>
       <c r="I55">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="J55" t="inlineStr">
         <is>
@@ -5974,13 +5974,13 @@
         <v>45151</v>
       </c>
       <c r="G56">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="H56" s="2">
         <v>45243</v>
       </c>
       <c r="I56">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="J56" t="inlineStr">
         <is>
@@ -6072,13 +6072,13 @@
         <v>45196</v>
       </c>
       <c r="G57">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="H57" s="2">
         <v>45287</v>
       </c>
       <c r="I57">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="J57" t="inlineStr">
         <is>
@@ -6175,13 +6175,13 @@
         <v>45069</v>
       </c>
       <c r="G58">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="H58" s="2">
         <v>45253</v>
       </c>
       <c r="I58">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="J58" t="inlineStr">
         <is>
@@ -6278,13 +6278,13 @@
         <v>45191</v>
       </c>
       <c r="G59">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="H59" s="2">
         <v>45282</v>
       </c>
       <c r="I59">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="J59" t="inlineStr">
         <is>
@@ -6373,10 +6373,10 @@
         </is>
       </c>
       <c r="F60" s="2">
-        <v>45113</v>
+        <v>45205</v>
       </c>
       <c r="G60">
-        <v>92</v>
+        <v>1</v>
       </c>
       <c r="J60" t="inlineStr">
         <is>
@@ -6473,13 +6473,13 @@
         <v>45127</v>
       </c>
       <c r="G61">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="H61" s="2">
         <v>45219</v>
       </c>
       <c r="I61">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="J61" t="inlineStr">
         <is>
@@ -6576,13 +6576,13 @@
         <v>45058</v>
       </c>
       <c r="G62">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="H62" s="2">
         <v>45242</v>
       </c>
       <c r="I62">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="J62" t="inlineStr">
         <is>
@@ -6679,13 +6679,13 @@
         <v>45194</v>
       </c>
       <c r="G63">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="H63" s="2">
         <v>45376</v>
       </c>
       <c r="I63">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="J63" t="inlineStr">
         <is>
@@ -6777,13 +6777,13 @@
         <v>45025</v>
       </c>
       <c r="G64">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="H64" s="2">
         <v>45208</v>
       </c>
       <c r="I64">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="J64" t="inlineStr">
         <is>
@@ -6880,13 +6880,13 @@
         <v>45025</v>
       </c>
       <c r="G65">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="H65" s="2">
         <v>45208</v>
       </c>
       <c r="I65">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="J65" t="inlineStr">
         <is>
@@ -6983,13 +6983,13 @@
         <v>45089</v>
       </c>
       <c r="G66">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="H66" s="2">
         <v>45272</v>
       </c>
       <c r="I66">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="J66" t="inlineStr">
         <is>
@@ -7086,13 +7086,13 @@
         <v>45178</v>
       </c>
       <c r="G67">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="H67" s="2">
         <v>45269</v>
       </c>
       <c r="I67">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="J67" t="inlineStr">
         <is>
@@ -7184,13 +7184,13 @@
         <v>45196</v>
       </c>
       <c r="G68">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="H68" s="2">
         <v>45287</v>
       </c>
       <c r="I68">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="J68" t="inlineStr">
         <is>
@@ -7287,13 +7287,13 @@
         <v>45149</v>
       </c>
       <c r="G69">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="H69" s="2">
         <v>45241</v>
       </c>
       <c r="I69">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="J69" t="inlineStr">
         <is>
@@ -7386,11 +7386,17 @@
           <t>1 000,00</t>
         </is>
       </c>
+      <c r="F70" s="2">
+        <v>45205</v>
+      </c>
+      <c r="G70">
+        <v>1</v>
+      </c>
       <c r="H70" s="2">
         <v>45296</v>
       </c>
       <c r="I70">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="J70" t="inlineStr">
         <is>
@@ -7484,10 +7490,10 @@
         </is>
       </c>
       <c r="F71" s="2">
-        <v>45114</v>
+        <v>45205</v>
       </c>
       <c r="G71">
-        <v>91</v>
+        <v>1</v>
       </c>
       <c r="J71" t="inlineStr">
         <is>
@@ -7584,13 +7590,13 @@
         <v>45115</v>
       </c>
       <c r="G72">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="H72" s="2">
         <v>45207</v>
       </c>
       <c r="I72">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J72" t="inlineStr">
         <is>
@@ -7687,13 +7693,13 @@
         <v>45189</v>
       </c>
       <c r="G73">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="H73" s="2">
         <v>45280</v>
       </c>
       <c r="I73">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="J73" t="inlineStr">
         <is>
@@ -7785,13 +7791,13 @@
         <v>45038</v>
       </c>
       <c r="G74">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="H74" s="2">
         <v>45221</v>
       </c>
       <c r="I74">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="J74" t="inlineStr">
         <is>
@@ -7883,13 +7889,13 @@
         <v>45117</v>
       </c>
       <c r="G75">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="H75" s="2">
         <v>45301</v>
       </c>
       <c r="I75">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="J75" t="inlineStr">
         <is>
@@ -7986,13 +7992,13 @@
         <v>45160</v>
       </c>
       <c r="G76">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="H76" s="2">
         <v>45344</v>
       </c>
       <c r="I76">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="J76" t="inlineStr">
         <is>
@@ -8089,13 +8095,13 @@
         <v>45186</v>
       </c>
       <c r="G77">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="H77" s="2">
         <v>45368</v>
       </c>
       <c r="I77">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="J77" t="inlineStr">
         <is>
@@ -8192,13 +8198,13 @@
         <v>45043</v>
       </c>
       <c r="G78">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="H78" s="2">
         <v>45226</v>
       </c>
       <c r="I78">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="J78" t="inlineStr">
         <is>
@@ -8295,13 +8301,13 @@
         <v>45079</v>
       </c>
       <c r="G79">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="H79" s="2">
         <v>45262</v>
       </c>
       <c r="I79">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="J79" t="inlineStr">
         <is>
@@ -8398,7 +8404,7 @@
         <v>45254</v>
       </c>
       <c r="I80">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="J80" t="inlineStr">
         <is>
@@ -8495,13 +8501,13 @@
         <v>45104</v>
       </c>
       <c r="G81">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="H81" s="2">
         <v>45287</v>
       </c>
       <c r="I81">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="J81" t="inlineStr">
         <is>
@@ -8598,7 +8604,7 @@
         <v>45288</v>
       </c>
       <c r="I82">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="J82" t="inlineStr">
         <is>
@@ -8690,13 +8696,13 @@
         <v>45175</v>
       </c>
       <c r="G83">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="H83" s="2">
         <v>45357</v>
       </c>
       <c r="I83">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="J83" t="inlineStr">
         <is>
@@ -8793,13 +8799,13 @@
         <v>45054</v>
       </c>
       <c r="G84">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="H84" s="2">
         <v>45238</v>
       </c>
       <c r="I84">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="J84" t="inlineStr">
         <is>
@@ -8896,13 +8902,13 @@
         <v>45056</v>
       </c>
       <c r="G85">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="H85" s="2">
         <v>45240</v>
       </c>
       <c r="I85">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="J85" t="inlineStr">
         <is>
@@ -8999,13 +9005,13 @@
         <v>45085</v>
       </c>
       <c r="G86">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="H86" s="2">
         <v>45268</v>
       </c>
       <c r="I86">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="J86" t="inlineStr">
         <is>
@@ -9102,13 +9108,13 @@
         <v>45194</v>
       </c>
       <c r="G87">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="H87" s="2">
         <v>45560</v>
       </c>
       <c r="I87">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="J87" t="inlineStr">
         <is>
@@ -9195,13 +9201,13 @@
         <v>45103</v>
       </c>
       <c r="G88">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="H88" s="2">
         <v>45286</v>
       </c>
       <c r="I88">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="J88" t="inlineStr">
         <is>
@@ -9298,13 +9304,13 @@
         <v>45103</v>
       </c>
       <c r="G89">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="H89" s="2">
         <v>45286</v>
       </c>
       <c r="I89">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="J89" t="inlineStr">
         <is>
@@ -9401,13 +9407,13 @@
         <v>45192</v>
       </c>
       <c r="G90">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="H90" s="2">
         <v>45374</v>
       </c>
       <c r="I90">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="J90" t="inlineStr">
         <is>
@@ -9499,13 +9505,13 @@
         <v>45100</v>
       </c>
       <c r="G91">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="H91" s="2">
         <v>45287</v>
       </c>
       <c r="I91">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="J91" t="inlineStr">
         <is>
@@ -9602,13 +9608,13 @@
         <v>45187</v>
       </c>
       <c r="G92">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="H92" s="2">
         <v>45369</v>
       </c>
       <c r="I92">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="J92" t="inlineStr">
         <is>
@@ -9705,13 +9711,13 @@
         <v>45104</v>
       </c>
       <c r="G93">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="H93" s="2">
         <v>45287</v>
       </c>
       <c r="I93">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="J93" t="inlineStr">
         <is>
@@ -9808,13 +9814,13 @@
         <v>45104</v>
       </c>
       <c r="G94">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="H94" s="2">
         <v>45287</v>
       </c>
       <c r="I94">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="J94" t="inlineStr">
         <is>
@@ -9911,13 +9917,13 @@
         <v>45049</v>
       </c>
       <c r="G95">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="H95" s="2">
         <v>45233</v>
       </c>
       <c r="I95">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="J95" t="inlineStr">
         <is>
@@ -10014,13 +10020,13 @@
         <v>45122</v>
       </c>
       <c r="G96">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="H96" s="2">
         <v>45306</v>
       </c>
       <c r="I96">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="J96" t="inlineStr">
         <is>
@@ -10112,13 +10118,13 @@
         <v>45141</v>
       </c>
       <c r="G97">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="H97" s="2">
         <v>45325</v>
       </c>
       <c r="I97">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="J97" t="inlineStr">
         <is>
@@ -10215,13 +10221,13 @@
         <v>45194</v>
       </c>
       <c r="G98">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="H98" s="2">
         <v>45376</v>
       </c>
       <c r="I98">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="J98" t="inlineStr">
         <is>
@@ -10313,13 +10319,13 @@
         <v>45093</v>
       </c>
       <c r="G99">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="H99" s="2">
         <v>45276</v>
       </c>
       <c r="I99">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="J99" t="inlineStr">
         <is>
@@ -10416,13 +10422,13 @@
         <v>45123</v>
       </c>
       <c r="G100">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="H100" s="2">
         <v>45307</v>
       </c>
       <c r="I100">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="J100" t="inlineStr">
         <is>
@@ -10519,13 +10525,13 @@
         <v>45198</v>
       </c>
       <c r="G101">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="H101" s="2">
         <v>45380</v>
       </c>
       <c r="I101">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="J101" t="inlineStr">
         <is>
@@ -10622,13 +10628,13 @@
         <v>45093</v>
       </c>
       <c r="G102">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="H102" s="2">
         <v>45276</v>
       </c>
       <c r="I102">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="J102" t="inlineStr">
         <is>
@@ -10725,13 +10731,13 @@
         <v>45122</v>
       </c>
       <c r="G103">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="H103" s="2">
         <v>45306</v>
       </c>
       <c r="I103">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="J103" t="inlineStr">
         <is>
@@ -10828,13 +10834,13 @@
         <v>45122</v>
       </c>
       <c r="G104">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="H104" s="2">
         <v>45306</v>
       </c>
       <c r="I104">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="J104" t="inlineStr">
         <is>
@@ -10926,13 +10932,13 @@
         <v>45050</v>
       </c>
       <c r="G105">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="H105" s="2">
         <v>45234</v>
       </c>
       <c r="I105">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="J105" t="inlineStr">
         <is>
@@ -11029,13 +11035,13 @@
         <v>45085</v>
       </c>
       <c r="G106">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="H106" s="2">
         <v>45268</v>
       </c>
       <c r="I106">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="J106" t="inlineStr">
         <is>
@@ -11132,13 +11138,13 @@
         <v>45185</v>
       </c>
       <c r="G107">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="H107" s="2">
         <v>45276</v>
       </c>
       <c r="I107">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="J107" t="inlineStr">
         <is>
@@ -11230,13 +11236,13 @@
         <v>45185</v>
       </c>
       <c r="G108">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="H108" s="2">
         <v>45276</v>
       </c>
       <c r="I108">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="J108" t="inlineStr">
         <is>
@@ -11328,13 +11334,13 @@
         <v>45185</v>
       </c>
       <c r="G109">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="H109" s="2">
         <v>45276</v>
       </c>
       <c r="I109">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="J109" t="inlineStr">
         <is>
@@ -11431,13 +11437,13 @@
         <v>45148</v>
       </c>
       <c r="G110">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="H110" s="2">
         <v>45240</v>
       </c>
       <c r="I110">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="J110" t="inlineStr">
         <is>
@@ -11534,13 +11540,13 @@
         <v>45119</v>
       </c>
       <c r="G111">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="H111" s="2">
         <v>45211</v>
       </c>
       <c r="I111">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="J111" t="inlineStr">
         <is>
@@ -11637,13 +11643,13 @@
         <v>45172</v>
       </c>
       <c r="G112">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="H112" s="2">
         <v>45263</v>
       </c>
       <c r="I112">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="J112" t="inlineStr">
         <is>
@@ -11740,13 +11746,13 @@
         <v>45023</v>
       </c>
       <c r="G113">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="H113" s="2">
-        <v>45206</v>
+        <v>45389</v>
       </c>
       <c r="I113">
-        <v>1</v>
+        <v>183</v>
       </c>
       <c r="J113" t="inlineStr">
         <is>
@@ -11843,13 +11849,13 @@
         <v>45203</v>
       </c>
       <c r="G114">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H114" s="2">
         <v>45295</v>
       </c>
       <c r="I114">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="J114" t="inlineStr">
         <is>
@@ -11946,7 +11952,7 @@
         <v>45218</v>
       </c>
       <c r="I115">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="J115" t="inlineStr">
         <is>
@@ -12043,13 +12049,13 @@
         <v>45161</v>
       </c>
       <c r="G116">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="H116" s="2">
         <v>45253</v>
       </c>
       <c r="I116">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="J116" t="inlineStr">
         <is>
@@ -12146,13 +12152,13 @@
         <v>45115</v>
       </c>
       <c r="G117">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="H117" s="2">
         <v>45299</v>
       </c>
       <c r="I117">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="J117" t="inlineStr">
         <is>
@@ -12244,13 +12250,13 @@
         <v>45094</v>
       </c>
       <c r="G118">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="H118" s="2">
         <v>45277</v>
       </c>
       <c r="I118">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="J118" t="inlineStr">
         <is>
@@ -12347,13 +12353,13 @@
         <v>45104</v>
       </c>
       <c r="G119">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="H119" s="2">
         <v>45287</v>
       </c>
       <c r="I119">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="J119" t="inlineStr">
         <is>
@@ -12450,13 +12456,13 @@
         <v>45104</v>
       </c>
       <c r="G120">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="H120" s="2">
         <v>45287</v>
       </c>
       <c r="I120">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="J120" t="inlineStr">
         <is>
@@ -12553,13 +12559,13 @@
         <v>45104</v>
       </c>
       <c r="G121">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="H121" s="2">
         <v>45287</v>
       </c>
       <c r="I121">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="J121" t="inlineStr">
         <is>
@@ -12656,13 +12662,13 @@
         <v>45104</v>
       </c>
       <c r="G122">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="H122" s="2">
         <v>45287</v>
       </c>
       <c r="I122">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="J122" t="inlineStr">
         <is>
@@ -12759,13 +12765,13 @@
         <v>45199</v>
       </c>
       <c r="G123">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="H123" s="2">
         <v>45291</v>
       </c>
       <c r="I123">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="J123" t="inlineStr">
         <is>
@@ -12862,13 +12868,13 @@
         <v>45197</v>
       </c>
       <c r="G124">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="H124" s="2">
         <v>45379</v>
       </c>
       <c r="I124">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="J124" t="inlineStr">
         <is>
@@ -12965,13 +12971,13 @@
         <v>45121</v>
       </c>
       <c r="G125">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="H125" s="2">
         <v>45213</v>
       </c>
       <c r="I125">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="J125" t="inlineStr">
         <is>
@@ -13068,13 +13074,13 @@
         <v>45134</v>
       </c>
       <c r="G126">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="H126" s="2">
         <v>45226</v>
       </c>
       <c r="I126">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="J126" t="inlineStr">
         <is>
@@ -13171,7 +13177,7 @@
         <v>45212</v>
       </c>
       <c r="I127">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="J127" t="inlineStr">
         <is>
@@ -13268,13 +13274,13 @@
         <v>45126</v>
       </c>
       <c r="G128">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="H128" s="2">
         <v>45218</v>
       </c>
       <c r="I128">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="J128" t="inlineStr">
         <is>
@@ -13366,13 +13372,13 @@
         <v>45158</v>
       </c>
       <c r="G129">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="H129" s="2">
         <v>45250</v>
       </c>
       <c r="I129">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="J129" t="inlineStr">
         <is>
@@ -13469,13 +13475,13 @@
         <v>45171</v>
       </c>
       <c r="G130">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="H130" s="2">
         <v>45262</v>
       </c>
       <c r="I130">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="J130" t="inlineStr">
         <is>
@@ -13572,13 +13578,13 @@
         <v>45203</v>
       </c>
       <c r="G131">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H131" s="2">
         <v>45295</v>
       </c>
       <c r="I131">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="J131" t="inlineStr">
         <is>
@@ -13675,13 +13681,13 @@
         <v>45144</v>
       </c>
       <c r="G132">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="H132" s="2">
         <v>45236</v>
       </c>
       <c r="I132">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="J132" t="inlineStr">
         <is>
@@ -13778,13 +13784,13 @@
         <v>45156</v>
       </c>
       <c r="G133">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="H133" s="2">
         <v>45248</v>
       </c>
       <c r="I133">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="J133" t="inlineStr">
         <is>
@@ -13876,13 +13882,13 @@
         <v>45146</v>
       </c>
       <c r="G134">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="H134" s="2">
         <v>45238</v>
       </c>
       <c r="I134">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="J134" t="inlineStr">
         <is>
@@ -13979,13 +13985,13 @@
         <v>45140</v>
       </c>
       <c r="G135">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="H135" s="2">
         <v>45232</v>
       </c>
       <c r="I135">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="J135" t="inlineStr">
         <is>
@@ -14082,13 +14088,13 @@
         <v>45196</v>
       </c>
       <c r="G136">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="H136" s="2">
         <v>45287</v>
       </c>
       <c r="I136">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="J136" t="inlineStr">
         <is>
@@ -14185,13 +14191,13 @@
         <v>45197</v>
       </c>
       <c r="G137">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="H137" s="2">
         <v>45288</v>
       </c>
       <c r="I137">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="J137" t="inlineStr">
         <is>
@@ -14288,13 +14294,13 @@
         <v>45179</v>
       </c>
       <c r="G138">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="H138" s="2">
         <v>45270</v>
       </c>
       <c r="I138">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="J138" t="inlineStr">
         <is>
@@ -14386,13 +14392,13 @@
         <v>45197</v>
       </c>
       <c r="G139">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="H139" s="2">
         <v>45288</v>
       </c>
       <c r="I139">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="J139" t="inlineStr">
         <is>
@@ -14489,13 +14495,13 @@
         <v>45182</v>
       </c>
       <c r="G140">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="H140" s="2">
         <v>45273</v>
       </c>
       <c r="I140">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="J140" t="inlineStr">
         <is>
@@ -14592,13 +14598,13 @@
         <v>45116</v>
       </c>
       <c r="G141">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="H141" s="2">
         <v>45208</v>
       </c>
       <c r="I141">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="J141" t="inlineStr">
         <is>
@@ -14690,13 +14696,13 @@
         <v>45150</v>
       </c>
       <c r="G142">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="H142" s="2">
         <v>45242</v>
       </c>
       <c r="I142">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="J142" t="inlineStr">
         <is>
@@ -14793,7 +14799,7 @@
         <v>45238</v>
       </c>
       <c r="I143">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="J143" t="inlineStr">
         <is>
@@ -14890,13 +14896,13 @@
         <v>45171</v>
       </c>
       <c r="G144">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="H144" s="2">
         <v>45262</v>
       </c>
       <c r="I144">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="J144" t="inlineStr">
         <is>
@@ -14993,13 +14999,13 @@
         <v>45194</v>
       </c>
       <c r="G145">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="H145" s="2">
         <v>45285</v>
       </c>
       <c r="I145">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="J145" t="inlineStr">
         <is>
@@ -15086,13 +15092,13 @@
         <v>45119</v>
       </c>
       <c r="G146">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="H146" s="2">
         <v>45211</v>
       </c>
       <c r="I146">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="J146" t="inlineStr">
         <is>
@@ -15189,13 +15195,13 @@
         <v>45165</v>
       </c>
       <c r="G147">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="H147" s="2">
         <v>45257</v>
       </c>
       <c r="I147">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="J147" t="inlineStr">
         <is>
@@ -15292,13 +15298,13 @@
         <v>45166</v>
       </c>
       <c r="G148">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="H148" s="2">
         <v>45258</v>
       </c>
       <c r="I148">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="J148" t="inlineStr">
         <is>
@@ -15395,13 +15401,13 @@
         <v>45185</v>
       </c>
       <c r="G149">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="H149" s="2">
         <v>45276</v>
       </c>
       <c r="I149">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="J149" t="inlineStr">
         <is>
@@ -15498,13 +15504,13 @@
         <v>45035</v>
       </c>
       <c r="G150">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="H150" s="2">
         <v>45218</v>
       </c>
       <c r="I150">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="J150" t="inlineStr">
         <is>
@@ -15601,13 +15607,13 @@
         <v>45174</v>
       </c>
       <c r="G151">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="H151" s="2">
         <v>45356</v>
       </c>
       <c r="I151">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="J151" t="inlineStr">
         <is>
@@ -15704,13 +15710,13 @@
         <v>45089</v>
       </c>
       <c r="G152">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="H152" s="2">
         <v>45272</v>
       </c>
       <c r="I152">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="J152" t="inlineStr">
         <is>
@@ -15807,13 +15813,13 @@
         <v>45124</v>
       </c>
       <c r="G153">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="H153" s="2">
         <v>45308</v>
       </c>
       <c r="I153">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="J153" t="inlineStr">
         <is>
@@ -15910,13 +15916,13 @@
         <v>45124</v>
       </c>
       <c r="G154">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="H154" s="2">
         <v>45308</v>
       </c>
       <c r="I154">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="J154" t="inlineStr">
         <is>
@@ -16013,13 +16019,13 @@
         <v>45026</v>
       </c>
       <c r="G155">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="H155" s="2">
         <v>45209</v>
       </c>
       <c r="I155">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="J155" t="inlineStr">
         <is>
@@ -16116,13 +16122,13 @@
         <v>45026</v>
       </c>
       <c r="G156">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="H156" s="2">
         <v>45209</v>
       </c>
       <c r="I156">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="J156" t="inlineStr">
         <is>
@@ -16219,13 +16225,13 @@
         <v>45026</v>
       </c>
       <c r="G157">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="H157" s="2">
         <v>45209</v>
       </c>
       <c r="I157">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="J157" t="inlineStr">
         <is>
@@ -16322,13 +16328,13 @@
         <v>45026</v>
       </c>
       <c r="G158">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="H158" s="2">
         <v>45209</v>
       </c>
       <c r="I158">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="J158" t="inlineStr">
         <is>
@@ -16425,13 +16431,13 @@
         <v>45156</v>
       </c>
       <c r="G159">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="H159" s="2">
         <v>45247</v>
       </c>
       <c r="I159">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="J159" t="inlineStr">
         <is>
@@ -16528,13 +16534,13 @@
         <v>45153</v>
       </c>
       <c r="G160">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="H160" s="2">
         <v>45245</v>
       </c>
       <c r="I160">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="J160" t="inlineStr">
         <is>
@@ -16631,13 +16637,13 @@
         <v>45135</v>
       </c>
       <c r="G161">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="H161" s="2">
         <v>45319</v>
       </c>
       <c r="I161">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="J161" t="inlineStr">
         <is>
@@ -16734,13 +16740,13 @@
         <v>45091</v>
       </c>
       <c r="G162">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="H162" s="2">
         <v>45274</v>
       </c>
       <c r="I162">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="J162" t="inlineStr">
         <is>
@@ -16832,13 +16838,13 @@
         <v>45091</v>
       </c>
       <c r="G163">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="H163" s="2">
         <v>45274</v>
       </c>
       <c r="I163">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="J163" t="inlineStr">
         <is>
@@ -16930,13 +16936,13 @@
         <v>45138</v>
       </c>
       <c r="G164">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="H164" s="2">
         <v>45322</v>
       </c>
       <c r="I164">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="J164" t="inlineStr">
         <is>
@@ -17033,13 +17039,13 @@
         <v>45138</v>
       </c>
       <c r="G165">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="H165" s="2">
         <v>45322</v>
       </c>
       <c r="I165">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="J165" t="inlineStr">
         <is>
@@ -17136,13 +17142,13 @@
         <v>45085</v>
       </c>
       <c r="G166">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="H166" s="2">
         <v>45268</v>
       </c>
       <c r="I166">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="J166" t="inlineStr">
         <is>
@@ -17239,13 +17245,13 @@
         <v>45085</v>
       </c>
       <c r="G167">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="H167" s="2">
         <v>45268</v>
       </c>
       <c r="I167">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="J167" t="inlineStr">
         <is>
@@ -17342,7 +17348,7 @@
         <v>45326</v>
       </c>
       <c r="I168">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="J168" t="inlineStr">
         <is>
@@ -17439,13 +17445,13 @@
         <v>45173</v>
       </c>
       <c r="G169">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="H169" s="2">
         <v>45355</v>
       </c>
       <c r="I169">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="J169" t="inlineStr">
         <is>
@@ -17542,13 +17548,13 @@
         <v>45056</v>
       </c>
       <c r="G170">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="H170" s="2">
         <v>45240</v>
       </c>
       <c r="I170">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="J170" t="inlineStr">
         <is>
@@ -17645,7 +17651,7 @@
         <v>45238</v>
       </c>
       <c r="I171">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="J171" t="inlineStr">
         <is>
@@ -17742,13 +17748,13 @@
         <v>45141</v>
       </c>
       <c r="G172">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="H172" s="2">
         <v>45325</v>
       </c>
       <c r="I172">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="J172" t="inlineStr">
         <is>
@@ -17845,13 +17851,13 @@
         <v>45037</v>
       </c>
       <c r="G173">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="H173" s="2">
         <v>45220</v>
       </c>
       <c r="I173">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="J173" t="inlineStr">
         <is>
@@ -17948,13 +17954,13 @@
         <v>45171</v>
       </c>
       <c r="G174">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="H174" s="2">
         <v>45262</v>
       </c>
       <c r="I174">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="J174" t="inlineStr">
         <is>
@@ -18051,13 +18057,13 @@
         <v>45197</v>
       </c>
       <c r="G175">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="H175" s="2">
         <v>45288</v>
       </c>
       <c r="I175">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="J175" t="inlineStr">
         <is>
@@ -18154,13 +18160,13 @@
         <v>45162</v>
       </c>
       <c r="G176">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="H176" s="2">
         <v>45254</v>
       </c>
       <c r="I176">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="J176" t="inlineStr">
         <is>
@@ -18257,13 +18263,13 @@
         <v>45061</v>
       </c>
       <c r="G177">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="H177" s="2">
         <v>45245</v>
       </c>
       <c r="I177">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="J177" t="inlineStr">
         <is>
@@ -18360,13 +18366,13 @@
         <v>45120</v>
       </c>
       <c r="G178">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="H178" s="2">
         <v>45212</v>
       </c>
       <c r="I178">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="J178" t="inlineStr">
         <is>
@@ -18463,13 +18469,13 @@
         <v>45191</v>
       </c>
       <c r="G179">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="H179" s="2">
         <v>45282</v>
       </c>
       <c r="I179">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="J179" t="inlineStr">
         <is>
@@ -18566,13 +18572,13 @@
         <v>45088</v>
       </c>
       <c r="G180">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="H180" s="2">
         <v>45271</v>
       </c>
       <c r="I180">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="J180" t="inlineStr">
         <is>
@@ -18669,13 +18675,13 @@
         <v>45192</v>
       </c>
       <c r="G181">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="H181" s="2">
         <v>45283</v>
       </c>
       <c r="I181">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="J181" t="inlineStr">
         <is>
@@ -18762,13 +18768,13 @@
         <v>45131</v>
       </c>
       <c r="G182">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="H182" s="2">
         <v>45223</v>
       </c>
       <c r="I182">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="J182" t="inlineStr">
         <is>
@@ -18860,13 +18866,13 @@
         <v>45136</v>
       </c>
       <c r="G183">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="H183" s="2">
         <v>45228</v>
       </c>
       <c r="I183">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="J183" t="inlineStr">
         <is>
@@ -18958,13 +18964,13 @@
         <v>45150</v>
       </c>
       <c r="G184">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="H184" s="2">
         <v>45242</v>
       </c>
       <c r="I184">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="J184" t="inlineStr">
         <is>
@@ -19056,13 +19062,13 @@
         <v>45118</v>
       </c>
       <c r="G185">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="H185" s="2">
         <v>45210</v>
       </c>
       <c r="I185">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="J185" t="inlineStr">
         <is>
@@ -19154,13 +19160,13 @@
         <v>45129</v>
       </c>
       <c r="G186">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="H186" s="2">
         <v>45221</v>
       </c>
       <c r="I186">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="J186" t="inlineStr">
         <is>
@@ -19252,13 +19258,13 @@
         <v>45189</v>
       </c>
       <c r="G187">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="H187" s="2">
         <v>45280</v>
       </c>
       <c r="I187">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="J187" t="inlineStr">
         <is>
@@ -19345,13 +19351,13 @@
         <v>45193</v>
       </c>
       <c r="G188">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="H188" s="2">
         <v>45284</v>
       </c>
       <c r="I188">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="J188" t="inlineStr">
         <is>
@@ -19438,13 +19444,13 @@
         <v>45165</v>
       </c>
       <c r="G189">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="H189" s="2">
         <v>45257</v>
       </c>
       <c r="I189">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="J189" t="inlineStr">
         <is>
@@ -19536,13 +19542,13 @@
         <v>45202</v>
       </c>
       <c r="G190">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="H190" s="2">
         <v>45385</v>
       </c>
       <c r="I190">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="J190" t="inlineStr">
         <is>
@@ -19639,13 +19645,13 @@
         <v>45081</v>
       </c>
       <c r="G191">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="H191" s="2">
         <v>45264</v>
       </c>
       <c r="I191">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="J191" t="inlineStr">
         <is>
@@ -19742,13 +19748,13 @@
         <v>45081</v>
       </c>
       <c r="G192">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="H192" s="2">
         <v>45264</v>
       </c>
       <c r="I192">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="J192" t="inlineStr">
         <is>
@@ -19845,7 +19851,7 @@
         <v>45319</v>
       </c>
       <c r="I193">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="J193" t="inlineStr">
         <is>
@@ -19942,7 +19948,7 @@
         <v>45319</v>
       </c>
       <c r="I194">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="J194" t="inlineStr">
         <is>
@@ -20034,13 +20040,13 @@
         <v>45046</v>
       </c>
       <c r="G195">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="H195" s="2">
         <v>45230</v>
       </c>
       <c r="I195">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="J195" t="inlineStr">
         <is>
@@ -20137,13 +20143,13 @@
         <v>45046</v>
       </c>
       <c r="G196">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="H196" s="2">
         <v>45230</v>
       </c>
       <c r="I196">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="J196" t="inlineStr">
         <is>
@@ -20240,13 +20246,13 @@
         <v>45031</v>
       </c>
       <c r="G197">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="H197" s="2">
         <v>45214</v>
       </c>
       <c r="I197">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="J197" t="inlineStr">
         <is>
@@ -20343,13 +20349,13 @@
         <v>45031</v>
       </c>
       <c r="G198">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="H198" s="2">
         <v>45214</v>
       </c>
       <c r="I198">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="J198" t="inlineStr">
         <is>
@@ -20446,13 +20452,13 @@
         <v>45031</v>
       </c>
       <c r="G199">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="H199" s="2">
         <v>45214</v>
       </c>
       <c r="I199">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="J199" t="inlineStr">
         <is>
@@ -20549,13 +20555,13 @@
         <v>45031</v>
       </c>
       <c r="G200">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="H200" s="2">
         <v>45214</v>
       </c>
       <c r="I200">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="J200" t="inlineStr">
         <is>
@@ -20652,13 +20658,13 @@
         <v>45067</v>
       </c>
       <c r="G201">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="H201" s="2">
         <v>45251</v>
       </c>
       <c r="I201">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="J201" t="inlineStr">
         <is>
@@ -20755,13 +20761,13 @@
         <v>45067</v>
       </c>
       <c r="G202">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="H202" s="2">
         <v>45251</v>
       </c>
       <c r="I202">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="J202" t="inlineStr">
         <is>
@@ -20858,13 +20864,13 @@
         <v>45067</v>
       </c>
       <c r="G203">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="H203" s="2">
         <v>45251</v>
       </c>
       <c r="I203">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="J203" t="inlineStr">
         <is>
@@ -20961,13 +20967,13 @@
         <v>45067</v>
       </c>
       <c r="G204">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="H204" s="2">
         <v>45251</v>
       </c>
       <c r="I204">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="J204" t="inlineStr">
         <is>
@@ -21064,13 +21070,13 @@
         <v>45178</v>
       </c>
       <c r="G205">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="H205" s="2">
         <v>45269</v>
       </c>
       <c r="I205">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="J205" t="inlineStr">
         <is>
@@ -21167,7 +21173,7 @@
         <v>45252</v>
       </c>
       <c r="I206">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="J206" t="inlineStr">
         <is>
@@ -21264,13 +21270,13 @@
         <v>45087</v>
       </c>
       <c r="G207">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="H207" s="2">
         <v>45270</v>
       </c>
       <c r="I207">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="J207" t="inlineStr">
         <is>
@@ -21367,13 +21373,13 @@
         <v>45099</v>
       </c>
       <c r="G208">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="H208" s="2">
         <v>45282</v>
       </c>
       <c r="I208">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="J208" t="inlineStr">
         <is>
@@ -21470,13 +21476,13 @@
         <v>45175</v>
       </c>
       <c r="G209">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="H209" s="2">
         <v>45356</v>
       </c>
       <c r="I209">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="J209" t="inlineStr">
         <is>
@@ -21573,13 +21579,13 @@
         <v>45175</v>
       </c>
       <c r="G210">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="H210" s="2">
         <v>45356</v>
       </c>
       <c r="I210">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="J210" t="inlineStr">
         <is>
@@ -21676,13 +21682,13 @@
         <v>45166</v>
       </c>
       <c r="G211">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="H211" s="2">
         <v>45350</v>
       </c>
       <c r="I211">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="J211" t="inlineStr">
         <is>
@@ -21779,13 +21785,13 @@
         <v>45166</v>
       </c>
       <c r="G212">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="H212" s="2">
         <v>45350</v>
       </c>
       <c r="I212">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="J212" t="inlineStr">
         <is>
@@ -21882,13 +21888,13 @@
         <v>45090</v>
       </c>
       <c r="G213">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="H213" s="2">
         <v>45273</v>
       </c>
       <c r="I213">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="J213" t="inlineStr">
         <is>
@@ -21985,13 +21991,13 @@
         <v>45106</v>
       </c>
       <c r="G214">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="H214" s="2">
         <v>45289</v>
       </c>
       <c r="I214">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="J214" t="inlineStr">
         <is>
@@ -22088,13 +22094,13 @@
         <v>45134</v>
       </c>
       <c r="G215">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="H215" s="2">
         <v>45226</v>
       </c>
       <c r="I215">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="J215" t="inlineStr">
         <is>
@@ -22191,13 +22197,13 @@
         <v>45132</v>
       </c>
       <c r="G216">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="H216" s="2">
         <v>45224</v>
       </c>
       <c r="I216">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="J216" t="inlineStr">
         <is>
@@ -22294,13 +22300,13 @@
         <v>45150</v>
       </c>
       <c r="G217">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="H217" s="2">
         <v>45242</v>
       </c>
       <c r="I217">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="J217" t="inlineStr">
         <is>
@@ -22397,13 +22403,13 @@
         <v>45187</v>
       </c>
       <c r="G218">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="H218" s="2">
         <v>45278</v>
       </c>
       <c r="I218">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="J218" t="inlineStr">
         <is>
@@ -22495,13 +22501,13 @@
         <v>45182</v>
       </c>
       <c r="G219">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="H219" s="2">
         <v>45273</v>
       </c>
       <c r="I219">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="J219" t="inlineStr">
         <is>
@@ -22598,13 +22604,13 @@
         <v>45196</v>
       </c>
       <c r="G220">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="H220" s="2">
         <v>45287</v>
       </c>
       <c r="I220">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="J220" t="inlineStr">
         <is>
@@ -22701,13 +22707,13 @@
         <v>45200</v>
       </c>
       <c r="G221">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="H221" s="2">
         <v>45292</v>
       </c>
       <c r="I221">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="J221" t="inlineStr">
         <is>
@@ -22804,13 +22810,13 @@
         <v>45135</v>
       </c>
       <c r="G222">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="H222" s="2">
         <v>45227</v>
       </c>
       <c r="I222">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="J222" t="inlineStr">
         <is>
@@ -22907,13 +22913,13 @@
         <v>45148</v>
       </c>
       <c r="G223">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="H223" s="2">
         <v>45240</v>
       </c>
       <c r="I223">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="J223" t="inlineStr">
         <is>
@@ -23005,13 +23011,13 @@
         <v>45192</v>
       </c>
       <c r="G224">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="H224" s="2">
         <v>45283</v>
       </c>
       <c r="I224">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="J224" t="inlineStr">
         <is>
@@ -23103,13 +23109,13 @@
         <v>45136</v>
       </c>
       <c r="G225">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="H225" s="2">
         <v>45320</v>
       </c>
       <c r="I225">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="J225" t="inlineStr">
         <is>
@@ -23206,13 +23212,13 @@
         <v>45136</v>
       </c>
       <c r="G226">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="H226" s="2">
         <v>45320</v>
       </c>
       <c r="I226">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="J226" t="inlineStr">
         <is>
@@ -23309,13 +23315,13 @@
         <v>45094</v>
       </c>
       <c r="G227">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="H227" s="2">
         <v>45277</v>
       </c>
       <c r="I227">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="J227" t="inlineStr">
         <is>
@@ -23412,13 +23418,13 @@
         <v>45081</v>
       </c>
       <c r="G228">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="H228" s="2">
         <v>45264</v>
       </c>
       <c r="I228">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="J228" t="inlineStr">
         <is>
@@ -23515,13 +23521,13 @@
         <v>45099</v>
       </c>
       <c r="G229">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="H229" s="2">
         <v>45282</v>
       </c>
       <c r="I229">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="J229" t="inlineStr">
         <is>
@@ -23618,13 +23624,13 @@
         <v>45201</v>
       </c>
       <c r="G230">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="H230" s="2">
         <v>45384</v>
       </c>
       <c r="I230">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="J230" t="inlineStr">
         <is>
@@ -23721,13 +23727,13 @@
         <v>45031</v>
       </c>
       <c r="G231">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="H231" s="2">
         <v>45214</v>
       </c>
       <c r="I231">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="J231" t="inlineStr">
         <is>
@@ -23824,7 +23830,7 @@
         <v>45294</v>
       </c>
       <c r="I232">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="J232" t="inlineStr">
         <is>
@@ -23921,13 +23927,13 @@
         <v>45079</v>
       </c>
       <c r="G233">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="H233" s="2">
         <v>45262</v>
       </c>
       <c r="I233">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="J233" t="inlineStr">
         <is>
@@ -24024,13 +24030,13 @@
         <v>45199</v>
       </c>
       <c r="G234">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="H234" s="2">
         <v>45382</v>
       </c>
       <c r="I234">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="J234" t="inlineStr">
         <is>
@@ -24127,13 +24133,13 @@
         <v>45204</v>
       </c>
       <c r="G235">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H235" s="2">
         <v>45387</v>
       </c>
       <c r="I235">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="J235" t="inlineStr">
         <is>
@@ -24230,13 +24236,13 @@
         <v>45204</v>
       </c>
       <c r="G236">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H236" s="2">
         <v>45387</v>
       </c>
       <c r="I236">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="J236" t="inlineStr">
         <is>
@@ -24333,13 +24339,13 @@
         <v>45080</v>
       </c>
       <c r="G237">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="H237" s="2">
         <v>45263</v>
       </c>
       <c r="I237">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="J237" t="inlineStr">
         <is>
@@ -24436,13 +24442,13 @@
         <v>45046</v>
       </c>
       <c r="G238">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="H238" s="2">
         <v>45229</v>
       </c>
       <c r="I238">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="J238" t="inlineStr">
         <is>
@@ -24539,13 +24545,13 @@
         <v>45204</v>
       </c>
       <c r="G239">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H239" s="2">
         <v>45296</v>
       </c>
       <c r="I239">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="J239" t="inlineStr">
         <is>
@@ -24633,13 +24639,13 @@
         <v>45204</v>
       </c>
       <c r="G240">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H240" s="2">
         <v>45296</v>
       </c>
       <c r="I240">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="J240" t="inlineStr">
         <is>
@@ -24727,13 +24733,13 @@
         <v>45199</v>
       </c>
       <c r="G241">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="H241" s="2">
         <v>45382</v>
       </c>
       <c r="I241">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="J241" t="inlineStr">
         <is>
@@ -24830,13 +24836,13 @@
         <v>45070</v>
       </c>
       <c r="G242">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="H242" s="2">
         <v>45254</v>
       </c>
       <c r="I242">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="J242" t="inlineStr">
         <is>
@@ -24933,13 +24939,13 @@
         <v>45168</v>
       </c>
       <c r="G243">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="H243" s="2">
         <v>45260</v>
       </c>
       <c r="I243">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="J243" t="inlineStr">
         <is>
@@ -25036,13 +25042,13 @@
         <v>45027</v>
       </c>
       <c r="G244">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="H244" s="2">
         <v>45210</v>
       </c>
       <c r="I244">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="J244" t="inlineStr">
         <is>
@@ -25139,13 +25145,13 @@
         <v>45077</v>
       </c>
       <c r="G245">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="H245" s="2">
         <v>45260</v>
       </c>
       <c r="I245">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="J245" t="inlineStr">
         <is>
@@ -25242,13 +25248,13 @@
         <v>45100</v>
       </c>
       <c r="G246">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="H246" s="2">
         <v>45283</v>
       </c>
       <c r="I246">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="J246" t="inlineStr">
         <is>
@@ -25345,7 +25351,7 @@
         <v>45281</v>
       </c>
       <c r="I247">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="J247" t="inlineStr">
         <is>
@@ -25442,13 +25448,13 @@
         <v>45044</v>
       </c>
       <c r="G248">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="H248" s="2">
         <v>45227</v>
       </c>
       <c r="I248">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="J248" t="inlineStr">
         <is>
@@ -25545,13 +25551,13 @@
         <v>45101</v>
       </c>
       <c r="G249">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="H249" s="2">
         <v>45283</v>
       </c>
       <c r="I249">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="J249" t="inlineStr">
         <is>
@@ -25648,13 +25654,13 @@
         <v>45134</v>
       </c>
       <c r="G250">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="H250" s="2">
         <v>45226</v>
       </c>
       <c r="I250">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="J250" t="inlineStr">
         <is>
@@ -25751,13 +25757,13 @@
         <v>45158</v>
       </c>
       <c r="G251">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="H251" s="2">
         <v>45250</v>
       </c>
       <c r="I251">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="J251" t="inlineStr">
         <is>
@@ -25854,13 +25860,13 @@
         <v>45200</v>
       </c>
       <c r="G252">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="H252" s="2">
         <v>45292</v>
       </c>
       <c r="I252">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="J252" t="inlineStr">
         <is>
@@ -25957,7 +25963,7 @@
         <v>45317</v>
       </c>
       <c r="I253">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="J253" t="inlineStr">
         <is>
@@ -26054,13 +26060,13 @@
         <v>45039</v>
       </c>
       <c r="G254">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="H254" s="2">
         <v>45222</v>
       </c>
       <c r="I254">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="J254" t="inlineStr">
         <is>
@@ -26152,13 +26158,13 @@
         <v>45129</v>
       </c>
       <c r="G255">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="H255" s="2">
         <v>45221</v>
       </c>
       <c r="I255">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="J255" t="inlineStr">
         <is>
@@ -26255,13 +26261,13 @@
         <v>45157</v>
       </c>
       <c r="G256">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="H256" s="2">
         <v>45341</v>
       </c>
       <c r="I256">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="J256" t="inlineStr">
         <is>
@@ -26358,13 +26364,13 @@
         <v>45063</v>
       </c>
       <c r="G257">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="H257" s="2">
         <v>45247</v>
       </c>
       <c r="I257">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="J257" t="inlineStr">
         <is>
@@ -26461,7 +26467,7 @@
         <v>45254</v>
       </c>
       <c r="I258">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="J258" t="inlineStr">
         <is>
@@ -26558,7 +26564,7 @@
         <v>45486</v>
       </c>
       <c r="I259">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="J259" t="inlineStr">
         <is>
@@ -26650,13 +26656,13 @@
         <v>45073</v>
       </c>
       <c r="G260">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="H260" s="2">
         <v>45439</v>
       </c>
       <c r="I260">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="J260" t="inlineStr">
         <is>
@@ -26748,7 +26754,7 @@
         <v>45323</v>
       </c>
       <c r="I261">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="J261" t="inlineStr">
         <is>
@@ -26840,7 +26846,7 @@
         <v>45303</v>
       </c>
       <c r="I262">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="J262" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
Bond dates update Mon Oct  9 23:16:23 UTC 2023
</commit_message>
<xml_diff>
--- a/Data/obligacje_screener.xlsx
+++ b/Data/obligacje_screener.xlsx
@@ -512,7 +512,7 @@
         <v>45340</v>
       </c>
       <c r="I2">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="J2" t="inlineStr">
         <is>
@@ -600,13 +600,13 @@
         <v>45121</v>
       </c>
       <c r="G3">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="H3" s="2">
         <v>45305</v>
       </c>
       <c r="I3">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="J3" t="inlineStr">
         <is>
@@ -703,13 +703,13 @@
         <v>45039</v>
       </c>
       <c r="G4">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="H4" s="2">
         <v>45222</v>
       </c>
       <c r="I4">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="J4" t="inlineStr">
         <is>
@@ -806,13 +806,13 @@
         <v>45039</v>
       </c>
       <c r="G5">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="H5" s="2">
         <v>45222</v>
       </c>
       <c r="I5">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="J5" t="inlineStr">
         <is>
@@ -909,13 +909,13 @@
         <v>45129</v>
       </c>
       <c r="G6">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="H6" s="2">
         <v>45221</v>
       </c>
       <c r="I6">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="J6" t="inlineStr">
         <is>
@@ -1012,13 +1012,13 @@
         <v>45162</v>
       </c>
       <c r="G7">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="H7" s="2">
         <v>45254</v>
       </c>
       <c r="I7">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="J7" t="inlineStr">
         <is>
@@ -1110,13 +1110,13 @@
         <v>45156</v>
       </c>
       <c r="G8">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="H8" s="2">
         <v>45248</v>
       </c>
       <c r="I8">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="J8" t="inlineStr">
         <is>
@@ -1213,13 +1213,13 @@
         <v>45141</v>
       </c>
       <c r="G9">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="H9" s="2">
         <v>45233</v>
       </c>
       <c r="I9">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="J9" t="inlineStr">
         <is>
@@ -1316,13 +1316,13 @@
         <v>45062</v>
       </c>
       <c r="G10">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="H10" s="2">
         <v>45246</v>
       </c>
       <c r="I10">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="J10" t="inlineStr">
         <is>
@@ -1419,7 +1419,7 @@
         <v>45286</v>
       </c>
       <c r="I11">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="J11" t="inlineStr">
         <is>
@@ -1516,13 +1516,13 @@
         <v>45195</v>
       </c>
       <c r="G12">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="H12" s="2">
         <v>45377</v>
       </c>
       <c r="I12">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="J12" t="inlineStr">
         <is>
@@ -1614,13 +1614,13 @@
         <v>45036</v>
       </c>
       <c r="G13">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="H13" s="2">
         <v>45219</v>
       </c>
       <c r="I13">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="J13" t="inlineStr">
         <is>
@@ -1717,13 +1717,13 @@
         <v>45036</v>
       </c>
       <c r="G14">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="H14" s="2">
         <v>45219</v>
       </c>
       <c r="I14">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="J14" t="inlineStr">
         <is>
@@ -1820,13 +1820,13 @@
         <v>45106</v>
       </c>
       <c r="G15">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="H15" s="2">
         <v>45289</v>
       </c>
       <c r="I15">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="J15" t="inlineStr">
         <is>
@@ -1923,13 +1923,13 @@
         <v>45186</v>
       </c>
       <c r="G16">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="H16" s="2">
         <v>45278</v>
       </c>
       <c r="I16">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="J16" t="inlineStr">
         <is>
@@ -2026,13 +2026,13 @@
         <v>45186</v>
       </c>
       <c r="G17">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="H17" s="2">
         <v>45277</v>
       </c>
       <c r="I17">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="J17" t="inlineStr">
         <is>
@@ -2129,13 +2129,13 @@
         <v>45132</v>
       </c>
       <c r="G18">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="H18" s="2">
         <v>45224</v>
       </c>
       <c r="I18">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="J18" t="inlineStr">
         <is>
@@ -2232,13 +2232,13 @@
         <v>45137</v>
       </c>
       <c r="G19">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="H19" s="2">
         <v>45229</v>
       </c>
       <c r="I19">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="J19" t="inlineStr">
         <is>
@@ -2330,13 +2330,13 @@
         <v>45183</v>
       </c>
       <c r="G20">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="H20" s="2">
         <v>45274</v>
       </c>
       <c r="I20">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="J20" t="inlineStr">
         <is>
@@ -2433,13 +2433,13 @@
         <v>45187</v>
       </c>
       <c r="G21">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="H21" s="2">
         <v>45278</v>
       </c>
       <c r="I21">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="J21" t="inlineStr">
         <is>
@@ -2536,13 +2536,13 @@
         <v>45187</v>
       </c>
       <c r="G22">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="H22" s="2">
         <v>45278</v>
       </c>
       <c r="I22">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="J22" t="inlineStr">
         <is>
@@ -2639,7 +2639,7 @@
         <v>45245</v>
       </c>
       <c r="I23">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="J23" t="inlineStr">
         <is>
@@ -2736,7 +2736,7 @@
         <v>45245</v>
       </c>
       <c r="I24">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="J24" t="inlineStr">
         <is>
@@ -2833,7 +2833,7 @@
         <v>45204</v>
       </c>
       <c r="G25">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="J25" t="inlineStr">
         <is>
@@ -2930,13 +2930,13 @@
         <v>45160</v>
       </c>
       <c r="G26">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="H26" s="2">
         <v>45344</v>
       </c>
       <c r="I26">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="J26" t="inlineStr">
         <is>
@@ -3033,13 +3033,13 @@
         <v>45118</v>
       </c>
       <c r="G27">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="H27" s="2">
         <v>45302</v>
       </c>
       <c r="I27">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="J27" t="inlineStr">
         <is>
@@ -3136,13 +3136,13 @@
         <v>45085</v>
       </c>
       <c r="G28">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="H28" s="2">
         <v>45268</v>
       </c>
       <c r="I28">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="J28" t="inlineStr">
         <is>
@@ -3239,13 +3239,13 @@
         <v>45183</v>
       </c>
       <c r="G29">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="H29" s="2">
         <v>45274</v>
       </c>
       <c r="I29">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="J29" t="inlineStr">
         <is>
@@ -3342,7 +3342,7 @@
         <v>45224</v>
       </c>
       <c r="I30">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="J30" t="inlineStr">
         <is>
@@ -3439,13 +3439,13 @@
         <v>45153</v>
       </c>
       <c r="G31">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="H31" s="2">
         <v>45245</v>
       </c>
       <c r="I31">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="J31" t="inlineStr">
         <is>
@@ -3542,13 +3542,13 @@
         <v>45155</v>
       </c>
       <c r="G32">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="H32" s="2">
         <v>45247</v>
       </c>
       <c r="I32">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="J32" t="inlineStr">
         <is>
@@ -3645,7 +3645,7 @@
         <v>45255</v>
       </c>
       <c r="I33">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="J33" t="inlineStr">
         <is>
@@ -3742,13 +3742,13 @@
         <v>45176</v>
       </c>
       <c r="G34">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="H34" s="2">
         <v>45267</v>
       </c>
       <c r="I34">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="J34" t="inlineStr">
         <is>
@@ -3845,13 +3845,13 @@
         <v>45130</v>
       </c>
       <c r="G35">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="H35" s="2">
         <v>45222</v>
       </c>
       <c r="I35">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="J35" t="inlineStr">
         <is>
@@ -3940,16 +3940,16 @@
         </is>
       </c>
       <c r="F36" s="2">
-        <v>45115</v>
+        <v>45207</v>
       </c>
       <c r="G36">
-        <v>92</v>
+        <v>1</v>
       </c>
       <c r="H36" s="2">
         <v>45299</v>
       </c>
       <c r="I36">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="J36" t="inlineStr">
         <is>
@@ -4046,13 +4046,13 @@
         <v>45189</v>
       </c>
       <c r="G37">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="H37" s="2">
         <v>45280</v>
       </c>
       <c r="I37">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="J37" t="inlineStr">
         <is>
@@ -4144,13 +4144,13 @@
         <v>45107</v>
       </c>
       <c r="G38">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="H38" s="2">
         <v>45290</v>
       </c>
       <c r="I38">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="J38" t="inlineStr">
         <is>
@@ -4247,13 +4247,13 @@
         <v>45063</v>
       </c>
       <c r="G39">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="H39" s="2">
         <v>45247</v>
       </c>
       <c r="I39">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="J39" t="inlineStr">
         <is>
@@ -4350,13 +4350,13 @@
         <v>45177</v>
       </c>
       <c r="G40">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="H40" s="2">
         <v>45359</v>
       </c>
       <c r="I40">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="J40" t="inlineStr">
         <is>
@@ -4453,13 +4453,13 @@
         <v>45107</v>
       </c>
       <c r="G41">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="H41" s="2">
         <v>45290</v>
       </c>
       <c r="I41">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="J41" t="inlineStr">
         <is>
@@ -4556,7 +4556,7 @@
         <v>45265</v>
       </c>
       <c r="I42">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="J42" t="inlineStr">
         <is>
@@ -4653,13 +4653,13 @@
         <v>45098</v>
       </c>
       <c r="G43">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="H43" s="2">
         <v>45281</v>
       </c>
       <c r="I43">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="J43" t="inlineStr">
         <is>
@@ -4756,13 +4756,13 @@
         <v>45099</v>
       </c>
       <c r="G44">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="H44" s="2">
         <v>45282</v>
       </c>
       <c r="I44">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="J44" t="inlineStr">
         <is>
@@ -4859,13 +4859,13 @@
         <v>45106</v>
       </c>
       <c r="G45">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="H45" s="2">
         <v>45289</v>
       </c>
       <c r="I45">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="J45" t="inlineStr">
         <is>
@@ -4962,13 +4962,13 @@
         <v>45106</v>
       </c>
       <c r="G46">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="H46" s="2">
         <v>45289</v>
       </c>
       <c r="I46">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="J46" t="inlineStr">
         <is>
@@ -5065,13 +5065,13 @@
         <v>45120</v>
       </c>
       <c r="G47">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="H47" s="2">
         <v>45304</v>
       </c>
       <c r="I47">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="J47" t="inlineStr">
         <is>
@@ -5168,13 +5168,13 @@
         <v>45118</v>
       </c>
       <c r="G48">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="H48" s="2">
         <v>45302</v>
       </c>
       <c r="I48">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="J48" t="inlineStr">
         <is>
@@ -5271,13 +5271,13 @@
         <v>45152</v>
       </c>
       <c r="G49">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="H49" s="2">
         <v>45336</v>
       </c>
       <c r="I49">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="J49" t="inlineStr">
         <is>
@@ -5374,13 +5374,13 @@
         <v>45042</v>
       </c>
       <c r="G50">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="H50" s="2">
         <v>45225</v>
       </c>
       <c r="I50">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="J50" t="inlineStr">
         <is>
@@ -5477,13 +5477,13 @@
         <v>45122</v>
       </c>
       <c r="G51">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="H51" s="2">
         <v>45306</v>
       </c>
       <c r="I51">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="J51" t="inlineStr">
         <is>
@@ -5580,13 +5580,13 @@
         <v>45139</v>
       </c>
       <c r="G52">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="H52" s="2">
         <v>45323</v>
       </c>
       <c r="I52">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="J52" t="inlineStr">
         <is>
@@ -5683,13 +5683,13 @@
         <v>45099</v>
       </c>
       <c r="G53">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="H53" s="2">
         <v>45282</v>
       </c>
       <c r="I53">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="J53" t="inlineStr">
         <is>
@@ -5786,13 +5786,13 @@
         <v>45196</v>
       </c>
       <c r="G54">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="H54" s="2">
         <v>45287</v>
       </c>
       <c r="I54">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="J54" t="inlineStr">
         <is>
@@ -5889,13 +5889,13 @@
         <v>45044</v>
       </c>
       <c r="G55">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="H55" s="2">
         <v>45227</v>
       </c>
       <c r="I55">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="J55" t="inlineStr">
         <is>
@@ -5992,13 +5992,13 @@
         <v>45151</v>
       </c>
       <c r="G56">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="H56" s="2">
         <v>45243</v>
       </c>
       <c r="I56">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="J56" t="inlineStr">
         <is>
@@ -6090,13 +6090,13 @@
         <v>45196</v>
       </c>
       <c r="G57">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="H57" s="2">
         <v>45287</v>
       </c>
       <c r="I57">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="J57" t="inlineStr">
         <is>
@@ -6193,13 +6193,13 @@
         <v>45069</v>
       </c>
       <c r="G58">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="H58" s="2">
         <v>45253</v>
       </c>
       <c r="I58">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="J58" t="inlineStr">
         <is>
@@ -6296,13 +6296,13 @@
         <v>45191</v>
       </c>
       <c r="G59">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="H59" s="2">
         <v>45282</v>
       </c>
       <c r="I59">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="J59" t="inlineStr">
         <is>
@@ -6394,7 +6394,7 @@
         <v>45205</v>
       </c>
       <c r="G60">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="J60" t="inlineStr">
         <is>
@@ -6491,13 +6491,13 @@
         <v>45127</v>
       </c>
       <c r="G61">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="H61" s="2">
         <v>45219</v>
       </c>
       <c r="I61">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="J61" t="inlineStr">
         <is>
@@ -6594,13 +6594,13 @@
         <v>45058</v>
       </c>
       <c r="G62">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="H62" s="2">
         <v>45242</v>
       </c>
       <c r="I62">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="J62" t="inlineStr">
         <is>
@@ -6697,13 +6697,13 @@
         <v>45194</v>
       </c>
       <c r="G63">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="H63" s="2">
         <v>45376</v>
       </c>
       <c r="I63">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="J63" t="inlineStr">
         <is>
@@ -6795,13 +6795,7 @@
         <v>45025</v>
       </c>
       <c r="G64">
-        <v>182</v>
-      </c>
-      <c r="H64" s="2">
-        <v>45208</v>
-      </c>
-      <c r="I64">
-        <v>1</v>
+        <v>183</v>
       </c>
       <c r="J64" t="inlineStr">
         <is>
@@ -6898,13 +6892,7 @@
         <v>45025</v>
       </c>
       <c r="G65">
-        <v>182</v>
-      </c>
-      <c r="H65" s="2">
-        <v>45208</v>
-      </c>
-      <c r="I65">
-        <v>1</v>
+        <v>183</v>
       </c>
       <c r="J65" t="inlineStr">
         <is>
@@ -7001,13 +6989,13 @@
         <v>45089</v>
       </c>
       <c r="G66">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="H66" s="2">
         <v>45272</v>
       </c>
       <c r="I66">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="J66" t="inlineStr">
         <is>
@@ -7104,13 +7092,13 @@
         <v>45178</v>
       </c>
       <c r="G67">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="H67" s="2">
         <v>45269</v>
       </c>
       <c r="I67">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="J67" t="inlineStr">
         <is>
@@ -7202,13 +7190,13 @@
         <v>45196</v>
       </c>
       <c r="G68">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="H68" s="2">
         <v>45287</v>
       </c>
       <c r="I68">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="J68" t="inlineStr">
         <is>
@@ -7305,13 +7293,13 @@
         <v>45149</v>
       </c>
       <c r="G69">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="H69" s="2">
         <v>45241</v>
       </c>
       <c r="I69">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="J69" t="inlineStr">
         <is>
@@ -7408,13 +7396,13 @@
         <v>45205</v>
       </c>
       <c r="G70">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H70" s="2">
         <v>45296</v>
       </c>
       <c r="I70">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="J70" t="inlineStr">
         <is>
@@ -7511,7 +7499,7 @@
         <v>45205</v>
       </c>
       <c r="G71">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="J71" t="inlineStr">
         <is>
@@ -7605,16 +7593,16 @@
         </is>
       </c>
       <c r="F72" s="2">
-        <v>45115</v>
+        <v>45207</v>
       </c>
       <c r="G72">
-        <v>92</v>
+        <v>1</v>
       </c>
       <c r="H72" s="2">
         <v>45299</v>
       </c>
       <c r="I72">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="J72" t="inlineStr">
         <is>
@@ -7711,13 +7699,13 @@
         <v>45189</v>
       </c>
       <c r="G73">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="H73" s="2">
         <v>45280</v>
       </c>
       <c r="I73">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="J73" t="inlineStr">
         <is>
@@ -7809,13 +7797,13 @@
         <v>45038</v>
       </c>
       <c r="G74">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="H74" s="2">
         <v>45221</v>
       </c>
       <c r="I74">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="J74" t="inlineStr">
         <is>
@@ -7907,13 +7895,13 @@
         <v>45117</v>
       </c>
       <c r="G75">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="H75" s="2">
         <v>45301</v>
       </c>
       <c r="I75">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="J75" t="inlineStr">
         <is>
@@ -8010,13 +7998,13 @@
         <v>45160</v>
       </c>
       <c r="G76">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="H76" s="2">
         <v>45344</v>
       </c>
       <c r="I76">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="J76" t="inlineStr">
         <is>
@@ -8113,13 +8101,13 @@
         <v>45186</v>
       </c>
       <c r="G77">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="H77" s="2">
         <v>45368</v>
       </c>
       <c r="I77">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="J77" t="inlineStr">
         <is>
@@ -8216,13 +8204,13 @@
         <v>45043</v>
       </c>
       <c r="G78">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="H78" s="2">
         <v>45226</v>
       </c>
       <c r="I78">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="J78" t="inlineStr">
         <is>
@@ -8319,13 +8307,13 @@
         <v>45079</v>
       </c>
       <c r="G79">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="H79" s="2">
         <v>45262</v>
       </c>
       <c r="I79">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="J79" t="inlineStr">
         <is>
@@ -8422,7 +8410,7 @@
         <v>45254</v>
       </c>
       <c r="I80">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="J80" t="inlineStr">
         <is>
@@ -8519,13 +8507,13 @@
         <v>45104</v>
       </c>
       <c r="G81">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="H81" s="2">
         <v>45287</v>
       </c>
       <c r="I81">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="J81" t="inlineStr">
         <is>
@@ -8622,7 +8610,7 @@
         <v>45288</v>
       </c>
       <c r="I82">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="J82" t="inlineStr">
         <is>
@@ -8714,13 +8702,13 @@
         <v>45175</v>
       </c>
       <c r="G83">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="H83" s="2">
         <v>45357</v>
       </c>
       <c r="I83">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="J83" t="inlineStr">
         <is>
@@ -8817,13 +8805,13 @@
         <v>45054</v>
       </c>
       <c r="G84">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="H84" s="2">
         <v>45238</v>
       </c>
       <c r="I84">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="J84" t="inlineStr">
         <is>
@@ -8920,13 +8908,13 @@
         <v>45056</v>
       </c>
       <c r="G85">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="H85" s="2">
         <v>45240</v>
       </c>
       <c r="I85">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="J85" t="inlineStr">
         <is>
@@ -9023,13 +9011,13 @@
         <v>45085</v>
       </c>
       <c r="G86">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="H86" s="2">
         <v>45268</v>
       </c>
       <c r="I86">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="J86" t="inlineStr">
         <is>
@@ -9126,13 +9114,13 @@
         <v>45194</v>
       </c>
       <c r="G87">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="H87" s="2">
         <v>45560</v>
       </c>
       <c r="I87">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="J87" t="inlineStr">
         <is>
@@ -9219,13 +9207,13 @@
         <v>45103</v>
       </c>
       <c r="G88">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="H88" s="2">
         <v>45286</v>
       </c>
       <c r="I88">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="J88" t="inlineStr">
         <is>
@@ -9322,13 +9310,13 @@
         <v>45103</v>
       </c>
       <c r="G89">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="H89" s="2">
         <v>45286</v>
       </c>
       <c r="I89">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="J89" t="inlineStr">
         <is>
@@ -9425,13 +9413,13 @@
         <v>45192</v>
       </c>
       <c r="G90">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H90" s="2">
         <v>45374</v>
       </c>
       <c r="I90">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="J90" t="inlineStr">
         <is>
@@ -9523,13 +9511,13 @@
         <v>45100</v>
       </c>
       <c r="G91">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="H91" s="2">
         <v>45287</v>
       </c>
       <c r="I91">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="J91" t="inlineStr">
         <is>
@@ -9626,13 +9614,13 @@
         <v>45187</v>
       </c>
       <c r="G92">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="H92" s="2">
         <v>45369</v>
       </c>
       <c r="I92">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="J92" t="inlineStr">
         <is>
@@ -9729,13 +9717,13 @@
         <v>45104</v>
       </c>
       <c r="G93">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="H93" s="2">
         <v>45287</v>
       </c>
       <c r="I93">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="J93" t="inlineStr">
         <is>
@@ -9832,13 +9820,13 @@
         <v>45104</v>
       </c>
       <c r="G94">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="H94" s="2">
         <v>45287</v>
       </c>
       <c r="I94">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="J94" t="inlineStr">
         <is>
@@ -9935,13 +9923,13 @@
         <v>45049</v>
       </c>
       <c r="G95">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="H95" s="2">
         <v>45233</v>
       </c>
       <c r="I95">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="J95" t="inlineStr">
         <is>
@@ -10038,13 +10026,13 @@
         <v>45122</v>
       </c>
       <c r="G96">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="H96" s="2">
         <v>45306</v>
       </c>
       <c r="I96">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="J96" t="inlineStr">
         <is>
@@ -10136,13 +10124,13 @@
         <v>45141</v>
       </c>
       <c r="G97">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="H97" s="2">
         <v>45325</v>
       </c>
       <c r="I97">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="J97" t="inlineStr">
         <is>
@@ -10239,13 +10227,13 @@
         <v>45194</v>
       </c>
       <c r="G98">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="H98" s="2">
         <v>45376</v>
       </c>
       <c r="I98">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="J98" t="inlineStr">
         <is>
@@ -10337,13 +10325,13 @@
         <v>45093</v>
       </c>
       <c r="G99">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="H99" s="2">
         <v>45276</v>
       </c>
       <c r="I99">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="J99" t="inlineStr">
         <is>
@@ -10440,13 +10428,13 @@
         <v>45123</v>
       </c>
       <c r="G100">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="H100" s="2">
         <v>45307</v>
       </c>
       <c r="I100">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="J100" t="inlineStr">
         <is>
@@ -10543,13 +10531,13 @@
         <v>45198</v>
       </c>
       <c r="G101">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="H101" s="2">
         <v>45380</v>
       </c>
       <c r="I101">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="J101" t="inlineStr">
         <is>
@@ -10646,13 +10634,13 @@
         <v>45093</v>
       </c>
       <c r="G102">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="H102" s="2">
         <v>45276</v>
       </c>
       <c r="I102">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="J102" t="inlineStr">
         <is>
@@ -10749,13 +10737,13 @@
         <v>45122</v>
       </c>
       <c r="G103">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="H103" s="2">
         <v>45306</v>
       </c>
       <c r="I103">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="J103" t="inlineStr">
         <is>
@@ -10852,13 +10840,13 @@
         <v>45122</v>
       </c>
       <c r="G104">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="H104" s="2">
         <v>45306</v>
       </c>
       <c r="I104">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="J104" t="inlineStr">
         <is>
@@ -10950,13 +10938,13 @@
         <v>45050</v>
       </c>
       <c r="G105">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="H105" s="2">
         <v>45234</v>
       </c>
       <c r="I105">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="J105" t="inlineStr">
         <is>
@@ -11053,13 +11041,13 @@
         <v>45085</v>
       </c>
       <c r="G106">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="H106" s="2">
         <v>45268</v>
       </c>
       <c r="I106">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="J106" t="inlineStr">
         <is>
@@ -11156,13 +11144,13 @@
         <v>45185</v>
       </c>
       <c r="G107">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="H107" s="2">
         <v>45276</v>
       </c>
       <c r="I107">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="J107" t="inlineStr">
         <is>
@@ -11254,13 +11242,13 @@
         <v>45185</v>
       </c>
       <c r="G108">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="H108" s="2">
         <v>45276</v>
       </c>
       <c r="I108">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="J108" t="inlineStr">
         <is>
@@ -11352,13 +11340,13 @@
         <v>45185</v>
       </c>
       <c r="G109">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="H109" s="2">
         <v>45276</v>
       </c>
       <c r="I109">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="J109" t="inlineStr">
         <is>
@@ -11455,13 +11443,13 @@
         <v>45148</v>
       </c>
       <c r="G110">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="H110" s="2">
         <v>45240</v>
       </c>
       <c r="I110">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="J110" t="inlineStr">
         <is>
@@ -11558,13 +11546,13 @@
         <v>45119</v>
       </c>
       <c r="G111">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="H111" s="2">
         <v>45211</v>
       </c>
       <c r="I111">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="J111" t="inlineStr">
         <is>
@@ -11661,13 +11649,13 @@
         <v>45172</v>
       </c>
       <c r="G112">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="H112" s="2">
         <v>45263</v>
       </c>
       <c r="I112">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="J112" t="inlineStr">
         <is>
@@ -11764,13 +11752,13 @@
         <v>45206</v>
       </c>
       <c r="G113">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H113" s="2">
         <v>45389</v>
       </c>
       <c r="I113">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="J113" t="inlineStr">
         <is>
@@ -11867,13 +11855,13 @@
         <v>45203</v>
       </c>
       <c r="G114">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="H114" s="2">
         <v>45295</v>
       </c>
       <c r="I114">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="J114" t="inlineStr">
         <is>
@@ -11970,7 +11958,7 @@
         <v>45218</v>
       </c>
       <c r="I115">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="J115" t="inlineStr">
         <is>
@@ -12067,13 +12055,13 @@
         <v>45161</v>
       </c>
       <c r="G116">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="H116" s="2">
         <v>45253</v>
       </c>
       <c r="I116">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="J116" t="inlineStr">
         <is>
@@ -12170,13 +12158,13 @@
         <v>45115</v>
       </c>
       <c r="G117">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="H117" s="2">
         <v>45299</v>
       </c>
       <c r="I117">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="J117" t="inlineStr">
         <is>
@@ -12268,13 +12256,13 @@
         <v>45094</v>
       </c>
       <c r="G118">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="H118" s="2">
         <v>45277</v>
       </c>
       <c r="I118">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="J118" t="inlineStr">
         <is>
@@ -12371,13 +12359,13 @@
         <v>45104</v>
       </c>
       <c r="G119">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="H119" s="2">
         <v>45287</v>
       </c>
       <c r="I119">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="J119" t="inlineStr">
         <is>
@@ -12474,13 +12462,13 @@
         <v>45104</v>
       </c>
       <c r="G120">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="H120" s="2">
         <v>45287</v>
       </c>
       <c r="I120">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="J120" t="inlineStr">
         <is>
@@ -12577,13 +12565,13 @@
         <v>45104</v>
       </c>
       <c r="G121">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="H121" s="2">
         <v>45287</v>
       </c>
       <c r="I121">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="J121" t="inlineStr">
         <is>
@@ -12680,13 +12668,13 @@
         <v>45104</v>
       </c>
       <c r="G122">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="H122" s="2">
         <v>45287</v>
       </c>
       <c r="I122">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="J122" t="inlineStr">
         <is>
@@ -12783,13 +12771,13 @@
         <v>45199</v>
       </c>
       <c r="G123">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="H123" s="2">
         <v>45291</v>
       </c>
       <c r="I123">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="J123" t="inlineStr">
         <is>
@@ -12886,13 +12874,13 @@
         <v>45197</v>
       </c>
       <c r="G124">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="H124" s="2">
         <v>45379</v>
       </c>
       <c r="I124">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="J124" t="inlineStr">
         <is>
@@ -12989,13 +12977,13 @@
         <v>45121</v>
       </c>
       <c r="G125">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="H125" s="2">
         <v>45213</v>
       </c>
       <c r="I125">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="J125" t="inlineStr">
         <is>
@@ -13092,13 +13080,13 @@
         <v>45134</v>
       </c>
       <c r="G126">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="H126" s="2">
         <v>45226</v>
       </c>
       <c r="I126">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="J126" t="inlineStr">
         <is>
@@ -13195,7 +13183,7 @@
         <v>45212</v>
       </c>
       <c r="I127">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="J127" t="inlineStr">
         <is>
@@ -13292,13 +13280,13 @@
         <v>45126</v>
       </c>
       <c r="G128">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="H128" s="2">
         <v>45218</v>
       </c>
       <c r="I128">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="J128" t="inlineStr">
         <is>
@@ -13390,13 +13378,13 @@
         <v>45158</v>
       </c>
       <c r="G129">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="H129" s="2">
         <v>45250</v>
       </c>
       <c r="I129">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="J129" t="inlineStr">
         <is>
@@ -13493,13 +13481,13 @@
         <v>45171</v>
       </c>
       <c r="G130">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="H130" s="2">
         <v>45262</v>
       </c>
       <c r="I130">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="J130" t="inlineStr">
         <is>
@@ -13596,13 +13584,13 @@
         <v>45203</v>
       </c>
       <c r="G131">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="H131" s="2">
         <v>45295</v>
       </c>
       <c r="I131">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="J131" t="inlineStr">
         <is>
@@ -13699,13 +13687,13 @@
         <v>45144</v>
       </c>
       <c r="G132">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="H132" s="2">
         <v>45236</v>
       </c>
       <c r="I132">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="J132" t="inlineStr">
         <is>
@@ -13802,13 +13790,13 @@
         <v>45156</v>
       </c>
       <c r="G133">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="H133" s="2">
         <v>45248</v>
       </c>
       <c r="I133">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="J133" t="inlineStr">
         <is>
@@ -13900,13 +13888,13 @@
         <v>45146</v>
       </c>
       <c r="G134">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="H134" s="2">
         <v>45238</v>
       </c>
       <c r="I134">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="J134" t="inlineStr">
         <is>
@@ -14003,13 +13991,13 @@
         <v>45140</v>
       </c>
       <c r="G135">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="H135" s="2">
         <v>45232</v>
       </c>
       <c r="I135">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="J135" t="inlineStr">
         <is>
@@ -14106,13 +14094,13 @@
         <v>45196</v>
       </c>
       <c r="G136">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="H136" s="2">
         <v>45287</v>
       </c>
       <c r="I136">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="J136" t="inlineStr">
         <is>
@@ -14209,13 +14197,13 @@
         <v>45197</v>
       </c>
       <c r="G137">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="H137" s="2">
         <v>45288</v>
       </c>
       <c r="I137">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="J137" t="inlineStr">
         <is>
@@ -14312,13 +14300,13 @@
         <v>45179</v>
       </c>
       <c r="G138">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="H138" s="2">
         <v>45270</v>
       </c>
       <c r="I138">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="J138" t="inlineStr">
         <is>
@@ -14410,13 +14398,13 @@
         <v>45197</v>
       </c>
       <c r="G139">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="H139" s="2">
         <v>45288</v>
       </c>
       <c r="I139">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="J139" t="inlineStr">
         <is>
@@ -14513,13 +14501,13 @@
         <v>45182</v>
       </c>
       <c r="G140">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="H140" s="2">
         <v>45273</v>
       </c>
       <c r="I140">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="J140" t="inlineStr">
         <is>
@@ -14616,13 +14604,13 @@
         <v>45116</v>
       </c>
       <c r="G141">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="H141" s="2">
-        <v>45208</v>
+        <v>45300</v>
       </c>
       <c r="I141">
-        <v>1</v>
+        <v>92</v>
       </c>
       <c r="J141" t="inlineStr">
         <is>
@@ -14714,13 +14702,13 @@
         <v>45150</v>
       </c>
       <c r="G142">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="H142" s="2">
         <v>45242</v>
       </c>
       <c r="I142">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="J142" t="inlineStr">
         <is>
@@ -14817,7 +14805,7 @@
         <v>45238</v>
       </c>
       <c r="I143">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="J143" t="inlineStr">
         <is>
@@ -14914,13 +14902,13 @@
         <v>45171</v>
       </c>
       <c r="G144">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="H144" s="2">
         <v>45262</v>
       </c>
       <c r="I144">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="J144" t="inlineStr">
         <is>
@@ -15017,13 +15005,13 @@
         <v>45194</v>
       </c>
       <c r="G145">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="H145" s="2">
         <v>45285</v>
       </c>
       <c r="I145">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="J145" t="inlineStr">
         <is>
@@ -15110,13 +15098,13 @@
         <v>45119</v>
       </c>
       <c r="G146">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="H146" s="2">
         <v>45211</v>
       </c>
       <c r="I146">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="J146" t="inlineStr">
         <is>
@@ -15213,13 +15201,13 @@
         <v>45165</v>
       </c>
       <c r="G147">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="H147" s="2">
         <v>45257</v>
       </c>
       <c r="I147">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="J147" t="inlineStr">
         <is>
@@ -15316,13 +15304,13 @@
         <v>45166</v>
       </c>
       <c r="G148">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="H148" s="2">
         <v>45258</v>
       </c>
       <c r="I148">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="J148" t="inlineStr">
         <is>
@@ -15419,13 +15407,13 @@
         <v>45185</v>
       </c>
       <c r="G149">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="H149" s="2">
         <v>45276</v>
       </c>
       <c r="I149">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="J149" t="inlineStr">
         <is>
@@ -15522,13 +15510,13 @@
         <v>45035</v>
       </c>
       <c r="G150">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="H150" s="2">
         <v>45218</v>
       </c>
       <c r="I150">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="J150" t="inlineStr">
         <is>
@@ -15625,13 +15613,13 @@
         <v>45174</v>
       </c>
       <c r="G151">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="H151" s="2">
         <v>45356</v>
       </c>
       <c r="I151">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="J151" t="inlineStr">
         <is>
@@ -15728,13 +15716,13 @@
         <v>45089</v>
       </c>
       <c r="G152">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="H152" s="2">
         <v>45272</v>
       </c>
       <c r="I152">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="J152" t="inlineStr">
         <is>
@@ -15831,13 +15819,13 @@
         <v>45124</v>
       </c>
       <c r="G153">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="H153" s="2">
         <v>45308</v>
       </c>
       <c r="I153">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="J153" t="inlineStr">
         <is>
@@ -15934,13 +15922,13 @@
         <v>45124</v>
       </c>
       <c r="G154">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="H154" s="2">
         <v>45308</v>
       </c>
       <c r="I154">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="J154" t="inlineStr">
         <is>
@@ -16037,13 +16025,13 @@
         <v>45026</v>
       </c>
       <c r="G155">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="H155" s="2">
         <v>45209</v>
       </c>
       <c r="I155">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J155" t="inlineStr">
         <is>
@@ -16140,13 +16128,13 @@
         <v>45026</v>
       </c>
       <c r="G156">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="H156" s="2">
         <v>45209</v>
       </c>
       <c r="I156">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J156" t="inlineStr">
         <is>
@@ -16243,13 +16231,13 @@
         <v>45026</v>
       </c>
       <c r="G157">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="H157" s="2">
         <v>45209</v>
       </c>
       <c r="I157">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J157" t="inlineStr">
         <is>
@@ -16346,13 +16334,13 @@
         <v>45026</v>
       </c>
       <c r="G158">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="H158" s="2">
         <v>45209</v>
       </c>
       <c r="I158">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J158" t="inlineStr">
         <is>
@@ -16449,13 +16437,13 @@
         <v>45156</v>
       </c>
       <c r="G159">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="H159" s="2">
         <v>45247</v>
       </c>
       <c r="I159">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="J159" t="inlineStr">
         <is>
@@ -16552,13 +16540,13 @@
         <v>45153</v>
       </c>
       <c r="G160">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="H160" s="2">
         <v>45245</v>
       </c>
       <c r="I160">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="J160" t="inlineStr">
         <is>
@@ -16655,13 +16643,13 @@
         <v>45135</v>
       </c>
       <c r="G161">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="H161" s="2">
         <v>45319</v>
       </c>
       <c r="I161">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="J161" t="inlineStr">
         <is>
@@ -16758,13 +16746,13 @@
         <v>45091</v>
       </c>
       <c r="G162">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="H162" s="2">
         <v>45274</v>
       </c>
       <c r="I162">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="J162" t="inlineStr">
         <is>
@@ -16856,13 +16844,13 @@
         <v>45091</v>
       </c>
       <c r="G163">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="H163" s="2">
         <v>45274</v>
       </c>
       <c r="I163">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="J163" t="inlineStr">
         <is>
@@ -16954,13 +16942,13 @@
         <v>45138</v>
       </c>
       <c r="G164">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="H164" s="2">
         <v>45322</v>
       </c>
       <c r="I164">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="J164" t="inlineStr">
         <is>
@@ -17057,13 +17045,13 @@
         <v>45138</v>
       </c>
       <c r="G165">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="H165" s="2">
         <v>45322</v>
       </c>
       <c r="I165">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="J165" t="inlineStr">
         <is>
@@ -17160,13 +17148,13 @@
         <v>45085</v>
       </c>
       <c r="G166">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="H166" s="2">
         <v>45268</v>
       </c>
       <c r="I166">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="J166" t="inlineStr">
         <is>
@@ -17263,13 +17251,13 @@
         <v>45085</v>
       </c>
       <c r="G167">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="H167" s="2">
         <v>45268</v>
       </c>
       <c r="I167">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="J167" t="inlineStr">
         <is>
@@ -17366,7 +17354,7 @@
         <v>45326</v>
       </c>
       <c r="I168">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="J168" t="inlineStr">
         <is>
@@ -17463,13 +17451,13 @@
         <v>45173</v>
       </c>
       <c r="G169">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="H169" s="2">
         <v>45355</v>
       </c>
       <c r="I169">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="J169" t="inlineStr">
         <is>
@@ -17566,13 +17554,13 @@
         <v>45056</v>
       </c>
       <c r="G170">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="H170" s="2">
         <v>45240</v>
       </c>
       <c r="I170">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="J170" t="inlineStr">
         <is>
@@ -17669,7 +17657,7 @@
         <v>45238</v>
       </c>
       <c r="I171">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="J171" t="inlineStr">
         <is>
@@ -17766,13 +17754,13 @@
         <v>45141</v>
       </c>
       <c r="G172">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="H172" s="2">
         <v>45325</v>
       </c>
       <c r="I172">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="J172" t="inlineStr">
         <is>
@@ -17869,13 +17857,13 @@
         <v>45037</v>
       </c>
       <c r="G173">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="H173" s="2">
         <v>45220</v>
       </c>
       <c r="I173">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="J173" t="inlineStr">
         <is>
@@ -17972,13 +17960,13 @@
         <v>45171</v>
       </c>
       <c r="G174">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="H174" s="2">
         <v>45262</v>
       </c>
       <c r="I174">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="J174" t="inlineStr">
         <is>
@@ -18075,13 +18063,13 @@
         <v>45197</v>
       </c>
       <c r="G175">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="H175" s="2">
         <v>45288</v>
       </c>
       <c r="I175">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="J175" t="inlineStr">
         <is>
@@ -18178,13 +18166,13 @@
         <v>45162</v>
       </c>
       <c r="G176">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="H176" s="2">
         <v>45254</v>
       </c>
       <c r="I176">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="J176" t="inlineStr">
         <is>
@@ -18281,13 +18269,13 @@
         <v>45061</v>
       </c>
       <c r="G177">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="H177" s="2">
         <v>45245</v>
       </c>
       <c r="I177">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="J177" t="inlineStr">
         <is>
@@ -18384,13 +18372,13 @@
         <v>45120</v>
       </c>
       <c r="G178">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="H178" s="2">
         <v>45212</v>
       </c>
       <c r="I178">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="J178" t="inlineStr">
         <is>
@@ -18487,13 +18475,13 @@
         <v>45191</v>
       </c>
       <c r="G179">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="H179" s="2">
         <v>45282</v>
       </c>
       <c r="I179">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="J179" t="inlineStr">
         <is>
@@ -18590,13 +18578,13 @@
         <v>45088</v>
       </c>
       <c r="G180">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="H180" s="2">
         <v>45271</v>
       </c>
       <c r="I180">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="J180" t="inlineStr">
         <is>
@@ -18693,13 +18681,13 @@
         <v>45192</v>
       </c>
       <c r="G181">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H181" s="2">
         <v>45283</v>
       </c>
       <c r="I181">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="J181" t="inlineStr">
         <is>
@@ -18786,13 +18774,13 @@
         <v>45131</v>
       </c>
       <c r="G182">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="H182" s="2">
         <v>45223</v>
       </c>
       <c r="I182">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="J182" t="inlineStr">
         <is>
@@ -18884,13 +18872,13 @@
         <v>45136</v>
       </c>
       <c r="G183">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="H183" s="2">
         <v>45228</v>
       </c>
       <c r="I183">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="J183" t="inlineStr">
         <is>
@@ -18982,13 +18970,13 @@
         <v>45150</v>
       </c>
       <c r="G184">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="H184" s="2">
         <v>45242</v>
       </c>
       <c r="I184">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="J184" t="inlineStr">
         <is>
@@ -19080,13 +19068,13 @@
         <v>45118</v>
       </c>
       <c r="G185">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="H185" s="2">
         <v>45210</v>
       </c>
       <c r="I185">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="J185" t="inlineStr">
         <is>
@@ -19178,13 +19166,13 @@
         <v>45129</v>
       </c>
       <c r="G186">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="H186" s="2">
         <v>45221</v>
       </c>
       <c r="I186">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="J186" t="inlineStr">
         <is>
@@ -19276,13 +19264,13 @@
         <v>45189</v>
       </c>
       <c r="G187">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="H187" s="2">
         <v>45280</v>
       </c>
       <c r="I187">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="J187" t="inlineStr">
         <is>
@@ -19369,13 +19357,13 @@
         <v>45193</v>
       </c>
       <c r="G188">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="H188" s="2">
         <v>45284</v>
       </c>
       <c r="I188">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="J188" t="inlineStr">
         <is>
@@ -19462,13 +19450,13 @@
         <v>45165</v>
       </c>
       <c r="G189">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="H189" s="2">
         <v>45257</v>
       </c>
       <c r="I189">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="J189" t="inlineStr">
         <is>
@@ -19560,13 +19548,13 @@
         <v>45202</v>
       </c>
       <c r="G190">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="H190" s="2">
         <v>45385</v>
       </c>
       <c r="I190">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="J190" t="inlineStr">
         <is>
@@ -19663,13 +19651,13 @@
         <v>45081</v>
       </c>
       <c r="G191">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="H191" s="2">
         <v>45264</v>
       </c>
       <c r="I191">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="J191" t="inlineStr">
         <is>
@@ -19766,13 +19754,13 @@
         <v>45081</v>
       </c>
       <c r="G192">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="H192" s="2">
         <v>45264</v>
       </c>
       <c r="I192">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="J192" t="inlineStr">
         <is>
@@ -19869,7 +19857,7 @@
         <v>45319</v>
       </c>
       <c r="I193">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="J193" t="inlineStr">
         <is>
@@ -19966,7 +19954,7 @@
         <v>45319</v>
       </c>
       <c r="I194">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="J194" t="inlineStr">
         <is>
@@ -20058,13 +20046,13 @@
         <v>45046</v>
       </c>
       <c r="G195">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="H195" s="2">
         <v>45230</v>
       </c>
       <c r="I195">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="J195" t="inlineStr">
         <is>
@@ -20161,13 +20149,13 @@
         <v>45046</v>
       </c>
       <c r="G196">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="H196" s="2">
         <v>45230</v>
       </c>
       <c r="I196">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="J196" t="inlineStr">
         <is>
@@ -20264,13 +20252,13 @@
         <v>45031</v>
       </c>
       <c r="G197">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="H197" s="2">
         <v>45214</v>
       </c>
       <c r="I197">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="J197" t="inlineStr">
         <is>
@@ -20367,13 +20355,13 @@
         <v>45031</v>
       </c>
       <c r="G198">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="H198" s="2">
         <v>45214</v>
       </c>
       <c r="I198">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="J198" t="inlineStr">
         <is>
@@ -20470,13 +20458,13 @@
         <v>45031</v>
       </c>
       <c r="G199">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="H199" s="2">
         <v>45214</v>
       </c>
       <c r="I199">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="J199" t="inlineStr">
         <is>
@@ -20573,13 +20561,13 @@
         <v>45031</v>
       </c>
       <c r="G200">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="H200" s="2">
         <v>45214</v>
       </c>
       <c r="I200">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="J200" t="inlineStr">
         <is>
@@ -20676,13 +20664,13 @@
         <v>45067</v>
       </c>
       <c r="G201">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="H201" s="2">
         <v>45251</v>
       </c>
       <c r="I201">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="J201" t="inlineStr">
         <is>
@@ -20779,13 +20767,13 @@
         <v>45067</v>
       </c>
       <c r="G202">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="H202" s="2">
         <v>45251</v>
       </c>
       <c r="I202">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="J202" t="inlineStr">
         <is>
@@ -20882,13 +20870,13 @@
         <v>45067</v>
       </c>
       <c r="G203">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="H203" s="2">
         <v>45251</v>
       </c>
       <c r="I203">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="J203" t="inlineStr">
         <is>
@@ -20985,13 +20973,13 @@
         <v>45067</v>
       </c>
       <c r="G204">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="H204" s="2">
         <v>45251</v>
       </c>
       <c r="I204">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="J204" t="inlineStr">
         <is>
@@ -21088,13 +21076,13 @@
         <v>45178</v>
       </c>
       <c r="G205">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="H205" s="2">
         <v>45269</v>
       </c>
       <c r="I205">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="J205" t="inlineStr">
         <is>
@@ -21191,7 +21179,7 @@
         <v>45252</v>
       </c>
       <c r="I206">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="J206" t="inlineStr">
         <is>
@@ -21288,13 +21276,13 @@
         <v>45087</v>
       </c>
       <c r="G207">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="H207" s="2">
         <v>45270</v>
       </c>
       <c r="I207">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="J207" t="inlineStr">
         <is>
@@ -21391,13 +21379,13 @@
         <v>45099</v>
       </c>
       <c r="G208">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="H208" s="2">
         <v>45282</v>
       </c>
       <c r="I208">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="J208" t="inlineStr">
         <is>
@@ -21494,13 +21482,13 @@
         <v>45175</v>
       </c>
       <c r="G209">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="H209" s="2">
         <v>45356</v>
       </c>
       <c r="I209">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="J209" t="inlineStr">
         <is>
@@ -21597,13 +21585,13 @@
         <v>45175</v>
       </c>
       <c r="G210">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="H210" s="2">
         <v>45356</v>
       </c>
       <c r="I210">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="J210" t="inlineStr">
         <is>
@@ -21700,13 +21688,13 @@
         <v>45166</v>
       </c>
       <c r="G211">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="H211" s="2">
         <v>45350</v>
       </c>
       <c r="I211">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="J211" t="inlineStr">
         <is>
@@ -21803,13 +21791,13 @@
         <v>45166</v>
       </c>
       <c r="G212">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="H212" s="2">
         <v>45350</v>
       </c>
       <c r="I212">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="J212" t="inlineStr">
         <is>
@@ -21906,13 +21894,13 @@
         <v>45090</v>
       </c>
       <c r="G213">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="H213" s="2">
         <v>45273</v>
       </c>
       <c r="I213">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="J213" t="inlineStr">
         <is>
@@ -22009,13 +21997,13 @@
         <v>45106</v>
       </c>
       <c r="G214">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="H214" s="2">
         <v>45289</v>
       </c>
       <c r="I214">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="J214" t="inlineStr">
         <is>
@@ -22112,13 +22100,13 @@
         <v>45134</v>
       </c>
       <c r="G215">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="H215" s="2">
         <v>45226</v>
       </c>
       <c r="I215">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="J215" t="inlineStr">
         <is>
@@ -22215,13 +22203,13 @@
         <v>45132</v>
       </c>
       <c r="G216">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="H216" s="2">
         <v>45224</v>
       </c>
       <c r="I216">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="J216" t="inlineStr">
         <is>
@@ -22318,13 +22306,13 @@
         <v>45150</v>
       </c>
       <c r="G217">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="H217" s="2">
         <v>45242</v>
       </c>
       <c r="I217">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="J217" t="inlineStr">
         <is>
@@ -22421,13 +22409,13 @@
         <v>45187</v>
       </c>
       <c r="G218">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="H218" s="2">
         <v>45278</v>
       </c>
       <c r="I218">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="J218" t="inlineStr">
         <is>
@@ -22519,13 +22507,13 @@
         <v>45182</v>
       </c>
       <c r="G219">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="H219" s="2">
         <v>45273</v>
       </c>
       <c r="I219">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="J219" t="inlineStr">
         <is>
@@ -22622,13 +22610,13 @@
         <v>45196</v>
       </c>
       <c r="G220">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="H220" s="2">
         <v>45287</v>
       </c>
       <c r="I220">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="J220" t="inlineStr">
         <is>
@@ -22725,13 +22713,13 @@
         <v>45200</v>
       </c>
       <c r="G221">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="H221" s="2">
         <v>45292</v>
       </c>
       <c r="I221">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="J221" t="inlineStr">
         <is>
@@ -22828,13 +22816,13 @@
         <v>45135</v>
       </c>
       <c r="G222">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="H222" s="2">
         <v>45227</v>
       </c>
       <c r="I222">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="J222" t="inlineStr">
         <is>
@@ -22931,13 +22919,13 @@
         <v>45148</v>
       </c>
       <c r="G223">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="H223" s="2">
         <v>45240</v>
       </c>
       <c r="I223">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="J223" t="inlineStr">
         <is>
@@ -23029,13 +23017,13 @@
         <v>45192</v>
       </c>
       <c r="G224">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H224" s="2">
         <v>45283</v>
       </c>
       <c r="I224">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="J224" t="inlineStr">
         <is>
@@ -23127,13 +23115,13 @@
         <v>45136</v>
       </c>
       <c r="G225">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="H225" s="2">
         <v>45320</v>
       </c>
       <c r="I225">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="J225" t="inlineStr">
         <is>
@@ -23230,13 +23218,13 @@
         <v>45136</v>
       </c>
       <c r="G226">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="H226" s="2">
         <v>45320</v>
       </c>
       <c r="I226">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="J226" t="inlineStr">
         <is>
@@ -23333,13 +23321,13 @@
         <v>45094</v>
       </c>
       <c r="G227">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="H227" s="2">
         <v>45277</v>
       </c>
       <c r="I227">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="J227" t="inlineStr">
         <is>
@@ -23436,13 +23424,13 @@
         <v>45081</v>
       </c>
       <c r="G228">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="H228" s="2">
         <v>45264</v>
       </c>
       <c r="I228">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="J228" t="inlineStr">
         <is>
@@ -23539,13 +23527,13 @@
         <v>45099</v>
       </c>
       <c r="G229">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="H229" s="2">
         <v>45282</v>
       </c>
       <c r="I229">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="J229" t="inlineStr">
         <is>
@@ -23642,13 +23630,13 @@
         <v>45201</v>
       </c>
       <c r="G230">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="H230" s="2">
         <v>45384</v>
       </c>
       <c r="I230">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="J230" t="inlineStr">
         <is>
@@ -23745,13 +23733,13 @@
         <v>45031</v>
       </c>
       <c r="G231">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="H231" s="2">
         <v>45214</v>
       </c>
       <c r="I231">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="J231" t="inlineStr">
         <is>
@@ -23848,7 +23836,7 @@
         <v>45294</v>
       </c>
       <c r="I232">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="J232" t="inlineStr">
         <is>
@@ -23945,13 +23933,13 @@
         <v>45079</v>
       </c>
       <c r="G233">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="H233" s="2">
         <v>45262</v>
       </c>
       <c r="I233">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="J233" t="inlineStr">
         <is>
@@ -24048,13 +24036,13 @@
         <v>45199</v>
       </c>
       <c r="G234">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="H234" s="2">
         <v>45382</v>
       </c>
       <c r="I234">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="J234" t="inlineStr">
         <is>
@@ -24151,13 +24139,13 @@
         <v>45204</v>
       </c>
       <c r="G235">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="H235" s="2">
         <v>45387</v>
       </c>
       <c r="I235">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="J235" t="inlineStr">
         <is>
@@ -24254,13 +24242,13 @@
         <v>45204</v>
       </c>
       <c r="G236">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="H236" s="2">
         <v>45387</v>
       </c>
       <c r="I236">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="J236" t="inlineStr">
         <is>
@@ -24357,13 +24345,13 @@
         <v>45080</v>
       </c>
       <c r="G237">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="H237" s="2">
         <v>45263</v>
       </c>
       <c r="I237">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="J237" t="inlineStr">
         <is>
@@ -24460,13 +24448,13 @@
         <v>45046</v>
       </c>
       <c r="G238">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="H238" s="2">
         <v>45229</v>
       </c>
       <c r="I238">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="J238" t="inlineStr">
         <is>
@@ -24563,13 +24551,13 @@
         <v>45204</v>
       </c>
       <c r="G239">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="H239" s="2">
         <v>45296</v>
       </c>
       <c r="I239">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="J239" t="inlineStr">
         <is>
@@ -24666,13 +24654,13 @@
         <v>45204</v>
       </c>
       <c r="G240">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="H240" s="2">
         <v>45296</v>
       </c>
       <c r="I240">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="J240" t="inlineStr">
         <is>
@@ -24769,13 +24757,13 @@
         <v>45199</v>
       </c>
       <c r="G241">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="H241" s="2">
         <v>45382</v>
       </c>
       <c r="I241">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="J241" t="inlineStr">
         <is>
@@ -24872,13 +24860,13 @@
         <v>45070</v>
       </c>
       <c r="G242">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="H242" s="2">
         <v>45254</v>
       </c>
       <c r="I242">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="J242" t="inlineStr">
         <is>
@@ -24975,13 +24963,13 @@
         <v>45168</v>
       </c>
       <c r="G243">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="H243" s="2">
         <v>45260</v>
       </c>
       <c r="I243">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="J243" t="inlineStr">
         <is>
@@ -25078,13 +25066,13 @@
         <v>45027</v>
       </c>
       <c r="G244">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="H244" s="2">
         <v>45210</v>
       </c>
       <c r="I244">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="J244" t="inlineStr">
         <is>
@@ -25181,13 +25169,13 @@
         <v>45077</v>
       </c>
       <c r="G245">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="H245" s="2">
         <v>45260</v>
       </c>
       <c r="I245">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="J245" t="inlineStr">
         <is>
@@ -25284,13 +25272,13 @@
         <v>45100</v>
       </c>
       <c r="G246">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="H246" s="2">
         <v>45283</v>
       </c>
       <c r="I246">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="J246" t="inlineStr">
         <is>
@@ -25387,7 +25375,7 @@
         <v>45281</v>
       </c>
       <c r="I247">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="J247" t="inlineStr">
         <is>
@@ -25484,13 +25472,13 @@
         <v>45044</v>
       </c>
       <c r="G248">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="H248" s="2">
         <v>45227</v>
       </c>
       <c r="I248">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="J248" t="inlineStr">
         <is>
@@ -25587,13 +25575,13 @@
         <v>45101</v>
       </c>
       <c r="G249">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="H249" s="2">
         <v>45283</v>
       </c>
       <c r="I249">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="J249" t="inlineStr">
         <is>
@@ -25690,13 +25678,13 @@
         <v>45134</v>
       </c>
       <c r="G250">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="H250" s="2">
         <v>45226</v>
       </c>
       <c r="I250">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="J250" t="inlineStr">
         <is>
@@ -25793,13 +25781,13 @@
         <v>45158</v>
       </c>
       <c r="G251">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="H251" s="2">
         <v>45250</v>
       </c>
       <c r="I251">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="J251" t="inlineStr">
         <is>
@@ -25896,13 +25884,13 @@
         <v>45200</v>
       </c>
       <c r="G252">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="H252" s="2">
         <v>45292</v>
       </c>
       <c r="I252">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="J252" t="inlineStr">
         <is>
@@ -25999,7 +25987,7 @@
         <v>45317</v>
       </c>
       <c r="I253">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="J253" t="inlineStr">
         <is>
@@ -26096,13 +26084,13 @@
         <v>45039</v>
       </c>
       <c r="G254">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="H254" s="2">
         <v>45222</v>
       </c>
       <c r="I254">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="J254" t="inlineStr">
         <is>
@@ -26194,13 +26182,13 @@
         <v>45129</v>
       </c>
       <c r="G255">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="H255" s="2">
         <v>45221</v>
       </c>
       <c r="I255">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="J255" t="inlineStr">
         <is>
@@ -26297,13 +26285,13 @@
         <v>45157</v>
       </c>
       <c r="G256">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="H256" s="2">
         <v>45341</v>
       </c>
       <c r="I256">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="J256" t="inlineStr">
         <is>
@@ -26400,13 +26388,13 @@
         <v>45063</v>
       </c>
       <c r="G257">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="H257" s="2">
         <v>45247</v>
       </c>
       <c r="I257">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="J257" t="inlineStr">
         <is>
@@ -26503,7 +26491,7 @@
         <v>45254</v>
       </c>
       <c r="I258">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="J258" t="inlineStr">
         <is>
@@ -26600,7 +26588,7 @@
         <v>45486</v>
       </c>
       <c r="I259">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="J259" t="inlineStr">
         <is>
@@ -26692,13 +26680,13 @@
         <v>45073</v>
       </c>
       <c r="G260">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="H260" s="2">
         <v>45439</v>
       </c>
       <c r="I260">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="J260" t="inlineStr">
         <is>
@@ -26790,7 +26778,7 @@
         <v>45323</v>
       </c>
       <c r="I261">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="J261" t="inlineStr">
         <is>
@@ -26882,7 +26870,7 @@
         <v>45303</v>
       </c>
       <c r="I262">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="J262" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
Bond dates update Tue Oct 10 20:22:19 UTC 2023
</commit_message>
<xml_diff>
--- a/Data/obligacje_screener.xlsx
+++ b/Data/obligacje_screener.xlsx
@@ -512,7 +512,7 @@
         <v>45340</v>
       </c>
       <c r="I2">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="J2" t="inlineStr">
         <is>
@@ -600,13 +600,13 @@
         <v>45121</v>
       </c>
       <c r="G3">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="H3" s="2">
         <v>45305</v>
       </c>
       <c r="I3">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="J3" t="inlineStr">
         <is>
@@ -703,13 +703,13 @@
         <v>45039</v>
       </c>
       <c r="G4">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="H4" s="2">
         <v>45222</v>
       </c>
       <c r="I4">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="J4" t="inlineStr">
         <is>
@@ -806,13 +806,13 @@
         <v>45039</v>
       </c>
       <c r="G5">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="H5" s="2">
         <v>45222</v>
       </c>
       <c r="I5">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="J5" t="inlineStr">
         <is>
@@ -909,13 +909,13 @@
         <v>45129</v>
       </c>
       <c r="G6">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="H6" s="2">
         <v>45221</v>
       </c>
       <c r="I6">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="J6" t="inlineStr">
         <is>
@@ -1012,13 +1012,13 @@
         <v>45162</v>
       </c>
       <c r="G7">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="H7" s="2">
         <v>45254</v>
       </c>
       <c r="I7">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="J7" t="inlineStr">
         <is>
@@ -1110,13 +1110,13 @@
         <v>45156</v>
       </c>
       <c r="G8">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="H8" s="2">
         <v>45248</v>
       </c>
       <c r="I8">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="J8" t="inlineStr">
         <is>
@@ -1213,13 +1213,13 @@
         <v>45141</v>
       </c>
       <c r="G9">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="H9" s="2">
         <v>45233</v>
       </c>
       <c r="I9">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="J9" t="inlineStr">
         <is>
@@ -1316,13 +1316,13 @@
         <v>45062</v>
       </c>
       <c r="G10">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="H10" s="2">
         <v>45246</v>
       </c>
       <c r="I10">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="J10" t="inlineStr">
         <is>
@@ -1419,7 +1419,7 @@
         <v>45286</v>
       </c>
       <c r="I11">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="J11" t="inlineStr">
         <is>
@@ -1516,13 +1516,13 @@
         <v>45195</v>
       </c>
       <c r="G12">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="H12" s="2">
         <v>45377</v>
       </c>
       <c r="I12">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="J12" t="inlineStr">
         <is>
@@ -1614,13 +1614,13 @@
         <v>45036</v>
       </c>
       <c r="G13">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="H13" s="2">
         <v>45219</v>
       </c>
       <c r="I13">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="J13" t="inlineStr">
         <is>
@@ -1717,13 +1717,13 @@
         <v>45036</v>
       </c>
       <c r="G14">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="H14" s="2">
         <v>45219</v>
       </c>
       <c r="I14">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="J14" t="inlineStr">
         <is>
@@ -1820,13 +1820,13 @@
         <v>45106</v>
       </c>
       <c r="G15">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="H15" s="2">
         <v>45289</v>
       </c>
       <c r="I15">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="J15" t="inlineStr">
         <is>
@@ -1923,13 +1923,13 @@
         <v>45186</v>
       </c>
       <c r="G16">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="H16" s="2">
         <v>45278</v>
       </c>
       <c r="I16">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="J16" t="inlineStr">
         <is>
@@ -2026,13 +2026,13 @@
         <v>45186</v>
       </c>
       <c r="G17">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="H17" s="2">
         <v>45277</v>
       </c>
       <c r="I17">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="J17" t="inlineStr">
         <is>
@@ -2129,13 +2129,13 @@
         <v>45132</v>
       </c>
       <c r="G18">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="H18" s="2">
         <v>45224</v>
       </c>
       <c r="I18">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="J18" t="inlineStr">
         <is>
@@ -2232,13 +2232,13 @@
         <v>45137</v>
       </c>
       <c r="G19">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="H19" s="2">
         <v>45229</v>
       </c>
       <c r="I19">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="J19" t="inlineStr">
         <is>
@@ -2330,13 +2330,13 @@
         <v>45183</v>
       </c>
       <c r="G20">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="H20" s="2">
         <v>45274</v>
       </c>
       <c r="I20">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="J20" t="inlineStr">
         <is>
@@ -2433,13 +2433,13 @@
         <v>45187</v>
       </c>
       <c r="G21">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="H21" s="2">
         <v>45278</v>
       </c>
       <c r="I21">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="J21" t="inlineStr">
         <is>
@@ -2536,13 +2536,13 @@
         <v>45187</v>
       </c>
       <c r="G22">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="H22" s="2">
         <v>45278</v>
       </c>
       <c r="I22">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="J22" t="inlineStr">
         <is>
@@ -2639,7 +2639,7 @@
         <v>45245</v>
       </c>
       <c r="I23">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="J23" t="inlineStr">
         <is>
@@ -2736,7 +2736,7 @@
         <v>45245</v>
       </c>
       <c r="I24">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="J24" t="inlineStr">
         <is>
@@ -2833,7 +2833,7 @@
         <v>45204</v>
       </c>
       <c r="G25">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="J25" t="inlineStr">
         <is>
@@ -2930,13 +2930,13 @@
         <v>45160</v>
       </c>
       <c r="G26">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="H26" s="2">
         <v>45344</v>
       </c>
       <c r="I26">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="J26" t="inlineStr">
         <is>
@@ -3033,13 +3033,13 @@
         <v>45118</v>
       </c>
       <c r="G27">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="H27" s="2">
         <v>45302</v>
       </c>
       <c r="I27">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="J27" t="inlineStr">
         <is>
@@ -3136,13 +3136,13 @@
         <v>45085</v>
       </c>
       <c r="G28">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="H28" s="2">
         <v>45268</v>
       </c>
       <c r="I28">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="J28" t="inlineStr">
         <is>
@@ -3239,13 +3239,13 @@
         <v>45183</v>
       </c>
       <c r="G29">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="H29" s="2">
         <v>45274</v>
       </c>
       <c r="I29">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="J29" t="inlineStr">
         <is>
@@ -3342,7 +3342,7 @@
         <v>45224</v>
       </c>
       <c r="I30">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="J30" t="inlineStr">
         <is>
@@ -3439,13 +3439,13 @@
         <v>45153</v>
       </c>
       <c r="G31">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="H31" s="2">
         <v>45245</v>
       </c>
       <c r="I31">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="J31" t="inlineStr">
         <is>
@@ -3542,13 +3542,13 @@
         <v>45155</v>
       </c>
       <c r="G32">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="H32" s="2">
         <v>45247</v>
       </c>
       <c r="I32">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="J32" t="inlineStr">
         <is>
@@ -3645,7 +3645,7 @@
         <v>45255</v>
       </c>
       <c r="I33">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="J33" t="inlineStr">
         <is>
@@ -3742,13 +3742,13 @@
         <v>45176</v>
       </c>
       <c r="G34">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="H34" s="2">
         <v>45267</v>
       </c>
       <c r="I34">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="J34" t="inlineStr">
         <is>
@@ -3845,13 +3845,13 @@
         <v>45130</v>
       </c>
       <c r="G35">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="H35" s="2">
         <v>45222</v>
       </c>
       <c r="I35">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="J35" t="inlineStr">
         <is>
@@ -3943,13 +3943,13 @@
         <v>45207</v>
       </c>
       <c r="G36">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H36" s="2">
         <v>45299</v>
       </c>
       <c r="I36">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="J36" t="inlineStr">
         <is>
@@ -4046,13 +4046,13 @@
         <v>45189</v>
       </c>
       <c r="G37">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="H37" s="2">
         <v>45280</v>
       </c>
       <c r="I37">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="J37" t="inlineStr">
         <is>
@@ -4144,13 +4144,13 @@
         <v>45107</v>
       </c>
       <c r="G38">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="H38" s="2">
         <v>45290</v>
       </c>
       <c r="I38">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="J38" t="inlineStr">
         <is>
@@ -4247,13 +4247,13 @@
         <v>45063</v>
       </c>
       <c r="G39">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="H39" s="2">
         <v>45247</v>
       </c>
       <c r="I39">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="J39" t="inlineStr">
         <is>
@@ -4350,13 +4350,13 @@
         <v>45177</v>
       </c>
       <c r="G40">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="H40" s="2">
         <v>45359</v>
       </c>
       <c r="I40">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="J40" t="inlineStr">
         <is>
@@ -4453,13 +4453,13 @@
         <v>45107</v>
       </c>
       <c r="G41">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="H41" s="2">
         <v>45290</v>
       </c>
       <c r="I41">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="J41" t="inlineStr">
         <is>
@@ -4556,7 +4556,7 @@
         <v>45265</v>
       </c>
       <c r="I42">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="J42" t="inlineStr">
         <is>
@@ -4653,13 +4653,13 @@
         <v>45098</v>
       </c>
       <c r="G43">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="H43" s="2">
         <v>45281</v>
       </c>
       <c r="I43">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="J43" t="inlineStr">
         <is>
@@ -4756,13 +4756,13 @@
         <v>45099</v>
       </c>
       <c r="G44">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="H44" s="2">
         <v>45282</v>
       </c>
       <c r="I44">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="J44" t="inlineStr">
         <is>
@@ -4859,13 +4859,13 @@
         <v>45106</v>
       </c>
       <c r="G45">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="H45" s="2">
         <v>45289</v>
       </c>
       <c r="I45">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="J45" t="inlineStr">
         <is>
@@ -4962,13 +4962,13 @@
         <v>45106</v>
       </c>
       <c r="G46">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="H46" s="2">
         <v>45289</v>
       </c>
       <c r="I46">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="J46" t="inlineStr">
         <is>
@@ -5065,13 +5065,13 @@
         <v>45120</v>
       </c>
       <c r="G47">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="H47" s="2">
         <v>45304</v>
       </c>
       <c r="I47">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="J47" t="inlineStr">
         <is>
@@ -5168,13 +5168,13 @@
         <v>45118</v>
       </c>
       <c r="G48">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="H48" s="2">
         <v>45302</v>
       </c>
       <c r="I48">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="J48" t="inlineStr">
         <is>
@@ -5271,13 +5271,13 @@
         <v>45152</v>
       </c>
       <c r="G49">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="H49" s="2">
         <v>45336</v>
       </c>
       <c r="I49">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="J49" t="inlineStr">
         <is>
@@ -5374,13 +5374,13 @@
         <v>45042</v>
       </c>
       <c r="G50">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="H50" s="2">
         <v>45225</v>
       </c>
       <c r="I50">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="J50" t="inlineStr">
         <is>
@@ -5477,13 +5477,13 @@
         <v>45122</v>
       </c>
       <c r="G51">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="H51" s="2">
         <v>45306</v>
       </c>
       <c r="I51">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="J51" t="inlineStr">
         <is>
@@ -5580,13 +5580,13 @@
         <v>45139</v>
       </c>
       <c r="G52">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="H52" s="2">
         <v>45323</v>
       </c>
       <c r="I52">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="J52" t="inlineStr">
         <is>
@@ -5683,13 +5683,13 @@
         <v>45099</v>
       </c>
       <c r="G53">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="H53" s="2">
         <v>45282</v>
       </c>
       <c r="I53">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="J53" t="inlineStr">
         <is>
@@ -5786,13 +5786,13 @@
         <v>45196</v>
       </c>
       <c r="G54">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="H54" s="2">
         <v>45287</v>
       </c>
       <c r="I54">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="J54" t="inlineStr">
         <is>
@@ -5889,13 +5889,13 @@
         <v>45044</v>
       </c>
       <c r="G55">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="H55" s="2">
         <v>45227</v>
       </c>
       <c r="I55">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="J55" t="inlineStr">
         <is>
@@ -5992,13 +5992,13 @@
         <v>45151</v>
       </c>
       <c r="G56">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="H56" s="2">
         <v>45243</v>
       </c>
       <c r="I56">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="J56" t="inlineStr">
         <is>
@@ -6090,13 +6090,13 @@
         <v>45196</v>
       </c>
       <c r="G57">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="H57" s="2">
         <v>45287</v>
       </c>
       <c r="I57">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="J57" t="inlineStr">
         <is>
@@ -6193,13 +6193,13 @@
         <v>45069</v>
       </c>
       <c r="G58">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="H58" s="2">
         <v>45253</v>
       </c>
       <c r="I58">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="J58" t="inlineStr">
         <is>
@@ -6296,13 +6296,13 @@
         <v>45191</v>
       </c>
       <c r="G59">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="H59" s="2">
         <v>45282</v>
       </c>
       <c r="I59">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="J59" t="inlineStr">
         <is>
@@ -6394,7 +6394,7 @@
         <v>45205</v>
       </c>
       <c r="G60">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="J60" t="inlineStr">
         <is>
@@ -6491,13 +6491,13 @@
         <v>45127</v>
       </c>
       <c r="G61">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="H61" s="2">
         <v>45219</v>
       </c>
       <c r="I61">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="J61" t="inlineStr">
         <is>
@@ -6594,13 +6594,13 @@
         <v>45058</v>
       </c>
       <c r="G62">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="H62" s="2">
         <v>45242</v>
       </c>
       <c r="I62">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="J62" t="inlineStr">
         <is>
@@ -6697,13 +6697,13 @@
         <v>45194</v>
       </c>
       <c r="G63">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="H63" s="2">
         <v>45376</v>
       </c>
       <c r="I63">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="J63" t="inlineStr">
         <is>
@@ -6792,10 +6792,10 @@
         </is>
       </c>
       <c r="F64" s="2">
-        <v>45025</v>
+        <v>45208</v>
       </c>
       <c r="G64">
-        <v>183</v>
+        <v>1</v>
       </c>
       <c r="J64" t="inlineStr">
         <is>
@@ -6889,10 +6889,10 @@
         </is>
       </c>
       <c r="F65" s="2">
-        <v>45025</v>
+        <v>45208</v>
       </c>
       <c r="G65">
-        <v>183</v>
+        <v>1</v>
       </c>
       <c r="J65" t="inlineStr">
         <is>
@@ -6989,13 +6989,13 @@
         <v>45089</v>
       </c>
       <c r="G66">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="H66" s="2">
         <v>45272</v>
       </c>
       <c r="I66">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="J66" t="inlineStr">
         <is>
@@ -7092,13 +7092,13 @@
         <v>45178</v>
       </c>
       <c r="G67">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="H67" s="2">
         <v>45269</v>
       </c>
       <c r="I67">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="J67" t="inlineStr">
         <is>
@@ -7190,13 +7190,13 @@
         <v>45196</v>
       </c>
       <c r="G68">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="H68" s="2">
         <v>45287</v>
       </c>
       <c r="I68">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="J68" t="inlineStr">
         <is>
@@ -7293,13 +7293,13 @@
         <v>45149</v>
       </c>
       <c r="G69">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="H69" s="2">
         <v>45241</v>
       </c>
       <c r="I69">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="J69" t="inlineStr">
         <is>
@@ -7396,13 +7396,13 @@
         <v>45205</v>
       </c>
       <c r="G70">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="H70" s="2">
         <v>45296</v>
       </c>
       <c r="I70">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="J70" t="inlineStr">
         <is>
@@ -7499,7 +7499,7 @@
         <v>45205</v>
       </c>
       <c r="G71">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="J71" t="inlineStr">
         <is>
@@ -7596,13 +7596,13 @@
         <v>45207</v>
       </c>
       <c r="G72">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H72" s="2">
         <v>45299</v>
       </c>
       <c r="I72">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="J72" t="inlineStr">
         <is>
@@ -7699,13 +7699,13 @@
         <v>45189</v>
       </c>
       <c r="G73">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="H73" s="2">
         <v>45280</v>
       </c>
       <c r="I73">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="J73" t="inlineStr">
         <is>
@@ -7797,13 +7797,13 @@
         <v>45038</v>
       </c>
       <c r="G74">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="H74" s="2">
         <v>45221</v>
       </c>
       <c r="I74">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="J74" t="inlineStr">
         <is>
@@ -7895,13 +7895,13 @@
         <v>45117</v>
       </c>
       <c r="G75">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="H75" s="2">
         <v>45301</v>
       </c>
       <c r="I75">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="J75" t="inlineStr">
         <is>
@@ -7998,13 +7998,13 @@
         <v>45160</v>
       </c>
       <c r="G76">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="H76" s="2">
         <v>45344</v>
       </c>
       <c r="I76">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="J76" t="inlineStr">
         <is>
@@ -8101,13 +8101,13 @@
         <v>45186</v>
       </c>
       <c r="G77">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="H77" s="2">
         <v>45368</v>
       </c>
       <c r="I77">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="J77" t="inlineStr">
         <is>
@@ -8204,13 +8204,13 @@
         <v>45043</v>
       </c>
       <c r="G78">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="H78" s="2">
         <v>45226</v>
       </c>
       <c r="I78">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="J78" t="inlineStr">
         <is>
@@ -8307,13 +8307,13 @@
         <v>45079</v>
       </c>
       <c r="G79">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="H79" s="2">
         <v>45262</v>
       </c>
       <c r="I79">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="J79" t="inlineStr">
         <is>
@@ -8410,7 +8410,7 @@
         <v>45254</v>
       </c>
       <c r="I80">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="J80" t="inlineStr">
         <is>
@@ -8507,13 +8507,13 @@
         <v>45104</v>
       </c>
       <c r="G81">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="H81" s="2">
         <v>45287</v>
       </c>
       <c r="I81">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="J81" t="inlineStr">
         <is>
@@ -8610,7 +8610,7 @@
         <v>45288</v>
       </c>
       <c r="I82">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="J82" t="inlineStr">
         <is>
@@ -8702,13 +8702,13 @@
         <v>45175</v>
       </c>
       <c r="G83">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="H83" s="2">
         <v>45357</v>
       </c>
       <c r="I83">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="J83" t="inlineStr">
         <is>
@@ -8805,13 +8805,13 @@
         <v>45054</v>
       </c>
       <c r="G84">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="H84" s="2">
         <v>45238</v>
       </c>
       <c r="I84">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="J84" t="inlineStr">
         <is>
@@ -8908,13 +8908,13 @@
         <v>45056</v>
       </c>
       <c r="G85">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="H85" s="2">
         <v>45240</v>
       </c>
       <c r="I85">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="J85" t="inlineStr">
         <is>
@@ -9011,13 +9011,13 @@
         <v>45085</v>
       </c>
       <c r="G86">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="H86" s="2">
         <v>45268</v>
       </c>
       <c r="I86">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="J86" t="inlineStr">
         <is>
@@ -9114,13 +9114,13 @@
         <v>45194</v>
       </c>
       <c r="G87">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="H87" s="2">
         <v>45560</v>
       </c>
       <c r="I87">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="J87" t="inlineStr">
         <is>
@@ -9207,13 +9207,13 @@
         <v>45103</v>
       </c>
       <c r="G88">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="H88" s="2">
         <v>45286</v>
       </c>
       <c r="I88">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="J88" t="inlineStr">
         <is>
@@ -9310,13 +9310,13 @@
         <v>45103</v>
       </c>
       <c r="G89">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="H89" s="2">
         <v>45286</v>
       </c>
       <c r="I89">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="J89" t="inlineStr">
         <is>
@@ -9413,13 +9413,13 @@
         <v>45192</v>
       </c>
       <c r="G90">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="H90" s="2">
         <v>45374</v>
       </c>
       <c r="I90">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="J90" t="inlineStr">
         <is>
@@ -9511,13 +9511,13 @@
         <v>45100</v>
       </c>
       <c r="G91">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="H91" s="2">
         <v>45287</v>
       </c>
       <c r="I91">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="J91" t="inlineStr">
         <is>
@@ -9614,13 +9614,13 @@
         <v>45187</v>
       </c>
       <c r="G92">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="H92" s="2">
         <v>45369</v>
       </c>
       <c r="I92">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="J92" t="inlineStr">
         <is>
@@ -9717,13 +9717,13 @@
         <v>45104</v>
       </c>
       <c r="G93">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="H93" s="2">
         <v>45287</v>
       </c>
       <c r="I93">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="J93" t="inlineStr">
         <is>
@@ -9820,13 +9820,13 @@
         <v>45104</v>
       </c>
       <c r="G94">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="H94" s="2">
         <v>45287</v>
       </c>
       <c r="I94">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="J94" t="inlineStr">
         <is>
@@ -9923,13 +9923,13 @@
         <v>45049</v>
       </c>
       <c r="G95">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="H95" s="2">
         <v>45233</v>
       </c>
       <c r="I95">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="J95" t="inlineStr">
         <is>
@@ -10026,13 +10026,13 @@
         <v>45122</v>
       </c>
       <c r="G96">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="H96" s="2">
         <v>45306</v>
       </c>
       <c r="I96">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="J96" t="inlineStr">
         <is>
@@ -10124,13 +10124,13 @@
         <v>45141</v>
       </c>
       <c r="G97">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="H97" s="2">
         <v>45325</v>
       </c>
       <c r="I97">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="J97" t="inlineStr">
         <is>
@@ -10227,13 +10227,13 @@
         <v>45194</v>
       </c>
       <c r="G98">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="H98" s="2">
         <v>45376</v>
       </c>
       <c r="I98">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="J98" t="inlineStr">
         <is>
@@ -10325,13 +10325,13 @@
         <v>45093</v>
       </c>
       <c r="G99">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="H99" s="2">
         <v>45276</v>
       </c>
       <c r="I99">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="J99" t="inlineStr">
         <is>
@@ -10428,13 +10428,13 @@
         <v>45123</v>
       </c>
       <c r="G100">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="H100" s="2">
         <v>45307</v>
       </c>
       <c r="I100">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="J100" t="inlineStr">
         <is>
@@ -10531,13 +10531,13 @@
         <v>45198</v>
       </c>
       <c r="G101">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="H101" s="2">
         <v>45380</v>
       </c>
       <c r="I101">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="J101" t="inlineStr">
         <is>
@@ -10634,13 +10634,13 @@
         <v>45093</v>
       </c>
       <c r="G102">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="H102" s="2">
         <v>45276</v>
       </c>
       <c r="I102">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="J102" t="inlineStr">
         <is>
@@ -10737,13 +10737,13 @@
         <v>45122</v>
       </c>
       <c r="G103">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="H103" s="2">
         <v>45306</v>
       </c>
       <c r="I103">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="J103" t="inlineStr">
         <is>
@@ -10840,13 +10840,13 @@
         <v>45122</v>
       </c>
       <c r="G104">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="H104" s="2">
         <v>45306</v>
       </c>
       <c r="I104">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="J104" t="inlineStr">
         <is>
@@ -10938,13 +10938,13 @@
         <v>45050</v>
       </c>
       <c r="G105">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="H105" s="2">
         <v>45234</v>
       </c>
       <c r="I105">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="J105" t="inlineStr">
         <is>
@@ -11041,13 +11041,13 @@
         <v>45085</v>
       </c>
       <c r="G106">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="H106" s="2">
         <v>45268</v>
       </c>
       <c r="I106">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="J106" t="inlineStr">
         <is>
@@ -11144,13 +11144,13 @@
         <v>45185</v>
       </c>
       <c r="G107">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="H107" s="2">
         <v>45276</v>
       </c>
       <c r="I107">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="J107" t="inlineStr">
         <is>
@@ -11242,13 +11242,13 @@
         <v>45185</v>
       </c>
       <c r="G108">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="H108" s="2">
         <v>45276</v>
       </c>
       <c r="I108">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="J108" t="inlineStr">
         <is>
@@ -11340,13 +11340,13 @@
         <v>45185</v>
       </c>
       <c r="G109">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="H109" s="2">
         <v>45276</v>
       </c>
       <c r="I109">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="J109" t="inlineStr">
         <is>
@@ -11443,13 +11443,13 @@
         <v>45148</v>
       </c>
       <c r="G110">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="H110" s="2">
         <v>45240</v>
       </c>
       <c r="I110">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="J110" t="inlineStr">
         <is>
@@ -11546,13 +11546,13 @@
         <v>45119</v>
       </c>
       <c r="G111">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="H111" s="2">
         <v>45211</v>
       </c>
       <c r="I111">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="J111" t="inlineStr">
         <is>
@@ -11649,13 +11649,13 @@
         <v>45172</v>
       </c>
       <c r="G112">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="H112" s="2">
         <v>45263</v>
       </c>
       <c r="I112">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="J112" t="inlineStr">
         <is>
@@ -11752,13 +11752,13 @@
         <v>45206</v>
       </c>
       <c r="G113">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H113" s="2">
         <v>45389</v>
       </c>
       <c r="I113">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="J113" t="inlineStr">
         <is>
@@ -11855,13 +11855,13 @@
         <v>45203</v>
       </c>
       <c r="G114">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="H114" s="2">
         <v>45295</v>
       </c>
       <c r="I114">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="J114" t="inlineStr">
         <is>
@@ -11958,7 +11958,7 @@
         <v>45218</v>
       </c>
       <c r="I115">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="J115" t="inlineStr">
         <is>
@@ -12055,13 +12055,13 @@
         <v>45161</v>
       </c>
       <c r="G116">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="H116" s="2">
         <v>45253</v>
       </c>
       <c r="I116">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="J116" t="inlineStr">
         <is>
@@ -12158,13 +12158,13 @@
         <v>45115</v>
       </c>
       <c r="G117">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="H117" s="2">
         <v>45299</v>
       </c>
       <c r="I117">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="J117" t="inlineStr">
         <is>
@@ -12256,13 +12256,13 @@
         <v>45094</v>
       </c>
       <c r="G118">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="H118" s="2">
         <v>45277</v>
       </c>
       <c r="I118">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="J118" t="inlineStr">
         <is>
@@ -12359,13 +12359,13 @@
         <v>45104</v>
       </c>
       <c r="G119">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="H119" s="2">
         <v>45287</v>
       </c>
       <c r="I119">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="J119" t="inlineStr">
         <is>
@@ -12462,13 +12462,13 @@
         <v>45104</v>
       </c>
       <c r="G120">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="H120" s="2">
         <v>45287</v>
       </c>
       <c r="I120">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="J120" t="inlineStr">
         <is>
@@ -12565,13 +12565,13 @@
         <v>45104</v>
       </c>
       <c r="G121">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="H121" s="2">
         <v>45287</v>
       </c>
       <c r="I121">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="J121" t="inlineStr">
         <is>
@@ -12668,13 +12668,13 @@
         <v>45104</v>
       </c>
       <c r="G122">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="H122" s="2">
         <v>45287</v>
       </c>
       <c r="I122">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="J122" t="inlineStr">
         <is>
@@ -12771,13 +12771,13 @@
         <v>45199</v>
       </c>
       <c r="G123">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="H123" s="2">
         <v>45291</v>
       </c>
       <c r="I123">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="J123" t="inlineStr">
         <is>
@@ -12874,13 +12874,13 @@
         <v>45197</v>
       </c>
       <c r="G124">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="H124" s="2">
         <v>45379</v>
       </c>
       <c r="I124">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="J124" t="inlineStr">
         <is>
@@ -12977,13 +12977,13 @@
         <v>45121</v>
       </c>
       <c r="G125">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="H125" s="2">
         <v>45213</v>
       </c>
       <c r="I125">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="J125" t="inlineStr">
         <is>
@@ -13080,13 +13080,13 @@
         <v>45134</v>
       </c>
       <c r="G126">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="H126" s="2">
         <v>45226</v>
       </c>
       <c r="I126">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="J126" t="inlineStr">
         <is>
@@ -13183,7 +13183,7 @@
         <v>45212</v>
       </c>
       <c r="I127">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="J127" t="inlineStr">
         <is>
@@ -13280,13 +13280,13 @@
         <v>45126</v>
       </c>
       <c r="G128">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="H128" s="2">
         <v>45218</v>
       </c>
       <c r="I128">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="J128" t="inlineStr">
         <is>
@@ -13378,13 +13378,13 @@
         <v>45158</v>
       </c>
       <c r="G129">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="H129" s="2">
         <v>45250</v>
       </c>
       <c r="I129">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="J129" t="inlineStr">
         <is>
@@ -13481,13 +13481,13 @@
         <v>45171</v>
       </c>
       <c r="G130">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="H130" s="2">
         <v>45262</v>
       </c>
       <c r="I130">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="J130" t="inlineStr">
         <is>
@@ -13584,13 +13584,13 @@
         <v>45203</v>
       </c>
       <c r="G131">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="H131" s="2">
         <v>45295</v>
       </c>
       <c r="I131">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="J131" t="inlineStr">
         <is>
@@ -13687,13 +13687,13 @@
         <v>45144</v>
       </c>
       <c r="G132">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="H132" s="2">
         <v>45236</v>
       </c>
       <c r="I132">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="J132" t="inlineStr">
         <is>
@@ -13790,13 +13790,13 @@
         <v>45156</v>
       </c>
       <c r="G133">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="H133" s="2">
         <v>45248</v>
       </c>
       <c r="I133">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="J133" t="inlineStr">
         <is>
@@ -13888,13 +13888,13 @@
         <v>45146</v>
       </c>
       <c r="G134">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="H134" s="2">
         <v>45238</v>
       </c>
       <c r="I134">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="J134" t="inlineStr">
         <is>
@@ -13991,13 +13991,13 @@
         <v>45140</v>
       </c>
       <c r="G135">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="H135" s="2">
         <v>45232</v>
       </c>
       <c r="I135">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="J135" t="inlineStr">
         <is>
@@ -14094,13 +14094,13 @@
         <v>45196</v>
       </c>
       <c r="G136">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="H136" s="2">
         <v>45287</v>
       </c>
       <c r="I136">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="J136" t="inlineStr">
         <is>
@@ -14197,13 +14197,13 @@
         <v>45197</v>
       </c>
       <c r="G137">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="H137" s="2">
         <v>45288</v>
       </c>
       <c r="I137">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="J137" t="inlineStr">
         <is>
@@ -14300,13 +14300,13 @@
         <v>45179</v>
       </c>
       <c r="G138">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="H138" s="2">
         <v>45270</v>
       </c>
       <c r="I138">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="J138" t="inlineStr">
         <is>
@@ -14398,13 +14398,13 @@
         <v>45197</v>
       </c>
       <c r="G139">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="H139" s="2">
         <v>45288</v>
       </c>
       <c r="I139">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="J139" t="inlineStr">
         <is>
@@ -14501,13 +14501,13 @@
         <v>45182</v>
       </c>
       <c r="G140">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="H140" s="2">
         <v>45273</v>
       </c>
       <c r="I140">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="J140" t="inlineStr">
         <is>
@@ -14601,16 +14601,16 @@
         </is>
       </c>
       <c r="F141" s="2">
-        <v>45116</v>
+        <v>45208</v>
       </c>
       <c r="G141">
-        <v>92</v>
+        <v>1</v>
       </c>
       <c r="H141" s="2">
         <v>45300</v>
       </c>
       <c r="I141">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="J141" t="inlineStr">
         <is>
@@ -14702,13 +14702,13 @@
         <v>45150</v>
       </c>
       <c r="G142">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="H142" s="2">
         <v>45242</v>
       </c>
       <c r="I142">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="J142" t="inlineStr">
         <is>
@@ -14805,7 +14805,7 @@
         <v>45238</v>
       </c>
       <c r="I143">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="J143" t="inlineStr">
         <is>
@@ -14902,13 +14902,13 @@
         <v>45171</v>
       </c>
       <c r="G144">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="H144" s="2">
         <v>45262</v>
       </c>
       <c r="I144">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="J144" t="inlineStr">
         <is>
@@ -15005,13 +15005,13 @@
         <v>45194</v>
       </c>
       <c r="G145">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="H145" s="2">
         <v>45285</v>
       </c>
       <c r="I145">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="J145" t="inlineStr">
         <is>
@@ -15098,13 +15098,13 @@
         <v>45119</v>
       </c>
       <c r="G146">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="H146" s="2">
         <v>45211</v>
       </c>
       <c r="I146">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="J146" t="inlineStr">
         <is>
@@ -15201,13 +15201,13 @@
         <v>45165</v>
       </c>
       <c r="G147">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="H147" s="2">
         <v>45257</v>
       </c>
       <c r="I147">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="J147" t="inlineStr">
         <is>
@@ -15304,13 +15304,13 @@
         <v>45166</v>
       </c>
       <c r="G148">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="H148" s="2">
         <v>45258</v>
       </c>
       <c r="I148">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="J148" t="inlineStr">
         <is>
@@ -15407,13 +15407,13 @@
         <v>45185</v>
       </c>
       <c r="G149">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="H149" s="2">
         <v>45276</v>
       </c>
       <c r="I149">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="J149" t="inlineStr">
         <is>
@@ -15510,13 +15510,13 @@
         <v>45035</v>
       </c>
       <c r="G150">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="H150" s="2">
         <v>45218</v>
       </c>
       <c r="I150">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="J150" t="inlineStr">
         <is>
@@ -15613,13 +15613,13 @@
         <v>45174</v>
       </c>
       <c r="G151">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="H151" s="2">
         <v>45356</v>
       </c>
       <c r="I151">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="J151" t="inlineStr">
         <is>
@@ -15716,13 +15716,13 @@
         <v>45089</v>
       </c>
       <c r="G152">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="H152" s="2">
         <v>45272</v>
       </c>
       <c r="I152">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="J152" t="inlineStr">
         <is>
@@ -15819,13 +15819,13 @@
         <v>45124</v>
       </c>
       <c r="G153">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="H153" s="2">
         <v>45308</v>
       </c>
       <c r="I153">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="J153" t="inlineStr">
         <is>
@@ -15922,13 +15922,13 @@
         <v>45124</v>
       </c>
       <c r="G154">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="H154" s="2">
         <v>45308</v>
       </c>
       <c r="I154">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="J154" t="inlineStr">
         <is>
@@ -16025,13 +16025,13 @@
         <v>45026</v>
       </c>
       <c r="G155">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="H155" s="2">
-        <v>45209</v>
+        <v>45392</v>
       </c>
       <c r="I155">
-        <v>1</v>
+        <v>183</v>
       </c>
       <c r="J155" t="inlineStr">
         <is>
@@ -16128,13 +16128,13 @@
         <v>45026</v>
       </c>
       <c r="G156">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="H156" s="2">
-        <v>45209</v>
+        <v>45392</v>
       </c>
       <c r="I156">
-        <v>1</v>
+        <v>183</v>
       </c>
       <c r="J156" t="inlineStr">
         <is>
@@ -16231,13 +16231,13 @@
         <v>45026</v>
       </c>
       <c r="G157">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="H157" s="2">
-        <v>45209</v>
+        <v>45392</v>
       </c>
       <c r="I157">
-        <v>1</v>
+        <v>183</v>
       </c>
       <c r="J157" t="inlineStr">
         <is>
@@ -16334,13 +16334,13 @@
         <v>45026</v>
       </c>
       <c r="G158">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="H158" s="2">
-        <v>45209</v>
+        <v>45392</v>
       </c>
       <c r="I158">
-        <v>1</v>
+        <v>183</v>
       </c>
       <c r="J158" t="inlineStr">
         <is>
@@ -16437,13 +16437,13 @@
         <v>45156</v>
       </c>
       <c r="G159">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="H159" s="2">
         <v>45247</v>
       </c>
       <c r="I159">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="J159" t="inlineStr">
         <is>
@@ -16540,13 +16540,13 @@
         <v>45153</v>
       </c>
       <c r="G160">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="H160" s="2">
         <v>45245</v>
       </c>
       <c r="I160">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="J160" t="inlineStr">
         <is>
@@ -16643,13 +16643,13 @@
         <v>45135</v>
       </c>
       <c r="G161">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="H161" s="2">
         <v>45319</v>
       </c>
       <c r="I161">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="J161" t="inlineStr">
         <is>
@@ -16746,13 +16746,13 @@
         <v>45091</v>
       </c>
       <c r="G162">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="H162" s="2">
         <v>45274</v>
       </c>
       <c r="I162">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="J162" t="inlineStr">
         <is>
@@ -16844,13 +16844,13 @@
         <v>45091</v>
       </c>
       <c r="G163">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="H163" s="2">
         <v>45274</v>
       </c>
       <c r="I163">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="J163" t="inlineStr">
         <is>
@@ -16942,13 +16942,13 @@
         <v>45138</v>
       </c>
       <c r="G164">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="H164" s="2">
         <v>45322</v>
       </c>
       <c r="I164">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="J164" t="inlineStr">
         <is>
@@ -17045,13 +17045,13 @@
         <v>45138</v>
       </c>
       <c r="G165">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="H165" s="2">
         <v>45322</v>
       </c>
       <c r="I165">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="J165" t="inlineStr">
         <is>
@@ -17148,13 +17148,13 @@
         <v>45085</v>
       </c>
       <c r="G166">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="H166" s="2">
         <v>45268</v>
       </c>
       <c r="I166">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="J166" t="inlineStr">
         <is>
@@ -17251,13 +17251,13 @@
         <v>45085</v>
       </c>
       <c r="G167">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="H167" s="2">
         <v>45268</v>
       </c>
       <c r="I167">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="J167" t="inlineStr">
         <is>
@@ -17354,7 +17354,7 @@
         <v>45326</v>
       </c>
       <c r="I168">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="J168" t="inlineStr">
         <is>
@@ -17451,13 +17451,13 @@
         <v>45173</v>
       </c>
       <c r="G169">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="H169" s="2">
         <v>45355</v>
       </c>
       <c r="I169">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="J169" t="inlineStr">
         <is>
@@ -17554,13 +17554,13 @@
         <v>45056</v>
       </c>
       <c r="G170">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="H170" s="2">
         <v>45240</v>
       </c>
       <c r="I170">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="J170" t="inlineStr">
         <is>
@@ -17657,7 +17657,7 @@
         <v>45238</v>
       </c>
       <c r="I171">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="J171" t="inlineStr">
         <is>
@@ -17754,13 +17754,13 @@
         <v>45141</v>
       </c>
       <c r="G172">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="H172" s="2">
         <v>45325</v>
       </c>
       <c r="I172">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="J172" t="inlineStr">
         <is>
@@ -17857,13 +17857,13 @@
         <v>45037</v>
       </c>
       <c r="G173">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="H173" s="2">
         <v>45220</v>
       </c>
       <c r="I173">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="J173" t="inlineStr">
         <is>
@@ -17960,13 +17960,13 @@
         <v>45171</v>
       </c>
       <c r="G174">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="H174" s="2">
         <v>45262</v>
       </c>
       <c r="I174">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="J174" t="inlineStr">
         <is>
@@ -18063,13 +18063,13 @@
         <v>45197</v>
       </c>
       <c r="G175">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="H175" s="2">
         <v>45288</v>
       </c>
       <c r="I175">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="J175" t="inlineStr">
         <is>
@@ -18166,13 +18166,13 @@
         <v>45162</v>
       </c>
       <c r="G176">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="H176" s="2">
         <v>45254</v>
       </c>
       <c r="I176">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="J176" t="inlineStr">
         <is>
@@ -18269,13 +18269,13 @@
         <v>45061</v>
       </c>
       <c r="G177">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="H177" s="2">
         <v>45245</v>
       </c>
       <c r="I177">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="J177" t="inlineStr">
         <is>
@@ -18372,13 +18372,13 @@
         <v>45120</v>
       </c>
       <c r="G178">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="H178" s="2">
         <v>45212</v>
       </c>
       <c r="I178">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="J178" t="inlineStr">
         <is>
@@ -18475,13 +18475,13 @@
         <v>45191</v>
       </c>
       <c r="G179">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="H179" s="2">
         <v>45282</v>
       </c>
       <c r="I179">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="J179" t="inlineStr">
         <is>
@@ -18578,13 +18578,13 @@
         <v>45088</v>
       </c>
       <c r="G180">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="H180" s="2">
         <v>45271</v>
       </c>
       <c r="I180">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="J180" t="inlineStr">
         <is>
@@ -18681,13 +18681,13 @@
         <v>45192</v>
       </c>
       <c r="G181">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="H181" s="2">
         <v>45283</v>
       </c>
       <c r="I181">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="J181" t="inlineStr">
         <is>
@@ -18774,13 +18774,13 @@
         <v>45131</v>
       </c>
       <c r="G182">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="H182" s="2">
         <v>45223</v>
       </c>
       <c r="I182">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="J182" t="inlineStr">
         <is>
@@ -18872,13 +18872,13 @@
         <v>45136</v>
       </c>
       <c r="G183">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="H183" s="2">
         <v>45228</v>
       </c>
       <c r="I183">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="J183" t="inlineStr">
         <is>
@@ -18970,13 +18970,13 @@
         <v>45150</v>
       </c>
       <c r="G184">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="H184" s="2">
         <v>45242</v>
       </c>
       <c r="I184">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="J184" t="inlineStr">
         <is>
@@ -19068,13 +19068,13 @@
         <v>45118</v>
       </c>
       <c r="G185">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="H185" s="2">
         <v>45210</v>
       </c>
       <c r="I185">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J185" t="inlineStr">
         <is>
@@ -19166,13 +19166,13 @@
         <v>45129</v>
       </c>
       <c r="G186">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="H186" s="2">
         <v>45221</v>
       </c>
       <c r="I186">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="J186" t="inlineStr">
         <is>
@@ -19264,13 +19264,13 @@
         <v>45189</v>
       </c>
       <c r="G187">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="H187" s="2">
         <v>45280</v>
       </c>
       <c r="I187">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="J187" t="inlineStr">
         <is>
@@ -19357,13 +19357,13 @@
         <v>45193</v>
       </c>
       <c r="G188">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H188" s="2">
         <v>45284</v>
       </c>
       <c r="I188">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="J188" t="inlineStr">
         <is>
@@ -19450,13 +19450,13 @@
         <v>45165</v>
       </c>
       <c r="G189">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="H189" s="2">
         <v>45257</v>
       </c>
       <c r="I189">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="J189" t="inlineStr">
         <is>
@@ -19548,13 +19548,13 @@
         <v>45202</v>
       </c>
       <c r="G190">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="H190" s="2">
         <v>45385</v>
       </c>
       <c r="I190">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="J190" t="inlineStr">
         <is>
@@ -19651,13 +19651,13 @@
         <v>45081</v>
       </c>
       <c r="G191">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="H191" s="2">
         <v>45264</v>
       </c>
       <c r="I191">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="J191" t="inlineStr">
         <is>
@@ -19754,13 +19754,13 @@
         <v>45081</v>
       </c>
       <c r="G192">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="H192" s="2">
         <v>45264</v>
       </c>
       <c r="I192">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="J192" t="inlineStr">
         <is>
@@ -19857,7 +19857,7 @@
         <v>45319</v>
       </c>
       <c r="I193">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="J193" t="inlineStr">
         <is>
@@ -19954,7 +19954,7 @@
         <v>45319</v>
       </c>
       <c r="I194">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="J194" t="inlineStr">
         <is>
@@ -20046,13 +20046,13 @@
         <v>45046</v>
       </c>
       <c r="G195">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="H195" s="2">
         <v>45230</v>
       </c>
       <c r="I195">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="J195" t="inlineStr">
         <is>
@@ -20149,13 +20149,13 @@
         <v>45046</v>
       </c>
       <c r="G196">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="H196" s="2">
         <v>45230</v>
       </c>
       <c r="I196">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="J196" t="inlineStr">
         <is>
@@ -20252,13 +20252,13 @@
         <v>45031</v>
       </c>
       <c r="G197">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="H197" s="2">
         <v>45214</v>
       </c>
       <c r="I197">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="J197" t="inlineStr">
         <is>
@@ -20355,13 +20355,13 @@
         <v>45031</v>
       </c>
       <c r="G198">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="H198" s="2">
         <v>45214</v>
       </c>
       <c r="I198">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="J198" t="inlineStr">
         <is>
@@ -20458,13 +20458,13 @@
         <v>45031</v>
       </c>
       <c r="G199">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="H199" s="2">
         <v>45214</v>
       </c>
       <c r="I199">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="J199" t="inlineStr">
         <is>
@@ -20561,13 +20561,13 @@
         <v>45031</v>
       </c>
       <c r="G200">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="H200" s="2">
         <v>45214</v>
       </c>
       <c r="I200">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="J200" t="inlineStr">
         <is>
@@ -20664,13 +20664,13 @@
         <v>45067</v>
       </c>
       <c r="G201">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="H201" s="2">
         <v>45251</v>
       </c>
       <c r="I201">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="J201" t="inlineStr">
         <is>
@@ -20767,13 +20767,13 @@
         <v>45067</v>
       </c>
       <c r="G202">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="H202" s="2">
         <v>45251</v>
       </c>
       <c r="I202">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="J202" t="inlineStr">
         <is>
@@ -20870,13 +20870,13 @@
         <v>45067</v>
       </c>
       <c r="G203">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="H203" s="2">
         <v>45251</v>
       </c>
       <c r="I203">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="J203" t="inlineStr">
         <is>
@@ -20973,13 +20973,13 @@
         <v>45067</v>
       </c>
       <c r="G204">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="H204" s="2">
         <v>45251</v>
       </c>
       <c r="I204">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="J204" t="inlineStr">
         <is>
@@ -21076,13 +21076,13 @@
         <v>45178</v>
       </c>
       <c r="G205">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="H205" s="2">
         <v>45269</v>
       </c>
       <c r="I205">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="J205" t="inlineStr">
         <is>
@@ -21179,7 +21179,7 @@
         <v>45252</v>
       </c>
       <c r="I206">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="J206" t="inlineStr">
         <is>
@@ -21276,13 +21276,13 @@
         <v>45087</v>
       </c>
       <c r="G207">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="H207" s="2">
         <v>45270</v>
       </c>
       <c r="I207">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="J207" t="inlineStr">
         <is>
@@ -21379,13 +21379,13 @@
         <v>45099</v>
       </c>
       <c r="G208">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="H208" s="2">
         <v>45282</v>
       </c>
       <c r="I208">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="J208" t="inlineStr">
         <is>
@@ -21482,13 +21482,13 @@
         <v>45175</v>
       </c>
       <c r="G209">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="H209" s="2">
         <v>45356</v>
       </c>
       <c r="I209">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="J209" t="inlineStr">
         <is>
@@ -21585,13 +21585,13 @@
         <v>45175</v>
       </c>
       <c r="G210">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="H210" s="2">
         <v>45356</v>
       </c>
       <c r="I210">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="J210" t="inlineStr">
         <is>
@@ -21688,13 +21688,13 @@
         <v>45166</v>
       </c>
       <c r="G211">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="H211" s="2">
         <v>45350</v>
       </c>
       <c r="I211">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="J211" t="inlineStr">
         <is>
@@ -21791,13 +21791,13 @@
         <v>45166</v>
       </c>
       <c r="G212">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="H212" s="2">
         <v>45350</v>
       </c>
       <c r="I212">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="J212" t="inlineStr">
         <is>
@@ -21894,13 +21894,13 @@
         <v>45090</v>
       </c>
       <c r="G213">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="H213" s="2">
         <v>45273</v>
       </c>
       <c r="I213">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="J213" t="inlineStr">
         <is>
@@ -21997,13 +21997,13 @@
         <v>45106</v>
       </c>
       <c r="G214">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="H214" s="2">
         <v>45289</v>
       </c>
       <c r="I214">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="J214" t="inlineStr">
         <is>
@@ -22100,13 +22100,13 @@
         <v>45134</v>
       </c>
       <c r="G215">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="H215" s="2">
         <v>45226</v>
       </c>
       <c r="I215">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="J215" t="inlineStr">
         <is>
@@ -22203,13 +22203,13 @@
         <v>45132</v>
       </c>
       <c r="G216">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="H216" s="2">
         <v>45224</v>
       </c>
       <c r="I216">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="J216" t="inlineStr">
         <is>
@@ -22306,13 +22306,13 @@
         <v>45150</v>
       </c>
       <c r="G217">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="H217" s="2">
         <v>45242</v>
       </c>
       <c r="I217">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="J217" t="inlineStr">
         <is>
@@ -22409,13 +22409,13 @@
         <v>45187</v>
       </c>
       <c r="G218">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="H218" s="2">
         <v>45278</v>
       </c>
       <c r="I218">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="J218" t="inlineStr">
         <is>
@@ -22507,13 +22507,13 @@
         <v>45182</v>
       </c>
       <c r="G219">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="H219" s="2">
         <v>45273</v>
       </c>
       <c r="I219">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="J219" t="inlineStr">
         <is>
@@ -22610,13 +22610,13 @@
         <v>45196</v>
       </c>
       <c r="G220">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="H220" s="2">
         <v>45287</v>
       </c>
       <c r="I220">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="J220" t="inlineStr">
         <is>
@@ -22713,13 +22713,13 @@
         <v>45200</v>
       </c>
       <c r="G221">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="H221" s="2">
         <v>45292</v>
       </c>
       <c r="I221">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="J221" t="inlineStr">
         <is>
@@ -22816,13 +22816,13 @@
         <v>45135</v>
       </c>
       <c r="G222">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="H222" s="2">
         <v>45227</v>
       </c>
       <c r="I222">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="J222" t="inlineStr">
         <is>
@@ -22919,13 +22919,13 @@
         <v>45148</v>
       </c>
       <c r="G223">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="H223" s="2">
         <v>45240</v>
       </c>
       <c r="I223">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="J223" t="inlineStr">
         <is>
@@ -23017,13 +23017,13 @@
         <v>45192</v>
       </c>
       <c r="G224">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="H224" s="2">
         <v>45283</v>
       </c>
       <c r="I224">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="J224" t="inlineStr">
         <is>
@@ -23115,13 +23115,13 @@
         <v>45136</v>
       </c>
       <c r="G225">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="H225" s="2">
         <v>45320</v>
       </c>
       <c r="I225">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="J225" t="inlineStr">
         <is>
@@ -23218,13 +23218,13 @@
         <v>45136</v>
       </c>
       <c r="G226">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="H226" s="2">
         <v>45320</v>
       </c>
       <c r="I226">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="J226" t="inlineStr">
         <is>
@@ -23321,13 +23321,13 @@
         <v>45094</v>
       </c>
       <c r="G227">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="H227" s="2">
         <v>45277</v>
       </c>
       <c r="I227">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="J227" t="inlineStr">
         <is>
@@ -23424,13 +23424,13 @@
         <v>45081</v>
       </c>
       <c r="G228">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="H228" s="2">
         <v>45264</v>
       </c>
       <c r="I228">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="J228" t="inlineStr">
         <is>
@@ -23527,13 +23527,13 @@
         <v>45099</v>
       </c>
       <c r="G229">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="H229" s="2">
         <v>45282</v>
       </c>
       <c r="I229">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="J229" t="inlineStr">
         <is>
@@ -23630,13 +23630,13 @@
         <v>45201</v>
       </c>
       <c r="G230">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="H230" s="2">
         <v>45384</v>
       </c>
       <c r="I230">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="J230" t="inlineStr">
         <is>
@@ -23733,13 +23733,13 @@
         <v>45031</v>
       </c>
       <c r="G231">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="H231" s="2">
         <v>45214</v>
       </c>
       <c r="I231">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="J231" t="inlineStr">
         <is>
@@ -23836,7 +23836,7 @@
         <v>45294</v>
       </c>
       <c r="I232">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="J232" t="inlineStr">
         <is>
@@ -23933,13 +23933,13 @@
         <v>45079</v>
       </c>
       <c r="G233">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="H233" s="2">
         <v>45262</v>
       </c>
       <c r="I233">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="J233" t="inlineStr">
         <is>
@@ -24036,13 +24036,13 @@
         <v>45199</v>
       </c>
       <c r="G234">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="H234" s="2">
         <v>45382</v>
       </c>
       <c r="I234">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="J234" t="inlineStr">
         <is>
@@ -24139,13 +24139,13 @@
         <v>45204</v>
       </c>
       <c r="G235">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="H235" s="2">
         <v>45387</v>
       </c>
       <c r="I235">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="J235" t="inlineStr">
         <is>
@@ -24242,13 +24242,13 @@
         <v>45204</v>
       </c>
       <c r="G236">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="H236" s="2">
         <v>45387</v>
       </c>
       <c r="I236">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="J236" t="inlineStr">
         <is>
@@ -24345,13 +24345,13 @@
         <v>45080</v>
       </c>
       <c r="G237">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="H237" s="2">
         <v>45263</v>
       </c>
       <c r="I237">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="J237" t="inlineStr">
         <is>
@@ -24448,13 +24448,13 @@
         <v>45046</v>
       </c>
       <c r="G238">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="H238" s="2">
         <v>45229</v>
       </c>
       <c r="I238">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="J238" t="inlineStr">
         <is>
@@ -24551,13 +24551,13 @@
         <v>45204</v>
       </c>
       <c r="G239">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="H239" s="2">
         <v>45296</v>
       </c>
       <c r="I239">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="J239" t="inlineStr">
         <is>
@@ -24654,13 +24654,13 @@
         <v>45204</v>
       </c>
       <c r="G240">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="H240" s="2">
         <v>45296</v>
       </c>
       <c r="I240">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="J240" t="inlineStr">
         <is>
@@ -24757,13 +24757,13 @@
         <v>45199</v>
       </c>
       <c r="G241">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="H241" s="2">
         <v>45382</v>
       </c>
       <c r="I241">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="J241" t="inlineStr">
         <is>
@@ -24860,13 +24860,13 @@
         <v>45070</v>
       </c>
       <c r="G242">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="H242" s="2">
         <v>45254</v>
       </c>
       <c r="I242">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="J242" t="inlineStr">
         <is>
@@ -24963,13 +24963,13 @@
         <v>45168</v>
       </c>
       <c r="G243">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="H243" s="2">
         <v>45260</v>
       </c>
       <c r="I243">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="J243" t="inlineStr">
         <is>
@@ -25066,13 +25066,13 @@
         <v>45027</v>
       </c>
       <c r="G244">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="H244" s="2">
         <v>45210</v>
       </c>
       <c r="I244">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J244" t="inlineStr">
         <is>
@@ -25169,13 +25169,13 @@
         <v>45077</v>
       </c>
       <c r="G245">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="H245" s="2">
         <v>45260</v>
       </c>
       <c r="I245">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="J245" t="inlineStr">
         <is>
@@ -25272,13 +25272,13 @@
         <v>45100</v>
       </c>
       <c r="G246">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="H246" s="2">
         <v>45283</v>
       </c>
       <c r="I246">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="J246" t="inlineStr">
         <is>
@@ -25375,7 +25375,7 @@
         <v>45281</v>
       </c>
       <c r="I247">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="J247" t="inlineStr">
         <is>
@@ -25472,13 +25472,13 @@
         <v>45044</v>
       </c>
       <c r="G248">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="H248" s="2">
         <v>45227</v>
       </c>
       <c r="I248">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="J248" t="inlineStr">
         <is>
@@ -25575,13 +25575,13 @@
         <v>45101</v>
       </c>
       <c r="G249">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="H249" s="2">
         <v>45283</v>
       </c>
       <c r="I249">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="J249" t="inlineStr">
         <is>
@@ -25678,13 +25678,13 @@
         <v>45134</v>
       </c>
       <c r="G250">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="H250" s="2">
         <v>45226</v>
       </c>
       <c r="I250">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="J250" t="inlineStr">
         <is>
@@ -25781,13 +25781,13 @@
         <v>45158</v>
       </c>
       <c r="G251">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="H251" s="2">
         <v>45250</v>
       </c>
       <c r="I251">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="J251" t="inlineStr">
         <is>
@@ -25884,13 +25884,13 @@
         <v>45200</v>
       </c>
       <c r="G252">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="H252" s="2">
         <v>45292</v>
       </c>
       <c r="I252">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="J252" t="inlineStr">
         <is>
@@ -25987,7 +25987,7 @@
         <v>45317</v>
       </c>
       <c r="I253">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="J253" t="inlineStr">
         <is>
@@ -26084,13 +26084,13 @@
         <v>45039</v>
       </c>
       <c r="G254">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="H254" s="2">
         <v>45222</v>
       </c>
       <c r="I254">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="J254" t="inlineStr">
         <is>
@@ -26182,13 +26182,13 @@
         <v>45129</v>
       </c>
       <c r="G255">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="H255" s="2">
         <v>45221</v>
       </c>
       <c r="I255">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="J255" t="inlineStr">
         <is>
@@ -26285,13 +26285,13 @@
         <v>45157</v>
       </c>
       <c r="G256">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="H256" s="2">
         <v>45341</v>
       </c>
       <c r="I256">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="J256" t="inlineStr">
         <is>
@@ -26388,13 +26388,13 @@
         <v>45063</v>
       </c>
       <c r="G257">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="H257" s="2">
         <v>45247</v>
       </c>
       <c r="I257">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="J257" t="inlineStr">
         <is>
@@ -26491,7 +26491,7 @@
         <v>45254</v>
       </c>
       <c r="I258">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="J258" t="inlineStr">
         <is>
@@ -26588,7 +26588,7 @@
         <v>45486</v>
       </c>
       <c r="I259">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="J259" t="inlineStr">
         <is>
@@ -26680,13 +26680,13 @@
         <v>45073</v>
       </c>
       <c r="G260">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="H260" s="2">
         <v>45439</v>
       </c>
       <c r="I260">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="J260" t="inlineStr">
         <is>
@@ -26778,7 +26778,7 @@
         <v>45323</v>
       </c>
       <c r="I261">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="J261" t="inlineStr">
         <is>
@@ -26870,7 +26870,7 @@
         <v>45303</v>
       </c>
       <c r="I262">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="J262" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
Bond dates update Wed Oct 11 23:16:05 UTC 2023
</commit_message>
<xml_diff>
--- a/Data/obligacje_screener.xlsx
+++ b/Data/obligacje_screener.xlsx
@@ -512,7 +512,7 @@
         <v>45340</v>
       </c>
       <c r="I2">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="J2" t="inlineStr">
         <is>
@@ -600,13 +600,13 @@
         <v>45121</v>
       </c>
       <c r="G3">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="H3" s="2">
         <v>45305</v>
       </c>
       <c r="I3">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="J3" t="inlineStr">
         <is>
@@ -703,13 +703,13 @@
         <v>45039</v>
       </c>
       <c r="G4">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="H4" s="2">
         <v>45222</v>
       </c>
       <c r="I4">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="J4" t="inlineStr">
         <is>
@@ -806,13 +806,13 @@
         <v>45039</v>
       </c>
       <c r="G5">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="H5" s="2">
         <v>45222</v>
       </c>
       <c r="I5">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="J5" t="inlineStr">
         <is>
@@ -909,13 +909,13 @@
         <v>45129</v>
       </c>
       <c r="G6">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="H6" s="2">
         <v>45221</v>
       </c>
       <c r="I6">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="J6" t="inlineStr">
         <is>
@@ -1012,13 +1012,13 @@
         <v>45162</v>
       </c>
       <c r="G7">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="H7" s="2">
         <v>45254</v>
       </c>
       <c r="I7">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="J7" t="inlineStr">
         <is>
@@ -1110,13 +1110,13 @@
         <v>45156</v>
       </c>
       <c r="G8">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="H8" s="2">
         <v>45248</v>
       </c>
       <c r="I8">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="J8" t="inlineStr">
         <is>
@@ -1213,13 +1213,13 @@
         <v>45141</v>
       </c>
       <c r="G9">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="H9" s="2">
         <v>45233</v>
       </c>
       <c r="I9">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="J9" t="inlineStr">
         <is>
@@ -1316,13 +1316,13 @@
         <v>45062</v>
       </c>
       <c r="G10">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="H10" s="2">
         <v>45246</v>
       </c>
       <c r="I10">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="J10" t="inlineStr">
         <is>
@@ -1419,7 +1419,7 @@
         <v>45286</v>
       </c>
       <c r="I11">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="J11" t="inlineStr">
         <is>
@@ -1516,13 +1516,13 @@
         <v>45195</v>
       </c>
       <c r="G12">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="H12" s="2">
         <v>45377</v>
       </c>
       <c r="I12">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="J12" t="inlineStr">
         <is>
@@ -1614,13 +1614,13 @@
         <v>45036</v>
       </c>
       <c r="G13">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="H13" s="2">
         <v>45219</v>
       </c>
       <c r="I13">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="J13" t="inlineStr">
         <is>
@@ -1717,13 +1717,13 @@
         <v>45036</v>
       </c>
       <c r="G14">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="H14" s="2">
         <v>45219</v>
       </c>
       <c r="I14">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="J14" t="inlineStr">
         <is>
@@ -1820,13 +1820,13 @@
         <v>45106</v>
       </c>
       <c r="G15">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="H15" s="2">
         <v>45289</v>
       </c>
       <c r="I15">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="J15" t="inlineStr">
         <is>
@@ -1923,13 +1923,13 @@
         <v>45186</v>
       </c>
       <c r="G16">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="H16" s="2">
         <v>45278</v>
       </c>
       <c r="I16">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="J16" t="inlineStr">
         <is>
@@ -2026,13 +2026,13 @@
         <v>45186</v>
       </c>
       <c r="G17">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="H17" s="2">
         <v>45277</v>
       </c>
       <c r="I17">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="J17" t="inlineStr">
         <is>
@@ -2129,13 +2129,13 @@
         <v>45132</v>
       </c>
       <c r="G18">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="H18" s="2">
         <v>45224</v>
       </c>
       <c r="I18">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="J18" t="inlineStr">
         <is>
@@ -2232,13 +2232,13 @@
         <v>45137</v>
       </c>
       <c r="G19">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="H19" s="2">
         <v>45229</v>
       </c>
       <c r="I19">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="J19" t="inlineStr">
         <is>
@@ -2330,13 +2330,13 @@
         <v>45183</v>
       </c>
       <c r="G20">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="H20" s="2">
         <v>45274</v>
       </c>
       <c r="I20">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="J20" t="inlineStr">
         <is>
@@ -2433,13 +2433,13 @@
         <v>45187</v>
       </c>
       <c r="G21">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="H21" s="2">
         <v>45278</v>
       </c>
       <c r="I21">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="J21" t="inlineStr">
         <is>
@@ -2536,13 +2536,13 @@
         <v>45187</v>
       </c>
       <c r="G22">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="H22" s="2">
         <v>45278</v>
       </c>
       <c r="I22">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="J22" t="inlineStr">
         <is>
@@ -2639,7 +2639,7 @@
         <v>45245</v>
       </c>
       <c r="I23">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="J23" t="inlineStr">
         <is>
@@ -2736,7 +2736,7 @@
         <v>45245</v>
       </c>
       <c r="I24">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="J24" t="inlineStr">
         <is>
@@ -2833,7 +2833,7 @@
         <v>45204</v>
       </c>
       <c r="G25">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="J25" t="inlineStr">
         <is>
@@ -2930,13 +2930,13 @@
         <v>45160</v>
       </c>
       <c r="G26">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="H26" s="2">
         <v>45344</v>
       </c>
       <c r="I26">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="J26" t="inlineStr">
         <is>
@@ -3033,13 +3033,13 @@
         <v>45118</v>
       </c>
       <c r="G27">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="H27" s="2">
         <v>45302</v>
       </c>
       <c r="I27">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="J27" t="inlineStr">
         <is>
@@ -3136,13 +3136,13 @@
         <v>45085</v>
       </c>
       <c r="G28">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="H28" s="2">
         <v>45268</v>
       </c>
       <c r="I28">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="J28" t="inlineStr">
         <is>
@@ -3239,13 +3239,13 @@
         <v>45183</v>
       </c>
       <c r="G29">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="H29" s="2">
         <v>45274</v>
       </c>
       <c r="I29">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="J29" t="inlineStr">
         <is>
@@ -3342,7 +3342,7 @@
         <v>45224</v>
       </c>
       <c r="I30">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="J30" t="inlineStr">
         <is>
@@ -3439,13 +3439,13 @@
         <v>45153</v>
       </c>
       <c r="G31">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="H31" s="2">
         <v>45245</v>
       </c>
       <c r="I31">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="J31" t="inlineStr">
         <is>
@@ -3542,13 +3542,13 @@
         <v>45155</v>
       </c>
       <c r="G32">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="H32" s="2">
         <v>45247</v>
       </c>
       <c r="I32">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="J32" t="inlineStr">
         <is>
@@ -3645,7 +3645,7 @@
         <v>45255</v>
       </c>
       <c r="I33">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="J33" t="inlineStr">
         <is>
@@ -3742,13 +3742,13 @@
         <v>45176</v>
       </c>
       <c r="G34">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="H34" s="2">
         <v>45267</v>
       </c>
       <c r="I34">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="J34" t="inlineStr">
         <is>
@@ -3845,13 +3845,13 @@
         <v>45130</v>
       </c>
       <c r="G35">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="H35" s="2">
         <v>45222</v>
       </c>
       <c r="I35">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="J35" t="inlineStr">
         <is>
@@ -3943,13 +3943,13 @@
         <v>45207</v>
       </c>
       <c r="G36">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H36" s="2">
         <v>45299</v>
       </c>
       <c r="I36">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="J36" t="inlineStr">
         <is>
@@ -4046,13 +4046,13 @@
         <v>45189</v>
       </c>
       <c r="G37">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="H37" s="2">
         <v>45280</v>
       </c>
       <c r="I37">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="J37" t="inlineStr">
         <is>
@@ -4144,13 +4144,13 @@
         <v>45107</v>
       </c>
       <c r="G38">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="H38" s="2">
         <v>45290</v>
       </c>
       <c r="I38">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="J38" t="inlineStr">
         <is>
@@ -4247,13 +4247,13 @@
         <v>45063</v>
       </c>
       <c r="G39">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="H39" s="2">
         <v>45247</v>
       </c>
       <c r="I39">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="J39" t="inlineStr">
         <is>
@@ -4350,13 +4350,13 @@
         <v>45177</v>
       </c>
       <c r="G40">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="H40" s="2">
         <v>45359</v>
       </c>
       <c r="I40">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="J40" t="inlineStr">
         <is>
@@ -4453,13 +4453,13 @@
         <v>45107</v>
       </c>
       <c r="G41">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="H41" s="2">
         <v>45290</v>
       </c>
       <c r="I41">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="J41" t="inlineStr">
         <is>
@@ -4556,7 +4556,7 @@
         <v>45265</v>
       </c>
       <c r="I42">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="J42" t="inlineStr">
         <is>
@@ -4653,13 +4653,13 @@
         <v>45098</v>
       </c>
       <c r="G43">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="H43" s="2">
         <v>45281</v>
       </c>
       <c r="I43">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="J43" t="inlineStr">
         <is>
@@ -4756,13 +4756,13 @@
         <v>45099</v>
       </c>
       <c r="G44">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="H44" s="2">
         <v>45282</v>
       </c>
       <c r="I44">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="J44" t="inlineStr">
         <is>
@@ -4859,13 +4859,13 @@
         <v>45106</v>
       </c>
       <c r="G45">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="H45" s="2">
         <v>45289</v>
       </c>
       <c r="I45">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="J45" t="inlineStr">
         <is>
@@ -4962,13 +4962,13 @@
         <v>45106</v>
       </c>
       <c r="G46">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="H46" s="2">
         <v>45289</v>
       </c>
       <c r="I46">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="J46" t="inlineStr">
         <is>
@@ -5065,13 +5065,13 @@
         <v>45120</v>
       </c>
       <c r="G47">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="H47" s="2">
         <v>45304</v>
       </c>
       <c r="I47">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="J47" t="inlineStr">
         <is>
@@ -5168,13 +5168,13 @@
         <v>45118</v>
       </c>
       <c r="G48">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="H48" s="2">
         <v>45302</v>
       </c>
       <c r="I48">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="J48" t="inlineStr">
         <is>
@@ -5271,13 +5271,13 @@
         <v>45152</v>
       </c>
       <c r="G49">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="H49" s="2">
         <v>45336</v>
       </c>
       <c r="I49">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="J49" t="inlineStr">
         <is>
@@ -5374,13 +5374,13 @@
         <v>45042</v>
       </c>
       <c r="G50">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="H50" s="2">
         <v>45225</v>
       </c>
       <c r="I50">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="J50" t="inlineStr">
         <is>
@@ -5477,13 +5477,13 @@
         <v>45122</v>
       </c>
       <c r="G51">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="H51" s="2">
         <v>45306</v>
       </c>
       <c r="I51">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="J51" t="inlineStr">
         <is>
@@ -5580,13 +5580,13 @@
         <v>45139</v>
       </c>
       <c r="G52">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="H52" s="2">
         <v>45323</v>
       </c>
       <c r="I52">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="J52" t="inlineStr">
         <is>
@@ -5683,13 +5683,13 @@
         <v>45099</v>
       </c>
       <c r="G53">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="H53" s="2">
         <v>45282</v>
       </c>
       <c r="I53">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="J53" t="inlineStr">
         <is>
@@ -5786,13 +5786,13 @@
         <v>45196</v>
       </c>
       <c r="G54">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="H54" s="2">
         <v>45287</v>
       </c>
       <c r="I54">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="J54" t="inlineStr">
         <is>
@@ -5889,13 +5889,13 @@
         <v>45044</v>
       </c>
       <c r="G55">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="H55" s="2">
         <v>45227</v>
       </c>
       <c r="I55">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="J55" t="inlineStr">
         <is>
@@ -5992,13 +5992,13 @@
         <v>45151</v>
       </c>
       <c r="G56">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="H56" s="2">
         <v>45243</v>
       </c>
       <c r="I56">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="J56" t="inlineStr">
         <is>
@@ -6090,13 +6090,13 @@
         <v>45196</v>
       </c>
       <c r="G57">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="H57" s="2">
         <v>45287</v>
       </c>
       <c r="I57">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="J57" t="inlineStr">
         <is>
@@ -6193,13 +6193,13 @@
         <v>45069</v>
       </c>
       <c r="G58">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="H58" s="2">
         <v>45253</v>
       </c>
       <c r="I58">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="J58" t="inlineStr">
         <is>
@@ -6296,13 +6296,13 @@
         <v>45191</v>
       </c>
       <c r="G59">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="H59" s="2">
         <v>45282</v>
       </c>
       <c r="I59">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="J59" t="inlineStr">
         <is>
@@ -6394,7 +6394,7 @@
         <v>45205</v>
       </c>
       <c r="G60">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="J60" t="inlineStr">
         <is>
@@ -6491,13 +6491,13 @@
         <v>45127</v>
       </c>
       <c r="G61">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="H61" s="2">
         <v>45219</v>
       </c>
       <c r="I61">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="J61" t="inlineStr">
         <is>
@@ -6594,13 +6594,13 @@
         <v>45058</v>
       </c>
       <c r="G62">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="H62" s="2">
         <v>45242</v>
       </c>
       <c r="I62">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="J62" t="inlineStr">
         <is>
@@ -6697,13 +6697,13 @@
         <v>45194</v>
       </c>
       <c r="G63">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H63" s="2">
         <v>45376</v>
       </c>
       <c r="I63">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="J63" t="inlineStr">
         <is>
@@ -6795,7 +6795,7 @@
         <v>45208</v>
       </c>
       <c r="G64">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J64" t="inlineStr">
         <is>
@@ -6892,7 +6892,7 @@
         <v>45208</v>
       </c>
       <c r="G65">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J65" t="inlineStr">
         <is>
@@ -6989,13 +6989,13 @@
         <v>45089</v>
       </c>
       <c r="G66">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="H66" s="2">
         <v>45272</v>
       </c>
       <c r="I66">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="J66" t="inlineStr">
         <is>
@@ -7092,13 +7092,13 @@
         <v>45178</v>
       </c>
       <c r="G67">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="H67" s="2">
         <v>45269</v>
       </c>
       <c r="I67">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="J67" t="inlineStr">
         <is>
@@ -7190,13 +7190,13 @@
         <v>45196</v>
       </c>
       <c r="G68">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="H68" s="2">
         <v>45287</v>
       </c>
       <c r="I68">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="J68" t="inlineStr">
         <is>
@@ -7293,13 +7293,13 @@
         <v>45149</v>
       </c>
       <c r="G69">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="H69" s="2">
         <v>45241</v>
       </c>
       <c r="I69">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="J69" t="inlineStr">
         <is>
@@ -7396,13 +7396,13 @@
         <v>45205</v>
       </c>
       <c r="G70">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="H70" s="2">
         <v>45296</v>
       </c>
       <c r="I70">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="J70" t="inlineStr">
         <is>
@@ -7499,7 +7499,7 @@
         <v>45205</v>
       </c>
       <c r="G71">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="J71" t="inlineStr">
         <is>
@@ -7596,13 +7596,13 @@
         <v>45207</v>
       </c>
       <c r="G72">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H72" s="2">
         <v>45299</v>
       </c>
       <c r="I72">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="J72" t="inlineStr">
         <is>
@@ -7699,13 +7699,13 @@
         <v>45189</v>
       </c>
       <c r="G73">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="H73" s="2">
         <v>45280</v>
       </c>
       <c r="I73">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="J73" t="inlineStr">
         <is>
@@ -7797,13 +7797,13 @@
         <v>45038</v>
       </c>
       <c r="G74">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="H74" s="2">
         <v>45221</v>
       </c>
       <c r="I74">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="J74" t="inlineStr">
         <is>
@@ -7895,13 +7895,13 @@
         <v>45117</v>
       </c>
       <c r="G75">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="H75" s="2">
         <v>45301</v>
       </c>
       <c r="I75">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="J75" t="inlineStr">
         <is>
@@ -7998,13 +7998,13 @@
         <v>45160</v>
       </c>
       <c r="G76">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="H76" s="2">
         <v>45344</v>
       </c>
       <c r="I76">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="J76" t="inlineStr">
         <is>
@@ -8101,13 +8101,13 @@
         <v>45186</v>
       </c>
       <c r="G77">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="H77" s="2">
         <v>45368</v>
       </c>
       <c r="I77">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="J77" t="inlineStr">
         <is>
@@ -8204,13 +8204,13 @@
         <v>45043</v>
       </c>
       <c r="G78">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="H78" s="2">
         <v>45226</v>
       </c>
       <c r="I78">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="J78" t="inlineStr">
         <is>
@@ -8307,13 +8307,13 @@
         <v>45079</v>
       </c>
       <c r="G79">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="H79" s="2">
         <v>45262</v>
       </c>
       <c r="I79">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="J79" t="inlineStr">
         <is>
@@ -8410,7 +8410,7 @@
         <v>45254</v>
       </c>
       <c r="I80">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="J80" t="inlineStr">
         <is>
@@ -8507,13 +8507,13 @@
         <v>45104</v>
       </c>
       <c r="G81">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="H81" s="2">
         <v>45287</v>
       </c>
       <c r="I81">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="J81" t="inlineStr">
         <is>
@@ -8610,7 +8610,7 @@
         <v>45288</v>
       </c>
       <c r="I82">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="J82" t="inlineStr">
         <is>
@@ -8702,13 +8702,13 @@
         <v>45175</v>
       </c>
       <c r="G83">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="H83" s="2">
         <v>45357</v>
       </c>
       <c r="I83">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="J83" t="inlineStr">
         <is>
@@ -8805,13 +8805,13 @@
         <v>45054</v>
       </c>
       <c r="G84">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="H84" s="2">
         <v>45238</v>
       </c>
       <c r="I84">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="J84" t="inlineStr">
         <is>
@@ -8908,13 +8908,13 @@
         <v>45056</v>
       </c>
       <c r="G85">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="H85" s="2">
         <v>45240</v>
       </c>
       <c r="I85">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="J85" t="inlineStr">
         <is>
@@ -9011,13 +9011,13 @@
         <v>45085</v>
       </c>
       <c r="G86">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="H86" s="2">
         <v>45268</v>
       </c>
       <c r="I86">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="J86" t="inlineStr">
         <is>
@@ -9114,13 +9114,13 @@
         <v>45194</v>
       </c>
       <c r="G87">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H87" s="2">
         <v>45560</v>
       </c>
       <c r="I87">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="J87" t="inlineStr">
         <is>
@@ -9207,13 +9207,13 @@
         <v>45103</v>
       </c>
       <c r="G88">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="H88" s="2">
         <v>45286</v>
       </c>
       <c r="I88">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="J88" t="inlineStr">
         <is>
@@ -9310,13 +9310,13 @@
         <v>45103</v>
       </c>
       <c r="G89">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="H89" s="2">
         <v>45286</v>
       </c>
       <c r="I89">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="J89" t="inlineStr">
         <is>
@@ -9413,13 +9413,13 @@
         <v>45192</v>
       </c>
       <c r="G90">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="H90" s="2">
         <v>45374</v>
       </c>
       <c r="I90">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="J90" t="inlineStr">
         <is>
@@ -9511,13 +9511,13 @@
         <v>45100</v>
       </c>
       <c r="G91">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="H91" s="2">
         <v>45287</v>
       </c>
       <c r="I91">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="J91" t="inlineStr">
         <is>
@@ -9614,13 +9614,13 @@
         <v>45187</v>
       </c>
       <c r="G92">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="H92" s="2">
         <v>45369</v>
       </c>
       <c r="I92">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="J92" t="inlineStr">
         <is>
@@ -9717,13 +9717,13 @@
         <v>45104</v>
       </c>
       <c r="G93">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="H93" s="2">
         <v>45287</v>
       </c>
       <c r="I93">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="J93" t="inlineStr">
         <is>
@@ -9820,13 +9820,13 @@
         <v>45104</v>
       </c>
       <c r="G94">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="H94" s="2">
         <v>45287</v>
       </c>
       <c r="I94">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="J94" t="inlineStr">
         <is>
@@ -9923,13 +9923,13 @@
         <v>45049</v>
       </c>
       <c r="G95">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="H95" s="2">
         <v>45233</v>
       </c>
       <c r="I95">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="J95" t="inlineStr">
         <is>
@@ -10026,13 +10026,13 @@
         <v>45122</v>
       </c>
       <c r="G96">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="H96" s="2">
         <v>45306</v>
       </c>
       <c r="I96">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="J96" t="inlineStr">
         <is>
@@ -10124,13 +10124,13 @@
         <v>45141</v>
       </c>
       <c r="G97">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="H97" s="2">
         <v>45325</v>
       </c>
       <c r="I97">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="J97" t="inlineStr">
         <is>
@@ -10227,13 +10227,13 @@
         <v>45194</v>
       </c>
       <c r="G98">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H98" s="2">
         <v>45376</v>
       </c>
       <c r="I98">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="J98" t="inlineStr">
         <is>
@@ -10325,13 +10325,13 @@
         <v>45093</v>
       </c>
       <c r="G99">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="H99" s="2">
         <v>45276</v>
       </c>
       <c r="I99">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="J99" t="inlineStr">
         <is>
@@ -10428,13 +10428,13 @@
         <v>45123</v>
       </c>
       <c r="G100">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="H100" s="2">
         <v>45307</v>
       </c>
       <c r="I100">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="J100" t="inlineStr">
         <is>
@@ -10531,13 +10531,13 @@
         <v>45198</v>
       </c>
       <c r="G101">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="H101" s="2">
         <v>45380</v>
       </c>
       <c r="I101">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="J101" t="inlineStr">
         <is>
@@ -10634,13 +10634,13 @@
         <v>45093</v>
       </c>
       <c r="G102">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="H102" s="2">
         <v>45276</v>
       </c>
       <c r="I102">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="J102" t="inlineStr">
         <is>
@@ -10737,13 +10737,13 @@
         <v>45122</v>
       </c>
       <c r="G103">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="H103" s="2">
         <v>45306</v>
       </c>
       <c r="I103">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="J103" t="inlineStr">
         <is>
@@ -10840,13 +10840,13 @@
         <v>45122</v>
       </c>
       <c r="G104">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="H104" s="2">
         <v>45306</v>
       </c>
       <c r="I104">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="J104" t="inlineStr">
         <is>
@@ -10938,13 +10938,13 @@
         <v>45050</v>
       </c>
       <c r="G105">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="H105" s="2">
         <v>45234</v>
       </c>
       <c r="I105">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="J105" t="inlineStr">
         <is>
@@ -11041,13 +11041,13 @@
         <v>45085</v>
       </c>
       <c r="G106">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="H106" s="2">
         <v>45268</v>
       </c>
       <c r="I106">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="J106" t="inlineStr">
         <is>
@@ -11144,13 +11144,13 @@
         <v>45185</v>
       </c>
       <c r="G107">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="H107" s="2">
         <v>45276</v>
       </c>
       <c r="I107">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="J107" t="inlineStr">
         <is>
@@ -11242,13 +11242,13 @@
         <v>45185</v>
       </c>
       <c r="G108">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="H108" s="2">
         <v>45276</v>
       </c>
       <c r="I108">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="J108" t="inlineStr">
         <is>
@@ -11340,13 +11340,13 @@
         <v>45185</v>
       </c>
       <c r="G109">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="H109" s="2">
         <v>45276</v>
       </c>
       <c r="I109">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="J109" t="inlineStr">
         <is>
@@ -11443,13 +11443,13 @@
         <v>45148</v>
       </c>
       <c r="G110">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="H110" s="2">
         <v>45240</v>
       </c>
       <c r="I110">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="J110" t="inlineStr">
         <is>
@@ -11546,13 +11546,13 @@
         <v>45119</v>
       </c>
       <c r="G111">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="H111" s="2">
         <v>45211</v>
       </c>
       <c r="I111">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J111" t="inlineStr">
         <is>
@@ -11649,13 +11649,13 @@
         <v>45172</v>
       </c>
       <c r="G112">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="H112" s="2">
         <v>45263</v>
       </c>
       <c r="I112">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="J112" t="inlineStr">
         <is>
@@ -11752,13 +11752,13 @@
         <v>45206</v>
       </c>
       <c r="G113">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="H113" s="2">
         <v>45389</v>
       </c>
       <c r="I113">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="J113" t="inlineStr">
         <is>
@@ -11855,13 +11855,13 @@
         <v>45203</v>
       </c>
       <c r="G114">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="H114" s="2">
         <v>45295</v>
       </c>
       <c r="I114">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="J114" t="inlineStr">
         <is>
@@ -11958,7 +11958,7 @@
         <v>45218</v>
       </c>
       <c r="I115">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="J115" t="inlineStr">
         <is>
@@ -12055,13 +12055,13 @@
         <v>45161</v>
       </c>
       <c r="G116">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="H116" s="2">
         <v>45253</v>
       </c>
       <c r="I116">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="J116" t="inlineStr">
         <is>
@@ -12158,13 +12158,13 @@
         <v>45115</v>
       </c>
       <c r="G117">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="H117" s="2">
         <v>45299</v>
       </c>
       <c r="I117">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="J117" t="inlineStr">
         <is>
@@ -12256,13 +12256,13 @@
         <v>45094</v>
       </c>
       <c r="G118">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="H118" s="2">
         <v>45277</v>
       </c>
       <c r="I118">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="J118" t="inlineStr">
         <is>
@@ -12359,13 +12359,13 @@
         <v>45104</v>
       </c>
       <c r="G119">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="H119" s="2">
         <v>45287</v>
       </c>
       <c r="I119">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="J119" t="inlineStr">
         <is>
@@ -12462,13 +12462,13 @@
         <v>45104</v>
       </c>
       <c r="G120">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="H120" s="2">
         <v>45287</v>
       </c>
       <c r="I120">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="J120" t="inlineStr">
         <is>
@@ -12565,13 +12565,13 @@
         <v>45104</v>
       </c>
       <c r="G121">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="H121" s="2">
         <v>45287</v>
       </c>
       <c r="I121">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="J121" t="inlineStr">
         <is>
@@ -12668,13 +12668,13 @@
         <v>45104</v>
       </c>
       <c r="G122">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="H122" s="2">
         <v>45287</v>
       </c>
       <c r="I122">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="J122" t="inlineStr">
         <is>
@@ -12771,13 +12771,13 @@
         <v>45199</v>
       </c>
       <c r="G123">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="H123" s="2">
         <v>45291</v>
       </c>
       <c r="I123">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="J123" t="inlineStr">
         <is>
@@ -12874,13 +12874,13 @@
         <v>45197</v>
       </c>
       <c r="G124">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="H124" s="2">
         <v>45379</v>
       </c>
       <c r="I124">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="J124" t="inlineStr">
         <is>
@@ -12977,13 +12977,13 @@
         <v>45121</v>
       </c>
       <c r="G125">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="H125" s="2">
         <v>45213</v>
       </c>
       <c r="I125">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="J125" t="inlineStr">
         <is>
@@ -13080,13 +13080,13 @@
         <v>45134</v>
       </c>
       <c r="G126">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="H126" s="2">
         <v>45226</v>
       </c>
       <c r="I126">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="J126" t="inlineStr">
         <is>
@@ -13183,7 +13183,7 @@
         <v>45212</v>
       </c>
       <c r="I127">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="J127" t="inlineStr">
         <is>
@@ -13280,13 +13280,13 @@
         <v>45126</v>
       </c>
       <c r="G128">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="H128" s="2">
         <v>45218</v>
       </c>
       <c r="I128">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="J128" t="inlineStr">
         <is>
@@ -13378,13 +13378,13 @@
         <v>45158</v>
       </c>
       <c r="G129">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="H129" s="2">
         <v>45250</v>
       </c>
       <c r="I129">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="J129" t="inlineStr">
         <is>
@@ -13481,13 +13481,13 @@
         <v>45171</v>
       </c>
       <c r="G130">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="H130" s="2">
         <v>45262</v>
       </c>
       <c r="I130">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="J130" t="inlineStr">
         <is>
@@ -13584,13 +13584,13 @@
         <v>45203</v>
       </c>
       <c r="G131">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="H131" s="2">
         <v>45295</v>
       </c>
       <c r="I131">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="J131" t="inlineStr">
         <is>
@@ -13687,13 +13687,13 @@
         <v>45144</v>
       </c>
       <c r="G132">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="H132" s="2">
         <v>45236</v>
       </c>
       <c r="I132">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="J132" t="inlineStr">
         <is>
@@ -13790,13 +13790,13 @@
         <v>45156</v>
       </c>
       <c r="G133">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="H133" s="2">
         <v>45248</v>
       </c>
       <c r="I133">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="J133" t="inlineStr">
         <is>
@@ -13888,13 +13888,13 @@
         <v>45146</v>
       </c>
       <c r="G134">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="H134" s="2">
         <v>45238</v>
       </c>
       <c r="I134">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="J134" t="inlineStr">
         <is>
@@ -13991,13 +13991,13 @@
         <v>45140</v>
       </c>
       <c r="G135">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="H135" s="2">
         <v>45232</v>
       </c>
       <c r="I135">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="J135" t="inlineStr">
         <is>
@@ -14094,13 +14094,13 @@
         <v>45196</v>
       </c>
       <c r="G136">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="H136" s="2">
         <v>45287</v>
       </c>
       <c r="I136">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="J136" t="inlineStr">
         <is>
@@ -14197,13 +14197,13 @@
         <v>45197</v>
       </c>
       <c r="G137">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="H137" s="2">
         <v>45288</v>
       </c>
       <c r="I137">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="J137" t="inlineStr">
         <is>
@@ -14300,13 +14300,13 @@
         <v>45179</v>
       </c>
       <c r="G138">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="H138" s="2">
         <v>45270</v>
       </c>
       <c r="I138">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="J138" t="inlineStr">
         <is>
@@ -14398,13 +14398,13 @@
         <v>45197</v>
       </c>
       <c r="G139">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="H139" s="2">
         <v>45288</v>
       </c>
       <c r="I139">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="J139" t="inlineStr">
         <is>
@@ -14501,13 +14501,13 @@
         <v>45182</v>
       </c>
       <c r="G140">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="H140" s="2">
         <v>45273</v>
       </c>
       <c r="I140">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="J140" t="inlineStr">
         <is>
@@ -14604,13 +14604,13 @@
         <v>45208</v>
       </c>
       <c r="G141">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H141" s="2">
         <v>45300</v>
       </c>
       <c r="I141">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="J141" t="inlineStr">
         <is>
@@ -14702,13 +14702,13 @@
         <v>45150</v>
       </c>
       <c r="G142">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="H142" s="2">
         <v>45242</v>
       </c>
       <c r="I142">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="J142" t="inlineStr">
         <is>
@@ -14805,7 +14805,7 @@
         <v>45238</v>
       </c>
       <c r="I143">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="J143" t="inlineStr">
         <is>
@@ -14902,13 +14902,13 @@
         <v>45171</v>
       </c>
       <c r="G144">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="H144" s="2">
         <v>45262</v>
       </c>
       <c r="I144">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="J144" t="inlineStr">
         <is>
@@ -15005,13 +15005,13 @@
         <v>45194</v>
       </c>
       <c r="G145">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H145" s="2">
         <v>45285</v>
       </c>
       <c r="I145">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="J145" t="inlineStr">
         <is>
@@ -15098,13 +15098,13 @@
         <v>45119</v>
       </c>
       <c r="G146">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="H146" s="2">
         <v>45211</v>
       </c>
       <c r="I146">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J146" t="inlineStr">
         <is>
@@ -15201,13 +15201,13 @@
         <v>45165</v>
       </c>
       <c r="G147">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="H147" s="2">
         <v>45257</v>
       </c>
       <c r="I147">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="J147" t="inlineStr">
         <is>
@@ -15304,13 +15304,13 @@
         <v>45166</v>
       </c>
       <c r="G148">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="H148" s="2">
         <v>45258</v>
       </c>
       <c r="I148">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="J148" t="inlineStr">
         <is>
@@ -15407,13 +15407,13 @@
         <v>45185</v>
       </c>
       <c r="G149">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="H149" s="2">
         <v>45276</v>
       </c>
       <c r="I149">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="J149" t="inlineStr">
         <is>
@@ -15510,13 +15510,13 @@
         <v>45035</v>
       </c>
       <c r="G150">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="H150" s="2">
         <v>45218</v>
       </c>
       <c r="I150">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="J150" t="inlineStr">
         <is>
@@ -15613,13 +15613,13 @@
         <v>45174</v>
       </c>
       <c r="G151">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="H151" s="2">
         <v>45356</v>
       </c>
       <c r="I151">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="J151" t="inlineStr">
         <is>
@@ -15716,13 +15716,13 @@
         <v>45089</v>
       </c>
       <c r="G152">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="H152" s="2">
         <v>45272</v>
       </c>
       <c r="I152">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="J152" t="inlineStr">
         <is>
@@ -15819,13 +15819,13 @@
         <v>45124</v>
       </c>
       <c r="G153">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="H153" s="2">
         <v>45308</v>
       </c>
       <c r="I153">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="J153" t="inlineStr">
         <is>
@@ -15922,13 +15922,13 @@
         <v>45124</v>
       </c>
       <c r="G154">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="H154" s="2">
         <v>45308</v>
       </c>
       <c r="I154">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="J154" t="inlineStr">
         <is>
@@ -16022,16 +16022,16 @@
         </is>
       </c>
       <c r="F155" s="2">
-        <v>45026</v>
+        <v>45209</v>
       </c>
       <c r="G155">
-        <v>183</v>
+        <v>1</v>
       </c>
       <c r="H155" s="2">
         <v>45392</v>
       </c>
       <c r="I155">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="J155" t="inlineStr">
         <is>
@@ -16125,16 +16125,16 @@
         </is>
       </c>
       <c r="F156" s="2">
-        <v>45026</v>
+        <v>45209</v>
       </c>
       <c r="G156">
-        <v>183</v>
+        <v>1</v>
       </c>
       <c r="H156" s="2">
         <v>45392</v>
       </c>
       <c r="I156">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="J156" t="inlineStr">
         <is>
@@ -16228,16 +16228,16 @@
         </is>
       </c>
       <c r="F157" s="2">
-        <v>45026</v>
+        <v>45209</v>
       </c>
       <c r="G157">
-        <v>183</v>
+        <v>1</v>
       </c>
       <c r="H157" s="2">
         <v>45392</v>
       </c>
       <c r="I157">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="J157" t="inlineStr">
         <is>
@@ -16331,16 +16331,16 @@
         </is>
       </c>
       <c r="F158" s="2">
-        <v>45026</v>
+        <v>45209</v>
       </c>
       <c r="G158">
-        <v>183</v>
+        <v>1</v>
       </c>
       <c r="H158" s="2">
         <v>45392</v>
       </c>
       <c r="I158">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="J158" t="inlineStr">
         <is>
@@ -16437,13 +16437,13 @@
         <v>45156</v>
       </c>
       <c r="G159">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="H159" s="2">
         <v>45247</v>
       </c>
       <c r="I159">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="J159" t="inlineStr">
         <is>
@@ -16540,13 +16540,13 @@
         <v>45153</v>
       </c>
       <c r="G160">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="H160" s="2">
         <v>45245</v>
       </c>
       <c r="I160">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="J160" t="inlineStr">
         <is>
@@ -16643,13 +16643,13 @@
         <v>45135</v>
       </c>
       <c r="G161">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="H161" s="2">
         <v>45319</v>
       </c>
       <c r="I161">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="J161" t="inlineStr">
         <is>
@@ -16746,13 +16746,13 @@
         <v>45091</v>
       </c>
       <c r="G162">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="H162" s="2">
         <v>45274</v>
       </c>
       <c r="I162">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="J162" t="inlineStr">
         <is>
@@ -16844,13 +16844,13 @@
         <v>45091</v>
       </c>
       <c r="G163">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="H163" s="2">
         <v>45274</v>
       </c>
       <c r="I163">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="J163" t="inlineStr">
         <is>
@@ -16942,13 +16942,13 @@
         <v>45138</v>
       </c>
       <c r="G164">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="H164" s="2">
         <v>45322</v>
       </c>
       <c r="I164">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="J164" t="inlineStr">
         <is>
@@ -17045,13 +17045,13 @@
         <v>45138</v>
       </c>
       <c r="G165">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="H165" s="2">
         <v>45322</v>
       </c>
       <c r="I165">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="J165" t="inlineStr">
         <is>
@@ -17148,13 +17148,13 @@
         <v>45085</v>
       </c>
       <c r="G166">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="H166" s="2">
         <v>45268</v>
       </c>
       <c r="I166">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="J166" t="inlineStr">
         <is>
@@ -17251,13 +17251,13 @@
         <v>45085</v>
       </c>
       <c r="G167">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="H167" s="2">
         <v>45268</v>
       </c>
       <c r="I167">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="J167" t="inlineStr">
         <is>
@@ -17354,7 +17354,7 @@
         <v>45326</v>
       </c>
       <c r="I168">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="J168" t="inlineStr">
         <is>
@@ -17451,13 +17451,13 @@
         <v>45173</v>
       </c>
       <c r="G169">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="H169" s="2">
         <v>45355</v>
       </c>
       <c r="I169">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="J169" t="inlineStr">
         <is>
@@ -17554,13 +17554,13 @@
         <v>45056</v>
       </c>
       <c r="G170">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="H170" s="2">
         <v>45240</v>
       </c>
       <c r="I170">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="J170" t="inlineStr">
         <is>
@@ -17657,7 +17657,7 @@
         <v>45238</v>
       </c>
       <c r="I171">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="J171" t="inlineStr">
         <is>
@@ -17754,13 +17754,13 @@
         <v>45141</v>
       </c>
       <c r="G172">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="H172" s="2">
         <v>45325</v>
       </c>
       <c r="I172">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="J172" t="inlineStr">
         <is>
@@ -17857,13 +17857,13 @@
         <v>45037</v>
       </c>
       <c r="G173">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="H173" s="2">
         <v>45220</v>
       </c>
       <c r="I173">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="J173" t="inlineStr">
         <is>
@@ -17960,13 +17960,13 @@
         <v>45171</v>
       </c>
       <c r="G174">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="H174" s="2">
         <v>45262</v>
       </c>
       <c r="I174">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="J174" t="inlineStr">
         <is>
@@ -18063,13 +18063,13 @@
         <v>45197</v>
       </c>
       <c r="G175">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="H175" s="2">
         <v>45288</v>
       </c>
       <c r="I175">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="J175" t="inlineStr">
         <is>
@@ -18166,13 +18166,13 @@
         <v>45162</v>
       </c>
       <c r="G176">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="H176" s="2">
         <v>45254</v>
       </c>
       <c r="I176">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="J176" t="inlineStr">
         <is>
@@ -18269,13 +18269,13 @@
         <v>45061</v>
       </c>
       <c r="G177">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="H177" s="2">
         <v>45245</v>
       </c>
       <c r="I177">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="J177" t="inlineStr">
         <is>
@@ -18372,13 +18372,13 @@
         <v>45120</v>
       </c>
       <c r="G178">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="H178" s="2">
         <v>45212</v>
       </c>
       <c r="I178">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="J178" t="inlineStr">
         <is>
@@ -18475,13 +18475,13 @@
         <v>45191</v>
       </c>
       <c r="G179">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="H179" s="2">
         <v>45282</v>
       </c>
       <c r="I179">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="J179" t="inlineStr">
         <is>
@@ -18578,13 +18578,13 @@
         <v>45088</v>
       </c>
       <c r="G180">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="H180" s="2">
         <v>45271</v>
       </c>
       <c r="I180">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="J180" t="inlineStr">
         <is>
@@ -18681,13 +18681,13 @@
         <v>45192</v>
       </c>
       <c r="G181">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="H181" s="2">
         <v>45283</v>
       </c>
       <c r="I181">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="J181" t="inlineStr">
         <is>
@@ -18774,13 +18774,13 @@
         <v>45131</v>
       </c>
       <c r="G182">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="H182" s="2">
         <v>45223</v>
       </c>
       <c r="I182">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="J182" t="inlineStr">
         <is>
@@ -18872,13 +18872,13 @@
         <v>45136</v>
       </c>
       <c r="G183">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="H183" s="2">
         <v>45228</v>
       </c>
       <c r="I183">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="J183" t="inlineStr">
         <is>
@@ -18970,13 +18970,13 @@
         <v>45150</v>
       </c>
       <c r="G184">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="H184" s="2">
         <v>45242</v>
       </c>
       <c r="I184">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="J184" t="inlineStr">
         <is>
@@ -19068,13 +19068,7 @@
         <v>45118</v>
       </c>
       <c r="G185">
-        <v>91</v>
-      </c>
-      <c r="H185" s="2">
-        <v>45210</v>
-      </c>
-      <c r="I185">
-        <v>1</v>
+        <v>92</v>
       </c>
       <c r="J185" t="inlineStr">
         <is>
@@ -19166,13 +19160,13 @@
         <v>45129</v>
       </c>
       <c r="G186">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="H186" s="2">
         <v>45221</v>
       </c>
       <c r="I186">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="J186" t="inlineStr">
         <is>
@@ -19264,13 +19258,13 @@
         <v>45189</v>
       </c>
       <c r="G187">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="H187" s="2">
         <v>45280</v>
       </c>
       <c r="I187">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="J187" t="inlineStr">
         <is>
@@ -19357,13 +19351,13 @@
         <v>45193</v>
       </c>
       <c r="G188">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="H188" s="2">
         <v>45284</v>
       </c>
       <c r="I188">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="J188" t="inlineStr">
         <is>
@@ -19450,13 +19444,13 @@
         <v>45165</v>
       </c>
       <c r="G189">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="H189" s="2">
         <v>45257</v>
       </c>
       <c r="I189">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="J189" t="inlineStr">
         <is>
@@ -19548,13 +19542,13 @@
         <v>45202</v>
       </c>
       <c r="G190">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="H190" s="2">
         <v>45385</v>
       </c>
       <c r="I190">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="J190" t="inlineStr">
         <is>
@@ -19651,13 +19645,13 @@
         <v>45081</v>
       </c>
       <c r="G191">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="H191" s="2">
         <v>45264</v>
       </c>
       <c r="I191">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="J191" t="inlineStr">
         <is>
@@ -19754,13 +19748,13 @@
         <v>45081</v>
       </c>
       <c r="G192">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="H192" s="2">
         <v>45264</v>
       </c>
       <c r="I192">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="J192" t="inlineStr">
         <is>
@@ -19857,7 +19851,7 @@
         <v>45319</v>
       </c>
       <c r="I193">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="J193" t="inlineStr">
         <is>
@@ -19954,7 +19948,7 @@
         <v>45319</v>
       </c>
       <c r="I194">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="J194" t="inlineStr">
         <is>
@@ -20046,13 +20040,13 @@
         <v>45046</v>
       </c>
       <c r="G195">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="H195" s="2">
         <v>45230</v>
       </c>
       <c r="I195">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="J195" t="inlineStr">
         <is>
@@ -20149,13 +20143,13 @@
         <v>45046</v>
       </c>
       <c r="G196">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="H196" s="2">
         <v>45230</v>
       </c>
       <c r="I196">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="J196" t="inlineStr">
         <is>
@@ -20252,13 +20246,13 @@
         <v>45031</v>
       </c>
       <c r="G197">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="H197" s="2">
         <v>45214</v>
       </c>
       <c r="I197">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="J197" t="inlineStr">
         <is>
@@ -20355,13 +20349,13 @@
         <v>45031</v>
       </c>
       <c r="G198">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="H198" s="2">
         <v>45214</v>
       </c>
       <c r="I198">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="J198" t="inlineStr">
         <is>
@@ -20458,13 +20452,13 @@
         <v>45031</v>
       </c>
       <c r="G199">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="H199" s="2">
         <v>45214</v>
       </c>
       <c r="I199">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="J199" t="inlineStr">
         <is>
@@ -20561,13 +20555,13 @@
         <v>45031</v>
       </c>
       <c r="G200">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="H200" s="2">
         <v>45214</v>
       </c>
       <c r="I200">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="J200" t="inlineStr">
         <is>
@@ -20664,13 +20658,13 @@
         <v>45067</v>
       </c>
       <c r="G201">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="H201" s="2">
         <v>45251</v>
       </c>
       <c r="I201">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="J201" t="inlineStr">
         <is>
@@ -20767,13 +20761,13 @@
         <v>45067</v>
       </c>
       <c r="G202">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="H202" s="2">
         <v>45251</v>
       </c>
       <c r="I202">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="J202" t="inlineStr">
         <is>
@@ -20870,13 +20864,13 @@
         <v>45067</v>
       </c>
       <c r="G203">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="H203" s="2">
         <v>45251</v>
       </c>
       <c r="I203">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="J203" t="inlineStr">
         <is>
@@ -20973,13 +20967,13 @@
         <v>45067</v>
       </c>
       <c r="G204">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="H204" s="2">
         <v>45251</v>
       </c>
       <c r="I204">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="J204" t="inlineStr">
         <is>
@@ -21076,13 +21070,13 @@
         <v>45178</v>
       </c>
       <c r="G205">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="H205" s="2">
         <v>45269</v>
       </c>
       <c r="I205">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="J205" t="inlineStr">
         <is>
@@ -21179,7 +21173,7 @@
         <v>45252</v>
       </c>
       <c r="I206">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="J206" t="inlineStr">
         <is>
@@ -21276,13 +21270,13 @@
         <v>45087</v>
       </c>
       <c r="G207">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="H207" s="2">
         <v>45270</v>
       </c>
       <c r="I207">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="J207" t="inlineStr">
         <is>
@@ -21379,13 +21373,13 @@
         <v>45099</v>
       </c>
       <c r="G208">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="H208" s="2">
         <v>45282</v>
       </c>
       <c r="I208">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="J208" t="inlineStr">
         <is>
@@ -21482,13 +21476,13 @@
         <v>45175</v>
       </c>
       <c r="G209">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="H209" s="2">
         <v>45356</v>
       </c>
       <c r="I209">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="J209" t="inlineStr">
         <is>
@@ -21585,13 +21579,13 @@
         <v>45175</v>
       </c>
       <c r="G210">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="H210" s="2">
         <v>45356</v>
       </c>
       <c r="I210">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="J210" t="inlineStr">
         <is>
@@ -21688,13 +21682,13 @@
         <v>45166</v>
       </c>
       <c r="G211">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="H211" s="2">
         <v>45350</v>
       </c>
       <c r="I211">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="J211" t="inlineStr">
         <is>
@@ -21791,13 +21785,13 @@
         <v>45166</v>
       </c>
       <c r="G212">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="H212" s="2">
         <v>45350</v>
       </c>
       <c r="I212">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="J212" t="inlineStr">
         <is>
@@ -21894,13 +21888,13 @@
         <v>45090</v>
       </c>
       <c r="G213">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="H213" s="2">
         <v>45273</v>
       </c>
       <c r="I213">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="J213" t="inlineStr">
         <is>
@@ -21997,13 +21991,13 @@
         <v>45106</v>
       </c>
       <c r="G214">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="H214" s="2">
         <v>45289</v>
       </c>
       <c r="I214">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="J214" t="inlineStr">
         <is>
@@ -22100,13 +22094,13 @@
         <v>45134</v>
       </c>
       <c r="G215">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="H215" s="2">
         <v>45226</v>
       </c>
       <c r="I215">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="J215" t="inlineStr">
         <is>
@@ -22203,13 +22197,13 @@
         <v>45132</v>
       </c>
       <c r="G216">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="H216" s="2">
         <v>45224</v>
       </c>
       <c r="I216">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="J216" t="inlineStr">
         <is>
@@ -22306,13 +22300,13 @@
         <v>45150</v>
       </c>
       <c r="G217">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="H217" s="2">
         <v>45242</v>
       </c>
       <c r="I217">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="J217" t="inlineStr">
         <is>
@@ -22409,13 +22403,13 @@
         <v>45187</v>
       </c>
       <c r="G218">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="H218" s="2">
         <v>45278</v>
       </c>
       <c r="I218">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="J218" t="inlineStr">
         <is>
@@ -22507,13 +22501,13 @@
         <v>45182</v>
       </c>
       <c r="G219">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="H219" s="2">
         <v>45273</v>
       </c>
       <c r="I219">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="J219" t="inlineStr">
         <is>
@@ -22610,13 +22604,13 @@
         <v>45196</v>
       </c>
       <c r="G220">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="H220" s="2">
         <v>45287</v>
       </c>
       <c r="I220">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="J220" t="inlineStr">
         <is>
@@ -22713,13 +22707,13 @@
         <v>45200</v>
       </c>
       <c r="G221">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="H221" s="2">
         <v>45292</v>
       </c>
       <c r="I221">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="J221" t="inlineStr">
         <is>
@@ -22816,13 +22810,13 @@
         <v>45135</v>
       </c>
       <c r="G222">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="H222" s="2">
         <v>45227</v>
       </c>
       <c r="I222">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="J222" t="inlineStr">
         <is>
@@ -22919,13 +22913,13 @@
         <v>45148</v>
       </c>
       <c r="G223">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="H223" s="2">
         <v>45240</v>
       </c>
       <c r="I223">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="J223" t="inlineStr">
         <is>
@@ -23017,13 +23011,13 @@
         <v>45192</v>
       </c>
       <c r="G224">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="H224" s="2">
         <v>45283</v>
       </c>
       <c r="I224">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="J224" t="inlineStr">
         <is>
@@ -23115,13 +23109,13 @@
         <v>45136</v>
       </c>
       <c r="G225">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="H225" s="2">
         <v>45320</v>
       </c>
       <c r="I225">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="J225" t="inlineStr">
         <is>
@@ -23218,13 +23212,13 @@
         <v>45136</v>
       </c>
       <c r="G226">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="H226" s="2">
         <v>45320</v>
       </c>
       <c r="I226">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="J226" t="inlineStr">
         <is>
@@ -23321,13 +23315,13 @@
         <v>45094</v>
       </c>
       <c r="G227">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="H227" s="2">
         <v>45277</v>
       </c>
       <c r="I227">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="J227" t="inlineStr">
         <is>
@@ -23424,13 +23418,13 @@
         <v>45081</v>
       </c>
       <c r="G228">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="H228" s="2">
         <v>45264</v>
       </c>
       <c r="I228">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="J228" t="inlineStr">
         <is>
@@ -23527,13 +23521,13 @@
         <v>45099</v>
       </c>
       <c r="G229">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="H229" s="2">
         <v>45282</v>
       </c>
       <c r="I229">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="J229" t="inlineStr">
         <is>
@@ -23630,13 +23624,13 @@
         <v>45201</v>
       </c>
       <c r="G230">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="H230" s="2">
         <v>45384</v>
       </c>
       <c r="I230">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="J230" t="inlineStr">
         <is>
@@ -23733,13 +23727,13 @@
         <v>45031</v>
       </c>
       <c r="G231">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="H231" s="2">
         <v>45214</v>
       </c>
       <c r="I231">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="J231" t="inlineStr">
         <is>
@@ -23836,7 +23830,7 @@
         <v>45294</v>
       </c>
       <c r="I232">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="J232" t="inlineStr">
         <is>
@@ -23933,13 +23927,13 @@
         <v>45079</v>
       </c>
       <c r="G233">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="H233" s="2">
         <v>45262</v>
       </c>
       <c r="I233">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="J233" t="inlineStr">
         <is>
@@ -24036,13 +24030,13 @@
         <v>45199</v>
       </c>
       <c r="G234">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="H234" s="2">
         <v>45382</v>
       </c>
       <c r="I234">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="J234" t="inlineStr">
         <is>
@@ -24139,13 +24133,13 @@
         <v>45204</v>
       </c>
       <c r="G235">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="H235" s="2">
         <v>45387</v>
       </c>
       <c r="I235">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="J235" t="inlineStr">
         <is>
@@ -24242,13 +24236,13 @@
         <v>45204</v>
       </c>
       <c r="G236">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="H236" s="2">
         <v>45387</v>
       </c>
       <c r="I236">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="J236" t="inlineStr">
         <is>
@@ -24345,13 +24339,13 @@
         <v>45080</v>
       </c>
       <c r="G237">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="H237" s="2">
         <v>45263</v>
       </c>
       <c r="I237">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="J237" t="inlineStr">
         <is>
@@ -24448,13 +24442,13 @@
         <v>45046</v>
       </c>
       <c r="G238">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="H238" s="2">
         <v>45229</v>
       </c>
       <c r="I238">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="J238" t="inlineStr">
         <is>
@@ -24551,13 +24545,13 @@
         <v>45204</v>
       </c>
       <c r="G239">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="H239" s="2">
         <v>45296</v>
       </c>
       <c r="I239">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="J239" t="inlineStr">
         <is>
@@ -24654,13 +24648,13 @@
         <v>45204</v>
       </c>
       <c r="G240">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="H240" s="2">
         <v>45296</v>
       </c>
       <c r="I240">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="J240" t="inlineStr">
         <is>
@@ -24757,13 +24751,13 @@
         <v>45199</v>
       </c>
       <c r="G241">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="H241" s="2">
         <v>45382</v>
       </c>
       <c r="I241">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="J241" t="inlineStr">
         <is>
@@ -24860,13 +24854,13 @@
         <v>45070</v>
       </c>
       <c r="G242">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="H242" s="2">
         <v>45254</v>
       </c>
       <c r="I242">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="J242" t="inlineStr">
         <is>
@@ -24963,13 +24957,13 @@
         <v>45168</v>
       </c>
       <c r="G243">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="H243" s="2">
         <v>45260</v>
       </c>
       <c r="I243">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="J243" t="inlineStr">
         <is>
@@ -25066,13 +25060,13 @@
         <v>45027</v>
       </c>
       <c r="G244">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="H244" s="2">
-        <v>45210</v>
+        <v>45393</v>
       </c>
       <c r="I244">
-        <v>1</v>
+        <v>183</v>
       </c>
       <c r="J244" t="inlineStr">
         <is>
@@ -25169,13 +25163,13 @@
         <v>45077</v>
       </c>
       <c r="G245">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="H245" s="2">
         <v>45260</v>
       </c>
       <c r="I245">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="J245" t="inlineStr">
         <is>
@@ -25272,13 +25266,13 @@
         <v>45100</v>
       </c>
       <c r="G246">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="H246" s="2">
         <v>45283</v>
       </c>
       <c r="I246">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="J246" t="inlineStr">
         <is>
@@ -25375,7 +25369,7 @@
         <v>45281</v>
       </c>
       <c r="I247">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="J247" t="inlineStr">
         <is>
@@ -25472,13 +25466,13 @@
         <v>45044</v>
       </c>
       <c r="G248">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="H248" s="2">
         <v>45227</v>
       </c>
       <c r="I248">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="J248" t="inlineStr">
         <is>
@@ -25575,13 +25569,13 @@
         <v>45101</v>
       </c>
       <c r="G249">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="H249" s="2">
         <v>45283</v>
       </c>
       <c r="I249">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="J249" t="inlineStr">
         <is>
@@ -25678,13 +25672,13 @@
         <v>45134</v>
       </c>
       <c r="G250">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="H250" s="2">
         <v>45226</v>
       </c>
       <c r="I250">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="J250" t="inlineStr">
         <is>
@@ -25781,13 +25775,13 @@
         <v>45158</v>
       </c>
       <c r="G251">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="H251" s="2">
         <v>45250</v>
       </c>
       <c r="I251">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="J251" t="inlineStr">
         <is>
@@ -25884,13 +25878,13 @@
         <v>45200</v>
       </c>
       <c r="G252">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="H252" s="2">
         <v>45292</v>
       </c>
       <c r="I252">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="J252" t="inlineStr">
         <is>
@@ -25987,7 +25981,7 @@
         <v>45317</v>
       </c>
       <c r="I253">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="J253" t="inlineStr">
         <is>
@@ -26084,13 +26078,13 @@
         <v>45039</v>
       </c>
       <c r="G254">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="H254" s="2">
         <v>45222</v>
       </c>
       <c r="I254">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="J254" t="inlineStr">
         <is>
@@ -26182,13 +26176,13 @@
         <v>45129</v>
       </c>
       <c r="G255">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="H255" s="2">
         <v>45221</v>
       </c>
       <c r="I255">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="J255" t="inlineStr">
         <is>
@@ -26285,13 +26279,13 @@
         <v>45157</v>
       </c>
       <c r="G256">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="H256" s="2">
         <v>45341</v>
       </c>
       <c r="I256">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="J256" t="inlineStr">
         <is>
@@ -26388,13 +26382,13 @@
         <v>45063</v>
       </c>
       <c r="G257">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="H257" s="2">
         <v>45247</v>
       </c>
       <c r="I257">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="J257" t="inlineStr">
         <is>
@@ -26491,7 +26485,7 @@
         <v>45254</v>
       </c>
       <c r="I258">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="J258" t="inlineStr">
         <is>
@@ -26588,7 +26582,7 @@
         <v>45486</v>
       </c>
       <c r="I259">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="J259" t="inlineStr">
         <is>
@@ -26680,13 +26674,13 @@
         <v>45073</v>
       </c>
       <c r="G260">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="H260" s="2">
         <v>45439</v>
       </c>
       <c r="I260">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="J260" t="inlineStr">
         <is>
@@ -26778,7 +26772,7 @@
         <v>45323</v>
       </c>
       <c r="I261">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="J261" t="inlineStr">
         <is>
@@ -26870,7 +26864,7 @@
         <v>45303</v>
       </c>
       <c r="I262">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="J262" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
Bond dates update Thu Oct 12 23:16:49 UTC 2023
</commit_message>
<xml_diff>
--- a/Data/obligacje_screener.xlsx
+++ b/Data/obligacje_screener.xlsx
@@ -512,7 +512,7 @@
         <v>45340</v>
       </c>
       <c r="I2">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="J2" t="inlineStr">
         <is>
@@ -600,13 +600,13 @@
         <v>45121</v>
       </c>
       <c r="G3">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="H3" s="2">
         <v>45305</v>
       </c>
       <c r="I3">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="J3" t="inlineStr">
         <is>
@@ -703,13 +703,13 @@
         <v>45039</v>
       </c>
       <c r="G4">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="H4" s="2">
         <v>45222</v>
       </c>
       <c r="I4">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="J4" t="inlineStr">
         <is>
@@ -806,13 +806,13 @@
         <v>45039</v>
       </c>
       <c r="G5">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="H5" s="2">
         <v>45222</v>
       </c>
       <c r="I5">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="J5" t="inlineStr">
         <is>
@@ -909,13 +909,13 @@
         <v>45129</v>
       </c>
       <c r="G6">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="H6" s="2">
         <v>45221</v>
       </c>
       <c r="I6">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="J6" t="inlineStr">
         <is>
@@ -1012,13 +1012,13 @@
         <v>45162</v>
       </c>
       <c r="G7">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="H7" s="2">
         <v>45254</v>
       </c>
       <c r="I7">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="J7" t="inlineStr">
         <is>
@@ -1110,13 +1110,13 @@
         <v>45156</v>
       </c>
       <c r="G8">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="H8" s="2">
         <v>45248</v>
       </c>
       <c r="I8">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="J8" t="inlineStr">
         <is>
@@ -1213,13 +1213,13 @@
         <v>45141</v>
       </c>
       <c r="G9">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="H9" s="2">
         <v>45233</v>
       </c>
       <c r="I9">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="J9" t="inlineStr">
         <is>
@@ -1316,13 +1316,13 @@
         <v>45062</v>
       </c>
       <c r="G10">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="H10" s="2">
         <v>45246</v>
       </c>
       <c r="I10">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="J10" t="inlineStr">
         <is>
@@ -1419,7 +1419,7 @@
         <v>45286</v>
       </c>
       <c r="I11">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="J11" t="inlineStr">
         <is>
@@ -1516,13 +1516,13 @@
         <v>45195</v>
       </c>
       <c r="G12">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H12" s="2">
         <v>45377</v>
       </c>
       <c r="I12">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="J12" t="inlineStr">
         <is>
@@ -1614,13 +1614,13 @@
         <v>45036</v>
       </c>
       <c r="G13">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="H13" s="2">
         <v>45219</v>
       </c>
       <c r="I13">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="J13" t="inlineStr">
         <is>
@@ -1717,13 +1717,13 @@
         <v>45036</v>
       </c>
       <c r="G14">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="H14" s="2">
         <v>45219</v>
       </c>
       <c r="I14">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="J14" t="inlineStr">
         <is>
@@ -1820,13 +1820,13 @@
         <v>45106</v>
       </c>
       <c r="G15">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="H15" s="2">
         <v>45289</v>
       </c>
       <c r="I15">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="J15" t="inlineStr">
         <is>
@@ -1923,13 +1923,13 @@
         <v>45186</v>
       </c>
       <c r="G16">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="H16" s="2">
         <v>45278</v>
       </c>
       <c r="I16">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="J16" t="inlineStr">
         <is>
@@ -2026,13 +2026,13 @@
         <v>45186</v>
       </c>
       <c r="G17">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="H17" s="2">
         <v>45277</v>
       </c>
       <c r="I17">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="J17" t="inlineStr">
         <is>
@@ -2129,13 +2129,13 @@
         <v>45132</v>
       </c>
       <c r="G18">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="H18" s="2">
         <v>45224</v>
       </c>
       <c r="I18">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="J18" t="inlineStr">
         <is>
@@ -2232,13 +2232,13 @@
         <v>45137</v>
       </c>
       <c r="G19">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="H19" s="2">
         <v>45229</v>
       </c>
       <c r="I19">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="J19" t="inlineStr">
         <is>
@@ -2330,13 +2330,13 @@
         <v>45183</v>
       </c>
       <c r="G20">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="H20" s="2">
         <v>45274</v>
       </c>
       <c r="I20">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="J20" t="inlineStr">
         <is>
@@ -2433,13 +2433,13 @@
         <v>45187</v>
       </c>
       <c r="G21">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="H21" s="2">
         <v>45278</v>
       </c>
       <c r="I21">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="J21" t="inlineStr">
         <is>
@@ -2536,13 +2536,13 @@
         <v>45187</v>
       </c>
       <c r="G22">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="H22" s="2">
         <v>45278</v>
       </c>
       <c r="I22">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="J22" t="inlineStr">
         <is>
@@ -2639,7 +2639,7 @@
         <v>45245</v>
       </c>
       <c r="I23">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="J23" t="inlineStr">
         <is>
@@ -2736,7 +2736,7 @@
         <v>45245</v>
       </c>
       <c r="I24">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="J24" t="inlineStr">
         <is>
@@ -2833,7 +2833,7 @@
         <v>45204</v>
       </c>
       <c r="G25">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="J25" t="inlineStr">
         <is>
@@ -2930,13 +2930,13 @@
         <v>45160</v>
       </c>
       <c r="G26">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="H26" s="2">
         <v>45344</v>
       </c>
       <c r="I26">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="J26" t="inlineStr">
         <is>
@@ -3033,13 +3033,13 @@
         <v>45118</v>
       </c>
       <c r="G27">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="H27" s="2">
         <v>45302</v>
       </c>
       <c r="I27">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="J27" t="inlineStr">
         <is>
@@ -3136,13 +3136,13 @@
         <v>45085</v>
       </c>
       <c r="G28">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="H28" s="2">
         <v>45268</v>
       </c>
       <c r="I28">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="J28" t="inlineStr">
         <is>
@@ -3239,13 +3239,13 @@
         <v>45183</v>
       </c>
       <c r="G29">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="H29" s="2">
         <v>45274</v>
       </c>
       <c r="I29">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="J29" t="inlineStr">
         <is>
@@ -3342,7 +3342,7 @@
         <v>45224</v>
       </c>
       <c r="I30">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="J30" t="inlineStr">
         <is>
@@ -3439,13 +3439,13 @@
         <v>45153</v>
       </c>
       <c r="G31">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="H31" s="2">
         <v>45245</v>
       </c>
       <c r="I31">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="J31" t="inlineStr">
         <is>
@@ -3542,13 +3542,13 @@
         <v>45155</v>
       </c>
       <c r="G32">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="H32" s="2">
         <v>45247</v>
       </c>
       <c r="I32">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="J32" t="inlineStr">
         <is>
@@ -3645,7 +3645,7 @@
         <v>45255</v>
       </c>
       <c r="I33">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="J33" t="inlineStr">
         <is>
@@ -3742,13 +3742,13 @@
         <v>45176</v>
       </c>
       <c r="G34">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="H34" s="2">
         <v>45267</v>
       </c>
       <c r="I34">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="J34" t="inlineStr">
         <is>
@@ -3845,13 +3845,13 @@
         <v>45130</v>
       </c>
       <c r="G35">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="H35" s="2">
         <v>45222</v>
       </c>
       <c r="I35">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="J35" t="inlineStr">
         <is>
@@ -3943,13 +3943,13 @@
         <v>45207</v>
       </c>
       <c r="G36">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="H36" s="2">
         <v>45299</v>
       </c>
       <c r="I36">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="J36" t="inlineStr">
         <is>
@@ -4046,13 +4046,13 @@
         <v>45189</v>
       </c>
       <c r="G37">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="H37" s="2">
         <v>45280</v>
       </c>
       <c r="I37">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="J37" t="inlineStr">
         <is>
@@ -4144,13 +4144,13 @@
         <v>45107</v>
       </c>
       <c r="G38">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="H38" s="2">
         <v>45290</v>
       </c>
       <c r="I38">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="J38" t="inlineStr">
         <is>
@@ -4247,13 +4247,13 @@
         <v>45063</v>
       </c>
       <c r="G39">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="H39" s="2">
         <v>45247</v>
       </c>
       <c r="I39">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="J39" t="inlineStr">
         <is>
@@ -4350,13 +4350,13 @@
         <v>45177</v>
       </c>
       <c r="G40">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="H40" s="2">
         <v>45359</v>
       </c>
       <c r="I40">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="J40" t="inlineStr">
         <is>
@@ -4453,13 +4453,13 @@
         <v>45107</v>
       </c>
       <c r="G41">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="H41" s="2">
         <v>45290</v>
       </c>
       <c r="I41">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="J41" t="inlineStr">
         <is>
@@ -4556,7 +4556,7 @@
         <v>45265</v>
       </c>
       <c r="I42">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="J42" t="inlineStr">
         <is>
@@ -4653,13 +4653,13 @@
         <v>45098</v>
       </c>
       <c r="G43">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="H43" s="2">
         <v>45281</v>
       </c>
       <c r="I43">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="J43" t="inlineStr">
         <is>
@@ -4756,13 +4756,13 @@
         <v>45099</v>
       </c>
       <c r="G44">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="H44" s="2">
         <v>45282</v>
       </c>
       <c r="I44">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="J44" t="inlineStr">
         <is>
@@ -4859,13 +4859,13 @@
         <v>45106</v>
       </c>
       <c r="G45">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="H45" s="2">
         <v>45289</v>
       </c>
       <c r="I45">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="J45" t="inlineStr">
         <is>
@@ -4962,13 +4962,13 @@
         <v>45106</v>
       </c>
       <c r="G46">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="H46" s="2">
         <v>45289</v>
       </c>
       <c r="I46">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="J46" t="inlineStr">
         <is>
@@ -5065,13 +5065,13 @@
         <v>45120</v>
       </c>
       <c r="G47">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="H47" s="2">
         <v>45304</v>
       </c>
       <c r="I47">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="J47" t="inlineStr">
         <is>
@@ -5168,13 +5168,13 @@
         <v>45118</v>
       </c>
       <c r="G48">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="H48" s="2">
         <v>45302</v>
       </c>
       <c r="I48">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="J48" t="inlineStr">
         <is>
@@ -5271,13 +5271,13 @@
         <v>45152</v>
       </c>
       <c r="G49">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="H49" s="2">
         <v>45336</v>
       </c>
       <c r="I49">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="J49" t="inlineStr">
         <is>
@@ -5374,13 +5374,13 @@
         <v>45042</v>
       </c>
       <c r="G50">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="H50" s="2">
         <v>45225</v>
       </c>
       <c r="I50">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="J50" t="inlineStr">
         <is>
@@ -5477,13 +5477,13 @@
         <v>45122</v>
       </c>
       <c r="G51">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="H51" s="2">
         <v>45306</v>
       </c>
       <c r="I51">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="J51" t="inlineStr">
         <is>
@@ -5580,13 +5580,13 @@
         <v>45139</v>
       </c>
       <c r="G52">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="H52" s="2">
         <v>45323</v>
       </c>
       <c r="I52">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="J52" t="inlineStr">
         <is>
@@ -5683,13 +5683,13 @@
         <v>45099</v>
       </c>
       <c r="G53">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="H53" s="2">
         <v>45282</v>
       </c>
       <c r="I53">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="J53" t="inlineStr">
         <is>
@@ -5786,13 +5786,13 @@
         <v>45196</v>
       </c>
       <c r="G54">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="H54" s="2">
         <v>45287</v>
       </c>
       <c r="I54">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="J54" t="inlineStr">
         <is>
@@ -5889,13 +5889,13 @@
         <v>45044</v>
       </c>
       <c r="G55">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="H55" s="2">
         <v>45227</v>
       </c>
       <c r="I55">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="J55" t="inlineStr">
         <is>
@@ -5992,13 +5992,13 @@
         <v>45151</v>
       </c>
       <c r="G56">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="H56" s="2">
         <v>45243</v>
       </c>
       <c r="I56">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="J56" t="inlineStr">
         <is>
@@ -6090,13 +6090,13 @@
         <v>45196</v>
       </c>
       <c r="G57">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="H57" s="2">
         <v>45287</v>
       </c>
       <c r="I57">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="J57" t="inlineStr">
         <is>
@@ -6193,13 +6193,13 @@
         <v>45069</v>
       </c>
       <c r="G58">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="H58" s="2">
         <v>45253</v>
       </c>
       <c r="I58">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="J58" t="inlineStr">
         <is>
@@ -6296,13 +6296,13 @@
         <v>45191</v>
       </c>
       <c r="G59">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="H59" s="2">
         <v>45282</v>
       </c>
       <c r="I59">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="J59" t="inlineStr">
         <is>
@@ -6394,7 +6394,7 @@
         <v>45205</v>
       </c>
       <c r="G60">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="J60" t="inlineStr">
         <is>
@@ -6491,13 +6491,13 @@
         <v>45127</v>
       </c>
       <c r="G61">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="H61" s="2">
         <v>45219</v>
       </c>
       <c r="I61">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="J61" t="inlineStr">
         <is>
@@ -6594,13 +6594,13 @@
         <v>45058</v>
       </c>
       <c r="G62">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="H62" s="2">
         <v>45242</v>
       </c>
       <c r="I62">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="J62" t="inlineStr">
         <is>
@@ -6697,13 +6697,13 @@
         <v>45194</v>
       </c>
       <c r="G63">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="H63" s="2">
         <v>45376</v>
       </c>
       <c r="I63">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="J63" t="inlineStr">
         <is>
@@ -6795,7 +6795,7 @@
         <v>45208</v>
       </c>
       <c r="G64">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="J64" t="inlineStr">
         <is>
@@ -6892,7 +6892,7 @@
         <v>45208</v>
       </c>
       <c r="G65">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="J65" t="inlineStr">
         <is>
@@ -6989,13 +6989,13 @@
         <v>45089</v>
       </c>
       <c r="G66">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="H66" s="2">
         <v>45272</v>
       </c>
       <c r="I66">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="J66" t="inlineStr">
         <is>
@@ -7092,13 +7092,13 @@
         <v>45178</v>
       </c>
       <c r="G67">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="H67" s="2">
         <v>45269</v>
       </c>
       <c r="I67">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="J67" t="inlineStr">
         <is>
@@ -7190,13 +7190,13 @@
         <v>45196</v>
       </c>
       <c r="G68">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="H68" s="2">
         <v>45287</v>
       </c>
       <c r="I68">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="J68" t="inlineStr">
         <is>
@@ -7293,13 +7293,13 @@
         <v>45149</v>
       </c>
       <c r="G69">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="H69" s="2">
         <v>45241</v>
       </c>
       <c r="I69">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="J69" t="inlineStr">
         <is>
@@ -7396,13 +7396,13 @@
         <v>45205</v>
       </c>
       <c r="G70">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="H70" s="2">
         <v>45296</v>
       </c>
       <c r="I70">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="J70" t="inlineStr">
         <is>
@@ -7499,7 +7499,7 @@
         <v>45205</v>
       </c>
       <c r="G71">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="J71" t="inlineStr">
         <is>
@@ -7596,13 +7596,13 @@
         <v>45207</v>
       </c>
       <c r="G72">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="H72" s="2">
         <v>45299</v>
       </c>
       <c r="I72">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="J72" t="inlineStr">
         <is>
@@ -7699,13 +7699,13 @@
         <v>45189</v>
       </c>
       <c r="G73">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="H73" s="2">
         <v>45280</v>
       </c>
       <c r="I73">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="J73" t="inlineStr">
         <is>
@@ -7797,13 +7797,13 @@
         <v>45038</v>
       </c>
       <c r="G74">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="H74" s="2">
         <v>45221</v>
       </c>
       <c r="I74">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="J74" t="inlineStr">
         <is>
@@ -7895,13 +7895,13 @@
         <v>45117</v>
       </c>
       <c r="G75">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="H75" s="2">
         <v>45301</v>
       </c>
       <c r="I75">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="J75" t="inlineStr">
         <is>
@@ -7998,13 +7998,13 @@
         <v>45160</v>
       </c>
       <c r="G76">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="H76" s="2">
         <v>45344</v>
       </c>
       <c r="I76">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="J76" t="inlineStr">
         <is>
@@ -8101,13 +8101,13 @@
         <v>45186</v>
       </c>
       <c r="G77">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="H77" s="2">
         <v>45368</v>
       </c>
       <c r="I77">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="J77" t="inlineStr">
         <is>
@@ -8204,13 +8204,13 @@
         <v>45043</v>
       </c>
       <c r="G78">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="H78" s="2">
         <v>45226</v>
       </c>
       <c r="I78">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="J78" t="inlineStr">
         <is>
@@ -8307,13 +8307,13 @@
         <v>45079</v>
       </c>
       <c r="G79">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="H79" s="2">
         <v>45262</v>
       </c>
       <c r="I79">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="J79" t="inlineStr">
         <is>
@@ -8410,7 +8410,7 @@
         <v>45254</v>
       </c>
       <c r="I80">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="J80" t="inlineStr">
         <is>
@@ -8507,13 +8507,13 @@
         <v>45104</v>
       </c>
       <c r="G81">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="H81" s="2">
         <v>45287</v>
       </c>
       <c r="I81">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="J81" t="inlineStr">
         <is>
@@ -8610,7 +8610,7 @@
         <v>45288</v>
       </c>
       <c r="I82">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="J82" t="inlineStr">
         <is>
@@ -8702,13 +8702,13 @@
         <v>45175</v>
       </c>
       <c r="G83">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="H83" s="2">
         <v>45357</v>
       </c>
       <c r="I83">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="J83" t="inlineStr">
         <is>
@@ -8805,13 +8805,13 @@
         <v>45054</v>
       </c>
       <c r="G84">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="H84" s="2">
         <v>45238</v>
       </c>
       <c r="I84">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="J84" t="inlineStr">
         <is>
@@ -8908,13 +8908,13 @@
         <v>45056</v>
       </c>
       <c r="G85">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="H85" s="2">
         <v>45240</v>
       </c>
       <c r="I85">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="J85" t="inlineStr">
         <is>
@@ -9011,13 +9011,13 @@
         <v>45085</v>
       </c>
       <c r="G86">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="H86" s="2">
         <v>45268</v>
       </c>
       <c r="I86">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="J86" t="inlineStr">
         <is>
@@ -9114,13 +9114,13 @@
         <v>45194</v>
       </c>
       <c r="G87">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="H87" s="2">
         <v>45560</v>
       </c>
       <c r="I87">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="J87" t="inlineStr">
         <is>
@@ -9207,13 +9207,13 @@
         <v>45103</v>
       </c>
       <c r="G88">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="H88" s="2">
         <v>45286</v>
       </c>
       <c r="I88">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="J88" t="inlineStr">
         <is>
@@ -9310,13 +9310,13 @@
         <v>45103</v>
       </c>
       <c r="G89">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="H89" s="2">
         <v>45286</v>
       </c>
       <c r="I89">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="J89" t="inlineStr">
         <is>
@@ -9413,13 +9413,13 @@
         <v>45192</v>
       </c>
       <c r="G90">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="H90" s="2">
         <v>45374</v>
       </c>
       <c r="I90">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="J90" t="inlineStr">
         <is>
@@ -9511,13 +9511,13 @@
         <v>45100</v>
       </c>
       <c r="G91">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="H91" s="2">
         <v>45287</v>
       </c>
       <c r="I91">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="J91" t="inlineStr">
         <is>
@@ -9614,13 +9614,13 @@
         <v>45187</v>
       </c>
       <c r="G92">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="H92" s="2">
         <v>45369</v>
       </c>
       <c r="I92">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="J92" t="inlineStr">
         <is>
@@ -9717,13 +9717,13 @@
         <v>45104</v>
       </c>
       <c r="G93">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="H93" s="2">
         <v>45287</v>
       </c>
       <c r="I93">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="J93" t="inlineStr">
         <is>
@@ -9820,13 +9820,13 @@
         <v>45104</v>
       </c>
       <c r="G94">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="H94" s="2">
         <v>45287</v>
       </c>
       <c r="I94">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="J94" t="inlineStr">
         <is>
@@ -9923,13 +9923,13 @@
         <v>45049</v>
       </c>
       <c r="G95">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="H95" s="2">
         <v>45233</v>
       </c>
       <c r="I95">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="J95" t="inlineStr">
         <is>
@@ -10026,13 +10026,13 @@
         <v>45122</v>
       </c>
       <c r="G96">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="H96" s="2">
         <v>45306</v>
       </c>
       <c r="I96">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="J96" t="inlineStr">
         <is>
@@ -10124,13 +10124,13 @@
         <v>45141</v>
       </c>
       <c r="G97">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="H97" s="2">
         <v>45325</v>
       </c>
       <c r="I97">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="J97" t="inlineStr">
         <is>
@@ -10227,13 +10227,13 @@
         <v>45194</v>
       </c>
       <c r="G98">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="H98" s="2">
         <v>45376</v>
       </c>
       <c r="I98">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="J98" t="inlineStr">
         <is>
@@ -10325,13 +10325,13 @@
         <v>45093</v>
       </c>
       <c r="G99">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="H99" s="2">
         <v>45276</v>
       </c>
       <c r="I99">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="J99" t="inlineStr">
         <is>
@@ -10428,13 +10428,13 @@
         <v>45123</v>
       </c>
       <c r="G100">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="H100" s="2">
         <v>45307</v>
       </c>
       <c r="I100">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="J100" t="inlineStr">
         <is>
@@ -10531,13 +10531,13 @@
         <v>45198</v>
       </c>
       <c r="G101">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="H101" s="2">
         <v>45380</v>
       </c>
       <c r="I101">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="J101" t="inlineStr">
         <is>
@@ -10634,13 +10634,13 @@
         <v>45093</v>
       </c>
       <c r="G102">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="H102" s="2">
         <v>45276</v>
       </c>
       <c r="I102">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="J102" t="inlineStr">
         <is>
@@ -10737,13 +10737,13 @@
         <v>45122</v>
       </c>
       <c r="G103">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="H103" s="2">
         <v>45306</v>
       </c>
       <c r="I103">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="J103" t="inlineStr">
         <is>
@@ -10840,13 +10840,13 @@
         <v>45122</v>
       </c>
       <c r="G104">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="H104" s="2">
         <v>45306</v>
       </c>
       <c r="I104">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="J104" t="inlineStr">
         <is>
@@ -10938,13 +10938,13 @@
         <v>45050</v>
       </c>
       <c r="G105">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="H105" s="2">
         <v>45234</v>
       </c>
       <c r="I105">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="J105" t="inlineStr">
         <is>
@@ -11041,13 +11041,13 @@
         <v>45085</v>
       </c>
       <c r="G106">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="H106" s="2">
         <v>45268</v>
       </c>
       <c r="I106">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="J106" t="inlineStr">
         <is>
@@ -11144,13 +11144,13 @@
         <v>45185</v>
       </c>
       <c r="G107">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="H107" s="2">
         <v>45276</v>
       </c>
       <c r="I107">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="J107" t="inlineStr">
         <is>
@@ -11242,13 +11242,13 @@
         <v>45185</v>
       </c>
       <c r="G108">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="H108" s="2">
         <v>45276</v>
       </c>
       <c r="I108">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="J108" t="inlineStr">
         <is>
@@ -11340,13 +11340,13 @@
         <v>45185</v>
       </c>
       <c r="G109">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="H109" s="2">
         <v>45276</v>
       </c>
       <c r="I109">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="J109" t="inlineStr">
         <is>
@@ -11443,13 +11443,13 @@
         <v>45148</v>
       </c>
       <c r="G110">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="H110" s="2">
         <v>45240</v>
       </c>
       <c r="I110">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="J110" t="inlineStr">
         <is>
@@ -11546,13 +11546,13 @@
         <v>45119</v>
       </c>
       <c r="G111">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="H111" s="2">
-        <v>45211</v>
+        <v>45303</v>
       </c>
       <c r="I111">
-        <v>1</v>
+        <v>92</v>
       </c>
       <c r="J111" t="inlineStr">
         <is>
@@ -11649,13 +11649,13 @@
         <v>45172</v>
       </c>
       <c r="G112">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="H112" s="2">
         <v>45263</v>
       </c>
       <c r="I112">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="J112" t="inlineStr">
         <is>
@@ -11752,13 +11752,13 @@
         <v>45206</v>
       </c>
       <c r="G113">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="H113" s="2">
         <v>45389</v>
       </c>
       <c r="I113">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="J113" t="inlineStr">
         <is>
@@ -11855,13 +11855,13 @@
         <v>45203</v>
       </c>
       <c r="G114">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="H114" s="2">
         <v>45295</v>
       </c>
       <c r="I114">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="J114" t="inlineStr">
         <is>
@@ -11958,7 +11958,7 @@
         <v>45218</v>
       </c>
       <c r="I115">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="J115" t="inlineStr">
         <is>
@@ -12055,13 +12055,13 @@
         <v>45161</v>
       </c>
       <c r="G116">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="H116" s="2">
         <v>45253</v>
       </c>
       <c r="I116">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="J116" t="inlineStr">
         <is>
@@ -12158,13 +12158,13 @@
         <v>45115</v>
       </c>
       <c r="G117">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="H117" s="2">
         <v>45299</v>
       </c>
       <c r="I117">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="J117" t="inlineStr">
         <is>
@@ -12256,13 +12256,13 @@
         <v>45094</v>
       </c>
       <c r="G118">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="H118" s="2">
         <v>45277</v>
       </c>
       <c r="I118">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="J118" t="inlineStr">
         <is>
@@ -12359,13 +12359,13 @@
         <v>45104</v>
       </c>
       <c r="G119">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="H119" s="2">
         <v>45287</v>
       </c>
       <c r="I119">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="J119" t="inlineStr">
         <is>
@@ -12462,13 +12462,13 @@
         <v>45104</v>
       </c>
       <c r="G120">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="H120" s="2">
         <v>45287</v>
       </c>
       <c r="I120">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="J120" t="inlineStr">
         <is>
@@ -12565,13 +12565,13 @@
         <v>45104</v>
       </c>
       <c r="G121">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="H121" s="2">
         <v>45287</v>
       </c>
       <c r="I121">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="J121" t="inlineStr">
         <is>
@@ -12668,13 +12668,13 @@
         <v>45104</v>
       </c>
       <c r="G122">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="H122" s="2">
         <v>45287</v>
       </c>
       <c r="I122">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="J122" t="inlineStr">
         <is>
@@ -12771,13 +12771,13 @@
         <v>45199</v>
       </c>
       <c r="G123">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="H123" s="2">
         <v>45291</v>
       </c>
       <c r="I123">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="J123" t="inlineStr">
         <is>
@@ -12874,13 +12874,13 @@
         <v>45197</v>
       </c>
       <c r="G124">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="H124" s="2">
         <v>45379</v>
       </c>
       <c r="I124">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="J124" t="inlineStr">
         <is>
@@ -12977,13 +12977,13 @@
         <v>45121</v>
       </c>
       <c r="G125">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="H125" s="2">
         <v>45213</v>
       </c>
       <c r="I125">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="J125" t="inlineStr">
         <is>
@@ -13080,13 +13080,13 @@
         <v>45134</v>
       </c>
       <c r="G126">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="H126" s="2">
         <v>45226</v>
       </c>
       <c r="I126">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="J126" t="inlineStr">
         <is>
@@ -13183,7 +13183,7 @@
         <v>45212</v>
       </c>
       <c r="I127">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J127" t="inlineStr">
         <is>
@@ -13280,13 +13280,13 @@
         <v>45126</v>
       </c>
       <c r="G128">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="H128" s="2">
         <v>45218</v>
       </c>
       <c r="I128">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="J128" t="inlineStr">
         <is>
@@ -13378,13 +13378,13 @@
         <v>45158</v>
       </c>
       <c r="G129">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="H129" s="2">
         <v>45250</v>
       </c>
       <c r="I129">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="J129" t="inlineStr">
         <is>
@@ -13481,13 +13481,13 @@
         <v>45171</v>
       </c>
       <c r="G130">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="H130" s="2">
         <v>45262</v>
       </c>
       <c r="I130">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="J130" t="inlineStr">
         <is>
@@ -13584,13 +13584,13 @@
         <v>45203</v>
       </c>
       <c r="G131">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="H131" s="2">
         <v>45295</v>
       </c>
       <c r="I131">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="J131" t="inlineStr">
         <is>
@@ -13687,13 +13687,13 @@
         <v>45144</v>
       </c>
       <c r="G132">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="H132" s="2">
         <v>45236</v>
       </c>
       <c r="I132">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="J132" t="inlineStr">
         <is>
@@ -13790,13 +13790,13 @@
         <v>45156</v>
       </c>
       <c r="G133">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="H133" s="2">
         <v>45248</v>
       </c>
       <c r="I133">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="J133" t="inlineStr">
         <is>
@@ -13888,13 +13888,13 @@
         <v>45146</v>
       </c>
       <c r="G134">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="H134" s="2">
         <v>45238</v>
       </c>
       <c r="I134">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="J134" t="inlineStr">
         <is>
@@ -13991,13 +13991,13 @@
         <v>45140</v>
       </c>
       <c r="G135">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="H135" s="2">
         <v>45232</v>
       </c>
       <c r="I135">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="J135" t="inlineStr">
         <is>
@@ -14094,13 +14094,13 @@
         <v>45196</v>
       </c>
       <c r="G136">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="H136" s="2">
         <v>45287</v>
       </c>
       <c r="I136">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="J136" t="inlineStr">
         <is>
@@ -14197,13 +14197,13 @@
         <v>45197</v>
       </c>
       <c r="G137">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="H137" s="2">
         <v>45288</v>
       </c>
       <c r="I137">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="J137" t="inlineStr">
         <is>
@@ -14300,13 +14300,13 @@
         <v>45179</v>
       </c>
       <c r="G138">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="H138" s="2">
         <v>45270</v>
       </c>
       <c r="I138">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="J138" t="inlineStr">
         <is>
@@ -14398,13 +14398,13 @@
         <v>45197</v>
       </c>
       <c r="G139">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="H139" s="2">
         <v>45288</v>
       </c>
       <c r="I139">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="J139" t="inlineStr">
         <is>
@@ -14501,13 +14501,13 @@
         <v>45182</v>
       </c>
       <c r="G140">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="H140" s="2">
         <v>45273</v>
       </c>
       <c r="I140">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="J140" t="inlineStr">
         <is>
@@ -14604,13 +14604,13 @@
         <v>45208</v>
       </c>
       <c r="G141">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H141" s="2">
         <v>45300</v>
       </c>
       <c r="I141">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="J141" t="inlineStr">
         <is>
@@ -14702,13 +14702,13 @@
         <v>45150</v>
       </c>
       <c r="G142">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="H142" s="2">
         <v>45242</v>
       </c>
       <c r="I142">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="J142" t="inlineStr">
         <is>
@@ -14805,7 +14805,7 @@
         <v>45238</v>
       </c>
       <c r="I143">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="J143" t="inlineStr">
         <is>
@@ -14902,13 +14902,13 @@
         <v>45171</v>
       </c>
       <c r="G144">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="H144" s="2">
         <v>45262</v>
       </c>
       <c r="I144">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="J144" t="inlineStr">
         <is>
@@ -15005,13 +15005,13 @@
         <v>45194</v>
       </c>
       <c r="G145">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="H145" s="2">
         <v>45285</v>
       </c>
       <c r="I145">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="J145" t="inlineStr">
         <is>
@@ -15098,13 +15098,7 @@
         <v>45119</v>
       </c>
       <c r="G146">
-        <v>91</v>
-      </c>
-      <c r="H146" s="2">
-        <v>45211</v>
-      </c>
-      <c r="I146">
-        <v>1</v>
+        <v>92</v>
       </c>
       <c r="J146" t="inlineStr">
         <is>
@@ -15201,13 +15195,13 @@
         <v>45165</v>
       </c>
       <c r="G147">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="H147" s="2">
         <v>45257</v>
       </c>
       <c r="I147">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="J147" t="inlineStr">
         <is>
@@ -15304,13 +15298,13 @@
         <v>45166</v>
       </c>
       <c r="G148">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="H148" s="2">
         <v>45258</v>
       </c>
       <c r="I148">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="J148" t="inlineStr">
         <is>
@@ -15407,13 +15401,13 @@
         <v>45185</v>
       </c>
       <c r="G149">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="H149" s="2">
         <v>45276</v>
       </c>
       <c r="I149">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="J149" t="inlineStr">
         <is>
@@ -15510,13 +15504,13 @@
         <v>45035</v>
       </c>
       <c r="G150">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="H150" s="2">
         <v>45218</v>
       </c>
       <c r="I150">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="J150" t="inlineStr">
         <is>
@@ -15613,13 +15607,13 @@
         <v>45174</v>
       </c>
       <c r="G151">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="H151" s="2">
         <v>45356</v>
       </c>
       <c r="I151">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="J151" t="inlineStr">
         <is>
@@ -15716,13 +15710,13 @@
         <v>45089</v>
       </c>
       <c r="G152">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="H152" s="2">
         <v>45272</v>
       </c>
       <c r="I152">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="J152" t="inlineStr">
         <is>
@@ -15819,13 +15813,13 @@
         <v>45124</v>
       </c>
       <c r="G153">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="H153" s="2">
         <v>45308</v>
       </c>
       <c r="I153">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="J153" t="inlineStr">
         <is>
@@ -15922,13 +15916,13 @@
         <v>45124</v>
       </c>
       <c r="G154">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="H154" s="2">
         <v>45308</v>
       </c>
       <c r="I154">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="J154" t="inlineStr">
         <is>
@@ -16025,13 +16019,13 @@
         <v>45209</v>
       </c>
       <c r="G155">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H155" s="2">
         <v>45392</v>
       </c>
       <c r="I155">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="J155" t="inlineStr">
         <is>
@@ -16128,13 +16122,13 @@
         <v>45209</v>
       </c>
       <c r="G156">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H156" s="2">
         <v>45392</v>
       </c>
       <c r="I156">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="J156" t="inlineStr">
         <is>
@@ -16231,13 +16225,13 @@
         <v>45209</v>
       </c>
       <c r="G157">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H157" s="2">
         <v>45392</v>
       </c>
       <c r="I157">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="J157" t="inlineStr">
         <is>
@@ -16334,13 +16328,13 @@
         <v>45209</v>
       </c>
       <c r="G158">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H158" s="2">
         <v>45392</v>
       </c>
       <c r="I158">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="J158" t="inlineStr">
         <is>
@@ -16437,13 +16431,13 @@
         <v>45156</v>
       </c>
       <c r="G159">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="H159" s="2">
         <v>45247</v>
       </c>
       <c r="I159">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="J159" t="inlineStr">
         <is>
@@ -16540,13 +16534,13 @@
         <v>45153</v>
       </c>
       <c r="G160">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="H160" s="2">
         <v>45245</v>
       </c>
       <c r="I160">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="J160" t="inlineStr">
         <is>
@@ -16643,13 +16637,13 @@
         <v>45135</v>
       </c>
       <c r="G161">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="H161" s="2">
         <v>45319</v>
       </c>
       <c r="I161">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="J161" t="inlineStr">
         <is>
@@ -16746,13 +16740,13 @@
         <v>45091</v>
       </c>
       <c r="G162">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="H162" s="2">
         <v>45274</v>
       </c>
       <c r="I162">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="J162" t="inlineStr">
         <is>
@@ -16844,13 +16838,13 @@
         <v>45091</v>
       </c>
       <c r="G163">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="H163" s="2">
         <v>45274</v>
       </c>
       <c r="I163">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="J163" t="inlineStr">
         <is>
@@ -16942,13 +16936,13 @@
         <v>45138</v>
       </c>
       <c r="G164">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="H164" s="2">
         <v>45322</v>
       </c>
       <c r="I164">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="J164" t="inlineStr">
         <is>
@@ -17045,13 +17039,13 @@
         <v>45138</v>
       </c>
       <c r="G165">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="H165" s="2">
         <v>45322</v>
       </c>
       <c r="I165">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="J165" t="inlineStr">
         <is>
@@ -17148,13 +17142,13 @@
         <v>45085</v>
       </c>
       <c r="G166">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="H166" s="2">
         <v>45268</v>
       </c>
       <c r="I166">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="J166" t="inlineStr">
         <is>
@@ -17251,13 +17245,13 @@
         <v>45085</v>
       </c>
       <c r="G167">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="H167" s="2">
         <v>45268</v>
       </c>
       <c r="I167">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="J167" t="inlineStr">
         <is>
@@ -17354,7 +17348,7 @@
         <v>45326</v>
       </c>
       <c r="I168">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="J168" t="inlineStr">
         <is>
@@ -17451,13 +17445,13 @@
         <v>45173</v>
       </c>
       <c r="G169">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="H169" s="2">
         <v>45355</v>
       </c>
       <c r="I169">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="J169" t="inlineStr">
         <is>
@@ -17554,13 +17548,13 @@
         <v>45056</v>
       </c>
       <c r="G170">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="H170" s="2">
         <v>45240</v>
       </c>
       <c r="I170">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="J170" t="inlineStr">
         <is>
@@ -17657,7 +17651,7 @@
         <v>45238</v>
       </c>
       <c r="I171">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="J171" t="inlineStr">
         <is>
@@ -17754,13 +17748,13 @@
         <v>45141</v>
       </c>
       <c r="G172">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="H172" s="2">
         <v>45325</v>
       </c>
       <c r="I172">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="J172" t="inlineStr">
         <is>
@@ -17857,13 +17851,13 @@
         <v>45037</v>
       </c>
       <c r="G173">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="H173" s="2">
         <v>45220</v>
       </c>
       <c r="I173">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="J173" t="inlineStr">
         <is>
@@ -17960,13 +17954,13 @@
         <v>45171</v>
       </c>
       <c r="G174">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="H174" s="2">
         <v>45262</v>
       </c>
       <c r="I174">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="J174" t="inlineStr">
         <is>
@@ -18063,13 +18057,13 @@
         <v>45197</v>
       </c>
       <c r="G175">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="H175" s="2">
         <v>45288</v>
       </c>
       <c r="I175">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="J175" t="inlineStr">
         <is>
@@ -18166,13 +18160,13 @@
         <v>45162</v>
       </c>
       <c r="G176">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="H176" s="2">
         <v>45254</v>
       </c>
       <c r="I176">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="J176" t="inlineStr">
         <is>
@@ -18269,13 +18263,13 @@
         <v>45061</v>
       </c>
       <c r="G177">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="H177" s="2">
         <v>45245</v>
       </c>
       <c r="I177">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="J177" t="inlineStr">
         <is>
@@ -18372,13 +18366,13 @@
         <v>45120</v>
       </c>
       <c r="G178">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="H178" s="2">
         <v>45212</v>
       </c>
       <c r="I178">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J178" t="inlineStr">
         <is>
@@ -18475,13 +18469,13 @@
         <v>45191</v>
       </c>
       <c r="G179">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="H179" s="2">
         <v>45282</v>
       </c>
       <c r="I179">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="J179" t="inlineStr">
         <is>
@@ -18578,13 +18572,13 @@
         <v>45088</v>
       </c>
       <c r="G180">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="H180" s="2">
         <v>45271</v>
       </c>
       <c r="I180">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="J180" t="inlineStr">
         <is>
@@ -18681,13 +18675,13 @@
         <v>45192</v>
       </c>
       <c r="G181">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="H181" s="2">
         <v>45283</v>
       </c>
       <c r="I181">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="J181" t="inlineStr">
         <is>
@@ -18774,13 +18768,13 @@
         <v>45131</v>
       </c>
       <c r="G182">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="H182" s="2">
         <v>45223</v>
       </c>
       <c r="I182">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="J182" t="inlineStr">
         <is>
@@ -18872,13 +18866,13 @@
         <v>45136</v>
       </c>
       <c r="G183">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="H183" s="2">
         <v>45228</v>
       </c>
       <c r="I183">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="J183" t="inlineStr">
         <is>
@@ -18970,13 +18964,13 @@
         <v>45150</v>
       </c>
       <c r="G184">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="H184" s="2">
         <v>45242</v>
       </c>
       <c r="I184">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="J184" t="inlineStr">
         <is>
@@ -19065,10 +19059,10 @@
         </is>
       </c>
       <c r="F185" s="2">
-        <v>45118</v>
+        <v>45210</v>
       </c>
       <c r="G185">
-        <v>92</v>
+        <v>1</v>
       </c>
       <c r="J185" t="inlineStr">
         <is>
@@ -19160,13 +19154,13 @@
         <v>45129</v>
       </c>
       <c r="G186">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="H186" s="2">
         <v>45221</v>
       </c>
       <c r="I186">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="J186" t="inlineStr">
         <is>
@@ -19258,13 +19252,13 @@
         <v>45189</v>
       </c>
       <c r="G187">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="H187" s="2">
         <v>45280</v>
       </c>
       <c r="I187">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="J187" t="inlineStr">
         <is>
@@ -19351,13 +19345,13 @@
         <v>45193</v>
       </c>
       <c r="G188">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="H188" s="2">
         <v>45284</v>
       </c>
       <c r="I188">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="J188" t="inlineStr">
         <is>
@@ -19444,13 +19438,13 @@
         <v>45165</v>
       </c>
       <c r="G189">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="H189" s="2">
         <v>45257</v>
       </c>
       <c r="I189">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="J189" t="inlineStr">
         <is>
@@ -19542,13 +19536,13 @@
         <v>45202</v>
       </c>
       <c r="G190">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="H190" s="2">
         <v>45385</v>
       </c>
       <c r="I190">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="J190" t="inlineStr">
         <is>
@@ -19645,13 +19639,13 @@
         <v>45081</v>
       </c>
       <c r="G191">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="H191" s="2">
         <v>45264</v>
       </c>
       <c r="I191">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="J191" t="inlineStr">
         <is>
@@ -19748,13 +19742,13 @@
         <v>45081</v>
       </c>
       <c r="G192">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="H192" s="2">
         <v>45264</v>
       </c>
       <c r="I192">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="J192" t="inlineStr">
         <is>
@@ -19851,7 +19845,7 @@
         <v>45319</v>
       </c>
       <c r="I193">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="J193" t="inlineStr">
         <is>
@@ -19948,7 +19942,7 @@
         <v>45319</v>
       </c>
       <c r="I194">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="J194" t="inlineStr">
         <is>
@@ -20040,13 +20034,13 @@
         <v>45046</v>
       </c>
       <c r="G195">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="H195" s="2">
         <v>45230</v>
       </c>
       <c r="I195">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="J195" t="inlineStr">
         <is>
@@ -20143,13 +20137,13 @@
         <v>45046</v>
       </c>
       <c r="G196">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="H196" s="2">
         <v>45230</v>
       </c>
       <c r="I196">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="J196" t="inlineStr">
         <is>
@@ -20246,13 +20240,13 @@
         <v>45031</v>
       </c>
       <c r="G197">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="H197" s="2">
         <v>45214</v>
       </c>
       <c r="I197">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="J197" t="inlineStr">
         <is>
@@ -20349,13 +20343,13 @@
         <v>45031</v>
       </c>
       <c r="G198">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="H198" s="2">
         <v>45214</v>
       </c>
       <c r="I198">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="J198" t="inlineStr">
         <is>
@@ -20452,13 +20446,13 @@
         <v>45031</v>
       </c>
       <c r="G199">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="H199" s="2">
         <v>45214</v>
       </c>
       <c r="I199">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="J199" t="inlineStr">
         <is>
@@ -20555,13 +20549,13 @@
         <v>45031</v>
       </c>
       <c r="G200">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="H200" s="2">
         <v>45214</v>
       </c>
       <c r="I200">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="J200" t="inlineStr">
         <is>
@@ -20658,13 +20652,13 @@
         <v>45067</v>
       </c>
       <c r="G201">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="H201" s="2">
         <v>45251</v>
       </c>
       <c r="I201">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="J201" t="inlineStr">
         <is>
@@ -20761,13 +20755,13 @@
         <v>45067</v>
       </c>
       <c r="G202">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="H202" s="2">
         <v>45251</v>
       </c>
       <c r="I202">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="J202" t="inlineStr">
         <is>
@@ -20864,13 +20858,13 @@
         <v>45067</v>
       </c>
       <c r="G203">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="H203" s="2">
         <v>45251</v>
       </c>
       <c r="I203">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="J203" t="inlineStr">
         <is>
@@ -20967,13 +20961,13 @@
         <v>45067</v>
       </c>
       <c r="G204">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="H204" s="2">
         <v>45251</v>
       </c>
       <c r="I204">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="J204" t="inlineStr">
         <is>
@@ -21070,13 +21064,13 @@
         <v>45178</v>
       </c>
       <c r="G205">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="H205" s="2">
         <v>45269</v>
       </c>
       <c r="I205">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="J205" t="inlineStr">
         <is>
@@ -21173,7 +21167,7 @@
         <v>45252</v>
       </c>
       <c r="I206">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="J206" t="inlineStr">
         <is>
@@ -21270,13 +21264,13 @@
         <v>45087</v>
       </c>
       <c r="G207">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="H207" s="2">
         <v>45270</v>
       </c>
       <c r="I207">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="J207" t="inlineStr">
         <is>
@@ -21373,13 +21367,13 @@
         <v>45099</v>
       </c>
       <c r="G208">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="H208" s="2">
         <v>45282</v>
       </c>
       <c r="I208">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="J208" t="inlineStr">
         <is>
@@ -21476,13 +21470,13 @@
         <v>45175</v>
       </c>
       <c r="G209">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="H209" s="2">
         <v>45356</v>
       </c>
       <c r="I209">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="J209" t="inlineStr">
         <is>
@@ -21579,13 +21573,13 @@
         <v>45175</v>
       </c>
       <c r="G210">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="H210" s="2">
         <v>45356</v>
       </c>
       <c r="I210">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="J210" t="inlineStr">
         <is>
@@ -21682,13 +21676,13 @@
         <v>45166</v>
       </c>
       <c r="G211">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="H211" s="2">
         <v>45350</v>
       </c>
       <c r="I211">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="J211" t="inlineStr">
         <is>
@@ -21785,13 +21779,13 @@
         <v>45166</v>
       </c>
       <c r="G212">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="H212" s="2">
         <v>45350</v>
       </c>
       <c r="I212">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="J212" t="inlineStr">
         <is>
@@ -21888,13 +21882,13 @@
         <v>45090</v>
       </c>
       <c r="G213">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="H213" s="2">
         <v>45273</v>
       </c>
       <c r="I213">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="J213" t="inlineStr">
         <is>
@@ -21991,13 +21985,13 @@
         <v>45106</v>
       </c>
       <c r="G214">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="H214" s="2">
         <v>45289</v>
       </c>
       <c r="I214">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="J214" t="inlineStr">
         <is>
@@ -22094,13 +22088,13 @@
         <v>45134</v>
       </c>
       <c r="G215">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="H215" s="2">
         <v>45226</v>
       </c>
       <c r="I215">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="J215" t="inlineStr">
         <is>
@@ -22197,13 +22191,13 @@
         <v>45132</v>
       </c>
       <c r="G216">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="H216" s="2">
         <v>45224</v>
       </c>
       <c r="I216">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="J216" t="inlineStr">
         <is>
@@ -22300,13 +22294,13 @@
         <v>45150</v>
       </c>
       <c r="G217">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="H217" s="2">
         <v>45242</v>
       </c>
       <c r="I217">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="J217" t="inlineStr">
         <is>
@@ -22403,13 +22397,13 @@
         <v>45187</v>
       </c>
       <c r="G218">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="H218" s="2">
         <v>45278</v>
       </c>
       <c r="I218">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="J218" t="inlineStr">
         <is>
@@ -22501,13 +22495,13 @@
         <v>45182</v>
       </c>
       <c r="G219">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="H219" s="2">
         <v>45273</v>
       </c>
       <c r="I219">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="J219" t="inlineStr">
         <is>
@@ -22604,13 +22598,13 @@
         <v>45196</v>
       </c>
       <c r="G220">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="H220" s="2">
         <v>45287</v>
       </c>
       <c r="I220">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="J220" t="inlineStr">
         <is>
@@ -22707,13 +22701,13 @@
         <v>45200</v>
       </c>
       <c r="G221">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="H221" s="2">
         <v>45292</v>
       </c>
       <c r="I221">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="J221" t="inlineStr">
         <is>
@@ -22810,13 +22804,13 @@
         <v>45135</v>
       </c>
       <c r="G222">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="H222" s="2">
         <v>45227</v>
       </c>
       <c r="I222">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="J222" t="inlineStr">
         <is>
@@ -22913,13 +22907,13 @@
         <v>45148</v>
       </c>
       <c r="G223">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="H223" s="2">
         <v>45240</v>
       </c>
       <c r="I223">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="J223" t="inlineStr">
         <is>
@@ -23011,13 +23005,13 @@
         <v>45192</v>
       </c>
       <c r="G224">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="H224" s="2">
         <v>45283</v>
       </c>
       <c r="I224">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="J224" t="inlineStr">
         <is>
@@ -23109,13 +23103,13 @@
         <v>45136</v>
       </c>
       <c r="G225">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="H225" s="2">
         <v>45320</v>
       </c>
       <c r="I225">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="J225" t="inlineStr">
         <is>
@@ -23212,13 +23206,13 @@
         <v>45136</v>
       </c>
       <c r="G226">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="H226" s="2">
         <v>45320</v>
       </c>
       <c r="I226">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="J226" t="inlineStr">
         <is>
@@ -23315,13 +23309,13 @@
         <v>45094</v>
       </c>
       <c r="G227">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="H227" s="2">
         <v>45277</v>
       </c>
       <c r="I227">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="J227" t="inlineStr">
         <is>
@@ -23418,13 +23412,13 @@
         <v>45081</v>
       </c>
       <c r="G228">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="H228" s="2">
         <v>45264</v>
       </c>
       <c r="I228">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="J228" t="inlineStr">
         <is>
@@ -23521,13 +23515,13 @@
         <v>45099</v>
       </c>
       <c r="G229">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="H229" s="2">
         <v>45282</v>
       </c>
       <c r="I229">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="J229" t="inlineStr">
         <is>
@@ -23624,13 +23618,13 @@
         <v>45201</v>
       </c>
       <c r="G230">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="H230" s="2">
         <v>45384</v>
       </c>
       <c r="I230">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="J230" t="inlineStr">
         <is>
@@ -23727,13 +23721,13 @@
         <v>45031</v>
       </c>
       <c r="G231">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="H231" s="2">
         <v>45214</v>
       </c>
       <c r="I231">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="J231" t="inlineStr">
         <is>
@@ -23830,7 +23824,7 @@
         <v>45294</v>
       </c>
       <c r="I232">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="J232" t="inlineStr">
         <is>
@@ -23927,13 +23921,13 @@
         <v>45079</v>
       </c>
       <c r="G233">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="H233" s="2">
         <v>45262</v>
       </c>
       <c r="I233">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="J233" t="inlineStr">
         <is>
@@ -24030,13 +24024,13 @@
         <v>45199</v>
       </c>
       <c r="G234">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="H234" s="2">
         <v>45382</v>
       </c>
       <c r="I234">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="J234" t="inlineStr">
         <is>
@@ -24133,13 +24127,13 @@
         <v>45204</v>
       </c>
       <c r="G235">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="H235" s="2">
         <v>45387</v>
       </c>
       <c r="I235">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="J235" t="inlineStr">
         <is>
@@ -24236,13 +24230,13 @@
         <v>45204</v>
       </c>
       <c r="G236">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="H236" s="2">
         <v>45387</v>
       </c>
       <c r="I236">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="J236" t="inlineStr">
         <is>
@@ -24339,13 +24333,13 @@
         <v>45080</v>
       </c>
       <c r="G237">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="H237" s="2">
         <v>45263</v>
       </c>
       <c r="I237">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="J237" t="inlineStr">
         <is>
@@ -24442,13 +24436,13 @@
         <v>45046</v>
       </c>
       <c r="G238">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="H238" s="2">
         <v>45229</v>
       </c>
       <c r="I238">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="J238" t="inlineStr">
         <is>
@@ -24545,13 +24539,13 @@
         <v>45204</v>
       </c>
       <c r="G239">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="H239" s="2">
         <v>45296</v>
       </c>
       <c r="I239">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="J239" t="inlineStr">
         <is>
@@ -24648,13 +24642,13 @@
         <v>45204</v>
       </c>
       <c r="G240">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="H240" s="2">
         <v>45296</v>
       </c>
       <c r="I240">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="J240" t="inlineStr">
         <is>
@@ -24751,13 +24745,13 @@
         <v>45199</v>
       </c>
       <c r="G241">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="H241" s="2">
         <v>45382</v>
       </c>
       <c r="I241">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="J241" t="inlineStr">
         <is>
@@ -24854,13 +24848,13 @@
         <v>45070</v>
       </c>
       <c r="G242">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="H242" s="2">
         <v>45254</v>
       </c>
       <c r="I242">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="J242" t="inlineStr">
         <is>
@@ -24957,13 +24951,13 @@
         <v>45168</v>
       </c>
       <c r="G243">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="H243" s="2">
         <v>45260</v>
       </c>
       <c r="I243">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="J243" t="inlineStr">
         <is>
@@ -25057,16 +25051,16 @@
         </is>
       </c>
       <c r="F244" s="2">
-        <v>45027</v>
+        <v>45210</v>
       </c>
       <c r="G244">
-        <v>183</v>
+        <v>1</v>
       </c>
       <c r="H244" s="2">
         <v>45393</v>
       </c>
       <c r="I244">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="J244" t="inlineStr">
         <is>
@@ -25163,13 +25157,13 @@
         <v>45077</v>
       </c>
       <c r="G245">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="H245" s="2">
         <v>45260</v>
       </c>
       <c r="I245">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="J245" t="inlineStr">
         <is>
@@ -25266,13 +25260,13 @@
         <v>45100</v>
       </c>
       <c r="G246">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="H246" s="2">
         <v>45283</v>
       </c>
       <c r="I246">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="J246" t="inlineStr">
         <is>
@@ -25369,7 +25363,7 @@
         <v>45281</v>
       </c>
       <c r="I247">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="J247" t="inlineStr">
         <is>
@@ -25466,13 +25460,13 @@
         <v>45044</v>
       </c>
       <c r="G248">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="H248" s="2">
         <v>45227</v>
       </c>
       <c r="I248">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="J248" t="inlineStr">
         <is>
@@ -25569,13 +25563,13 @@
         <v>45101</v>
       </c>
       <c r="G249">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="H249" s="2">
         <v>45283</v>
       </c>
       <c r="I249">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="J249" t="inlineStr">
         <is>
@@ -25672,13 +25666,13 @@
         <v>45134</v>
       </c>
       <c r="G250">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="H250" s="2">
         <v>45226</v>
       </c>
       <c r="I250">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="J250" t="inlineStr">
         <is>
@@ -25775,13 +25769,13 @@
         <v>45158</v>
       </c>
       <c r="G251">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="H251" s="2">
         <v>45250</v>
       </c>
       <c r="I251">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="J251" t="inlineStr">
         <is>
@@ -25878,13 +25872,13 @@
         <v>45200</v>
       </c>
       <c r="G252">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="H252" s="2">
         <v>45292</v>
       </c>
       <c r="I252">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="J252" t="inlineStr">
         <is>
@@ -25981,7 +25975,7 @@
         <v>45317</v>
       </c>
       <c r="I253">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="J253" t="inlineStr">
         <is>
@@ -26078,13 +26072,13 @@
         <v>45039</v>
       </c>
       <c r="G254">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="H254" s="2">
         <v>45222</v>
       </c>
       <c r="I254">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="J254" t="inlineStr">
         <is>
@@ -26176,13 +26170,13 @@
         <v>45129</v>
       </c>
       <c r="G255">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="H255" s="2">
         <v>45221</v>
       </c>
       <c r="I255">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="J255" t="inlineStr">
         <is>
@@ -26279,13 +26273,13 @@
         <v>45157</v>
       </c>
       <c r="G256">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="H256" s="2">
         <v>45341</v>
       </c>
       <c r="I256">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="J256" t="inlineStr">
         <is>
@@ -26382,13 +26376,13 @@
         <v>45063</v>
       </c>
       <c r="G257">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="H257" s="2">
         <v>45247</v>
       </c>
       <c r="I257">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="J257" t="inlineStr">
         <is>
@@ -26485,7 +26479,7 @@
         <v>45254</v>
       </c>
       <c r="I258">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="J258" t="inlineStr">
         <is>
@@ -26582,7 +26576,7 @@
         <v>45486</v>
       </c>
       <c r="I259">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="J259" t="inlineStr">
         <is>
@@ -26674,13 +26668,13 @@
         <v>45073</v>
       </c>
       <c r="G260">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="H260" s="2">
         <v>45439</v>
       </c>
       <c r="I260">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="J260" t="inlineStr">
         <is>
@@ -26772,7 +26766,7 @@
         <v>45323</v>
       </c>
       <c r="I261">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="J261" t="inlineStr">
         <is>
@@ -26864,7 +26858,7 @@
         <v>45303</v>
       </c>
       <c r="I262">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="J262" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
Bond dates update Fri Oct 13 23:16:09 UTC 2023
</commit_message>
<xml_diff>
--- a/Data/obligacje_screener.xlsx
+++ b/Data/obligacje_screener.xlsx
@@ -512,7 +512,7 @@
         <v>45340</v>
       </c>
       <c r="I2">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="J2" t="inlineStr">
         <is>
@@ -600,13 +600,13 @@
         <v>45121</v>
       </c>
       <c r="G3">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="H3" s="2">
         <v>45305</v>
       </c>
       <c r="I3">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="J3" t="inlineStr">
         <is>
@@ -703,13 +703,13 @@
         <v>45039</v>
       </c>
       <c r="G4">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="H4" s="2">
         <v>45222</v>
       </c>
       <c r="I4">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="J4" t="inlineStr">
         <is>
@@ -806,13 +806,13 @@
         <v>45039</v>
       </c>
       <c r="G5">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="H5" s="2">
         <v>45222</v>
       </c>
       <c r="I5">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="J5" t="inlineStr">
         <is>
@@ -909,13 +909,13 @@
         <v>45129</v>
       </c>
       <c r="G6">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="H6" s="2">
         <v>45221</v>
       </c>
       <c r="I6">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="J6" t="inlineStr">
         <is>
@@ -1012,13 +1012,13 @@
         <v>45162</v>
       </c>
       <c r="G7">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="H7" s="2">
         <v>45254</v>
       </c>
       <c r="I7">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="J7" t="inlineStr">
         <is>
@@ -1110,13 +1110,13 @@
         <v>45156</v>
       </c>
       <c r="G8">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="H8" s="2">
         <v>45248</v>
       </c>
       <c r="I8">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="J8" t="inlineStr">
         <is>
@@ -1213,13 +1213,13 @@
         <v>45141</v>
       </c>
       <c r="G9">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="H9" s="2">
         <v>45233</v>
       </c>
       <c r="I9">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="J9" t="inlineStr">
         <is>
@@ -1316,13 +1316,13 @@
         <v>45062</v>
       </c>
       <c r="G10">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="H10" s="2">
         <v>45246</v>
       </c>
       <c r="I10">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="J10" t="inlineStr">
         <is>
@@ -1419,7 +1419,7 @@
         <v>45286</v>
       </c>
       <c r="I11">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="J11" t="inlineStr">
         <is>
@@ -1516,13 +1516,13 @@
         <v>45195</v>
       </c>
       <c r="G12">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="H12" s="2">
         <v>45377</v>
       </c>
       <c r="I12">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="J12" t="inlineStr">
         <is>
@@ -1614,13 +1614,13 @@
         <v>45036</v>
       </c>
       <c r="G13">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="H13" s="2">
         <v>45219</v>
       </c>
       <c r="I13">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="J13" t="inlineStr">
         <is>
@@ -1717,13 +1717,13 @@
         <v>45036</v>
       </c>
       <c r="G14">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="H14" s="2">
         <v>45219</v>
       </c>
       <c r="I14">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="J14" t="inlineStr">
         <is>
@@ -1820,13 +1820,13 @@
         <v>45106</v>
       </c>
       <c r="G15">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="H15" s="2">
         <v>45289</v>
       </c>
       <c r="I15">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="J15" t="inlineStr">
         <is>
@@ -1923,13 +1923,13 @@
         <v>45186</v>
       </c>
       <c r="G16">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="H16" s="2">
         <v>45278</v>
       </c>
       <c r="I16">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="J16" t="inlineStr">
         <is>
@@ -2026,13 +2026,13 @@
         <v>45186</v>
       </c>
       <c r="G17">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="H17" s="2">
         <v>45277</v>
       </c>
       <c r="I17">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="J17" t="inlineStr">
         <is>
@@ -2129,13 +2129,13 @@
         <v>45132</v>
       </c>
       <c r="G18">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="H18" s="2">
         <v>45224</v>
       </c>
       <c r="I18">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="J18" t="inlineStr">
         <is>
@@ -2232,13 +2232,13 @@
         <v>45137</v>
       </c>
       <c r="G19">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="H19" s="2">
         <v>45229</v>
       </c>
       <c r="I19">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="J19" t="inlineStr">
         <is>
@@ -2330,13 +2330,13 @@
         <v>45183</v>
       </c>
       <c r="G20">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="H20" s="2">
         <v>45274</v>
       </c>
       <c r="I20">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="J20" t="inlineStr">
         <is>
@@ -2433,13 +2433,13 @@
         <v>45187</v>
       </c>
       <c r="G21">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="H21" s="2">
         <v>45278</v>
       </c>
       <c r="I21">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="J21" t="inlineStr">
         <is>
@@ -2536,13 +2536,13 @@
         <v>45187</v>
       </c>
       <c r="G22">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="H22" s="2">
         <v>45278</v>
       </c>
       <c r="I22">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="J22" t="inlineStr">
         <is>
@@ -2639,7 +2639,7 @@
         <v>45245</v>
       </c>
       <c r="I23">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="J23" t="inlineStr">
         <is>
@@ -2736,7 +2736,7 @@
         <v>45245</v>
       </c>
       <c r="I24">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="J24" t="inlineStr">
         <is>
@@ -2833,7 +2833,7 @@
         <v>45204</v>
       </c>
       <c r="G25">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="J25" t="inlineStr">
         <is>
@@ -2930,13 +2930,13 @@
         <v>45160</v>
       </c>
       <c r="G26">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="H26" s="2">
         <v>45344</v>
       </c>
       <c r="I26">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="J26" t="inlineStr">
         <is>
@@ -3033,13 +3033,13 @@
         <v>45118</v>
       </c>
       <c r="G27">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="H27" s="2">
         <v>45302</v>
       </c>
       <c r="I27">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="J27" t="inlineStr">
         <is>
@@ -3136,13 +3136,13 @@
         <v>45085</v>
       </c>
       <c r="G28">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="H28" s="2">
         <v>45268</v>
       </c>
       <c r="I28">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="J28" t="inlineStr">
         <is>
@@ -3239,13 +3239,13 @@
         <v>45183</v>
       </c>
       <c r="G29">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="H29" s="2">
         <v>45274</v>
       </c>
       <c r="I29">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="J29" t="inlineStr">
         <is>
@@ -3342,7 +3342,7 @@
         <v>45224</v>
       </c>
       <c r="I30">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="J30" t="inlineStr">
         <is>
@@ -3439,13 +3439,13 @@
         <v>45153</v>
       </c>
       <c r="G31">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="H31" s="2">
         <v>45245</v>
       </c>
       <c r="I31">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="J31" t="inlineStr">
         <is>
@@ -3542,13 +3542,13 @@
         <v>45155</v>
       </c>
       <c r="G32">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="H32" s="2">
         <v>45247</v>
       </c>
       <c r="I32">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="J32" t="inlineStr">
         <is>
@@ -3645,7 +3645,7 @@
         <v>45255</v>
       </c>
       <c r="I33">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="J33" t="inlineStr">
         <is>
@@ -3742,13 +3742,13 @@
         <v>45176</v>
       </c>
       <c r="G34">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="H34" s="2">
         <v>45267</v>
       </c>
       <c r="I34">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="J34" t="inlineStr">
         <is>
@@ -3845,13 +3845,13 @@
         <v>45130</v>
       </c>
       <c r="G35">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="H35" s="2">
         <v>45222</v>
       </c>
       <c r="I35">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="J35" t="inlineStr">
         <is>
@@ -3943,13 +3943,13 @@
         <v>45207</v>
       </c>
       <c r="G36">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="H36" s="2">
         <v>45299</v>
       </c>
       <c r="I36">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="J36" t="inlineStr">
         <is>
@@ -4046,13 +4046,13 @@
         <v>45189</v>
       </c>
       <c r="G37">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="H37" s="2">
         <v>45280</v>
       </c>
       <c r="I37">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="J37" t="inlineStr">
         <is>
@@ -4144,13 +4144,13 @@
         <v>45107</v>
       </c>
       <c r="G38">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="H38" s="2">
         <v>45290</v>
       </c>
       <c r="I38">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="J38" t="inlineStr">
         <is>
@@ -4247,13 +4247,13 @@
         <v>45063</v>
       </c>
       <c r="G39">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="H39" s="2">
         <v>45247</v>
       </c>
       <c r="I39">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="J39" t="inlineStr">
         <is>
@@ -4350,13 +4350,13 @@
         <v>45177</v>
       </c>
       <c r="G40">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="H40" s="2">
         <v>45359</v>
       </c>
       <c r="I40">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="J40" t="inlineStr">
         <is>
@@ -4453,13 +4453,13 @@
         <v>45107</v>
       </c>
       <c r="G41">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="H41" s="2">
         <v>45290</v>
       </c>
       <c r="I41">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="J41" t="inlineStr">
         <is>
@@ -4556,7 +4556,7 @@
         <v>45265</v>
       </c>
       <c r="I42">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="J42" t="inlineStr">
         <is>
@@ -4653,13 +4653,13 @@
         <v>45098</v>
       </c>
       <c r="G43">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="H43" s="2">
         <v>45281</v>
       </c>
       <c r="I43">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="J43" t="inlineStr">
         <is>
@@ -4756,13 +4756,13 @@
         <v>45099</v>
       </c>
       <c r="G44">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="H44" s="2">
         <v>45282</v>
       </c>
       <c r="I44">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="J44" t="inlineStr">
         <is>
@@ -4859,13 +4859,13 @@
         <v>45106</v>
       </c>
       <c r="G45">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="H45" s="2">
         <v>45289</v>
       </c>
       <c r="I45">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="J45" t="inlineStr">
         <is>
@@ -4962,13 +4962,13 @@
         <v>45106</v>
       </c>
       <c r="G46">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="H46" s="2">
         <v>45289</v>
       </c>
       <c r="I46">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="J46" t="inlineStr">
         <is>
@@ -5065,13 +5065,13 @@
         <v>45120</v>
       </c>
       <c r="G47">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="H47" s="2">
         <v>45304</v>
       </c>
       <c r="I47">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="J47" t="inlineStr">
         <is>
@@ -5168,13 +5168,13 @@
         <v>45118</v>
       </c>
       <c r="G48">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="H48" s="2">
         <v>45302</v>
       </c>
       <c r="I48">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="J48" t="inlineStr">
         <is>
@@ -5271,13 +5271,13 @@
         <v>45152</v>
       </c>
       <c r="G49">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="H49" s="2">
         <v>45336</v>
       </c>
       <c r="I49">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="J49" t="inlineStr">
         <is>
@@ -5374,13 +5374,13 @@
         <v>45042</v>
       </c>
       <c r="G50">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="H50" s="2">
         <v>45225</v>
       </c>
       <c r="I50">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="J50" t="inlineStr">
         <is>
@@ -5477,13 +5477,13 @@
         <v>45122</v>
       </c>
       <c r="G51">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="H51" s="2">
         <v>45306</v>
       </c>
       <c r="I51">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="J51" t="inlineStr">
         <is>
@@ -5580,13 +5580,13 @@
         <v>45139</v>
       </c>
       <c r="G52">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="H52" s="2">
         <v>45323</v>
       </c>
       <c r="I52">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="J52" t="inlineStr">
         <is>
@@ -5683,13 +5683,13 @@
         <v>45099</v>
       </c>
       <c r="G53">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="H53" s="2">
         <v>45282</v>
       </c>
       <c r="I53">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="J53" t="inlineStr">
         <is>
@@ -5786,13 +5786,13 @@
         <v>45196</v>
       </c>
       <c r="G54">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H54" s="2">
         <v>45287</v>
       </c>
       <c r="I54">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="J54" t="inlineStr">
         <is>
@@ -5889,13 +5889,13 @@
         <v>45044</v>
       </c>
       <c r="G55">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="H55" s="2">
         <v>45227</v>
       </c>
       <c r="I55">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="J55" t="inlineStr">
         <is>
@@ -5992,13 +5992,13 @@
         <v>45151</v>
       </c>
       <c r="G56">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="H56" s="2">
         <v>45243</v>
       </c>
       <c r="I56">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="J56" t="inlineStr">
         <is>
@@ -6090,13 +6090,13 @@
         <v>45196</v>
       </c>
       <c r="G57">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H57" s="2">
         <v>45287</v>
       </c>
       <c r="I57">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="J57" t="inlineStr">
         <is>
@@ -6193,13 +6193,13 @@
         <v>45069</v>
       </c>
       <c r="G58">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="H58" s="2">
         <v>45253</v>
       </c>
       <c r="I58">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="J58" t="inlineStr">
         <is>
@@ -6296,13 +6296,13 @@
         <v>45191</v>
       </c>
       <c r="G59">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="H59" s="2">
         <v>45282</v>
       </c>
       <c r="I59">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="J59" t="inlineStr">
         <is>
@@ -6394,7 +6394,7 @@
         <v>45205</v>
       </c>
       <c r="G60">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="J60" t="inlineStr">
         <is>
@@ -6491,13 +6491,13 @@
         <v>45127</v>
       </c>
       <c r="G61">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="H61" s="2">
         <v>45219</v>
       </c>
       <c r="I61">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="J61" t="inlineStr">
         <is>
@@ -6594,13 +6594,13 @@
         <v>45058</v>
       </c>
       <c r="G62">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="H62" s="2">
         <v>45242</v>
       </c>
       <c r="I62">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="J62" t="inlineStr">
         <is>
@@ -6697,13 +6697,13 @@
         <v>45194</v>
       </c>
       <c r="G63">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="H63" s="2">
         <v>45376</v>
       </c>
       <c r="I63">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="J63" t="inlineStr">
         <is>
@@ -6795,7 +6795,7 @@
         <v>45208</v>
       </c>
       <c r="G64">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="J64" t="inlineStr">
         <is>
@@ -6892,7 +6892,7 @@
         <v>45208</v>
       </c>
       <c r="G65">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="J65" t="inlineStr">
         <is>
@@ -6989,13 +6989,13 @@
         <v>45089</v>
       </c>
       <c r="G66">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="H66" s="2">
         <v>45272</v>
       </c>
       <c r="I66">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="J66" t="inlineStr">
         <is>
@@ -7092,13 +7092,13 @@
         <v>45178</v>
       </c>
       <c r="G67">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="H67" s="2">
         <v>45269</v>
       </c>
       <c r="I67">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="J67" t="inlineStr">
         <is>
@@ -7190,13 +7190,13 @@
         <v>45196</v>
       </c>
       <c r="G68">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H68" s="2">
         <v>45287</v>
       </c>
       <c r="I68">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="J68" t="inlineStr">
         <is>
@@ -7293,13 +7293,13 @@
         <v>45149</v>
       </c>
       <c r="G69">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="H69" s="2">
         <v>45241</v>
       </c>
       <c r="I69">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="J69" t="inlineStr">
         <is>
@@ -7396,13 +7396,13 @@
         <v>45205</v>
       </c>
       <c r="G70">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="H70" s="2">
         <v>45296</v>
       </c>
       <c r="I70">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="J70" t="inlineStr">
         <is>
@@ -7499,7 +7499,7 @@
         <v>45205</v>
       </c>
       <c r="G71">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="J71" t="inlineStr">
         <is>
@@ -7596,13 +7596,13 @@
         <v>45207</v>
       </c>
       <c r="G72">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="H72" s="2">
         <v>45299</v>
       </c>
       <c r="I72">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="J72" t="inlineStr">
         <is>
@@ -7699,13 +7699,13 @@
         <v>45189</v>
       </c>
       <c r="G73">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="H73" s="2">
         <v>45280</v>
       </c>
       <c r="I73">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="J73" t="inlineStr">
         <is>
@@ -7797,13 +7797,13 @@
         <v>45038</v>
       </c>
       <c r="G74">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="H74" s="2">
         <v>45221</v>
       </c>
       <c r="I74">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="J74" t="inlineStr">
         <is>
@@ -7895,13 +7895,13 @@
         <v>45117</v>
       </c>
       <c r="G75">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="H75" s="2">
         <v>45301</v>
       </c>
       <c r="I75">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="J75" t="inlineStr">
         <is>
@@ -7998,13 +7998,13 @@
         <v>45160</v>
       </c>
       <c r="G76">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="H76" s="2">
         <v>45344</v>
       </c>
       <c r="I76">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="J76" t="inlineStr">
         <is>
@@ -8101,13 +8101,13 @@
         <v>45186</v>
       </c>
       <c r="G77">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="H77" s="2">
         <v>45368</v>
       </c>
       <c r="I77">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="J77" t="inlineStr">
         <is>
@@ -8204,13 +8204,13 @@
         <v>45043</v>
       </c>
       <c r="G78">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="H78" s="2">
         <v>45226</v>
       </c>
       <c r="I78">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="J78" t="inlineStr">
         <is>
@@ -8307,13 +8307,13 @@
         <v>45079</v>
       </c>
       <c r="G79">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="H79" s="2">
         <v>45262</v>
       </c>
       <c r="I79">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="J79" t="inlineStr">
         <is>
@@ -8410,7 +8410,7 @@
         <v>45254</v>
       </c>
       <c r="I80">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="J80" t="inlineStr">
         <is>
@@ -8507,13 +8507,13 @@
         <v>45104</v>
       </c>
       <c r="G81">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="H81" s="2">
         <v>45287</v>
       </c>
       <c r="I81">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="J81" t="inlineStr">
         <is>
@@ -8610,7 +8610,7 @@
         <v>45288</v>
       </c>
       <c r="I82">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="J82" t="inlineStr">
         <is>
@@ -8702,13 +8702,13 @@
         <v>45175</v>
       </c>
       <c r="G83">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="H83" s="2">
         <v>45357</v>
       </c>
       <c r="I83">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="J83" t="inlineStr">
         <is>
@@ -8805,13 +8805,13 @@
         <v>45054</v>
       </c>
       <c r="G84">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="H84" s="2">
         <v>45238</v>
       </c>
       <c r="I84">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="J84" t="inlineStr">
         <is>
@@ -8908,13 +8908,13 @@
         <v>45056</v>
       </c>
       <c r="G85">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="H85" s="2">
         <v>45240</v>
       </c>
       <c r="I85">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="J85" t="inlineStr">
         <is>
@@ -9011,13 +9011,13 @@
         <v>45085</v>
       </c>
       <c r="G86">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="H86" s="2">
         <v>45268</v>
       </c>
       <c r="I86">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="J86" t="inlineStr">
         <is>
@@ -9114,13 +9114,13 @@
         <v>45194</v>
       </c>
       <c r="G87">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="H87" s="2">
         <v>45560</v>
       </c>
       <c r="I87">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="J87" t="inlineStr">
         <is>
@@ -9207,13 +9207,13 @@
         <v>45103</v>
       </c>
       <c r="G88">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="H88" s="2">
         <v>45286</v>
       </c>
       <c r="I88">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="J88" t="inlineStr">
         <is>
@@ -9310,13 +9310,13 @@
         <v>45103</v>
       </c>
       <c r="G89">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="H89" s="2">
         <v>45286</v>
       </c>
       <c r="I89">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="J89" t="inlineStr">
         <is>
@@ -9413,13 +9413,13 @@
         <v>45192</v>
       </c>
       <c r="G90">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="H90" s="2">
         <v>45374</v>
       </c>
       <c r="I90">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="J90" t="inlineStr">
         <is>
@@ -9511,13 +9511,13 @@
         <v>45100</v>
       </c>
       <c r="G91">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="H91" s="2">
         <v>45287</v>
       </c>
       <c r="I91">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="J91" t="inlineStr">
         <is>
@@ -9614,13 +9614,13 @@
         <v>45187</v>
       </c>
       <c r="G92">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="H92" s="2">
         <v>45369</v>
       </c>
       <c r="I92">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="J92" t="inlineStr">
         <is>
@@ -9717,13 +9717,13 @@
         <v>45104</v>
       </c>
       <c r="G93">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="H93" s="2">
         <v>45287</v>
       </c>
       <c r="I93">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="J93" t="inlineStr">
         <is>
@@ -9820,13 +9820,13 @@
         <v>45104</v>
       </c>
       <c r="G94">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="H94" s="2">
         <v>45287</v>
       </c>
       <c r="I94">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="J94" t="inlineStr">
         <is>
@@ -9923,13 +9923,13 @@
         <v>45049</v>
       </c>
       <c r="G95">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="H95" s="2">
         <v>45233</v>
       </c>
       <c r="I95">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="J95" t="inlineStr">
         <is>
@@ -10026,13 +10026,13 @@
         <v>45122</v>
       </c>
       <c r="G96">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="H96" s="2">
         <v>45306</v>
       </c>
       <c r="I96">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="J96" t="inlineStr">
         <is>
@@ -10124,13 +10124,13 @@
         <v>45141</v>
       </c>
       <c r="G97">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="H97" s="2">
         <v>45325</v>
       </c>
       <c r="I97">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="J97" t="inlineStr">
         <is>
@@ -10227,13 +10227,13 @@
         <v>45194</v>
       </c>
       <c r="G98">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="H98" s="2">
         <v>45376</v>
       </c>
       <c r="I98">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="J98" t="inlineStr">
         <is>
@@ -10325,13 +10325,13 @@
         <v>45093</v>
       </c>
       <c r="G99">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="H99" s="2">
         <v>45276</v>
       </c>
       <c r="I99">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="J99" t="inlineStr">
         <is>
@@ -10428,13 +10428,13 @@
         <v>45123</v>
       </c>
       <c r="G100">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="H100" s="2">
         <v>45307</v>
       </c>
       <c r="I100">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="J100" t="inlineStr">
         <is>
@@ -10531,13 +10531,13 @@
         <v>45198</v>
       </c>
       <c r="G101">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="H101" s="2">
         <v>45380</v>
       </c>
       <c r="I101">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="J101" t="inlineStr">
         <is>
@@ -10634,13 +10634,13 @@
         <v>45093</v>
       </c>
       <c r="G102">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="H102" s="2">
         <v>45276</v>
       </c>
       <c r="I102">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="J102" t="inlineStr">
         <is>
@@ -10737,13 +10737,13 @@
         <v>45122</v>
       </c>
       <c r="G103">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="H103" s="2">
         <v>45306</v>
       </c>
       <c r="I103">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="J103" t="inlineStr">
         <is>
@@ -10840,13 +10840,13 @@
         <v>45122</v>
       </c>
       <c r="G104">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="H104" s="2">
         <v>45306</v>
       </c>
       <c r="I104">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="J104" t="inlineStr">
         <is>
@@ -10938,13 +10938,13 @@
         <v>45050</v>
       </c>
       <c r="G105">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="H105" s="2">
         <v>45234</v>
       </c>
       <c r="I105">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="J105" t="inlineStr">
         <is>
@@ -11041,13 +11041,13 @@
         <v>45085</v>
       </c>
       <c r="G106">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="H106" s="2">
         <v>45268</v>
       </c>
       <c r="I106">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="J106" t="inlineStr">
         <is>
@@ -11144,13 +11144,13 @@
         <v>45185</v>
       </c>
       <c r="G107">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="H107" s="2">
         <v>45276</v>
       </c>
       <c r="I107">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="J107" t="inlineStr">
         <is>
@@ -11242,13 +11242,13 @@
         <v>45185</v>
       </c>
       <c r="G108">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="H108" s="2">
         <v>45276</v>
       </c>
       <c r="I108">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="J108" t="inlineStr">
         <is>
@@ -11340,13 +11340,13 @@
         <v>45185</v>
       </c>
       <c r="G109">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="H109" s="2">
         <v>45276</v>
       </c>
       <c r="I109">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="J109" t="inlineStr">
         <is>
@@ -11443,13 +11443,13 @@
         <v>45148</v>
       </c>
       <c r="G110">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="H110" s="2">
         <v>45240</v>
       </c>
       <c r="I110">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="J110" t="inlineStr">
         <is>
@@ -11543,16 +11543,16 @@
         </is>
       </c>
       <c r="F111" s="2">
-        <v>45119</v>
+        <v>45211</v>
       </c>
       <c r="G111">
-        <v>92</v>
+        <v>1</v>
       </c>
       <c r="H111" s="2">
         <v>45303</v>
       </c>
       <c r="I111">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="J111" t="inlineStr">
         <is>
@@ -11649,13 +11649,13 @@
         <v>45172</v>
       </c>
       <c r="G112">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="H112" s="2">
         <v>45263</v>
       </c>
       <c r="I112">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="J112" t="inlineStr">
         <is>
@@ -11752,13 +11752,13 @@
         <v>45206</v>
       </c>
       <c r="G113">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="H113" s="2">
         <v>45389</v>
       </c>
       <c r="I113">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="J113" t="inlineStr">
         <is>
@@ -11855,13 +11855,13 @@
         <v>45203</v>
       </c>
       <c r="G114">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="H114" s="2">
         <v>45295</v>
       </c>
       <c r="I114">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="J114" t="inlineStr">
         <is>
@@ -11958,7 +11958,7 @@
         <v>45218</v>
       </c>
       <c r="I115">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="J115" t="inlineStr">
         <is>
@@ -12055,13 +12055,13 @@
         <v>45161</v>
       </c>
       <c r="G116">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="H116" s="2">
         <v>45253</v>
       </c>
       <c r="I116">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="J116" t="inlineStr">
         <is>
@@ -12158,13 +12158,13 @@
         <v>45115</v>
       </c>
       <c r="G117">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="H117" s="2">
         <v>45299</v>
       </c>
       <c r="I117">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="J117" t="inlineStr">
         <is>
@@ -12256,13 +12256,13 @@
         <v>45094</v>
       </c>
       <c r="G118">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="H118" s="2">
         <v>45277</v>
       </c>
       <c r="I118">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="J118" t="inlineStr">
         <is>
@@ -12359,13 +12359,13 @@
         <v>45104</v>
       </c>
       <c r="G119">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="H119" s="2">
         <v>45287</v>
       </c>
       <c r="I119">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="J119" t="inlineStr">
         <is>
@@ -12462,13 +12462,13 @@
         <v>45104</v>
       </c>
       <c r="G120">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="H120" s="2">
         <v>45287</v>
       </c>
       <c r="I120">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="J120" t="inlineStr">
         <is>
@@ -12565,13 +12565,13 @@
         <v>45104</v>
       </c>
       <c r="G121">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="H121" s="2">
         <v>45287</v>
       </c>
       <c r="I121">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="J121" t="inlineStr">
         <is>
@@ -12668,13 +12668,13 @@
         <v>45104</v>
       </c>
       <c r="G122">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="H122" s="2">
         <v>45287</v>
       </c>
       <c r="I122">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="J122" t="inlineStr">
         <is>
@@ -12771,13 +12771,13 @@
         <v>45199</v>
       </c>
       <c r="G123">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="H123" s="2">
         <v>45291</v>
       </c>
       <c r="I123">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="J123" t="inlineStr">
         <is>
@@ -12874,13 +12874,13 @@
         <v>45197</v>
       </c>
       <c r="G124">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="H124" s="2">
         <v>45379</v>
       </c>
       <c r="I124">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="J124" t="inlineStr">
         <is>
@@ -12977,13 +12977,13 @@
         <v>45121</v>
       </c>
       <c r="G125">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="H125" s="2">
         <v>45213</v>
       </c>
       <c r="I125">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J125" t="inlineStr">
         <is>
@@ -13080,13 +13080,13 @@
         <v>45134</v>
       </c>
       <c r="G126">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="H126" s="2">
         <v>45226</v>
       </c>
       <c r="I126">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="J126" t="inlineStr">
         <is>
@@ -13180,10 +13180,10 @@
         </is>
       </c>
       <c r="H127" s="2">
-        <v>45212</v>
+        <v>45304</v>
       </c>
       <c r="I127">
-        <v>1</v>
+        <v>92</v>
       </c>
       <c r="J127" t="inlineStr">
         <is>
@@ -13280,13 +13280,13 @@
         <v>45126</v>
       </c>
       <c r="G128">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="H128" s="2">
         <v>45218</v>
       </c>
       <c r="I128">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="J128" t="inlineStr">
         <is>
@@ -13378,13 +13378,13 @@
         <v>45158</v>
       </c>
       <c r="G129">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="H129" s="2">
         <v>45250</v>
       </c>
       <c r="I129">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="J129" t="inlineStr">
         <is>
@@ -13481,13 +13481,13 @@
         <v>45171</v>
       </c>
       <c r="G130">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="H130" s="2">
         <v>45262</v>
       </c>
       <c r="I130">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="J130" t="inlineStr">
         <is>
@@ -13584,13 +13584,13 @@
         <v>45203</v>
       </c>
       <c r="G131">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="H131" s="2">
         <v>45295</v>
       </c>
       <c r="I131">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="J131" t="inlineStr">
         <is>
@@ -13687,13 +13687,13 @@
         <v>45144</v>
       </c>
       <c r="G132">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="H132" s="2">
         <v>45236</v>
       </c>
       <c r="I132">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="J132" t="inlineStr">
         <is>
@@ -13790,13 +13790,13 @@
         <v>45156</v>
       </c>
       <c r="G133">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="H133" s="2">
         <v>45248</v>
       </c>
       <c r="I133">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="J133" t="inlineStr">
         <is>
@@ -13888,13 +13888,13 @@
         <v>45146</v>
       </c>
       <c r="G134">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="H134" s="2">
         <v>45238</v>
       </c>
       <c r="I134">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="J134" t="inlineStr">
         <is>
@@ -13991,13 +13991,13 @@
         <v>45140</v>
       </c>
       <c r="G135">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="H135" s="2">
         <v>45232</v>
       </c>
       <c r="I135">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="J135" t="inlineStr">
         <is>
@@ -14094,13 +14094,13 @@
         <v>45196</v>
       </c>
       <c r="G136">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H136" s="2">
         <v>45287</v>
       </c>
       <c r="I136">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="J136" t="inlineStr">
         <is>
@@ -14197,13 +14197,13 @@
         <v>45197</v>
       </c>
       <c r="G137">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="H137" s="2">
         <v>45288</v>
       </c>
       <c r="I137">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="J137" t="inlineStr">
         <is>
@@ -14300,13 +14300,13 @@
         <v>45179</v>
       </c>
       <c r="G138">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="H138" s="2">
         <v>45270</v>
       </c>
       <c r="I138">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="J138" t="inlineStr">
         <is>
@@ -14398,13 +14398,13 @@
         <v>45197</v>
       </c>
       <c r="G139">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="H139" s="2">
         <v>45288</v>
       </c>
       <c r="I139">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="J139" t="inlineStr">
         <is>
@@ -14501,13 +14501,13 @@
         <v>45182</v>
       </c>
       <c r="G140">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="H140" s="2">
         <v>45273</v>
       </c>
       <c r="I140">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="J140" t="inlineStr">
         <is>
@@ -14604,13 +14604,13 @@
         <v>45208</v>
       </c>
       <c r="G141">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="H141" s="2">
         <v>45300</v>
       </c>
       <c r="I141">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="J141" t="inlineStr">
         <is>
@@ -14702,13 +14702,13 @@
         <v>45150</v>
       </c>
       <c r="G142">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="H142" s="2">
         <v>45242</v>
       </c>
       <c r="I142">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="J142" t="inlineStr">
         <is>
@@ -14805,7 +14805,7 @@
         <v>45238</v>
       </c>
       <c r="I143">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="J143" t="inlineStr">
         <is>
@@ -14902,13 +14902,13 @@
         <v>45171</v>
       </c>
       <c r="G144">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="H144" s="2">
         <v>45262</v>
       </c>
       <c r="I144">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="J144" t="inlineStr">
         <is>
@@ -15005,13 +15005,13 @@
         <v>45194</v>
       </c>
       <c r="G145">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="H145" s="2">
         <v>45285</v>
       </c>
       <c r="I145">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="J145" t="inlineStr">
         <is>
@@ -15095,10 +15095,10 @@
         </is>
       </c>
       <c r="F146" s="2">
-        <v>45119</v>
+        <v>45211</v>
       </c>
       <c r="G146">
-        <v>92</v>
+        <v>1</v>
       </c>
       <c r="J146" t="inlineStr">
         <is>
@@ -15195,13 +15195,13 @@
         <v>45165</v>
       </c>
       <c r="G147">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="H147" s="2">
         <v>45257</v>
       </c>
       <c r="I147">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="J147" t="inlineStr">
         <is>
@@ -15298,13 +15298,13 @@
         <v>45166</v>
       </c>
       <c r="G148">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="H148" s="2">
         <v>45258</v>
       </c>
       <c r="I148">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="J148" t="inlineStr">
         <is>
@@ -15401,13 +15401,13 @@
         <v>45185</v>
       </c>
       <c r="G149">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="H149" s="2">
         <v>45276</v>
       </c>
       <c r="I149">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="J149" t="inlineStr">
         <is>
@@ -15504,13 +15504,13 @@
         <v>45035</v>
       </c>
       <c r="G150">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="H150" s="2">
         <v>45218</v>
       </c>
       <c r="I150">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="J150" t="inlineStr">
         <is>
@@ -15607,13 +15607,13 @@
         <v>45174</v>
       </c>
       <c r="G151">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="H151" s="2">
         <v>45356</v>
       </c>
       <c r="I151">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="J151" t="inlineStr">
         <is>
@@ -15710,13 +15710,13 @@
         <v>45089</v>
       </c>
       <c r="G152">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="H152" s="2">
         <v>45272</v>
       </c>
       <c r="I152">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="J152" t="inlineStr">
         <is>
@@ -15813,13 +15813,13 @@
         <v>45124</v>
       </c>
       <c r="G153">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="H153" s="2">
         <v>45308</v>
       </c>
       <c r="I153">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="J153" t="inlineStr">
         <is>
@@ -15916,13 +15916,13 @@
         <v>45124</v>
       </c>
       <c r="G154">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="H154" s="2">
         <v>45308</v>
       </c>
       <c r="I154">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="J154" t="inlineStr">
         <is>
@@ -16019,13 +16019,13 @@
         <v>45209</v>
       </c>
       <c r="G155">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H155" s="2">
         <v>45392</v>
       </c>
       <c r="I155">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="J155" t="inlineStr">
         <is>
@@ -16122,13 +16122,13 @@
         <v>45209</v>
       </c>
       <c r="G156">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H156" s="2">
         <v>45392</v>
       </c>
       <c r="I156">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="J156" t="inlineStr">
         <is>
@@ -16225,13 +16225,13 @@
         <v>45209</v>
       </c>
       <c r="G157">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H157" s="2">
         <v>45392</v>
       </c>
       <c r="I157">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="J157" t="inlineStr">
         <is>
@@ -16328,13 +16328,13 @@
         <v>45209</v>
       </c>
       <c r="G158">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H158" s="2">
         <v>45392</v>
       </c>
       <c r="I158">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="J158" t="inlineStr">
         <is>
@@ -16431,13 +16431,13 @@
         <v>45156</v>
       </c>
       <c r="G159">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="H159" s="2">
         <v>45247</v>
       </c>
       <c r="I159">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="J159" t="inlineStr">
         <is>
@@ -16534,13 +16534,13 @@
         <v>45153</v>
       </c>
       <c r="G160">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="H160" s="2">
         <v>45245</v>
       </c>
       <c r="I160">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="J160" t="inlineStr">
         <is>
@@ -16637,13 +16637,13 @@
         <v>45135</v>
       </c>
       <c r="G161">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="H161" s="2">
         <v>45319</v>
       </c>
       <c r="I161">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="J161" t="inlineStr">
         <is>
@@ -16740,13 +16740,13 @@
         <v>45091</v>
       </c>
       <c r="G162">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="H162" s="2">
         <v>45274</v>
       </c>
       <c r="I162">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="J162" t="inlineStr">
         <is>
@@ -16838,13 +16838,13 @@
         <v>45091</v>
       </c>
       <c r="G163">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="H163" s="2">
         <v>45274</v>
       </c>
       <c r="I163">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="J163" t="inlineStr">
         <is>
@@ -16936,13 +16936,13 @@
         <v>45138</v>
       </c>
       <c r="G164">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="H164" s="2">
         <v>45322</v>
       </c>
       <c r="I164">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="J164" t="inlineStr">
         <is>
@@ -17039,13 +17039,13 @@
         <v>45138</v>
       </c>
       <c r="G165">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="H165" s="2">
         <v>45322</v>
       </c>
       <c r="I165">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="J165" t="inlineStr">
         <is>
@@ -17142,13 +17142,13 @@
         <v>45085</v>
       </c>
       <c r="G166">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="H166" s="2">
         <v>45268</v>
       </c>
       <c r="I166">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="J166" t="inlineStr">
         <is>
@@ -17245,13 +17245,13 @@
         <v>45085</v>
       </c>
       <c r="G167">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="H167" s="2">
         <v>45268</v>
       </c>
       <c r="I167">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="J167" t="inlineStr">
         <is>
@@ -17348,7 +17348,7 @@
         <v>45326</v>
       </c>
       <c r="I168">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="J168" t="inlineStr">
         <is>
@@ -17445,13 +17445,13 @@
         <v>45173</v>
       </c>
       <c r="G169">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="H169" s="2">
         <v>45355</v>
       </c>
       <c r="I169">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="J169" t="inlineStr">
         <is>
@@ -17548,13 +17548,13 @@
         <v>45056</v>
       </c>
       <c r="G170">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="H170" s="2">
         <v>45240</v>
       </c>
       <c r="I170">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="J170" t="inlineStr">
         <is>
@@ -17651,7 +17651,7 @@
         <v>45238</v>
       </c>
       <c r="I171">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="J171" t="inlineStr">
         <is>
@@ -17748,13 +17748,13 @@
         <v>45141</v>
       </c>
       <c r="G172">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="H172" s="2">
         <v>45325</v>
       </c>
       <c r="I172">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="J172" t="inlineStr">
         <is>
@@ -17851,13 +17851,13 @@
         <v>45037</v>
       </c>
       <c r="G173">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="H173" s="2">
         <v>45220</v>
       </c>
       <c r="I173">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="J173" t="inlineStr">
         <is>
@@ -17954,13 +17954,13 @@
         <v>45171</v>
       </c>
       <c r="G174">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="H174" s="2">
         <v>45262</v>
       </c>
       <c r="I174">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="J174" t="inlineStr">
         <is>
@@ -18057,13 +18057,13 @@
         <v>45197</v>
       </c>
       <c r="G175">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="H175" s="2">
         <v>45288</v>
       </c>
       <c r="I175">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="J175" t="inlineStr">
         <is>
@@ -18160,13 +18160,13 @@
         <v>45162</v>
       </c>
       <c r="G176">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="H176" s="2">
         <v>45254</v>
       </c>
       <c r="I176">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="J176" t="inlineStr">
         <is>
@@ -18263,13 +18263,13 @@
         <v>45061</v>
       </c>
       <c r="G177">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="H177" s="2">
         <v>45245</v>
       </c>
       <c r="I177">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="J177" t="inlineStr">
         <is>
@@ -18366,13 +18366,13 @@
         <v>45120</v>
       </c>
       <c r="G178">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="H178" s="2">
-        <v>45212</v>
+        <v>45304</v>
       </c>
       <c r="I178">
-        <v>1</v>
+        <v>92</v>
       </c>
       <c r="J178" t="inlineStr">
         <is>
@@ -18469,13 +18469,13 @@
         <v>45191</v>
       </c>
       <c r="G179">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="H179" s="2">
         <v>45282</v>
       </c>
       <c r="I179">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="J179" t="inlineStr">
         <is>
@@ -18572,13 +18572,13 @@
         <v>45088</v>
       </c>
       <c r="G180">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="H180" s="2">
         <v>45271</v>
       </c>
       <c r="I180">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="J180" t="inlineStr">
         <is>
@@ -18675,13 +18675,13 @@
         <v>45192</v>
       </c>
       <c r="G181">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="H181" s="2">
         <v>45283</v>
       </c>
       <c r="I181">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="J181" t="inlineStr">
         <is>
@@ -18768,13 +18768,13 @@
         <v>45131</v>
       </c>
       <c r="G182">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="H182" s="2">
         <v>45223</v>
       </c>
       <c r="I182">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="J182" t="inlineStr">
         <is>
@@ -18866,13 +18866,13 @@
         <v>45136</v>
       </c>
       <c r="G183">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="H183" s="2">
         <v>45228</v>
       </c>
       <c r="I183">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="J183" t="inlineStr">
         <is>
@@ -18964,13 +18964,13 @@
         <v>45150</v>
       </c>
       <c r="G184">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="H184" s="2">
         <v>45242</v>
       </c>
       <c r="I184">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="J184" t="inlineStr">
         <is>
@@ -19062,7 +19062,7 @@
         <v>45210</v>
       </c>
       <c r="G185">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J185" t="inlineStr">
         <is>
@@ -19154,13 +19154,13 @@
         <v>45129</v>
       </c>
       <c r="G186">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="H186" s="2">
         <v>45221</v>
       </c>
       <c r="I186">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="J186" t="inlineStr">
         <is>
@@ -19252,13 +19252,13 @@
         <v>45189</v>
       </c>
       <c r="G187">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="H187" s="2">
         <v>45280</v>
       </c>
       <c r="I187">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="J187" t="inlineStr">
         <is>
@@ -19345,13 +19345,13 @@
         <v>45193</v>
       </c>
       <c r="G188">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="H188" s="2">
         <v>45284</v>
       </c>
       <c r="I188">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="J188" t="inlineStr">
         <is>
@@ -19438,13 +19438,13 @@
         <v>45165</v>
       </c>
       <c r="G189">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="H189" s="2">
         <v>45257</v>
       </c>
       <c r="I189">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="J189" t="inlineStr">
         <is>
@@ -19536,13 +19536,13 @@
         <v>45202</v>
       </c>
       <c r="G190">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="H190" s="2">
         <v>45385</v>
       </c>
       <c r="I190">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="J190" t="inlineStr">
         <is>
@@ -19639,13 +19639,13 @@
         <v>45081</v>
       </c>
       <c r="G191">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="H191" s="2">
         <v>45264</v>
       </c>
       <c r="I191">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="J191" t="inlineStr">
         <is>
@@ -19742,13 +19742,13 @@
         <v>45081</v>
       </c>
       <c r="G192">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="H192" s="2">
         <v>45264</v>
       </c>
       <c r="I192">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="J192" t="inlineStr">
         <is>
@@ -19845,7 +19845,7 @@
         <v>45319</v>
       </c>
       <c r="I193">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="J193" t="inlineStr">
         <is>
@@ -19942,7 +19942,7 @@
         <v>45319</v>
       </c>
       <c r="I194">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="J194" t="inlineStr">
         <is>
@@ -20034,13 +20034,13 @@
         <v>45046</v>
       </c>
       <c r="G195">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="H195" s="2">
         <v>45230</v>
       </c>
       <c r="I195">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="J195" t="inlineStr">
         <is>
@@ -20137,13 +20137,13 @@
         <v>45046</v>
       </c>
       <c r="G196">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="H196" s="2">
         <v>45230</v>
       </c>
       <c r="I196">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="J196" t="inlineStr">
         <is>
@@ -20240,13 +20240,13 @@
         <v>45031</v>
       </c>
       <c r="G197">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="H197" s="2">
         <v>45214</v>
       </c>
       <c r="I197">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="J197" t="inlineStr">
         <is>
@@ -20343,13 +20343,13 @@
         <v>45031</v>
       </c>
       <c r="G198">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="H198" s="2">
         <v>45214</v>
       </c>
       <c r="I198">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="J198" t="inlineStr">
         <is>
@@ -20446,13 +20446,13 @@
         <v>45031</v>
       </c>
       <c r="G199">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="H199" s="2">
         <v>45214</v>
       </c>
       <c r="I199">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="J199" t="inlineStr">
         <is>
@@ -20549,13 +20549,13 @@
         <v>45031</v>
       </c>
       <c r="G200">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="H200" s="2">
         <v>45214</v>
       </c>
       <c r="I200">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="J200" t="inlineStr">
         <is>
@@ -20652,13 +20652,13 @@
         <v>45067</v>
       </c>
       <c r="G201">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="H201" s="2">
         <v>45251</v>
       </c>
       <c r="I201">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="J201" t="inlineStr">
         <is>
@@ -20755,13 +20755,13 @@
         <v>45067</v>
       </c>
       <c r="G202">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="H202" s="2">
         <v>45251</v>
       </c>
       <c r="I202">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="J202" t="inlineStr">
         <is>
@@ -20858,13 +20858,13 @@
         <v>45067</v>
       </c>
       <c r="G203">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="H203" s="2">
         <v>45251</v>
       </c>
       <c r="I203">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="J203" t="inlineStr">
         <is>
@@ -20961,13 +20961,13 @@
         <v>45067</v>
       </c>
       <c r="G204">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="H204" s="2">
         <v>45251</v>
       </c>
       <c r="I204">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="J204" t="inlineStr">
         <is>
@@ -21064,13 +21064,13 @@
         <v>45178</v>
       </c>
       <c r="G205">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="H205" s="2">
         <v>45269</v>
       </c>
       <c r="I205">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="J205" t="inlineStr">
         <is>
@@ -21167,7 +21167,7 @@
         <v>45252</v>
       </c>
       <c r="I206">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="J206" t="inlineStr">
         <is>
@@ -21264,13 +21264,13 @@
         <v>45087</v>
       </c>
       <c r="G207">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="H207" s="2">
         <v>45270</v>
       </c>
       <c r="I207">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="J207" t="inlineStr">
         <is>
@@ -21367,13 +21367,13 @@
         <v>45099</v>
       </c>
       <c r="G208">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="H208" s="2">
         <v>45282</v>
       </c>
       <c r="I208">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="J208" t="inlineStr">
         <is>
@@ -21470,13 +21470,13 @@
         <v>45175</v>
       </c>
       <c r="G209">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="H209" s="2">
         <v>45356</v>
       </c>
       <c r="I209">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="J209" t="inlineStr">
         <is>
@@ -21573,13 +21573,13 @@
         <v>45175</v>
       </c>
       <c r="G210">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="H210" s="2">
         <v>45356</v>
       </c>
       <c r="I210">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="J210" t="inlineStr">
         <is>
@@ -21676,13 +21676,13 @@
         <v>45166</v>
       </c>
       <c r="G211">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="H211" s="2">
         <v>45350</v>
       </c>
       <c r="I211">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="J211" t="inlineStr">
         <is>
@@ -21779,13 +21779,13 @@
         <v>45166</v>
       </c>
       <c r="G212">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="H212" s="2">
         <v>45350</v>
       </c>
       <c r="I212">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="J212" t="inlineStr">
         <is>
@@ -21882,13 +21882,13 @@
         <v>45090</v>
       </c>
       <c r="G213">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="H213" s="2">
         <v>45273</v>
       </c>
       <c r="I213">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="J213" t="inlineStr">
         <is>
@@ -21985,13 +21985,13 @@
         <v>45106</v>
       </c>
       <c r="G214">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="H214" s="2">
         <v>45289</v>
       </c>
       <c r="I214">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="J214" t="inlineStr">
         <is>
@@ -22088,13 +22088,13 @@
         <v>45134</v>
       </c>
       <c r="G215">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="H215" s="2">
         <v>45226</v>
       </c>
       <c r="I215">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="J215" t="inlineStr">
         <is>
@@ -22191,13 +22191,13 @@
         <v>45132</v>
       </c>
       <c r="G216">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="H216" s="2">
         <v>45224</v>
       </c>
       <c r="I216">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="J216" t="inlineStr">
         <is>
@@ -22294,13 +22294,13 @@
         <v>45150</v>
       </c>
       <c r="G217">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="H217" s="2">
         <v>45242</v>
       </c>
       <c r="I217">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="J217" t="inlineStr">
         <is>
@@ -22397,13 +22397,13 @@
         <v>45187</v>
       </c>
       <c r="G218">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="H218" s="2">
         <v>45278</v>
       </c>
       <c r="I218">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="J218" t="inlineStr">
         <is>
@@ -22495,13 +22495,13 @@
         <v>45182</v>
       </c>
       <c r="G219">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="H219" s="2">
         <v>45273</v>
       </c>
       <c r="I219">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="J219" t="inlineStr">
         <is>
@@ -22598,13 +22598,13 @@
         <v>45196</v>
       </c>
       <c r="G220">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H220" s="2">
         <v>45287</v>
       </c>
       <c r="I220">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="J220" t="inlineStr">
         <is>
@@ -22701,13 +22701,13 @@
         <v>45200</v>
       </c>
       <c r="G221">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="H221" s="2">
         <v>45292</v>
       </c>
       <c r="I221">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="J221" t="inlineStr">
         <is>
@@ -22804,13 +22804,13 @@
         <v>45135</v>
       </c>
       <c r="G222">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="H222" s="2">
         <v>45227</v>
       </c>
       <c r="I222">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="J222" t="inlineStr">
         <is>
@@ -22907,13 +22907,13 @@
         <v>45148</v>
       </c>
       <c r="G223">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="H223" s="2">
         <v>45240</v>
       </c>
       <c r="I223">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="J223" t="inlineStr">
         <is>
@@ -23005,13 +23005,13 @@
         <v>45192</v>
       </c>
       <c r="G224">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="H224" s="2">
         <v>45283</v>
       </c>
       <c r="I224">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="J224" t="inlineStr">
         <is>
@@ -23103,13 +23103,13 @@
         <v>45136</v>
       </c>
       <c r="G225">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="H225" s="2">
         <v>45320</v>
       </c>
       <c r="I225">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="J225" t="inlineStr">
         <is>
@@ -23206,13 +23206,13 @@
         <v>45136</v>
       </c>
       <c r="G226">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="H226" s="2">
         <v>45320</v>
       </c>
       <c r="I226">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="J226" t="inlineStr">
         <is>
@@ -23309,13 +23309,13 @@
         <v>45094</v>
       </c>
       <c r="G227">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="H227" s="2">
         <v>45277</v>
       </c>
       <c r="I227">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="J227" t="inlineStr">
         <is>
@@ -23412,13 +23412,13 @@
         <v>45081</v>
       </c>
       <c r="G228">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="H228" s="2">
         <v>45264</v>
       </c>
       <c r="I228">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="J228" t="inlineStr">
         <is>
@@ -23515,13 +23515,13 @@
         <v>45099</v>
       </c>
       <c r="G229">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="H229" s="2">
         <v>45282</v>
       </c>
       <c r="I229">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="J229" t="inlineStr">
         <is>
@@ -23618,13 +23618,13 @@
         <v>45201</v>
       </c>
       <c r="G230">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="H230" s="2">
         <v>45384</v>
       </c>
       <c r="I230">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="J230" t="inlineStr">
         <is>
@@ -23721,13 +23721,13 @@
         <v>45031</v>
       </c>
       <c r="G231">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="H231" s="2">
         <v>45214</v>
       </c>
       <c r="I231">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="J231" t="inlineStr">
         <is>
@@ -23824,7 +23824,7 @@
         <v>45294</v>
       </c>
       <c r="I232">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="J232" t="inlineStr">
         <is>
@@ -23921,13 +23921,13 @@
         <v>45079</v>
       </c>
       <c r="G233">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="H233" s="2">
         <v>45262</v>
       </c>
       <c r="I233">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="J233" t="inlineStr">
         <is>
@@ -24024,13 +24024,13 @@
         <v>45199</v>
       </c>
       <c r="G234">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="H234" s="2">
         <v>45382</v>
       </c>
       <c r="I234">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="J234" t="inlineStr">
         <is>
@@ -24127,13 +24127,13 @@
         <v>45204</v>
       </c>
       <c r="G235">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="H235" s="2">
         <v>45387</v>
       </c>
       <c r="I235">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="J235" t="inlineStr">
         <is>
@@ -24230,13 +24230,13 @@
         <v>45204</v>
       </c>
       <c r="G236">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="H236" s="2">
         <v>45387</v>
       </c>
       <c r="I236">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="J236" t="inlineStr">
         <is>
@@ -24333,13 +24333,13 @@
         <v>45080</v>
       </c>
       <c r="G237">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="H237" s="2">
         <v>45263</v>
       </c>
       <c r="I237">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="J237" t="inlineStr">
         <is>
@@ -24436,13 +24436,13 @@
         <v>45046</v>
       </c>
       <c r="G238">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="H238" s="2">
         <v>45229</v>
       </c>
       <c r="I238">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="J238" t="inlineStr">
         <is>
@@ -24539,13 +24539,13 @@
         <v>45204</v>
       </c>
       <c r="G239">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="H239" s="2">
         <v>45296</v>
       </c>
       <c r="I239">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="J239" t="inlineStr">
         <is>
@@ -24642,13 +24642,13 @@
         <v>45204</v>
       </c>
       <c r="G240">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="H240" s="2">
         <v>45296</v>
       </c>
       <c r="I240">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="J240" t="inlineStr">
         <is>
@@ -24745,13 +24745,13 @@
         <v>45199</v>
       </c>
       <c r="G241">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="H241" s="2">
         <v>45382</v>
       </c>
       <c r="I241">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="J241" t="inlineStr">
         <is>
@@ -24848,13 +24848,13 @@
         <v>45070</v>
       </c>
       <c r="G242">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="H242" s="2">
         <v>45254</v>
       </c>
       <c r="I242">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="J242" t="inlineStr">
         <is>
@@ -24951,13 +24951,13 @@
         <v>45168</v>
       </c>
       <c r="G243">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="H243" s="2">
         <v>45260</v>
       </c>
       <c r="I243">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="J243" t="inlineStr">
         <is>
@@ -25054,13 +25054,13 @@
         <v>45210</v>
       </c>
       <c r="G244">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H244" s="2">
         <v>45393</v>
       </c>
       <c r="I244">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="J244" t="inlineStr">
         <is>
@@ -25157,13 +25157,13 @@
         <v>45077</v>
       </c>
       <c r="G245">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="H245" s="2">
         <v>45260</v>
       </c>
       <c r="I245">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="J245" t="inlineStr">
         <is>
@@ -25260,13 +25260,13 @@
         <v>45100</v>
       </c>
       <c r="G246">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="H246" s="2">
         <v>45283</v>
       </c>
       <c r="I246">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="J246" t="inlineStr">
         <is>
@@ -25363,7 +25363,7 @@
         <v>45281</v>
       </c>
       <c r="I247">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="J247" t="inlineStr">
         <is>
@@ -25460,13 +25460,13 @@
         <v>45044</v>
       </c>
       <c r="G248">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="H248" s="2">
         <v>45227</v>
       </c>
       <c r="I248">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="J248" t="inlineStr">
         <is>
@@ -25563,13 +25563,13 @@
         <v>45101</v>
       </c>
       <c r="G249">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="H249" s="2">
         <v>45283</v>
       </c>
       <c r="I249">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="J249" t="inlineStr">
         <is>
@@ -25666,13 +25666,13 @@
         <v>45134</v>
       </c>
       <c r="G250">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="H250" s="2">
         <v>45226</v>
       </c>
       <c r="I250">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="J250" t="inlineStr">
         <is>
@@ -25769,13 +25769,13 @@
         <v>45158</v>
       </c>
       <c r="G251">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="H251" s="2">
         <v>45250</v>
       </c>
       <c r="I251">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="J251" t="inlineStr">
         <is>
@@ -25872,13 +25872,13 @@
         <v>45200</v>
       </c>
       <c r="G252">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="H252" s="2">
         <v>45292</v>
       </c>
       <c r="I252">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="J252" t="inlineStr">
         <is>
@@ -25975,7 +25975,7 @@
         <v>45317</v>
       </c>
       <c r="I253">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="J253" t="inlineStr">
         <is>
@@ -26072,13 +26072,13 @@
         <v>45039</v>
       </c>
       <c r="G254">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="H254" s="2">
         <v>45222</v>
       </c>
       <c r="I254">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="J254" t="inlineStr">
         <is>
@@ -26170,13 +26170,13 @@
         <v>45129</v>
       </c>
       <c r="G255">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="H255" s="2">
         <v>45221</v>
       </c>
       <c r="I255">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="J255" t="inlineStr">
         <is>
@@ -26273,13 +26273,13 @@
         <v>45157</v>
       </c>
       <c r="G256">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="H256" s="2">
         <v>45341</v>
       </c>
       <c r="I256">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="J256" t="inlineStr">
         <is>
@@ -26376,13 +26376,13 @@
         <v>45063</v>
       </c>
       <c r="G257">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="H257" s="2">
         <v>45247</v>
       </c>
       <c r="I257">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="J257" t="inlineStr">
         <is>
@@ -26479,7 +26479,7 @@
         <v>45254</v>
       </c>
       <c r="I258">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="J258" t="inlineStr">
         <is>
@@ -26576,7 +26576,7 @@
         <v>45486</v>
       </c>
       <c r="I259">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="J259" t="inlineStr">
         <is>
@@ -26668,13 +26668,13 @@
         <v>45073</v>
       </c>
       <c r="G260">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="H260" s="2">
         <v>45439</v>
       </c>
       <c r="I260">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="J260" t="inlineStr">
         <is>
@@ -26766,7 +26766,7 @@
         <v>45323</v>
       </c>
       <c r="I261">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="J261" t="inlineStr">
         <is>
@@ -26858,7 +26858,7 @@
         <v>45303</v>
       </c>
       <c r="I262">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="J262" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
Bond dates update Sat Oct 14 23:16:07 UTC 2023
</commit_message>
<xml_diff>
--- a/Data/obligacje_screener.xlsx
+++ b/Data/obligacje_screener.xlsx
@@ -512,7 +512,7 @@
         <v>45340</v>
       </c>
       <c r="I2">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="J2" t="inlineStr">
         <is>
@@ -600,13 +600,13 @@
         <v>45121</v>
       </c>
       <c r="G3">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="H3" s="2">
         <v>45305</v>
       </c>
       <c r="I3">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="J3" t="inlineStr">
         <is>
@@ -703,13 +703,13 @@
         <v>45039</v>
       </c>
       <c r="G4">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="H4" s="2">
         <v>45222</v>
       </c>
       <c r="I4">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="J4" t="inlineStr">
         <is>
@@ -806,13 +806,13 @@
         <v>45039</v>
       </c>
       <c r="G5">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="H5" s="2">
         <v>45222</v>
       </c>
       <c r="I5">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="J5" t="inlineStr">
         <is>
@@ -909,13 +909,13 @@
         <v>45129</v>
       </c>
       <c r="G6">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="H6" s="2">
         <v>45221</v>
       </c>
       <c r="I6">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="J6" t="inlineStr">
         <is>
@@ -1012,13 +1012,13 @@
         <v>45162</v>
       </c>
       <c r="G7">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="H7" s="2">
         <v>45254</v>
       </c>
       <c r="I7">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="J7" t="inlineStr">
         <is>
@@ -1110,13 +1110,13 @@
         <v>45156</v>
       </c>
       <c r="G8">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="H8" s="2">
         <v>45248</v>
       </c>
       <c r="I8">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="J8" t="inlineStr">
         <is>
@@ -1213,13 +1213,13 @@
         <v>45141</v>
       </c>
       <c r="G9">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="H9" s="2">
         <v>45233</v>
       </c>
       <c r="I9">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="J9" t="inlineStr">
         <is>
@@ -1316,13 +1316,13 @@
         <v>45062</v>
       </c>
       <c r="G10">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="H10" s="2">
         <v>45246</v>
       </c>
       <c r="I10">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="J10" t="inlineStr">
         <is>
@@ -1419,7 +1419,7 @@
         <v>45286</v>
       </c>
       <c r="I11">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="J11" t="inlineStr">
         <is>
@@ -1516,13 +1516,13 @@
         <v>45195</v>
       </c>
       <c r="G12">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="H12" s="2">
         <v>45377</v>
       </c>
       <c r="I12">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="J12" t="inlineStr">
         <is>
@@ -1614,13 +1614,13 @@
         <v>45036</v>
       </c>
       <c r="G13">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="H13" s="2">
         <v>45219</v>
       </c>
       <c r="I13">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="J13" t="inlineStr">
         <is>
@@ -1717,13 +1717,13 @@
         <v>45036</v>
       </c>
       <c r="G14">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="H14" s="2">
         <v>45219</v>
       </c>
       <c r="I14">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="J14" t="inlineStr">
         <is>
@@ -1820,13 +1820,13 @@
         <v>45106</v>
       </c>
       <c r="G15">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="H15" s="2">
         <v>45289</v>
       </c>
       <c r="I15">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="J15" t="inlineStr">
         <is>
@@ -1923,13 +1923,13 @@
         <v>45186</v>
       </c>
       <c r="G16">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="H16" s="2">
         <v>45278</v>
       </c>
       <c r="I16">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="J16" t="inlineStr">
         <is>
@@ -2026,13 +2026,13 @@
         <v>45186</v>
       </c>
       <c r="G17">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="H17" s="2">
         <v>45277</v>
       </c>
       <c r="I17">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="J17" t="inlineStr">
         <is>
@@ -2129,13 +2129,13 @@
         <v>45132</v>
       </c>
       <c r="G18">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="H18" s="2">
         <v>45224</v>
       </c>
       <c r="I18">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="J18" t="inlineStr">
         <is>
@@ -2232,13 +2232,13 @@
         <v>45137</v>
       </c>
       <c r="G19">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="H19" s="2">
         <v>45229</v>
       </c>
       <c r="I19">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="J19" t="inlineStr">
         <is>
@@ -2330,13 +2330,13 @@
         <v>45183</v>
       </c>
       <c r="G20">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="H20" s="2">
         <v>45274</v>
       </c>
       <c r="I20">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="J20" t="inlineStr">
         <is>
@@ -2433,13 +2433,13 @@
         <v>45187</v>
       </c>
       <c r="G21">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="H21" s="2">
         <v>45278</v>
       </c>
       <c r="I21">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="J21" t="inlineStr">
         <is>
@@ -2536,13 +2536,13 @@
         <v>45187</v>
       </c>
       <c r="G22">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="H22" s="2">
         <v>45278</v>
       </c>
       <c r="I22">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="J22" t="inlineStr">
         <is>
@@ -2639,7 +2639,7 @@
         <v>45245</v>
       </c>
       <c r="I23">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="J23" t="inlineStr">
         <is>
@@ -2736,7 +2736,7 @@
         <v>45245</v>
       </c>
       <c r="I24">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="J24" t="inlineStr">
         <is>
@@ -2833,7 +2833,7 @@
         <v>45204</v>
       </c>
       <c r="G25">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="J25" t="inlineStr">
         <is>
@@ -2930,13 +2930,13 @@
         <v>45160</v>
       </c>
       <c r="G26">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="H26" s="2">
         <v>45344</v>
       </c>
       <c r="I26">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="J26" t="inlineStr">
         <is>
@@ -3033,13 +3033,13 @@
         <v>45118</v>
       </c>
       <c r="G27">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="H27" s="2">
         <v>45302</v>
       </c>
       <c r="I27">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="J27" t="inlineStr">
         <is>
@@ -3136,13 +3136,13 @@
         <v>45085</v>
       </c>
       <c r="G28">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="H28" s="2">
         <v>45268</v>
       </c>
       <c r="I28">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="J28" t="inlineStr">
         <is>
@@ -3239,13 +3239,13 @@
         <v>45183</v>
       </c>
       <c r="G29">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="H29" s="2">
         <v>45274</v>
       </c>
       <c r="I29">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="J29" t="inlineStr">
         <is>
@@ -3342,7 +3342,7 @@
         <v>45224</v>
       </c>
       <c r="I30">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="J30" t="inlineStr">
         <is>
@@ -3439,13 +3439,13 @@
         <v>45153</v>
       </c>
       <c r="G31">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="H31" s="2">
         <v>45245</v>
       </c>
       <c r="I31">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="J31" t="inlineStr">
         <is>
@@ -3542,13 +3542,13 @@
         <v>45155</v>
       </c>
       <c r="G32">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="H32" s="2">
         <v>45247</v>
       </c>
       <c r="I32">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="J32" t="inlineStr">
         <is>
@@ -3645,7 +3645,7 @@
         <v>45255</v>
       </c>
       <c r="I33">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="J33" t="inlineStr">
         <is>
@@ -3742,13 +3742,13 @@
         <v>45176</v>
       </c>
       <c r="G34">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="H34" s="2">
         <v>45267</v>
       </c>
       <c r="I34">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="J34" t="inlineStr">
         <is>
@@ -3845,13 +3845,13 @@
         <v>45130</v>
       </c>
       <c r="G35">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="H35" s="2">
         <v>45222</v>
       </c>
       <c r="I35">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="J35" t="inlineStr">
         <is>
@@ -3943,13 +3943,13 @@
         <v>45207</v>
       </c>
       <c r="G36">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="H36" s="2">
         <v>45299</v>
       </c>
       <c r="I36">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="J36" t="inlineStr">
         <is>
@@ -4046,13 +4046,13 @@
         <v>45189</v>
       </c>
       <c r="G37">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="H37" s="2">
         <v>45280</v>
       </c>
       <c r="I37">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="J37" t="inlineStr">
         <is>
@@ -4144,13 +4144,13 @@
         <v>45107</v>
       </c>
       <c r="G38">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="H38" s="2">
         <v>45290</v>
       </c>
       <c r="I38">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="J38" t="inlineStr">
         <is>
@@ -4247,13 +4247,13 @@
         <v>45063</v>
       </c>
       <c r="G39">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="H39" s="2">
         <v>45247</v>
       </c>
       <c r="I39">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="J39" t="inlineStr">
         <is>
@@ -4350,13 +4350,13 @@
         <v>45177</v>
       </c>
       <c r="G40">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="H40" s="2">
         <v>45359</v>
       </c>
       <c r="I40">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="J40" t="inlineStr">
         <is>
@@ -4453,13 +4453,13 @@
         <v>45107</v>
       </c>
       <c r="G41">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="H41" s="2">
         <v>45290</v>
       </c>
       <c r="I41">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="J41" t="inlineStr">
         <is>
@@ -4556,7 +4556,7 @@
         <v>45265</v>
       </c>
       <c r="I42">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="J42" t="inlineStr">
         <is>
@@ -4653,13 +4653,13 @@
         <v>45098</v>
       </c>
       <c r="G43">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="H43" s="2">
         <v>45281</v>
       </c>
       <c r="I43">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="J43" t="inlineStr">
         <is>
@@ -4756,13 +4756,13 @@
         <v>45099</v>
       </c>
       <c r="G44">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="H44" s="2">
         <v>45282</v>
       </c>
       <c r="I44">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="J44" t="inlineStr">
         <is>
@@ -4859,13 +4859,13 @@
         <v>45106</v>
       </c>
       <c r="G45">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="H45" s="2">
         <v>45289</v>
       </c>
       <c r="I45">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="J45" t="inlineStr">
         <is>
@@ -4962,13 +4962,13 @@
         <v>45106</v>
       </c>
       <c r="G46">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="H46" s="2">
         <v>45289</v>
       </c>
       <c r="I46">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="J46" t="inlineStr">
         <is>
@@ -5065,13 +5065,13 @@
         <v>45120</v>
       </c>
       <c r="G47">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="H47" s="2">
         <v>45304</v>
       </c>
       <c r="I47">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="J47" t="inlineStr">
         <is>
@@ -5168,13 +5168,13 @@
         <v>45118</v>
       </c>
       <c r="G48">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="H48" s="2">
         <v>45302</v>
       </c>
       <c r="I48">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="J48" t="inlineStr">
         <is>
@@ -5271,13 +5271,13 @@
         <v>45152</v>
       </c>
       <c r="G49">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="H49" s="2">
         <v>45336</v>
       </c>
       <c r="I49">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="J49" t="inlineStr">
         <is>
@@ -5374,13 +5374,13 @@
         <v>45042</v>
       </c>
       <c r="G50">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="H50" s="2">
         <v>45225</v>
       </c>
       <c r="I50">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="J50" t="inlineStr">
         <is>
@@ -5477,13 +5477,13 @@
         <v>45122</v>
       </c>
       <c r="G51">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="H51" s="2">
         <v>45306</v>
       </c>
       <c r="I51">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="J51" t="inlineStr">
         <is>
@@ -5580,13 +5580,13 @@
         <v>45139</v>
       </c>
       <c r="G52">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="H52" s="2">
         <v>45323</v>
       </c>
       <c r="I52">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="J52" t="inlineStr">
         <is>
@@ -5683,13 +5683,13 @@
         <v>45099</v>
       </c>
       <c r="G53">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="H53" s="2">
         <v>45282</v>
       </c>
       <c r="I53">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="J53" t="inlineStr">
         <is>
@@ -5786,13 +5786,13 @@
         <v>45196</v>
       </c>
       <c r="G54">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="H54" s="2">
         <v>45287</v>
       </c>
       <c r="I54">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="J54" t="inlineStr">
         <is>
@@ -5889,13 +5889,13 @@
         <v>45044</v>
       </c>
       <c r="G55">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="H55" s="2">
         <v>45227</v>
       </c>
       <c r="I55">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="J55" t="inlineStr">
         <is>
@@ -5992,13 +5992,13 @@
         <v>45151</v>
       </c>
       <c r="G56">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="H56" s="2">
         <v>45243</v>
       </c>
       <c r="I56">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="J56" t="inlineStr">
         <is>
@@ -6090,13 +6090,13 @@
         <v>45196</v>
       </c>
       <c r="G57">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="H57" s="2">
         <v>45287</v>
       </c>
       <c r="I57">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="J57" t="inlineStr">
         <is>
@@ -6193,13 +6193,13 @@
         <v>45069</v>
       </c>
       <c r="G58">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="H58" s="2">
         <v>45253</v>
       </c>
       <c r="I58">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="J58" t="inlineStr">
         <is>
@@ -6296,13 +6296,13 @@
         <v>45191</v>
       </c>
       <c r="G59">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="H59" s="2">
         <v>45282</v>
       </c>
       <c r="I59">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="J59" t="inlineStr">
         <is>
@@ -6394,7 +6394,7 @@
         <v>45205</v>
       </c>
       <c r="G60">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="J60" t="inlineStr">
         <is>
@@ -6491,13 +6491,13 @@
         <v>45127</v>
       </c>
       <c r="G61">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="H61" s="2">
         <v>45219</v>
       </c>
       <c r="I61">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="J61" t="inlineStr">
         <is>
@@ -6594,13 +6594,13 @@
         <v>45058</v>
       </c>
       <c r="G62">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="H62" s="2">
         <v>45242</v>
       </c>
       <c r="I62">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="J62" t="inlineStr">
         <is>
@@ -6697,13 +6697,13 @@
         <v>45194</v>
       </c>
       <c r="G63">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="H63" s="2">
         <v>45376</v>
       </c>
       <c r="I63">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="J63" t="inlineStr">
         <is>
@@ -6795,7 +6795,7 @@
         <v>45208</v>
       </c>
       <c r="G64">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="J64" t="inlineStr">
         <is>
@@ -6892,7 +6892,7 @@
         <v>45208</v>
       </c>
       <c r="G65">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="J65" t="inlineStr">
         <is>
@@ -6989,13 +6989,13 @@
         <v>45089</v>
       </c>
       <c r="G66">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="H66" s="2">
         <v>45272</v>
       </c>
       <c r="I66">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="J66" t="inlineStr">
         <is>
@@ -7092,13 +7092,13 @@
         <v>45178</v>
       </c>
       <c r="G67">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="H67" s="2">
         <v>45269</v>
       </c>
       <c r="I67">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="J67" t="inlineStr">
         <is>
@@ -7190,13 +7190,13 @@
         <v>45196</v>
       </c>
       <c r="G68">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="H68" s="2">
         <v>45287</v>
       </c>
       <c r="I68">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="J68" t="inlineStr">
         <is>
@@ -7293,13 +7293,13 @@
         <v>45149</v>
       </c>
       <c r="G69">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="H69" s="2">
         <v>45241</v>
       </c>
       <c r="I69">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="J69" t="inlineStr">
         <is>
@@ -7396,13 +7396,13 @@
         <v>45205</v>
       </c>
       <c r="G70">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="H70" s="2">
         <v>45296</v>
       </c>
       <c r="I70">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="J70" t="inlineStr">
         <is>
@@ -7499,7 +7499,7 @@
         <v>45205</v>
       </c>
       <c r="G71">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="J71" t="inlineStr">
         <is>
@@ -7596,13 +7596,13 @@
         <v>45207</v>
       </c>
       <c r="G72">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="H72" s="2">
         <v>45299</v>
       </c>
       <c r="I72">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="J72" t="inlineStr">
         <is>
@@ -7699,13 +7699,13 @@
         <v>45189</v>
       </c>
       <c r="G73">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="H73" s="2">
         <v>45280</v>
       </c>
       <c r="I73">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="J73" t="inlineStr">
         <is>
@@ -7797,13 +7797,13 @@
         <v>45038</v>
       </c>
       <c r="G74">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="H74" s="2">
         <v>45221</v>
       </c>
       <c r="I74">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="J74" t="inlineStr">
         <is>
@@ -7895,13 +7895,13 @@
         <v>45117</v>
       </c>
       <c r="G75">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="H75" s="2">
         <v>45301</v>
       </c>
       <c r="I75">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="J75" t="inlineStr">
         <is>
@@ -7998,13 +7998,13 @@
         <v>45160</v>
       </c>
       <c r="G76">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="H76" s="2">
         <v>45344</v>
       </c>
       <c r="I76">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="J76" t="inlineStr">
         <is>
@@ -8101,13 +8101,13 @@
         <v>45186</v>
       </c>
       <c r="G77">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="H77" s="2">
         <v>45368</v>
       </c>
       <c r="I77">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="J77" t="inlineStr">
         <is>
@@ -8204,13 +8204,13 @@
         <v>45043</v>
       </c>
       <c r="G78">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="H78" s="2">
         <v>45226</v>
       </c>
       <c r="I78">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="J78" t="inlineStr">
         <is>
@@ -8307,13 +8307,13 @@
         <v>45079</v>
       </c>
       <c r="G79">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="H79" s="2">
         <v>45262</v>
       </c>
       <c r="I79">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="J79" t="inlineStr">
         <is>
@@ -8410,7 +8410,7 @@
         <v>45254</v>
       </c>
       <c r="I80">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="J80" t="inlineStr">
         <is>
@@ -8507,13 +8507,13 @@
         <v>45104</v>
       </c>
       <c r="G81">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="H81" s="2">
         <v>45287</v>
       </c>
       <c r="I81">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="J81" t="inlineStr">
         <is>
@@ -8610,7 +8610,7 @@
         <v>45288</v>
       </c>
       <c r="I82">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="J82" t="inlineStr">
         <is>
@@ -8702,13 +8702,13 @@
         <v>45175</v>
       </c>
       <c r="G83">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="H83" s="2">
         <v>45357</v>
       </c>
       <c r="I83">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="J83" t="inlineStr">
         <is>
@@ -8805,13 +8805,13 @@
         <v>45054</v>
       </c>
       <c r="G84">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="H84" s="2">
         <v>45238</v>
       </c>
       <c r="I84">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="J84" t="inlineStr">
         <is>
@@ -8908,13 +8908,13 @@
         <v>45056</v>
       </c>
       <c r="G85">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="H85" s="2">
         <v>45240</v>
       </c>
       <c r="I85">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="J85" t="inlineStr">
         <is>
@@ -9011,13 +9011,13 @@
         <v>45085</v>
       </c>
       <c r="G86">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="H86" s="2">
         <v>45268</v>
       </c>
       <c r="I86">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="J86" t="inlineStr">
         <is>
@@ -9114,13 +9114,13 @@
         <v>45194</v>
       </c>
       <c r="G87">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="H87" s="2">
         <v>45560</v>
       </c>
       <c r="I87">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="J87" t="inlineStr">
         <is>
@@ -9207,13 +9207,13 @@
         <v>45103</v>
       </c>
       <c r="G88">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="H88" s="2">
         <v>45286</v>
       </c>
       <c r="I88">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="J88" t="inlineStr">
         <is>
@@ -9310,13 +9310,13 @@
         <v>45103</v>
       </c>
       <c r="G89">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="H89" s="2">
         <v>45286</v>
       </c>
       <c r="I89">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="J89" t="inlineStr">
         <is>
@@ -9413,13 +9413,13 @@
         <v>45192</v>
       </c>
       <c r="G90">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="H90" s="2">
         <v>45374</v>
       </c>
       <c r="I90">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="J90" t="inlineStr">
         <is>
@@ -9511,13 +9511,13 @@
         <v>45100</v>
       </c>
       <c r="G91">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="H91" s="2">
         <v>45287</v>
       </c>
       <c r="I91">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="J91" t="inlineStr">
         <is>
@@ -9614,13 +9614,13 @@
         <v>45187</v>
       </c>
       <c r="G92">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="H92" s="2">
         <v>45369</v>
       </c>
       <c r="I92">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="J92" t="inlineStr">
         <is>
@@ -9717,13 +9717,13 @@
         <v>45104</v>
       </c>
       <c r="G93">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="H93" s="2">
         <v>45287</v>
       </c>
       <c r="I93">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="J93" t="inlineStr">
         <is>
@@ -9820,13 +9820,13 @@
         <v>45104</v>
       </c>
       <c r="G94">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="H94" s="2">
         <v>45287</v>
       </c>
       <c r="I94">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="J94" t="inlineStr">
         <is>
@@ -9923,13 +9923,13 @@
         <v>45049</v>
       </c>
       <c r="G95">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="H95" s="2">
         <v>45233</v>
       </c>
       <c r="I95">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="J95" t="inlineStr">
         <is>
@@ -10026,13 +10026,13 @@
         <v>45122</v>
       </c>
       <c r="G96">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="H96" s="2">
         <v>45306</v>
       </c>
       <c r="I96">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="J96" t="inlineStr">
         <is>
@@ -10124,13 +10124,13 @@
         <v>45141</v>
       </c>
       <c r="G97">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="H97" s="2">
         <v>45325</v>
       </c>
       <c r="I97">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="J97" t="inlineStr">
         <is>
@@ -10227,13 +10227,13 @@
         <v>45194</v>
       </c>
       <c r="G98">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="H98" s="2">
         <v>45376</v>
       </c>
       <c r="I98">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="J98" t="inlineStr">
         <is>
@@ -10325,13 +10325,13 @@
         <v>45093</v>
       </c>
       <c r="G99">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="H99" s="2">
         <v>45276</v>
       </c>
       <c r="I99">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="J99" t="inlineStr">
         <is>
@@ -10428,13 +10428,13 @@
         <v>45123</v>
       </c>
       <c r="G100">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="H100" s="2">
         <v>45307</v>
       </c>
       <c r="I100">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="J100" t="inlineStr">
         <is>
@@ -10531,13 +10531,13 @@
         <v>45198</v>
       </c>
       <c r="G101">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="H101" s="2">
         <v>45380</v>
       </c>
       <c r="I101">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="J101" t="inlineStr">
         <is>
@@ -10634,13 +10634,13 @@
         <v>45093</v>
       </c>
       <c r="G102">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="H102" s="2">
         <v>45276</v>
       </c>
       <c r="I102">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="J102" t="inlineStr">
         <is>
@@ -10737,13 +10737,13 @@
         <v>45122</v>
       </c>
       <c r="G103">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="H103" s="2">
         <v>45306</v>
       </c>
       <c r="I103">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="J103" t="inlineStr">
         <is>
@@ -10840,13 +10840,13 @@
         <v>45122</v>
       </c>
       <c r="G104">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="H104" s="2">
         <v>45306</v>
       </c>
       <c r="I104">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="J104" t="inlineStr">
         <is>
@@ -10938,13 +10938,13 @@
         <v>45050</v>
       </c>
       <c r="G105">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="H105" s="2">
         <v>45234</v>
       </c>
       <c r="I105">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="J105" t="inlineStr">
         <is>
@@ -11041,13 +11041,13 @@
         <v>45085</v>
       </c>
       <c r="G106">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="H106" s="2">
         <v>45268</v>
       </c>
       <c r="I106">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="J106" t="inlineStr">
         <is>
@@ -11144,13 +11144,13 @@
         <v>45185</v>
       </c>
       <c r="G107">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="H107" s="2">
         <v>45276</v>
       </c>
       <c r="I107">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="J107" t="inlineStr">
         <is>
@@ -11242,13 +11242,13 @@
         <v>45185</v>
       </c>
       <c r="G108">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="H108" s="2">
         <v>45276</v>
       </c>
       <c r="I108">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="J108" t="inlineStr">
         <is>
@@ -11340,13 +11340,13 @@
         <v>45185</v>
       </c>
       <c r="G109">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="H109" s="2">
         <v>45276</v>
       </c>
       <c r="I109">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="J109" t="inlineStr">
         <is>
@@ -11443,13 +11443,13 @@
         <v>45148</v>
       </c>
       <c r="G110">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="H110" s="2">
         <v>45240</v>
       </c>
       <c r="I110">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="J110" t="inlineStr">
         <is>
@@ -11546,13 +11546,13 @@
         <v>45211</v>
       </c>
       <c r="G111">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H111" s="2">
         <v>45303</v>
       </c>
       <c r="I111">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="J111" t="inlineStr">
         <is>
@@ -11649,13 +11649,13 @@
         <v>45172</v>
       </c>
       <c r="G112">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="H112" s="2">
         <v>45263</v>
       </c>
       <c r="I112">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="J112" t="inlineStr">
         <is>
@@ -11752,13 +11752,13 @@
         <v>45206</v>
       </c>
       <c r="G113">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="H113" s="2">
         <v>45389</v>
       </c>
       <c r="I113">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="J113" t="inlineStr">
         <is>
@@ -11855,13 +11855,13 @@
         <v>45203</v>
       </c>
       <c r="G114">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="H114" s="2">
         <v>45295</v>
       </c>
       <c r="I114">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="J114" t="inlineStr">
         <is>
@@ -11958,7 +11958,7 @@
         <v>45218</v>
       </c>
       <c r="I115">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="J115" t="inlineStr">
         <is>
@@ -12055,13 +12055,13 @@
         <v>45161</v>
       </c>
       <c r="G116">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="H116" s="2">
         <v>45253</v>
       </c>
       <c r="I116">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="J116" t="inlineStr">
         <is>
@@ -12158,13 +12158,13 @@
         <v>45115</v>
       </c>
       <c r="G117">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="H117" s="2">
         <v>45299</v>
       </c>
       <c r="I117">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="J117" t="inlineStr">
         <is>
@@ -12256,13 +12256,13 @@
         <v>45094</v>
       </c>
       <c r="G118">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="H118" s="2">
         <v>45277</v>
       </c>
       <c r="I118">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="J118" t="inlineStr">
         <is>
@@ -12359,13 +12359,13 @@
         <v>45104</v>
       </c>
       <c r="G119">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="H119" s="2">
         <v>45287</v>
       </c>
       <c r="I119">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="J119" t="inlineStr">
         <is>
@@ -12462,13 +12462,13 @@
         <v>45104</v>
       </c>
       <c r="G120">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="H120" s="2">
         <v>45287</v>
       </c>
       <c r="I120">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="J120" t="inlineStr">
         <is>
@@ -12565,13 +12565,13 @@
         <v>45104</v>
       </c>
       <c r="G121">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="H121" s="2">
         <v>45287</v>
       </c>
       <c r="I121">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="J121" t="inlineStr">
         <is>
@@ -12668,13 +12668,13 @@
         <v>45104</v>
       </c>
       <c r="G122">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="H122" s="2">
         <v>45287</v>
       </c>
       <c r="I122">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="J122" t="inlineStr">
         <is>
@@ -12771,13 +12771,13 @@
         <v>45199</v>
       </c>
       <c r="G123">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="H123" s="2">
         <v>45291</v>
       </c>
       <c r="I123">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="J123" t="inlineStr">
         <is>
@@ -12874,13 +12874,13 @@
         <v>45197</v>
       </c>
       <c r="G124">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H124" s="2">
         <v>45379</v>
       </c>
       <c r="I124">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="J124" t="inlineStr">
         <is>
@@ -12977,13 +12977,13 @@
         <v>45121</v>
       </c>
       <c r="G125">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="H125" s="2">
-        <v>45213</v>
+        <v>45305</v>
       </c>
       <c r="I125">
-        <v>1</v>
+        <v>92</v>
       </c>
       <c r="J125" t="inlineStr">
         <is>
@@ -13080,13 +13080,13 @@
         <v>45134</v>
       </c>
       <c r="G126">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="H126" s="2">
         <v>45226</v>
       </c>
       <c r="I126">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="J126" t="inlineStr">
         <is>
@@ -13179,11 +13179,17 @@
           <t>1 000,00</t>
         </is>
       </c>
+      <c r="F127" s="2">
+        <v>45212</v>
+      </c>
+      <c r="G127">
+        <v>1</v>
+      </c>
       <c r="H127" s="2">
         <v>45304</v>
       </c>
       <c r="I127">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="J127" t="inlineStr">
         <is>
@@ -13280,13 +13286,13 @@
         <v>45126</v>
       </c>
       <c r="G128">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="H128" s="2">
         <v>45218</v>
       </c>
       <c r="I128">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="J128" t="inlineStr">
         <is>
@@ -13378,13 +13384,13 @@
         <v>45158</v>
       </c>
       <c r="G129">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="H129" s="2">
         <v>45250</v>
       </c>
       <c r="I129">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="J129" t="inlineStr">
         <is>
@@ -13481,13 +13487,13 @@
         <v>45171</v>
       </c>
       <c r="G130">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="H130" s="2">
         <v>45262</v>
       </c>
       <c r="I130">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="J130" t="inlineStr">
         <is>
@@ -13584,13 +13590,13 @@
         <v>45203</v>
       </c>
       <c r="G131">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="H131" s="2">
         <v>45295</v>
       </c>
       <c r="I131">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="J131" t="inlineStr">
         <is>
@@ -13687,13 +13693,13 @@
         <v>45144</v>
       </c>
       <c r="G132">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="H132" s="2">
         <v>45236</v>
       </c>
       <c r="I132">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="J132" t="inlineStr">
         <is>
@@ -13790,13 +13796,13 @@
         <v>45156</v>
       </c>
       <c r="G133">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="H133" s="2">
         <v>45248</v>
       </c>
       <c r="I133">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="J133" t="inlineStr">
         <is>
@@ -13888,13 +13894,13 @@
         <v>45146</v>
       </c>
       <c r="G134">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="H134" s="2">
         <v>45238</v>
       </c>
       <c r="I134">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="J134" t="inlineStr">
         <is>
@@ -13991,13 +13997,13 @@
         <v>45140</v>
       </c>
       <c r="G135">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="H135" s="2">
         <v>45232</v>
       </c>
       <c r="I135">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="J135" t="inlineStr">
         <is>
@@ -14094,13 +14100,13 @@
         <v>45196</v>
       </c>
       <c r="G136">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="H136" s="2">
         <v>45287</v>
       </c>
       <c r="I136">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="J136" t="inlineStr">
         <is>
@@ -14197,13 +14203,13 @@
         <v>45197</v>
       </c>
       <c r="G137">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H137" s="2">
         <v>45288</v>
       </c>
       <c r="I137">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="J137" t="inlineStr">
         <is>
@@ -14300,13 +14306,13 @@
         <v>45179</v>
       </c>
       <c r="G138">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="H138" s="2">
         <v>45270</v>
       </c>
       <c r="I138">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="J138" t="inlineStr">
         <is>
@@ -14398,13 +14404,13 @@
         <v>45197</v>
       </c>
       <c r="G139">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H139" s="2">
         <v>45288</v>
       </c>
       <c r="I139">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="J139" t="inlineStr">
         <is>
@@ -14501,13 +14507,13 @@
         <v>45182</v>
       </c>
       <c r="G140">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="H140" s="2">
         <v>45273</v>
       </c>
       <c r="I140">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="J140" t="inlineStr">
         <is>
@@ -14604,13 +14610,13 @@
         <v>45208</v>
       </c>
       <c r="G141">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="H141" s="2">
         <v>45300</v>
       </c>
       <c r="I141">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="J141" t="inlineStr">
         <is>
@@ -14702,13 +14708,13 @@
         <v>45150</v>
       </c>
       <c r="G142">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="H142" s="2">
         <v>45242</v>
       </c>
       <c r="I142">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="J142" t="inlineStr">
         <is>
@@ -14805,7 +14811,7 @@
         <v>45238</v>
       </c>
       <c r="I143">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="J143" t="inlineStr">
         <is>
@@ -14902,13 +14908,13 @@
         <v>45171</v>
       </c>
       <c r="G144">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="H144" s="2">
         <v>45262</v>
       </c>
       <c r="I144">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="J144" t="inlineStr">
         <is>
@@ -15005,13 +15011,13 @@
         <v>45194</v>
       </c>
       <c r="G145">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="H145" s="2">
         <v>45285</v>
       </c>
       <c r="I145">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="J145" t="inlineStr">
         <is>
@@ -15098,7 +15104,7 @@
         <v>45211</v>
       </c>
       <c r="G146">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J146" t="inlineStr">
         <is>
@@ -15195,13 +15201,13 @@
         <v>45165</v>
       </c>
       <c r="G147">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="H147" s="2">
         <v>45257</v>
       </c>
       <c r="I147">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="J147" t="inlineStr">
         <is>
@@ -15298,13 +15304,13 @@
         <v>45166</v>
       </c>
       <c r="G148">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="H148" s="2">
         <v>45258</v>
       </c>
       <c r="I148">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="J148" t="inlineStr">
         <is>
@@ -15401,13 +15407,13 @@
         <v>45185</v>
       </c>
       <c r="G149">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="H149" s="2">
         <v>45276</v>
       </c>
       <c r="I149">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="J149" t="inlineStr">
         <is>
@@ -15504,13 +15510,13 @@
         <v>45035</v>
       </c>
       <c r="G150">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="H150" s="2">
         <v>45218</v>
       </c>
       <c r="I150">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="J150" t="inlineStr">
         <is>
@@ -15607,13 +15613,13 @@
         <v>45174</v>
       </c>
       <c r="G151">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="H151" s="2">
         <v>45356</v>
       </c>
       <c r="I151">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="J151" t="inlineStr">
         <is>
@@ -15710,13 +15716,13 @@
         <v>45089</v>
       </c>
       <c r="G152">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="H152" s="2">
         <v>45272</v>
       </c>
       <c r="I152">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="J152" t="inlineStr">
         <is>
@@ -15813,13 +15819,13 @@
         <v>45124</v>
       </c>
       <c r="G153">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="H153" s="2">
         <v>45308</v>
       </c>
       <c r="I153">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="J153" t="inlineStr">
         <is>
@@ -15916,13 +15922,13 @@
         <v>45124</v>
       </c>
       <c r="G154">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="H154" s="2">
         <v>45308</v>
       </c>
       <c r="I154">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="J154" t="inlineStr">
         <is>
@@ -16019,13 +16025,13 @@
         <v>45209</v>
       </c>
       <c r="G155">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="H155" s="2">
         <v>45392</v>
       </c>
       <c r="I155">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="J155" t="inlineStr">
         <is>
@@ -16122,13 +16128,13 @@
         <v>45209</v>
       </c>
       <c r="G156">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="H156" s="2">
         <v>45392</v>
       </c>
       <c r="I156">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="J156" t="inlineStr">
         <is>
@@ -16225,13 +16231,13 @@
         <v>45209</v>
       </c>
       <c r="G157">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="H157" s="2">
         <v>45392</v>
       </c>
       <c r="I157">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="J157" t="inlineStr">
         <is>
@@ -16328,13 +16334,13 @@
         <v>45209</v>
       </c>
       <c r="G158">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="H158" s="2">
         <v>45392</v>
       </c>
       <c r="I158">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="J158" t="inlineStr">
         <is>
@@ -16431,13 +16437,13 @@
         <v>45156</v>
       </c>
       <c r="G159">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="H159" s="2">
         <v>45247</v>
       </c>
       <c r="I159">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="J159" t="inlineStr">
         <is>
@@ -16534,13 +16540,13 @@
         <v>45153</v>
       </c>
       <c r="G160">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="H160" s="2">
         <v>45245</v>
       </c>
       <c r="I160">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="J160" t="inlineStr">
         <is>
@@ -16637,13 +16643,13 @@
         <v>45135</v>
       </c>
       <c r="G161">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="H161" s="2">
         <v>45319</v>
       </c>
       <c r="I161">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="J161" t="inlineStr">
         <is>
@@ -16740,13 +16746,13 @@
         <v>45091</v>
       </c>
       <c r="G162">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="H162" s="2">
         <v>45274</v>
       </c>
       <c r="I162">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="J162" t="inlineStr">
         <is>
@@ -16838,13 +16844,13 @@
         <v>45091</v>
       </c>
       <c r="G163">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="H163" s="2">
         <v>45274</v>
       </c>
       <c r="I163">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="J163" t="inlineStr">
         <is>
@@ -16936,13 +16942,13 @@
         <v>45138</v>
       </c>
       <c r="G164">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="H164" s="2">
         <v>45322</v>
       </c>
       <c r="I164">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="J164" t="inlineStr">
         <is>
@@ -17039,13 +17045,13 @@
         <v>45138</v>
       </c>
       <c r="G165">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="H165" s="2">
         <v>45322</v>
       </c>
       <c r="I165">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="J165" t="inlineStr">
         <is>
@@ -17142,13 +17148,13 @@
         <v>45085</v>
       </c>
       <c r="G166">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="H166" s="2">
         <v>45268</v>
       </c>
       <c r="I166">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="J166" t="inlineStr">
         <is>
@@ -17245,13 +17251,13 @@
         <v>45085</v>
       </c>
       <c r="G167">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="H167" s="2">
         <v>45268</v>
       </c>
       <c r="I167">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="J167" t="inlineStr">
         <is>
@@ -17348,7 +17354,7 @@
         <v>45326</v>
       </c>
       <c r="I168">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="J168" t="inlineStr">
         <is>
@@ -17445,13 +17451,13 @@
         <v>45173</v>
       </c>
       <c r="G169">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="H169" s="2">
         <v>45355</v>
       </c>
       <c r="I169">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="J169" t="inlineStr">
         <is>
@@ -17548,13 +17554,13 @@
         <v>45056</v>
       </c>
       <c r="G170">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="H170" s="2">
         <v>45240</v>
       </c>
       <c r="I170">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="J170" t="inlineStr">
         <is>
@@ -17651,7 +17657,7 @@
         <v>45238</v>
       </c>
       <c r="I171">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="J171" t="inlineStr">
         <is>
@@ -17748,13 +17754,13 @@
         <v>45141</v>
       </c>
       <c r="G172">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="H172" s="2">
         <v>45325</v>
       </c>
       <c r="I172">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="J172" t="inlineStr">
         <is>
@@ -17851,13 +17857,13 @@
         <v>45037</v>
       </c>
       <c r="G173">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="H173" s="2">
         <v>45220</v>
       </c>
       <c r="I173">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="J173" t="inlineStr">
         <is>
@@ -17954,13 +17960,13 @@
         <v>45171</v>
       </c>
       <c r="G174">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="H174" s="2">
         <v>45262</v>
       </c>
       <c r="I174">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="J174" t="inlineStr">
         <is>
@@ -18057,13 +18063,13 @@
         <v>45197</v>
       </c>
       <c r="G175">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H175" s="2">
         <v>45288</v>
       </c>
       <c r="I175">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="J175" t="inlineStr">
         <is>
@@ -18160,13 +18166,13 @@
         <v>45162</v>
       </c>
       <c r="G176">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="H176" s="2">
         <v>45254</v>
       </c>
       <c r="I176">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="J176" t="inlineStr">
         <is>
@@ -18263,13 +18269,13 @@
         <v>45061</v>
       </c>
       <c r="G177">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="H177" s="2">
         <v>45245</v>
       </c>
       <c r="I177">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="J177" t="inlineStr">
         <is>
@@ -18363,16 +18369,16 @@
         </is>
       </c>
       <c r="F178" s="2">
-        <v>45120</v>
+        <v>45212</v>
       </c>
       <c r="G178">
-        <v>92</v>
+        <v>1</v>
       </c>
       <c r="H178" s="2">
         <v>45304</v>
       </c>
       <c r="I178">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="J178" t="inlineStr">
         <is>
@@ -18469,13 +18475,13 @@
         <v>45191</v>
       </c>
       <c r="G179">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="H179" s="2">
         <v>45282</v>
       </c>
       <c r="I179">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="J179" t="inlineStr">
         <is>
@@ -18572,13 +18578,13 @@
         <v>45088</v>
       </c>
       <c r="G180">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="H180" s="2">
         <v>45271</v>
       </c>
       <c r="I180">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="J180" t="inlineStr">
         <is>
@@ -18675,13 +18681,13 @@
         <v>45192</v>
       </c>
       <c r="G181">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="H181" s="2">
         <v>45283</v>
       </c>
       <c r="I181">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="J181" t="inlineStr">
         <is>
@@ -18768,13 +18774,13 @@
         <v>45131</v>
       </c>
       <c r="G182">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="H182" s="2">
         <v>45223</v>
       </c>
       <c r="I182">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="J182" t="inlineStr">
         <is>
@@ -18866,13 +18872,13 @@
         <v>45136</v>
       </c>
       <c r="G183">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="H183" s="2">
         <v>45228</v>
       </c>
       <c r="I183">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="J183" t="inlineStr">
         <is>
@@ -18964,13 +18970,13 @@
         <v>45150</v>
       </c>
       <c r="G184">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="H184" s="2">
         <v>45242</v>
       </c>
       <c r="I184">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="J184" t="inlineStr">
         <is>
@@ -19062,7 +19068,7 @@
         <v>45210</v>
       </c>
       <c r="G185">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="J185" t="inlineStr">
         <is>
@@ -19154,13 +19160,13 @@
         <v>45129</v>
       </c>
       <c r="G186">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="H186" s="2">
         <v>45221</v>
       </c>
       <c r="I186">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="J186" t="inlineStr">
         <is>
@@ -19252,13 +19258,13 @@
         <v>45189</v>
       </c>
       <c r="G187">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="H187" s="2">
         <v>45280</v>
       </c>
       <c r="I187">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="J187" t="inlineStr">
         <is>
@@ -19345,13 +19351,13 @@
         <v>45193</v>
       </c>
       <c r="G188">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="H188" s="2">
         <v>45284</v>
       </c>
       <c r="I188">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="J188" t="inlineStr">
         <is>
@@ -19438,13 +19444,13 @@
         <v>45165</v>
       </c>
       <c r="G189">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="H189" s="2">
         <v>45257</v>
       </c>
       <c r="I189">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="J189" t="inlineStr">
         <is>
@@ -19536,13 +19542,13 @@
         <v>45202</v>
       </c>
       <c r="G190">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="H190" s="2">
         <v>45385</v>
       </c>
       <c r="I190">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="J190" t="inlineStr">
         <is>
@@ -19639,13 +19645,13 @@
         <v>45081</v>
       </c>
       <c r="G191">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="H191" s="2">
         <v>45264</v>
       </c>
       <c r="I191">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="J191" t="inlineStr">
         <is>
@@ -19742,13 +19748,13 @@
         <v>45081</v>
       </c>
       <c r="G192">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="H192" s="2">
         <v>45264</v>
       </c>
       <c r="I192">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="J192" t="inlineStr">
         <is>
@@ -19845,7 +19851,7 @@
         <v>45319</v>
       </c>
       <c r="I193">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="J193" t="inlineStr">
         <is>
@@ -19942,7 +19948,7 @@
         <v>45319</v>
       </c>
       <c r="I194">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="J194" t="inlineStr">
         <is>
@@ -20034,13 +20040,13 @@
         <v>45046</v>
       </c>
       <c r="G195">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="H195" s="2">
         <v>45230</v>
       </c>
       <c r="I195">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="J195" t="inlineStr">
         <is>
@@ -20137,13 +20143,13 @@
         <v>45046</v>
       </c>
       <c r="G196">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="H196" s="2">
         <v>45230</v>
       </c>
       <c r="I196">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="J196" t="inlineStr">
         <is>
@@ -20240,13 +20246,13 @@
         <v>45031</v>
       </c>
       <c r="G197">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="H197" s="2">
         <v>45214</v>
       </c>
       <c r="I197">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J197" t="inlineStr">
         <is>
@@ -20343,13 +20349,13 @@
         <v>45031</v>
       </c>
       <c r="G198">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="H198" s="2">
         <v>45214</v>
       </c>
       <c r="I198">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J198" t="inlineStr">
         <is>
@@ -20446,13 +20452,13 @@
         <v>45031</v>
       </c>
       <c r="G199">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="H199" s="2">
         <v>45214</v>
       </c>
       <c r="I199">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J199" t="inlineStr">
         <is>
@@ -20549,13 +20555,13 @@
         <v>45031</v>
       </c>
       <c r="G200">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="H200" s="2">
         <v>45214</v>
       </c>
       <c r="I200">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J200" t="inlineStr">
         <is>
@@ -20652,13 +20658,13 @@
         <v>45067</v>
       </c>
       <c r="G201">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="H201" s="2">
         <v>45251</v>
       </c>
       <c r="I201">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="J201" t="inlineStr">
         <is>
@@ -20755,13 +20761,13 @@
         <v>45067</v>
       </c>
       <c r="G202">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="H202" s="2">
         <v>45251</v>
       </c>
       <c r="I202">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="J202" t="inlineStr">
         <is>
@@ -20858,13 +20864,13 @@
         <v>45067</v>
       </c>
       <c r="G203">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="H203" s="2">
         <v>45251</v>
       </c>
       <c r="I203">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="J203" t="inlineStr">
         <is>
@@ -20961,13 +20967,13 @@
         <v>45067</v>
       </c>
       <c r="G204">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="H204" s="2">
         <v>45251</v>
       </c>
       <c r="I204">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="J204" t="inlineStr">
         <is>
@@ -21064,13 +21070,13 @@
         <v>45178</v>
       </c>
       <c r="G205">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="H205" s="2">
         <v>45269</v>
       </c>
       <c r="I205">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="J205" t="inlineStr">
         <is>
@@ -21167,7 +21173,7 @@
         <v>45252</v>
       </c>
       <c r="I206">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="J206" t="inlineStr">
         <is>
@@ -21264,13 +21270,13 @@
         <v>45087</v>
       </c>
       <c r="G207">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="H207" s="2">
         <v>45270</v>
       </c>
       <c r="I207">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="J207" t="inlineStr">
         <is>
@@ -21367,13 +21373,13 @@
         <v>45099</v>
       </c>
       <c r="G208">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="H208" s="2">
         <v>45282</v>
       </c>
       <c r="I208">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="J208" t="inlineStr">
         <is>
@@ -21470,13 +21476,13 @@
         <v>45175</v>
       </c>
       <c r="G209">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="H209" s="2">
         <v>45356</v>
       </c>
       <c r="I209">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="J209" t="inlineStr">
         <is>
@@ -21573,13 +21579,13 @@
         <v>45175</v>
       </c>
       <c r="G210">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="H210" s="2">
         <v>45356</v>
       </c>
       <c r="I210">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="J210" t="inlineStr">
         <is>
@@ -21676,13 +21682,13 @@
         <v>45166</v>
       </c>
       <c r="G211">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="H211" s="2">
         <v>45350</v>
       </c>
       <c r="I211">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="J211" t="inlineStr">
         <is>
@@ -21779,13 +21785,13 @@
         <v>45166</v>
       </c>
       <c r="G212">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="H212" s="2">
         <v>45350</v>
       </c>
       <c r="I212">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="J212" t="inlineStr">
         <is>
@@ -21882,13 +21888,13 @@
         <v>45090</v>
       </c>
       <c r="G213">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="H213" s="2">
         <v>45273</v>
       </c>
       <c r="I213">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="J213" t="inlineStr">
         <is>
@@ -21985,13 +21991,13 @@
         <v>45106</v>
       </c>
       <c r="G214">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="H214" s="2">
         <v>45289</v>
       </c>
       <c r="I214">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="J214" t="inlineStr">
         <is>
@@ -22088,13 +22094,13 @@
         <v>45134</v>
       </c>
       <c r="G215">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="H215" s="2">
         <v>45226</v>
       </c>
       <c r="I215">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="J215" t="inlineStr">
         <is>
@@ -22191,13 +22197,13 @@
         <v>45132</v>
       </c>
       <c r="G216">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="H216" s="2">
         <v>45224</v>
       </c>
       <c r="I216">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="J216" t="inlineStr">
         <is>
@@ -22294,13 +22300,13 @@
         <v>45150</v>
       </c>
       <c r="G217">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="H217" s="2">
         <v>45242</v>
       </c>
       <c r="I217">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="J217" t="inlineStr">
         <is>
@@ -22397,13 +22403,13 @@
         <v>45187</v>
       </c>
       <c r="G218">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="H218" s="2">
         <v>45278</v>
       </c>
       <c r="I218">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="J218" t="inlineStr">
         <is>
@@ -22495,13 +22501,13 @@
         <v>45182</v>
       </c>
       <c r="G219">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="H219" s="2">
         <v>45273</v>
       </c>
       <c r="I219">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="J219" t="inlineStr">
         <is>
@@ -22598,13 +22604,13 @@
         <v>45196</v>
       </c>
       <c r="G220">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="H220" s="2">
         <v>45287</v>
       </c>
       <c r="I220">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="J220" t="inlineStr">
         <is>
@@ -22701,13 +22707,13 @@
         <v>45200</v>
       </c>
       <c r="G221">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="H221" s="2">
         <v>45292</v>
       </c>
       <c r="I221">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="J221" t="inlineStr">
         <is>
@@ -22804,13 +22810,13 @@
         <v>45135</v>
       </c>
       <c r="G222">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="H222" s="2">
         <v>45227</v>
       </c>
       <c r="I222">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="J222" t="inlineStr">
         <is>
@@ -22907,13 +22913,13 @@
         <v>45148</v>
       </c>
       <c r="G223">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="H223" s="2">
         <v>45240</v>
       </c>
       <c r="I223">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="J223" t="inlineStr">
         <is>
@@ -23005,13 +23011,13 @@
         <v>45192</v>
       </c>
       <c r="G224">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="H224" s="2">
         <v>45283</v>
       </c>
       <c r="I224">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="J224" t="inlineStr">
         <is>
@@ -23103,13 +23109,13 @@
         <v>45136</v>
       </c>
       <c r="G225">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="H225" s="2">
         <v>45320</v>
       </c>
       <c r="I225">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="J225" t="inlineStr">
         <is>
@@ -23206,13 +23212,13 @@
         <v>45136</v>
       </c>
       <c r="G226">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="H226" s="2">
         <v>45320</v>
       </c>
       <c r="I226">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="J226" t="inlineStr">
         <is>
@@ -23309,13 +23315,13 @@
         <v>45094</v>
       </c>
       <c r="G227">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="H227" s="2">
         <v>45277</v>
       </c>
       <c r="I227">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="J227" t="inlineStr">
         <is>
@@ -23412,13 +23418,13 @@
         <v>45081</v>
       </c>
       <c r="G228">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="H228" s="2">
         <v>45264</v>
       </c>
       <c r="I228">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="J228" t="inlineStr">
         <is>
@@ -23515,13 +23521,13 @@
         <v>45099</v>
       </c>
       <c r="G229">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="H229" s="2">
         <v>45282</v>
       </c>
       <c r="I229">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="J229" t="inlineStr">
         <is>
@@ -23618,13 +23624,13 @@
         <v>45201</v>
       </c>
       <c r="G230">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="H230" s="2">
         <v>45384</v>
       </c>
       <c r="I230">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="J230" t="inlineStr">
         <is>
@@ -23721,13 +23727,13 @@
         <v>45031</v>
       </c>
       <c r="G231">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="H231" s="2">
         <v>45214</v>
       </c>
       <c r="I231">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J231" t="inlineStr">
         <is>
@@ -23824,7 +23830,7 @@
         <v>45294</v>
       </c>
       <c r="I232">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="J232" t="inlineStr">
         <is>
@@ -23921,13 +23927,13 @@
         <v>45079</v>
       </c>
       <c r="G233">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="H233" s="2">
         <v>45262</v>
       </c>
       <c r="I233">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="J233" t="inlineStr">
         <is>
@@ -24024,13 +24030,13 @@
         <v>45199</v>
       </c>
       <c r="G234">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="H234" s="2">
         <v>45382</v>
       </c>
       <c r="I234">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="J234" t="inlineStr">
         <is>
@@ -24127,13 +24133,13 @@
         <v>45204</v>
       </c>
       <c r="G235">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="H235" s="2">
         <v>45387</v>
       </c>
       <c r="I235">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="J235" t="inlineStr">
         <is>
@@ -24230,13 +24236,13 @@
         <v>45204</v>
       </c>
       <c r="G236">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="H236" s="2">
         <v>45387</v>
       </c>
       <c r="I236">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="J236" t="inlineStr">
         <is>
@@ -24333,13 +24339,13 @@
         <v>45080</v>
       </c>
       <c r="G237">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="H237" s="2">
         <v>45263</v>
       </c>
       <c r="I237">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="J237" t="inlineStr">
         <is>
@@ -24436,13 +24442,13 @@
         <v>45046</v>
       </c>
       <c r="G238">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="H238" s="2">
         <v>45229</v>
       </c>
       <c r="I238">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="J238" t="inlineStr">
         <is>
@@ -24539,13 +24545,13 @@
         <v>45204</v>
       </c>
       <c r="G239">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="H239" s="2">
         <v>45296</v>
       </c>
       <c r="I239">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="J239" t="inlineStr">
         <is>
@@ -24642,13 +24648,13 @@
         <v>45204</v>
       </c>
       <c r="G240">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="H240" s="2">
         <v>45296</v>
       </c>
       <c r="I240">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="J240" t="inlineStr">
         <is>
@@ -24745,13 +24751,13 @@
         <v>45199</v>
       </c>
       <c r="G241">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="H241" s="2">
         <v>45382</v>
       </c>
       <c r="I241">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="J241" t="inlineStr">
         <is>
@@ -24848,13 +24854,13 @@
         <v>45070</v>
       </c>
       <c r="G242">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="H242" s="2">
         <v>45254</v>
       </c>
       <c r="I242">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="J242" t="inlineStr">
         <is>
@@ -24951,13 +24957,13 @@
         <v>45168</v>
       </c>
       <c r="G243">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="H243" s="2">
         <v>45260</v>
       </c>
       <c r="I243">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="J243" t="inlineStr">
         <is>
@@ -25054,13 +25060,13 @@
         <v>45210</v>
       </c>
       <c r="G244">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H244" s="2">
         <v>45393</v>
       </c>
       <c r="I244">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="J244" t="inlineStr">
         <is>
@@ -25157,13 +25163,13 @@
         <v>45077</v>
       </c>
       <c r="G245">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="H245" s="2">
         <v>45260</v>
       </c>
       <c r="I245">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="J245" t="inlineStr">
         <is>
@@ -25260,13 +25266,13 @@
         <v>45100</v>
       </c>
       <c r="G246">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="H246" s="2">
         <v>45283</v>
       </c>
       <c r="I246">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="J246" t="inlineStr">
         <is>
@@ -25363,7 +25369,7 @@
         <v>45281</v>
       </c>
       <c r="I247">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="J247" t="inlineStr">
         <is>
@@ -25460,13 +25466,13 @@
         <v>45044</v>
       </c>
       <c r="G248">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="H248" s="2">
         <v>45227</v>
       </c>
       <c r="I248">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="J248" t="inlineStr">
         <is>
@@ -25563,13 +25569,13 @@
         <v>45101</v>
       </c>
       <c r="G249">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="H249" s="2">
         <v>45283</v>
       </c>
       <c r="I249">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="J249" t="inlineStr">
         <is>
@@ -25666,13 +25672,13 @@
         <v>45134</v>
       </c>
       <c r="G250">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="H250" s="2">
         <v>45226</v>
       </c>
       <c r="I250">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="J250" t="inlineStr">
         <is>
@@ -25769,13 +25775,13 @@
         <v>45158</v>
       </c>
       <c r="G251">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="H251" s="2">
         <v>45250</v>
       </c>
       <c r="I251">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="J251" t="inlineStr">
         <is>
@@ -25872,13 +25878,13 @@
         <v>45200</v>
       </c>
       <c r="G252">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="H252" s="2">
         <v>45292</v>
       </c>
       <c r="I252">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="J252" t="inlineStr">
         <is>
@@ -25975,7 +25981,7 @@
         <v>45317</v>
       </c>
       <c r="I253">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="J253" t="inlineStr">
         <is>
@@ -26072,13 +26078,13 @@
         <v>45039</v>
       </c>
       <c r="G254">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="H254" s="2">
         <v>45222</v>
       </c>
       <c r="I254">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="J254" t="inlineStr">
         <is>
@@ -26170,13 +26176,13 @@
         <v>45129</v>
       </c>
       <c r="G255">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="H255" s="2">
         <v>45221</v>
       </c>
       <c r="I255">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="J255" t="inlineStr">
         <is>
@@ -26273,13 +26279,13 @@
         <v>45157</v>
       </c>
       <c r="G256">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="H256" s="2">
         <v>45341</v>
       </c>
       <c r="I256">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="J256" t="inlineStr">
         <is>
@@ -26376,13 +26382,13 @@
         <v>45063</v>
       </c>
       <c r="G257">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="H257" s="2">
         <v>45247</v>
       </c>
       <c r="I257">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="J257" t="inlineStr">
         <is>
@@ -26479,7 +26485,7 @@
         <v>45254</v>
       </c>
       <c r="I258">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="J258" t="inlineStr">
         <is>
@@ -26576,7 +26582,7 @@
         <v>45486</v>
       </c>
       <c r="I259">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="J259" t="inlineStr">
         <is>
@@ -26668,13 +26674,13 @@
         <v>45073</v>
       </c>
       <c r="G260">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="H260" s="2">
         <v>45439</v>
       </c>
       <c r="I260">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="J260" t="inlineStr">
         <is>
@@ -26766,7 +26772,7 @@
         <v>45323</v>
       </c>
       <c r="I261">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="J261" t="inlineStr">
         <is>
@@ -26858,7 +26864,7 @@
         <v>45303</v>
       </c>
       <c r="I262">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="J262" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
Bond dates update Sun Oct 15 23:15:56 UTC 2023
</commit_message>
<xml_diff>
--- a/Data/obligacje_screener.xlsx
+++ b/Data/obligacje_screener.xlsx
@@ -512,7 +512,7 @@
         <v>45340</v>
       </c>
       <c r="I2">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="J2" t="inlineStr">
         <is>
@@ -600,13 +600,13 @@
         <v>45121</v>
       </c>
       <c r="G3">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="H3" s="2">
         <v>45305</v>
       </c>
       <c r="I3">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="J3" t="inlineStr">
         <is>
@@ -703,13 +703,13 @@
         <v>45039</v>
       </c>
       <c r="G4">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="H4" s="2">
         <v>45222</v>
       </c>
       <c r="I4">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="J4" t="inlineStr">
         <is>
@@ -806,13 +806,13 @@
         <v>45039</v>
       </c>
       <c r="G5">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="H5" s="2">
         <v>45222</v>
       </c>
       <c r="I5">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="J5" t="inlineStr">
         <is>
@@ -909,13 +909,13 @@
         <v>45129</v>
       </c>
       <c r="G6">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="H6" s="2">
         <v>45221</v>
       </c>
       <c r="I6">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="J6" t="inlineStr">
         <is>
@@ -1012,13 +1012,13 @@
         <v>45162</v>
       </c>
       <c r="G7">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="H7" s="2">
         <v>45254</v>
       </c>
       <c r="I7">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="J7" t="inlineStr">
         <is>
@@ -1110,13 +1110,13 @@
         <v>45156</v>
       </c>
       <c r="G8">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="H8" s="2">
         <v>45248</v>
       </c>
       <c r="I8">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="J8" t="inlineStr">
         <is>
@@ -1213,13 +1213,13 @@
         <v>45141</v>
       </c>
       <c r="G9">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="H9" s="2">
         <v>45233</v>
       </c>
       <c r="I9">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="J9" t="inlineStr">
         <is>
@@ -1316,13 +1316,13 @@
         <v>45062</v>
       </c>
       <c r="G10">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="H10" s="2">
         <v>45246</v>
       </c>
       <c r="I10">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="J10" t="inlineStr">
         <is>
@@ -1419,7 +1419,7 @@
         <v>45286</v>
       </c>
       <c r="I11">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="J11" t="inlineStr">
         <is>
@@ -1516,13 +1516,13 @@
         <v>45195</v>
       </c>
       <c r="G12">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="H12" s="2">
         <v>45377</v>
       </c>
       <c r="I12">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="J12" t="inlineStr">
         <is>
@@ -1614,13 +1614,13 @@
         <v>45036</v>
       </c>
       <c r="G13">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="H13" s="2">
         <v>45219</v>
       </c>
       <c r="I13">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="J13" t="inlineStr">
         <is>
@@ -1717,13 +1717,13 @@
         <v>45036</v>
       </c>
       <c r="G14">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="H14" s="2">
         <v>45219</v>
       </c>
       <c r="I14">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="J14" t="inlineStr">
         <is>
@@ -1820,13 +1820,13 @@
         <v>45106</v>
       </c>
       <c r="G15">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="H15" s="2">
         <v>45289</v>
       </c>
       <c r="I15">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="J15" t="inlineStr">
         <is>
@@ -1923,13 +1923,13 @@
         <v>45186</v>
       </c>
       <c r="G16">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="H16" s="2">
         <v>45278</v>
       </c>
       <c r="I16">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="J16" t="inlineStr">
         <is>
@@ -2026,13 +2026,13 @@
         <v>45186</v>
       </c>
       <c r="G17">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="H17" s="2">
         <v>45277</v>
       </c>
       <c r="I17">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="J17" t="inlineStr">
         <is>
@@ -2129,13 +2129,13 @@
         <v>45132</v>
       </c>
       <c r="G18">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="H18" s="2">
         <v>45224</v>
       </c>
       <c r="I18">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="J18" t="inlineStr">
         <is>
@@ -2232,13 +2232,13 @@
         <v>45137</v>
       </c>
       <c r="G19">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="H19" s="2">
         <v>45229</v>
       </c>
       <c r="I19">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="J19" t="inlineStr">
         <is>
@@ -2330,13 +2330,13 @@
         <v>45183</v>
       </c>
       <c r="G20">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="H20" s="2">
         <v>45274</v>
       </c>
       <c r="I20">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="J20" t="inlineStr">
         <is>
@@ -2433,13 +2433,13 @@
         <v>45187</v>
       </c>
       <c r="G21">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="H21" s="2">
         <v>45278</v>
       </c>
       <c r="I21">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="J21" t="inlineStr">
         <is>
@@ -2536,13 +2536,13 @@
         <v>45187</v>
       </c>
       <c r="G22">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="H22" s="2">
         <v>45278</v>
       </c>
       <c r="I22">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="J22" t="inlineStr">
         <is>
@@ -2639,7 +2639,7 @@
         <v>45245</v>
       </c>
       <c r="I23">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="J23" t="inlineStr">
         <is>
@@ -2736,7 +2736,7 @@
         <v>45245</v>
       </c>
       <c r="I24">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="J24" t="inlineStr">
         <is>
@@ -2833,7 +2833,7 @@
         <v>45204</v>
       </c>
       <c r="G25">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="J25" t="inlineStr">
         <is>
@@ -2930,13 +2930,13 @@
         <v>45160</v>
       </c>
       <c r="G26">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="H26" s="2">
         <v>45344</v>
       </c>
       <c r="I26">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="J26" t="inlineStr">
         <is>
@@ -3033,13 +3033,13 @@
         <v>45118</v>
       </c>
       <c r="G27">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="H27" s="2">
         <v>45302</v>
       </c>
       <c r="I27">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="J27" t="inlineStr">
         <is>
@@ -3136,13 +3136,13 @@
         <v>45085</v>
       </c>
       <c r="G28">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="H28" s="2">
         <v>45268</v>
       </c>
       <c r="I28">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="J28" t="inlineStr">
         <is>
@@ -3239,13 +3239,13 @@
         <v>45183</v>
       </c>
       <c r="G29">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="H29" s="2">
         <v>45274</v>
       </c>
       <c r="I29">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="J29" t="inlineStr">
         <is>
@@ -3342,7 +3342,7 @@
         <v>45224</v>
       </c>
       <c r="I30">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="J30" t="inlineStr">
         <is>
@@ -3439,13 +3439,13 @@
         <v>45153</v>
       </c>
       <c r="G31">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="H31" s="2">
         <v>45245</v>
       </c>
       <c r="I31">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="J31" t="inlineStr">
         <is>
@@ -3542,13 +3542,13 @@
         <v>45155</v>
       </c>
       <c r="G32">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="H32" s="2">
         <v>45247</v>
       </c>
       <c r="I32">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="J32" t="inlineStr">
         <is>
@@ -3645,7 +3645,7 @@
         <v>45255</v>
       </c>
       <c r="I33">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="J33" t="inlineStr">
         <is>
@@ -3742,13 +3742,13 @@
         <v>45176</v>
       </c>
       <c r="G34">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="H34" s="2">
         <v>45267</v>
       </c>
       <c r="I34">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="J34" t="inlineStr">
         <is>
@@ -3845,13 +3845,13 @@
         <v>45130</v>
       </c>
       <c r="G35">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="H35" s="2">
         <v>45222</v>
       </c>
       <c r="I35">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="J35" t="inlineStr">
         <is>
@@ -3943,13 +3943,13 @@
         <v>45207</v>
       </c>
       <c r="G36">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="H36" s="2">
         <v>45299</v>
       </c>
       <c r="I36">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="J36" t="inlineStr">
         <is>
@@ -4046,13 +4046,13 @@
         <v>45189</v>
       </c>
       <c r="G37">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="H37" s="2">
         <v>45280</v>
       </c>
       <c r="I37">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="J37" t="inlineStr">
         <is>
@@ -4144,13 +4144,13 @@
         <v>45107</v>
       </c>
       <c r="G38">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="H38" s="2">
         <v>45290</v>
       </c>
       <c r="I38">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="J38" t="inlineStr">
         <is>
@@ -4247,13 +4247,13 @@
         <v>45063</v>
       </c>
       <c r="G39">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="H39" s="2">
         <v>45247</v>
       </c>
       <c r="I39">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="J39" t="inlineStr">
         <is>
@@ -4350,13 +4350,13 @@
         <v>45177</v>
       </c>
       <c r="G40">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="H40" s="2">
         <v>45359</v>
       </c>
       <c r="I40">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="J40" t="inlineStr">
         <is>
@@ -4453,13 +4453,13 @@
         <v>45107</v>
       </c>
       <c r="G41">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="H41" s="2">
         <v>45290</v>
       </c>
       <c r="I41">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="J41" t="inlineStr">
         <is>
@@ -4556,7 +4556,7 @@
         <v>45265</v>
       </c>
       <c r="I42">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="J42" t="inlineStr">
         <is>
@@ -4653,13 +4653,13 @@
         <v>45098</v>
       </c>
       <c r="G43">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="H43" s="2">
         <v>45281</v>
       </c>
       <c r="I43">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="J43" t="inlineStr">
         <is>
@@ -4756,13 +4756,13 @@
         <v>45099</v>
       </c>
       <c r="G44">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="H44" s="2">
         <v>45282</v>
       </c>
       <c r="I44">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="J44" t="inlineStr">
         <is>
@@ -4859,13 +4859,13 @@
         <v>45106</v>
       </c>
       <c r="G45">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="H45" s="2">
         <v>45289</v>
       </c>
       <c r="I45">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="J45" t="inlineStr">
         <is>
@@ -4962,13 +4962,13 @@
         <v>45106</v>
       </c>
       <c r="G46">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="H46" s="2">
         <v>45289</v>
       </c>
       <c r="I46">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="J46" t="inlineStr">
         <is>
@@ -5065,13 +5065,13 @@
         <v>45120</v>
       </c>
       <c r="G47">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="H47" s="2">
         <v>45304</v>
       </c>
       <c r="I47">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="J47" t="inlineStr">
         <is>
@@ -5168,13 +5168,13 @@
         <v>45118</v>
       </c>
       <c r="G48">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="H48" s="2">
         <v>45302</v>
       </c>
       <c r="I48">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="J48" t="inlineStr">
         <is>
@@ -5271,13 +5271,13 @@
         <v>45152</v>
       </c>
       <c r="G49">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="H49" s="2">
         <v>45336</v>
       </c>
       <c r="I49">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="J49" t="inlineStr">
         <is>
@@ -5374,13 +5374,13 @@
         <v>45042</v>
       </c>
       <c r="G50">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="H50" s="2">
         <v>45225</v>
       </c>
       <c r="I50">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="J50" t="inlineStr">
         <is>
@@ -5477,13 +5477,13 @@
         <v>45122</v>
       </c>
       <c r="G51">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="H51" s="2">
         <v>45306</v>
       </c>
       <c r="I51">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="J51" t="inlineStr">
         <is>
@@ -5580,13 +5580,13 @@
         <v>45139</v>
       </c>
       <c r="G52">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="H52" s="2">
         <v>45323</v>
       </c>
       <c r="I52">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="J52" t="inlineStr">
         <is>
@@ -5683,13 +5683,13 @@
         <v>45099</v>
       </c>
       <c r="G53">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="H53" s="2">
         <v>45282</v>
       </c>
       <c r="I53">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="J53" t="inlineStr">
         <is>
@@ -5786,13 +5786,13 @@
         <v>45196</v>
       </c>
       <c r="G54">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="H54" s="2">
         <v>45287</v>
       </c>
       <c r="I54">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="J54" t="inlineStr">
         <is>
@@ -5889,13 +5889,13 @@
         <v>45044</v>
       </c>
       <c r="G55">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="H55" s="2">
         <v>45227</v>
       </c>
       <c r="I55">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="J55" t="inlineStr">
         <is>
@@ -5992,13 +5992,13 @@
         <v>45151</v>
       </c>
       <c r="G56">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="H56" s="2">
         <v>45243</v>
       </c>
       <c r="I56">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="J56" t="inlineStr">
         <is>
@@ -6090,13 +6090,13 @@
         <v>45196</v>
       </c>
       <c r="G57">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="H57" s="2">
         <v>45287</v>
       </c>
       <c r="I57">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="J57" t="inlineStr">
         <is>
@@ -6193,13 +6193,13 @@
         <v>45069</v>
       </c>
       <c r="G58">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="H58" s="2">
         <v>45253</v>
       </c>
       <c r="I58">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="J58" t="inlineStr">
         <is>
@@ -6296,13 +6296,13 @@
         <v>45191</v>
       </c>
       <c r="G59">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="H59" s="2">
         <v>45282</v>
       </c>
       <c r="I59">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="J59" t="inlineStr">
         <is>
@@ -6394,7 +6394,7 @@
         <v>45205</v>
       </c>
       <c r="G60">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="J60" t="inlineStr">
         <is>
@@ -6491,13 +6491,13 @@
         <v>45127</v>
       </c>
       <c r="G61">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="H61" s="2">
         <v>45219</v>
       </c>
       <c r="I61">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="J61" t="inlineStr">
         <is>
@@ -6594,13 +6594,13 @@
         <v>45058</v>
       </c>
       <c r="G62">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="H62" s="2">
         <v>45242</v>
       </c>
       <c r="I62">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="J62" t="inlineStr">
         <is>
@@ -6697,13 +6697,13 @@
         <v>45194</v>
       </c>
       <c r="G63">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="H63" s="2">
         <v>45376</v>
       </c>
       <c r="I63">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="J63" t="inlineStr">
         <is>
@@ -6795,7 +6795,7 @@
         <v>45208</v>
       </c>
       <c r="G64">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="J64" t="inlineStr">
         <is>
@@ -6892,7 +6892,7 @@
         <v>45208</v>
       </c>
       <c r="G65">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="J65" t="inlineStr">
         <is>
@@ -6989,13 +6989,13 @@
         <v>45089</v>
       </c>
       <c r="G66">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="H66" s="2">
         <v>45272</v>
       </c>
       <c r="I66">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="J66" t="inlineStr">
         <is>
@@ -7092,13 +7092,13 @@
         <v>45178</v>
       </c>
       <c r="G67">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="H67" s="2">
         <v>45269</v>
       </c>
       <c r="I67">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="J67" t="inlineStr">
         <is>
@@ -7190,13 +7190,13 @@
         <v>45196</v>
       </c>
       <c r="G68">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="H68" s="2">
         <v>45287</v>
       </c>
       <c r="I68">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="J68" t="inlineStr">
         <is>
@@ -7293,13 +7293,13 @@
         <v>45149</v>
       </c>
       <c r="G69">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="H69" s="2">
         <v>45241</v>
       </c>
       <c r="I69">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="J69" t="inlineStr">
         <is>
@@ -7396,13 +7396,13 @@
         <v>45205</v>
       </c>
       <c r="G70">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="H70" s="2">
         <v>45296</v>
       </c>
       <c r="I70">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="J70" t="inlineStr">
         <is>
@@ -7499,7 +7499,7 @@
         <v>45205</v>
       </c>
       <c r="G71">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="J71" t="inlineStr">
         <is>
@@ -7596,13 +7596,13 @@
         <v>45207</v>
       </c>
       <c r="G72">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="H72" s="2">
         <v>45299</v>
       </c>
       <c r="I72">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="J72" t="inlineStr">
         <is>
@@ -7699,13 +7699,13 @@
         <v>45189</v>
       </c>
       <c r="G73">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="H73" s="2">
         <v>45280</v>
       </c>
       <c r="I73">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="J73" t="inlineStr">
         <is>
@@ -7797,13 +7797,13 @@
         <v>45038</v>
       </c>
       <c r="G74">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="H74" s="2">
         <v>45221</v>
       </c>
       <c r="I74">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="J74" t="inlineStr">
         <is>
@@ -7895,13 +7895,13 @@
         <v>45117</v>
       </c>
       <c r="G75">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="H75" s="2">
         <v>45301</v>
       </c>
       <c r="I75">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="J75" t="inlineStr">
         <is>
@@ -7998,13 +7998,13 @@
         <v>45160</v>
       </c>
       <c r="G76">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="H76" s="2">
         <v>45344</v>
       </c>
       <c r="I76">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="J76" t="inlineStr">
         <is>
@@ -8101,13 +8101,13 @@
         <v>45186</v>
       </c>
       <c r="G77">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="H77" s="2">
         <v>45368</v>
       </c>
       <c r="I77">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="J77" t="inlineStr">
         <is>
@@ -8204,13 +8204,13 @@
         <v>45043</v>
       </c>
       <c r="G78">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="H78" s="2">
         <v>45226</v>
       </c>
       <c r="I78">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="J78" t="inlineStr">
         <is>
@@ -8307,13 +8307,13 @@
         <v>45079</v>
       </c>
       <c r="G79">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="H79" s="2">
         <v>45262</v>
       </c>
       <c r="I79">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="J79" t="inlineStr">
         <is>
@@ -8410,7 +8410,7 @@
         <v>45254</v>
       </c>
       <c r="I80">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="J80" t="inlineStr">
         <is>
@@ -8507,13 +8507,13 @@
         <v>45104</v>
       </c>
       <c r="G81">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="H81" s="2">
         <v>45287</v>
       </c>
       <c r="I81">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="J81" t="inlineStr">
         <is>
@@ -8610,7 +8610,7 @@
         <v>45288</v>
       </c>
       <c r="I82">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="J82" t="inlineStr">
         <is>
@@ -8702,13 +8702,13 @@
         <v>45175</v>
       </c>
       <c r="G83">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="H83" s="2">
         <v>45357</v>
       </c>
       <c r="I83">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="J83" t="inlineStr">
         <is>
@@ -8805,13 +8805,13 @@
         <v>45054</v>
       </c>
       <c r="G84">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="H84" s="2">
         <v>45238</v>
       </c>
       <c r="I84">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="J84" t="inlineStr">
         <is>
@@ -8908,13 +8908,13 @@
         <v>45056</v>
       </c>
       <c r="G85">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="H85" s="2">
         <v>45240</v>
       </c>
       <c r="I85">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="J85" t="inlineStr">
         <is>
@@ -9011,13 +9011,13 @@
         <v>45085</v>
       </c>
       <c r="G86">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="H86" s="2">
         <v>45268</v>
       </c>
       <c r="I86">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="J86" t="inlineStr">
         <is>
@@ -9114,13 +9114,13 @@
         <v>45194</v>
       </c>
       <c r="G87">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="H87" s="2">
         <v>45560</v>
       </c>
       <c r="I87">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="J87" t="inlineStr">
         <is>
@@ -9207,13 +9207,13 @@
         <v>45103</v>
       </c>
       <c r="G88">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="H88" s="2">
         <v>45286</v>
       </c>
       <c r="I88">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="J88" t="inlineStr">
         <is>
@@ -9310,13 +9310,13 @@
         <v>45103</v>
       </c>
       <c r="G89">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="H89" s="2">
         <v>45286</v>
       </c>
       <c r="I89">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="J89" t="inlineStr">
         <is>
@@ -9413,13 +9413,13 @@
         <v>45192</v>
       </c>
       <c r="G90">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="H90" s="2">
         <v>45374</v>
       </c>
       <c r="I90">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="J90" t="inlineStr">
         <is>
@@ -9511,13 +9511,13 @@
         <v>45100</v>
       </c>
       <c r="G91">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="H91" s="2">
         <v>45287</v>
       </c>
       <c r="I91">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="J91" t="inlineStr">
         <is>
@@ -9614,13 +9614,13 @@
         <v>45187</v>
       </c>
       <c r="G92">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="H92" s="2">
         <v>45369</v>
       </c>
       <c r="I92">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="J92" t="inlineStr">
         <is>
@@ -9717,13 +9717,13 @@
         <v>45104</v>
       </c>
       <c r="G93">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="H93" s="2">
         <v>45287</v>
       </c>
       <c r="I93">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="J93" t="inlineStr">
         <is>
@@ -9820,13 +9820,13 @@
         <v>45104</v>
       </c>
       <c r="G94">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="H94" s="2">
         <v>45287</v>
       </c>
       <c r="I94">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="J94" t="inlineStr">
         <is>
@@ -9923,13 +9923,13 @@
         <v>45049</v>
       </c>
       <c r="G95">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="H95" s="2">
         <v>45233</v>
       </c>
       <c r="I95">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="J95" t="inlineStr">
         <is>
@@ -10026,13 +10026,13 @@
         <v>45122</v>
       </c>
       <c r="G96">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="H96" s="2">
         <v>45306</v>
       </c>
       <c r="I96">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="J96" t="inlineStr">
         <is>
@@ -10124,13 +10124,13 @@
         <v>45141</v>
       </c>
       <c r="G97">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="H97" s="2">
         <v>45325</v>
       </c>
       <c r="I97">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="J97" t="inlineStr">
         <is>
@@ -10227,13 +10227,13 @@
         <v>45194</v>
       </c>
       <c r="G98">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="H98" s="2">
         <v>45376</v>
       </c>
       <c r="I98">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="J98" t="inlineStr">
         <is>
@@ -10325,13 +10325,13 @@
         <v>45093</v>
       </c>
       <c r="G99">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="H99" s="2">
         <v>45276</v>
       </c>
       <c r="I99">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="J99" t="inlineStr">
         <is>
@@ -10428,13 +10428,13 @@
         <v>45123</v>
       </c>
       <c r="G100">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="H100" s="2">
         <v>45307</v>
       </c>
       <c r="I100">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="J100" t="inlineStr">
         <is>
@@ -10531,13 +10531,13 @@
         <v>45198</v>
       </c>
       <c r="G101">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H101" s="2">
         <v>45380</v>
       </c>
       <c r="I101">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="J101" t="inlineStr">
         <is>
@@ -10634,13 +10634,13 @@
         <v>45093</v>
       </c>
       <c r="G102">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="H102" s="2">
         <v>45276</v>
       </c>
       <c r="I102">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="J102" t="inlineStr">
         <is>
@@ -10737,13 +10737,13 @@
         <v>45122</v>
       </c>
       <c r="G103">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="H103" s="2">
         <v>45306</v>
       </c>
       <c r="I103">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="J103" t="inlineStr">
         <is>
@@ -10840,13 +10840,13 @@
         <v>45122</v>
       </c>
       <c r="G104">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="H104" s="2">
         <v>45306</v>
       </c>
       <c r="I104">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="J104" t="inlineStr">
         <is>
@@ -10938,13 +10938,13 @@
         <v>45050</v>
       </c>
       <c r="G105">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="H105" s="2">
         <v>45234</v>
       </c>
       <c r="I105">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="J105" t="inlineStr">
         <is>
@@ -11041,13 +11041,13 @@
         <v>45085</v>
       </c>
       <c r="G106">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="H106" s="2">
         <v>45268</v>
       </c>
       <c r="I106">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="J106" t="inlineStr">
         <is>
@@ -11144,13 +11144,13 @@
         <v>45185</v>
       </c>
       <c r="G107">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="H107" s="2">
         <v>45276</v>
       </c>
       <c r="I107">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="J107" t="inlineStr">
         <is>
@@ -11242,13 +11242,13 @@
         <v>45185</v>
       </c>
       <c r="G108">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="H108" s="2">
         <v>45276</v>
       </c>
       <c r="I108">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="J108" t="inlineStr">
         <is>
@@ -11340,13 +11340,13 @@
         <v>45185</v>
       </c>
       <c r="G109">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="H109" s="2">
         <v>45276</v>
       </c>
       <c r="I109">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="J109" t="inlineStr">
         <is>
@@ -11443,13 +11443,13 @@
         <v>45148</v>
       </c>
       <c r="G110">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="H110" s="2">
         <v>45240</v>
       </c>
       <c r="I110">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="J110" t="inlineStr">
         <is>
@@ -11546,13 +11546,13 @@
         <v>45211</v>
       </c>
       <c r="G111">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H111" s="2">
         <v>45303</v>
       </c>
       <c r="I111">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="J111" t="inlineStr">
         <is>
@@ -11649,13 +11649,13 @@
         <v>45172</v>
       </c>
       <c r="G112">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="H112" s="2">
         <v>45263</v>
       </c>
       <c r="I112">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="J112" t="inlineStr">
         <is>
@@ -11752,13 +11752,13 @@
         <v>45206</v>
       </c>
       <c r="G113">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="H113" s="2">
         <v>45389</v>
       </c>
       <c r="I113">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="J113" t="inlineStr">
         <is>
@@ -11855,13 +11855,13 @@
         <v>45203</v>
       </c>
       <c r="G114">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="H114" s="2">
         <v>45295</v>
       </c>
       <c r="I114">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="J114" t="inlineStr">
         <is>
@@ -11958,7 +11958,7 @@
         <v>45218</v>
       </c>
       <c r="I115">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="J115" t="inlineStr">
         <is>
@@ -12055,13 +12055,13 @@
         <v>45161</v>
       </c>
       <c r="G116">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="H116" s="2">
         <v>45253</v>
       </c>
       <c r="I116">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="J116" t="inlineStr">
         <is>
@@ -12158,13 +12158,13 @@
         <v>45115</v>
       </c>
       <c r="G117">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="H117" s="2">
         <v>45299</v>
       </c>
       <c r="I117">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="J117" t="inlineStr">
         <is>
@@ -12256,13 +12256,13 @@
         <v>45094</v>
       </c>
       <c r="G118">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="H118" s="2">
         <v>45277</v>
       </c>
       <c r="I118">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="J118" t="inlineStr">
         <is>
@@ -12359,13 +12359,13 @@
         <v>45104</v>
       </c>
       <c r="G119">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="H119" s="2">
         <v>45287</v>
       </c>
       <c r="I119">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="J119" t="inlineStr">
         <is>
@@ -12462,13 +12462,13 @@
         <v>45104</v>
       </c>
       <c r="G120">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="H120" s="2">
         <v>45287</v>
       </c>
       <c r="I120">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="J120" t="inlineStr">
         <is>
@@ -12565,13 +12565,13 @@
         <v>45104</v>
       </c>
       <c r="G121">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="H121" s="2">
         <v>45287</v>
       </c>
       <c r="I121">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="J121" t="inlineStr">
         <is>
@@ -12668,13 +12668,13 @@
         <v>45104</v>
       </c>
       <c r="G122">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="H122" s="2">
         <v>45287</v>
       </c>
       <c r="I122">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="J122" t="inlineStr">
         <is>
@@ -12771,13 +12771,13 @@
         <v>45199</v>
       </c>
       <c r="G123">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="H123" s="2">
         <v>45291</v>
       </c>
       <c r="I123">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="J123" t="inlineStr">
         <is>
@@ -12874,13 +12874,13 @@
         <v>45197</v>
       </c>
       <c r="G124">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="H124" s="2">
         <v>45379</v>
       </c>
       <c r="I124">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="J124" t="inlineStr">
         <is>
@@ -12974,16 +12974,16 @@
         </is>
       </c>
       <c r="F125" s="2">
-        <v>45121</v>
+        <v>45213</v>
       </c>
       <c r="G125">
-        <v>92</v>
+        <v>1</v>
       </c>
       <c r="H125" s="2">
         <v>45305</v>
       </c>
       <c r="I125">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="J125" t="inlineStr">
         <is>
@@ -13080,13 +13080,13 @@
         <v>45134</v>
       </c>
       <c r="G126">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="H126" s="2">
         <v>45226</v>
       </c>
       <c r="I126">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="J126" t="inlineStr">
         <is>
@@ -13183,13 +13183,13 @@
         <v>45212</v>
       </c>
       <c r="G127">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H127" s="2">
         <v>45304</v>
       </c>
       <c r="I127">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="J127" t="inlineStr">
         <is>
@@ -13286,13 +13286,13 @@
         <v>45126</v>
       </c>
       <c r="G128">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="H128" s="2">
         <v>45218</v>
       </c>
       <c r="I128">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="J128" t="inlineStr">
         <is>
@@ -13384,13 +13384,13 @@
         <v>45158</v>
       </c>
       <c r="G129">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="H129" s="2">
         <v>45250</v>
       </c>
       <c r="I129">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="J129" t="inlineStr">
         <is>
@@ -13487,13 +13487,13 @@
         <v>45171</v>
       </c>
       <c r="G130">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="H130" s="2">
         <v>45262</v>
       </c>
       <c r="I130">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="J130" t="inlineStr">
         <is>
@@ -13590,13 +13590,13 @@
         <v>45203</v>
       </c>
       <c r="G131">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="H131" s="2">
         <v>45295</v>
       </c>
       <c r="I131">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="J131" t="inlineStr">
         <is>
@@ -13693,13 +13693,13 @@
         <v>45144</v>
       </c>
       <c r="G132">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="H132" s="2">
         <v>45236</v>
       </c>
       <c r="I132">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="J132" t="inlineStr">
         <is>
@@ -13796,13 +13796,13 @@
         <v>45156</v>
       </c>
       <c r="G133">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="H133" s="2">
         <v>45248</v>
       </c>
       <c r="I133">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="J133" t="inlineStr">
         <is>
@@ -13894,13 +13894,13 @@
         <v>45146</v>
       </c>
       <c r="G134">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="H134" s="2">
         <v>45238</v>
       </c>
       <c r="I134">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="J134" t="inlineStr">
         <is>
@@ -13997,13 +13997,13 @@
         <v>45140</v>
       </c>
       <c r="G135">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="H135" s="2">
         <v>45232</v>
       </c>
       <c r="I135">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="J135" t="inlineStr">
         <is>
@@ -14100,13 +14100,13 @@
         <v>45196</v>
       </c>
       <c r="G136">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="H136" s="2">
         <v>45287</v>
       </c>
       <c r="I136">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="J136" t="inlineStr">
         <is>
@@ -14203,13 +14203,13 @@
         <v>45197</v>
       </c>
       <c r="G137">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="H137" s="2">
         <v>45288</v>
       </c>
       <c r="I137">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="J137" t="inlineStr">
         <is>
@@ -14306,13 +14306,13 @@
         <v>45179</v>
       </c>
       <c r="G138">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="H138" s="2">
         <v>45270</v>
       </c>
       <c r="I138">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="J138" t="inlineStr">
         <is>
@@ -14404,13 +14404,13 @@
         <v>45197</v>
       </c>
       <c r="G139">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="H139" s="2">
         <v>45288</v>
       </c>
       <c r="I139">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="J139" t="inlineStr">
         <is>
@@ -14507,13 +14507,13 @@
         <v>45182</v>
       </c>
       <c r="G140">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="H140" s="2">
         <v>45273</v>
       </c>
       <c r="I140">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="J140" t="inlineStr">
         <is>
@@ -14610,13 +14610,13 @@
         <v>45208</v>
       </c>
       <c r="G141">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="H141" s="2">
         <v>45300</v>
       </c>
       <c r="I141">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="J141" t="inlineStr">
         <is>
@@ -14708,13 +14708,13 @@
         <v>45150</v>
       </c>
       <c r="G142">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="H142" s="2">
         <v>45242</v>
       </c>
       <c r="I142">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="J142" t="inlineStr">
         <is>
@@ -14811,7 +14811,7 @@
         <v>45238</v>
       </c>
       <c r="I143">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="J143" t="inlineStr">
         <is>
@@ -14908,13 +14908,13 @@
         <v>45171</v>
       </c>
       <c r="G144">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="H144" s="2">
         <v>45262</v>
       </c>
       <c r="I144">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="J144" t="inlineStr">
         <is>
@@ -15011,13 +15011,13 @@
         <v>45194</v>
       </c>
       <c r="G145">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="H145" s="2">
         <v>45285</v>
       </c>
       <c r="I145">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="J145" t="inlineStr">
         <is>
@@ -15104,7 +15104,7 @@
         <v>45211</v>
       </c>
       <c r="G146">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="J146" t="inlineStr">
         <is>
@@ -15201,13 +15201,13 @@
         <v>45165</v>
       </c>
       <c r="G147">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="H147" s="2">
         <v>45257</v>
       </c>
       <c r="I147">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="J147" t="inlineStr">
         <is>
@@ -15304,13 +15304,13 @@
         <v>45166</v>
       </c>
       <c r="G148">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="H148" s="2">
         <v>45258</v>
       </c>
       <c r="I148">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="J148" t="inlineStr">
         <is>
@@ -15407,13 +15407,13 @@
         <v>45185</v>
       </c>
       <c r="G149">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="H149" s="2">
         <v>45276</v>
       </c>
       <c r="I149">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="J149" t="inlineStr">
         <is>
@@ -15510,13 +15510,13 @@
         <v>45035</v>
       </c>
       <c r="G150">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="H150" s="2">
         <v>45218</v>
       </c>
       <c r="I150">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="J150" t="inlineStr">
         <is>
@@ -15613,13 +15613,13 @@
         <v>45174</v>
       </c>
       <c r="G151">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="H151" s="2">
         <v>45356</v>
       </c>
       <c r="I151">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="J151" t="inlineStr">
         <is>
@@ -15716,13 +15716,13 @@
         <v>45089</v>
       </c>
       <c r="G152">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="H152" s="2">
         <v>45272</v>
       </c>
       <c r="I152">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="J152" t="inlineStr">
         <is>
@@ -15819,13 +15819,13 @@
         <v>45124</v>
       </c>
       <c r="G153">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="H153" s="2">
         <v>45308</v>
       </c>
       <c r="I153">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="J153" t="inlineStr">
         <is>
@@ -15922,13 +15922,13 @@
         <v>45124</v>
       </c>
       <c r="G154">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="H154" s="2">
         <v>45308</v>
       </c>
       <c r="I154">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="J154" t="inlineStr">
         <is>
@@ -16025,13 +16025,13 @@
         <v>45209</v>
       </c>
       <c r="G155">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="H155" s="2">
         <v>45392</v>
       </c>
       <c r="I155">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="J155" t="inlineStr">
         <is>
@@ -16128,13 +16128,13 @@
         <v>45209</v>
       </c>
       <c r="G156">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="H156" s="2">
         <v>45392</v>
       </c>
       <c r="I156">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="J156" t="inlineStr">
         <is>
@@ -16231,13 +16231,13 @@
         <v>45209</v>
       </c>
       <c r="G157">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="H157" s="2">
         <v>45392</v>
       </c>
       <c r="I157">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="J157" t="inlineStr">
         <is>
@@ -16334,13 +16334,13 @@
         <v>45209</v>
       </c>
       <c r="G158">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="H158" s="2">
         <v>45392</v>
       </c>
       <c r="I158">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="J158" t="inlineStr">
         <is>
@@ -16437,13 +16437,13 @@
         <v>45156</v>
       </c>
       <c r="G159">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="H159" s="2">
         <v>45247</v>
       </c>
       <c r="I159">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="J159" t="inlineStr">
         <is>
@@ -16540,13 +16540,13 @@
         <v>45153</v>
       </c>
       <c r="G160">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="H160" s="2">
         <v>45245</v>
       </c>
       <c r="I160">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="J160" t="inlineStr">
         <is>
@@ -16643,13 +16643,13 @@
         <v>45135</v>
       </c>
       <c r="G161">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="H161" s="2">
         <v>45319</v>
       </c>
       <c r="I161">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="J161" t="inlineStr">
         <is>
@@ -16746,13 +16746,13 @@
         <v>45091</v>
       </c>
       <c r="G162">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="H162" s="2">
         <v>45274</v>
       </c>
       <c r="I162">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="J162" t="inlineStr">
         <is>
@@ -16844,13 +16844,13 @@
         <v>45091</v>
       </c>
       <c r="G163">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="H163" s="2">
         <v>45274</v>
       </c>
       <c r="I163">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="J163" t="inlineStr">
         <is>
@@ -16942,13 +16942,13 @@
         <v>45138</v>
       </c>
       <c r="G164">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="H164" s="2">
         <v>45322</v>
       </c>
       <c r="I164">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="J164" t="inlineStr">
         <is>
@@ -17045,13 +17045,13 @@
         <v>45138</v>
       </c>
       <c r="G165">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="H165" s="2">
         <v>45322</v>
       </c>
       <c r="I165">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="J165" t="inlineStr">
         <is>
@@ -17148,13 +17148,13 @@
         <v>45085</v>
       </c>
       <c r="G166">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="H166" s="2">
         <v>45268</v>
       </c>
       <c r="I166">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="J166" t="inlineStr">
         <is>
@@ -17251,13 +17251,13 @@
         <v>45085</v>
       </c>
       <c r="G167">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="H167" s="2">
         <v>45268</v>
       </c>
       <c r="I167">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="J167" t="inlineStr">
         <is>
@@ -17354,7 +17354,7 @@
         <v>45326</v>
       </c>
       <c r="I168">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="J168" t="inlineStr">
         <is>
@@ -17451,13 +17451,13 @@
         <v>45173</v>
       </c>
       <c r="G169">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="H169" s="2">
         <v>45355</v>
       </c>
       <c r="I169">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="J169" t="inlineStr">
         <is>
@@ -17554,13 +17554,13 @@
         <v>45056</v>
       </c>
       <c r="G170">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="H170" s="2">
         <v>45240</v>
       </c>
       <c r="I170">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="J170" t="inlineStr">
         <is>
@@ -17657,7 +17657,7 @@
         <v>45238</v>
       </c>
       <c r="I171">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="J171" t="inlineStr">
         <is>
@@ -17754,13 +17754,13 @@
         <v>45141</v>
       </c>
       <c r="G172">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="H172" s="2">
         <v>45325</v>
       </c>
       <c r="I172">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="J172" t="inlineStr">
         <is>
@@ -17857,13 +17857,13 @@
         <v>45037</v>
       </c>
       <c r="G173">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="H173" s="2">
         <v>45220</v>
       </c>
       <c r="I173">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="J173" t="inlineStr">
         <is>
@@ -17960,13 +17960,13 @@
         <v>45171</v>
       </c>
       <c r="G174">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="H174" s="2">
         <v>45262</v>
       </c>
       <c r="I174">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="J174" t="inlineStr">
         <is>
@@ -18063,13 +18063,13 @@
         <v>45197</v>
       </c>
       <c r="G175">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="H175" s="2">
         <v>45288</v>
       </c>
       <c r="I175">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="J175" t="inlineStr">
         <is>
@@ -18166,13 +18166,13 @@
         <v>45162</v>
       </c>
       <c r="G176">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="H176" s="2">
         <v>45254</v>
       </c>
       <c r="I176">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="J176" t="inlineStr">
         <is>
@@ -18269,13 +18269,13 @@
         <v>45061</v>
       </c>
       <c r="G177">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="H177" s="2">
         <v>45245</v>
       </c>
       <c r="I177">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="J177" t="inlineStr">
         <is>
@@ -18372,13 +18372,13 @@
         <v>45212</v>
       </c>
       <c r="G178">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H178" s="2">
         <v>45304</v>
       </c>
       <c r="I178">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="J178" t="inlineStr">
         <is>
@@ -18475,13 +18475,13 @@
         <v>45191</v>
       </c>
       <c r="G179">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="H179" s="2">
         <v>45282</v>
       </c>
       <c r="I179">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="J179" t="inlineStr">
         <is>
@@ -18578,13 +18578,13 @@
         <v>45088</v>
       </c>
       <c r="G180">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="H180" s="2">
         <v>45271</v>
       </c>
       <c r="I180">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="J180" t="inlineStr">
         <is>
@@ -18681,13 +18681,13 @@
         <v>45192</v>
       </c>
       <c r="G181">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="H181" s="2">
         <v>45283</v>
       </c>
       <c r="I181">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="J181" t="inlineStr">
         <is>
@@ -18774,13 +18774,13 @@
         <v>45131</v>
       </c>
       <c r="G182">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="H182" s="2">
         <v>45223</v>
       </c>
       <c r="I182">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="J182" t="inlineStr">
         <is>
@@ -18872,13 +18872,13 @@
         <v>45136</v>
       </c>
       <c r="G183">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="H183" s="2">
         <v>45228</v>
       </c>
       <c r="I183">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="J183" t="inlineStr">
         <is>
@@ -18970,13 +18970,13 @@
         <v>45150</v>
       </c>
       <c r="G184">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="H184" s="2">
         <v>45242</v>
       </c>
       <c r="I184">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="J184" t="inlineStr">
         <is>
@@ -19068,7 +19068,7 @@
         <v>45210</v>
       </c>
       <c r="G185">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="J185" t="inlineStr">
         <is>
@@ -19160,13 +19160,13 @@
         <v>45129</v>
       </c>
       <c r="G186">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="H186" s="2">
         <v>45221</v>
       </c>
       <c r="I186">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="J186" t="inlineStr">
         <is>
@@ -19258,13 +19258,13 @@
         <v>45189</v>
       </c>
       <c r="G187">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="H187" s="2">
         <v>45280</v>
       </c>
       <c r="I187">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="J187" t="inlineStr">
         <is>
@@ -19351,13 +19351,13 @@
         <v>45193</v>
       </c>
       <c r="G188">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="H188" s="2">
         <v>45284</v>
       </c>
       <c r="I188">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="J188" t="inlineStr">
         <is>
@@ -19444,13 +19444,13 @@
         <v>45165</v>
       </c>
       <c r="G189">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="H189" s="2">
         <v>45257</v>
       </c>
       <c r="I189">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="J189" t="inlineStr">
         <is>
@@ -19542,13 +19542,13 @@
         <v>45202</v>
       </c>
       <c r="G190">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="H190" s="2">
         <v>45385</v>
       </c>
       <c r="I190">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="J190" t="inlineStr">
         <is>
@@ -19645,13 +19645,13 @@
         <v>45081</v>
       </c>
       <c r="G191">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="H191" s="2">
         <v>45264</v>
       </c>
       <c r="I191">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="J191" t="inlineStr">
         <is>
@@ -19748,13 +19748,13 @@
         <v>45081</v>
       </c>
       <c r="G192">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="H192" s="2">
         <v>45264</v>
       </c>
       <c r="I192">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="J192" t="inlineStr">
         <is>
@@ -19851,7 +19851,7 @@
         <v>45319</v>
       </c>
       <c r="I193">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="J193" t="inlineStr">
         <is>
@@ -19948,7 +19948,7 @@
         <v>45319</v>
       </c>
       <c r="I194">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="J194" t="inlineStr">
         <is>
@@ -20040,13 +20040,13 @@
         <v>45046</v>
       </c>
       <c r="G195">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="H195" s="2">
         <v>45230</v>
       </c>
       <c r="I195">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="J195" t="inlineStr">
         <is>
@@ -20143,13 +20143,13 @@
         <v>45046</v>
       </c>
       <c r="G196">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="H196" s="2">
         <v>45230</v>
       </c>
       <c r="I196">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="J196" t="inlineStr">
         <is>
@@ -20246,13 +20246,13 @@
         <v>45031</v>
       </c>
       <c r="G197">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="H197" s="2">
-        <v>45214</v>
+        <v>45397</v>
       </c>
       <c r="I197">
-        <v>1</v>
+        <v>183</v>
       </c>
       <c r="J197" t="inlineStr">
         <is>
@@ -20349,13 +20349,13 @@
         <v>45031</v>
       </c>
       <c r="G198">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="H198" s="2">
-        <v>45214</v>
+        <v>45397</v>
       </c>
       <c r="I198">
-        <v>1</v>
+        <v>183</v>
       </c>
       <c r="J198" t="inlineStr">
         <is>
@@ -20452,13 +20452,13 @@
         <v>45031</v>
       </c>
       <c r="G199">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="H199" s="2">
-        <v>45214</v>
+        <v>45397</v>
       </c>
       <c r="I199">
-        <v>1</v>
+        <v>183</v>
       </c>
       <c r="J199" t="inlineStr">
         <is>
@@ -20555,13 +20555,13 @@
         <v>45031</v>
       </c>
       <c r="G200">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="H200" s="2">
-        <v>45214</v>
+        <v>45397</v>
       </c>
       <c r="I200">
-        <v>1</v>
+        <v>183</v>
       </c>
       <c r="J200" t="inlineStr">
         <is>
@@ -20658,13 +20658,13 @@
         <v>45067</v>
       </c>
       <c r="G201">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="H201" s="2">
         <v>45251</v>
       </c>
       <c r="I201">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="J201" t="inlineStr">
         <is>
@@ -20761,13 +20761,13 @@
         <v>45067</v>
       </c>
       <c r="G202">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="H202" s="2">
         <v>45251</v>
       </c>
       <c r="I202">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="J202" t="inlineStr">
         <is>
@@ -20864,13 +20864,13 @@
         <v>45067</v>
       </c>
       <c r="G203">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="H203" s="2">
         <v>45251</v>
       </c>
       <c r="I203">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="J203" t="inlineStr">
         <is>
@@ -20967,13 +20967,13 @@
         <v>45067</v>
       </c>
       <c r="G204">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="H204" s="2">
         <v>45251</v>
       </c>
       <c r="I204">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="J204" t="inlineStr">
         <is>
@@ -21070,13 +21070,13 @@
         <v>45178</v>
       </c>
       <c r="G205">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="H205" s="2">
         <v>45269</v>
       </c>
       <c r="I205">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="J205" t="inlineStr">
         <is>
@@ -21173,7 +21173,7 @@
         <v>45252</v>
       </c>
       <c r="I206">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="J206" t="inlineStr">
         <is>
@@ -21270,13 +21270,13 @@
         <v>45087</v>
       </c>
       <c r="G207">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="H207" s="2">
         <v>45270</v>
       </c>
       <c r="I207">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="J207" t="inlineStr">
         <is>
@@ -21373,13 +21373,13 @@
         <v>45099</v>
       </c>
       <c r="G208">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="H208" s="2">
         <v>45282</v>
       </c>
       <c r="I208">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="J208" t="inlineStr">
         <is>
@@ -21476,13 +21476,13 @@
         <v>45175</v>
       </c>
       <c r="G209">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="H209" s="2">
         <v>45356</v>
       </c>
       <c r="I209">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="J209" t="inlineStr">
         <is>
@@ -21579,13 +21579,13 @@
         <v>45175</v>
       </c>
       <c r="G210">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="H210" s="2">
         <v>45356</v>
       </c>
       <c r="I210">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="J210" t="inlineStr">
         <is>
@@ -21682,13 +21682,13 @@
         <v>45166</v>
       </c>
       <c r="G211">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="H211" s="2">
         <v>45350</v>
       </c>
       <c r="I211">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="J211" t="inlineStr">
         <is>
@@ -21785,13 +21785,13 @@
         <v>45166</v>
       </c>
       <c r="G212">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="H212" s="2">
         <v>45350</v>
       </c>
       <c r="I212">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="J212" t="inlineStr">
         <is>
@@ -21888,13 +21888,13 @@
         <v>45090</v>
       </c>
       <c r="G213">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="H213" s="2">
         <v>45273</v>
       </c>
       <c r="I213">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="J213" t="inlineStr">
         <is>
@@ -21991,13 +21991,13 @@
         <v>45106</v>
       </c>
       <c r="G214">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="H214" s="2">
         <v>45289</v>
       </c>
       <c r="I214">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="J214" t="inlineStr">
         <is>
@@ -22094,13 +22094,13 @@
         <v>45134</v>
       </c>
       <c r="G215">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="H215" s="2">
         <v>45226</v>
       </c>
       <c r="I215">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="J215" t="inlineStr">
         <is>
@@ -22197,13 +22197,13 @@
         <v>45132</v>
       </c>
       <c r="G216">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="H216" s="2">
         <v>45224</v>
       </c>
       <c r="I216">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="J216" t="inlineStr">
         <is>
@@ -22300,13 +22300,13 @@
         <v>45150</v>
       </c>
       <c r="G217">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="H217" s="2">
         <v>45242</v>
       </c>
       <c r="I217">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="J217" t="inlineStr">
         <is>
@@ -22403,13 +22403,13 @@
         <v>45187</v>
       </c>
       <c r="G218">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="H218" s="2">
         <v>45278</v>
       </c>
       <c r="I218">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="J218" t="inlineStr">
         <is>
@@ -22501,13 +22501,13 @@
         <v>45182</v>
       </c>
       <c r="G219">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="H219" s="2">
         <v>45273</v>
       </c>
       <c r="I219">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="J219" t="inlineStr">
         <is>
@@ -22604,13 +22604,13 @@
         <v>45196</v>
       </c>
       <c r="G220">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="H220" s="2">
         <v>45287</v>
       </c>
       <c r="I220">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="J220" t="inlineStr">
         <is>
@@ -22707,13 +22707,13 @@
         <v>45200</v>
       </c>
       <c r="G221">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="H221" s="2">
         <v>45292</v>
       </c>
       <c r="I221">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="J221" t="inlineStr">
         <is>
@@ -22810,13 +22810,13 @@
         <v>45135</v>
       </c>
       <c r="G222">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="H222" s="2">
         <v>45227</v>
       </c>
       <c r="I222">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="J222" t="inlineStr">
         <is>
@@ -22913,13 +22913,13 @@
         <v>45148</v>
       </c>
       <c r="G223">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="H223" s="2">
         <v>45240</v>
       </c>
       <c r="I223">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="J223" t="inlineStr">
         <is>
@@ -23011,13 +23011,13 @@
         <v>45192</v>
       </c>
       <c r="G224">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="H224" s="2">
         <v>45283</v>
       </c>
       <c r="I224">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="J224" t="inlineStr">
         <is>
@@ -23109,13 +23109,13 @@
         <v>45136</v>
       </c>
       <c r="G225">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="H225" s="2">
         <v>45320</v>
       </c>
       <c r="I225">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="J225" t="inlineStr">
         <is>
@@ -23212,13 +23212,13 @@
         <v>45136</v>
       </c>
       <c r="G226">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="H226" s="2">
         <v>45320</v>
       </c>
       <c r="I226">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="J226" t="inlineStr">
         <is>
@@ -23315,13 +23315,13 @@
         <v>45094</v>
       </c>
       <c r="G227">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="H227" s="2">
         <v>45277</v>
       </c>
       <c r="I227">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="J227" t="inlineStr">
         <is>
@@ -23418,13 +23418,13 @@
         <v>45081</v>
       </c>
       <c r="G228">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="H228" s="2">
         <v>45264</v>
       </c>
       <c r="I228">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="J228" t="inlineStr">
         <is>
@@ -23521,13 +23521,13 @@
         <v>45099</v>
       </c>
       <c r="G229">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="H229" s="2">
         <v>45282</v>
       </c>
       <c r="I229">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="J229" t="inlineStr">
         <is>
@@ -23624,13 +23624,13 @@
         <v>45201</v>
       </c>
       <c r="G230">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="H230" s="2">
         <v>45384</v>
       </c>
       <c r="I230">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="J230" t="inlineStr">
         <is>
@@ -23727,13 +23727,13 @@
         <v>45031</v>
       </c>
       <c r="G231">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="H231" s="2">
-        <v>45214</v>
+        <v>45397</v>
       </c>
       <c r="I231">
-        <v>1</v>
+        <v>183</v>
       </c>
       <c r="J231" t="inlineStr">
         <is>
@@ -23830,7 +23830,7 @@
         <v>45294</v>
       </c>
       <c r="I232">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="J232" t="inlineStr">
         <is>
@@ -23927,13 +23927,13 @@
         <v>45079</v>
       </c>
       <c r="G233">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="H233" s="2">
         <v>45262</v>
       </c>
       <c r="I233">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="J233" t="inlineStr">
         <is>
@@ -24030,13 +24030,13 @@
         <v>45199</v>
       </c>
       <c r="G234">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="H234" s="2">
         <v>45382</v>
       </c>
       <c r="I234">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="J234" t="inlineStr">
         <is>
@@ -24133,13 +24133,13 @@
         <v>45204</v>
       </c>
       <c r="G235">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="H235" s="2">
         <v>45387</v>
       </c>
       <c r="I235">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="J235" t="inlineStr">
         <is>
@@ -24236,13 +24236,13 @@
         <v>45204</v>
       </c>
       <c r="G236">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="H236" s="2">
         <v>45387</v>
       </c>
       <c r="I236">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="J236" t="inlineStr">
         <is>
@@ -24339,13 +24339,13 @@
         <v>45080</v>
       </c>
       <c r="G237">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="H237" s="2">
         <v>45263</v>
       </c>
       <c r="I237">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="J237" t="inlineStr">
         <is>
@@ -24442,13 +24442,13 @@
         <v>45046</v>
       </c>
       <c r="G238">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="H238" s="2">
         <v>45229</v>
       </c>
       <c r="I238">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="J238" t="inlineStr">
         <is>
@@ -24545,13 +24545,13 @@
         <v>45204</v>
       </c>
       <c r="G239">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="H239" s="2">
         <v>45296</v>
       </c>
       <c r="I239">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="J239" t="inlineStr">
         <is>
@@ -24648,13 +24648,13 @@
         <v>45204</v>
       </c>
       <c r="G240">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="H240" s="2">
         <v>45296</v>
       </c>
       <c r="I240">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="J240" t="inlineStr">
         <is>
@@ -24751,13 +24751,13 @@
         <v>45199</v>
       </c>
       <c r="G241">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="H241" s="2">
         <v>45382</v>
       </c>
       <c r="I241">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="J241" t="inlineStr">
         <is>
@@ -24854,13 +24854,13 @@
         <v>45070</v>
       </c>
       <c r="G242">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="H242" s="2">
         <v>45254</v>
       </c>
       <c r="I242">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="J242" t="inlineStr">
         <is>
@@ -24957,13 +24957,13 @@
         <v>45168</v>
       </c>
       <c r="G243">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="H243" s="2">
         <v>45260</v>
       </c>
       <c r="I243">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="J243" t="inlineStr">
         <is>
@@ -25060,13 +25060,13 @@
         <v>45210</v>
       </c>
       <c r="G244">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="H244" s="2">
         <v>45393</v>
       </c>
       <c r="I244">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="J244" t="inlineStr">
         <is>
@@ -25163,13 +25163,13 @@
         <v>45077</v>
       </c>
       <c r="G245">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="H245" s="2">
         <v>45260</v>
       </c>
       <c r="I245">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="J245" t="inlineStr">
         <is>
@@ -25266,13 +25266,13 @@
         <v>45100</v>
       </c>
       <c r="G246">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="H246" s="2">
         <v>45283</v>
       </c>
       <c r="I246">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="J246" t="inlineStr">
         <is>
@@ -25369,7 +25369,7 @@
         <v>45281</v>
       </c>
       <c r="I247">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="J247" t="inlineStr">
         <is>
@@ -25466,13 +25466,13 @@
         <v>45044</v>
       </c>
       <c r="G248">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="H248" s="2">
         <v>45227</v>
       </c>
       <c r="I248">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="J248" t="inlineStr">
         <is>
@@ -25569,13 +25569,13 @@
         <v>45101</v>
       </c>
       <c r="G249">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="H249" s="2">
         <v>45283</v>
       </c>
       <c r="I249">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="J249" t="inlineStr">
         <is>
@@ -25672,13 +25672,13 @@
         <v>45134</v>
       </c>
       <c r="G250">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="H250" s="2">
         <v>45226</v>
       </c>
       <c r="I250">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="J250" t="inlineStr">
         <is>
@@ -25775,13 +25775,13 @@
         <v>45158</v>
       </c>
       <c r="G251">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="H251" s="2">
         <v>45250</v>
       </c>
       <c r="I251">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="J251" t="inlineStr">
         <is>
@@ -25878,13 +25878,13 @@
         <v>45200</v>
       </c>
       <c r="G252">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="H252" s="2">
         <v>45292</v>
       </c>
       <c r="I252">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="J252" t="inlineStr">
         <is>
@@ -25981,7 +25981,7 @@
         <v>45317</v>
       </c>
       <c r="I253">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="J253" t="inlineStr">
         <is>
@@ -26078,13 +26078,13 @@
         <v>45039</v>
       </c>
       <c r="G254">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="H254" s="2">
         <v>45222</v>
       </c>
       <c r="I254">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="J254" t="inlineStr">
         <is>
@@ -26176,13 +26176,13 @@
         <v>45129</v>
       </c>
       <c r="G255">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="H255" s="2">
         <v>45221</v>
       </c>
       <c r="I255">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="J255" t="inlineStr">
         <is>
@@ -26279,13 +26279,13 @@
         <v>45157</v>
       </c>
       <c r="G256">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="H256" s="2">
         <v>45341</v>
       </c>
       <c r="I256">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="J256" t="inlineStr">
         <is>
@@ -26382,13 +26382,13 @@
         <v>45063</v>
       </c>
       <c r="G257">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="H257" s="2">
         <v>45247</v>
       </c>
       <c r="I257">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="J257" t="inlineStr">
         <is>
@@ -26485,7 +26485,7 @@
         <v>45254</v>
       </c>
       <c r="I258">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="J258" t="inlineStr">
         <is>
@@ -26582,7 +26582,7 @@
         <v>45486</v>
       </c>
       <c r="I259">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="J259" t="inlineStr">
         <is>
@@ -26674,13 +26674,13 @@
         <v>45073</v>
       </c>
       <c r="G260">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="H260" s="2">
         <v>45439</v>
       </c>
       <c r="I260">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="J260" t="inlineStr">
         <is>
@@ -26772,7 +26772,7 @@
         <v>45323</v>
       </c>
       <c r="I261">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="J261" t="inlineStr">
         <is>
@@ -26864,7 +26864,7 @@
         <v>45303</v>
       </c>
       <c r="I262">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="J262" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
Bond dates update Mon Oct 16 23:15:57 UTC 2023
</commit_message>
<xml_diff>
--- a/Data/obligacje_screener.xlsx
+++ b/Data/obligacje_screener.xlsx
@@ -512,7 +512,7 @@
         <v>45340</v>
       </c>
       <c r="I2">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="J2" t="inlineStr">
         <is>
@@ -600,13 +600,13 @@
         <v>45121</v>
       </c>
       <c r="G3">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="H3" s="2">
         <v>45305</v>
       </c>
       <c r="I3">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="J3" t="inlineStr">
         <is>
@@ -703,13 +703,13 @@
         <v>45039</v>
       </c>
       <c r="G4">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="H4" s="2">
         <v>45222</v>
       </c>
       <c r="I4">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="J4" t="inlineStr">
         <is>
@@ -806,13 +806,13 @@
         <v>45039</v>
       </c>
       <c r="G5">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="H5" s="2">
         <v>45222</v>
       </c>
       <c r="I5">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="J5" t="inlineStr">
         <is>
@@ -909,13 +909,13 @@
         <v>45129</v>
       </c>
       <c r="G6">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="H6" s="2">
         <v>45221</v>
       </c>
       <c r="I6">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="J6" t="inlineStr">
         <is>
@@ -1012,13 +1012,13 @@
         <v>45162</v>
       </c>
       <c r="G7">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="H7" s="2">
         <v>45254</v>
       </c>
       <c r="I7">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="J7" t="inlineStr">
         <is>
@@ -1110,13 +1110,13 @@
         <v>45156</v>
       </c>
       <c r="G8">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="H8" s="2">
         <v>45248</v>
       </c>
       <c r="I8">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="J8" t="inlineStr">
         <is>
@@ -1213,13 +1213,13 @@
         <v>45141</v>
       </c>
       <c r="G9">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="H9" s="2">
         <v>45233</v>
       </c>
       <c r="I9">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="J9" t="inlineStr">
         <is>
@@ -1316,13 +1316,13 @@
         <v>45062</v>
       </c>
       <c r="G10">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="H10" s="2">
         <v>45246</v>
       </c>
       <c r="I10">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="J10" t="inlineStr">
         <is>
@@ -1419,7 +1419,7 @@
         <v>45286</v>
       </c>
       <c r="I11">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="J11" t="inlineStr">
         <is>
@@ -1516,13 +1516,13 @@
         <v>45195</v>
       </c>
       <c r="G12">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="H12" s="2">
         <v>45377</v>
       </c>
       <c r="I12">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="J12" t="inlineStr">
         <is>
@@ -1614,13 +1614,13 @@
         <v>45036</v>
       </c>
       <c r="G13">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="H13" s="2">
         <v>45219</v>
       </c>
       <c r="I13">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="J13" t="inlineStr">
         <is>
@@ -1717,13 +1717,13 @@
         <v>45036</v>
       </c>
       <c r="G14">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="H14" s="2">
         <v>45219</v>
       </c>
       <c r="I14">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="J14" t="inlineStr">
         <is>
@@ -1820,13 +1820,13 @@
         <v>45106</v>
       </c>
       <c r="G15">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="H15" s="2">
         <v>45289</v>
       </c>
       <c r="I15">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="J15" t="inlineStr">
         <is>
@@ -1923,13 +1923,13 @@
         <v>45186</v>
       </c>
       <c r="G16">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="H16" s="2">
         <v>45278</v>
       </c>
       <c r="I16">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="J16" t="inlineStr">
         <is>
@@ -2026,13 +2026,13 @@
         <v>45186</v>
       </c>
       <c r="G17">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="H17" s="2">
         <v>45277</v>
       </c>
       <c r="I17">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="J17" t="inlineStr">
         <is>
@@ -2129,13 +2129,13 @@
         <v>45132</v>
       </c>
       <c r="G18">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="H18" s="2">
         <v>45224</v>
       </c>
       <c r="I18">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="J18" t="inlineStr">
         <is>
@@ -2232,13 +2232,13 @@
         <v>45137</v>
       </c>
       <c r="G19">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="H19" s="2">
         <v>45229</v>
       </c>
       <c r="I19">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="J19" t="inlineStr">
         <is>
@@ -2330,13 +2330,13 @@
         <v>45183</v>
       </c>
       <c r="G20">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="H20" s="2">
         <v>45274</v>
       </c>
       <c r="I20">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="J20" t="inlineStr">
         <is>
@@ -2433,13 +2433,13 @@
         <v>45187</v>
       </c>
       <c r="G21">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="H21" s="2">
         <v>45278</v>
       </c>
       <c r="I21">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="J21" t="inlineStr">
         <is>
@@ -2536,13 +2536,13 @@
         <v>45187</v>
       </c>
       <c r="G22">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="H22" s="2">
         <v>45278</v>
       </c>
       <c r="I22">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="J22" t="inlineStr">
         <is>
@@ -2639,7 +2639,7 @@
         <v>45245</v>
       </c>
       <c r="I23">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="J23" t="inlineStr">
         <is>
@@ -2736,7 +2736,7 @@
         <v>45245</v>
       </c>
       <c r="I24">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="J24" t="inlineStr">
         <is>
@@ -2833,7 +2833,7 @@
         <v>45204</v>
       </c>
       <c r="G25">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="J25" t="inlineStr">
         <is>
@@ -2930,13 +2930,13 @@
         <v>45160</v>
       </c>
       <c r="G26">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="H26" s="2">
         <v>45344</v>
       </c>
       <c r="I26">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="J26" t="inlineStr">
         <is>
@@ -3033,13 +3033,13 @@
         <v>45118</v>
       </c>
       <c r="G27">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="H27" s="2">
         <v>45302</v>
       </c>
       <c r="I27">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="J27" t="inlineStr">
         <is>
@@ -3136,13 +3136,13 @@
         <v>45085</v>
       </c>
       <c r="G28">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="H28" s="2">
         <v>45268</v>
       </c>
       <c r="I28">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="J28" t="inlineStr">
         <is>
@@ -3239,13 +3239,13 @@
         <v>45183</v>
       </c>
       <c r="G29">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="H29" s="2">
         <v>45274</v>
       </c>
       <c r="I29">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="J29" t="inlineStr">
         <is>
@@ -3342,7 +3342,7 @@
         <v>45224</v>
       </c>
       <c r="I30">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="J30" t="inlineStr">
         <is>
@@ -3439,13 +3439,13 @@
         <v>45153</v>
       </c>
       <c r="G31">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="H31" s="2">
         <v>45245</v>
       </c>
       <c r="I31">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="J31" t="inlineStr">
         <is>
@@ -3542,13 +3542,13 @@
         <v>45155</v>
       </c>
       <c r="G32">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="H32" s="2">
         <v>45247</v>
       </c>
       <c r="I32">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="J32" t="inlineStr">
         <is>
@@ -3645,7 +3645,7 @@
         <v>45255</v>
       </c>
       <c r="I33">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="J33" t="inlineStr">
         <is>
@@ -3742,13 +3742,13 @@
         <v>45176</v>
       </c>
       <c r="G34">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="H34" s="2">
         <v>45267</v>
       </c>
       <c r="I34">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="J34" t="inlineStr">
         <is>
@@ -3845,13 +3845,13 @@
         <v>45130</v>
       </c>
       <c r="G35">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="H35" s="2">
         <v>45222</v>
       </c>
       <c r="I35">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="J35" t="inlineStr">
         <is>
@@ -3943,13 +3943,13 @@
         <v>45207</v>
       </c>
       <c r="G36">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="H36" s="2">
         <v>45299</v>
       </c>
       <c r="I36">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="J36" t="inlineStr">
         <is>
@@ -4046,13 +4046,13 @@
         <v>45189</v>
       </c>
       <c r="G37">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="H37" s="2">
         <v>45280</v>
       </c>
       <c r="I37">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="J37" t="inlineStr">
         <is>
@@ -4144,13 +4144,13 @@
         <v>45107</v>
       </c>
       <c r="G38">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="H38" s="2">
         <v>45290</v>
       </c>
       <c r="I38">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="J38" t="inlineStr">
         <is>
@@ -4247,13 +4247,13 @@
         <v>45063</v>
       </c>
       <c r="G39">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="H39" s="2">
         <v>45247</v>
       </c>
       <c r="I39">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="J39" t="inlineStr">
         <is>
@@ -4350,13 +4350,13 @@
         <v>45177</v>
       </c>
       <c r="G40">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="H40" s="2">
         <v>45359</v>
       </c>
       <c r="I40">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="J40" t="inlineStr">
         <is>
@@ -4453,13 +4453,13 @@
         <v>45107</v>
       </c>
       <c r="G41">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="H41" s="2">
         <v>45290</v>
       </c>
       <c r="I41">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="J41" t="inlineStr">
         <is>
@@ -4556,7 +4556,7 @@
         <v>45265</v>
       </c>
       <c r="I42">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="J42" t="inlineStr">
         <is>
@@ -4653,13 +4653,13 @@
         <v>45098</v>
       </c>
       <c r="G43">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="H43" s="2">
         <v>45281</v>
       </c>
       <c r="I43">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="J43" t="inlineStr">
         <is>
@@ -4756,13 +4756,13 @@
         <v>45099</v>
       </c>
       <c r="G44">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="H44" s="2">
         <v>45282</v>
       </c>
       <c r="I44">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="J44" t="inlineStr">
         <is>
@@ -4859,13 +4859,13 @@
         <v>45106</v>
       </c>
       <c r="G45">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="H45" s="2">
         <v>45289</v>
       </c>
       <c r="I45">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="J45" t="inlineStr">
         <is>
@@ -4962,13 +4962,13 @@
         <v>45106</v>
       </c>
       <c r="G46">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="H46" s="2">
         <v>45289</v>
       </c>
       <c r="I46">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="J46" t="inlineStr">
         <is>
@@ -5065,13 +5065,13 @@
         <v>45120</v>
       </c>
       <c r="G47">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="H47" s="2">
         <v>45304</v>
       </c>
       <c r="I47">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="J47" t="inlineStr">
         <is>
@@ -5168,13 +5168,13 @@
         <v>45118</v>
       </c>
       <c r="G48">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="H48" s="2">
         <v>45302</v>
       </c>
       <c r="I48">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="J48" t="inlineStr">
         <is>
@@ -5271,13 +5271,13 @@
         <v>45152</v>
       </c>
       <c r="G49">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="H49" s="2">
         <v>45336</v>
       </c>
       <c r="I49">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="J49" t="inlineStr">
         <is>
@@ -5374,13 +5374,13 @@
         <v>45042</v>
       </c>
       <c r="G50">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="H50" s="2">
         <v>45225</v>
       </c>
       <c r="I50">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="J50" t="inlineStr">
         <is>
@@ -5477,13 +5477,13 @@
         <v>45122</v>
       <